<commit_message>
Update standby badges to be yellow for better visibility
Change the color of the 'Standby' badge from purple to yellow in the contestant table and standbys page, aligning with the 'Reschedule' badge styling.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 9c2f8590-8f03-4213-b20d-8645ac967b2c
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/qJaXBZ0
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -6,8 +6,9 @@
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
     <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
+    <sheet name="Groups" sheetId="5" r:id="rId5"/>
+    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -730,69 +731,69 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B2" t="str">
-        <v>Peter Adamidis</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C2">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
-        <v/>
+        <v>Melbourne</v>
       </c>
       <c r="I2" t="str">
         <v>assigned</v>
       </c>
       <c r="J2" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L2" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M2" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B3" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C3">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v>Melbourne</v>
+        <v>Footscray</v>
       </c>
       <c r="I3" t="str">
         <v>assigned</v>
       </c>
       <c r="J3" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -806,40 +807,40 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B4" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v>Footscray</v>
+        <v/>
       </c>
       <c r="I4" t="str">
         <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L4" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M4" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +852,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -884,78 +885,100 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>d87fb44f-0654-4aed-82a5-2ec6179bc2ab</v>
+        <v>1bd961ce-a605-4d4f-8bdd-844664d1b140</v>
       </c>
       <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" t="str">
         <v>B4</v>
       </c>
       <c r="F2" s="1">
-        <v>45994.48252188657</v>
-      </c>
-      <c r="G2" s="1">
-        <v>45994.35363413194</v>
+        <v>45994.1424034375</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1bd961ce-a605-4d4f-8bdd-844664d1b140</v>
+        <v>df836401-667b-4ac1-a68f-afe59d04a8b5</v>
       </c>
       <c r="B3" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C3" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="str">
-        <v>B4</v>
+        <v>B5</v>
       </c>
       <c r="F3" s="1">
-        <v>45994.1424034375</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>df836401-667b-4ac1-a68f-afe59d04a8b5</v>
-      </c>
-      <c r="B4" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C4" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="str">
-        <v>B5</v>
-      </c>
-      <c r="F4" s="1">
         <v>45994.26563376158</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G3" s="1">
         <v>45994.266912141204</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+      </c>
+      <c r="D2" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -985,7 +1008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add player role labeling to seating chart with colored tags
Implement player type selection (Player, Backup, Player Partner) in the seating chart, updating the UI and API to display colored tags in hover cards and persist changes.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 145fe5f0-8264-4130-a6d9-673d556b78e1
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/OQLXwTk
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Standbys" sheetId="4" r:id="rId4"/>
     <sheet name="Groups" sheetId="5" r:id="rId5"/>
     <sheet name="Block Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -769,78 +770,78 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B3" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v>Footscray</v>
+        <v/>
       </c>
       <c r="I3" t="str">
         <v>assigned</v>
       </c>
       <c r="J3" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L3" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M3" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B4" t="str">
-        <v>Peter Adamidis</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C4">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v/>
+        <v>Footscray</v>
       </c>
       <c r="I4" t="str">
         <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L4" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M4" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
   </sheetData>
@@ -852,7 +853,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -903,39 +904,16 @@
         <v>45994.1424034375</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>df836401-667b-4ac1-a68f-afe59d04a8b5</v>
-      </c>
-      <c r="B3" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C3" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="str">
-        <v>B5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>45994.26563376158</v>
-      </c>
-      <c r="G3" s="1">
-        <v>45994.266912141204</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -959,21 +937,35 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
+        <v>4e437be8-c154-44a8-b28d-d663c725a9a7</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D2" t="str">
         <v>pending</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
+      </c>
+      <c r="B3" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C3" t="str">
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+      </c>
+      <c r="D3" t="str">
+        <v>pending</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1398,4 +1390,52 @@
     <ignoredError numberStoredAsText="1" sqref="A1:D27"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Reason</v>
+      </c>
+      <c r="E1" t="str">
+        <v>CanceledAt</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>53071bc2-2450-41b6-ae7a-68a1ab35e988</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Standby - eligible for reschedule</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45998.113707662036</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update contestant details to allow player type selection
Adds local state for optimistic UI updates to the player type selector in the contestant detail view, ensuring the selected value is immediately reflected.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 78b033ad-838b-4f0e-976c-f4215fc2222a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/YW02W0t
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,11 +5,10 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
-    <sheet name="Groups" sheetId="5" r:id="rId5"/>
-    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
-    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
+    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -732,107 +731,107 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B2" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
-        <v>Melbourne</v>
+        <v/>
       </c>
       <c r="I2" t="str">
         <v>assigned</v>
       </c>
       <c r="J2" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L2" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M2" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B3" t="str">
-        <v>Peter Adamidis</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v/>
+        <v>Footscray</v>
       </c>
       <c r="I3" t="str">
         <v>assigned</v>
       </c>
       <c r="J3" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L3" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M3" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B4" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v>Footscray</v>
+        <v>Melbourne</v>
       </c>
       <c r="I4" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J4" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -853,66 +852,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Block</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Seat</v>
-      </c>
-      <c r="F1" t="str">
-        <v>BookingEmailSent</v>
-      </c>
-      <c r="G1" t="str">
-        <v>ConfirmedRSVP</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>1bd961ce-a605-4d4f-8bdd-844664d1b140</v>
-      </c>
-      <c r="B2" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="str">
-        <v>B4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45994.1424034375</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -970,7 +909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1000,7 +939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -1392,7 +1331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Show player type badges on the seating chart hover cards
Add playerType to the seat assignment data structure passed to SeatCard components in the seating chart page.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 2e76a460-5751-4abf-aee9-c5d6ec764a4f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/YW02W0t
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,10 +5,11 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
-    <sheet name="Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
-    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
+    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
+    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
+    <sheet name="Groups" sheetId="5" r:id="rId5"/>
+    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -828,7 +829,7 @@
         <v>Melbourne</v>
       </c>
       <c r="I4" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J4" t="str">
         <v>Peter Adamidis, Kathleen Reynolds</v>
@@ -852,6 +853,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Block</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="F1" t="str">
+        <v>BookingEmailSent</v>
+      </c>
+      <c r="G1" t="str">
+        <v>ConfirmedRSVP</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>15977bf4-12f1-4e38-bb08-bbd14d25e263</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -909,7 +967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -939,7 +997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -1331,7 +1389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update contestant import to include audition rating and fix column mappings
Correctly map Excel columns for audition rating, attending, mobility, and criminal records, and include audition rating in contestant data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 20b6e1a9-5bd3-4e9a-b84a-e2c3622f323b
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/PxMsbMJ
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -732,110 +732,110 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B2" t="str">
-        <v>Peter Adamidis</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C2">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
+        <v>Melbourne</v>
+      </c>
+      <c r="H2" t="str">
         <v/>
       </c>
       <c r="I2" t="str">
         <v>assigned</v>
       </c>
       <c r="J2" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L2" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M2" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B3" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v>Footscray</v>
+        <v/>
       </c>
       <c r="I3" t="str">
         <v>assigned</v>
       </c>
       <c r="J3" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L3" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M3" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B4" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v>Melbourne</v>
-      </c>
-      <c r="H4" t="str">
-        <v/>
+        <v>Footscray</v>
       </c>
       <c r="I4" t="str">
         <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>15977bf4-12f1-4e38-bb08-bbd14d25e263</v>
+        <v>c1c5b1c6-2598-472f-b2bc-c2b063643aa5</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
@@ -901,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>B1</v>
+        <v>A1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update contestant record day groups and backup timestamps
Update storage/backups/automatic-backup.json by modifying the exportedAt timestamp and adding new record day groups. Also, update the counts for groups within the backup data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 286eb5b5-5548-4c36-beaf-cc6894f85a69
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/XfYCHM7
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -972,7 +972,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -993,9 +993,41 @@
         <v>GRP001</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>8a692ea1-5300-494c-8074-19f479c5284d</v>
+      </c>
+      <c r="B3" t="str">
+        <v>GRP002</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>6f3cbd80-aae5-463e-836b-f1ecf0c504a2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>GRP003</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>3e3161fd-95f1-4ce9-9810-0ab1d377e2b2</v>
+      </c>
+      <c r="B5" t="str">
+        <v>GRP004</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>5b77330c-45dc-4177-b704-50e8d2e75d75</v>
+      </c>
+      <c r="B6" t="str">
+        <v>GRP005</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Resolve attendee names to IDs for accurate seating connections
Update server routes to map 'attendingWith' names to contestant IDs, ensuring correct linking logic in seat assignments.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 11a73985-94bb-4804-a56b-08d490333300
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/aNNKINw
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -732,110 +732,110 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B2" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
-        <v>Melbourne</v>
-      </c>
-      <c r="H2" t="str">
         <v/>
       </c>
       <c r="I2" t="str">
         <v>assigned</v>
       </c>
       <c r="J2" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L2" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M2" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B3" t="str">
-        <v>Peter Adamidis</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v/>
+        <v>Footscray</v>
       </c>
       <c r="I3" t="str">
         <v>assigned</v>
       </c>
       <c r="J3" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L3" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M3" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B4" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v>Footscray</v>
+        <v>Melbourne</v>
+      </c>
+      <c r="H4" t="str">
+        <v/>
       </c>
       <c r="I4" t="str">
         <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -856,7 +856,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -889,7 +889,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>c1c5b1c6-2598-472f-b2bc-c2b063643aa5</v>
+        <v>91e25164-6f67-42f7-b978-9132a406c060</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
@@ -901,19 +901,36 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>A1</v>
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>ff87f03b-8891-4bb6-ac5c-a510d216fdd6</v>
+      </c>
+      <c r="B3" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C3" t="str">
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>B1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -937,35 +954,21 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>4e437be8-c154-44a8-b28d-d663c725a9a7</v>
+        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D2" t="str">
         <v>pending</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
-      </c>
-      <c r="B3" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C3" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
-      </c>
-      <c r="D3" t="str">
-        <v>pending</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Resolve multiple linked contestants for seat assignments
Update the server route logic to correctly parse and resolve multiple comma-separated contestant names from the `attendingWith` field to their respective IDs. This change also updates a backup file with new identifiers and timestamps.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 3dc9e4f5-87e3-4c13-8ce0-617908d0059c
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/QJCF739
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -889,36 +889,36 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>91e25164-6f67-42f7-b978-9132a406c060</v>
+        <v>ff87f03b-8891-4bb6-ac5c-a510d216fdd6</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>C2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>ff87f03b-8891-4bb6-ac5c-a510d216fdd6</v>
+        <v>91e25164-6f67-42f7-b978-9132a406c060</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update contestant seating assignments with new identifiers
Updates record day and seat assignment data, including contestant IDs and assignment IDs, within the backup files.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 3306eff3-a970-4c1b-b9ff-e27e7da4d6c8
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/B0ltKDu
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -889,13 +889,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ff87f03b-8891-4bb6-ac5c-a510d216fdd6</v>
+        <v>91e25164-6f67-42f7-b978-9132a406c060</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -906,13 +906,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>91e25164-6f67-42f7-b978-9132a406c060</v>
+        <v>ff87f03b-8891-4bb6-ac5c-a510d216fdd6</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D3">
         <v>1</v>

</xml_diff>

<commit_message>
Add player type display and functionality to contestant details
Adds the `playerType` field to the `Contestant` interface, schema, and frontend display, allowing users to set and view a contestant's role (Player, Backup, or Partner) on their card.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 2e2801eb-7e60-476c-9b19-d87a056a0727
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/YhLUoqn
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -770,31 +770,34 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B3" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v>Footscray</v>
+        <v>Melbourne</v>
+      </c>
+      <c r="H3" t="str">
+        <v/>
       </c>
       <c r="I3" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J3" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -808,34 +811,31 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B4" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v>Melbourne</v>
-      </c>
-      <c r="H4" t="str">
-        <v/>
+        <v>Footscray</v>
       </c>
       <c r="I4" t="str">
         <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -856,7 +856,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -889,41 +889,24 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>91e25164-6f67-42f7-b978-9132a406c060</v>
+        <v>6da0092e-89ab-452b-80c7-216b45398ce1</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="str">
-        <v>B1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>ff87f03b-8891-4bb6-ac5c-a510d216fdd6</v>
-      </c>
-      <c r="B3" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C3" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="str">
-        <v>B2</v>
+        <v>B5</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Save contestant player type directly to their record
Adjusted the contestant update logic to include `playerType` in the contestant mutation, ensuring it persists correctly even for unseated contestants.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 038d4295-9e17-4f5d-8f78-626213d0527c
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/YhLUoqn
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,11 +5,10 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
-    <sheet name="Groups" sheetId="5" r:id="rId5"/>
-    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
-    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
+    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -770,34 +769,31 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B3" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C3">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v>Melbourne</v>
-      </c>
-      <c r="H3" t="str">
-        <v/>
+        <v>Footscray</v>
       </c>
       <c r="I3" t="str">
         <v>available</v>
       </c>
       <c r="J3" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -811,31 +807,34 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B4" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v>Footscray</v>
+        <v>Melbourne</v>
+      </c>
+      <c r="H4" t="str">
+        <v/>
       </c>
       <c r="I4" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J4" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -856,7 +855,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -872,46 +871,488 @@
         <v>ContestantID</v>
       </c>
       <c r="D1" t="str">
-        <v>Block</v>
+        <v>Status</v>
       </c>
       <c r="E1" t="str">
-        <v>Seat</v>
-      </c>
-      <c r="F1" t="str">
-        <v>BookingEmailSent</v>
-      </c>
-      <c r="G1" t="str">
-        <v>ConfirmedRSVP</v>
-      </c>
-      <c r="H1" t="str">
         <v>Notes</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>6da0092e-89ab-452b-80c7-216b45398ce1</v>
+        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="str">
-        <v>B5</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+      </c>
+      <c r="D2" t="str">
+        <v>pending</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>ReferenceNumber</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="B2" t="str">
+        <v>GRP001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>8a692ea1-5300-494c-8074-19f479c5284d</v>
+      </c>
+      <c r="B3" t="str">
+        <v>GRP002</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>6f3cbd80-aae5-463e-836b-f1ecf0c504a2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>GRP003</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>3e3161fd-95f1-4ce9-9810-0ab1d377e2b2</v>
+      </c>
+      <c r="B5" t="str">
+        <v>GRP004</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>5b77330c-45dc-4177-b704-50e8d2e75d75</v>
+      </c>
+      <c r="B6" t="str">
+        <v>GRP005</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>BlockNumber</v>
+      </c>
+      <c r="D1" t="str">
+        <v>BlockType</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>4d9813bd-7b99-4771-8da1-ad6fa01c1c6a</v>
+      </c>
+      <c r="B2" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>0aa42536-5b93-4be9-b0f5-95b1834f5cbf</v>
+      </c>
+      <c r="B3" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>ecc52a7a-af9e-483f-acfd-a9f947700b0c</v>
+      </c>
+      <c r="B4" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>d549fe45-cf7d-48a4-80c8-ad5d61aff471</v>
+      </c>
+      <c r="B5" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>9a62a9c4-3466-4b55-b61e-18cd2c67c4c1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>5b28e1f6-5c8a-4113-8834-9e8ab82228d6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>1d8f41b4-ac68-4c0d-89d5-3b22e715bc79</v>
+      </c>
+      <c r="B8" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>ef4554b1-e13a-4273-b9e6-c22d7e345256</v>
+      </c>
+      <c r="B9" t="str">
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>a679d473-0969-4bba-8648-2709c720fd24</v>
+      </c>
+      <c r="B10" t="str">
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>4ef50f67-0475-4c43-9591-c16952e5bb9d</v>
+      </c>
+      <c r="B11" t="str">
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>10be29ee-cd87-4370-993f-5ec424bdf89a</v>
+      </c>
+      <c r="B12" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>5a87fc3a-f172-456c-8817-1d2e9f749c41</v>
+      </c>
+      <c r="B13" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>ae5c8cf8-cd08-4a5b-9aa5-fdcd1f521fec</v>
+      </c>
+      <c r="B14" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>932323f8-f98a-4463-9650-1af4327df3a0</v>
+      </c>
+      <c r="B15" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>53eb80a7-59e5-4b78-b5f0-a3b366587096</v>
+      </c>
+      <c r="B16" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>690c620f-62d8-4293-b265-ce93eda1b896</v>
+      </c>
+      <c r="B17" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>306f44e0-79d0-424a-9eb7-126bbf71f301</v>
+      </c>
+      <c r="B18" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>badc1981-587e-4ebe-a4ca-d09f25a98a6b</v>
+      </c>
+      <c r="B19" t="str">
+        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>321d3111-fcc3-4246-8800-231133dd823d</v>
+      </c>
+      <c r="B20" t="str">
+        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>b248391e-18a0-4a53-bb54-8a0953ee2107</v>
+      </c>
+      <c r="B21" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>60ae8d96-a0a8-4bf5-ab37-7d9bbc68104a</v>
+      </c>
+      <c r="B22" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>19e49e78-cb04-48f1-b38c-1b5ae955926c</v>
+      </c>
+      <c r="B23" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>ff774508-8faa-437d-b90c-98020b4fce99</v>
+      </c>
+      <c r="B24" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>a2d47c69-208d-44d2-9033-3b6ab96616bd</v>
+      </c>
+      <c r="B25" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>d1e4b23c-d687-4444-8a8d-c54032f59162</v>
+      </c>
+      <c r="B26" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>51e9e36b-3d3e-42bb-87d4-4f6a5085828d</v>
+      </c>
+      <c r="B27" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D27"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -929,505 +1370,6 @@
         <v>ContestantID</v>
       </c>
       <c r="D1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
-      </c>
-      <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
-      </c>
-      <c r="D2" t="str">
-        <v>pending</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>ReferenceNumber</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="B2" t="str">
-        <v>GRP001</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>8a692ea1-5300-494c-8074-19f479c5284d</v>
-      </c>
-      <c r="B3" t="str">
-        <v>GRP002</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>6f3cbd80-aae5-463e-836b-f1ecf0c504a2</v>
-      </c>
-      <c r="B4" t="str">
-        <v>GRP003</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>3e3161fd-95f1-4ce9-9810-0ab1d377e2b2</v>
-      </c>
-      <c r="B5" t="str">
-        <v>GRP004</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>5b77330c-45dc-4177-b704-50e8d2e75d75</v>
-      </c>
-      <c r="B6" t="str">
-        <v>GRP005</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>BlockNumber</v>
-      </c>
-      <c r="D1" t="str">
-        <v>BlockType</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>4d9813bd-7b99-4771-8da1-ad6fa01c1c6a</v>
-      </c>
-      <c r="B2" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>0aa42536-5b93-4be9-b0f5-95b1834f5cbf</v>
-      </c>
-      <c r="B3" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>ecc52a7a-af9e-483f-acfd-a9f947700b0c</v>
-      </c>
-      <c r="B4" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>d549fe45-cf7d-48a4-80c8-ad5d61aff471</v>
-      </c>
-      <c r="B5" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>9a62a9c4-3466-4b55-b61e-18cd2c67c4c1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>5b28e1f6-5c8a-4113-8834-9e8ab82228d6</v>
-      </c>
-      <c r="B7" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>1d8f41b4-ac68-4c0d-89d5-3b22e715bc79</v>
-      </c>
-      <c r="B8" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>ef4554b1-e13a-4273-b9e6-c22d7e345256</v>
-      </c>
-      <c r="B9" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>a679d473-0969-4bba-8648-2709c720fd24</v>
-      </c>
-      <c r="B10" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>4ef50f67-0475-4c43-9591-c16952e5bb9d</v>
-      </c>
-      <c r="B11" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>10be29ee-cd87-4370-993f-5ec424bdf89a</v>
-      </c>
-      <c r="B12" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="D12" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>5a87fc3a-f172-456c-8817-1d2e9f749c41</v>
-      </c>
-      <c r="B13" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>ae5c8cf8-cd08-4a5b-9aa5-fdcd1f521fec</v>
-      </c>
-      <c r="B14" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C14">
-        <v>6</v>
-      </c>
-      <c r="D14" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>932323f8-f98a-4463-9650-1af4327df3a0</v>
-      </c>
-      <c r="B15" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>53eb80a7-59e5-4b78-b5f0-a3b366587096</v>
-      </c>
-      <c r="B16" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>690c620f-62d8-4293-b265-ce93eda1b896</v>
-      </c>
-      <c r="B17" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>306f44e0-79d0-424a-9eb7-126bbf71f301</v>
-      </c>
-      <c r="B18" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>badc1981-587e-4ebe-a4ca-d09f25a98a6b</v>
-      </c>
-      <c r="B19" t="str">
-        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>321d3111-fcc3-4246-8800-231133dd823d</v>
-      </c>
-      <c r="B20" t="str">
-        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>b248391e-18a0-4a53-bb54-8a0953ee2107</v>
-      </c>
-      <c r="B21" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>60ae8d96-a0a8-4bf5-ab37-7d9bbc68104a</v>
-      </c>
-      <c r="B22" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>19e49e78-cb04-48f1-b38c-1b5ae955926c</v>
-      </c>
-      <c r="B23" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="D23" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>ff774508-8faa-437d-b90c-98020b4fce99</v>
-      </c>
-      <c r="B24" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>a2d47c69-208d-44d2-9033-3b6ab96616bd</v>
-      </c>
-      <c r="B25" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>d1e4b23c-d687-4444-8a8d-c54032f59162</v>
-      </c>
-      <c r="B26" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C26">
-        <v>6</v>
-      </c>
-      <c r="D26" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>51e9e36b-3d3e-42bb-87d4-4f6a5085828d</v>
-      </c>
-      <c r="B27" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C27">
-        <v>7</v>
-      </c>
-      <c r="D27" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D27"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
         <v>Reason</v>
       </c>
       <c r="E1" t="str">

</xml_diff>

<commit_message>
Add player type information to contestant hover cards on seating chart
Adds player type display to the seating chart hover card by modifying the `SeatCard` component and updating the `automatic-backup.json` file to include player type data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 54a600d0-75c6-4172-82ac-30b0a77a86cc
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/kgVhT3T
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,10 +5,11 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
-    <sheet name="Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
-    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
+    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
+    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
+    <sheet name="Groups" sheetId="5" r:id="rId5"/>
+    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -731,40 +732,43 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B2" t="str">
-        <v>Peter Adamidis</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C2">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
+        <v>Melbourne</v>
+      </c>
+      <c r="H2" t="str">
         <v/>
       </c>
       <c r="I2" t="str">
         <v>assigned</v>
       </c>
       <c r="J2" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L2" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M2" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="3">
@@ -807,43 +811,43 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B4" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v>Melbourne</v>
+        <v/>
       </c>
       <c r="H4" t="str">
         <v/>
       </c>
       <c r="I4" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L4" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M4" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
   </sheetData>
@@ -855,6 +859,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Block</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="F1" t="str">
+        <v>BookingEmailSent</v>
+      </c>
+      <c r="G1" t="str">
+        <v>ConfirmedRSVP</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>ccd6460c-a021-4806-8e21-22177e70d8ba</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>B3</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -898,7 +959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -960,7 +1021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -1352,7 +1413,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update contestant data and remove seat assignments from backup
Add the `player_type` column to the database schema to resolve an import error and update contestant records.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f83d7cc0-fc2d-4ef0-98b9-d421175f3a9f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/kgVhT3T
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,11 +5,10 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
-    <sheet name="Groups" sheetId="5" r:id="rId5"/>
-    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
-    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
+    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -732,43 +731,43 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B2" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
-        <v>Melbourne</v>
+        <v/>
       </c>
       <c r="H2" t="str">
         <v/>
       </c>
       <c r="I2" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J2" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L2" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M2" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="3">
@@ -811,43 +810,43 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B4" t="str">
-        <v>Peter Adamidis</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C4">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v/>
+        <v>Melbourne</v>
       </c>
       <c r="H4" t="str">
         <v/>
       </c>
       <c r="I4" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J4" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L4" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M4" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
   </sheetData>
@@ -859,7 +858,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -875,46 +874,488 @@
         <v>ContestantID</v>
       </c>
       <c r="D1" t="str">
-        <v>Block</v>
+        <v>Status</v>
       </c>
       <c r="E1" t="str">
-        <v>Seat</v>
-      </c>
-      <c r="F1" t="str">
-        <v>BookingEmailSent</v>
-      </c>
-      <c r="G1" t="str">
-        <v>ConfirmedRSVP</v>
-      </c>
-      <c r="H1" t="str">
         <v>Notes</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ccd6460c-a021-4806-8e21-22177e70d8ba</v>
+        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="str">
-        <v>B3</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+      </c>
+      <c r="D2" t="str">
+        <v>pending</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>ReferenceNumber</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="B2" t="str">
+        <v>GRP001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>8a692ea1-5300-494c-8074-19f479c5284d</v>
+      </c>
+      <c r="B3" t="str">
+        <v>GRP002</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>6f3cbd80-aae5-463e-836b-f1ecf0c504a2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>GRP003</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>3e3161fd-95f1-4ce9-9810-0ab1d377e2b2</v>
+      </c>
+      <c r="B5" t="str">
+        <v>GRP004</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>5b77330c-45dc-4177-b704-50e8d2e75d75</v>
+      </c>
+      <c r="B6" t="str">
+        <v>GRP005</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>BlockNumber</v>
+      </c>
+      <c r="D1" t="str">
+        <v>BlockType</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>4d9813bd-7b99-4771-8da1-ad6fa01c1c6a</v>
+      </c>
+      <c r="B2" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>0aa42536-5b93-4be9-b0f5-95b1834f5cbf</v>
+      </c>
+      <c r="B3" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>ecc52a7a-af9e-483f-acfd-a9f947700b0c</v>
+      </c>
+      <c r="B4" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>d549fe45-cf7d-48a4-80c8-ad5d61aff471</v>
+      </c>
+      <c r="B5" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>9a62a9c4-3466-4b55-b61e-18cd2c67c4c1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>5b28e1f6-5c8a-4113-8834-9e8ab82228d6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>1d8f41b4-ac68-4c0d-89d5-3b22e715bc79</v>
+      </c>
+      <c r="B8" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>ef4554b1-e13a-4273-b9e6-c22d7e345256</v>
+      </c>
+      <c r="B9" t="str">
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>a679d473-0969-4bba-8648-2709c720fd24</v>
+      </c>
+      <c r="B10" t="str">
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>4ef50f67-0475-4c43-9591-c16952e5bb9d</v>
+      </c>
+      <c r="B11" t="str">
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>10be29ee-cd87-4370-993f-5ec424bdf89a</v>
+      </c>
+      <c r="B12" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>5a87fc3a-f172-456c-8817-1d2e9f749c41</v>
+      </c>
+      <c r="B13" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>ae5c8cf8-cd08-4a5b-9aa5-fdcd1f521fec</v>
+      </c>
+      <c r="B14" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>932323f8-f98a-4463-9650-1af4327df3a0</v>
+      </c>
+      <c r="B15" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>53eb80a7-59e5-4b78-b5f0-a3b366587096</v>
+      </c>
+      <c r="B16" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>690c620f-62d8-4293-b265-ce93eda1b896</v>
+      </c>
+      <c r="B17" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>306f44e0-79d0-424a-9eb7-126bbf71f301</v>
+      </c>
+      <c r="B18" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>badc1981-587e-4ebe-a4ca-d09f25a98a6b</v>
+      </c>
+      <c r="B19" t="str">
+        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>321d3111-fcc3-4246-8800-231133dd823d</v>
+      </c>
+      <c r="B20" t="str">
+        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>b248391e-18a0-4a53-bb54-8a0953ee2107</v>
+      </c>
+      <c r="B21" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>60ae8d96-a0a8-4bf5-ab37-7d9bbc68104a</v>
+      </c>
+      <c r="B22" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>19e49e78-cb04-48f1-b38c-1b5ae955926c</v>
+      </c>
+      <c r="B23" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>ff774508-8faa-437d-b90c-98020b4fce99</v>
+      </c>
+      <c r="B24" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>a2d47c69-208d-44d2-9033-3b6ab96616bd</v>
+      </c>
+      <c r="B25" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>d1e4b23c-d687-4444-8a8d-c54032f59162</v>
+      </c>
+      <c r="B26" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26" t="str">
+        <v>NPB</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>51e9e36b-3d3e-42bb-87d4-4f6a5085828d</v>
+      </c>
+      <c r="B27" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27" t="str">
+        <v>PB</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D27"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -932,505 +1373,6 @@
         <v>ContestantID</v>
       </c>
       <c r="D1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
-      </c>
-      <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
-      </c>
-      <c r="D2" t="str">
-        <v>pending</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>ReferenceNumber</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="B2" t="str">
-        <v>GRP001</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>8a692ea1-5300-494c-8074-19f479c5284d</v>
-      </c>
-      <c r="B3" t="str">
-        <v>GRP002</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>6f3cbd80-aae5-463e-836b-f1ecf0c504a2</v>
-      </c>
-      <c r="B4" t="str">
-        <v>GRP003</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>3e3161fd-95f1-4ce9-9810-0ab1d377e2b2</v>
-      </c>
-      <c r="B5" t="str">
-        <v>GRP004</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>5b77330c-45dc-4177-b704-50e8d2e75d75</v>
-      </c>
-      <c r="B6" t="str">
-        <v>GRP005</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>BlockNumber</v>
-      </c>
-      <c r="D1" t="str">
-        <v>BlockType</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>4d9813bd-7b99-4771-8da1-ad6fa01c1c6a</v>
-      </c>
-      <c r="B2" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>0aa42536-5b93-4be9-b0f5-95b1834f5cbf</v>
-      </c>
-      <c r="B3" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>ecc52a7a-af9e-483f-acfd-a9f947700b0c</v>
-      </c>
-      <c r="B4" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>d549fe45-cf7d-48a4-80c8-ad5d61aff471</v>
-      </c>
-      <c r="B5" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>9a62a9c4-3466-4b55-b61e-18cd2c67c4c1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>5b28e1f6-5c8a-4113-8834-9e8ab82228d6</v>
-      </c>
-      <c r="B7" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>1d8f41b4-ac68-4c0d-89d5-3b22e715bc79</v>
-      </c>
-      <c r="B8" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>ef4554b1-e13a-4273-b9e6-c22d7e345256</v>
-      </c>
-      <c r="B9" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>a679d473-0969-4bba-8648-2709c720fd24</v>
-      </c>
-      <c r="B10" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>4ef50f67-0475-4c43-9591-c16952e5bb9d</v>
-      </c>
-      <c r="B11" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>10be29ee-cd87-4370-993f-5ec424bdf89a</v>
-      </c>
-      <c r="B12" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="D12" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>5a87fc3a-f172-456c-8817-1d2e9f749c41</v>
-      </c>
-      <c r="B13" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>ae5c8cf8-cd08-4a5b-9aa5-fdcd1f521fec</v>
-      </c>
-      <c r="B14" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C14">
-        <v>6</v>
-      </c>
-      <c r="D14" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>932323f8-f98a-4463-9650-1af4327df3a0</v>
-      </c>
-      <c r="B15" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>53eb80a7-59e5-4b78-b5f0-a3b366587096</v>
-      </c>
-      <c r="B16" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>690c620f-62d8-4293-b265-ce93eda1b896</v>
-      </c>
-      <c r="B17" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>306f44e0-79d0-424a-9eb7-126bbf71f301</v>
-      </c>
-      <c r="B18" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>badc1981-587e-4ebe-a4ca-d09f25a98a6b</v>
-      </c>
-      <c r="B19" t="str">
-        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>321d3111-fcc3-4246-8800-231133dd823d</v>
-      </c>
-      <c r="B20" t="str">
-        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>b248391e-18a0-4a53-bb54-8a0953ee2107</v>
-      </c>
-      <c r="B21" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>60ae8d96-a0a8-4bf5-ab37-7d9bbc68104a</v>
-      </c>
-      <c r="B22" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>19e49e78-cb04-48f1-b38c-1b5ae955926c</v>
-      </c>
-      <c r="B23" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="D23" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>ff774508-8faa-437d-b90c-98020b4fce99</v>
-      </c>
-      <c r="B24" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>a2d47c69-208d-44d2-9033-3b6ab96616bd</v>
-      </c>
-      <c r="B25" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>d1e4b23c-d687-4444-8a8d-c54032f59162</v>
-      </c>
-      <c r="B26" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C26">
-        <v>6</v>
-      </c>
-      <c r="D26" t="str">
-        <v>NPB</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>51e9e36b-3d3e-42bb-87d4-4f6a5085828d</v>
-      </c>
-      <c r="B27" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C27">
-        <v>7</v>
-      </c>
-      <c r="D27" t="str">
-        <v>PB</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D27"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
         <v>Reason</v>
       </c>
       <c r="E1" t="str">

</xml_diff>

<commit_message>
Remove canceled contestants from backup data for accurate record keeping
Update the backup JSON by removing canceled assignment data for a contestant, resetting the canceled assignments count to zero.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 861ed045-a8d6-43ea-92af-a0a37176003a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/DHIhBWB
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -8,7 +8,6 @@
     <sheet name="Standbys" sheetId="3" r:id="rId3"/>
     <sheet name="Groups" sheetId="4" r:id="rId4"/>
     <sheet name="Block Types" sheetId="5" r:id="rId5"/>
-    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -69,9 +68,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,72 +729,72 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B2" t="str">
-        <v>Peter Adamidis</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <v/>
+        <v>Footscray</v>
       </c>
       <c r="I2" t="str">
         <v>available</v>
       </c>
       <c r="J2" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L2" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M2" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B3" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v>Footscray</v>
+        <v>Melbourne</v>
+      </c>
+      <c r="H3" t="str">
+        <v/>
       </c>
       <c r="I3" t="str">
         <v>available</v>
       </c>
       <c r="J3" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -810,25 +808,25 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B4" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v>Melbourne</v>
+        <v/>
       </c>
       <c r="H4" t="str">
         <v/>
@@ -837,16 +835,16 @@
         <v>available</v>
       </c>
       <c r="J4" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L4" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M4" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
   </sheetData>
@@ -1353,52 +1351,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:D27"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Reason</v>
-      </c>
-      <c r="E1" t="str">
-        <v>CanceledAt</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>53071bc2-2450-41b6-ae7a-68a1ab35e988</v>
-      </c>
-      <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Standby - eligible for reschedule</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45998.113707662036</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update button color to yellow and fix standby count
Modify the "Book as Standby" button's appearance to have a yellow background. Also, update the backup data to reflect zero standbys and adjust the export timestamp.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 422897ed-a68e-4f9b-843c-e89d008acb38
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/DHIhBWB
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,9 +5,8 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
-    <sheet name="Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Groups" sheetId="3" r:id="rId3"/>
+    <sheet name="Block Types" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -856,51 +855,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>69511596-e3b5-41be-a93b-920748af4fe0</v>
-      </c>
-      <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
-      </c>
-      <c r="D2" t="str">
-        <v>pending</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -961,7 +915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Replace Google Sheets sync with SharePoint Excel integration placeholder
Removes Google Sheets integration and adds a placeholder for future SharePoint Excel integration, updating component imports and removing unused logic.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 3cde51dc-ede0-44a4-be10-930a167f36c0
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/57glLrI
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -648,27 +648,27 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>628994d9-3a33-43b2-9214-c3bd9793ccd4</v>
       </c>
       <c r="B18" t="str">
-        <v>2026-02-04</v>
-      </c>
-      <c r="C18" t="str">
-        <v>RX1 - 1-5</v>
+        <v>2026-02-18</v>
       </c>
       <c r="D18" t="str">
-        <v>ready</v>
+        <v>draft</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>628994d9-3a33-43b2-9214-c3bd9793ccd4</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="B19" t="str">
-        <v>2026-02-18</v>
+        <v>2026-02-04</v>
+      </c>
+      <c r="C19" t="str">
+        <v>RX EP 1 - 5</v>
       </c>
       <c r="D19" t="str">
-        <v>draft</v>
+        <v>ready</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update contestant status and seat assignments for game show management
Modifies 'storage/backups/automatic-backup.json' to reflect updated 'exportedAt' timestamp, changes contestant availability status from 'available' to 'assigned' for specific contestants, and adds new 'seatAssignments' entries with detailed contestant and seat information, including null values for standby/swap fields.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: b512a484-c2e3-41fe-a6c6-53b854630926
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/b9xQrXb
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,8 +5,9 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Groups" sheetId="3" r:id="rId3"/>
-    <sheet name="Block Types" sheetId="4" r:id="rId4"/>
+    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -728,31 +729,34 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B2" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
-        <v>Footscray</v>
+        <v>Melbourne</v>
+      </c>
+      <c r="H2" t="str">
+        <v/>
       </c>
       <c r="I2" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J2" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -766,84 +770,81 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B3" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C3">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v>Melbourne</v>
+        <v/>
       </c>
       <c r="H3" t="str">
         <v/>
       </c>
       <c r="I3" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J3" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L3" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M3" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B4" t="str">
-        <v>Peter Adamidis</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C4">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v/>
-      </c>
-      <c r="H4" t="str">
-        <v/>
+        <v>Footscray</v>
       </c>
       <c r="I4" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L4" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M4" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
   </sheetData>
@@ -855,6 +856,97 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Block</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="F1" t="str">
+        <v>BookingEmailSent</v>
+      </c>
+      <c r="G1" t="str">
+        <v>ConfirmedRSVP</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>a001b03c-7c5b-46ba-957e-bb1aeca919d8</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>d5957e66-cb7f-4267-bbb8-1c8c7298b62b</v>
+      </c>
+      <c r="B3" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C3" t="str">
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>36cd33af-9bac-49bf-bb65-5b0cc9ad1077</v>
+      </c>
+      <c r="B4" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C4" t="str">
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -915,7 +1007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update status badge colors on the standbys page to match the contestants page
Adjusted status badge styling in `standbys.tsx` to align with the visual theme of the contestants page, specifically updating colors for 'Assigned', 'Invited', 'Booked', 'Declined', and 'Seated' statuses. Also updated backup data in `automatic-backup.json` and `automatic-backup.xlsx` to reflect a new standby entry and adjust counts.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 8a707bb6-45e7-49d0-a2d4-3c31db280d80
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/N3C1Mnm
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -6,8 +6,9 @@
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
     <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
+    <sheet name="Groups" sheetId="5" r:id="rId5"/>
+    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -856,7 +857,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -889,63 +890,94 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>a001b03c-7c5b-46ba-957e-bb1aeca919d8</v>
+        <v>d5957e66-cb7f-4267-bbb8-1c8c7298b62b</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>A1</v>
+        <v>A2</v>
+      </c>
+      <c r="H2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>d5957e66-cb7f-4267-bbb8-1c8c7298b62b</v>
+        <v>36cd33af-9bac-49bf-bb65-5b0cc9ad1077</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>A2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>36cd33af-9bac-49bf-bb65-5b0cc9ad1077</v>
-      </c>
-      <c r="B4" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C4" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="str">
         <v>A3</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>cc98ff1c-1a1d-43f8-82ea-abcca3482b1e</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+      </c>
+      <c r="D2" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1007,7 +1039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Make booking tracking columns hideable and highlight the signed-in status
Update `COLUMN_CONFIG` in `booking-master.tsx` to make columns from "emailSent" onwards hideable by setting `alwaysVisible` to `false`. Also, update the styling for the "SIGNED IN" column header and cell to use a distinct green background, and modify the checkbox styling within the "Signed In" column to use a green border and fill color.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 8ff3f5e2-2677-486f-902e-d0f78b0cfeff
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/N3C1Mnm
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -650,32 +650,21 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>628994d9-3a33-43b2-9214-c3bd9793ccd4</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="B18" t="str">
-        <v>2026-02-18</v>
+        <v>2026-02-04</v>
+      </c>
+      <c r="C18" t="str">
+        <v>RX EP 1 - 5</v>
       </c>
       <c r="D18" t="str">
-        <v>draft</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="B19" t="str">
-        <v>2026-02-04</v>
-      </c>
-      <c r="C19" t="str">
-        <v>RX EP 1 - 5</v>
-      </c>
-      <c r="D19" t="str">
         <v>ready</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E18"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix layout issue with group ID on contestant cards
Truncate long group IDs on the contestant details dialog and add overflow handling to prevent text overlap.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f9b5f05a-461c-48f5-8a0a-369b3b5f7950
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/N3C1Mnm
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -6,9 +6,8 @@
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
     <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
-    <sheet name="Groups" sheetId="5" r:id="rId5"/>
-    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -821,6 +820,9 @@
       <c r="G4" t="str">
         <v>Footscray</v>
       </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
       <c r="I4" t="str">
         <v>assigned</v>
       </c>
@@ -846,7 +848,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -899,74 +901,46 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>36cd33af-9bac-49bf-bb65-5b0cc9ad1077</v>
+        <v>479fcb75-5c6b-42a9-a757-6e4ae8cef47e</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>36cd33af-9bac-49bf-bb65-5b0cc9ad1077</v>
+      </c>
+      <c r="B4" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C4" t="str">
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
         <v>A3</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>cc98ff1c-1a1d-43f8-82ea-abcca3482b1e</v>
-      </c>
-      <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
-      </c>
-      <c r="D2" t="str">
-        <v>pending</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1028,7 +1002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add RX Day Mode to the contestant management system
Updates backup data and documentation to reflect the addition of the RX Day Mode feature, including lock/unlock functionality, tracked swaps, and relevant API endpoints.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 3ca98112-8e1a-4fc7-893d-69c7fdb6aa48
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/aSqXDn9
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -881,39 +881,39 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>d5957e66-cb7f-4267-bbb8-1c8c7298b62b</v>
+        <v>479fcb75-5c6b-42a9-a757-6e4ae8cef47e</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>A2</v>
-      </c>
-      <c r="H2" t="str">
-        <v/>
+        <v>A4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>479fcb75-5c6b-42a9-a757-6e4ae8cef47e</v>
+        <v>d5957e66-cb7f-4267-bbb8-1c8c7298b62b</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>A4</v>
+        <v>A2</v>
+      </c>
+      <c r="H3" t="str">
+        <v/>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Add visual indicators and confirmation dialogs for locked contestant swaps
Introduces the "MOVED" badge with tooltips for swapped contestants, and implements a confirmation dialog for swaps when RX Day Mode is locked, preserving original seat data and updating the UI.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: 415c3ba7-5c5d-44db-a361-dfc8fc3edc06
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/bmiD0kY
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -898,39 +898,39 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>d5957e66-cb7f-4267-bbb8-1c8c7298b62b</v>
+        <v>36cd33af-9bac-49bf-bb65-5b0cc9ad1077</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>A2</v>
-      </c>
-      <c r="H3" t="str">
-        <v/>
+        <v>A3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>36cd33af-9bac-49bf-bb65-5b0cc9ad1077</v>
+        <v>d5957e66-cb7f-4267-bbb8-1c8c7298b62b</v>
       </c>
       <c r="B4" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C4" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <v>A3</v>
+        <v>A2</v>
+      </c>
+      <c r="H4" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve seat assignment tracking and display for moved contestants
Add `swappedAt` to API response for seat assignments, implement tracked move API endpoint, and enhance seat card and hover card to display moved contestant information including their original seat.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 505810f6-df70-4424-b670-24365735e435
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/hRPdIWM
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -718,25 +718,25 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B2" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
-        <v>Melbourne</v>
+        <v>Footscray</v>
       </c>
       <c r="H2" t="str">
         <v/>
@@ -745,7 +745,7 @@
         <v>assigned</v>
       </c>
       <c r="J2" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -759,25 +759,25 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B3" t="str">
-        <v>Peter Adamidis</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C3">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D3" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E3" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F3" t="str">
         <v>498086080</v>
       </c>
       <c r="G3" t="str">
-        <v/>
+        <v>Melbourne</v>
       </c>
       <c r="H3" t="str">
         <v/>
@@ -786,39 +786,39 @@
         <v>assigned</v>
       </c>
       <c r="J3" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K3" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L3" t="str">
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="M3" t="str">
-        <v>Broken Leg</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B4" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E4" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F4" t="str">
         <v>498086080</v>
       </c>
       <c r="G4" t="str">
-        <v>Footscray</v>
+        <v/>
       </c>
       <c r="H4" t="str">
         <v/>
@@ -827,16 +827,16 @@
         <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
       <c r="K4" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
       <c r="L4" t="str">
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="M4" t="str">
-        <v>N/A</v>
+        <v>Broken Leg</v>
       </c>
     </row>
   </sheetData>
@@ -881,24 +881,24 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>36cd33af-9bac-49bf-bb65-5b0cc9ad1077</v>
+        <v>20946cbf-8f88-4629-a6d2-d8510554cb9a</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>479fcb75-5c6b-42a9-a757-6e4ae8cef47e</v>
+        <v>c1d29895-e1ab-4926-8d3b-29a9df7058de</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
@@ -910,27 +910,24 @@
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>B4</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>d5957e66-cb7f-4267-bbb8-1c8c7298b62b</v>
+        <v>f8463207-3f82-429c-bf09-986ae9a6cc97</v>
       </c>
       <c r="B4" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C4" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <v>B2</v>
-      </c>
-      <c r="H4" t="str">
-        <v/>
+        <v>D3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refine seat assignment tracking and add test contestants
Update automatic backup file to reflect changes in seat assignment tracking logic, including original positions and swap timestamps, and add 100 generated test contestants to the system.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 8ec2c28a-34db-433c-9d1c-a76470f1d806
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/hRPdIWM
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -893,41 +893,41 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>C1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>c1d29895-e1ab-4926-8d3b-29a9df7058de</v>
+        <v>f8463207-3f82-429c-bf09-986ae9a6cc97</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>C3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>f8463207-3f82-429c-bf09-986ae9a6cc97</v>
+        <v>c1d29895-e1ab-4926-8d3b-29a9df7058de</v>
       </c>
       <c r="B4" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C4" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <v>D3</v>
+        <v>B4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enable horizontal scrolling for the contestant table and add placeholder images
Update contestant table layout to include horizontal scrolling with overflow-x-auto and a min-width of 1400px. Also, populate `photoUrl` fields for existing and new contestants in the backup data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 5f20c4c3-4086-4a28-a3a2-86e2de641f10
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/G1e7c0s
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,9 +5,8 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Groups" sheetId="3" r:id="rId3"/>
+    <sheet name="Block Types" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -670,7 +669,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -742,7 +741,7 @@
         <v/>
       </c>
       <c r="I2" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J2" t="str">
         <v>Peter Adamidis, Felicity Parker-Hill</v>
@@ -783,7 +782,7 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J3" t="str">
         <v>Peter Adamidis, Kathleen Reynolds</v>
@@ -800,144 +799,2953 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
+        <v>8e115c7e-8033-4466-bcb9-07ea089eb4be</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Chloe Taylor</v>
+      </c>
+      <c r="C4">
+        <v>64</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E4" t="str">
+        <v>chloe.taylor7@gmail.com</v>
+      </c>
+      <c r="F4" t="str">
+        <v>0412 903 254</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Townsville</v>
+      </c>
+      <c r="H4" t="str">
+        <v>C</v>
+      </c>
+      <c r="I4" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Audrey Ramirez</v>
+      </c>
+      <c r="C5">
+        <v>43</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E5" t="str">
+        <v>audrey.ramirez12@gmail.com</v>
+      </c>
+      <c r="F5" t="str">
+        <v>0411 212 619</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Brisbane</v>
+      </c>
+      <c r="H5" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I5" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Maya Moore</v>
+      </c>
+      <c r="C6">
+        <v>43</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E6" t="str">
+        <v>maya.moore54@outlook.com</v>
+      </c>
+      <c r="F6" t="str">
+        <v>0400 718 585</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Toowoomba</v>
+      </c>
+      <c r="H6" t="str">
+        <v>C</v>
+      </c>
+      <c r="I6" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
         <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B7" t="str">
         <v>Peter Adamidis</v>
       </c>
-      <c r="C4">
+      <c r="C7">
         <v>34</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D7" t="str">
         <v>Not Specified</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E7" t="str">
         <v>peter.adamidis@gmail.com</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F7" t="str">
         <v>498086080</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G7" t="str">
         <v/>
       </c>
-      <c r="H4" t="str">
+      <c r="H7" t="str">
         <v/>
       </c>
-      <c r="I4" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J4" t="str">
+      <c r="I7" t="str">
+        <v>available</v>
+      </c>
+      <c r="J7" t="str">
         <v>Kathleen Reynolds, Felicity Parker-Hill</v>
       </c>
-      <c r="K4" t="str">
+      <c r="K7" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
       </c>
-      <c r="L4" t="str">
+      <c r="L7" t="str">
         <v>Y</v>
       </c>
-      <c r="M4" t="str">
+      <c r="M7" t="str">
         <v>Broken Leg</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>b9e02c2d-410d-4307-811c-7e52cf93b14b</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Emily Moore</v>
+      </c>
+      <c r="C8">
+        <v>49</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E8" t="str">
+        <v>emily.moore11@hotmail.com</v>
+      </c>
+      <c r="F8" t="str">
+        <v>0410 362 279</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="H8" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I8" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Caroline Taylor</v>
+      </c>
+      <c r="C9">
+        <v>41</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E9" t="str">
+        <v>caroline.taylor54@outlook.com</v>
+      </c>
+      <c r="F9" t="str">
+        <v>0402 864 601</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Darwin</v>
+      </c>
+      <c r="H9" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I9" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Stella Martinez</v>
+      </c>
+      <c r="C10">
+        <v>47</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E10" t="str">
+        <v>stella.martinez75@gmail.com</v>
+      </c>
+      <c r="F10" t="str">
+        <v>0404 227 272</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Ballarat</v>
+      </c>
+      <c r="H10" t="str">
+        <v>C</v>
+      </c>
+      <c r="I10" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Ella Anderson</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E11" t="str">
+        <v>ella.anderson1@yahoo.com</v>
+      </c>
+      <c r="F11" t="str">
+        <v>0412 908 910</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Geelong</v>
+      </c>
+      <c r="H11" t="str">
+        <v>B</v>
+      </c>
+      <c r="I11" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Abigail Jackson</v>
+      </c>
+      <c r="C12">
+        <v>36</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E12" t="str">
+        <v>abigail.jackson65@outlook.com</v>
+      </c>
+      <c r="F12" t="str">
+        <v>0411 824 257</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Newcastle</v>
+      </c>
+      <c r="H12" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I12" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Evelyn Sanchez</v>
+      </c>
+      <c r="C13">
+        <v>56</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E13" t="str">
+        <v>evelyn.sanchez9@gmail.com</v>
+      </c>
+      <c r="F13" t="str">
+        <v>0404 119 469</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Gold Coast</v>
+      </c>
+      <c r="H13" t="str">
+        <v>B</v>
+      </c>
+      <c r="I13" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Hannah Torres</v>
+      </c>
+      <c r="C14">
+        <v>41</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E14" t="str">
+        <v>hannah.torres86@yahoo.com</v>
+      </c>
+      <c r="F14" t="str">
+        <v>0402 688 409</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Wollongong</v>
+      </c>
+      <c r="H14" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I14" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Audrey Smith</v>
+      </c>
+      <c r="C15">
+        <v>23</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E15" t="str">
+        <v>audrey.smith66@gmail.com</v>
+      </c>
+      <c r="F15" t="str">
+        <v>0410 904 568</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Ballarat</v>
+      </c>
+      <c r="H15" t="str">
+        <v>B</v>
+      </c>
+      <c r="I15" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>97646711-3e33-4ee9-8d83-bd6e0363ece0</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Audrey Martin</v>
+      </c>
+      <c r="C16">
+        <v>32</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E16" t="str">
+        <v>audrey.martin33@yahoo.com</v>
+      </c>
+      <c r="F16" t="str">
+        <v>0403 767 239</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Adelaide</v>
+      </c>
+      <c r="H16" t="str">
+        <v>A</v>
+      </c>
+      <c r="I16" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>d37f9e40-d1a2-4238-9089-80517a709859</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Mia Roberts</v>
+      </c>
+      <c r="C17">
+        <v>28</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E17" t="str">
+        <v>mia.roberts81@hotmail.com</v>
+      </c>
+      <c r="F17" t="str">
+        <v>0412 368 553</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Toowoomba</v>
+      </c>
+      <c r="H17" t="str">
+        <v>C</v>
+      </c>
+      <c r="I17" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Chloe Jones</v>
+      </c>
+      <c r="C18">
+        <v>46</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E18" t="str">
+        <v>chloe.jones20@outlook.com</v>
+      </c>
+      <c r="F18" t="str">
+        <v>0411 294 635</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Toowoomba</v>
+      </c>
+      <c r="H18" t="str">
+        <v>C</v>
+      </c>
+      <c r="I18" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>eff76f3c-c868-4954-99ea-92a4ae6c8067</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Abigail Lee</v>
+      </c>
+      <c r="C19">
+        <v>27</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E19" t="str">
+        <v>abigail.lee94@hotmail.com</v>
+      </c>
+      <c r="F19" t="str">
+        <v>0402 888 384</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Wollongong</v>
+      </c>
+      <c r="H19" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I19" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Grace Scott</v>
+      </c>
+      <c r="C20">
+        <v>35</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E20" t="str">
+        <v>grace.scott40@outlook.com</v>
+      </c>
+      <c r="F20" t="str">
+        <v>0401 870 853</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Ballarat</v>
+      </c>
+      <c r="H20" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I20" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Aurora Rodriguez</v>
+      </c>
+      <c r="C21">
+        <v>25</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E21" t="str">
+        <v>aurora.rodriguez20@yahoo.com</v>
+      </c>
+      <c r="F21" t="str">
+        <v>0404 720 692</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Hobart</v>
+      </c>
+      <c r="H21" t="str">
+        <v>A</v>
+      </c>
+      <c r="I21" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>992418b2-3029-4752-9552-0aa886433657</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Zoe Brown</v>
+      </c>
+      <c r="C22">
+        <v>44</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E22" t="str">
+        <v>zoe.brown45@outlook.com</v>
+      </c>
+      <c r="F22" t="str">
+        <v>0401 578 107</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Sydney</v>
+      </c>
+      <c r="H22" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I22" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>210066e7-58e9-4ebb-a504-dfbf383961b5</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Grace Scott</v>
+      </c>
+      <c r="C23">
+        <v>47</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E23" t="str">
+        <v>grace.scott94@hotmail.com</v>
+      </c>
+      <c r="F23" t="str">
+        <v>0410 377 869</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Toowoomba</v>
+      </c>
+      <c r="H23" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I23" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Paisley Lee</v>
+      </c>
+      <c r="C24">
+        <v>61</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E24" t="str">
+        <v>paisley.lee78@hotmail.com</v>
+      </c>
+      <c r="F24" t="str">
+        <v>0400 179 607</v>
+      </c>
+      <c r="G24" t="str">
+        <v>Ballarat</v>
+      </c>
+      <c r="H24" t="str">
+        <v>B</v>
+      </c>
+      <c r="I24" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>0a153155-dcf5-4d56-9ed1-8960501157f8</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Aurora Gonzalez</v>
+      </c>
+      <c r="C25">
+        <v>42</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E25" t="str">
+        <v>aurora.gonzalez29@outlook.com</v>
+      </c>
+      <c r="F25" t="str">
+        <v>0404 610 172</v>
+      </c>
+      <c r="G25" t="str">
+        <v>Toowoomba</v>
+      </c>
+      <c r="H25" t="str">
+        <v>A</v>
+      </c>
+      <c r="I25" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>5c5fe7f9-35dd-4685-af6b-e44a56c1d47c</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Charlotte Johnson</v>
+      </c>
+      <c r="C26">
+        <v>59</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E26" t="str">
+        <v>charlotte.johnson36@yahoo.com</v>
+      </c>
+      <c r="F26" t="str">
+        <v>0410 304 177</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="H26" t="str">
+        <v>A</v>
+      </c>
+      <c r="I26" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Audrey Thomas</v>
+      </c>
+      <c r="C27">
+        <v>21</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E27" t="str">
+        <v>audrey.thomas38@gmail.com</v>
+      </c>
+      <c r="F27" t="str">
+        <v>0400 437 270</v>
+      </c>
+      <c r="G27" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="H27" t="str">
+        <v>C</v>
+      </c>
+      <c r="I27" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Emilia Thompson</v>
+      </c>
+      <c r="C28">
+        <v>48</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E28" t="str">
+        <v>emilia.thompson0@gmail.com</v>
+      </c>
+      <c r="F28" t="str">
+        <v>0404 992 451</v>
+      </c>
+      <c r="G28" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="H28" t="str">
+        <v>B</v>
+      </c>
+      <c r="I28" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>0dd7de5c-0409-45e3-84a5-5f2ffbd591d8</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Harper Sanchez</v>
+      </c>
+      <c r="C29">
+        <v>21</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E29" t="str">
+        <v>harper.sanchez76@gmail.com</v>
+      </c>
+      <c r="F29" t="str">
+        <v>0411 422 972</v>
+      </c>
+      <c r="G29" t="str">
+        <v>Geelong</v>
+      </c>
+      <c r="H29" t="str">
+        <v>C</v>
+      </c>
+      <c r="I29" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>0669e014-c952-45fd-9791-36cbe1d51444</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Sofia Williams</v>
+      </c>
+      <c r="C30">
+        <v>31</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E30" t="str">
+        <v>sofia.williams39@yahoo.com</v>
+      </c>
+      <c r="F30" t="str">
+        <v>0403 299 421</v>
+      </c>
+      <c r="G30" t="str">
+        <v>Geelong</v>
+      </c>
+      <c r="H30" t="str">
+        <v>A</v>
+      </c>
+      <c r="I30" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Harper Lewis</v>
+      </c>
+      <c r="C31">
+        <v>44</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E31" t="str">
+        <v>harper.lewis57@hotmail.com</v>
+      </c>
+      <c r="F31" t="str">
+        <v>0411 652 121</v>
+      </c>
+      <c r="G31" t="str">
+        <v>Geelong</v>
+      </c>
+      <c r="H31" t="str">
+        <v>B</v>
+      </c>
+      <c r="I31" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Aria Scott</v>
+      </c>
+      <c r="C32">
+        <v>60</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E32" t="str">
+        <v>aria.scott42@outlook.com</v>
+      </c>
+      <c r="F32" t="str">
+        <v>0401 330 548</v>
+      </c>
+      <c r="G32" t="str">
+        <v>Hobart</v>
+      </c>
+      <c r="H32" t="str">
+        <v>C</v>
+      </c>
+      <c r="I32" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Emilia Miller</v>
+      </c>
+      <c r="C33">
+        <v>40</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E33" t="str">
+        <v>emilia.miller56@outlook.com</v>
+      </c>
+      <c r="F33" t="str">
+        <v>0403 506 698</v>
+      </c>
+      <c r="G33" t="str">
+        <v>Melbourne</v>
+      </c>
+      <c r="H33" t="str">
+        <v>B</v>
+      </c>
+      <c r="I33" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Emily Thomas</v>
+      </c>
+      <c r="C34">
+        <v>57</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E34" t="str">
+        <v>emily.thomas25@outlook.com</v>
+      </c>
+      <c r="F34" t="str">
+        <v>0402 648 577</v>
+      </c>
+      <c r="G34" t="str">
+        <v>Geelong</v>
+      </c>
+      <c r="H34" t="str">
+        <v>C</v>
+      </c>
+      <c r="I34" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>2c188398-79a8-4bf6-b740-1ad9d535662e</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Everly Torres</v>
+      </c>
+      <c r="C35">
+        <v>42</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E35" t="str">
+        <v>everly.torres12@gmail.com</v>
+      </c>
+      <c r="F35" t="str">
+        <v>0412 804 179</v>
+      </c>
+      <c r="G35" t="str">
+        <v>Sydney</v>
+      </c>
+      <c r="H35" t="str">
+        <v>A+</v>
+      </c>
+      <c r="I35" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>55099144-967b-4cf2-b4ed-3cfe46413c92</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Maya Hernandez</v>
+      </c>
+      <c r="C36">
+        <v>43</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E36" t="str">
+        <v>maya.hernandez32@outlook.com</v>
+      </c>
+      <c r="F36" t="str">
+        <v>0400 358 904</v>
+      </c>
+      <c r="G36" t="str">
+        <v>Brisbane</v>
+      </c>
+      <c r="H36" t="str">
+        <v>C</v>
+      </c>
+      <c r="I36" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Paisley Scott</v>
+      </c>
+      <c r="C37">
+        <v>27</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E37" t="str">
+        <v>paisley.scott78@yahoo.com</v>
+      </c>
+      <c r="F37" t="str">
+        <v>0410 215 419</v>
+      </c>
+      <c r="G37" t="str">
+        <v>Ballarat</v>
+      </c>
+      <c r="H37" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I37" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Aria Lopez</v>
+      </c>
+      <c r="C38">
+        <v>44</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E38" t="str">
+        <v>aria.lopez55@hotmail.com</v>
+      </c>
+      <c r="F38" t="str">
+        <v>0404 812 491</v>
+      </c>
+      <c r="G38" t="str">
+        <v>Sydney</v>
+      </c>
+      <c r="H38" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I38" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Isabella Brown</v>
+      </c>
+      <c r="C39">
+        <v>55</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E39" t="str">
+        <v>isabella.brown43@outlook.com</v>
+      </c>
+      <c r="F39" t="str">
+        <v>0403 771 690</v>
+      </c>
+      <c r="G39" t="str">
+        <v>Darwin</v>
+      </c>
+      <c r="H39" t="str">
+        <v>B</v>
+      </c>
+      <c r="I39" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Stella Garcia</v>
+      </c>
+      <c r="C40">
+        <v>53</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E40" t="str">
+        <v>stella.garcia89@hotmail.com</v>
+      </c>
+      <c r="F40" t="str">
+        <v>0403 655 540</v>
+      </c>
+      <c r="G40" t="str">
+        <v>Toowoomba</v>
+      </c>
+      <c r="H40" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I40" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>c1783cdf-a656-46b4-9331-4d9d18d40b51</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Aurora Walker</v>
+      </c>
+      <c r="C41">
+        <v>61</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E41" t="str">
+        <v>aurora.walker1@outlook.com</v>
+      </c>
+      <c r="F41" t="str">
+        <v>0403 522 404</v>
+      </c>
+      <c r="G41" t="str">
+        <v>Darwin</v>
+      </c>
+      <c r="H41" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I41" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>32ffeaf9-5f22-4db7-a70b-cbaab834db0d</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Isabella Hill</v>
+      </c>
+      <c r="C42">
+        <v>30</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E42" t="str">
+        <v>isabella.hill77@hotmail.com</v>
+      </c>
+      <c r="F42" t="str">
+        <v>0412 663 356</v>
+      </c>
+      <c r="G42" t="str">
+        <v>Darwin</v>
+      </c>
+      <c r="H42" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I42" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Victoria Carter</v>
+      </c>
+      <c r="C43">
+        <v>25</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E43" t="str">
+        <v>victoria.carter74@gmail.com</v>
+      </c>
+      <c r="F43" t="str">
+        <v>0411 641 632</v>
+      </c>
+      <c r="G43" t="str">
+        <v>Gold Coast</v>
+      </c>
+      <c r="H43" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I43" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>c5fdfaeb-862e-43ab-bf0e-ff3e14e5dbb3</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Hannah Martin</v>
+      </c>
+      <c r="C44">
+        <v>27</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E44" t="str">
+        <v>hannah.martin78@yahoo.com</v>
+      </c>
+      <c r="F44" t="str">
+        <v>0410 940 985</v>
+      </c>
+      <c r="G44" t="str">
+        <v>Hobart</v>
+      </c>
+      <c r="H44" t="str">
+        <v>B</v>
+      </c>
+      <c r="I44" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>f6a281bb-caec-44cf-a596-a6e92d6e2610</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Leah Scott</v>
+      </c>
+      <c r="C45">
+        <v>21</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E45" t="str">
+        <v>leah.scott74@gmail.com</v>
+      </c>
+      <c r="F45" t="str">
+        <v>0402 414 358</v>
+      </c>
+      <c r="G45" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="H45" t="str">
+        <v>B</v>
+      </c>
+      <c r="I45" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Stella Hall</v>
+      </c>
+      <c r="C46">
+        <v>58</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E46" t="str">
+        <v>stella.hall72@gmail.com</v>
+      </c>
+      <c r="F46" t="str">
+        <v>0410 133 818</v>
+      </c>
+      <c r="G46" t="str">
+        <v>Wollongong</v>
+      </c>
+      <c r="H46" t="str">
+        <v>B</v>
+      </c>
+      <c r="I46" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Evelyn Clark</v>
+      </c>
+      <c r="C47">
+        <v>22</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E47" t="str">
+        <v>evelyn.clark47@outlook.com</v>
+      </c>
+      <c r="F47" t="str">
+        <v>0410 941 656</v>
+      </c>
+      <c r="G47" t="str">
+        <v>Hobart</v>
+      </c>
+      <c r="H47" t="str">
+        <v>C</v>
+      </c>
+      <c r="I47" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Stella Green</v>
+      </c>
+      <c r="C48">
+        <v>65</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E48" t="str">
+        <v>stella.green92@gmail.com</v>
+      </c>
+      <c r="F48" t="str">
+        <v>0404 230 858</v>
+      </c>
+      <c r="G48" t="str">
+        <v>Wollongong</v>
+      </c>
+      <c r="H48" t="str">
+        <v>A</v>
+      </c>
+      <c r="I48" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Violet Hall</v>
+      </c>
+      <c r="C49">
+        <v>61</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E49" t="str">
+        <v>violet.hall8@yahoo.com</v>
+      </c>
+      <c r="F49" t="str">
+        <v>0404 640 755</v>
+      </c>
+      <c r="G49" t="str">
+        <v>Adelaide</v>
+      </c>
+      <c r="H49" t="str">
+        <v>C</v>
+      </c>
+      <c r="I49" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Victoria Torres</v>
+      </c>
+      <c r="C50">
+        <v>46</v>
+      </c>
+      <c r="D50" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E50" t="str">
+        <v>victoria.torres48@outlook.com</v>
+      </c>
+      <c r="F50" t="str">
+        <v>0411 539 271</v>
+      </c>
+      <c r="G50" t="str">
+        <v>Geelong</v>
+      </c>
+      <c r="H50" t="str">
+        <v>B</v>
+      </c>
+      <c r="I50" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Hazel Mitchell</v>
+      </c>
+      <c r="C51">
+        <v>28</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E51" t="str">
+        <v>hazel.mitchell91@gmail.com</v>
+      </c>
+      <c r="F51" t="str">
+        <v>0400 683 761</v>
+      </c>
+      <c r="G51" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="H51" t="str">
+        <v>A</v>
+      </c>
+      <c r="I51" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Emilia Lopez</v>
+      </c>
+      <c r="C52">
+        <v>50</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E52" t="str">
+        <v>emilia.lopez21@gmail.com</v>
+      </c>
+      <c r="F52" t="str">
+        <v>0403 491 553</v>
+      </c>
+      <c r="G52" t="str">
+        <v>Cairns</v>
+      </c>
+      <c r="H52" t="str">
+        <v>B</v>
+      </c>
+      <c r="I52" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>222469f4-a8d9-4550-b6ee-db9d00e24edd</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Chloe Flores</v>
+      </c>
+      <c r="C53">
+        <v>63</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E53" t="str">
+        <v>chloe.flores93@yahoo.com</v>
+      </c>
+      <c r="F53" t="str">
+        <v>0400 918 463</v>
+      </c>
+      <c r="G53" t="str">
+        <v>Townsville</v>
+      </c>
+      <c r="H53" t="str">
+        <v>C</v>
+      </c>
+      <c r="I53" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>7664257a-dce4-407a-8f24-692043d568be</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Nora Jackson</v>
+      </c>
+      <c r="C54">
+        <v>49</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E54" t="str">
+        <v>nora.jackson83@hotmail.com</v>
+      </c>
+      <c r="F54" t="str">
+        <v>0404 434 899</v>
+      </c>
+      <c r="G54" t="str">
+        <v>Wollongong</v>
+      </c>
+      <c r="H54" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I54" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Genesis Jones</v>
+      </c>
+      <c r="C55">
+        <v>39</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E55" t="str">
+        <v>genesis.jones50@yahoo.com</v>
+      </c>
+      <c r="F55" t="str">
+        <v>0404 967 604</v>
+      </c>
+      <c r="G55" t="str">
+        <v>Sydney</v>
+      </c>
+      <c r="H55" t="str">
+        <v>B</v>
+      </c>
+      <c r="I55" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>3d2128a1-336f-41e1-973b-b5dd54d90b19</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Nova Brown</v>
+      </c>
+      <c r="C56">
+        <v>62</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E56" t="str">
+        <v>nova.brown80@outlook.com</v>
+      </c>
+      <c r="F56" t="str">
+        <v>0411 154 614</v>
+      </c>
+      <c r="G56" t="str">
+        <v>Ballarat</v>
+      </c>
+      <c r="H56" t="str">
+        <v>A</v>
+      </c>
+      <c r="I56" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>0faec83d-7c29-4269-bf33-391ef02d60e4</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Anna White</v>
+      </c>
+      <c r="C57">
+        <v>48</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E57" t="str">
+        <v>anna.white24@yahoo.com</v>
+      </c>
+      <c r="F57" t="str">
+        <v>0400 132 564</v>
+      </c>
+      <c r="G57" t="str">
+        <v>Adelaide</v>
+      </c>
+      <c r="H57" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I57" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Hunter Jackson</v>
+      </c>
+      <c r="C58">
+        <v>64</v>
+      </c>
+      <c r="D58" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E58" t="str">
+        <v>hunter.jackson50@outlook.com</v>
+      </c>
+      <c r="F58" t="str">
+        <v>0404 841 788</v>
+      </c>
+      <c r="G58" t="str">
+        <v>Townsville</v>
+      </c>
+      <c r="H58" t="str">
+        <v>C</v>
+      </c>
+      <c r="I58" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Nathan Allen</v>
+      </c>
+      <c r="C59">
+        <v>60</v>
+      </c>
+      <c r="D59" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E59" t="str">
+        <v>nathan.allen87@outlook.com</v>
+      </c>
+      <c r="F59" t="str">
+        <v>0403 587 263</v>
+      </c>
+      <c r="G59" t="str">
+        <v>Adelaide</v>
+      </c>
+      <c r="H59" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I59" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Noah Hernandez</v>
+      </c>
+      <c r="C60">
+        <v>36</v>
+      </c>
+      <c r="D60" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E60" t="str">
+        <v>noah.hernandez9@hotmail.com</v>
+      </c>
+      <c r="F60" t="str">
+        <v>0404 855 230</v>
+      </c>
+      <c r="G60" t="str">
+        <v>Cairns</v>
+      </c>
+      <c r="H60" t="str">
+        <v>C</v>
+      </c>
+      <c r="I60" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Ryan Williams</v>
+      </c>
+      <c r="C61">
+        <v>24</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E61" t="str">
+        <v>ryan.williams82@hotmail.com</v>
+      </c>
+      <c r="F61" t="str">
+        <v>0401 450 673</v>
+      </c>
+      <c r="G61" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="H61" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I61" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Oliver Rivera</v>
+      </c>
+      <c r="C62">
+        <v>33</v>
+      </c>
+      <c r="D62" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E62" t="str">
+        <v>oliver.rivera58@outlook.com</v>
+      </c>
+      <c r="F62" t="str">
+        <v>0412 991 121</v>
+      </c>
+      <c r="G62" t="str">
+        <v>Canberra</v>
+      </c>
+      <c r="H62" t="str">
+        <v>C</v>
+      </c>
+      <c r="I62" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Joshua Walker</v>
+      </c>
+      <c r="C63">
+        <v>55</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E63" t="str">
+        <v>joshua.walker97@gmail.com</v>
+      </c>
+      <c r="F63" t="str">
+        <v>0402 640 379</v>
+      </c>
+      <c r="G63" t="str">
+        <v>Darwin</v>
+      </c>
+      <c r="H63" t="str">
+        <v>B</v>
+      </c>
+      <c r="I63" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Carter Harris</v>
+      </c>
+      <c r="C64">
+        <v>59</v>
+      </c>
+      <c r="D64" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E64" t="str">
+        <v>carter.harris82@yahoo.com</v>
+      </c>
+      <c r="F64" t="str">
+        <v>0412 175 744</v>
+      </c>
+      <c r="G64" t="str">
+        <v>Geelong</v>
+      </c>
+      <c r="H64" t="str">
+        <v>C</v>
+      </c>
+      <c r="I64" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
+      </c>
+      <c r="B65" t="str">
+        <v>Andrew Garcia</v>
+      </c>
+      <c r="C65">
+        <v>41</v>
+      </c>
+      <c r="D65" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E65" t="str">
+        <v>andrew.garcia26@hotmail.com</v>
+      </c>
+      <c r="F65" t="str">
+        <v>0400 450 222</v>
+      </c>
+      <c r="G65" t="str">
+        <v>Darwin</v>
+      </c>
+      <c r="H65" t="str">
+        <v>B</v>
+      </c>
+      <c r="I65" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>f1466859-7323-4893-a189-a0ce994068ba</v>
+      </c>
+      <c r="B66" t="str">
+        <v>Anthony Thompson</v>
+      </c>
+      <c r="C66">
+        <v>56</v>
+      </c>
+      <c r="D66" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E66" t="str">
+        <v>anthony.thompson29@yahoo.com</v>
+      </c>
+      <c r="F66" t="str">
+        <v>0412 442 587</v>
+      </c>
+      <c r="G66" t="str">
+        <v>Townsville</v>
+      </c>
+      <c r="H66" t="str">
+        <v>A</v>
+      </c>
+      <c r="I66" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+      </c>
+      <c r="B67" t="str">
+        <v>Samuel King</v>
+      </c>
+      <c r="C67">
+        <v>54</v>
+      </c>
+      <c r="D67" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E67" t="str">
+        <v>samuel.king24@yahoo.com</v>
+      </c>
+      <c r="F67" t="str">
+        <v>0400 774 736</v>
+      </c>
+      <c r="G67" t="str">
+        <v>Newcastle</v>
+      </c>
+      <c r="H67" t="str">
+        <v>B</v>
+      </c>
+      <c r="I67" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Mason Hill</v>
+      </c>
+      <c r="C68">
+        <v>40</v>
+      </c>
+      <c r="D68" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E68" t="str">
+        <v>mason.hill27@outlook.com</v>
+      </c>
+      <c r="F68" t="str">
+        <v>0410 682 884</v>
+      </c>
+      <c r="G68" t="str">
+        <v>Canberra</v>
+      </c>
+      <c r="H68" t="str">
+        <v>A</v>
+      </c>
+      <c r="I68" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
+      </c>
+      <c r="B69" t="str">
+        <v>Jackson Young</v>
+      </c>
+      <c r="C69">
+        <v>50</v>
+      </c>
+      <c r="D69" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E69" t="str">
+        <v>jackson.young79@yahoo.com</v>
+      </c>
+      <c r="F69" t="str">
+        <v>0412 940 993</v>
+      </c>
+      <c r="G69" t="str">
+        <v>Ballarat</v>
+      </c>
+      <c r="H69" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I69" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>182bd5d2-7f68-4c83-b156-e80856f3b6b7</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Mason Nelson</v>
+      </c>
+      <c r="C70">
+        <v>59</v>
+      </c>
+      <c r="D70" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E70" t="str">
+        <v>mason.nelson14@hotmail.com</v>
+      </c>
+      <c r="F70" t="str">
+        <v>0403 485 650</v>
+      </c>
+      <c r="G70" t="str">
+        <v>Canberra</v>
+      </c>
+      <c r="H70" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I70" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Cameron Lee</v>
+      </c>
+      <c r="C71">
+        <v>44</v>
+      </c>
+      <c r="D71" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E71" t="str">
+        <v>cameron.lee78@yahoo.com</v>
+      </c>
+      <c r="F71" t="str">
+        <v>0404 821 708</v>
+      </c>
+      <c r="G71" t="str">
+        <v>Cairns</v>
+      </c>
+      <c r="H71" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I71" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Emily Johnson</v>
+      </c>
+      <c r="C72">
+        <v>37</v>
+      </c>
+      <c r="D72" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E72" t="str">
+        <v>emily.johnson58@hotmail.com</v>
+      </c>
+      <c r="F72" t="str">
+        <v>0412 663 939</v>
+      </c>
+      <c r="G72" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="H72" t="str">
+        <v>B</v>
+      </c>
+      <c r="I72" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>3db7cdb3-9a92-467c-b554-d23b524f42f5</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Claire Campbell</v>
+      </c>
+      <c r="C73">
+        <v>23</v>
+      </c>
+      <c r="D73" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E73" t="str">
+        <v>claire.campbell9@outlook.com</v>
+      </c>
+      <c r="F73" t="str">
+        <v>0401 164 490</v>
+      </c>
+      <c r="G73" t="str">
+        <v>Darwin</v>
+      </c>
+      <c r="H73" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I73" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Aurora Williams</v>
+      </c>
+      <c r="C74">
+        <v>27</v>
+      </c>
+      <c r="D74" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E74" t="str">
+        <v>aurora.williams76@outlook.com</v>
+      </c>
+      <c r="F74" t="str">
+        <v>0401 416 170</v>
+      </c>
+      <c r="G74" t="str">
+        <v>Darwin</v>
+      </c>
+      <c r="H74" t="str">
+        <v>C</v>
+      </c>
+      <c r="I74" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Aria Nguyen</v>
+      </c>
+      <c r="C75">
+        <v>32</v>
+      </c>
+      <c r="D75" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E75" t="str">
+        <v>aria.nguyen36@gmail.com</v>
+      </c>
+      <c r="F75" t="str">
+        <v>0401 618 716</v>
+      </c>
+      <c r="G75" t="str">
+        <v>Sydney</v>
+      </c>
+      <c r="H75" t="str">
+        <v>C</v>
+      </c>
+      <c r="I75" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Nora Mitchell</v>
+      </c>
+      <c r="C76">
+        <v>29</v>
+      </c>
+      <c r="D76" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E76" t="str">
+        <v>nora.mitchell66@outlook.com</v>
+      </c>
+      <c r="F76" t="str">
+        <v>0412 196 419</v>
+      </c>
+      <c r="G76" t="str">
+        <v>Adelaide</v>
+      </c>
+      <c r="H76" t="str">
+        <v>C</v>
+      </c>
+      <c r="I76" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Scarlett Wright</v>
+      </c>
+      <c r="C77">
+        <v>34</v>
+      </c>
+      <c r="D77" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E77" t="str">
+        <v>scarlett.wright68@outlook.com</v>
+      </c>
+      <c r="F77" t="str">
+        <v>0412 487 763</v>
+      </c>
+      <c r="G77" t="str">
+        <v>Newcastle</v>
+      </c>
+      <c r="H77" t="str">
+        <v>B</v>
+      </c>
+      <c r="I77" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Abigail Williams</v>
+      </c>
+      <c r="C78">
+        <v>64</v>
+      </c>
+      <c r="D78" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E78" t="str">
+        <v>abigail.williams45@yahoo.com</v>
+      </c>
+      <c r="F78" t="str">
+        <v>0403 497 445</v>
+      </c>
+      <c r="G78" t="str">
+        <v>Toowoomba</v>
+      </c>
+      <c r="H78" t="str">
+        <v>C</v>
+      </c>
+      <c r="I78" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>6591420b-4762-4d90-b738-8a5b70458c40</v>
+      </c>
+      <c r="B79" t="str">
+        <v>Aurora Hill</v>
+      </c>
+      <c r="C79">
+        <v>34</v>
+      </c>
+      <c r="D79" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E79" t="str">
+        <v>aurora.hill33@hotmail.com</v>
+      </c>
+      <c r="F79" t="str">
+        <v>0410 373 844</v>
+      </c>
+      <c r="G79" t="str">
+        <v>Gold Coast</v>
+      </c>
+      <c r="H79" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I79" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Lily Walker</v>
+      </c>
+      <c r="C80">
+        <v>62</v>
+      </c>
+      <c r="D80" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E80" t="str">
+        <v>lily.walker96@outlook.com</v>
+      </c>
+      <c r="F80" t="str">
+        <v>0410 155 426</v>
+      </c>
+      <c r="G80" t="str">
+        <v>Hobart</v>
+      </c>
+      <c r="H80" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I80" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Scarlett Lopez</v>
+      </c>
+      <c r="C81">
+        <v>64</v>
+      </c>
+      <c r="D81" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E81" t="str">
+        <v>scarlett.lopez53@yahoo.com</v>
+      </c>
+      <c r="F81" t="str">
+        <v>0400 509 641</v>
+      </c>
+      <c r="G81" t="str">
+        <v>Sydney</v>
+      </c>
+      <c r="H81" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I81" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>34685ff7-6e85-4bbd-b546-77cfe11d7f7d</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Grace Walker</v>
+      </c>
+      <c r="C82">
+        <v>56</v>
+      </c>
+      <c r="D82" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E82" t="str">
+        <v>grace.walker52@hotmail.com</v>
+      </c>
+      <c r="F82" t="str">
+        <v>0412 754 780</v>
+      </c>
+      <c r="G82" t="str">
+        <v>Canberra</v>
+      </c>
+      <c r="H82" t="str">
+        <v>A+</v>
+      </c>
+      <c r="I82" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>da40ad70-95be-413c-b0f1-d089ef285cc8</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Emily Smith</v>
+      </c>
+      <c r="C83">
+        <v>24</v>
+      </c>
+      <c r="D83" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E83" t="str">
+        <v>emily.smith56@hotmail.com</v>
+      </c>
+      <c r="F83" t="str">
+        <v>0410 101 780</v>
+      </c>
+      <c r="G83" t="str">
+        <v>Toowoomba</v>
+      </c>
+      <c r="H83" t="str">
+        <v>A+</v>
+      </c>
+      <c r="I83" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>ee7f9d33-09d6-417b-a45f-3e6554489f5b</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Dylan Miller</v>
+      </c>
+      <c r="C84">
+        <v>35</v>
+      </c>
+      <c r="D84" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E84" t="str">
+        <v>dylan.miller23@hotmail.com</v>
+      </c>
+      <c r="F84" t="str">
+        <v>0402 417 876</v>
+      </c>
+      <c r="G84" t="str">
+        <v>Melbourne</v>
+      </c>
+      <c r="H84" t="str">
+        <v>A</v>
+      </c>
+      <c r="I84" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Christian Rivera</v>
+      </c>
+      <c r="C85">
+        <v>65</v>
+      </c>
+      <c r="D85" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E85" t="str">
+        <v>christian.rivera86@hotmail.com</v>
+      </c>
+      <c r="F85" t="str">
+        <v>0400 135 743</v>
+      </c>
+      <c r="G85" t="str">
+        <v>Adelaide</v>
+      </c>
+      <c r="H85" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I85" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>5a6b21ec-9fac-4adc-b5ab-bcad20d0eca4</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Hunter Harris</v>
+      </c>
+      <c r="C86">
+        <v>37</v>
+      </c>
+      <c r="D86" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E86" t="str">
+        <v>hunter.harris1@gmail.com</v>
+      </c>
+      <c r="F86" t="str">
+        <v>0404 782 485</v>
+      </c>
+      <c r="G86" t="str">
+        <v>Gold Coast</v>
+      </c>
+      <c r="H86" t="str">
+        <v>A</v>
+      </c>
+      <c r="I86" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Ethan Taylor</v>
+      </c>
+      <c r="C87">
+        <v>30</v>
+      </c>
+      <c r="D87" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E87" t="str">
+        <v>ethan.taylor22@yahoo.com</v>
+      </c>
+      <c r="F87" t="str">
+        <v>0410 363 173</v>
+      </c>
+      <c r="G87" t="str">
+        <v>Adelaide</v>
+      </c>
+      <c r="H87" t="str">
+        <v>B</v>
+      </c>
+      <c r="I87" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Charles Torres</v>
+      </c>
+      <c r="C88">
+        <v>46</v>
+      </c>
+      <c r="D88" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E88" t="str">
+        <v>charles.torres98@outlook.com</v>
+      </c>
+      <c r="F88" t="str">
+        <v>0401 744 176</v>
+      </c>
+      <c r="G88" t="str">
+        <v>Wollongong</v>
+      </c>
+      <c r="H88" t="str">
+        <v>B</v>
+      </c>
+      <c r="I88" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Julian Rivera</v>
+      </c>
+      <c r="C89">
+        <v>53</v>
+      </c>
+      <c r="D89" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E89" t="str">
+        <v>julian.rivera31@outlook.com</v>
+      </c>
+      <c r="F89" t="str">
+        <v>0401 414 502</v>
+      </c>
+      <c r="G89" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="H89" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I89" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Joshua Carter</v>
+      </c>
+      <c r="C90">
+        <v>62</v>
+      </c>
+      <c r="D90" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E90" t="str">
+        <v>joshua.carter41@hotmail.com</v>
+      </c>
+      <c r="F90" t="str">
+        <v>0404 538 442</v>
+      </c>
+      <c r="G90" t="str">
+        <v>Wollongong</v>
+      </c>
+      <c r="H90" t="str">
+        <v>B</v>
+      </c>
+      <c r="I90" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
+      </c>
+      <c r="B91" t="str">
+        <v>Ryan Lewis</v>
+      </c>
+      <c r="C91">
+        <v>31</v>
+      </c>
+      <c r="D91" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E91" t="str">
+        <v>ryan.lewis85@yahoo.com</v>
+      </c>
+      <c r="F91" t="str">
+        <v>0400 187 811</v>
+      </c>
+      <c r="G91" t="str">
+        <v>Canberra</v>
+      </c>
+      <c r="H91" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I91" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Lucas Thomas</v>
+      </c>
+      <c r="C92">
+        <v>33</v>
+      </c>
+      <c r="D92" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E92" t="str">
+        <v>lucas.thomas30@yahoo.com</v>
+      </c>
+      <c r="F92" t="str">
+        <v>0412 527 117</v>
+      </c>
+      <c r="G92" t="str">
+        <v>Brisbane</v>
+      </c>
+      <c r="H92" t="str">
+        <v>B</v>
+      </c>
+      <c r="I92" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
+      </c>
+      <c r="B93" t="str">
+        <v>Joshua Jones</v>
+      </c>
+      <c r="C93">
+        <v>32</v>
+      </c>
+      <c r="D93" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E93" t="str">
+        <v>joshua.jones82@yahoo.com</v>
+      </c>
+      <c r="F93" t="str">
+        <v>0400 652 840</v>
+      </c>
+      <c r="G93" t="str">
+        <v>Toowoomba</v>
+      </c>
+      <c r="H93" t="str">
+        <v>B</v>
+      </c>
+      <c r="I93" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
+      </c>
+      <c r="B94" t="str">
+        <v>Carter Hill</v>
+      </c>
+      <c r="C94">
+        <v>25</v>
+      </c>
+      <c r="D94" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E94" t="str">
+        <v>carter.hill93@gmail.com</v>
+      </c>
+      <c r="F94" t="str">
+        <v>0404 349 309</v>
+      </c>
+      <c r="G94" t="str">
+        <v>Newcastle</v>
+      </c>
+      <c r="H94" t="str">
+        <v>B</v>
+      </c>
+      <c r="I94" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
+      </c>
+      <c r="B95" t="str">
+        <v>Jayden Nguyen</v>
+      </c>
+      <c r="C95">
+        <v>53</v>
+      </c>
+      <c r="D95" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E95" t="str">
+        <v>jayden.nguyen88@hotmail.com</v>
+      </c>
+      <c r="F95" t="str">
+        <v>0401 108 628</v>
+      </c>
+      <c r="G95" t="str">
+        <v>Hobart</v>
+      </c>
+      <c r="H95" t="str">
+        <v>B</v>
+      </c>
+      <c r="I95" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>8956e289-91e9-4c15-bf2b-a13dee2fa476</v>
+      </c>
+      <c r="B96" t="str">
+        <v>Landon Wright</v>
+      </c>
+      <c r="C96">
+        <v>41</v>
+      </c>
+      <c r="D96" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E96" t="str">
+        <v>landon.wright36@outlook.com</v>
+      </c>
+      <c r="F96" t="str">
+        <v>0402 415 597</v>
+      </c>
+      <c r="G96" t="str">
+        <v>Cairns</v>
+      </c>
+      <c r="H96" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I96" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
+      </c>
+      <c r="B97" t="str">
+        <v>Luke Flores</v>
+      </c>
+      <c r="C97">
+        <v>65</v>
+      </c>
+      <c r="D97" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E97" t="str">
+        <v>luke.flores39@hotmail.com</v>
+      </c>
+      <c r="F97" t="str">
+        <v>0403 225 544</v>
+      </c>
+      <c r="G97" t="str">
+        <v>Melbourne</v>
+      </c>
+      <c r="H97" t="str">
+        <v>B</v>
+      </c>
+      <c r="I97" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
+      </c>
+      <c r="B98" t="str">
+        <v>Theodore Nelson</v>
+      </c>
+      <c r="C98">
+        <v>41</v>
+      </c>
+      <c r="D98" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E98" t="str">
+        <v>theodore.nelson79@gmail.com</v>
+      </c>
+      <c r="F98" t="str">
+        <v>0403 813 793</v>
+      </c>
+      <c r="G98" t="str">
+        <v>Canberra</v>
+      </c>
+      <c r="H98" t="str">
+        <v>B</v>
+      </c>
+      <c r="I98" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
+      </c>
+      <c r="B99" t="str">
+        <v>Ethan Rodriguez</v>
+      </c>
+      <c r="C99">
+        <v>57</v>
+      </c>
+      <c r="D99" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E99" t="str">
+        <v>ethan.rodriguez60@hotmail.com</v>
+      </c>
+      <c r="F99" t="str">
+        <v>0411 690 563</v>
+      </c>
+      <c r="G99" t="str">
+        <v>Townsville</v>
+      </c>
+      <c r="H99" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I99" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>ecc70875-f282-4849-9e60-071edc278977</v>
+      </c>
+      <c r="B100" t="str">
+        <v>Noah White</v>
+      </c>
+      <c r="C100">
+        <v>22</v>
+      </c>
+      <c r="D100" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E100" t="str">
+        <v>noah.white20@gmail.com</v>
+      </c>
+      <c r="F100" t="str">
+        <v>0410 565 594</v>
+      </c>
+      <c r="G100" t="str">
+        <v>Adelaide</v>
+      </c>
+      <c r="H100" t="str">
+        <v>A</v>
+      </c>
+      <c r="I100" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
+      </c>
+      <c r="B101" t="str">
+        <v>Theodore Allen</v>
+      </c>
+      <c r="C101">
+        <v>49</v>
+      </c>
+      <c r="D101" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E101" t="str">
+        <v>theodore.allen25@outlook.com</v>
+      </c>
+      <c r="F101" t="str">
+        <v>0400 438 819</v>
+      </c>
+      <c r="G101" t="str">
+        <v>Newcastle</v>
+      </c>
+      <c r="H101" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I101" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
+      </c>
+      <c r="B102" t="str">
+        <v>Joshua Clark</v>
+      </c>
+      <c r="C102">
+        <v>25</v>
+      </c>
+      <c r="D102" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E102" t="str">
+        <v>joshua.clark16@outlook.com</v>
+      </c>
+      <c r="F102" t="str">
+        <v>0403 901 485</v>
+      </c>
+      <c r="G102" t="str">
+        <v>Sydney</v>
+      </c>
+      <c r="H102" t="str">
+        <v>B</v>
+      </c>
+      <c r="I102" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
+      </c>
+      <c r="B103" t="str">
+        <v>Joshua Scott</v>
+      </c>
+      <c r="C103">
+        <v>56</v>
+      </c>
+      <c r="D103" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E103" t="str">
+        <v>joshua.scott95@outlook.com</v>
+      </c>
+      <c r="F103" t="str">
+        <v>0410 137 561</v>
+      </c>
+      <c r="G103" t="str">
+        <v>Canberra</v>
+      </c>
+      <c r="H103" t="str">
+        <v>B</v>
+      </c>
+      <c r="I103" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
+      </c>
+      <c r="B104" t="str">
+        <v>Liam Lewis</v>
+      </c>
+      <c r="C104">
+        <v>23</v>
+      </c>
+      <c r="D104" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E104" t="str">
+        <v>liam.lewis79@yahoo.com</v>
+      </c>
+      <c r="F104" t="str">
+        <v>0404 203 198</v>
+      </c>
+      <c r="G104" t="str">
+        <v>Hobart</v>
+      </c>
+      <c r="H104" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I104" t="str">
+        <v>available</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M104"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Block</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Seat</v>
-      </c>
-      <c r="F1" t="str">
-        <v>BookingEmailSent</v>
-      </c>
-      <c r="G1" t="str">
-        <v>ConfirmedRSVP</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>20946cbf-8f88-4629-a6d2-d8510554cb9a</v>
-      </c>
-      <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="str">
-        <v>B2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>f8463207-3f82-429c-bf09-986ae9a6cc97</v>
-      </c>
-      <c r="B3" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C3" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="str">
-        <v>B3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>c1d29895-e1ab-4926-8d3b-29a9df7058de</v>
-      </c>
-      <c r="B4" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C4" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="str">
-        <v>B4</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -999,7 +3807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Correctly account for existing contestants when assigning seats automatically
Fixes an issue where auto-assign capacity calculation did not account for already seated contestants by pre-loading existing assignments before running the placement algorithm in `server/routes.ts`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 906a8178-c420-48a3-9c3d-828b1b7869c1
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/G1e7c0s
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,8 +5,9 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Groups" sheetId="3" r:id="rId3"/>
-    <sheet name="Block Types" sheetId="4" r:id="rId4"/>
+    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -717,25 +718,25 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B2" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D2" t="str">
         <v>Not Specified</v>
       </c>
       <c r="E2" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F2" t="str">
         <v>498086080</v>
       </c>
       <c r="G2" t="str">
-        <v>Footscray</v>
+        <v>Melbourne</v>
       </c>
       <c r="H2" t="str">
         <v/>
@@ -744,7 +745,7 @@
         <v>available</v>
       </c>
       <c r="J2" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
       </c>
       <c r="K2" t="str">
         <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
@@ -758,66 +759,60 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="B3" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Caroline Taylor</v>
       </c>
       <c r="C3">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D3" t="str">
-        <v>Not Specified</v>
+        <v>Female</v>
       </c>
       <c r="E3" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>caroline.taylor54@outlook.com</v>
       </c>
       <c r="F3" t="str">
-        <v>498086080</v>
+        <v>0402 864 601</v>
       </c>
       <c r="G3" t="str">
-        <v>Melbourne</v>
+        <v>Darwin</v>
       </c>
       <c r="H3" t="str">
-        <v/>
+        <v>B+</v>
       </c>
       <c r="I3" t="str">
         <v>available</v>
       </c>
       <c r="J3" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
-      </c>
-      <c r="K3" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L3" t="str">
-        <v>N</v>
+        <v>Hazel Mitchell</v>
       </c>
       <c r="M3" t="str">
-        <v>N/A</v>
+        <v>Arthritis - prefers aisle seating for easy exit</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>8e115c7e-8033-4466-bcb9-07ea089eb4be</v>
+        <v>0dd7de5c-0409-45e3-84a5-5f2ffbd591d8</v>
       </c>
       <c r="B4" t="str">
-        <v>Chloe Taylor</v>
+        <v>Harper Sanchez</v>
       </c>
       <c r="C4">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="D4" t="str">
         <v>Female</v>
       </c>
       <c r="E4" t="str">
-        <v>chloe.taylor7@gmail.com</v>
+        <v>harper.sanchez76@gmail.com</v>
       </c>
       <c r="F4" t="str">
-        <v>0412 903 254</v>
+        <v>0411 422 972</v>
       </c>
       <c r="G4" t="str">
-        <v>Townsville</v>
+        <v>Geelong</v>
       </c>
       <c r="H4" t="str">
         <v>C</v>
@@ -825,156 +820,156 @@
       <c r="I4" t="str">
         <v>available</v>
       </c>
+      <c r="J4" t="str">
+        <v>Leah Scott</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
+        <v>8e115c7e-8033-4466-bcb9-07ea089eb4be</v>
       </c>
       <c r="B5" t="str">
-        <v>Audrey Ramirez</v>
+        <v>Chloe Taylor</v>
       </c>
       <c r="C5">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D5" t="str">
         <v>Female</v>
       </c>
       <c r="E5" t="str">
-        <v>audrey.ramirez12@gmail.com</v>
+        <v>chloe.taylor7@gmail.com</v>
       </c>
       <c r="F5" t="str">
-        <v>0411 212 619</v>
+        <v>0412 903 254</v>
       </c>
       <c r="G5" t="str">
-        <v>Brisbane</v>
+        <v>Townsville</v>
       </c>
       <c r="H5" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I5" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
+        <v>992418b2-3029-4752-9552-0aa886433657</v>
       </c>
       <c r="B6" t="str">
-        <v>Maya Moore</v>
+        <v>Zoe Brown</v>
       </c>
       <c r="C6">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D6" t="str">
         <v>Female</v>
       </c>
       <c r="E6" t="str">
-        <v>maya.moore54@outlook.com</v>
+        <v>zoe.brown45@outlook.com</v>
       </c>
       <c r="F6" t="str">
-        <v>0400 718 585</v>
+        <v>0401 578 107</v>
       </c>
       <c r="G6" t="str">
-        <v>Toowoomba</v>
+        <v>Sydney</v>
       </c>
       <c r="H6" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I6" t="str">
         <v>available</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Chloe Jones</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="B7" t="str">
-        <v>Peter Adamidis</v>
+        <v>Paisley Lee</v>
       </c>
       <c r="C7">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="D7" t="str">
-        <v>Not Specified</v>
+        <v>Female</v>
       </c>
       <c r="E7" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>paisley.lee78@hotmail.com</v>
       </c>
       <c r="F7" t="str">
-        <v>498086080</v>
+        <v>0400 179 607</v>
       </c>
       <c r="G7" t="str">
-        <v/>
+        <v>Ballarat</v>
       </c>
       <c r="H7" t="str">
-        <v/>
+        <v>B</v>
       </c>
       <c r="I7" t="str">
         <v>available</v>
       </c>
       <c r="J7" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
-      </c>
-      <c r="K7" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L7" t="str">
-        <v>Y</v>
-      </c>
-      <c r="M7" t="str">
-        <v>Broken Leg</v>
+        <v>Aria Lopez</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>b9e02c2d-410d-4307-811c-7e52cf93b14b</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="B8" t="str">
-        <v>Emily Moore</v>
+        <v>Ella Anderson</v>
       </c>
       <c r="C8">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D8" t="str">
         <v>Female</v>
       </c>
       <c r="E8" t="str">
-        <v>emily.moore11@hotmail.com</v>
+        <v>ella.anderson1@yahoo.com</v>
       </c>
       <c r="F8" t="str">
-        <v>0410 362 279</v>
+        <v>0412 908 910</v>
       </c>
       <c r="G8" t="str">
-        <v>Perth</v>
+        <v>Geelong</v>
       </c>
       <c r="H8" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I8" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Isabella Brown</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>210066e7-58e9-4ebb-a504-dfbf383961b5</v>
       </c>
       <c r="B9" t="str">
-        <v>Caroline Taylor</v>
+        <v>Grace Scott</v>
       </c>
       <c r="C9">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D9" t="str">
         <v>Female</v>
       </c>
       <c r="E9" t="str">
-        <v>caroline.taylor54@outlook.com</v>
+        <v>grace.scott94@hotmail.com</v>
       </c>
       <c r="F9" t="str">
-        <v>0402 864 601</v>
+        <v>0410 377 869</v>
       </c>
       <c r="G9" t="str">
-        <v>Darwin</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H9" t="str">
         <v>B+</v>
@@ -982,31 +977,34 @@
       <c r="I9" t="str">
         <v>available</v>
       </c>
+      <c r="J9" t="str">
+        <v>Audrey Smith</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
+        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
       </c>
       <c r="B10" t="str">
-        <v>Stella Martinez</v>
+        <v>Abigail Jackson</v>
       </c>
       <c r="C10">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D10" t="str">
         <v>Female</v>
       </c>
       <c r="E10" t="str">
-        <v>stella.martinez75@gmail.com</v>
+        <v>abigail.jackson65@outlook.com</v>
       </c>
       <c r="F10" t="str">
-        <v>0404 227 272</v>
+        <v>0411 824 257</v>
       </c>
       <c r="G10" t="str">
-        <v>Ballarat</v>
+        <v>Newcastle</v>
       </c>
       <c r="H10" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I10" t="str">
         <v>available</v>
@@ -1014,89 +1012,98 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
       </c>
       <c r="B11" t="str">
-        <v>Ella Anderson</v>
+        <v>Aria Scott</v>
       </c>
       <c r="C11">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D11" t="str">
         <v>Female</v>
       </c>
       <c r="E11" t="str">
-        <v>ella.anderson1@yahoo.com</v>
+        <v>aria.scott42@outlook.com</v>
       </c>
       <c r="F11" t="str">
-        <v>0412 908 910</v>
+        <v>0401 330 548</v>
       </c>
       <c r="G11" t="str">
-        <v>Geelong</v>
+        <v>Hobart</v>
       </c>
       <c r="H11" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I11" t="str">
         <v>available</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Maya Hernandez</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
       </c>
       <c r="B12" t="str">
-        <v>Abigail Jackson</v>
+        <v>Audrey Thomas</v>
       </c>
       <c r="C12">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D12" t="str">
         <v>Female</v>
       </c>
       <c r="E12" t="str">
-        <v>abigail.jackson65@outlook.com</v>
+        <v>audrey.thomas38@gmail.com</v>
       </c>
       <c r="F12" t="str">
-        <v>0411 824 257</v>
+        <v>0400 437 270</v>
       </c>
       <c r="G12" t="str">
-        <v>Newcastle</v>
+        <v>Perth</v>
       </c>
       <c r="H12" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I12" t="str">
         <v>available</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Hannah Torres</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
+        <v>2c188398-79a8-4bf6-b740-1ad9d535662e</v>
       </c>
       <c r="B13" t="str">
-        <v>Evelyn Sanchez</v>
+        <v>Everly Torres</v>
       </c>
       <c r="C13">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D13" t="str">
         <v>Female</v>
       </c>
       <c r="E13" t="str">
-        <v>evelyn.sanchez9@gmail.com</v>
+        <v>everly.torres12@gmail.com</v>
       </c>
       <c r="F13" t="str">
-        <v>0404 119 469</v>
+        <v>0412 804 179</v>
       </c>
       <c r="G13" t="str">
-        <v>Gold Coast</v>
+        <v>Sydney</v>
       </c>
       <c r="H13" t="str">
-        <v>B</v>
+        <v>A+</v>
       </c>
       <c r="I13" t="str">
         <v>available</v>
+      </c>
+      <c r="J13" t="str">
+        <v>Stella Green</v>
       </c>
     </row>
     <row r="14">
@@ -1127,28 +1134,31 @@
       <c r="I14" t="str">
         <v>available</v>
       </c>
+      <c r="J14" t="str">
+        <v>Audrey Thomas</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
+        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
       </c>
       <c r="B15" t="str">
-        <v>Audrey Smith</v>
+        <v>Evelyn Sanchez</v>
       </c>
       <c r="C15">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D15" t="str">
         <v>Female</v>
       </c>
       <c r="E15" t="str">
-        <v>audrey.smith66@gmail.com</v>
+        <v>evelyn.sanchez9@gmail.com</v>
       </c>
       <c r="F15" t="str">
-        <v>0410 904 568</v>
+        <v>0404 119 469</v>
       </c>
       <c r="G15" t="str">
-        <v>Ballarat</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H15" t="str">
         <v>B</v>
@@ -1156,234 +1166,258 @@
       <c r="I15" t="str">
         <v>available</v>
       </c>
+      <c r="J15" t="str">
+        <v>Chloe Flores</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>97646711-3e33-4ee9-8d83-bd6e0363ece0</v>
+        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
       </c>
       <c r="B16" t="str">
-        <v>Audrey Martin</v>
+        <v>Stella Martinez</v>
       </c>
       <c r="C16">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D16" t="str">
         <v>Female</v>
       </c>
       <c r="E16" t="str">
-        <v>audrey.martin33@yahoo.com</v>
+        <v>stella.martinez75@gmail.com</v>
       </c>
       <c r="F16" t="str">
-        <v>0403 767 239</v>
+        <v>0404 227 272</v>
       </c>
       <c r="G16" t="str">
-        <v>Adelaide</v>
+        <v>Ballarat</v>
       </c>
       <c r="H16" t="str">
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="I16" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>d37f9e40-d1a2-4238-9089-80517a709859</v>
+        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
       </c>
       <c r="B17" t="str">
-        <v>Mia Roberts</v>
+        <v>Harper Lewis</v>
       </c>
       <c r="C17">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D17" t="str">
         <v>Female</v>
       </c>
       <c r="E17" t="str">
-        <v>mia.roberts81@hotmail.com</v>
+        <v>harper.lewis57@hotmail.com</v>
       </c>
       <c r="F17" t="str">
-        <v>0412 368 553</v>
+        <v>0411 652 121</v>
       </c>
       <c r="G17" t="str">
-        <v>Toowoomba</v>
+        <v>Geelong</v>
       </c>
       <c r="H17" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I17" t="str">
         <v>available</v>
+      </c>
+      <c r="J17" t="str">
+        <v>Audrey Ramirez</v>
+      </c>
+      <c r="M17" t="str">
+        <v>Back issues - needs lumbar support chair</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
+        <v>b9e02c2d-410d-4307-811c-7e52cf93b14b</v>
       </c>
       <c r="B18" t="str">
-        <v>Chloe Jones</v>
+        <v>Emily Moore</v>
       </c>
       <c r="C18">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D18" t="str">
         <v>Female</v>
       </c>
       <c r="E18" t="str">
-        <v>chloe.jones20@outlook.com</v>
+        <v>emily.moore11@hotmail.com</v>
       </c>
       <c r="F18" t="str">
-        <v>0411 294 635</v>
+        <v>0410 362 279</v>
       </c>
       <c r="G18" t="str">
-        <v>Toowoomba</v>
+        <v>Perth</v>
       </c>
       <c r="H18" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I18" t="str">
         <v>available</v>
+      </c>
+      <c r="J18" t="str">
+        <v>Grace Scott</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>eff76f3c-c868-4954-99ea-92a4ae6c8067</v>
+        <v>d37f9e40-d1a2-4238-9089-80517a709859</v>
       </c>
       <c r="B19" t="str">
-        <v>Abigail Lee</v>
+        <v>Mia Roberts</v>
       </c>
       <c r="C19">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D19" t="str">
         <v>Female</v>
       </c>
       <c r="E19" t="str">
-        <v>abigail.lee94@hotmail.com</v>
+        <v>mia.roberts81@hotmail.com</v>
       </c>
       <c r="F19" t="str">
-        <v>0402 888 384</v>
+        <v>0412 368 553</v>
       </c>
       <c r="G19" t="str">
-        <v>Wollongong</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H19" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I19" t="str">
         <v>available</v>
+      </c>
+      <c r="J19" t="str">
+        <v>Paisley Scott</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
+        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
       </c>
       <c r="B20" t="str">
-        <v>Grace Scott</v>
+        <v>Chloe Jones</v>
       </c>
       <c r="C20">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D20" t="str">
         <v>Female</v>
       </c>
       <c r="E20" t="str">
-        <v>grace.scott40@outlook.com</v>
+        <v>chloe.jones20@outlook.com</v>
       </c>
       <c r="F20" t="str">
-        <v>0401 870 853</v>
+        <v>0411 294 635</v>
       </c>
       <c r="G20" t="str">
-        <v>Ballarat</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H20" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I20" t="str">
         <v>available</v>
+      </c>
+      <c r="J20" t="str">
+        <v>Zoe Brown</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
+        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
       </c>
       <c r="B21" t="str">
-        <v>Aurora Rodriguez</v>
+        <v>Emilia Miller</v>
       </c>
       <c r="C21">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D21" t="str">
         <v>Female</v>
       </c>
       <c r="E21" t="str">
-        <v>aurora.rodriguez20@yahoo.com</v>
+        <v>emilia.miller56@outlook.com</v>
       </c>
       <c r="F21" t="str">
-        <v>0404 720 692</v>
+        <v>0403 506 698</v>
       </c>
       <c r="G21" t="str">
-        <v>Hobart</v>
+        <v>Melbourne</v>
       </c>
       <c r="H21" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I21" t="str">
         <v>available</v>
+      </c>
+      <c r="J21" t="str">
+        <v>Victoria Carter</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>992418b2-3029-4752-9552-0aa886433657</v>
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
       </c>
       <c r="B22" t="str">
-        <v>Zoe Brown</v>
+        <v>Emilia Thompson</v>
       </c>
       <c r="C22">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D22" t="str">
         <v>Female</v>
       </c>
       <c r="E22" t="str">
-        <v>zoe.brown45@outlook.com</v>
+        <v>emilia.thompson0@gmail.com</v>
       </c>
       <c r="F22" t="str">
-        <v>0401 578 107</v>
+        <v>0404 992 451</v>
       </c>
       <c r="G22" t="str">
-        <v>Sydney</v>
+        <v>Perth</v>
       </c>
       <c r="H22" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I22" t="str">
         <v>available</v>
+      </c>
+      <c r="J22" t="str">
+        <v>Violet Hall</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>210066e7-58e9-4ebb-a504-dfbf383961b5</v>
+        <v>0a153155-dcf5-4d56-9ed1-8960501157f8</v>
       </c>
       <c r="B23" t="str">
-        <v>Grace Scott</v>
+        <v>Aurora Gonzalez</v>
       </c>
       <c r="C23">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D23" t="str">
         <v>Female</v>
       </c>
       <c r="E23" t="str">
-        <v>grace.scott94@hotmail.com</v>
+        <v>aurora.gonzalez29@outlook.com</v>
       </c>
       <c r="F23" t="str">
-        <v>0410 377 869</v>
+        <v>0404 610 172</v>
       </c>
       <c r="G23" t="str">
         <v>Toowoomba</v>
       </c>
       <c r="H23" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I23" t="str">
         <v>available</v>
@@ -1391,60 +1425,66 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>97646711-3e33-4ee9-8d83-bd6e0363ece0</v>
       </c>
       <c r="B24" t="str">
-        <v>Paisley Lee</v>
+        <v>Audrey Martin</v>
       </c>
       <c r="C24">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="D24" t="str">
         <v>Female</v>
       </c>
       <c r="E24" t="str">
-        <v>paisley.lee78@hotmail.com</v>
+        <v>audrey.martin33@yahoo.com</v>
       </c>
       <c r="F24" t="str">
-        <v>0400 179 607</v>
+        <v>0403 767 239</v>
       </c>
       <c r="G24" t="str">
-        <v>Ballarat</v>
+        <v>Adelaide</v>
       </c>
       <c r="H24" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I24" t="str">
         <v>available</v>
+      </c>
+      <c r="J24" t="str">
+        <v>Charlotte Johnson</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>0a153155-dcf5-4d56-9ed1-8960501157f8</v>
+        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
       </c>
       <c r="B25" t="str">
-        <v>Aurora Gonzalez</v>
+        <v>Audrey Ramirez</v>
       </c>
       <c r="C25">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D25" t="str">
         <v>Female</v>
       </c>
       <c r="E25" t="str">
-        <v>aurora.gonzalez29@outlook.com</v>
+        <v>audrey.ramirez12@gmail.com</v>
       </c>
       <c r="F25" t="str">
-        <v>0404 610 172</v>
+        <v>0411 212 619</v>
       </c>
       <c r="G25" t="str">
-        <v>Toowoomba</v>
+        <v>Brisbane</v>
       </c>
       <c r="H25" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I25" t="str">
         <v>available</v>
+      </c>
+      <c r="J25" t="str">
+        <v>Harper Lewis</v>
       </c>
     </row>
     <row r="26">
@@ -1475,28 +1515,31 @@
       <c r="I26" t="str">
         <v>available</v>
       </c>
+      <c r="J26" t="str">
+        <v>Audrey Martin</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
       </c>
       <c r="B27" t="str">
-        <v>Audrey Thomas</v>
+        <v>Emily Thomas</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D27" t="str">
         <v>Female</v>
       </c>
       <c r="E27" t="str">
-        <v>audrey.thomas38@gmail.com</v>
+        <v>emily.thomas25@outlook.com</v>
       </c>
       <c r="F27" t="str">
-        <v>0400 437 270</v>
+        <v>0402 648 577</v>
       </c>
       <c r="G27" t="str">
-        <v>Perth</v>
+        <v>Geelong</v>
       </c>
       <c r="H27" t="str">
         <v>C</v>
@@ -1504,28 +1547,34 @@
       <c r="I27" t="str">
         <v>available</v>
       </c>
+      <c r="J27" t="str">
+        <v>Stella Garcia</v>
+      </c>
+      <c r="M27" t="str">
+        <v>Knee replacement - cannot climb stairs</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
       </c>
       <c r="B28" t="str">
-        <v>Emilia Thompson</v>
+        <v>Audrey Smith</v>
       </c>
       <c r="C28">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D28" t="str">
         <v>Female</v>
       </c>
       <c r="E28" t="str">
-        <v>emilia.thompson0@gmail.com</v>
+        <v>audrey.smith66@gmail.com</v>
       </c>
       <c r="F28" t="str">
-        <v>0404 992 451</v>
+        <v>0410 904 568</v>
       </c>
       <c r="G28" t="str">
-        <v>Perth</v>
+        <v>Ballarat</v>
       </c>
       <c r="H28" t="str">
         <v>B</v>
@@ -1533,34 +1582,40 @@
       <c r="I28" t="str">
         <v>available</v>
       </c>
+      <c r="J28" t="str">
+        <v>Grace Scott</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>0dd7de5c-0409-45e3-84a5-5f2ffbd591d8</v>
+        <v>eff76f3c-c868-4954-99ea-92a4ae6c8067</v>
       </c>
       <c r="B29" t="str">
-        <v>Harper Sanchez</v>
+        <v>Abigail Lee</v>
       </c>
       <c r="C29">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D29" t="str">
         <v>Female</v>
       </c>
       <c r="E29" t="str">
-        <v>harper.sanchez76@gmail.com</v>
+        <v>abigail.lee94@hotmail.com</v>
       </c>
       <c r="F29" t="str">
-        <v>0411 422 972</v>
+        <v>0402 888 384</v>
       </c>
       <c r="G29" t="str">
-        <v>Geelong</v>
+        <v>Wollongong</v>
       </c>
       <c r="H29" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I29" t="str">
         <v>available</v>
+      </c>
+      <c r="J29" t="str">
+        <v>Hannah Martin</v>
       </c>
     </row>
     <row r="30">
@@ -1591,57 +1646,63 @@
       <c r="I30" t="str">
         <v>available</v>
       </c>
+      <c r="J30" t="str">
+        <v>Maya Moore</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
+        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
       </c>
       <c r="B31" t="str">
-        <v>Harper Lewis</v>
+        <v>Violet Hall</v>
       </c>
       <c r="C31">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D31" t="str">
         <v>Female</v>
       </c>
       <c r="E31" t="str">
-        <v>harper.lewis57@hotmail.com</v>
+        <v>violet.hall8@yahoo.com</v>
       </c>
       <c r="F31" t="str">
-        <v>0411 652 121</v>
+        <v>0404 640 755</v>
       </c>
       <c r="G31" t="str">
-        <v>Geelong</v>
+        <v>Adelaide</v>
       </c>
       <c r="H31" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I31" t="str">
         <v>available</v>
+      </c>
+      <c r="J31" t="str">
+        <v>Emilia Thompson</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
+        <v>55099144-967b-4cf2-b4ed-3cfe46413c92</v>
       </c>
       <c r="B32" t="str">
-        <v>Aria Scott</v>
+        <v>Maya Hernandez</v>
       </c>
       <c r="C32">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D32" t="str">
         <v>Female</v>
       </c>
       <c r="E32" t="str">
-        <v>aria.scott42@outlook.com</v>
+        <v>maya.hernandez32@outlook.com</v>
       </c>
       <c r="F32" t="str">
-        <v>0401 330 548</v>
+        <v>0400 358 904</v>
       </c>
       <c r="G32" t="str">
-        <v>Hobart</v>
+        <v>Brisbane</v>
       </c>
       <c r="H32" t="str">
         <v>C</v>
@@ -1649,118 +1710,127 @@
       <c r="I32" t="str">
         <v>available</v>
       </c>
+      <c r="J32" t="str">
+        <v>Aria Scott</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
+        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
       </c>
       <c r="B33" t="str">
-        <v>Emilia Miller</v>
+        <v>Paisley Scott</v>
       </c>
       <c r="C33">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D33" t="str">
         <v>Female</v>
       </c>
       <c r="E33" t="str">
-        <v>emilia.miller56@outlook.com</v>
+        <v>paisley.scott78@yahoo.com</v>
       </c>
       <c r="F33" t="str">
-        <v>0403 506 698</v>
+        <v>0410 215 419</v>
       </c>
       <c r="G33" t="str">
-        <v>Melbourne</v>
+        <v>Ballarat</v>
       </c>
       <c r="H33" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I33" t="str">
         <v>available</v>
+      </c>
+      <c r="J33" t="str">
+        <v>Mia Roberts</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
+        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
       </c>
       <c r="B34" t="str">
-        <v>Emily Thomas</v>
+        <v>Hunter Jackson</v>
       </c>
       <c r="C34">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D34" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E34" t="str">
-        <v>emily.thomas25@outlook.com</v>
+        <v>hunter.jackson50@outlook.com</v>
       </c>
       <c r="F34" t="str">
-        <v>0402 648 577</v>
+        <v>0404 841 788</v>
       </c>
       <c r="G34" t="str">
-        <v>Geelong</v>
+        <v>Townsville</v>
       </c>
       <c r="H34" t="str">
         <v>C</v>
       </c>
       <c r="I34" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>2c188398-79a8-4bf6-b740-1ad9d535662e</v>
+        <v>c5fdfaeb-862e-43ab-bf0e-ff3e14e5dbb3</v>
       </c>
       <c r="B35" t="str">
-        <v>Everly Torres</v>
+        <v>Hannah Martin</v>
       </c>
       <c r="C35">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D35" t="str">
         <v>Female</v>
       </c>
       <c r="E35" t="str">
-        <v>everly.torres12@gmail.com</v>
+        <v>hannah.martin78@yahoo.com</v>
       </c>
       <c r="F35" t="str">
-        <v>0412 804 179</v>
+        <v>0410 940 985</v>
       </c>
       <c r="G35" t="str">
-        <v>Sydney</v>
+        <v>Hobart</v>
       </c>
       <c r="H35" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I35" t="str">
         <v>available</v>
+      </c>
+      <c r="J35" t="str">
+        <v>Abigail Lee</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>55099144-967b-4cf2-b4ed-3cfe46413c92</v>
+        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
       </c>
       <c r="B36" t="str">
-        <v>Maya Hernandez</v>
+        <v>Ryan Williams</v>
       </c>
       <c r="C36">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D36" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E36" t="str">
-        <v>maya.hernandez32@outlook.com</v>
+        <v>ryan.williams82@hotmail.com</v>
       </c>
       <c r="F36" t="str">
-        <v>0400 358 904</v>
+        <v>0401 450 673</v>
       </c>
       <c r="G36" t="str">
-        <v>Brisbane</v>
+        <v>Perth</v>
       </c>
       <c r="H36" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I36" t="str">
         <v>available</v>
@@ -1768,25 +1838,25 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
+        <v>32ffeaf9-5f22-4db7-a70b-cbaab834db0d</v>
       </c>
       <c r="B37" t="str">
-        <v>Paisley Scott</v>
+        <v>Isabella Hill</v>
       </c>
       <c r="C37">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D37" t="str">
         <v>Female</v>
       </c>
       <c r="E37" t="str">
-        <v>paisley.scott78@yahoo.com</v>
+        <v>isabella.hill77@hotmail.com</v>
       </c>
       <c r="F37" t="str">
-        <v>0410 215 419</v>
+        <v>0412 663 356</v>
       </c>
       <c r="G37" t="str">
-        <v>Ballarat</v>
+        <v>Darwin</v>
       </c>
       <c r="H37" t="str">
         <v>B+</v>
@@ -1797,83 +1867,86 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
       </c>
       <c r="B38" t="str">
-        <v>Aria Lopez</v>
+        <v>Genesis Jones</v>
       </c>
       <c r="C38">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D38" t="str">
         <v>Female</v>
       </c>
       <c r="E38" t="str">
-        <v>aria.lopez55@hotmail.com</v>
+        <v>genesis.jones50@yahoo.com</v>
       </c>
       <c r="F38" t="str">
-        <v>0404 812 491</v>
+        <v>0404 967 604</v>
       </c>
       <c r="G38" t="str">
         <v>Sydney</v>
       </c>
       <c r="H38" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I38" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
       </c>
       <c r="B39" t="str">
-        <v>Isabella Brown</v>
+        <v>Hazel Mitchell</v>
       </c>
       <c r="C39">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D39" t="str">
         <v>Female</v>
       </c>
       <c r="E39" t="str">
-        <v>isabella.brown43@outlook.com</v>
+        <v>hazel.mitchell91@gmail.com</v>
       </c>
       <c r="F39" t="str">
-        <v>0403 771 690</v>
+        <v>0400 683 761</v>
       </c>
       <c r="G39" t="str">
-        <v>Darwin</v>
+        <v>Perth</v>
       </c>
       <c r="H39" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I39" t="str">
         <v>available</v>
+      </c>
+      <c r="J39" t="str">
+        <v>Caroline Taylor</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
+        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
       </c>
       <c r="B40" t="str">
-        <v>Stella Garcia</v>
+        <v>Victoria Carter</v>
       </c>
       <c r="C40">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D40" t="str">
         <v>Female</v>
       </c>
       <c r="E40" t="str">
-        <v>stella.garcia89@hotmail.com</v>
+        <v>victoria.carter74@gmail.com</v>
       </c>
       <c r="F40" t="str">
-        <v>0403 655 540</v>
+        <v>0411 641 632</v>
       </c>
       <c r="G40" t="str">
-        <v>Toowoomba</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H40" t="str">
         <v>B+</v>
@@ -1881,86 +1954,92 @@
       <c r="I40" t="str">
         <v>available</v>
       </c>
+      <c r="J40" t="str">
+        <v>Emilia Miller</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>c1783cdf-a656-46b4-9331-4d9d18d40b51</v>
+        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
       </c>
       <c r="B41" t="str">
-        <v>Aurora Walker</v>
+        <v>Andrew Garcia</v>
       </c>
       <c r="C41">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D41" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E41" t="str">
-        <v>aurora.walker1@outlook.com</v>
+        <v>andrew.garcia26@hotmail.com</v>
       </c>
       <c r="F41" t="str">
-        <v>0403 522 404</v>
+        <v>0400 450 222</v>
       </c>
       <c r="G41" t="str">
         <v>Darwin</v>
       </c>
       <c r="H41" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I41" t="str">
         <v>available</v>
+      </c>
+      <c r="M41" t="str">
+        <v>Limited mobility - prefers ground floor seating</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>32ffeaf9-5f22-4db7-a70b-cbaab834db0d</v>
+        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
       </c>
       <c r="B42" t="str">
-        <v>Isabella Hill</v>
+        <v>Noah Hernandez</v>
       </c>
       <c r="C42">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D42" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E42" t="str">
-        <v>isabella.hill77@hotmail.com</v>
+        <v>noah.hernandez9@hotmail.com</v>
       </c>
       <c r="F42" t="str">
-        <v>0412 663 356</v>
+        <v>0404 855 230</v>
       </c>
       <c r="G42" t="str">
-        <v>Darwin</v>
+        <v>Cairns</v>
       </c>
       <c r="H42" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I42" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
+        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
       </c>
       <c r="B43" t="str">
-        <v>Victoria Carter</v>
+        <v>Stella Garcia</v>
       </c>
       <c r="C43">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D43" t="str">
         <v>Female</v>
       </c>
       <c r="E43" t="str">
-        <v>victoria.carter74@gmail.com</v>
+        <v>stella.garcia89@hotmail.com</v>
       </c>
       <c r="F43" t="str">
-        <v>0411 641 632</v>
+        <v>0403 655 540</v>
       </c>
       <c r="G43" t="str">
-        <v>Gold Coast</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H43" t="str">
         <v>B+</v>
@@ -1968,31 +2047,34 @@
       <c r="I43" t="str">
         <v>available</v>
       </c>
+      <c r="J43" t="str">
+        <v>Emily Thomas</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>c5fdfaeb-862e-43ab-bf0e-ff3e14e5dbb3</v>
+        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
       </c>
       <c r="B44" t="str">
-        <v>Hannah Martin</v>
+        <v>Nathan Allen</v>
       </c>
       <c r="C44">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="D44" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E44" t="str">
-        <v>hannah.martin78@yahoo.com</v>
+        <v>nathan.allen87@outlook.com</v>
       </c>
       <c r="F44" t="str">
-        <v>0410 940 985</v>
+        <v>0403 587 263</v>
       </c>
       <c r="G44" t="str">
-        <v>Hobart</v>
+        <v>Adelaide</v>
       </c>
       <c r="H44" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I44" t="str">
         <v>available</v>
@@ -2000,28 +2082,28 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>f6a281bb-caec-44cf-a596-a6e92d6e2610</v>
+        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
       </c>
       <c r="B45" t="str">
-        <v>Leah Scott</v>
+        <v>Jackson Young</v>
       </c>
       <c r="C45">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="D45" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E45" t="str">
-        <v>leah.scott74@gmail.com</v>
+        <v>jackson.young79@yahoo.com</v>
       </c>
       <c r="F45" t="str">
-        <v>0402 414 358</v>
+        <v>0412 940 993</v>
       </c>
       <c r="G45" t="str">
-        <v>Perth</v>
+        <v>Ballarat</v>
       </c>
       <c r="H45" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I45" t="str">
         <v>available</v>
@@ -2029,25 +2111,25 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
+        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
       </c>
       <c r="B46" t="str">
-        <v>Stella Hall</v>
+        <v>Emilia Lopez</v>
       </c>
       <c r="C46">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D46" t="str">
         <v>Female</v>
       </c>
       <c r="E46" t="str">
-        <v>stella.hall72@gmail.com</v>
+        <v>emilia.lopez21@gmail.com</v>
       </c>
       <c r="F46" t="str">
-        <v>0410 133 818</v>
+        <v>0403 491 553</v>
       </c>
       <c r="G46" t="str">
-        <v>Wollongong</v>
+        <v>Cairns</v>
       </c>
       <c r="H46" t="str">
         <v>B</v>
@@ -2055,31 +2137,34 @@
       <c r="I46" t="str">
         <v>available</v>
       </c>
+      <c r="J46" t="str">
+        <v>Aurora Rodriguez</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
+        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
       </c>
       <c r="B47" t="str">
-        <v>Evelyn Clark</v>
+        <v>Cameron Lee</v>
       </c>
       <c r="C47">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D47" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E47" t="str">
-        <v>evelyn.clark47@outlook.com</v>
+        <v>cameron.lee78@yahoo.com</v>
       </c>
       <c r="F47" t="str">
-        <v>0410 941 656</v>
+        <v>0404 821 708</v>
       </c>
       <c r="G47" t="str">
-        <v>Hobart</v>
+        <v>Cairns</v>
       </c>
       <c r="H47" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I47" t="str">
         <v>available</v>
@@ -2087,57 +2172,60 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
+        <v>c1783cdf-a656-46b4-9331-4d9d18d40b51</v>
       </c>
       <c r="B48" t="str">
-        <v>Stella Green</v>
+        <v>Aurora Walker</v>
       </c>
       <c r="C48">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D48" t="str">
         <v>Female</v>
       </c>
       <c r="E48" t="str">
-        <v>stella.green92@gmail.com</v>
+        <v>aurora.walker1@outlook.com</v>
       </c>
       <c r="F48" t="str">
-        <v>0404 230 858</v>
+        <v>0403 522 404</v>
       </c>
       <c r="G48" t="str">
-        <v>Wollongong</v>
+        <v>Darwin</v>
       </c>
       <c r="H48" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I48" t="str">
         <v>available</v>
+      </c>
+      <c r="M48" t="str">
+        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+        <v>182bd5d2-7f68-4c83-b156-e80856f3b6b7</v>
       </c>
       <c r="B49" t="str">
-        <v>Violet Hall</v>
+        <v>Mason Nelson</v>
       </c>
       <c r="C49">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D49" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E49" t="str">
-        <v>violet.hall8@yahoo.com</v>
+        <v>mason.nelson14@hotmail.com</v>
       </c>
       <c r="F49" t="str">
-        <v>0404 640 755</v>
+        <v>0403 485 650</v>
       </c>
       <c r="G49" t="str">
-        <v>Adelaide</v>
+        <v>Canberra</v>
       </c>
       <c r="H49" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I49" t="str">
         <v>available</v>
@@ -2145,54 +2233,57 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
+        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
       </c>
       <c r="B50" t="str">
-        <v>Victoria Torres</v>
+        <v>Oliver Rivera</v>
       </c>
       <c r="C50">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D50" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E50" t="str">
-        <v>victoria.torres48@outlook.com</v>
+        <v>oliver.rivera58@outlook.com</v>
       </c>
       <c r="F50" t="str">
-        <v>0411 539 271</v>
+        <v>0412 991 121</v>
       </c>
       <c r="G50" t="str">
-        <v>Geelong</v>
+        <v>Canberra</v>
       </c>
       <c r="H50" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I50" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="M50" t="str">
+        <v>Requires wheelchair access</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
+        <v>3d2128a1-336f-41e1-973b-b5dd54d90b19</v>
       </c>
       <c r="B51" t="str">
-        <v>Hazel Mitchell</v>
+        <v>Nova Brown</v>
       </c>
       <c r="C51">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D51" t="str">
         <v>Female</v>
       </c>
       <c r="E51" t="str">
-        <v>hazel.mitchell91@gmail.com</v>
+        <v>nova.brown80@outlook.com</v>
       </c>
       <c r="F51" t="str">
-        <v>0400 683 761</v>
+        <v>0411 154 614</v>
       </c>
       <c r="G51" t="str">
-        <v>Perth</v>
+        <v>Ballarat</v>
       </c>
       <c r="H51" t="str">
         <v>A</v>
@@ -2203,28 +2294,28 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
+        <v>0faec83d-7c29-4269-bf33-391ef02d60e4</v>
       </c>
       <c r="B52" t="str">
-        <v>Emilia Lopez</v>
+        <v>Anna White</v>
       </c>
       <c r="C52">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D52" t="str">
         <v>Female</v>
       </c>
       <c r="E52" t="str">
-        <v>emilia.lopez21@gmail.com</v>
+        <v>anna.white24@yahoo.com</v>
       </c>
       <c r="F52" t="str">
-        <v>0403 491 553</v>
+        <v>0400 132 564</v>
       </c>
       <c r="G52" t="str">
-        <v>Cairns</v>
+        <v>Adelaide</v>
       </c>
       <c r="H52" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I52" t="str">
         <v>available</v>
@@ -2232,202 +2323,211 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>222469f4-a8d9-4550-b6ee-db9d00e24edd</v>
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
       </c>
       <c r="B53" t="str">
-        <v>Chloe Flores</v>
+        <v>Carter Harris</v>
       </c>
       <c r="C53">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D53" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E53" t="str">
-        <v>chloe.flores93@yahoo.com</v>
+        <v>carter.harris82@yahoo.com</v>
       </c>
       <c r="F53" t="str">
-        <v>0400 918 463</v>
+        <v>0412 175 744</v>
       </c>
       <c r="G53" t="str">
-        <v>Townsville</v>
+        <v>Geelong</v>
       </c>
       <c r="H53" t="str">
         <v>C</v>
       </c>
       <c r="I53" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>7664257a-dce4-407a-8f24-692043d568be</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="B54" t="str">
-        <v>Nora Jackson</v>
+        <v>Isabella Brown</v>
       </c>
       <c r="C54">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D54" t="str">
         <v>Female</v>
       </c>
       <c r="E54" t="str">
-        <v>nora.jackson83@hotmail.com</v>
+        <v>isabella.brown43@outlook.com</v>
       </c>
       <c r="F54" t="str">
-        <v>0404 434 899</v>
+        <v>0403 771 690</v>
       </c>
       <c r="G54" t="str">
-        <v>Wollongong</v>
+        <v>Darwin</v>
       </c>
       <c r="H54" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I54" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J54" t="str">
+        <v>Ella Anderson</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
+        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
       </c>
       <c r="B55" t="str">
-        <v>Genesis Jones</v>
+        <v>Stella Hall</v>
       </c>
       <c r="C55">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D55" t="str">
         <v>Female</v>
       </c>
       <c r="E55" t="str">
-        <v>genesis.jones50@yahoo.com</v>
+        <v>stella.hall72@gmail.com</v>
       </c>
       <c r="F55" t="str">
-        <v>0404 967 604</v>
+        <v>0410 133 818</v>
       </c>
       <c r="G55" t="str">
-        <v>Sydney</v>
+        <v>Wollongong</v>
       </c>
       <c r="H55" t="str">
         <v>B</v>
       </c>
       <c r="I55" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>3d2128a1-336f-41e1-973b-b5dd54d90b19</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="B56" t="str">
-        <v>Nova Brown</v>
+        <v>Aria Lopez</v>
       </c>
       <c r="C56">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D56" t="str">
         <v>Female</v>
       </c>
       <c r="E56" t="str">
-        <v>nova.brown80@outlook.com</v>
+        <v>aria.lopez55@hotmail.com</v>
       </c>
       <c r="F56" t="str">
-        <v>0411 154 614</v>
+        <v>0404 812 491</v>
       </c>
       <c r="G56" t="str">
-        <v>Ballarat</v>
+        <v>Sydney</v>
       </c>
       <c r="H56" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I56" t="str">
         <v>available</v>
+      </c>
+      <c r="J56" t="str">
+        <v>Paisley Lee</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>0faec83d-7c29-4269-bf33-391ef02d60e4</v>
+        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
       </c>
       <c r="B57" t="str">
-        <v>Anna White</v>
+        <v>Evelyn Clark</v>
       </c>
       <c r="C57">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D57" t="str">
         <v>Female</v>
       </c>
       <c r="E57" t="str">
-        <v>anna.white24@yahoo.com</v>
+        <v>evelyn.clark47@outlook.com</v>
       </c>
       <c r="F57" t="str">
-        <v>0400 132 564</v>
+        <v>0410 941 656</v>
       </c>
       <c r="G57" t="str">
-        <v>Adelaide</v>
+        <v>Hobart</v>
       </c>
       <c r="H57" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I57" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
+        <v>f1466859-7323-4893-a189-a0ce994068ba</v>
       </c>
       <c r="B58" t="str">
-        <v>Hunter Jackson</v>
+        <v>Anthony Thompson</v>
       </c>
       <c r="C58">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D58" t="str">
         <v>Male</v>
       </c>
       <c r="E58" t="str">
-        <v>hunter.jackson50@outlook.com</v>
+        <v>anthony.thompson29@yahoo.com</v>
       </c>
       <c r="F58" t="str">
-        <v>0404 841 788</v>
+        <v>0412 442 587</v>
       </c>
       <c r="G58" t="str">
         <v>Townsville</v>
       </c>
       <c r="H58" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="I58" t="str">
         <v>available</v>
+      </c>
+      <c r="M58" t="str">
+        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
+        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
       </c>
       <c r="B59" t="str">
-        <v>Nathan Allen</v>
+        <v>Mason Hill</v>
       </c>
       <c r="C59">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D59" t="str">
         <v>Male</v>
       </c>
       <c r="E59" t="str">
-        <v>nathan.allen87@outlook.com</v>
+        <v>mason.hill27@outlook.com</v>
       </c>
       <c r="F59" t="str">
-        <v>0403 587 263</v>
+        <v>0410 682 884</v>
       </c>
       <c r="G59" t="str">
-        <v>Adelaide</v>
+        <v>Canberra</v>
       </c>
       <c r="H59" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I59" t="str">
         <v>available</v>
@@ -2435,28 +2535,28 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
+        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
       </c>
       <c r="B60" t="str">
-        <v>Noah Hernandez</v>
+        <v>Scarlett Lopez</v>
       </c>
       <c r="C60">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="D60" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E60" t="str">
-        <v>noah.hernandez9@hotmail.com</v>
+        <v>scarlett.lopez53@yahoo.com</v>
       </c>
       <c r="F60" t="str">
-        <v>0404 855 230</v>
+        <v>0400 509 641</v>
       </c>
       <c r="G60" t="str">
-        <v>Cairns</v>
+        <v>Sydney</v>
       </c>
       <c r="H60" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I60" t="str">
         <v>available</v>
@@ -2464,28 +2564,28 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
+        <v>34685ff7-6e85-4bbd-b546-77cfe11d7f7d</v>
       </c>
       <c r="B61" t="str">
-        <v>Ryan Williams</v>
+        <v>Grace Walker</v>
       </c>
       <c r="C61">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D61" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E61" t="str">
-        <v>ryan.williams82@hotmail.com</v>
+        <v>grace.walker52@hotmail.com</v>
       </c>
       <c r="F61" t="str">
-        <v>0401 450 673</v>
+        <v>0412 754 780</v>
       </c>
       <c r="G61" t="str">
-        <v>Perth</v>
+        <v>Canberra</v>
       </c>
       <c r="H61" t="str">
-        <v>B+</v>
+        <v>A+</v>
       </c>
       <c r="I61" t="str">
         <v>available</v>
@@ -2493,28 +2593,28 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
+        <v>ee7f9d33-09d6-417b-a45f-3e6554489f5b</v>
       </c>
       <c r="B62" t="str">
-        <v>Oliver Rivera</v>
+        <v>Dylan Miller</v>
       </c>
       <c r="C62">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D62" t="str">
         <v>Male</v>
       </c>
       <c r="E62" t="str">
-        <v>oliver.rivera58@outlook.com</v>
+        <v>dylan.miller23@hotmail.com</v>
       </c>
       <c r="F62" t="str">
-        <v>0412 991 121</v>
+        <v>0402 417 876</v>
       </c>
       <c r="G62" t="str">
-        <v>Canberra</v>
+        <v>Melbourne</v>
       </c>
       <c r="H62" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="I62" t="str">
         <v>available</v>
@@ -2522,28 +2622,28 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
+        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
       </c>
       <c r="B63" t="str">
-        <v>Joshua Walker</v>
+        <v>Christian Rivera</v>
       </c>
       <c r="C63">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D63" t="str">
         <v>Male</v>
       </c>
       <c r="E63" t="str">
-        <v>joshua.walker97@gmail.com</v>
+        <v>christian.rivera86@hotmail.com</v>
       </c>
       <c r="F63" t="str">
-        <v>0402 640 379</v>
+        <v>0400 135 743</v>
       </c>
       <c r="G63" t="str">
-        <v>Darwin</v>
+        <v>Adelaide</v>
       </c>
       <c r="H63" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I63" t="str">
         <v>available</v>
@@ -2551,28 +2651,28 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+        <v>5a6b21ec-9fac-4adc-b5ab-bcad20d0eca4</v>
       </c>
       <c r="B64" t="str">
-        <v>Carter Harris</v>
+        <v>Hunter Harris</v>
       </c>
       <c r="C64">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D64" t="str">
         <v>Male</v>
       </c>
       <c r="E64" t="str">
-        <v>carter.harris82@yahoo.com</v>
+        <v>hunter.harris1@gmail.com</v>
       </c>
       <c r="F64" t="str">
-        <v>0412 175 744</v>
+        <v>0404 782 485</v>
       </c>
       <c r="G64" t="str">
-        <v>Geelong</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H64" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="I64" t="str">
         <v>available</v>
@@ -2580,86 +2680,86 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
+        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
       </c>
       <c r="B65" t="str">
-        <v>Andrew Garcia</v>
+        <v>Joshua Carter</v>
       </c>
       <c r="C65">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D65" t="str">
         <v>Male</v>
       </c>
       <c r="E65" t="str">
-        <v>andrew.garcia26@hotmail.com</v>
+        <v>joshua.carter41@hotmail.com</v>
       </c>
       <c r="F65" t="str">
-        <v>0400 450 222</v>
+        <v>0404 538 442</v>
       </c>
       <c r="G65" t="str">
-        <v>Darwin</v>
+        <v>Wollongong</v>
       </c>
       <c r="H65" t="str">
         <v>B</v>
       </c>
       <c r="I65" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>f1466859-7323-4893-a189-a0ce994068ba</v>
+        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
       </c>
       <c r="B66" t="str">
-        <v>Anthony Thompson</v>
+        <v>Lucas Thomas</v>
       </c>
       <c r="C66">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D66" t="str">
         <v>Male</v>
       </c>
       <c r="E66" t="str">
-        <v>anthony.thompson29@yahoo.com</v>
+        <v>lucas.thomas30@yahoo.com</v>
       </c>
       <c r="F66" t="str">
-        <v>0412 442 587</v>
+        <v>0412 527 117</v>
       </c>
       <c r="G66" t="str">
-        <v>Townsville</v>
+        <v>Brisbane</v>
       </c>
       <c r="H66" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I66" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
       </c>
       <c r="B67" t="str">
-        <v>Samuel King</v>
+        <v>Julian Rivera</v>
       </c>
       <c r="C67">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D67" t="str">
         <v>Male</v>
       </c>
       <c r="E67" t="str">
-        <v>samuel.king24@yahoo.com</v>
+        <v>julian.rivera31@outlook.com</v>
       </c>
       <c r="F67" t="str">
-        <v>0400 774 736</v>
+        <v>0401 414 502</v>
       </c>
       <c r="G67" t="str">
-        <v>Newcastle</v>
+        <v>Perth</v>
       </c>
       <c r="H67" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I67" t="str">
         <v>available</v>
@@ -2667,54 +2767,54 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
+        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
       </c>
       <c r="B68" t="str">
-        <v>Mason Hill</v>
+        <v>Joshua Jones</v>
       </c>
       <c r="C68">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D68" t="str">
         <v>Male</v>
       </c>
       <c r="E68" t="str">
-        <v>mason.hill27@outlook.com</v>
+        <v>joshua.jones82@yahoo.com</v>
       </c>
       <c r="F68" t="str">
-        <v>0410 682 884</v>
+        <v>0400 652 840</v>
       </c>
       <c r="G68" t="str">
-        <v>Canberra</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H68" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I68" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
+        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
       </c>
       <c r="B69" t="str">
-        <v>Jackson Young</v>
+        <v>Ryan Lewis</v>
       </c>
       <c r="C69">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D69" t="str">
         <v>Male</v>
       </c>
       <c r="E69" t="str">
-        <v>jackson.young79@yahoo.com</v>
+        <v>ryan.lewis85@yahoo.com</v>
       </c>
       <c r="F69" t="str">
-        <v>0412 940 993</v>
+        <v>0400 187 811</v>
       </c>
       <c r="G69" t="str">
-        <v>Ballarat</v>
+        <v>Canberra</v>
       </c>
       <c r="H69" t="str">
         <v>B+</v>
@@ -2725,434 +2825,446 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>182bd5d2-7f68-4c83-b156-e80856f3b6b7</v>
+        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
       </c>
       <c r="B70" t="str">
-        <v>Mason Nelson</v>
+        <v>Carter Hill</v>
       </c>
       <c r="C70">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="D70" t="str">
         <v>Male</v>
       </c>
       <c r="E70" t="str">
-        <v>mason.nelson14@hotmail.com</v>
+        <v>carter.hill93@gmail.com</v>
       </c>
       <c r="F70" t="str">
-        <v>0403 485 650</v>
+        <v>0404 349 309</v>
       </c>
       <c r="G70" t="str">
-        <v>Canberra</v>
+        <v>Newcastle</v>
       </c>
       <c r="H70" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I70" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
+        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
       </c>
       <c r="B71" t="str">
-        <v>Cameron Lee</v>
+        <v>Nora Mitchell</v>
       </c>
       <c r="C71">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D71" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E71" t="str">
-        <v>cameron.lee78@yahoo.com</v>
+        <v>nora.mitchell66@outlook.com</v>
       </c>
       <c r="F71" t="str">
-        <v>0404 821 708</v>
+        <v>0412 196 419</v>
       </c>
       <c r="G71" t="str">
-        <v>Cairns</v>
+        <v>Adelaide</v>
       </c>
       <c r="H71" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I71" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
       </c>
       <c r="B72" t="str">
-        <v>Emily Johnson</v>
+        <v>Abigail Williams</v>
       </c>
       <c r="C72">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D72" t="str">
         <v>Female</v>
       </c>
       <c r="E72" t="str">
-        <v>emily.johnson58@hotmail.com</v>
+        <v>abigail.williams45@yahoo.com</v>
       </c>
       <c r="F72" t="str">
-        <v>0412 663 939</v>
+        <v>0403 497 445</v>
       </c>
       <c r="G72" t="str">
-        <v>Perth</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H72" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I72" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>3db7cdb3-9a92-467c-b554-d23b524f42f5</v>
+        <v>ecc70875-f282-4849-9e60-071edc278977</v>
       </c>
       <c r="B73" t="str">
-        <v>Claire Campbell</v>
+        <v>Noah White</v>
       </c>
       <c r="C73">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D73" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E73" t="str">
-        <v>claire.campbell9@outlook.com</v>
+        <v>noah.white20@gmail.com</v>
       </c>
       <c r="F73" t="str">
-        <v>0401 164 490</v>
+        <v>0410 565 594</v>
       </c>
       <c r="G73" t="str">
-        <v>Darwin</v>
+        <v>Adelaide</v>
       </c>
       <c r="H73" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I73" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="M73" t="str">
+        <v>Requires wheelchair access</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
+        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
       </c>
       <c r="B74" t="str">
-        <v>Aurora Williams</v>
+        <v>Joshua Clark</v>
       </c>
       <c r="C74">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D74" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E74" t="str">
-        <v>aurora.williams76@outlook.com</v>
+        <v>joshua.clark16@outlook.com</v>
       </c>
       <c r="F74" t="str">
-        <v>0401 416 170</v>
+        <v>0403 901 485</v>
       </c>
       <c r="G74" t="str">
-        <v>Darwin</v>
+        <v>Sydney</v>
       </c>
       <c r="H74" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I74" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
+        <v>da40ad70-95be-413c-b0f1-d089ef285cc8</v>
       </c>
       <c r="B75" t="str">
-        <v>Aria Nguyen</v>
+        <v>Emily Smith</v>
       </c>
       <c r="C75">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D75" t="str">
         <v>Female</v>
       </c>
       <c r="E75" t="str">
-        <v>aria.nguyen36@gmail.com</v>
+        <v>emily.smith56@hotmail.com</v>
       </c>
       <c r="F75" t="str">
-        <v>0401 618 716</v>
+        <v>0410 101 780</v>
       </c>
       <c r="G75" t="str">
-        <v>Sydney</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H75" t="str">
-        <v>C</v>
+        <v>A+</v>
       </c>
       <c r="I75" t="str">
         <v>available</v>
+      </c>
+      <c r="M75" t="str">
+        <v>Limited mobility - prefers ground floor seating</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
+        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
       </c>
       <c r="B76" t="str">
-        <v>Nora Mitchell</v>
+        <v>Joshua Scott</v>
       </c>
       <c r="C76">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D76" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E76" t="str">
-        <v>nora.mitchell66@outlook.com</v>
+        <v>joshua.scott95@outlook.com</v>
       </c>
       <c r="F76" t="str">
-        <v>0412 196 419</v>
+        <v>0410 137 561</v>
       </c>
       <c r="G76" t="str">
-        <v>Adelaide</v>
+        <v>Canberra</v>
       </c>
       <c r="H76" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I76" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
+        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
       </c>
       <c r="B77" t="str">
-        <v>Scarlett Wright</v>
+        <v>Aria Nguyen</v>
       </c>
       <c r="C77">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D77" t="str">
         <v>Female</v>
       </c>
       <c r="E77" t="str">
-        <v>scarlett.wright68@outlook.com</v>
+        <v>aria.nguyen36@gmail.com</v>
       </c>
       <c r="F77" t="str">
-        <v>0412 487 763</v>
+        <v>0401 618 716</v>
       </c>
       <c r="G77" t="str">
-        <v>Newcastle</v>
+        <v>Sydney</v>
       </c>
       <c r="H77" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I77" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
+        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
       </c>
       <c r="B78" t="str">
-        <v>Abigail Williams</v>
+        <v>Ethan Taylor</v>
       </c>
       <c r="C78">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="D78" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E78" t="str">
-        <v>abigail.williams45@yahoo.com</v>
+        <v>ethan.taylor22@yahoo.com</v>
       </c>
       <c r="F78" t="str">
-        <v>0403 497 445</v>
+        <v>0410 363 173</v>
       </c>
       <c r="G78" t="str">
-        <v>Toowoomba</v>
+        <v>Adelaide</v>
       </c>
       <c r="H78" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I78" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>6591420b-4762-4d90-b738-8a5b70458c40</v>
+        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
       </c>
       <c r="B79" t="str">
-        <v>Aurora Hill</v>
+        <v>Theodore Nelson</v>
       </c>
       <c r="C79">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D79" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E79" t="str">
-        <v>aurora.hill33@hotmail.com</v>
+        <v>theodore.nelson79@gmail.com</v>
       </c>
       <c r="F79" t="str">
-        <v>0410 373 844</v>
+        <v>0403 813 793</v>
       </c>
       <c r="G79" t="str">
-        <v>Gold Coast</v>
+        <v>Canberra</v>
       </c>
       <c r="H79" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I79" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
+        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
       </c>
       <c r="B80" t="str">
-        <v>Lily Walker</v>
+        <v>Maya Moore</v>
       </c>
       <c r="C80">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D80" t="str">
         <v>Female</v>
       </c>
       <c r="E80" t="str">
-        <v>lily.walker96@outlook.com</v>
+        <v>maya.moore54@outlook.com</v>
       </c>
       <c r="F80" t="str">
-        <v>0410 155 426</v>
+        <v>0400 718 585</v>
       </c>
       <c r="G80" t="str">
-        <v>Hobart</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H80" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I80" t="str">
         <v>available</v>
+      </c>
+      <c r="J80" t="str">
+        <v>Sofia Williams</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
+        <v>222469f4-a8d9-4550-b6ee-db9d00e24edd</v>
       </c>
       <c r="B81" t="str">
-        <v>Scarlett Lopez</v>
+        <v>Chloe Flores</v>
       </c>
       <c r="C81">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D81" t="str">
         <v>Female</v>
       </c>
       <c r="E81" t="str">
-        <v>scarlett.lopez53@yahoo.com</v>
+        <v>chloe.flores93@yahoo.com</v>
       </c>
       <c r="F81" t="str">
-        <v>0400 509 641</v>
+        <v>0400 918 463</v>
       </c>
       <c r="G81" t="str">
-        <v>Sydney</v>
+        <v>Townsville</v>
       </c>
       <c r="H81" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I81" t="str">
         <v>available</v>
+      </c>
+      <c r="J81" t="str">
+        <v>Evelyn Sanchez</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>34685ff7-6e85-4bbd-b546-77cfe11d7f7d</v>
+        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
       </c>
       <c r="B82" t="str">
-        <v>Grace Walker</v>
+        <v>Theodore Allen</v>
       </c>
       <c r="C82">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D82" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E82" t="str">
-        <v>grace.walker52@hotmail.com</v>
+        <v>theodore.allen25@outlook.com</v>
       </c>
       <c r="F82" t="str">
-        <v>0412 754 780</v>
+        <v>0400 438 819</v>
       </c>
       <c r="G82" t="str">
-        <v>Canberra</v>
+        <v>Newcastle</v>
       </c>
       <c r="H82" t="str">
-        <v>A+</v>
+        <v>B+</v>
       </c>
       <c r="I82" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>da40ad70-95be-413c-b0f1-d089ef285cc8</v>
+        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
       </c>
       <c r="B83" t="str">
-        <v>Emily Smith</v>
+        <v>Charles Torres</v>
       </c>
       <c r="C83">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D83" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E83" t="str">
-        <v>emily.smith56@hotmail.com</v>
+        <v>charles.torres98@outlook.com</v>
       </c>
       <c r="F83" t="str">
-        <v>0410 101 780</v>
+        <v>0401 744 176</v>
       </c>
       <c r="G83" t="str">
-        <v>Toowoomba</v>
+        <v>Wollongong</v>
       </c>
       <c r="H83" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I83" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>ee7f9d33-09d6-417b-a45f-3e6554489f5b</v>
+        <v>6591420b-4762-4d90-b738-8a5b70458c40</v>
       </c>
       <c r="B84" t="str">
-        <v>Dylan Miller</v>
+        <v>Aurora Hill</v>
       </c>
       <c r="C84">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D84" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E84" t="str">
-        <v>dylan.miller23@hotmail.com</v>
+        <v>aurora.hill33@hotmail.com</v>
       </c>
       <c r="F84" t="str">
-        <v>0402 417 876</v>
+        <v>0410 373 844</v>
       </c>
       <c r="G84" t="str">
-        <v>Melbourne</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H84" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I84" t="str">
         <v>available</v>
@@ -3160,25 +3272,25 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
+        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
       </c>
       <c r="B85" t="str">
-        <v>Christian Rivera</v>
+        <v>Lily Walker</v>
       </c>
       <c r="C85">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D85" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E85" t="str">
-        <v>christian.rivera86@hotmail.com</v>
+        <v>lily.walker96@outlook.com</v>
       </c>
       <c r="F85" t="str">
-        <v>0400 135 743</v>
+        <v>0410 155 426</v>
       </c>
       <c r="G85" t="str">
-        <v>Adelaide</v>
+        <v>Hobart</v>
       </c>
       <c r="H85" t="str">
         <v>B+</v>
@@ -3189,28 +3301,28 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>5a6b21ec-9fac-4adc-b5ab-bcad20d0eca4</v>
+        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
       </c>
       <c r="B86" t="str">
-        <v>Hunter Harris</v>
+        <v>Jayden Nguyen</v>
       </c>
       <c r="C86">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D86" t="str">
         <v>Male</v>
       </c>
       <c r="E86" t="str">
-        <v>hunter.harris1@gmail.com</v>
+        <v>jayden.nguyen88@hotmail.com</v>
       </c>
       <c r="F86" t="str">
-        <v>0404 782 485</v>
+        <v>0401 108 628</v>
       </c>
       <c r="G86" t="str">
-        <v>Gold Coast</v>
+        <v>Hobart</v>
       </c>
       <c r="H86" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I86" t="str">
         <v>available</v>
@@ -3218,57 +3330,60 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
+        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
       </c>
       <c r="B87" t="str">
-        <v>Ethan Taylor</v>
+        <v>Aurora Williams</v>
       </c>
       <c r="C87">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D87" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E87" t="str">
-        <v>ethan.taylor22@yahoo.com</v>
+        <v>aurora.williams76@outlook.com</v>
       </c>
       <c r="F87" t="str">
-        <v>0410 363 173</v>
+        <v>0401 416 170</v>
       </c>
       <c r="G87" t="str">
-        <v>Adelaide</v>
+        <v>Darwin</v>
       </c>
       <c r="H87" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I87" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="M87" t="str">
+        <v>Uses walking cane</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
+        <v>3db7cdb3-9a92-467c-b554-d23b524f42f5</v>
       </c>
       <c r="B88" t="str">
-        <v>Charles Torres</v>
+        <v>Claire Campbell</v>
       </c>
       <c r="C88">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="D88" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E88" t="str">
-        <v>charles.torres98@outlook.com</v>
+        <v>claire.campbell9@outlook.com</v>
       </c>
       <c r="F88" t="str">
-        <v>0401 744 176</v>
+        <v>0401 164 490</v>
       </c>
       <c r="G88" t="str">
-        <v>Wollongong</v>
+        <v>Darwin</v>
       </c>
       <c r="H88" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I88" t="str">
         <v>available</v>
@@ -3276,28 +3391,28 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
+        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
       </c>
       <c r="B89" t="str">
-        <v>Julian Rivera</v>
+        <v>Emily Johnson</v>
       </c>
       <c r="C89">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D89" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E89" t="str">
-        <v>julian.rivera31@outlook.com</v>
+        <v>emily.johnson58@hotmail.com</v>
       </c>
       <c r="F89" t="str">
-        <v>0401 414 502</v>
+        <v>0412 663 939</v>
       </c>
       <c r="G89" t="str">
         <v>Perth</v>
       </c>
       <c r="H89" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I89" t="str">
         <v>available</v>
@@ -3305,54 +3420,60 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
+        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
       </c>
       <c r="B90" t="str">
-        <v>Joshua Carter</v>
+        <v>Aurora Rodriguez</v>
       </c>
       <c r="C90">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="D90" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E90" t="str">
-        <v>joshua.carter41@hotmail.com</v>
+        <v>aurora.rodriguez20@yahoo.com</v>
       </c>
       <c r="F90" t="str">
-        <v>0404 538 442</v>
+        <v>0404 720 692</v>
       </c>
       <c r="G90" t="str">
-        <v>Wollongong</v>
+        <v>Hobart</v>
       </c>
       <c r="H90" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I90" t="str">
         <v>available</v>
+      </c>
+      <c r="J90" t="str">
+        <v>Emilia Lopez</v>
+      </c>
+      <c r="M90" t="str">
+        <v>Arthritis - prefers aisle seating for easy exit</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
+        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
       </c>
       <c r="B91" t="str">
-        <v>Ryan Lewis</v>
+        <v>Grace Scott</v>
       </c>
       <c r="C91">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D91" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E91" t="str">
-        <v>ryan.lewis85@yahoo.com</v>
+        <v>grace.scott40@outlook.com</v>
       </c>
       <c r="F91" t="str">
-        <v>0400 187 811</v>
+        <v>0401 870 853</v>
       </c>
       <c r="G91" t="str">
-        <v>Canberra</v>
+        <v>Ballarat</v>
       </c>
       <c r="H91" t="str">
         <v>B+</v>
@@ -3360,28 +3481,34 @@
       <c r="I91" t="str">
         <v>available</v>
       </c>
+      <c r="J91" t="str">
+        <v>Emily Moore</v>
+      </c>
+      <c r="M91" t="str">
+        <v>Hearing impaired - requires front row seating</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
+        <v>f6a281bb-caec-44cf-a596-a6e92d6e2610</v>
       </c>
       <c r="B92" t="str">
-        <v>Lucas Thomas</v>
+        <v>Leah Scott</v>
       </c>
       <c r="C92">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D92" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E92" t="str">
-        <v>lucas.thomas30@yahoo.com</v>
+        <v>leah.scott74@gmail.com</v>
       </c>
       <c r="F92" t="str">
-        <v>0412 527 117</v>
+        <v>0402 414 358</v>
       </c>
       <c r="G92" t="str">
-        <v>Brisbane</v>
+        <v>Perth</v>
       </c>
       <c r="H92" t="str">
         <v>B</v>
@@ -3389,173 +3516,212 @@
       <c r="I92" t="str">
         <v>available</v>
       </c>
+      <c r="J92" t="str">
+        <v>Harper Sanchez</v>
+      </c>
+      <c r="M92" t="str">
+        <v>Limited mobility - prefers ground floor seating</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
+        <v>7664257a-dce4-407a-8f24-692043d568be</v>
       </c>
       <c r="B93" t="str">
-        <v>Joshua Jones</v>
+        <v>Nora Jackson</v>
       </c>
       <c r="C93">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D93" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E93" t="str">
-        <v>joshua.jones82@yahoo.com</v>
+        <v>nora.jackson83@hotmail.com</v>
       </c>
       <c r="F93" t="str">
-        <v>0400 652 840</v>
+        <v>0404 434 899</v>
       </c>
       <c r="G93" t="str">
-        <v>Toowoomba</v>
+        <v>Wollongong</v>
       </c>
       <c r="H93" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I93" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
+        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
       </c>
       <c r="B94" t="str">
-        <v>Carter Hill</v>
+        <v>Ethan Rodriguez</v>
       </c>
       <c r="C94">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D94" t="str">
         <v>Male</v>
       </c>
       <c r="E94" t="str">
-        <v>carter.hill93@gmail.com</v>
+        <v>ethan.rodriguez60@hotmail.com</v>
       </c>
       <c r="F94" t="str">
-        <v>0404 349 309</v>
+        <v>0411 690 563</v>
       </c>
       <c r="G94" t="str">
-        <v>Newcastle</v>
+        <v>Townsville</v>
       </c>
       <c r="H94" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I94" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="M94" t="str">
+        <v>Hearing impaired - requires front row seating</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B95" t="str">
-        <v>Jayden Nguyen</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C95">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D95" t="str">
-        <v>Male</v>
+        <v>Not Specified</v>
       </c>
       <c r="E95" t="str">
-        <v>jayden.nguyen88@hotmail.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F95" t="str">
-        <v>0401 108 628</v>
+        <v>498086080</v>
       </c>
       <c r="G95" t="str">
-        <v>Hobart</v>
+        <v>Footscray</v>
       </c>
       <c r="H95" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="I95" t="str">
         <v>available</v>
+      </c>
+      <c r="J95" t="str">
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
+      </c>
+      <c r="K95" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L95" t="str">
+        <v>N</v>
+      </c>
+      <c r="M95" t="str">
+        <v>N/A</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>8956e289-91e9-4c15-bf2b-a13dee2fa476</v>
+        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
       </c>
       <c r="B96" t="str">
-        <v>Landon Wright</v>
+        <v>Stella Green</v>
       </c>
       <c r="C96">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="D96" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E96" t="str">
-        <v>landon.wright36@outlook.com</v>
+        <v>stella.green92@gmail.com</v>
       </c>
       <c r="F96" t="str">
-        <v>0402 415 597</v>
+        <v>0404 230 858</v>
       </c>
       <c r="G96" t="str">
-        <v>Cairns</v>
+        <v>Wollongong</v>
       </c>
       <c r="H96" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I96" t="str">
         <v>available</v>
+      </c>
+      <c r="J96" t="str">
+        <v>Everly Torres</v>
+      </c>
+      <c r="M96" t="str">
+        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B97" t="str">
-        <v>Luke Flores</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C97">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D97" t="str">
-        <v>Male</v>
+        <v>Not Specified</v>
       </c>
       <c r="E97" t="str">
-        <v>luke.flores39@hotmail.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F97" t="str">
-        <v>0403 225 544</v>
+        <v>498086080</v>
       </c>
       <c r="G97" t="str">
-        <v>Melbourne</v>
+        <v/>
       </c>
       <c r="H97" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="I97" t="str">
         <v>available</v>
+      </c>
+      <c r="J97" t="str">
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+      </c>
+      <c r="K97" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L97" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M97" t="str">
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
+        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
       </c>
       <c r="B98" t="str">
-        <v>Theodore Nelson</v>
+        <v>Victoria Torres</v>
       </c>
       <c r="C98">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D98" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E98" t="str">
-        <v>theodore.nelson79@gmail.com</v>
+        <v>victoria.torres48@outlook.com</v>
       </c>
       <c r="F98" t="str">
-        <v>0403 813 793</v>
+        <v>0411 539 271</v>
       </c>
       <c r="G98" t="str">
-        <v>Canberra</v>
+        <v>Geelong</v>
       </c>
       <c r="H98" t="str">
         <v>B</v>
@@ -3566,28 +3732,28 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
       </c>
       <c r="B99" t="str">
-        <v>Ethan Rodriguez</v>
+        <v>Samuel King</v>
       </c>
       <c r="C99">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D99" t="str">
         <v>Male</v>
       </c>
       <c r="E99" t="str">
-        <v>ethan.rodriguez60@hotmail.com</v>
+        <v>samuel.king24@yahoo.com</v>
       </c>
       <c r="F99" t="str">
-        <v>0411 690 563</v>
+        <v>0400 774 736</v>
       </c>
       <c r="G99" t="str">
-        <v>Townsville</v>
+        <v>Newcastle</v>
       </c>
       <c r="H99" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I99" t="str">
         <v>available</v>
@@ -3595,28 +3761,28 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>ecc70875-f282-4849-9e60-071edc278977</v>
+        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
       </c>
       <c r="B100" t="str">
-        <v>Noah White</v>
+        <v>Joshua Walker</v>
       </c>
       <c r="C100">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="D100" t="str">
         <v>Male</v>
       </c>
       <c r="E100" t="str">
-        <v>noah.white20@gmail.com</v>
+        <v>joshua.walker97@gmail.com</v>
       </c>
       <c r="F100" t="str">
-        <v>0410 565 594</v>
+        <v>0402 640 379</v>
       </c>
       <c r="G100" t="str">
-        <v>Adelaide</v>
+        <v>Darwin</v>
       </c>
       <c r="H100" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I100" t="str">
         <v>available</v>
@@ -3624,28 +3790,28 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
+        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
       </c>
       <c r="B101" t="str">
-        <v>Theodore Allen</v>
+        <v>Scarlett Wright</v>
       </c>
       <c r="C101">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D101" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E101" t="str">
-        <v>theodore.allen25@outlook.com</v>
+        <v>scarlett.wright68@outlook.com</v>
       </c>
       <c r="F101" t="str">
-        <v>0400 438 819</v>
+        <v>0412 487 763</v>
       </c>
       <c r="G101" t="str">
         <v>Newcastle</v>
       </c>
       <c r="H101" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I101" t="str">
         <v>available</v>
@@ -3653,28 +3819,28 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
+        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
       </c>
       <c r="B102" t="str">
-        <v>Joshua Clark</v>
+        <v>Liam Lewis</v>
       </c>
       <c r="C102">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D102" t="str">
         <v>Male</v>
       </c>
       <c r="E102" t="str">
-        <v>joshua.clark16@outlook.com</v>
+        <v>liam.lewis79@yahoo.com</v>
       </c>
       <c r="F102" t="str">
-        <v>0403 901 485</v>
+        <v>0404 203 198</v>
       </c>
       <c r="G102" t="str">
-        <v>Sydney</v>
+        <v>Hobart</v>
       </c>
       <c r="H102" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I102" t="str">
         <v>available</v>
@@ -3682,25 +3848,25 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
+        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
       </c>
       <c r="B103" t="str">
-        <v>Joshua Scott</v>
+        <v>Luke Flores</v>
       </c>
       <c r="C103">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D103" t="str">
         <v>Male</v>
       </c>
       <c r="E103" t="str">
-        <v>joshua.scott95@outlook.com</v>
+        <v>luke.flores39@hotmail.com</v>
       </c>
       <c r="F103" t="str">
-        <v>0410 137 561</v>
+        <v>0403 225 544</v>
       </c>
       <c r="G103" t="str">
-        <v>Canberra</v>
+        <v>Melbourne</v>
       </c>
       <c r="H103" t="str">
         <v>B</v>
@@ -3711,25 +3877,25 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
+        <v>8956e289-91e9-4c15-bf2b-a13dee2fa476</v>
       </c>
       <c r="B104" t="str">
-        <v>Liam Lewis</v>
+        <v>Landon Wright</v>
       </c>
       <c r="C104">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D104" t="str">
         <v>Male</v>
       </c>
       <c r="E104" t="str">
-        <v>liam.lewis79@yahoo.com</v>
+        <v>landon.wright36@outlook.com</v>
       </c>
       <c r="F104" t="str">
-        <v>0404 203 198</v>
+        <v>0402 415 597</v>
       </c>
       <c r="G104" t="str">
-        <v>Hobart</v>
+        <v>Cairns</v>
       </c>
       <c r="H104" t="str">
         <v>B+</v>
@@ -3747,6 +3913,522 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Block</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="F1" t="str">
+        <v>BookingEmailSent</v>
+      </c>
+      <c r="G1" t="str">
+        <v>ConfirmedRSVP</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>a634c290-4c9c-414a-93fc-745bd097e76d</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>ecc70875-f282-4849-9e60-071edc278977</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="str">
+        <v>A5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>b8c8e258-37be-4899-875e-6d388063ccde</v>
+      </c>
+      <c r="B3" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C3" t="str">
+        <v>7664257a-dce4-407a-8f24-692043d568be</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>45375cb0-bd1b-4b9a-a6a6-27fee2fb4945</v>
+      </c>
+      <c r="B4" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C4" t="str">
+        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>a616aafc-3ff8-4449-a8f9-1a4dbc9350d0</v>
+      </c>
+      <c r="B5" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>d5b88b57-aa91-49ce-afab-69ab3e297842</v>
+      </c>
+      <c r="B6" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C6" t="str">
+        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>40d2ebf0-17a6-485d-9dc1-2b1c6f764b92</v>
+      </c>
+      <c r="B7" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C7" t="str">
+        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>e860e9bf-0085-4cdd-a9d0-594335337f42</v>
+      </c>
+      <c r="B8" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C8" t="str">
+        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="str">
+        <v>A5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>231cd33c-26f8-47eb-abdb-18be9cb04e40</v>
+      </c>
+      <c r="B9" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C9" t="str">
+        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>373d1ffe-5ae4-49a1-938f-0247d30da633</v>
+      </c>
+      <c r="B10" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C10" t="str">
+        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>a18d0693-98ff-4e9e-848f-9d3411c9f601</v>
+      </c>
+      <c r="B11" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C11" t="str">
+        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>c0a18a7e-4e83-408c-9071-eb8eacc5af4b</v>
+      </c>
+      <c r="B12" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C12" t="str">
+        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>05863c6a-b5c7-4f02-9310-ed16f475fa5b</v>
+      </c>
+      <c r="B13" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C13" t="str">
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13" t="str">
+        <v>A5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>39179962-2dc4-430e-989a-8b933f871bc8</v>
+      </c>
+      <c r="B14" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C14" t="str">
+        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>8fea80c2-f010-418e-9912-3e1811738244</v>
+      </c>
+      <c r="B15" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C15" t="str">
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>ec5bdd9f-9a20-4c40-b36a-6b6c4bb850da</v>
+      </c>
+      <c r="B16" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C16" t="str">
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="str">
+        <v>B3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>47c2c439-7c97-4019-80fd-93fc83d7c8e6</v>
+      </c>
+      <c r="B17" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C17" t="str">
+        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17" t="str">
+        <v>B4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>55aae62f-a92f-49f5-a5a2-f0aba343014a</v>
+      </c>
+      <c r="B18" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C18" t="str">
+        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="str">
+        <v>B5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>eaacb9fd-9bff-4952-8551-663c60df9878</v>
+      </c>
+      <c r="B19" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C19" t="str">
+        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19" t="str">
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>190fda70-e765-41a5-9147-b1f36392b50d</v>
+      </c>
+      <c r="B20" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C20" t="str">
+        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" t="str">
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>7b5bf219-72c4-4e76-a04a-d00f276902e9</v>
+      </c>
+      <c r="B21" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C21" t="str">
+        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" t="str">
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>a18846fc-8b75-4224-90ca-0ac6b286ea5a</v>
+      </c>
+      <c r="B22" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C22" t="str">
+        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22" t="str">
+        <v>C4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>77f1ebcc-83e6-48b3-aeee-af901920079c</v>
+      </c>
+      <c r="B23" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C23" t="str">
+        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23" t="str">
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>a86ddb54-5d1b-4d80-940e-b1f381a6333f</v>
+      </c>
+      <c r="B24" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C24" t="str">
+        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" t="str">
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>abe65c79-379e-46ec-aded-2652f9e64961</v>
+      </c>
+      <c r="B25" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C25" t="str">
+        <v>8e115c7e-8033-4466-bcb9-07ea089eb4be</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>e46419c3-c90e-4432-a3bb-19dedad4bb04</v>
+      </c>
+      <c r="B26" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C26" t="str">
+        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>e2f751de-9d53-4fe5-8f08-756bfc12bb83</v>
+      </c>
+      <c r="B27" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C27" t="str">
+        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="E27" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>dadf3bea-2f2a-48bf-9e6e-7947f8313921</v>
+      </c>
+      <c r="B28" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C28" t="str">
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>2707752c-605e-4a31-871c-ece5c863b517</v>
+      </c>
+      <c r="B29" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C29" t="str">
+        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" t="str">
+        <v>A5</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H29"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3807,7 +4489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update contestant availability status and backup data
Modify the storage/backups/automatic-backup.json file to correct contestant availability statuses and update exportedAt timestamp.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 1538b186-6a53-4a6c-9609-fc2552a475b3
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/ywDH2YF
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -718,351 +718,348 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
       </c>
       <c r="B2" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Abigail Jackson</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D2" t="str">
-        <v>Not Specified</v>
+        <v>Female</v>
       </c>
       <c r="E2" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>abigail.jackson65@outlook.com</v>
       </c>
       <c r="F2" t="str">
-        <v>498086080</v>
+        <v>0411 824 257</v>
       </c>
       <c r="G2" t="str">
-        <v>Melbourne</v>
+        <v>Newcastle</v>
       </c>
       <c r="H2" t="str">
-        <v/>
+        <v>B+</v>
       </c>
       <c r="I2" t="str">
         <v>available</v>
-      </c>
-      <c r="J2" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
-      </c>
-      <c r="K2" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L2" t="str">
-        <v>N</v>
-      </c>
-      <c r="M2" t="str">
-        <v>N/A</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>8e115c7e-8033-4466-bcb9-07ea089eb4be</v>
       </c>
       <c r="B3" t="str">
-        <v>Caroline Taylor</v>
+        <v>Chloe Taylor</v>
       </c>
       <c r="C3">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D3" t="str">
         <v>Female</v>
       </c>
       <c r="E3" t="str">
-        <v>caroline.taylor54@outlook.com</v>
+        <v>chloe.taylor7@gmail.com</v>
       </c>
       <c r="F3" t="str">
-        <v>0402 864 601</v>
+        <v>0412 903 254</v>
       </c>
       <c r="G3" t="str">
-        <v>Darwin</v>
+        <v>Townsville</v>
       </c>
       <c r="H3" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I3" t="str">
         <v>available</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Hazel Mitchell</v>
-      </c>
-      <c r="M3" t="str">
-        <v>Arthritis - prefers aisle seating for easy exit</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>0dd7de5c-0409-45e3-84a5-5f2ffbd591d8</v>
+        <v>0a153155-dcf5-4d56-9ed1-8960501157f8</v>
       </c>
       <c r="B4" t="str">
-        <v>Harper Sanchez</v>
+        <v>Aurora Gonzalez</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D4" t="str">
         <v>Female</v>
       </c>
       <c r="E4" t="str">
-        <v>harper.sanchez76@gmail.com</v>
+        <v>aurora.gonzalez29@outlook.com</v>
       </c>
       <c r="F4" t="str">
-        <v>0411 422 972</v>
+        <v>0404 610 172</v>
       </c>
       <c r="G4" t="str">
-        <v>Geelong</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H4" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="I4" t="str">
         <v>available</v>
-      </c>
-      <c r="J4" t="str">
-        <v>Leah Scott</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>8e115c7e-8033-4466-bcb9-07ea089eb4be</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="B5" t="str">
-        <v>Chloe Taylor</v>
+        <v>Caroline Taylor</v>
       </c>
       <c r="C5">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D5" t="str">
         <v>Female</v>
       </c>
       <c r="E5" t="str">
-        <v>chloe.taylor7@gmail.com</v>
+        <v>caroline.taylor54@outlook.com</v>
       </c>
       <c r="F5" t="str">
-        <v>0412 903 254</v>
+        <v>0402 864 601</v>
       </c>
       <c r="G5" t="str">
-        <v>Townsville</v>
+        <v>Darwin</v>
       </c>
       <c r="H5" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I5" t="str">
         <v>assigned</v>
       </c>
+      <c r="J5" t="str">
+        <v>Hazel Mitchell</v>
+      </c>
+      <c r="M5" t="str">
+        <v>Arthritis - prefers aisle seating for easy exit</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>992418b2-3029-4752-9552-0aa886433657</v>
+        <v>0dd7de5c-0409-45e3-84a5-5f2ffbd591d8</v>
       </c>
       <c r="B6" t="str">
-        <v>Zoe Brown</v>
+        <v>Harper Sanchez</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D6" t="str">
         <v>Female</v>
       </c>
       <c r="E6" t="str">
-        <v>zoe.brown45@outlook.com</v>
+        <v>harper.sanchez76@gmail.com</v>
       </c>
       <c r="F6" t="str">
-        <v>0401 578 107</v>
+        <v>0411 422 972</v>
       </c>
       <c r="G6" t="str">
-        <v>Sydney</v>
+        <v>Geelong</v>
       </c>
       <c r="H6" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I6" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J6" t="str">
-        <v>Chloe Jones</v>
+        <v>Leah Scott</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B7" t="str">
-        <v>Paisley Lee</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C7">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="D7" t="str">
-        <v>Female</v>
+        <v>Not Specified</v>
       </c>
       <c r="E7" t="str">
-        <v>paisley.lee78@hotmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F7" t="str">
-        <v>0400 179 607</v>
+        <v>498086080</v>
       </c>
       <c r="G7" t="str">
-        <v>Ballarat</v>
+        <v>Melbourne</v>
       </c>
       <c r="H7" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="I7" t="str">
         <v>available</v>
       </c>
       <c r="J7" t="str">
-        <v>Aria Lopez</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
+      </c>
+      <c r="K7" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L7" t="str">
+        <v>N</v>
+      </c>
+      <c r="M7" t="str">
+        <v>N/A</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>992418b2-3029-4752-9552-0aa886433657</v>
       </c>
       <c r="B8" t="str">
-        <v>Ella Anderson</v>
+        <v>Zoe Brown</v>
       </c>
       <c r="C8">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D8" t="str">
         <v>Female</v>
       </c>
       <c r="E8" t="str">
-        <v>ella.anderson1@yahoo.com</v>
+        <v>zoe.brown45@outlook.com</v>
       </c>
       <c r="F8" t="str">
-        <v>0412 908 910</v>
+        <v>0401 578 107</v>
       </c>
       <c r="G8" t="str">
-        <v>Geelong</v>
+        <v>Sydney</v>
       </c>
       <c r="H8" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I8" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J8" t="str">
-        <v>Isabella Brown</v>
+        <v>Chloe Jones</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>210066e7-58e9-4ebb-a504-dfbf383961b5</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="B9" t="str">
-        <v>Grace Scott</v>
+        <v>Paisley Lee</v>
       </c>
       <c r="C9">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D9" t="str">
         <v>Female</v>
       </c>
       <c r="E9" t="str">
-        <v>grace.scott94@hotmail.com</v>
+        <v>paisley.lee78@hotmail.com</v>
       </c>
       <c r="F9" t="str">
-        <v>0410 377 869</v>
+        <v>0400 179 607</v>
       </c>
       <c r="G9" t="str">
-        <v>Toowoomba</v>
+        <v>Ballarat</v>
       </c>
       <c r="H9" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I9" t="str">
         <v>available</v>
       </c>
       <c r="J9" t="str">
-        <v>Audrey Smith</v>
+        <v>Aria Lopez</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="B10" t="str">
-        <v>Abigail Jackson</v>
+        <v>Ella Anderson</v>
       </c>
       <c r="C10">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" t="str">
         <v>Female</v>
       </c>
       <c r="E10" t="str">
-        <v>abigail.jackson65@outlook.com</v>
+        <v>ella.anderson1@yahoo.com</v>
       </c>
       <c r="F10" t="str">
-        <v>0411 824 257</v>
+        <v>0412 908 910</v>
       </c>
       <c r="G10" t="str">
-        <v>Newcastle</v>
+        <v>Geelong</v>
       </c>
       <c r="H10" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I10" t="str">
         <v>available</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Isabella Brown</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
+        <v>210066e7-58e9-4ebb-a504-dfbf383961b5</v>
       </c>
       <c r="B11" t="str">
-        <v>Aria Scott</v>
+        <v>Grace Scott</v>
       </c>
       <c r="C11">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D11" t="str">
         <v>Female</v>
       </c>
       <c r="E11" t="str">
-        <v>aria.scott42@outlook.com</v>
+        <v>grace.scott94@hotmail.com</v>
       </c>
       <c r="F11" t="str">
-        <v>0401 330 548</v>
+        <v>0410 377 869</v>
       </c>
       <c r="G11" t="str">
-        <v>Hobart</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H11" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I11" t="str">
         <v>available</v>
       </c>
       <c r="J11" t="str">
-        <v>Maya Hernandez</v>
+        <v>Audrey Smith</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
       </c>
       <c r="B12" t="str">
-        <v>Audrey Thomas</v>
+        <v>Aria Scott</v>
       </c>
       <c r="C12">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="D12" t="str">
         <v>Female</v>
       </c>
       <c r="E12" t="str">
-        <v>audrey.thomas38@gmail.com</v>
+        <v>aria.scott42@outlook.com</v>
       </c>
       <c r="F12" t="str">
-        <v>0400 437 270</v>
+        <v>0401 330 548</v>
       </c>
       <c r="G12" t="str">
-        <v>Perth</v>
+        <v>Hobart</v>
       </c>
       <c r="H12" t="str">
         <v>C</v>
@@ -1071,132 +1068,135 @@
         <v>available</v>
       </c>
       <c r="J12" t="str">
-        <v>Hannah Torres</v>
+        <v>Maya Hernandez</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2c188398-79a8-4bf6-b740-1ad9d535662e</v>
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
       </c>
       <c r="B13" t="str">
-        <v>Everly Torres</v>
+        <v>Audrey Thomas</v>
       </c>
       <c r="C13">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D13" t="str">
         <v>Female</v>
       </c>
       <c r="E13" t="str">
-        <v>everly.torres12@gmail.com</v>
+        <v>audrey.thomas38@gmail.com</v>
       </c>
       <c r="F13" t="str">
-        <v>0412 804 179</v>
+        <v>0400 437 270</v>
       </c>
       <c r="G13" t="str">
-        <v>Sydney</v>
+        <v>Perth</v>
       </c>
       <c r="H13" t="str">
-        <v>A+</v>
+        <v>C</v>
       </c>
       <c r="I13" t="str">
         <v>available</v>
       </c>
       <c r="J13" t="str">
-        <v>Stella Green</v>
+        <v>Hannah Torres</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>2c188398-79a8-4bf6-b740-1ad9d535662e</v>
       </c>
       <c r="B14" t="str">
-        <v>Hannah Torres</v>
+        <v>Everly Torres</v>
       </c>
       <c r="C14">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" t="str">
         <v>Female</v>
       </c>
       <c r="E14" t="str">
-        <v>hannah.torres86@yahoo.com</v>
+        <v>everly.torres12@gmail.com</v>
       </c>
       <c r="F14" t="str">
-        <v>0402 688 409</v>
+        <v>0412 804 179</v>
       </c>
       <c r="G14" t="str">
-        <v>Wollongong</v>
+        <v>Sydney</v>
       </c>
       <c r="H14" t="str">
-        <v>B+</v>
+        <v>A+</v>
       </c>
       <c r="I14" t="str">
         <v>available</v>
       </c>
       <c r="J14" t="str">
-        <v>Audrey Thomas</v>
+        <v>Stella Green</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
       </c>
       <c r="B15" t="str">
-        <v>Evelyn Sanchez</v>
+        <v>Hannah Torres</v>
       </c>
       <c r="C15">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D15" t="str">
         <v>Female</v>
       </c>
       <c r="E15" t="str">
-        <v>evelyn.sanchez9@gmail.com</v>
+        <v>hannah.torres86@yahoo.com</v>
       </c>
       <c r="F15" t="str">
-        <v>0404 119 469</v>
+        <v>0402 688 409</v>
       </c>
       <c r="G15" t="str">
-        <v>Gold Coast</v>
+        <v>Wollongong</v>
       </c>
       <c r="H15" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I15" t="str">
         <v>available</v>
       </c>
       <c r="J15" t="str">
-        <v>Chloe Flores</v>
+        <v>Audrey Thomas</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
+        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
       </c>
       <c r="B16" t="str">
-        <v>Stella Martinez</v>
+        <v>Evelyn Sanchez</v>
       </c>
       <c r="C16">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D16" t="str">
         <v>Female</v>
       </c>
       <c r="E16" t="str">
-        <v>stella.martinez75@gmail.com</v>
+        <v>evelyn.sanchez9@gmail.com</v>
       </c>
       <c r="F16" t="str">
-        <v>0404 227 272</v>
+        <v>0404 119 469</v>
       </c>
       <c r="G16" t="str">
-        <v>Ballarat</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H16" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I16" t="str">
-        <v>assigned</v>
+        <v>available</v>
+      </c>
+      <c r="J16" t="str">
+        <v>Chloe Flores</v>
       </c>
     </row>
     <row r="17">
@@ -1396,28 +1396,28 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>0a153155-dcf5-4d56-9ed1-8960501157f8</v>
+        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
       </c>
       <c r="B23" t="str">
-        <v>Aurora Gonzalez</v>
+        <v>Stella Martinez</v>
       </c>
       <c r="C23">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D23" t="str">
         <v>Female</v>
       </c>
       <c r="E23" t="str">
-        <v>aurora.gonzalez29@outlook.com</v>
+        <v>stella.martinez75@gmail.com</v>
       </c>
       <c r="F23" t="str">
-        <v>0404 610 172</v>
+        <v>0404 227 272</v>
       </c>
       <c r="G23" t="str">
-        <v>Toowoomba</v>
+        <v>Ballarat</v>
       </c>
       <c r="H23" t="str">
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="I23" t="str">
         <v>available</v>
@@ -1748,31 +1748,31 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
+        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
       </c>
       <c r="B34" t="str">
-        <v>Hunter Jackson</v>
+        <v>Jackson Young</v>
       </c>
       <c r="C34">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D34" t="str">
         <v>Male</v>
       </c>
       <c r="E34" t="str">
-        <v>hunter.jackson50@outlook.com</v>
+        <v>jackson.young79@yahoo.com</v>
       </c>
       <c r="F34" t="str">
-        <v>0404 841 788</v>
+        <v>0412 940 993</v>
       </c>
       <c r="G34" t="str">
-        <v>Townsville</v>
+        <v>Ballarat</v>
       </c>
       <c r="H34" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I34" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="35">
@@ -1809,25 +1809,25 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
+        <v>c1783cdf-a656-46b4-9331-4d9d18d40b51</v>
       </c>
       <c r="B36" t="str">
-        <v>Ryan Williams</v>
+        <v>Aurora Walker</v>
       </c>
       <c r="C36">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="D36" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E36" t="str">
-        <v>ryan.williams82@hotmail.com</v>
+        <v>aurora.walker1@outlook.com</v>
       </c>
       <c r="F36" t="str">
-        <v>0401 450 673</v>
+        <v>0403 522 404</v>
       </c>
       <c r="G36" t="str">
-        <v>Perth</v>
+        <v>Darwin</v>
       </c>
       <c r="H36" t="str">
         <v>B+</v>
@@ -1835,31 +1835,34 @@
       <c r="I36" t="str">
         <v>available</v>
       </c>
+      <c r="M36" t="str">
+        <v>Vision impaired - needs assistance</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>32ffeaf9-5f22-4db7-a70b-cbaab834db0d</v>
+        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
       </c>
       <c r="B37" t="str">
-        <v>Isabella Hill</v>
+        <v>Mason Hill</v>
       </c>
       <c r="C37">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D37" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E37" t="str">
-        <v>isabella.hill77@hotmail.com</v>
+        <v>mason.hill27@outlook.com</v>
       </c>
       <c r="F37" t="str">
-        <v>0412 663 356</v>
+        <v>0410 682 884</v>
       </c>
       <c r="G37" t="str">
-        <v>Darwin</v>
+        <v>Canberra</v>
       </c>
       <c r="H37" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I37" t="str">
         <v>available</v>
@@ -1867,31 +1870,31 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
+        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
       </c>
       <c r="B38" t="str">
-        <v>Genesis Jones</v>
+        <v>Nathan Allen</v>
       </c>
       <c r="C38">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D38" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E38" t="str">
-        <v>genesis.jones50@yahoo.com</v>
+        <v>nathan.allen87@outlook.com</v>
       </c>
       <c r="F38" t="str">
-        <v>0404 967 604</v>
+        <v>0403 587 263</v>
       </c>
       <c r="G38" t="str">
-        <v>Sydney</v>
+        <v>Adelaide</v>
       </c>
       <c r="H38" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I38" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="39">
@@ -1960,63 +1963,63 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
+        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
       </c>
       <c r="B41" t="str">
-        <v>Andrew Garcia</v>
+        <v>Oliver Rivera</v>
       </c>
       <c r="C41">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D41" t="str">
         <v>Male</v>
       </c>
       <c r="E41" t="str">
-        <v>andrew.garcia26@hotmail.com</v>
+        <v>oliver.rivera58@outlook.com</v>
       </c>
       <c r="F41" t="str">
-        <v>0400 450 222</v>
+        <v>0412 991 121</v>
       </c>
       <c r="G41" t="str">
-        <v>Darwin</v>
+        <v>Canberra</v>
       </c>
       <c r="H41" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I41" t="str">
         <v>available</v>
       </c>
       <c r="M41" t="str">
-        <v>Limited mobility - prefers ground floor seating</v>
+        <v>Requires wheelchair access</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
+        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
       </c>
       <c r="B42" t="str">
-        <v>Noah Hernandez</v>
+        <v>Evelyn Clark</v>
       </c>
       <c r="C42">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D42" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E42" t="str">
-        <v>noah.hernandez9@hotmail.com</v>
+        <v>evelyn.clark47@outlook.com</v>
       </c>
       <c r="F42" t="str">
-        <v>0404 855 230</v>
+        <v>0410 941 656</v>
       </c>
       <c r="G42" t="str">
-        <v>Cairns</v>
+        <v>Hobart</v>
       </c>
       <c r="H42" t="str">
         <v>C</v>
       </c>
       <c r="I42" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="43">
@@ -2053,28 +2056,28 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
+        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
       </c>
       <c r="B44" t="str">
-        <v>Nathan Allen</v>
+        <v>Hunter Jackson</v>
       </c>
       <c r="C44">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D44" t="str">
         <v>Male</v>
       </c>
       <c r="E44" t="str">
-        <v>nathan.allen87@outlook.com</v>
+        <v>hunter.jackson50@outlook.com</v>
       </c>
       <c r="F44" t="str">
-        <v>0403 587 263</v>
+        <v>0404 841 788</v>
       </c>
       <c r="G44" t="str">
-        <v>Adelaide</v>
+        <v>Townsville</v>
       </c>
       <c r="H44" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I44" t="str">
         <v>available</v>
@@ -2082,28 +2085,28 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
       </c>
       <c r="B45" t="str">
-        <v>Jackson Young</v>
+        <v>Carter Harris</v>
       </c>
       <c r="C45">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D45" t="str">
         <v>Male</v>
       </c>
       <c r="E45" t="str">
-        <v>jackson.young79@yahoo.com</v>
+        <v>carter.harris82@yahoo.com</v>
       </c>
       <c r="F45" t="str">
-        <v>0412 940 993</v>
+        <v>0412 175 744</v>
       </c>
       <c r="G45" t="str">
-        <v>Ballarat</v>
+        <v>Geelong</v>
       </c>
       <c r="H45" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I45" t="str">
         <v>available</v>
@@ -2143,28 +2146,28 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
+        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
       </c>
       <c r="B47" t="str">
-        <v>Cameron Lee</v>
+        <v>Noah Hernandez</v>
       </c>
       <c r="C47">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D47" t="str">
         <v>Male</v>
       </c>
       <c r="E47" t="str">
-        <v>cameron.lee78@yahoo.com</v>
+        <v>noah.hernandez9@hotmail.com</v>
       </c>
       <c r="F47" t="str">
-        <v>0404 821 708</v>
+        <v>0404 855 230</v>
       </c>
       <c r="G47" t="str">
         <v>Cairns</v>
       </c>
       <c r="H47" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I47" t="str">
         <v>available</v>
@@ -2172,57 +2175,57 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>c1783cdf-a656-46b4-9331-4d9d18d40b51</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="B48" t="str">
-        <v>Aurora Walker</v>
+        <v>Isabella Brown</v>
       </c>
       <c r="C48">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D48" t="str">
         <v>Female</v>
       </c>
       <c r="E48" t="str">
-        <v>aurora.walker1@outlook.com</v>
+        <v>isabella.brown43@outlook.com</v>
       </c>
       <c r="F48" t="str">
-        <v>0403 522 404</v>
+        <v>0403 771 690</v>
       </c>
       <c r="G48" t="str">
         <v>Darwin</v>
       </c>
       <c r="H48" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I48" t="str">
         <v>available</v>
       </c>
-      <c r="M48" t="str">
-        <v>Vision impaired - needs assistance</v>
+      <c r="J48" t="str">
+        <v>Ella Anderson</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>182bd5d2-7f68-4c83-b156-e80856f3b6b7</v>
+        <v>0faec83d-7c29-4269-bf33-391ef02d60e4</v>
       </c>
       <c r="B49" t="str">
-        <v>Mason Nelson</v>
+        <v>Anna White</v>
       </c>
       <c r="C49">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D49" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E49" t="str">
-        <v>mason.nelson14@hotmail.com</v>
+        <v>anna.white24@yahoo.com</v>
       </c>
       <c r="F49" t="str">
-        <v>0403 485 650</v>
+        <v>0400 132 564</v>
       </c>
       <c r="G49" t="str">
-        <v>Canberra</v>
+        <v>Adelaide</v>
       </c>
       <c r="H49" t="str">
         <v>B+</v>
@@ -2233,60 +2236,57 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
+        <v>3d2128a1-336f-41e1-973b-b5dd54d90b19</v>
       </c>
       <c r="B50" t="str">
-        <v>Oliver Rivera</v>
+        <v>Nova Brown</v>
       </c>
       <c r="C50">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D50" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E50" t="str">
-        <v>oliver.rivera58@outlook.com</v>
+        <v>nova.brown80@outlook.com</v>
       </c>
       <c r="F50" t="str">
-        <v>0412 991 121</v>
+        <v>0411 154 614</v>
       </c>
       <c r="G50" t="str">
-        <v>Canberra</v>
+        <v>Ballarat</v>
       </c>
       <c r="H50" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="I50" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="M50" t="str">
-        <v>Requires wheelchair access</v>
+        <v>available</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>3d2128a1-336f-41e1-973b-b5dd54d90b19</v>
+        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
       </c>
       <c r="B51" t="str">
-        <v>Nova Brown</v>
+        <v>Stella Hall</v>
       </c>
       <c r="C51">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D51" t="str">
         <v>Female</v>
       </c>
       <c r="E51" t="str">
-        <v>nova.brown80@outlook.com</v>
+        <v>stella.hall72@gmail.com</v>
       </c>
       <c r="F51" t="str">
-        <v>0411 154 614</v>
+        <v>0410 133 818</v>
       </c>
       <c r="G51" t="str">
-        <v>Ballarat</v>
+        <v>Wollongong</v>
       </c>
       <c r="H51" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I51" t="str">
         <v>available</v>
@@ -2294,25 +2294,25 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>0faec83d-7c29-4269-bf33-391ef02d60e4</v>
+        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
       </c>
       <c r="B52" t="str">
-        <v>Anna White</v>
+        <v>Cameron Lee</v>
       </c>
       <c r="C52">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D52" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E52" t="str">
-        <v>anna.white24@yahoo.com</v>
+        <v>cameron.lee78@yahoo.com</v>
       </c>
       <c r="F52" t="str">
-        <v>0400 132 564</v>
+        <v>0404 821 708</v>
       </c>
       <c r="G52" t="str">
-        <v>Adelaide</v>
+        <v>Cairns</v>
       </c>
       <c r="H52" t="str">
         <v>B+</v>
@@ -2323,211 +2323,211 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
       </c>
       <c r="B53" t="str">
-        <v>Carter Harris</v>
+        <v>Ryan Williams</v>
       </c>
       <c r="C53">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D53" t="str">
         <v>Male</v>
       </c>
       <c r="E53" t="str">
-        <v>carter.harris82@yahoo.com</v>
+        <v>ryan.williams82@hotmail.com</v>
       </c>
       <c r="F53" t="str">
-        <v>0412 175 744</v>
+        <v>0401 450 673</v>
       </c>
       <c r="G53" t="str">
-        <v>Geelong</v>
+        <v>Perth</v>
       </c>
       <c r="H53" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I53" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="B54" t="str">
-        <v>Isabella Brown</v>
+        <v>Aria Lopez</v>
       </c>
       <c r="C54">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D54" t="str">
         <v>Female</v>
       </c>
       <c r="E54" t="str">
-        <v>isabella.brown43@outlook.com</v>
+        <v>aria.lopez55@hotmail.com</v>
       </c>
       <c r="F54" t="str">
-        <v>0403 771 690</v>
+        <v>0404 812 491</v>
       </c>
       <c r="G54" t="str">
-        <v>Darwin</v>
+        <v>Sydney</v>
       </c>
       <c r="H54" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I54" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J54" t="str">
-        <v>Ella Anderson</v>
+        <v>Paisley Lee</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
+        <v>f1466859-7323-4893-a189-a0ce994068ba</v>
       </c>
       <c r="B55" t="str">
-        <v>Stella Hall</v>
+        <v>Anthony Thompson</v>
       </c>
       <c r="C55">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D55" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E55" t="str">
-        <v>stella.hall72@gmail.com</v>
+        <v>anthony.thompson29@yahoo.com</v>
       </c>
       <c r="F55" t="str">
-        <v>0410 133 818</v>
+        <v>0412 442 587</v>
       </c>
       <c r="G55" t="str">
-        <v>Wollongong</v>
+        <v>Townsville</v>
       </c>
       <c r="H55" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I55" t="str">
-        <v>assigned</v>
+        <v>available</v>
+      </c>
+      <c r="M55" t="str">
+        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
       </c>
       <c r="B56" t="str">
-        <v>Aria Lopez</v>
+        <v>Andrew Garcia</v>
       </c>
       <c r="C56">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D56" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E56" t="str">
-        <v>aria.lopez55@hotmail.com</v>
+        <v>andrew.garcia26@hotmail.com</v>
       </c>
       <c r="F56" t="str">
-        <v>0404 812 491</v>
+        <v>0400 450 222</v>
       </c>
       <c r="G56" t="str">
-        <v>Sydney</v>
+        <v>Darwin</v>
       </c>
       <c r="H56" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I56" t="str">
         <v>available</v>
       </c>
-      <c r="J56" t="str">
-        <v>Paisley Lee</v>
+      <c r="M56" t="str">
+        <v>Limited mobility - prefers ground floor seating</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
+        <v>32ffeaf9-5f22-4db7-a70b-cbaab834db0d</v>
       </c>
       <c r="B57" t="str">
-        <v>Evelyn Clark</v>
+        <v>Isabella Hill</v>
       </c>
       <c r="C57">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D57" t="str">
         <v>Female</v>
       </c>
       <c r="E57" t="str">
-        <v>evelyn.clark47@outlook.com</v>
+        <v>isabella.hill77@hotmail.com</v>
       </c>
       <c r="F57" t="str">
-        <v>0410 941 656</v>
+        <v>0412 663 356</v>
       </c>
       <c r="G57" t="str">
-        <v>Hobart</v>
+        <v>Darwin</v>
       </c>
       <c r="H57" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I57" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>f1466859-7323-4893-a189-a0ce994068ba</v>
+        <v>182bd5d2-7f68-4c83-b156-e80856f3b6b7</v>
       </c>
       <c r="B58" t="str">
-        <v>Anthony Thompson</v>
+        <v>Mason Nelson</v>
       </c>
       <c r="C58">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D58" t="str">
         <v>Male</v>
       </c>
       <c r="E58" t="str">
-        <v>anthony.thompson29@yahoo.com</v>
+        <v>mason.nelson14@hotmail.com</v>
       </c>
       <c r="F58" t="str">
-        <v>0412 442 587</v>
+        <v>0403 485 650</v>
       </c>
       <c r="G58" t="str">
-        <v>Townsville</v>
+        <v>Canberra</v>
       </c>
       <c r="H58" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I58" t="str">
         <v>available</v>
-      </c>
-      <c r="M58" t="str">
-        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
+        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
       </c>
       <c r="B59" t="str">
-        <v>Mason Hill</v>
+        <v>Genesis Jones</v>
       </c>
       <c r="C59">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D59" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E59" t="str">
-        <v>mason.hill27@outlook.com</v>
+        <v>genesis.jones50@yahoo.com</v>
       </c>
       <c r="F59" t="str">
-        <v>0410 682 884</v>
+        <v>0404 967 604</v>
       </c>
       <c r="G59" t="str">
-        <v>Canberra</v>
+        <v>Sydney</v>
       </c>
       <c r="H59" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I59" t="str">
         <v>available</v>
@@ -2535,28 +2535,28 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
+        <v>34685ff7-6e85-4bbd-b546-77cfe11d7f7d</v>
       </c>
       <c r="B60" t="str">
-        <v>Scarlett Lopez</v>
+        <v>Grace Walker</v>
       </c>
       <c r="C60">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D60" t="str">
         <v>Female</v>
       </c>
       <c r="E60" t="str">
-        <v>scarlett.lopez53@yahoo.com</v>
+        <v>grace.walker52@hotmail.com</v>
       </c>
       <c r="F60" t="str">
-        <v>0400 509 641</v>
+        <v>0412 754 780</v>
       </c>
       <c r="G60" t="str">
-        <v>Sydney</v>
+        <v>Canberra</v>
       </c>
       <c r="H60" t="str">
-        <v>B+</v>
+        <v>A+</v>
       </c>
       <c r="I60" t="str">
         <v>available</v>
@@ -2564,57 +2564,60 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>34685ff7-6e85-4bbd-b546-77cfe11d7f7d</v>
+        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
       </c>
       <c r="B61" t="str">
-        <v>Grace Walker</v>
+        <v>Aurora Williams</v>
       </c>
       <c r="C61">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="D61" t="str">
         <v>Female</v>
       </c>
       <c r="E61" t="str">
-        <v>grace.walker52@hotmail.com</v>
+        <v>aurora.williams76@outlook.com</v>
       </c>
       <c r="F61" t="str">
-        <v>0412 754 780</v>
+        <v>0401 416 170</v>
       </c>
       <c r="G61" t="str">
-        <v>Canberra</v>
+        <v>Darwin</v>
       </c>
       <c r="H61" t="str">
-        <v>A+</v>
+        <v>C</v>
       </c>
       <c r="I61" t="str">
         <v>available</v>
+      </c>
+      <c r="M61" t="str">
+        <v>Uses walking cane</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>ee7f9d33-09d6-417b-a45f-3e6554489f5b</v>
+        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
       </c>
       <c r="B62" t="str">
-        <v>Dylan Miller</v>
+        <v>Christian Rivera</v>
       </c>
       <c r="C62">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D62" t="str">
         <v>Male</v>
       </c>
       <c r="E62" t="str">
-        <v>dylan.miller23@hotmail.com</v>
+        <v>christian.rivera86@hotmail.com</v>
       </c>
       <c r="F62" t="str">
-        <v>0402 417 876</v>
+        <v>0400 135 743</v>
       </c>
       <c r="G62" t="str">
-        <v>Melbourne</v>
+        <v>Adelaide</v>
       </c>
       <c r="H62" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I62" t="str">
         <v>available</v>
@@ -2622,28 +2625,28 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
+        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
       </c>
       <c r="B63" t="str">
-        <v>Christian Rivera</v>
+        <v>Joshua Clark</v>
       </c>
       <c r="C63">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="D63" t="str">
         <v>Male</v>
       </c>
       <c r="E63" t="str">
-        <v>christian.rivera86@hotmail.com</v>
+        <v>joshua.clark16@outlook.com</v>
       </c>
       <c r="F63" t="str">
-        <v>0400 135 743</v>
+        <v>0403 901 485</v>
       </c>
       <c r="G63" t="str">
-        <v>Adelaide</v>
+        <v>Sydney</v>
       </c>
       <c r="H63" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I63" t="str">
         <v>available</v>
@@ -2651,28 +2654,28 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>5a6b21ec-9fac-4adc-b5ab-bcad20d0eca4</v>
+        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
       </c>
       <c r="B64" t="str">
-        <v>Hunter Harris</v>
+        <v>Ryan Lewis</v>
       </c>
       <c r="C64">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D64" t="str">
         <v>Male</v>
       </c>
       <c r="E64" t="str">
-        <v>hunter.harris1@gmail.com</v>
+        <v>ryan.lewis85@yahoo.com</v>
       </c>
       <c r="F64" t="str">
-        <v>0404 782 485</v>
+        <v>0400 187 811</v>
       </c>
       <c r="G64" t="str">
-        <v>Gold Coast</v>
+        <v>Canberra</v>
       </c>
       <c r="H64" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I64" t="str">
         <v>available</v>
@@ -2680,144 +2683,147 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
+        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
       </c>
       <c r="B65" t="str">
-        <v>Joshua Carter</v>
+        <v>Joshua Scott</v>
       </c>
       <c r="C65">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D65" t="str">
         <v>Male</v>
       </c>
       <c r="E65" t="str">
-        <v>joshua.carter41@hotmail.com</v>
+        <v>joshua.scott95@outlook.com</v>
       </c>
       <c r="F65" t="str">
-        <v>0404 538 442</v>
+        <v>0410 137 561</v>
       </c>
       <c r="G65" t="str">
-        <v>Wollongong</v>
+        <v>Canberra</v>
       </c>
       <c r="H65" t="str">
         <v>B</v>
       </c>
       <c r="I65" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
+        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
       </c>
       <c r="B66" t="str">
-        <v>Lucas Thomas</v>
+        <v>Theodore Allen</v>
       </c>
       <c r="C66">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D66" t="str">
         <v>Male</v>
       </c>
       <c r="E66" t="str">
-        <v>lucas.thomas30@yahoo.com</v>
+        <v>theodore.allen25@outlook.com</v>
       </c>
       <c r="F66" t="str">
-        <v>0412 527 117</v>
+        <v>0400 438 819</v>
       </c>
       <c r="G66" t="str">
-        <v>Brisbane</v>
+        <v>Newcastle</v>
       </c>
       <c r="H66" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I66" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
+        <v>ecc70875-f282-4849-9e60-071edc278977</v>
       </c>
       <c r="B67" t="str">
-        <v>Julian Rivera</v>
+        <v>Noah White</v>
       </c>
       <c r="C67">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="D67" t="str">
         <v>Male</v>
       </c>
       <c r="E67" t="str">
-        <v>julian.rivera31@outlook.com</v>
+        <v>noah.white20@gmail.com</v>
       </c>
       <c r="F67" t="str">
-        <v>0401 414 502</v>
+        <v>0410 565 594</v>
       </c>
       <c r="G67" t="str">
-        <v>Perth</v>
+        <v>Adelaide</v>
       </c>
       <c r="H67" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I67" t="str">
         <v>available</v>
+      </c>
+      <c r="M67" t="str">
+        <v>Requires wheelchair access</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
+        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
       </c>
       <c r="B68" t="str">
-        <v>Joshua Jones</v>
+        <v>Jayden Nguyen</v>
       </c>
       <c r="C68">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="D68" t="str">
         <v>Male</v>
       </c>
       <c r="E68" t="str">
-        <v>joshua.jones82@yahoo.com</v>
+        <v>jayden.nguyen88@hotmail.com</v>
       </c>
       <c r="F68" t="str">
-        <v>0400 652 840</v>
+        <v>0401 108 628</v>
       </c>
       <c r="G68" t="str">
-        <v>Toowoomba</v>
+        <v>Hobart</v>
       </c>
       <c r="H68" t="str">
         <v>B</v>
       </c>
       <c r="I68" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
+        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
       </c>
       <c r="B69" t="str">
-        <v>Ryan Lewis</v>
+        <v>Carter Hill</v>
       </c>
       <c r="C69">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D69" t="str">
         <v>Male</v>
       </c>
       <c r="E69" t="str">
-        <v>ryan.lewis85@yahoo.com</v>
+        <v>carter.hill93@gmail.com</v>
       </c>
       <c r="F69" t="str">
-        <v>0400 187 811</v>
+        <v>0404 349 309</v>
       </c>
       <c r="G69" t="str">
-        <v>Canberra</v>
+        <v>Newcastle</v>
       </c>
       <c r="H69" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I69" t="str">
         <v>available</v>
@@ -2825,321 +2831,321 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
+        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
       </c>
       <c r="B70" t="str">
-        <v>Carter Hill</v>
+        <v>Aria Nguyen</v>
       </c>
       <c r="C70">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D70" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E70" t="str">
-        <v>carter.hill93@gmail.com</v>
+        <v>aria.nguyen36@gmail.com</v>
       </c>
       <c r="F70" t="str">
-        <v>0404 349 309</v>
+        <v>0401 618 716</v>
       </c>
       <c r="G70" t="str">
-        <v>Newcastle</v>
+        <v>Sydney</v>
       </c>
       <c r="H70" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I70" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
+        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
       </c>
       <c r="B71" t="str">
-        <v>Nora Mitchell</v>
+        <v>Joshua Jones</v>
       </c>
       <c r="C71">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D71" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E71" t="str">
-        <v>nora.mitchell66@outlook.com</v>
+        <v>joshua.jones82@yahoo.com</v>
       </c>
       <c r="F71" t="str">
-        <v>0412 196 419</v>
+        <v>0400 652 840</v>
       </c>
       <c r="G71" t="str">
-        <v>Adelaide</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H71" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I71" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
+        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
       </c>
       <c r="B72" t="str">
-        <v>Abigail Williams</v>
+        <v>Ethan Taylor</v>
       </c>
       <c r="C72">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="D72" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E72" t="str">
-        <v>abigail.williams45@yahoo.com</v>
+        <v>ethan.taylor22@yahoo.com</v>
       </c>
       <c r="F72" t="str">
-        <v>0403 497 445</v>
+        <v>0410 363 173</v>
       </c>
       <c r="G72" t="str">
-        <v>Toowoomba</v>
+        <v>Adelaide</v>
       </c>
       <c r="H72" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I72" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>ecc70875-f282-4849-9e60-071edc278977</v>
+        <v>da40ad70-95be-413c-b0f1-d089ef285cc8</v>
       </c>
       <c r="B73" t="str">
-        <v>Noah White</v>
+        <v>Emily Smith</v>
       </c>
       <c r="C73">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D73" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E73" t="str">
-        <v>noah.white20@gmail.com</v>
+        <v>emily.smith56@hotmail.com</v>
       </c>
       <c r="F73" t="str">
-        <v>0410 565 594</v>
+        <v>0410 101 780</v>
       </c>
       <c r="G73" t="str">
-        <v>Adelaide</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H73" t="str">
-        <v>A</v>
+        <v>A+</v>
       </c>
       <c r="I73" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="M73" t="str">
-        <v>Requires wheelchair access</v>
+        <v>Limited mobility - prefers ground floor seating</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
+        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
       </c>
       <c r="B74" t="str">
-        <v>Joshua Clark</v>
+        <v>Emily Johnson</v>
       </c>
       <c r="C74">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D74" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E74" t="str">
-        <v>joshua.clark16@outlook.com</v>
+        <v>emily.johnson58@hotmail.com</v>
       </c>
       <c r="F74" t="str">
-        <v>0403 901 485</v>
+        <v>0412 663 939</v>
       </c>
       <c r="G74" t="str">
-        <v>Sydney</v>
+        <v>Perth</v>
       </c>
       <c r="H74" t="str">
         <v>B</v>
       </c>
       <c r="I74" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>da40ad70-95be-413c-b0f1-d089ef285cc8</v>
+        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
       </c>
       <c r="B75" t="str">
-        <v>Emily Smith</v>
+        <v>Joshua Carter</v>
       </c>
       <c r="C75">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="D75" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E75" t="str">
-        <v>emily.smith56@hotmail.com</v>
+        <v>joshua.carter41@hotmail.com</v>
       </c>
       <c r="F75" t="str">
-        <v>0410 101 780</v>
+        <v>0404 538 442</v>
       </c>
       <c r="G75" t="str">
-        <v>Toowoomba</v>
+        <v>Wollongong</v>
       </c>
       <c r="H75" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I75" t="str">
         <v>available</v>
-      </c>
-      <c r="M75" t="str">
-        <v>Limited mobility - prefers ground floor seating</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
+        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
       </c>
       <c r="B76" t="str">
-        <v>Joshua Scott</v>
+        <v>Charles Torres</v>
       </c>
       <c r="C76">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D76" t="str">
         <v>Male</v>
       </c>
       <c r="E76" t="str">
-        <v>joshua.scott95@outlook.com</v>
+        <v>charles.torres98@outlook.com</v>
       </c>
       <c r="F76" t="str">
-        <v>0410 137 561</v>
+        <v>0401 744 176</v>
       </c>
       <c r="G76" t="str">
-        <v>Canberra</v>
+        <v>Wollongong</v>
       </c>
       <c r="H76" t="str">
         <v>B</v>
       </c>
       <c r="I76" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
+        <v>6591420b-4762-4d90-b738-8a5b70458c40</v>
       </c>
       <c r="B77" t="str">
-        <v>Aria Nguyen</v>
+        <v>Aurora Hill</v>
       </c>
       <c r="C77">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D77" t="str">
         <v>Female</v>
       </c>
       <c r="E77" t="str">
-        <v>aria.nguyen36@gmail.com</v>
+        <v>aurora.hill33@hotmail.com</v>
       </c>
       <c r="F77" t="str">
-        <v>0401 618 716</v>
+        <v>0410 373 844</v>
       </c>
       <c r="G77" t="str">
-        <v>Sydney</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H77" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I77" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
+        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
       </c>
       <c r="B78" t="str">
-        <v>Ethan Taylor</v>
+        <v>Nora Mitchell</v>
       </c>
       <c r="C78">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D78" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E78" t="str">
-        <v>ethan.taylor22@yahoo.com</v>
+        <v>nora.mitchell66@outlook.com</v>
       </c>
       <c r="F78" t="str">
-        <v>0410 363 173</v>
+        <v>0412 196 419</v>
       </c>
       <c r="G78" t="str">
         <v>Adelaide</v>
       </c>
       <c r="H78" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I78" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
+        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
       </c>
       <c r="B79" t="str">
-        <v>Theodore Nelson</v>
+        <v>Maya Moore</v>
       </c>
       <c r="C79">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D79" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E79" t="str">
-        <v>theodore.nelson79@gmail.com</v>
+        <v>maya.moore54@outlook.com</v>
       </c>
       <c r="F79" t="str">
-        <v>0403 813 793</v>
+        <v>0400 718 585</v>
       </c>
       <c r="G79" t="str">
-        <v>Canberra</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H79" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I79" t="str">
-        <v>assigned</v>
+        <v>available</v>
+      </c>
+      <c r="J79" t="str">
+        <v>Sofia Williams</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
+        <v>222469f4-a8d9-4550-b6ee-db9d00e24edd</v>
       </c>
       <c r="B80" t="str">
-        <v>Maya Moore</v>
+        <v>Chloe Flores</v>
       </c>
       <c r="C80">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D80" t="str">
         <v>Female</v>
       </c>
       <c r="E80" t="str">
-        <v>maya.moore54@outlook.com</v>
+        <v>chloe.flores93@yahoo.com</v>
       </c>
       <c r="F80" t="str">
-        <v>0400 718 585</v>
+        <v>0400 918 463</v>
       </c>
       <c r="G80" t="str">
-        <v>Toowoomba</v>
+        <v>Townsville</v>
       </c>
       <c r="H80" t="str">
         <v>C</v>
@@ -3148,123 +3154,120 @@
         <v>available</v>
       </c>
       <c r="J80" t="str">
-        <v>Sofia Williams</v>
+        <v>Evelyn Sanchez</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>222469f4-a8d9-4550-b6ee-db9d00e24edd</v>
+        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
       </c>
       <c r="B81" t="str">
-        <v>Chloe Flores</v>
+        <v>Theodore Nelson</v>
       </c>
       <c r="C81">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="D81" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E81" t="str">
-        <v>chloe.flores93@yahoo.com</v>
+        <v>theodore.nelson79@gmail.com</v>
       </c>
       <c r="F81" t="str">
-        <v>0400 918 463</v>
+        <v>0403 813 793</v>
       </c>
       <c r="G81" t="str">
-        <v>Townsville</v>
+        <v>Canberra</v>
       </c>
       <c r="H81" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I81" t="str">
         <v>available</v>
-      </c>
-      <c r="J81" t="str">
-        <v>Evelyn Sanchez</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
+        <v>3db7cdb3-9a92-467c-b554-d23b524f42f5</v>
       </c>
       <c r="B82" t="str">
-        <v>Theodore Allen</v>
+        <v>Claire Campbell</v>
       </c>
       <c r="C82">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D82" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E82" t="str">
-        <v>theodore.allen25@outlook.com</v>
+        <v>claire.campbell9@outlook.com</v>
       </c>
       <c r="F82" t="str">
-        <v>0400 438 819</v>
+        <v>0401 164 490</v>
       </c>
       <c r="G82" t="str">
-        <v>Newcastle</v>
+        <v>Darwin</v>
       </c>
       <c r="H82" t="str">
         <v>B+</v>
       </c>
       <c r="I82" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
       </c>
       <c r="B83" t="str">
-        <v>Charles Torres</v>
+        <v>Abigail Williams</v>
       </c>
       <c r="C83">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D83" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E83" t="str">
-        <v>charles.torres98@outlook.com</v>
+        <v>abigail.williams45@yahoo.com</v>
       </c>
       <c r="F83" t="str">
-        <v>0401 744 176</v>
+        <v>0403 497 445</v>
       </c>
       <c r="G83" t="str">
-        <v>Wollongong</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H83" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I83" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>6591420b-4762-4d90-b738-8a5b70458c40</v>
+        <v>ee7f9d33-09d6-417b-a45f-3e6554489f5b</v>
       </c>
       <c r="B84" t="str">
-        <v>Aurora Hill</v>
+        <v>Dylan Miller</v>
       </c>
       <c r="C84">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D84" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E84" t="str">
-        <v>aurora.hill33@hotmail.com</v>
+        <v>dylan.miller23@hotmail.com</v>
       </c>
       <c r="F84" t="str">
-        <v>0410 373 844</v>
+        <v>0402 417 876</v>
       </c>
       <c r="G84" t="str">
-        <v>Gold Coast</v>
+        <v>Melbourne</v>
       </c>
       <c r="H84" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I84" t="str">
         <v>available</v>
@@ -3272,28 +3275,28 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
+        <v>5a6b21ec-9fac-4adc-b5ab-bcad20d0eca4</v>
       </c>
       <c r="B85" t="str">
-        <v>Lily Walker</v>
+        <v>Hunter Harris</v>
       </c>
       <c r="C85">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="D85" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E85" t="str">
-        <v>lily.walker96@outlook.com</v>
+        <v>hunter.harris1@gmail.com</v>
       </c>
       <c r="F85" t="str">
-        <v>0410 155 426</v>
+        <v>0404 782 485</v>
       </c>
       <c r="G85" t="str">
-        <v>Hobart</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H85" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I85" t="str">
         <v>available</v>
@@ -3301,10 +3304,10 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
+        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
       </c>
       <c r="B86" t="str">
-        <v>Jayden Nguyen</v>
+        <v>Julian Rivera</v>
       </c>
       <c r="C86">
         <v>53</v>
@@ -3313,16 +3316,16 @@
         <v>Male</v>
       </c>
       <c r="E86" t="str">
-        <v>jayden.nguyen88@hotmail.com</v>
+        <v>julian.rivera31@outlook.com</v>
       </c>
       <c r="F86" t="str">
-        <v>0401 108 628</v>
+        <v>0401 414 502</v>
       </c>
       <c r="G86" t="str">
-        <v>Hobart</v>
+        <v>Perth</v>
       </c>
       <c r="H86" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I86" t="str">
         <v>available</v>
@@ -3330,57 +3333,54 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
+        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
       </c>
       <c r="B87" t="str">
-        <v>Aurora Williams</v>
+        <v>Lucas Thomas</v>
       </c>
       <c r="C87">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D87" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E87" t="str">
-        <v>aurora.williams76@outlook.com</v>
+        <v>lucas.thomas30@yahoo.com</v>
       </c>
       <c r="F87" t="str">
-        <v>0401 416 170</v>
+        <v>0412 527 117</v>
       </c>
       <c r="G87" t="str">
-        <v>Darwin</v>
+        <v>Brisbane</v>
       </c>
       <c r="H87" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I87" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="M87" t="str">
-        <v>Uses walking cane</v>
+        <v>available</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>3db7cdb3-9a92-467c-b554-d23b524f42f5</v>
+        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
       </c>
       <c r="B88" t="str">
-        <v>Claire Campbell</v>
+        <v>Scarlett Lopez</v>
       </c>
       <c r="C88">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="D88" t="str">
         <v>Female</v>
       </c>
       <c r="E88" t="str">
-        <v>claire.campbell9@outlook.com</v>
+        <v>scarlett.lopez53@yahoo.com</v>
       </c>
       <c r="F88" t="str">
-        <v>0401 164 490</v>
+        <v>0400 509 641</v>
       </c>
       <c r="G88" t="str">
-        <v>Darwin</v>
+        <v>Sydney</v>
       </c>
       <c r="H88" t="str">
         <v>B+</v>
@@ -3391,28 +3391,28 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
+        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
       </c>
       <c r="B89" t="str">
-        <v>Emily Johnson</v>
+        <v>Lily Walker</v>
       </c>
       <c r="C89">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D89" t="str">
         <v>Female</v>
       </c>
       <c r="E89" t="str">
-        <v>emily.johnson58@hotmail.com</v>
+        <v>lily.walker96@outlook.com</v>
       </c>
       <c r="F89" t="str">
-        <v>0412 663 939</v>
+        <v>0410 155 426</v>
       </c>
       <c r="G89" t="str">
-        <v>Perth</v>
+        <v>Hobart</v>
       </c>
       <c r="H89" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I89" t="str">
         <v>available</v>
@@ -3525,206 +3525,191 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>7664257a-dce4-407a-8f24-692043d568be</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B93" t="str">
-        <v>Nora Jackson</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C93">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D93" t="str">
-        <v>Female</v>
+        <v>Not Specified</v>
       </c>
       <c r="E93" t="str">
-        <v>nora.jackson83@hotmail.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F93" t="str">
-        <v>0404 434 899</v>
+        <v>498086080</v>
       </c>
       <c r="G93" t="str">
-        <v>Wollongong</v>
+        <v>Footscray</v>
       </c>
       <c r="H93" t="str">
-        <v>B+</v>
+        <v/>
       </c>
       <c r="I93" t="str">
-        <v>assigned</v>
+        <v>available</v>
+      </c>
+      <c r="J93" t="str">
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
+      </c>
+      <c r="K93" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L93" t="str">
+        <v>N</v>
+      </c>
+      <c r="M93" t="str">
+        <v>N/A</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
+        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
       </c>
       <c r="B94" t="str">
-        <v>Ethan Rodriguez</v>
+        <v>Victoria Torres</v>
       </c>
       <c r="C94">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D94" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E94" t="str">
-        <v>ethan.rodriguez60@hotmail.com</v>
+        <v>victoria.torres48@outlook.com</v>
       </c>
       <c r="F94" t="str">
-        <v>0411 690 563</v>
+        <v>0411 539 271</v>
       </c>
       <c r="G94" t="str">
-        <v>Townsville</v>
+        <v>Geelong</v>
       </c>
       <c r="H94" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I94" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="M94" t="str">
-        <v>Hearing impaired - requires front row seating</v>
+        <v>available</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
       </c>
       <c r="B95" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Stella Green</v>
       </c>
       <c r="C95">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D95" t="str">
-        <v>Not Specified</v>
+        <v>Female</v>
       </c>
       <c r="E95" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>stella.green92@gmail.com</v>
       </c>
       <c r="F95" t="str">
-        <v>498086080</v>
+        <v>0404 230 858</v>
       </c>
       <c r="G95" t="str">
-        <v>Footscray</v>
+        <v>Wollongong</v>
       </c>
       <c r="H95" t="str">
-        <v/>
+        <v>A</v>
       </c>
       <c r="I95" t="str">
         <v>available</v>
       </c>
       <c r="J95" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
-      </c>
-      <c r="K95" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L95" t="str">
-        <v>N</v>
+        <v>Everly Torres</v>
       </c>
       <c r="M95" t="str">
-        <v>N/A</v>
+        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
+        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
       </c>
       <c r="B96" t="str">
-        <v>Stella Green</v>
+        <v>Scarlett Wright</v>
       </c>
       <c r="C96">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D96" t="str">
         <v>Female</v>
       </c>
       <c r="E96" t="str">
-        <v>stella.green92@gmail.com</v>
+        <v>scarlett.wright68@outlook.com</v>
       </c>
       <c r="F96" t="str">
-        <v>0404 230 858</v>
+        <v>0412 487 763</v>
       </c>
       <c r="G96" t="str">
-        <v>Wollongong</v>
+        <v>Newcastle</v>
       </c>
       <c r="H96" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I96" t="str">
         <v>available</v>
-      </c>
-      <c r="J96" t="str">
-        <v>Everly Torres</v>
-      </c>
-      <c r="M96" t="str">
-        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
       </c>
       <c r="B97" t="str">
-        <v>Peter Adamidis</v>
+        <v>Luke Flores</v>
       </c>
       <c r="C97">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D97" t="str">
-        <v>Not Specified</v>
+        <v>Male</v>
       </c>
       <c r="E97" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>luke.flores39@hotmail.com</v>
       </c>
       <c r="F97" t="str">
-        <v>498086080</v>
+        <v>0403 225 544</v>
       </c>
       <c r="G97" t="str">
-        <v/>
+        <v>Melbourne</v>
       </c>
       <c r="H97" t="str">
-        <v/>
+        <v>B</v>
       </c>
       <c r="I97" t="str">
         <v>available</v>
-      </c>
-      <c r="J97" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
-      </c>
-      <c r="K97" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L97" t="str">
-        <v>Y</v>
-      </c>
-      <c r="M97" t="str">
-        <v>Broken Leg</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
+        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
       </c>
       <c r="B98" t="str">
-        <v>Victoria Torres</v>
+        <v>Liam Lewis</v>
       </c>
       <c r="C98">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="D98" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E98" t="str">
-        <v>victoria.torres48@outlook.com</v>
+        <v>liam.lewis79@yahoo.com</v>
       </c>
       <c r="F98" t="str">
-        <v>0411 539 271</v>
+        <v>0404 203 198</v>
       </c>
       <c r="G98" t="str">
-        <v>Geelong</v>
+        <v>Hobart</v>
       </c>
       <c r="H98" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I98" t="str">
         <v>available</v>
@@ -3790,28 +3775,28 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
+        <v>7664257a-dce4-407a-8f24-692043d568be</v>
       </c>
       <c r="B101" t="str">
-        <v>Scarlett Wright</v>
+        <v>Nora Jackson</v>
       </c>
       <c r="C101">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D101" t="str">
         <v>Female</v>
       </c>
       <c r="E101" t="str">
-        <v>scarlett.wright68@outlook.com</v>
+        <v>nora.jackson83@hotmail.com</v>
       </c>
       <c r="F101" t="str">
-        <v>0412 487 763</v>
+        <v>0404 434 899</v>
       </c>
       <c r="G101" t="str">
-        <v>Newcastle</v>
+        <v>Wollongong</v>
       </c>
       <c r="H101" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I101" t="str">
         <v>available</v>
@@ -3819,25 +3804,25 @@
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
+        <v>8956e289-91e9-4c15-bf2b-a13dee2fa476</v>
       </c>
       <c r="B102" t="str">
-        <v>Liam Lewis</v>
+        <v>Landon Wright</v>
       </c>
       <c r="C102">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D102" t="str">
         <v>Male</v>
       </c>
       <c r="E102" t="str">
-        <v>liam.lewis79@yahoo.com</v>
+        <v>landon.wright36@outlook.com</v>
       </c>
       <c r="F102" t="str">
-        <v>0404 203 198</v>
+        <v>0402 415 597</v>
       </c>
       <c r="G102" t="str">
-        <v>Hobart</v>
+        <v>Cairns</v>
       </c>
       <c r="H102" t="str">
         <v>B+</v>
@@ -3848,60 +3833,75 @@
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
+        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
       </c>
       <c r="B103" t="str">
-        <v>Luke Flores</v>
+        <v>Ethan Rodriguez</v>
       </c>
       <c r="C103">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D103" t="str">
         <v>Male</v>
       </c>
       <c r="E103" t="str">
-        <v>luke.flores39@hotmail.com</v>
+        <v>ethan.rodriguez60@hotmail.com</v>
       </c>
       <c r="F103" t="str">
-        <v>0403 225 544</v>
+        <v>0411 690 563</v>
       </c>
       <c r="G103" t="str">
-        <v>Melbourne</v>
+        <v>Townsville</v>
       </c>
       <c r="H103" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I103" t="str">
         <v>available</v>
+      </c>
+      <c r="M103" t="str">
+        <v>Hearing impaired - requires front row seating</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>8956e289-91e9-4c15-bf2b-a13dee2fa476</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B104" t="str">
-        <v>Landon Wright</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C104">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D104" t="str">
-        <v>Male</v>
+        <v>Not Specified</v>
       </c>
       <c r="E104" t="str">
-        <v>landon.wright36@outlook.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F104" t="str">
-        <v>0402 415 597</v>
+        <v>498086080</v>
       </c>
       <c r="G104" t="str">
-        <v>Cairns</v>
+        <v/>
       </c>
       <c r="H104" t="str">
-        <v>B+</v>
+        <v/>
       </c>
       <c r="I104" t="str">
         <v>available</v>
+      </c>
+      <c r="J104" t="str">
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+      </c>
+      <c r="K104" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L104" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M104" t="str">
+        <v>Broken Leg</v>
       </c>
     </row>
   </sheetData>
@@ -3913,7 +3913,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3946,483 +3946,41 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>a634c290-4c9c-414a-93fc-745bd097e76d</v>
+        <v>cf3cf946-cf37-4a6d-b4aa-533fb3b9633f</v>
       </c>
       <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C2" t="str">
-        <v>ecc70875-f282-4849-9e60-071edc278977</v>
+        <v>0dd7de5c-0409-45e3-84a5-5f2ffbd591d8</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>A5</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>b8c8e258-37be-4899-875e-6d388063ccde</v>
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
       </c>
       <c r="B3" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C3" t="str">
-        <v>7664257a-dce4-407a-8f24-692043d568be</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>B1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>45375cb0-bd1b-4b9a-a6a6-27fee2fb4945</v>
-      </c>
-      <c r="B4" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C4" t="str">
-        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="str">
         <v>A1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>a616aafc-3ff8-4449-a8f9-1a4dbc9350d0</v>
-      </c>
-      <c r="B5" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C5" t="str">
-        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="str">
-        <v>A2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>d5b88b57-aa91-49ce-afab-69ab3e297842</v>
-      </c>
-      <c r="B6" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C6" t="str">
-        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" t="str">
-        <v>A3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>40d2ebf0-17a6-485d-9dc1-2b1c6f764b92</v>
-      </c>
-      <c r="B7" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C7" t="str">
-        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="str">
-        <v>A4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>e860e9bf-0085-4cdd-a9d0-594335337f42</v>
-      </c>
-      <c r="B8" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C8" t="str">
-        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8" t="str">
-        <v>A5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>231cd33c-26f8-47eb-abdb-18be9cb04e40</v>
-      </c>
-      <c r="B9" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C9" t="str">
-        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9" t="str">
-        <v>A1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>373d1ffe-5ae4-49a1-938f-0247d30da633</v>
-      </c>
-      <c r="B10" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C10" t="str">
-        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10" t="str">
-        <v>A2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>a18d0693-98ff-4e9e-848f-9d3411c9f601</v>
-      </c>
-      <c r="B11" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C11" t="str">
-        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
-      </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
-      <c r="E11" t="str">
-        <v>A3</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>c0a18a7e-4e83-408c-9071-eb8eacc5af4b</v>
-      </c>
-      <c r="B12" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C12" t="str">
-        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12" t="str">
-        <v>A4</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>05863c6a-b5c7-4f02-9310-ed16f475fa5b</v>
-      </c>
-      <c r="B13" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C13" t="str">
-        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13" t="str">
-        <v>A5</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>39179962-2dc4-430e-989a-8b933f871bc8</v>
-      </c>
-      <c r="B14" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C14" t="str">
-        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14" t="str">
-        <v>B1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>8fea80c2-f010-418e-9912-3e1811738244</v>
-      </c>
-      <c r="B15" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C15" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15" t="str">
-        <v>B2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>ec5bdd9f-9a20-4c40-b36a-6b6c4bb850da</v>
-      </c>
-      <c r="B16" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C16" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c r="E16" t="str">
-        <v>B3</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>47c2c439-7c97-4019-80fd-93fc83d7c8e6</v>
-      </c>
-      <c r="B17" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C17" t="str">
-        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17" t="str">
-        <v>B4</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>55aae62f-a92f-49f5-a5a2-f0aba343014a</v>
-      </c>
-      <c r="B18" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C18" t="str">
-        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
-      </c>
-      <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="E18" t="str">
-        <v>B5</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>eaacb9fd-9bff-4952-8551-663c60df9878</v>
-      </c>
-      <c r="B19" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C19" t="str">
-        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19" t="str">
-        <v>C1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>190fda70-e765-41a5-9147-b1f36392b50d</v>
-      </c>
-      <c r="B20" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C20" t="str">
-        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20" t="str">
-        <v>C2</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>7b5bf219-72c4-4e76-a04a-d00f276902e9</v>
-      </c>
-      <c r="B21" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C21" t="str">
-        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
-      </c>
-      <c r="D21">
-        <v>5</v>
-      </c>
-      <c r="E21" t="str">
-        <v>C3</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>a18846fc-8b75-4224-90ca-0ac6b286ea5a</v>
-      </c>
-      <c r="B22" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C22" t="str">
-        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
-      </c>
-      <c r="D22">
-        <v>5</v>
-      </c>
-      <c r="E22" t="str">
-        <v>C4</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>77f1ebcc-83e6-48b3-aeee-af901920079c</v>
-      </c>
-      <c r="B23" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C23" t="str">
-        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
-      </c>
-      <c r="D23">
-        <v>5</v>
-      </c>
-      <c r="E23" t="str">
-        <v>D1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>a86ddb54-5d1b-4d80-940e-b1f381a6333f</v>
-      </c>
-      <c r="B24" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C24" t="str">
-        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
-      </c>
-      <c r="D24">
-        <v>5</v>
-      </c>
-      <c r="E24" t="str">
-        <v>D2</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>abe65c79-379e-46ec-aded-2652f9e64961</v>
-      </c>
-      <c r="B25" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C25" t="str">
-        <v>8e115c7e-8033-4466-bcb9-07ea089eb4be</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-      <c r="E25" t="str">
-        <v>A1</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>e46419c3-c90e-4432-a3bb-19dedad4bb04</v>
-      </c>
-      <c r="B26" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C26" t="str">
-        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
-      </c>
-      <c r="D26">
-        <v>6</v>
-      </c>
-      <c r="E26" t="str">
-        <v>A2</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>e2f751de-9d53-4fe5-8f08-756bfc12bb83</v>
-      </c>
-      <c r="B27" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C27" t="str">
-        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
-      </c>
-      <c r="D27">
-        <v>6</v>
-      </c>
-      <c r="E27" t="str">
-        <v>A3</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>dadf3bea-2f2a-48bf-9e6e-7947f8313921</v>
-      </c>
-      <c r="B28" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C28" t="str">
-        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
-      </c>
-      <c r="D28">
-        <v>6</v>
-      </c>
-      <c r="E28" t="str">
-        <v>A4</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>2707752c-605e-4a31-871c-ece5c863b517</v>
-      </c>
-      <c r="B29" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C29" t="str">
-        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-      <c r="E29" t="str">
-        <v>A5</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Improve contestant seating assignment logic for groups and demographics
Adjust auto-assignment logic to allow groups in empty blocks by modifying the 70% female constraint to only apply when a block has at least 4 contestants. Includes debug logging for contestant grouping and updates to backup data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 6fa8c239-2617-48bf-881b-510f95449ae6
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/Kbk0MEj
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -718,25 +718,25 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>d37f9e40-d1a2-4238-9089-80517a709859</v>
       </c>
       <c r="B2" t="str">
-        <v>Audrey Thomas</v>
+        <v>Mia Roberts</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D2" t="str">
         <v>Female</v>
       </c>
       <c r="E2" t="str">
-        <v>audrey.thomas38@gmail.com</v>
+        <v>mia.roberts81@hotmail.com</v>
       </c>
       <c r="F2" t="str">
-        <v>0400 437 270</v>
+        <v>0412 368 553</v>
       </c>
       <c r="G2" t="str">
-        <v>Perth</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H2" t="str">
         <v>C</v>
@@ -745,27 +745,27 @@
         <v>available</v>
       </c>
       <c r="J2" t="str">
-        <v>Hannah Torres</v>
+        <v>Paisley Scott</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>d37f9e40-d1a2-4238-9089-80517a709859</v>
+        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
       </c>
       <c r="B3" t="str">
-        <v>Mia Roberts</v>
+        <v>Chloe Jones</v>
       </c>
       <c r="C3">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D3" t="str">
         <v>Female</v>
       </c>
       <c r="E3" t="str">
-        <v>mia.roberts81@hotmail.com</v>
+        <v>chloe.jones20@outlook.com</v>
       </c>
       <c r="F3" t="str">
-        <v>0412 368 553</v>
+        <v>0411 294 635</v>
       </c>
       <c r="G3" t="str">
         <v>Toowoomba</v>
@@ -777,100 +777,106 @@
         <v>available</v>
       </c>
       <c r="J3" t="str">
-        <v>Paisley Scott</v>
+        <v>Zoe Brown</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
       </c>
       <c r="B4" t="str">
-        <v>Chloe Jones</v>
+        <v>Samuel King</v>
       </c>
       <c r="C4">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D4" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E4" t="str">
-        <v>chloe.jones20@outlook.com</v>
+        <v>samuel.king24@yahoo.com</v>
       </c>
       <c r="F4" t="str">
-        <v>0411 294 635</v>
+        <v>0400 774 736</v>
       </c>
       <c r="G4" t="str">
-        <v>Toowoomba</v>
+        <v>Newcastle</v>
       </c>
       <c r="H4" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I4" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Zoe Brown</v>
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <v>afasdf</v>
+      </c>
+      <c r="M4" t="str">
+        <v>sdfasdfa</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
+        <v>0669e014-c952-45fd-9791-36cbe1d51444</v>
       </c>
       <c r="B5" t="str">
-        <v>Jackson Young</v>
+        <v>Sofia Williams</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D5" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E5" t="str">
-        <v>jackson.young79@yahoo.com</v>
+        <v>sofia.williams39@yahoo.com</v>
       </c>
       <c r="F5" t="str">
-        <v>0412 940 993</v>
+        <v>0403 299 421</v>
       </c>
       <c r="G5" t="str">
-        <v>Ballarat</v>
+        <v>Geelong</v>
       </c>
       <c r="H5" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I5" t="str">
         <v>assigned</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Maya Moore</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>992418b2-3029-4752-9552-0aa886433657</v>
+        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
       </c>
       <c r="B6" t="str">
-        <v>Zoe Brown</v>
+        <v>Jackson Young</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D6" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E6" t="str">
-        <v>zoe.brown45@outlook.com</v>
+        <v>jackson.young79@yahoo.com</v>
       </c>
       <c r="F6" t="str">
-        <v>0401 578 107</v>
+        <v>0412 940 993</v>
       </c>
       <c r="G6" t="str">
-        <v>Sydney</v>
+        <v>Ballarat</v>
       </c>
       <c r="H6" t="str">
         <v>B+</v>
       </c>
       <c r="I6" t="str">
-        <v>available</v>
-      </c>
-      <c r="J6" t="str">
-        <v>Chloe Jones</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="7">
@@ -931,7 +937,7 @@
         <v>B+</v>
       </c>
       <c r="I8" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J8" t="str">
         <v>Audrey Thomas</v>
@@ -968,95 +974,98 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>0669e014-c952-45fd-9791-36cbe1d51444</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="B10" t="str">
-        <v>Sofia Williams</v>
+        <v>Ella Anderson</v>
       </c>
       <c r="C10">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D10" t="str">
         <v>Female</v>
       </c>
       <c r="E10" t="str">
-        <v>sofia.williams39@yahoo.com</v>
+        <v>ella.anderson1@yahoo.com</v>
       </c>
       <c r="F10" t="str">
-        <v>0403 299 421</v>
+        <v>0412 908 910</v>
       </c>
       <c r="G10" t="str">
         <v>Geelong</v>
       </c>
       <c r="H10" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I10" t="str">
         <v>available</v>
       </c>
       <c r="J10" t="str">
-        <v>Maya Moore</v>
+        <v>Isabella Brown</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
       </c>
       <c r="B11" t="str">
-        <v>Ella Anderson</v>
+        <v>Audrey Thomas</v>
       </c>
       <c r="C11">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D11" t="str">
         <v>Female</v>
       </c>
       <c r="E11" t="str">
-        <v>ella.anderson1@yahoo.com</v>
+        <v>audrey.thomas38@gmail.com</v>
       </c>
       <c r="F11" t="str">
-        <v>0412 908 910</v>
+        <v>0400 437 270</v>
       </c>
       <c r="G11" t="str">
-        <v>Geelong</v>
+        <v>Perth</v>
       </c>
       <c r="H11" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I11" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J11" t="str">
-        <v>Isabella Brown</v>
+        <v>Hannah Torres</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>992418b2-3029-4752-9552-0aa886433657</v>
       </c>
       <c r="B12" t="str">
-        <v>Samuel King</v>
+        <v>Zoe Brown</v>
       </c>
       <c r="C12">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D12" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E12" t="str">
-        <v>samuel.king24@yahoo.com</v>
+        <v>zoe.brown45@outlook.com</v>
       </c>
       <c r="F12" t="str">
-        <v>0400 774 736</v>
+        <v>0401 578 107</v>
       </c>
       <c r="G12" t="str">
-        <v>Newcastle</v>
+        <v>Sydney</v>
       </c>
       <c r="H12" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I12" t="str">
         <v>assigned</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Chloe Jones</v>
       </c>
     </row>
     <row r="13">
@@ -1643,28 +1652,28 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>0a153155-dcf5-4d56-9ed1-8960501157f8</v>
+        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
       </c>
       <c r="B31" t="str">
-        <v>Aurora Gonzalez</v>
+        <v>Noah Hernandez</v>
       </c>
       <c r="C31">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D31" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E31" t="str">
-        <v>aurora.gonzalez29@outlook.com</v>
+        <v>noah.hernandez9@hotmail.com</v>
       </c>
       <c r="F31" t="str">
-        <v>0404 610 172</v>
+        <v>0404 855 230</v>
       </c>
       <c r="G31" t="str">
-        <v>Toowoomba</v>
+        <v>Cairns</v>
       </c>
       <c r="H31" t="str">
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="I31" t="str">
         <v>assigned</v>
@@ -1672,25 +1681,25 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
+        <v>0a153155-dcf5-4d56-9ed1-8960501157f8</v>
       </c>
       <c r="B32" t="str">
-        <v>Mason Hill</v>
+        <v>Aurora Gonzalez</v>
       </c>
       <c r="C32">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D32" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E32" t="str">
-        <v>mason.hill27@outlook.com</v>
+        <v>aurora.gonzalez29@outlook.com</v>
       </c>
       <c r="F32" t="str">
-        <v>0410 682 884</v>
+        <v>0404 610 172</v>
       </c>
       <c r="G32" t="str">
-        <v>Canberra</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H32" t="str">
         <v>A</v>
@@ -1701,28 +1710,28 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
+        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
       </c>
       <c r="B33" t="str">
-        <v>Nathan Allen</v>
+        <v>Mason Hill</v>
       </c>
       <c r="C33">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D33" t="str">
         <v>Male</v>
       </c>
       <c r="E33" t="str">
-        <v>nathan.allen87@outlook.com</v>
+        <v>mason.hill27@outlook.com</v>
       </c>
       <c r="F33" t="str">
-        <v>0403 587 263</v>
+        <v>0410 682 884</v>
       </c>
       <c r="G33" t="str">
-        <v>Adelaide</v>
+        <v>Canberra</v>
       </c>
       <c r="H33" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I33" t="str">
         <v>assigned</v>
@@ -1730,25 +1739,25 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
+        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
       </c>
       <c r="B34" t="str">
-        <v>Abigail Jackson</v>
+        <v>Nathan Allen</v>
       </c>
       <c r="C34">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="D34" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E34" t="str">
-        <v>abigail.jackson65@outlook.com</v>
+        <v>nathan.allen87@outlook.com</v>
       </c>
       <c r="F34" t="str">
-        <v>0411 824 257</v>
+        <v>0403 587 263</v>
       </c>
       <c r="G34" t="str">
-        <v>Newcastle</v>
+        <v>Adelaide</v>
       </c>
       <c r="H34" t="str">
         <v>B+</v>
@@ -1759,28 +1768,28 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>3d2128a1-336f-41e1-973b-b5dd54d90b19</v>
+        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
       </c>
       <c r="B35" t="str">
-        <v>Nova Brown</v>
+        <v>Abigail Jackson</v>
       </c>
       <c r="C35">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="D35" t="str">
         <v>Female</v>
       </c>
       <c r="E35" t="str">
-        <v>nova.brown80@outlook.com</v>
+        <v>abigail.jackson65@outlook.com</v>
       </c>
       <c r="F35" t="str">
-        <v>0411 154 614</v>
+        <v>0411 824 257</v>
       </c>
       <c r="G35" t="str">
-        <v>Ballarat</v>
+        <v>Newcastle</v>
       </c>
       <c r="H35" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I35" t="str">
         <v>assigned</v>
@@ -1788,188 +1797,185 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
+        <v>3d2128a1-336f-41e1-973b-b5dd54d90b19</v>
       </c>
       <c r="B36" t="str">
-        <v>Paisley Scott</v>
+        <v>Nova Brown</v>
       </c>
       <c r="C36">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="D36" t="str">
         <v>Female</v>
       </c>
       <c r="E36" t="str">
-        <v>paisley.scott78@yahoo.com</v>
+        <v>nova.brown80@outlook.com</v>
       </c>
       <c r="F36" t="str">
-        <v>0410 215 419</v>
+        <v>0411 154 614</v>
       </c>
       <c r="G36" t="str">
         <v>Ballarat</v>
       </c>
       <c r="H36" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I36" t="str">
-        <v>available</v>
-      </c>
-      <c r="J36" t="str">
-        <v>Mia Roberts</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
       </c>
       <c r="B37" t="str">
-        <v>Stella Garcia</v>
+        <v>Carter Harris</v>
       </c>
       <c r="C37">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D37" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E37" t="str">
-        <v>stella.garcia89@hotmail.com</v>
+        <v>carter.harris82@yahoo.com</v>
       </c>
       <c r="F37" t="str">
-        <v>0403 655 540</v>
+        <v>0412 175 744</v>
       </c>
       <c r="G37" t="str">
-        <v>Toowoomba</v>
+        <v>Geelong</v>
       </c>
       <c r="H37" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I37" t="str">
-        <v>available</v>
-      </c>
-      <c r="J37" t="str">
-        <v>Emily Thomas</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
+        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
       </c>
       <c r="B38" t="str">
-        <v>Noah Hernandez</v>
+        <v>Paisley Scott</v>
       </c>
       <c r="C38">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D38" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E38" t="str">
-        <v>noah.hernandez9@hotmail.com</v>
+        <v>paisley.scott78@yahoo.com</v>
       </c>
       <c r="F38" t="str">
-        <v>0404 855 230</v>
+        <v>0410 215 419</v>
       </c>
       <c r="G38" t="str">
-        <v>Cairns</v>
+        <v>Ballarat</v>
       </c>
       <c r="H38" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I38" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J38" t="str">
+        <v>Mia Roberts</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B39" t="str">
-        <v>Carter Harris</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C39">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="D39" t="str">
-        <v>Male</v>
+        <v>Not Specified</v>
       </c>
       <c r="E39" t="str">
-        <v>carter.harris82@yahoo.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F39" t="str">
-        <v>0412 175 744</v>
+        <v>498086080</v>
       </c>
       <c r="G39" t="str">
-        <v>Geelong</v>
+        <v>Melbourne</v>
       </c>
       <c r="H39" t="str">
-        <v>C</v>
+        <v/>
       </c>
       <c r="I39" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J39" t="str">
+        <v>Peter Adamidis, Kathleen Reynolds</v>
+      </c>
+      <c r="K39" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L39" t="str">
+        <v>N</v>
+      </c>
+      <c r="M39" t="str">
+        <v>N/A</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
       </c>
       <c r="B40" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Ryan Williams</v>
       </c>
       <c r="C40">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D40" t="str">
-        <v>Not Specified</v>
+        <v>Male</v>
       </c>
       <c r="E40" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>ryan.williams82@hotmail.com</v>
       </c>
       <c r="F40" t="str">
-        <v>498086080</v>
+        <v>0401 450 673</v>
       </c>
       <c r="G40" t="str">
-        <v>Melbourne</v>
+        <v>Perth</v>
       </c>
       <c r="H40" t="str">
-        <v/>
+        <v>B+</v>
       </c>
       <c r="I40" t="str">
         <v>assigned</v>
-      </c>
-      <c r="J40" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
-      </c>
-      <c r="K40" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L40" t="str">
-        <v>N</v>
-      </c>
-      <c r="M40" t="str">
-        <v>N/A</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
+        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
       </c>
       <c r="B41" t="str">
-        <v>Ryan Williams</v>
+        <v>Cameron Lee</v>
       </c>
       <c r="C41">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D41" t="str">
         <v>Male</v>
       </c>
       <c r="E41" t="str">
-        <v>ryan.williams82@hotmail.com</v>
+        <v>cameron.lee78@yahoo.com</v>
       </c>
       <c r="F41" t="str">
-        <v>0401 450 673</v>
+        <v>0404 821 708</v>
       </c>
       <c r="G41" t="str">
-        <v>Perth</v>
+        <v>Cairns</v>
       </c>
       <c r="H41" t="str">
         <v>B+</v>
@@ -1980,31 +1986,34 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
+        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
       </c>
       <c r="B42" t="str">
-        <v>Cameron Lee</v>
+        <v>Stella Garcia</v>
       </c>
       <c r="C42">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D42" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E42" t="str">
-        <v>cameron.lee78@yahoo.com</v>
+        <v>stella.garcia89@hotmail.com</v>
       </c>
       <c r="F42" t="str">
-        <v>0404 821 708</v>
+        <v>0403 655 540</v>
       </c>
       <c r="G42" t="str">
-        <v>Cairns</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H42" t="str">
         <v>B+</v>
       </c>
       <c r="I42" t="str">
         <v>assigned</v>
+      </c>
+      <c r="J42" t="str">
+        <v>Emily Thomas</v>
       </c>
     </row>
     <row r="43">
@@ -2201,208 +2210,205 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
+        <v>6591420b-4762-4d90-b738-8a5b70458c40</v>
       </c>
       <c r="B49" t="str">
-        <v>Nora Mitchell</v>
+        <v>Aurora Hill</v>
       </c>
       <c r="C49">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D49" t="str">
         <v>Female</v>
       </c>
       <c r="E49" t="str">
-        <v>nora.mitchell66@outlook.com</v>
+        <v>aurora.hill33@hotmail.com</v>
       </c>
       <c r="F49" t="str">
-        <v>0412 196 419</v>
+        <v>0410 373 844</v>
       </c>
       <c r="G49" t="str">
-        <v>Adelaide</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H49" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I49" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
+        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
       </c>
       <c r="B50" t="str">
-        <v>Stella Martinez</v>
+        <v>Stella Hall</v>
       </c>
       <c r="C50">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D50" t="str">
         <v>Female</v>
       </c>
       <c r="E50" t="str">
-        <v>stella.martinez75@gmail.com</v>
+        <v>stella.hall72@gmail.com</v>
       </c>
       <c r="F50" t="str">
-        <v>0404 227 272</v>
+        <v>0410 133 818</v>
       </c>
       <c r="G50" t="str">
-        <v>Ballarat</v>
+        <v>Wollongong</v>
       </c>
       <c r="H50" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I50" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="B51" t="str">
-        <v>Aria Nguyen</v>
+        <v>Isabella Brown</v>
       </c>
       <c r="C51">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D51" t="str">
         <v>Female</v>
       </c>
       <c r="E51" t="str">
-        <v>aria.nguyen36@gmail.com</v>
+        <v>isabella.brown43@outlook.com</v>
       </c>
       <c r="F51" t="str">
-        <v>0401 618 716</v>
+        <v>0403 771 690</v>
       </c>
       <c r="G51" t="str">
-        <v>Sydney</v>
+        <v>Darwin</v>
       </c>
       <c r="H51" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I51" t="str">
         <v>available</v>
       </c>
+      <c r="J51" t="str">
+        <v>Ella Anderson</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>32ffeaf9-5f22-4db7-a70b-cbaab834db0d</v>
       </c>
       <c r="B52" t="str">
-        <v>Isabella Brown</v>
+        <v>Isabella Hill</v>
       </c>
       <c r="C52">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D52" t="str">
         <v>Female</v>
       </c>
       <c r="E52" t="str">
-        <v>isabella.brown43@outlook.com</v>
+        <v>isabella.hill77@hotmail.com</v>
       </c>
       <c r="F52" t="str">
-        <v>0403 771 690</v>
+        <v>0412 663 356</v>
       </c>
       <c r="G52" t="str">
         <v>Darwin</v>
       </c>
       <c r="H52" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I52" t="str">
-        <v>available</v>
-      </c>
-      <c r="J52" t="str">
-        <v>Ella Anderson</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
+        <v>ee7f9d33-09d6-417b-a45f-3e6554489f5b</v>
       </c>
       <c r="B53" t="str">
-        <v>Stella Hall</v>
+        <v>Dylan Miller</v>
       </c>
       <c r="C53">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D53" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E53" t="str">
-        <v>stella.hall72@gmail.com</v>
+        <v>dylan.miller23@hotmail.com</v>
       </c>
       <c r="F53" t="str">
-        <v>0410 133 818</v>
+        <v>0402 417 876</v>
       </c>
       <c r="G53" t="str">
-        <v>Wollongong</v>
+        <v>Melbourne</v>
       </c>
       <c r="H53" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I53" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
+        <v>3db7cdb3-9a92-467c-b554-d23b524f42f5</v>
       </c>
       <c r="B54" t="str">
-        <v>Andrew Garcia</v>
+        <v>Claire Campbell</v>
       </c>
       <c r="C54">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D54" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E54" t="str">
-        <v>andrew.garcia26@hotmail.com</v>
+        <v>claire.campbell9@outlook.com</v>
       </c>
       <c r="F54" t="str">
-        <v>0400 450 222</v>
+        <v>0401 164 490</v>
       </c>
       <c r="G54" t="str">
         <v>Darwin</v>
       </c>
       <c r="H54" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I54" t="str">
-        <v>available</v>
-      </c>
-      <c r="M54" t="str">
-        <v>Limited mobility - prefers ground floor seating</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>ee7f9d33-09d6-417b-a45f-3e6554489f5b</v>
+        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
       </c>
       <c r="B55" t="str">
-        <v>Dylan Miller</v>
+        <v>Carter Hill</v>
       </c>
       <c r="C55">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D55" t="str">
         <v>Male</v>
       </c>
       <c r="E55" t="str">
-        <v>dylan.miller23@hotmail.com</v>
+        <v>carter.hill93@gmail.com</v>
       </c>
       <c r="F55" t="str">
-        <v>0402 417 876</v>
+        <v>0404 349 309</v>
       </c>
       <c r="G55" t="str">
-        <v>Melbourne</v>
+        <v>Newcastle</v>
       </c>
       <c r="H55" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I55" t="str">
         <v>assigned</v>
@@ -2410,28 +2416,28 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>3db7cdb3-9a92-467c-b554-d23b524f42f5</v>
+        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
       </c>
       <c r="B56" t="str">
-        <v>Claire Campbell</v>
+        <v>Charles Torres</v>
       </c>
       <c r="C56">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D56" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E56" t="str">
-        <v>claire.campbell9@outlook.com</v>
+        <v>charles.torres98@outlook.com</v>
       </c>
       <c r="F56" t="str">
-        <v>0401 164 490</v>
+        <v>0401 744 176</v>
       </c>
       <c r="G56" t="str">
-        <v>Darwin</v>
+        <v>Wollongong</v>
       </c>
       <c r="H56" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I56" t="str">
         <v>assigned</v>
@@ -2465,60 +2471,69 @@
       <c r="I57" t="str">
         <v>assigned</v>
       </c>
+      <c r="J57" t="str">
+        <v/>
+      </c>
+      <c r="L57" t="str">
+        <v>sdfasdf</v>
+      </c>
+      <c r="M57" t="str">
+        <v>sdfasdfa</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
+        <v>34685ff7-6e85-4bbd-b546-77cfe11d7f7d</v>
       </c>
       <c r="B58" t="str">
-        <v>Carter Hill</v>
+        <v>Grace Walker</v>
       </c>
       <c r="C58">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="D58" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E58" t="str">
-        <v>carter.hill93@gmail.com</v>
+        <v>grace.walker52@hotmail.com</v>
       </c>
       <c r="F58" t="str">
-        <v>0404 349 309</v>
+        <v>0412 754 780</v>
       </c>
       <c r="G58" t="str">
-        <v>Newcastle</v>
+        <v>Canberra</v>
       </c>
       <c r="H58" t="str">
-        <v>B</v>
+        <v>A+</v>
       </c>
       <c r="I58" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
+        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
       </c>
       <c r="B59" t="str">
-        <v>Charles Torres</v>
+        <v>Nora Mitchell</v>
       </c>
       <c r="C59">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D59" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E59" t="str">
-        <v>charles.torres98@outlook.com</v>
+        <v>nora.mitchell66@outlook.com</v>
       </c>
       <c r="F59" t="str">
-        <v>0401 744 176</v>
+        <v>0412 196 419</v>
       </c>
       <c r="G59" t="str">
-        <v>Wollongong</v>
+        <v>Adelaide</v>
       </c>
       <c r="H59" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I59" t="str">
         <v>assigned</v>
@@ -2526,182 +2541,185 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>34685ff7-6e85-4bbd-b546-77cfe11d7f7d</v>
+        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
       </c>
       <c r="B60" t="str">
-        <v>Grace Walker</v>
+        <v>Stella Martinez</v>
       </c>
       <c r="C60">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D60" t="str">
         <v>Female</v>
       </c>
       <c r="E60" t="str">
-        <v>grace.walker52@hotmail.com</v>
+        <v>stella.martinez75@gmail.com</v>
       </c>
       <c r="F60" t="str">
-        <v>0412 754 780</v>
+        <v>0404 227 272</v>
       </c>
       <c r="G60" t="str">
-        <v>Canberra</v>
+        <v>Ballarat</v>
       </c>
       <c r="H60" t="str">
-        <v>A+</v>
+        <v>C</v>
       </c>
       <c r="I60" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
+        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
       </c>
       <c r="B61" t="str">
-        <v>Genesis Jones</v>
+        <v>Aria Nguyen</v>
       </c>
       <c r="C61">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D61" t="str">
         <v>Female</v>
       </c>
       <c r="E61" t="str">
-        <v>genesis.jones50@yahoo.com</v>
+        <v>aria.nguyen36@gmail.com</v>
       </c>
       <c r="F61" t="str">
-        <v>0404 967 604</v>
+        <v>0401 618 716</v>
       </c>
       <c r="G61" t="str">
         <v>Sydney</v>
       </c>
       <c r="H61" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I61" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>6591420b-4762-4d90-b738-8a5b70458c40</v>
+        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
       </c>
       <c r="B62" t="str">
-        <v>Aurora Hill</v>
+        <v>Maya Moore</v>
       </c>
       <c r="C62">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D62" t="str">
         <v>Female</v>
       </c>
       <c r="E62" t="str">
-        <v>aurora.hill33@hotmail.com</v>
+        <v>maya.moore54@outlook.com</v>
       </c>
       <c r="F62" t="str">
-        <v>0410 373 844</v>
+        <v>0400 718 585</v>
       </c>
       <c r="G62" t="str">
-        <v>Gold Coast</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H62" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I62" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J62" t="str">
+        <v>Sofia Williams</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>32ffeaf9-5f22-4db7-a70b-cbaab834db0d</v>
+        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
       </c>
       <c r="B63" t="str">
-        <v>Isabella Hill</v>
+        <v>Andrew Garcia</v>
       </c>
       <c r="C63">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D63" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E63" t="str">
-        <v>isabella.hill77@hotmail.com</v>
+        <v>andrew.garcia26@hotmail.com</v>
       </c>
       <c r="F63" t="str">
-        <v>0412 663 356</v>
+        <v>0400 450 222</v>
       </c>
       <c r="G63" t="str">
         <v>Darwin</v>
       </c>
       <c r="H63" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I63" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="M63" t="str">
+        <v>Limited mobility - prefers ground floor seating</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>da40ad70-95be-413c-b0f1-d089ef285cc8</v>
+        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
       </c>
       <c r="B64" t="str">
-        <v>Emily Smith</v>
+        <v>Genesis Jones</v>
       </c>
       <c r="C64">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D64" t="str">
         <v>Female</v>
       </c>
       <c r="E64" t="str">
-        <v>emily.smith56@hotmail.com</v>
+        <v>genesis.jones50@yahoo.com</v>
       </c>
       <c r="F64" t="str">
-        <v>0410 101 780</v>
+        <v>0404 967 604</v>
       </c>
       <c r="G64" t="str">
-        <v>Toowoomba</v>
+        <v>Sydney</v>
       </c>
       <c r="H64" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I64" t="str">
-        <v>available</v>
-      </c>
-      <c r="M64" t="str">
-        <v>Limited mobility - prefers ground floor seating</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
+        <v>da40ad70-95be-413c-b0f1-d089ef285cc8</v>
       </c>
       <c r="B65" t="str">
-        <v>Maya Moore</v>
+        <v>Emily Smith</v>
       </c>
       <c r="C65">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D65" t="str">
         <v>Female</v>
       </c>
       <c r="E65" t="str">
-        <v>maya.moore54@outlook.com</v>
+        <v>emily.smith56@hotmail.com</v>
       </c>
       <c r="F65" t="str">
-        <v>0400 718 585</v>
+        <v>0410 101 780</v>
       </c>
       <c r="G65" t="str">
         <v>Toowoomba</v>
       </c>
       <c r="H65" t="str">
-        <v>C</v>
+        <v>A+</v>
       </c>
       <c r="I65" t="str">
         <v>available</v>
       </c>
-      <c r="J65" t="str">
-        <v>Sofia Williams</v>
+      <c r="M65" t="str">
+        <v>Limited mobility - prefers ground floor seating</v>
       </c>
     </row>
     <row r="66">
@@ -2864,7 +2882,7 @@
         <v>B+</v>
       </c>
       <c r="I70" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="71">
@@ -2893,7 +2911,7 @@
         <v>C</v>
       </c>
       <c r="I71" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="M71" t="str">
         <v>Requires wheelchair access</v>
@@ -2925,7 +2943,7 @@
         <v>C</v>
       </c>
       <c r="I72" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="73">
@@ -2954,7 +2972,7 @@
         <v>C</v>
       </c>
       <c r="I73" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="74">
@@ -3015,7 +3033,7 @@
         <v>B+</v>
       </c>
       <c r="I75" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="76">
@@ -3055,853 +3073,853 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
+        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
       </c>
       <c r="B77" t="str">
-        <v>Victoria Torres</v>
+        <v>Scarlett Wright</v>
       </c>
       <c r="C77">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D77" t="str">
         <v>Female</v>
       </c>
       <c r="E77" t="str">
-        <v>victoria.torres48@outlook.com</v>
+        <v>scarlett.wright68@outlook.com</v>
       </c>
       <c r="F77" t="str">
-        <v>0411 539 271</v>
+        <v>0412 487 763</v>
       </c>
       <c r="G77" t="str">
-        <v>Geelong</v>
+        <v>Newcastle</v>
       </c>
       <c r="H77" t="str">
         <v>B</v>
       </c>
       <c r="I77" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>7664257a-dce4-407a-8f24-692043d568be</v>
+        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
       </c>
       <c r="B78" t="str">
-        <v>Nora Jackson</v>
+        <v>Theodore Nelson</v>
       </c>
       <c r="C78">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D78" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E78" t="str">
-        <v>nora.jackson83@hotmail.com</v>
+        <v>theodore.nelson79@gmail.com</v>
       </c>
       <c r="F78" t="str">
-        <v>0404 434 899</v>
+        <v>0403 813 793</v>
       </c>
       <c r="G78" t="str">
-        <v>Wollongong</v>
+        <v>Canberra</v>
       </c>
       <c r="H78" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I78" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
+        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
       </c>
       <c r="B79" t="str">
-        <v>Abigail Williams</v>
+        <v>Aurora Williams</v>
       </c>
       <c r="C79">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="D79" t="str">
         <v>Female</v>
       </c>
       <c r="E79" t="str">
-        <v>abigail.williams45@yahoo.com</v>
+        <v>aurora.williams76@outlook.com</v>
       </c>
       <c r="F79" t="str">
-        <v>0403 497 445</v>
+        <v>0401 416 170</v>
       </c>
       <c r="G79" t="str">
-        <v>Toowoomba</v>
+        <v>Darwin</v>
       </c>
       <c r="H79" t="str">
         <v>C</v>
       </c>
       <c r="I79" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="M79" t="str">
+        <v>Uses walking cane</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
+        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
       </c>
       <c r="B80" t="str">
-        <v>Joshua Clark</v>
+        <v>Emily Johnson</v>
       </c>
       <c r="C80">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D80" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E80" t="str">
-        <v>joshua.clark16@outlook.com</v>
+        <v>emily.johnson58@hotmail.com</v>
       </c>
       <c r="F80" t="str">
-        <v>0403 901 485</v>
+        <v>0412 663 939</v>
       </c>
       <c r="G80" t="str">
-        <v>Sydney</v>
+        <v>Perth</v>
       </c>
       <c r="H80" t="str">
         <v>B</v>
       </c>
       <c r="I80" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>8956e289-91e9-4c15-bf2b-a13dee2fa476</v>
+        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
       </c>
       <c r="B81" t="str">
-        <v>Landon Wright</v>
+        <v>Joshua Scott</v>
       </c>
       <c r="C81">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D81" t="str">
         <v>Male</v>
       </c>
       <c r="E81" t="str">
-        <v>landon.wright36@outlook.com</v>
+        <v>joshua.scott95@outlook.com</v>
       </c>
       <c r="F81" t="str">
-        <v>0402 415 597</v>
+        <v>0410 137 561</v>
       </c>
       <c r="G81" t="str">
-        <v>Cairns</v>
+        <v>Canberra</v>
       </c>
       <c r="H81" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I81" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
+        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
       </c>
       <c r="B82" t="str">
-        <v>Theodore Allen</v>
+        <v>Lucas Thomas</v>
       </c>
       <c r="C82">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D82" t="str">
         <v>Male</v>
       </c>
       <c r="E82" t="str">
-        <v>theodore.allen25@outlook.com</v>
+        <v>lucas.thomas30@yahoo.com</v>
       </c>
       <c r="F82" t="str">
-        <v>0400 438 819</v>
+        <v>0412 527 117</v>
       </c>
       <c r="G82" t="str">
-        <v>Newcastle</v>
+        <v>Brisbane</v>
       </c>
       <c r="H82" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I82" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
+        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
       </c>
       <c r="B83" t="str">
-        <v>Christian Rivera</v>
+        <v>Joshua Jones</v>
       </c>
       <c r="C83">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="D83" t="str">
         <v>Male</v>
       </c>
       <c r="E83" t="str">
-        <v>christian.rivera86@hotmail.com</v>
+        <v>joshua.jones82@yahoo.com</v>
       </c>
       <c r="F83" t="str">
-        <v>0400 135 743</v>
+        <v>0400 652 840</v>
       </c>
       <c r="G83" t="str">
-        <v>Adelaide</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H83" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I83" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>c1783cdf-a656-46b4-9331-4d9d18d40b51</v>
+        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
       </c>
       <c r="B84" t="str">
-        <v>Aurora Walker</v>
+        <v>Joshua Walker</v>
       </c>
       <c r="C84">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D84" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E84" t="str">
-        <v>aurora.walker1@outlook.com</v>
+        <v>joshua.walker97@gmail.com</v>
       </c>
       <c r="F84" t="str">
-        <v>0403 522 404</v>
+        <v>0402 640 379</v>
       </c>
       <c r="G84" t="str">
         <v>Darwin</v>
       </c>
       <c r="H84" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I84" t="str">
-        <v>available</v>
-      </c>
-      <c r="M84" t="str">
-        <v>Vision impaired - needs assistance</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
+        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
       </c>
       <c r="B85" t="str">
-        <v>Scarlett Wright</v>
+        <v>Lily Walker</v>
       </c>
       <c r="C85">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="D85" t="str">
         <v>Female</v>
       </c>
       <c r="E85" t="str">
-        <v>scarlett.wright68@outlook.com</v>
+        <v>lily.walker96@outlook.com</v>
       </c>
       <c r="F85" t="str">
-        <v>0412 487 763</v>
+        <v>0410 155 426</v>
       </c>
       <c r="G85" t="str">
-        <v>Newcastle</v>
+        <v>Hobart</v>
       </c>
       <c r="H85" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I85" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
+        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
       </c>
       <c r="B86" t="str">
-        <v>Theodore Nelson</v>
+        <v>Liam Lewis</v>
       </c>
       <c r="C86">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D86" t="str">
         <v>Male</v>
       </c>
       <c r="E86" t="str">
-        <v>theodore.nelson79@gmail.com</v>
+        <v>liam.lewis79@yahoo.com</v>
       </c>
       <c r="F86" t="str">
-        <v>0403 813 793</v>
+        <v>0404 203 198</v>
       </c>
       <c r="G86" t="str">
-        <v>Canberra</v>
+        <v>Hobart</v>
       </c>
       <c r="H86" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I86" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
+        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
       </c>
       <c r="B87" t="str">
-        <v>Emily Johnson</v>
+        <v>Ethan Rodriguez</v>
       </c>
       <c r="C87">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="D87" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E87" t="str">
-        <v>emily.johnson58@hotmail.com</v>
+        <v>ethan.rodriguez60@hotmail.com</v>
       </c>
       <c r="F87" t="str">
-        <v>0412 663 939</v>
+        <v>0411 690 563</v>
       </c>
       <c r="G87" t="str">
-        <v>Perth</v>
+        <v>Townsville</v>
       </c>
       <c r="H87" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I87" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="M87" t="str">
+        <v>Hearing impaired - requires front row seating</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
+        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
       </c>
       <c r="B88" t="str">
-        <v>Jayden Nguyen</v>
+        <v>Stella Green</v>
       </c>
       <c r="C88">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D88" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E88" t="str">
-        <v>jayden.nguyen88@hotmail.com</v>
+        <v>stella.green92@gmail.com</v>
       </c>
       <c r="F88" t="str">
-        <v>0401 108 628</v>
+        <v>0404 230 858</v>
       </c>
       <c r="G88" t="str">
-        <v>Hobart</v>
+        <v>Wollongong</v>
       </c>
       <c r="H88" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I88" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J88" t="str">
+        <v>Everly Torres</v>
+      </c>
+      <c r="M88" t="str">
+        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
+        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
       </c>
       <c r="B89" t="str">
-        <v>Joshua Scott</v>
+        <v>Victoria Torres</v>
       </c>
       <c r="C89">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D89" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E89" t="str">
-        <v>joshua.scott95@outlook.com</v>
+        <v>victoria.torres48@outlook.com</v>
       </c>
       <c r="F89" t="str">
-        <v>0410 137 561</v>
+        <v>0411 539 271</v>
       </c>
       <c r="G89" t="str">
-        <v>Canberra</v>
+        <v>Geelong</v>
       </c>
       <c r="H89" t="str">
         <v>B</v>
       </c>
       <c r="I89" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
+        <v>7664257a-dce4-407a-8f24-692043d568be</v>
       </c>
       <c r="B90" t="str">
-        <v>Lucas Thomas</v>
+        <v>Nora Jackson</v>
       </c>
       <c r="C90">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D90" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E90" t="str">
-        <v>lucas.thomas30@yahoo.com</v>
+        <v>nora.jackson83@hotmail.com</v>
       </c>
       <c r="F90" t="str">
-        <v>0412 527 117</v>
+        <v>0404 434 899</v>
       </c>
       <c r="G90" t="str">
-        <v>Brisbane</v>
+        <v>Wollongong</v>
       </c>
       <c r="H90" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I90" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
+        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
       </c>
       <c r="B91" t="str">
-        <v>Joshua Jones</v>
+        <v>Joshua Clark</v>
       </c>
       <c r="C91">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D91" t="str">
         <v>Male</v>
       </c>
       <c r="E91" t="str">
-        <v>joshua.jones82@yahoo.com</v>
+        <v>joshua.clark16@outlook.com</v>
       </c>
       <c r="F91" t="str">
-        <v>0400 652 840</v>
+        <v>0403 901 485</v>
       </c>
       <c r="G91" t="str">
-        <v>Toowoomba</v>
+        <v>Sydney</v>
       </c>
       <c r="H91" t="str">
         <v>B</v>
       </c>
       <c r="I91" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
+        <v>8956e289-91e9-4c15-bf2b-a13dee2fa476</v>
       </c>
       <c r="B92" t="str">
-        <v>Aurora Williams</v>
+        <v>Landon Wright</v>
       </c>
       <c r="C92">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D92" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E92" t="str">
-        <v>aurora.williams76@outlook.com</v>
+        <v>landon.wright36@outlook.com</v>
       </c>
       <c r="F92" t="str">
-        <v>0401 416 170</v>
+        <v>0402 415 597</v>
       </c>
       <c r="G92" t="str">
-        <v>Darwin</v>
+        <v>Cairns</v>
       </c>
       <c r="H92" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I92" t="str">
-        <v>available</v>
-      </c>
-      <c r="M92" t="str">
-        <v>Uses walking cane</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
+        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
       </c>
       <c r="B93" t="str">
-        <v>Joshua Walker</v>
+        <v>Theodore Allen</v>
       </c>
       <c r="C93">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D93" t="str">
         <v>Male</v>
       </c>
       <c r="E93" t="str">
-        <v>joshua.walker97@gmail.com</v>
+        <v>theodore.allen25@outlook.com</v>
       </c>
       <c r="F93" t="str">
-        <v>0402 640 379</v>
+        <v>0400 438 819</v>
       </c>
       <c r="G93" t="str">
-        <v>Darwin</v>
+        <v>Newcastle</v>
       </c>
       <c r="H93" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I93" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
+        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
       </c>
       <c r="B94" t="str">
-        <v>Joshua Carter</v>
+        <v>Christian Rivera</v>
       </c>
       <c r="C94">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D94" t="str">
         <v>Male</v>
       </c>
       <c r="E94" t="str">
-        <v>joshua.carter41@hotmail.com</v>
+        <v>christian.rivera86@hotmail.com</v>
       </c>
       <c r="F94" t="str">
-        <v>0404 538 442</v>
+        <v>0400 135 743</v>
       </c>
       <c r="G94" t="str">
-        <v>Wollongong</v>
+        <v>Adelaide</v>
       </c>
       <c r="H94" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I94" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
       </c>
       <c r="B95" t="str">
-        <v>Peter Adamidis</v>
+        <v>Luke Flores</v>
       </c>
       <c r="C95">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D95" t="str">
-        <v>Not Specified</v>
+        <v>Male</v>
       </c>
       <c r="E95" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>luke.flores39@hotmail.com</v>
       </c>
       <c r="F95" t="str">
-        <v>498086080</v>
+        <v>0403 225 544</v>
       </c>
       <c r="G95" t="str">
-        <v/>
+        <v>Melbourne</v>
       </c>
       <c r="H95" t="str">
-        <v/>
+        <v>B</v>
       </c>
       <c r="I95" t="str">
         <v>assigned</v>
-      </c>
-      <c r="J95" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
-      </c>
-      <c r="K95" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L95" t="str">
-        <v>Y</v>
-      </c>
-      <c r="M95" t="str">
-        <v>Broken Leg</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>c1783cdf-a656-46b4-9331-4d9d18d40b51</v>
       </c>
       <c r="B96" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Aurora Walker</v>
       </c>
       <c r="C96">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="D96" t="str">
-        <v>Not Specified</v>
+        <v>Female</v>
       </c>
       <c r="E96" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>aurora.walker1@outlook.com</v>
       </c>
       <c r="F96" t="str">
-        <v>498086080</v>
+        <v>0403 522 404</v>
       </c>
       <c r="G96" t="str">
-        <v>Footscray</v>
+        <v>Darwin</v>
       </c>
       <c r="H96" t="str">
-        <v/>
+        <v>B+</v>
       </c>
       <c r="I96" t="str">
         <v>assigned</v>
       </c>
-      <c r="J96" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
-      </c>
-      <c r="K96" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L96" t="str">
-        <v>N</v>
-      </c>
       <c r="M96" t="str">
-        <v>N/A</v>
+        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B97" t="str">
-        <v>Lily Walker</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C97">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="D97" t="str">
-        <v>Female</v>
+        <v>Not Specified</v>
       </c>
       <c r="E97" t="str">
-        <v>lily.walker96@outlook.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F97" t="str">
-        <v>0410 155 426</v>
+        <v>498086080</v>
       </c>
       <c r="G97" t="str">
-        <v>Hobart</v>
+        <v/>
       </c>
       <c r="H97" t="str">
-        <v>B+</v>
+        <v/>
       </c>
       <c r="I97" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J97" t="str">
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+      </c>
+      <c r="K97" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L97" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M97" t="str">
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B98" t="str">
-        <v>Julian Rivera</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C98">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D98" t="str">
-        <v>Male</v>
+        <v>Not Specified</v>
       </c>
       <c r="E98" t="str">
-        <v>julian.rivera31@outlook.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F98" t="str">
-        <v>0401 414 502</v>
+        <v>498086080</v>
       </c>
       <c r="G98" t="str">
-        <v>Perth</v>
+        <v>Footscray</v>
       </c>
       <c r="H98" t="str">
-        <v>B+</v>
+        <v/>
       </c>
       <c r="I98" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J98" t="str">
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
+      </c>
+      <c r="K98" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L98" t="str">
+        <v>N</v>
+      </c>
+      <c r="M98" t="str">
+        <v>N/A</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
+        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
       </c>
       <c r="B99" t="str">
-        <v>Scarlett Lopez</v>
+        <v>Jayden Nguyen</v>
       </c>
       <c r="C99">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D99" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E99" t="str">
-        <v>scarlett.lopez53@yahoo.com</v>
+        <v>jayden.nguyen88@hotmail.com</v>
       </c>
       <c r="F99" t="str">
-        <v>0400 509 641</v>
+        <v>0401 108 628</v>
       </c>
       <c r="G99" t="str">
-        <v>Sydney</v>
+        <v>Hobart</v>
       </c>
       <c r="H99" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I99" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
       </c>
       <c r="B100" t="str">
-        <v>Ethan Taylor</v>
+        <v>Abigail Williams</v>
       </c>
       <c r="C100">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="D100" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E100" t="str">
-        <v>ethan.taylor22@yahoo.com</v>
+        <v>abigail.williams45@yahoo.com</v>
       </c>
       <c r="F100" t="str">
-        <v>0410 363 173</v>
+        <v>0403 497 445</v>
       </c>
       <c r="G100" t="str">
-        <v>Adelaide</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H100" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I100" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
+        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
       </c>
       <c r="B101" t="str">
-        <v>Liam Lewis</v>
+        <v>Joshua Carter</v>
       </c>
       <c r="C101">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="D101" t="str">
         <v>Male</v>
       </c>
       <c r="E101" t="str">
-        <v>liam.lewis79@yahoo.com</v>
+        <v>joshua.carter41@hotmail.com</v>
       </c>
       <c r="F101" t="str">
-        <v>0404 203 198</v>
+        <v>0404 538 442</v>
       </c>
       <c r="G101" t="str">
-        <v>Hobart</v>
+        <v>Wollongong</v>
       </c>
       <c r="H101" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I101" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
+        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
       </c>
       <c r="B102" t="str">
-        <v>Ethan Rodriguez</v>
+        <v>Julian Rivera</v>
       </c>
       <c r="C102">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D102" t="str">
         <v>Male</v>
       </c>
       <c r="E102" t="str">
-        <v>ethan.rodriguez60@hotmail.com</v>
+        <v>julian.rivera31@outlook.com</v>
       </c>
       <c r="F102" t="str">
-        <v>0411 690 563</v>
+        <v>0401 414 502</v>
       </c>
       <c r="G102" t="str">
-        <v>Townsville</v>
+        <v>Perth</v>
       </c>
       <c r="H102" t="str">
         <v>B+</v>
       </c>
       <c r="I102" t="str">
-        <v>available</v>
-      </c>
-      <c r="M102" t="str">
-        <v>Hearing impaired - requires front row seating</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
+        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
       </c>
       <c r="B103" t="str">
-        <v>Stella Green</v>
+        <v>Scarlett Lopez</v>
       </c>
       <c r="C103">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D103" t="str">
         <v>Female</v>
       </c>
       <c r="E103" t="str">
-        <v>stella.green92@gmail.com</v>
+        <v>scarlett.lopez53@yahoo.com</v>
       </c>
       <c r="F103" t="str">
-        <v>0404 230 858</v>
+        <v>0400 509 641</v>
       </c>
       <c r="G103" t="str">
-        <v>Wollongong</v>
+        <v>Sydney</v>
       </c>
       <c r="H103" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I103" t="str">
-        <v>available</v>
-      </c>
-      <c r="J103" t="str">
-        <v>Everly Torres</v>
-      </c>
-      <c r="M103" t="str">
-        <v>Vision impaired - needs assistance</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
+        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
       </c>
       <c r="B104" t="str">
-        <v>Luke Flores</v>
+        <v>Ethan Taylor</v>
       </c>
       <c r="C104">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="D104" t="str">
         <v>Male</v>
       </c>
       <c r="E104" t="str">
-        <v>luke.flores39@hotmail.com</v>
+        <v>ethan.taylor22@yahoo.com</v>
       </c>
       <c r="F104" t="str">
-        <v>0403 225 544</v>
+        <v>0410 363 173</v>
       </c>
       <c r="G104" t="str">
-        <v>Melbourne</v>
+        <v>Adelaide</v>
       </c>
       <c r="H104" t="str">
         <v>B</v>
       </c>
       <c r="I104" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
     </row>
   </sheetData>
@@ -3913,7 +3931,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4303,24 +4321,840 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+        <v>315d4c8e-42aa-496a-8267-35eedf823cb1</v>
       </c>
       <c r="B23" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C23" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" t="str">
         <v>A1</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>aa35cd2f-32f1-4cd5-879a-11e79202bf56</v>
+      </c>
+      <c r="B24" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C24" t="str">
+        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>1a1c989a-199f-4151-99dd-6e70ee5e964c</v>
+      </c>
+      <c r="B25" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C25" t="str">
+        <v>6591420b-4762-4d90-b738-8a5b70458c40</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>63f2b141-aa64-4b0d-8dba-6817f2ed187a</v>
+      </c>
+      <c r="B26" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C26" t="str">
+        <v>182bd5d2-7f68-4c83-b156-e80856f3b6b7</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>0b5aba6b-e20e-494f-bd3a-53ceda317bb9</v>
+      </c>
+      <c r="B27" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C27" t="str">
+        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="str">
+        <v>A5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>6aaf8d74-b0b2-43db-babc-0bd6a3714b0b</v>
+      </c>
+      <c r="B28" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C28" t="str">
+        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>d320153e-4282-4906-b685-0dd2690a81ea</v>
+      </c>
+      <c r="B29" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C29" t="str">
+        <v>7664257a-dce4-407a-8f24-692043d568be</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>db010e25-acf8-45ad-bf4a-07177997ba81</v>
+      </c>
+      <c r="B30" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C30" t="str">
+        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="str">
+        <v>B3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>4310488c-a718-40f9-a725-71d2a29db2cd</v>
+      </c>
+      <c r="B31" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C31" t="str">
+        <v>8956e289-91e9-4c15-bf2b-a13dee2fa476</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" t="str">
+        <v>B4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>977fe2a0-ee04-4a91-aef6-589e98451eac</v>
+      </c>
+      <c r="B32" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C32" t="str">
+        <v>2fa810c7-61d0-4519-a314-824cf0873e30</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="str">
+        <v>B5</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>f9c1c44a-4ff5-4be5-8c5d-3ce5e7d3dc72</v>
+      </c>
+      <c r="B33" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C33" t="str">
+        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" t="str">
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>34784079-fc4e-42a0-a64b-2618a78ed14e</v>
+      </c>
+      <c r="B34" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C34" t="str">
+        <v>c1783cdf-a656-46b4-9331-4d9d18d40b51</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" t="str">
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>b7d2981c-343a-4314-a84c-9c580ab5f103</v>
+      </c>
+      <c r="B35" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C35" t="str">
+        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="str">
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>7c8837a4-4a08-4eb6-a3c3-9566e2025f8a</v>
+      </c>
+      <c r="B36" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C36" t="str">
+        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="str">
+        <v>C4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>99dd2005-0db9-42d2-96f7-76180002a8f8</v>
+      </c>
+      <c r="B37" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C37" t="str">
+        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="str">
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>312f5f58-60ef-4019-9aff-e675f31a3b69</v>
+      </c>
+      <c r="B38" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C38" t="str">
+        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="str">
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>aefe43f9-b9f1-4442-ba0d-6f5b81cc116e</v>
+      </c>
+      <c r="B39" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C39" t="str">
+        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39" t="str">
+        <v>D3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>784583e4-16c5-415d-9898-8dda09f0e5af</v>
+      </c>
+      <c r="B40" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C40" t="str">
+        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" t="str">
+        <v>D4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>c112544f-6ac0-464e-a06d-67df85f82f33</v>
+      </c>
+      <c r="B41" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C41" t="str">
+        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" t="str">
+        <v>E1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>ed7dbbc2-1327-48a2-be28-a812aed96e81</v>
+      </c>
+      <c r="B42" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C42" t="str">
+        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="str">
+        <v>E2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>5ff58ffb-30be-40f0-9ca1-94165940b657</v>
+      </c>
+      <c r="B43" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C43" t="str">
+        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>a64425a0-0325-4b62-8079-386836efdff0</v>
+      </c>
+      <c r="B44" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C44" t="str">
+        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>129e8507-9a27-48d9-af9e-3689a8598957</v>
+      </c>
+      <c r="B45" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C45" t="str">
+        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>4962de2d-65ed-43c4-b794-87fcdd42ed1b</v>
+      </c>
+      <c r="B46" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C46" t="str">
+        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>5710f758-b224-467f-93ee-8490916c10e9</v>
+      </c>
+      <c r="B47" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C47" t="str">
+        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47" t="str">
+        <v>A5</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>854f2397-5935-4854-bd17-c06a487bb142</v>
+      </c>
+      <c r="B48" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C48" t="str">
+        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>e04bd714-ef7d-4548-adc1-f990450dedd4</v>
+      </c>
+      <c r="B49" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C49" t="str">
+        <v>5331c6bd-19f8-416a-9166-06280a3c547e</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>e5c1c785-47b5-40a3-b771-bbeb376b6581</v>
+      </c>
+      <c r="B50" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C50" t="str">
+        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50" t="str">
+        <v>B3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>dc96f223-ab88-4d41-bdb1-5054fbf412bf</v>
+      </c>
+      <c r="B51" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C51" t="str">
+        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51" t="str">
+        <v>B4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>4dbe5764-b6bc-4ae5-8ae4-2719af54b9f4</v>
+      </c>
+      <c r="B52" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C52" t="str">
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52" t="str">
+        <v>B5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>b0296a5a-9827-406e-9697-454a472f99ec</v>
+      </c>
+      <c r="B53" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C53" t="str">
+        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53" t="str">
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>9b63fe68-2861-429b-a493-7f156d82b025</v>
+      </c>
+      <c r="B54" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C54" t="str">
+        <v>992418b2-3029-4752-9552-0aa886433657</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54" t="str">
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>4a06773b-d5aa-4d39-b70a-7c909c889ea6</v>
+      </c>
+      <c r="B55" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C55" t="str">
+        <v>0669e014-c952-45fd-9791-36cbe1d51444</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55" t="str">
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>a3067e36-1e4a-4cc1-83ae-335398a1e3be</v>
+      </c>
+      <c r="B56" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C56" t="str">
+        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56" t="str">
+        <v>C4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>910ad705-cbac-4ef7-8a22-9e03c252f756</v>
+      </c>
+      <c r="B57" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C57" t="str">
+        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57" t="str">
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>ec890304-ce9c-4f6a-ba3c-1e3f6af22605</v>
+      </c>
+      <c r="B58" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C58" t="str">
+        <v>32ffeaf9-5f22-4db7-a70b-cbaab834db0d</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58" t="str">
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>f8d9a4a0-cf1c-4a4a-8892-d616fb702116</v>
+      </c>
+      <c r="B59" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C59" t="str">
+        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>d99e1cec-f16c-4e69-be58-c21b819a4358</v>
+      </c>
+      <c r="B60" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C60" t="str">
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+      </c>
+      <c r="D60">
+        <v>5</v>
+      </c>
+      <c r="E60" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>9551f680-6993-4ec3-a834-f1a32ec44ea0</v>
+      </c>
+      <c r="B61" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C61" t="str">
+        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
+      </c>
+      <c r="D61">
+        <v>5</v>
+      </c>
+      <c r="E61" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>8926a7fb-86cb-49f8-8740-1ed0caa8d18a</v>
+      </c>
+      <c r="B62" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C62" t="str">
+        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>bae2ac85-4d87-4569-a8f6-daa6c8f63088</v>
+      </c>
+      <c r="B63" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C63" t="str">
+        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63" t="str">
+        <v>A5</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>da4c4aec-70d9-4418-abbc-7a9e4a209c06</v>
+      </c>
+      <c r="B64" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C64" t="str">
+        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
+      </c>
+      <c r="D64">
+        <v>5</v>
+      </c>
+      <c r="E64" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+      </c>
+      <c r="B65" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C65" t="str">
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>105881ec-344b-423d-9ca0-5dbfc2c2ba8f</v>
+      </c>
+      <c r="B66" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C66" t="str">
+        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
+      </c>
+      <c r="D66">
+        <v>6</v>
+      </c>
+      <c r="E66" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>b90ab53e-7513-471e-9487-e490e1672e7d</v>
+      </c>
+      <c r="B67" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C67" t="str">
+        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
+      </c>
+      <c r="D67">
+        <v>6</v>
+      </c>
+      <c r="E67" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>4c838d83-e6ab-4f5e-8d16-c31da12045fd</v>
+      </c>
+      <c r="B68" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C68" t="str">
+        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
+      </c>
+      <c r="D68">
+        <v>6</v>
+      </c>
+      <c r="E68" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>7c5babfc-96ed-4aa6-8470-b7a20672ad6d</v>
+      </c>
+      <c r="B69" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C69" t="str">
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
+      </c>
+      <c r="D69">
+        <v>6</v>
+      </c>
+      <c r="E69" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>10b75cbb-714d-4a77-8f14-1efbed7f5860</v>
+      </c>
+      <c r="B70" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C70" t="str">
+        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
+      </c>
+      <c r="D70">
+        <v>6</v>
+      </c>
+      <c r="E70" t="str">
+        <v>A5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>875a2c3b-7136-4491-9777-f2ce4e647a4c</v>
+      </c>
+      <c r="B71" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C71" t="str">
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+      </c>
+      <c r="D71">
+        <v>6</v>
+      </c>
+      <c r="E71" t="str">
+        <v>B1</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H71"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Improve contestant linking logic by prioritizing group IDs and falling back to name matching
Refactors the contestant linking logic in `server/routes.ts` to use `groupId` as the primary method for resolving `attendingWith` relationships. If `groupId` is not present, it falls back to name matching but only within the current record day's assignments, and only if there is exactly one unique match to avoid false positives caused by duplicate names. The `exportedAt` timestamp in `automatic-backup.json` is also updated, and some minor adjustments are made to assignment data within the backup file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 53a85640-05ce-41cb-92f6-3a2207e7f331
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/vnGm1eg
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -8199,625 +8199,625 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>8ae073c9-2fdb-45a9-bae8-a2430dd540d1</v>
+        <v>6a4f32c6-4084-4fcd-bbd8-0a6aaa03e309</v>
       </c>
       <c r="B11" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C11" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>210066e7-58e9-4ebb-a504-dfbf383961b5</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>6a4f32c6-4084-4fcd-bbd8-0a6aaa03e309</v>
+        <v>fba90ec2-6961-46aa-873c-068db20d280c</v>
       </c>
       <c r="B12" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C12" t="str">
-        <v>210066e7-58e9-4ebb-a504-dfbf383961b5</v>
+        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>fba90ec2-6961-46aa-873c-068db20d280c</v>
+        <v>8aef956b-0e32-4fe1-b497-e4add14986b2</v>
       </c>
       <c r="B13" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C13" t="str">
-        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
+        <v>97646711-3e33-4ee9-8d83-bd6e0363ece0</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="str">
-        <v>D2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>8aef956b-0e32-4fe1-b497-e4add14986b2</v>
+        <v>fc728d42-ef5d-4d22-9365-874bb28c193c</v>
       </c>
       <c r="B14" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C14" t="str">
-        <v>97646711-3e33-4ee9-8d83-bd6e0363ece0</v>
+        <v>5c5fe7f9-35dd-4685-af6b-e44a56c1d47c</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>fc728d42-ef5d-4d22-9365-874bb28c193c</v>
+        <v>ca069f0c-64db-4114-854a-90af0ec9319c</v>
       </c>
       <c r="B15" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C15" t="str">
-        <v>5c5fe7f9-35dd-4685-af6b-e44a56c1d47c</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>ca069f0c-64db-4114-854a-90af0ec9319c</v>
+        <v>3450dbe3-0816-4fd4-98c9-f191cfe69170</v>
       </c>
       <c r="B16" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C16" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>3450dbe3-0816-4fd4-98c9-f191cfe69170</v>
+        <v>f55e9ee8-4105-4e45-b7d9-436b07c69d14</v>
       </c>
       <c r="B17" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C17" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>f55e9ee8-4105-4e45-b7d9-436b07c69d14</v>
+        <v>91050ab0-27a3-4b00-af21-683958d5322e</v>
       </c>
       <c r="B18" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C18" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" t="str">
-        <v>A3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>91050ab0-27a3-4b00-af21-683958d5322e</v>
+        <v>7d5ab531-f767-41a0-86dc-a8e27c91b8ba</v>
       </c>
       <c r="B19" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C19" t="str">
-        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19" t="str">
-        <v>B3</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>7d5ab531-f767-41a0-86dc-a8e27c91b8ba</v>
+        <v>6c545985-ac3b-47b7-ae24-ef455c260584</v>
       </c>
       <c r="B20" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C20" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="str">
-        <v>B4</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>6c545985-ac3b-47b7-ae24-ef455c260584</v>
+        <v>54351c21-bb3a-43ee-b957-d923082db8ba</v>
       </c>
       <c r="B21" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C21" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="str">
-        <v>B5</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>54351c21-bb3a-43ee-b957-d923082db8ba</v>
+        <v>89feec40-99df-4fe0-bb9f-86fe536c8212</v>
       </c>
       <c r="B22" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C22" t="str">
-        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
+        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>89feec40-99df-4fe0-bb9f-86fe536c8212</v>
+        <v>c6a9cc3d-3f73-4083-9108-5d1e95dd075a</v>
       </c>
       <c r="B23" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C23" t="str">
-        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
+        <v>6366884b-6583-493e-80bc-a1dff1926c59</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>c6a9cc3d-3f73-4083-9108-5d1e95dd075a</v>
+        <v>ffa70008-a9f8-4422-b990-f3dead129aaf</v>
       </c>
       <c r="B24" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C24" t="str">
-        <v>6366884b-6583-493e-80bc-a1dff1926c59</v>
+        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" t="str">
-        <v>C3</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>ffa70008-a9f8-4422-b990-f3dead129aaf</v>
+        <v>cb296f50-db5e-40ac-93d1-ad7af9c95e25</v>
       </c>
       <c r="B25" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C25" t="str">
-        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
+        <v>1b5fc1ce-1ed8-4255-a8a4-b02892b2b03a</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="str">
-        <v>C4</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>cb296f50-db5e-40ac-93d1-ad7af9c95e25</v>
+        <v>e185398c-fc7d-4620-abc0-17d7bc7006d0</v>
       </c>
       <c r="B26" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C26" t="str">
-        <v>1b5fc1ce-1ed8-4255-a8a4-b02892b2b03a</v>
+        <v>1a539e8e-7b02-422a-991f-99fdb84688f5</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>e185398c-fc7d-4620-abc0-17d7bc7006d0</v>
+        <v>3a343830-4df1-4493-838b-3822b7eee672</v>
       </c>
       <c r="B27" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C27" t="str">
-        <v>1a539e8e-7b02-422a-991f-99fdb84688f5</v>
+        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>3a343830-4df1-4493-838b-3822b7eee672</v>
+        <v>b9b3c857-4587-4ad3-9724-9e8bb934561f</v>
       </c>
       <c r="B28" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C28" t="str">
-        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
+        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="str">
-        <v>D3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>b9b3c857-4587-4ad3-9724-9e8bb934561f</v>
+        <v>68c19ac9-89f8-4709-b432-ffe847157616</v>
       </c>
       <c r="B29" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C29" t="str">
-        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
+        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>68c19ac9-89f8-4709-b432-ffe847157616</v>
+        <v>f2e9a5fc-e340-4671-91f2-d74d0527295b</v>
       </c>
       <c r="B30" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C30" t="str">
-        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
+        <v>f878ab7f-ae59-4af0-b19a-e9bf4573c116</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>f2e9a5fc-e340-4671-91f2-d74d0527295b</v>
+        <v>0d7ee93c-dd0c-4825-a501-b8567f7ded2d</v>
       </c>
       <c r="B31" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C31" t="str">
-        <v>f878ab7f-ae59-4af0-b19a-e9bf4573c116</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>0d7ee93c-dd0c-4825-a501-b8567f7ded2d</v>
+        <v>6d3cff7d-f4eb-45ff-a548-5a7837cb4b17</v>
       </c>
       <c r="B32" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C32" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>6d3cff7d-f4eb-45ff-a548-5a7837cb4b17</v>
+        <v>fad608df-b93b-4c14-963e-59082c8f0ced</v>
       </c>
       <c r="B33" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C33" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="D33">
         <v>3</v>
       </c>
       <c r="E33" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>fad608df-b93b-4c14-963e-59082c8f0ced</v>
+        <v>897a5cf6-21ab-49b3-992e-5f5a99ded612</v>
       </c>
       <c r="B34" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C34" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>897a5cf6-21ab-49b3-992e-5f5a99ded612</v>
+        <v>c0db21be-8cb7-462b-b734-93e936f7668c</v>
       </c>
       <c r="B35" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C35" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>c0db21be-8cb7-462b-b734-93e936f7668c</v>
+        <v>c840b9a5-0493-4cb6-a015-2960e788476c</v>
       </c>
       <c r="B36" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C36" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
       </c>
       <c r="D36">
         <v>3</v>
       </c>
       <c r="E36" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>c840b9a5-0493-4cb6-a015-2960e788476c</v>
+        <v>55df5967-7cae-45c6-aa58-55a45221da03</v>
       </c>
       <c r="B37" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C37" t="str">
-        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="D37">
         <v>3</v>
       </c>
       <c r="E37" t="str">
-        <v>B3</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>55df5967-7cae-45c6-aa58-55a45221da03</v>
+        <v>0eca0d6e-83f3-4de8-94d0-e1cd5b0a3c30</v>
       </c>
       <c r="B38" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C38" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="str">
-        <v>B4</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>0eca0d6e-83f3-4de8-94d0-e1cd5b0a3c30</v>
+        <v>fbfb1778-e8d9-45d6-9c93-4a4772ade022</v>
       </c>
       <c r="B39" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C39" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
       </c>
       <c r="D39">
         <v>3</v>
       </c>
       <c r="E39" t="str">
-        <v>B5</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>fbfb1778-e8d9-45d6-9c93-4a4772ade022</v>
+        <v>f28c4369-e7b6-4426-b541-662187618875</v>
       </c>
       <c r="B40" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C40" t="str">
-        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
+        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>f28c4369-e7b6-4426-b541-662187618875</v>
+        <v>7497a387-6e5e-43fe-ac3b-30933a32ddc9</v>
       </c>
       <c r="B41" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C41" t="str">
-        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>7497a387-6e5e-43fe-ac3b-30933a32ddc9</v>
+        <v>0faf817a-5e9b-4e5b-b185-2e2e520092de</v>
       </c>
       <c r="B42" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C42" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
       <c r="E42" t="str">
-        <v>C3</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>0faf817a-5e9b-4e5b-b185-2e2e520092de</v>
+        <v>f5055392-579d-4d29-b935-bd323849b850</v>
       </c>
       <c r="B43" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C43" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>cd2f354f-9f45-4422-af14-1c94758ec1c1</v>
       </c>
       <c r="D43">
         <v>3</v>
       </c>
       <c r="E43" t="str">
-        <v>C4</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>f5055392-579d-4d29-b935-bd323849b850</v>
+        <v>771814c8-fb5a-4414-9923-95f5cadd52a2</v>
       </c>
       <c r="B44" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C44" t="str">
-        <v>cd2f354f-9f45-4422-af14-1c94758ec1c1</v>
+        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
       </c>
       <c r="D44">
         <v>3</v>
       </c>
       <c r="E44" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>771814c8-fb5a-4414-9923-95f5cadd52a2</v>
+        <v>fa1ab0e8-4cfe-4bb5-bc34-bd6d32e3a450</v>
       </c>
       <c r="B45" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C45" t="str">
-        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
+        <v>9d6b206c-c62d-4b71-b83d-fb61ac2fd06b</v>
       </c>
       <c r="D45">
         <v>3</v>
       </c>
       <c r="E45" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>fa1ab0e8-4cfe-4bb5-bc34-bd6d32e3a450</v>
+        <v>8ae073c9-2fdb-45a9-bae8-a2430dd540d1</v>
       </c>
       <c r="B46" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C46" t="str">
-        <v>9d6b206c-c62d-4b71-b83d-fb61ac2fd06b</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E46" t="str">
-        <v>D3</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>28aa8da1-d094-49c5-93a7-3ed287f33069</v>
+        <v>13b5c13d-11b8-464c-9889-1a1bef825355</v>
       </c>
       <c r="B47" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C47" t="str">
-        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
+        <v>b9e02c2d-410d-4307-811c-7e52cf93b14b</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -8828,16 +8828,16 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>13b5c13d-11b8-464c-9889-1a1bef825355</v>
+        <v>6d481455-14e0-426a-8e3b-e3d0342f932b</v>
       </c>
       <c r="B48" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C48" t="str">
-        <v>b9e02c2d-410d-4307-811c-7e52cf93b14b</v>
+        <v>5e93a4d1-9d7c-4b53-9898-a1ae2a0319c1</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E48" t="str">
         <v>D4</v>
@@ -8845,713 +8845,713 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>6d481455-14e0-426a-8e3b-e3d0342f932b</v>
+        <v>46ab772a-b14b-4bc2-a4ff-72a1d62cd491</v>
       </c>
       <c r="B49" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C49" t="str">
-        <v>5e93a4d1-9d7c-4b53-9898-a1ae2a0319c1</v>
+        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
       </c>
       <c r="D49">
         <v>3</v>
       </c>
       <c r="E49" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>46ab772a-b14b-4bc2-a4ff-72a1d62cd491</v>
+        <v>e0fe5545-7d94-4e58-b765-424b595ef4b5</v>
       </c>
       <c r="B50" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C50" t="str">
-        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D50">
         <v>3</v>
       </c>
       <c r="E50" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>e0fe5545-7d94-4e58-b765-424b595ef4b5</v>
+        <v>1c444d0e-f8bc-400e-a191-6c4901d83e2e</v>
       </c>
       <c r="B51" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C51" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
       </c>
       <c r="D51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E51" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>1c444d0e-f8bc-400e-a191-6c4901d83e2e</v>
+        <v>3238b338-7d16-49a6-b3cb-1f58dbfc253d</v>
       </c>
       <c r="B52" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C52" t="str">
-        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
+        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
       </c>
       <c r="D52">
         <v>4</v>
       </c>
       <c r="E52" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>3238b338-7d16-49a6-b3cb-1f58dbfc253d</v>
+        <v>afe051b9-6c88-4e3c-bbcf-ed522b90a2e7</v>
       </c>
       <c r="B53" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C53" t="str">
-        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
+        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
       </c>
       <c r="D53">
         <v>4</v>
       </c>
       <c r="E53" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>afe051b9-6c88-4e3c-bbcf-ed522b90a2e7</v>
+        <v>a5806ba9-5bae-46a4-abfc-7d715f3dd948</v>
       </c>
       <c r="B54" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C54" t="str">
-        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
+        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
       </c>
       <c r="D54">
         <v>4</v>
       </c>
       <c r="E54" t="str">
-        <v>A3</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>a5806ba9-5bae-46a4-abfc-7d715f3dd948</v>
+        <v>7968c7eb-38a2-4db1-8c62-356f188b33de</v>
       </c>
       <c r="B55" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C55" t="str">
-        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
+        <v>921da7b6-596c-4a0e-a647-022bbd8cef26</v>
       </c>
       <c r="D55">
         <v>4</v>
       </c>
       <c r="E55" t="str">
-        <v>A4</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>7968c7eb-38a2-4db1-8c62-356f188b33de</v>
+        <v>5b896f9b-2042-4460-a8eb-d79e0f5489e7</v>
       </c>
       <c r="B56" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C56" t="str">
-        <v>921da7b6-596c-4a0e-a647-022bbd8cef26</v>
+        <v>8e30e99d-0594-4a73-840e-1f5ef32387ae</v>
       </c>
       <c r="D56">
         <v>4</v>
       </c>
       <c r="E56" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>5b896f9b-2042-4460-a8eb-d79e0f5489e7</v>
+        <v>6372ee13-9085-44c7-ab02-4e59826042c2</v>
       </c>
       <c r="B57" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C57" t="str">
-        <v>8e30e99d-0594-4a73-840e-1f5ef32387ae</v>
+        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
       </c>
       <c r="D57">
         <v>4</v>
       </c>
       <c r="E57" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>6372ee13-9085-44c7-ab02-4e59826042c2</v>
+        <v>094f4b46-1ba6-48b2-b9ea-fde27a3e7089</v>
       </c>
       <c r="B58" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C58" t="str">
-        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
+        <v>ba63a5c0-c76e-4c1b-b6e4-afed15dfdcd4</v>
       </c>
       <c r="D58">
         <v>4</v>
       </c>
       <c r="E58" t="str">
-        <v>B3</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>094f4b46-1ba6-48b2-b9ea-fde27a3e7089</v>
+        <v>2789a07f-04c7-4ddf-a9e5-6b62d4b6e31b</v>
       </c>
       <c r="B59" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C59" t="str">
-        <v>ba63a5c0-c76e-4c1b-b6e4-afed15dfdcd4</v>
+        <v>992418b2-3029-4752-9552-0aa886433657</v>
       </c>
       <c r="D59">
         <v>4</v>
       </c>
       <c r="E59" t="str">
-        <v>B4</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>2789a07f-04c7-4ddf-a9e5-6b62d4b6e31b</v>
+        <v>633df747-9daf-4c78-bb0d-3fa04cf57526</v>
       </c>
       <c r="B60" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C60" t="str">
-        <v>992418b2-3029-4752-9552-0aa886433657</v>
+        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
       </c>
       <c r="D60">
         <v>4</v>
       </c>
       <c r="E60" t="str">
-        <v>B5</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>633df747-9daf-4c78-bb0d-3fa04cf57526</v>
+        <v>5150a4e7-80fd-4363-ba03-0fea4d7cfc30</v>
       </c>
       <c r="B61" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C61" t="str">
-        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
       </c>
       <c r="D61">
         <v>4</v>
       </c>
       <c r="E61" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>5150a4e7-80fd-4363-ba03-0fea4d7cfc30</v>
+        <v>7c9db114-68d8-443a-b661-f971bde50222</v>
       </c>
       <c r="B62" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C62" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>0669e014-c952-45fd-9791-36cbe1d51444</v>
       </c>
       <c r="D62">
         <v>4</v>
       </c>
       <c r="E62" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>7c9db114-68d8-443a-b661-f971bde50222</v>
+        <v>746062c8-3193-4143-82b3-304bcc6035f4</v>
       </c>
       <c r="B63" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C63" t="str">
-        <v>0669e014-c952-45fd-9791-36cbe1d51444</v>
+        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
       </c>
       <c r="D63">
         <v>4</v>
       </c>
       <c r="E63" t="str">
-        <v>C3</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>746062c8-3193-4143-82b3-304bcc6035f4</v>
+        <v>85b2420e-b2f1-461b-b307-6f4e3368e1b4</v>
       </c>
       <c r="B64" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C64" t="str">
-        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="D64">
         <v>4</v>
       </c>
       <c r="E64" t="str">
-        <v>C4</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>85b2420e-b2f1-461b-b307-6f4e3368e1b4</v>
+        <v>7bfcef17-f6b6-4167-9981-5d7716473aba</v>
       </c>
       <c r="B65" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C65" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D65">
         <v>4</v>
       </c>
       <c r="E65" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>7bfcef17-f6b6-4167-9981-5d7716473aba</v>
+        <v>8e2fc035-5bd7-40a8-9128-e035fc78e774</v>
       </c>
       <c r="B66" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C66" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D66">
         <v>4</v>
       </c>
       <c r="E66" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>8e2fc035-5bd7-40a8-9128-e035fc78e774</v>
+        <v>4c87bd8e-1cb4-4326-9829-650c834a833c</v>
       </c>
       <c r="B67" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C67" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>0d8894f6-9a60-421c-a7c0-144fe2f8c85f</v>
       </c>
       <c r="D67">
         <v>4</v>
       </c>
       <c r="E67" t="str">
-        <v>D3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>4c87bd8e-1cb4-4326-9829-650c834a833c</v>
+        <v>bb968d8e-9746-4741-bafd-155a753a5dee</v>
       </c>
       <c r="B68" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C68" t="str">
-        <v>0d8894f6-9a60-421c-a7c0-144fe2f8c85f</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="D68">
         <v>4</v>
       </c>
       <c r="E68" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>bb968d8e-9746-4741-bafd-155a753a5dee</v>
+        <v>c252cf65-93f9-4569-81de-ce8f76281f5f</v>
       </c>
       <c r="B69" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C69" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>4fba0674-c979-4177-b29d-9a882e08ad0d</v>
       </c>
       <c r="D69">
         <v>4</v>
       </c>
       <c r="E69" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>c252cf65-93f9-4569-81de-ce8f76281f5f</v>
+        <v>2c776a04-80be-4ef1-b3a3-3f7032ffd211</v>
       </c>
       <c r="B70" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C70" t="str">
-        <v>4fba0674-c979-4177-b29d-9a882e08ad0d</v>
+        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
       </c>
       <c r="D70">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E70" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>2c776a04-80be-4ef1-b3a3-3f7032ffd211</v>
+        <v>b12c13c7-0971-40ad-842c-7896062d28a9</v>
       </c>
       <c r="B71" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C71" t="str">
-        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
+        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
       </c>
       <c r="D71">
         <v>5</v>
       </c>
       <c r="E71" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>b12c13c7-0971-40ad-842c-7896062d28a9</v>
+        <v>dd66fb84-b993-41ed-b13c-b0134ad5e7cd</v>
       </c>
       <c r="B72" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C72" t="str">
-        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
+        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
       </c>
       <c r="D72">
         <v>5</v>
       </c>
       <c r="E72" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>dd66fb84-b993-41ed-b13c-b0134ad5e7cd</v>
+        <v>c46d1300-2dc7-4de3-b7d9-626b3dff9249</v>
       </c>
       <c r="B73" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C73" t="str">
-        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
+        <v>55099144-967b-4cf2-b4ed-3cfe46413c92</v>
       </c>
       <c r="D73">
         <v>5</v>
       </c>
       <c r="E73" t="str">
-        <v>A3</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>c46d1300-2dc7-4de3-b7d9-626b3dff9249</v>
+        <v>9a3f50c1-674b-4206-95ec-354a542ddd9f</v>
       </c>
       <c r="B74" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C74" t="str">
-        <v>55099144-967b-4cf2-b4ed-3cfe46413c92</v>
+        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
       </c>
       <c r="D74">
         <v>5</v>
       </c>
       <c r="E74" t="str">
-        <v>A4</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>9a3f50c1-674b-4206-95ec-354a542ddd9f</v>
+        <v>90453ac4-0aab-42c5-8454-c1e546bdbdfe</v>
       </c>
       <c r="B75" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C75" t="str">
-        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
+        <v>5965e7f9-ebf0-4e66-a197-03be16110662</v>
       </c>
       <c r="D75">
         <v>5</v>
       </c>
       <c r="E75" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>90453ac4-0aab-42c5-8454-c1e546bdbdfe</v>
+        <v>c5ed3982-20b1-400b-b7e5-3f4e29f8475a</v>
       </c>
       <c r="B76" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C76" t="str">
-        <v>5965e7f9-ebf0-4e66-a197-03be16110662</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D76">
         <v>5</v>
       </c>
       <c r="E76" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>c5ed3982-20b1-400b-b7e5-3f4e29f8475a</v>
+        <v>e523b75c-4ce8-4fe6-9327-e9e61b371f45</v>
       </c>
       <c r="B77" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C77" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D77">
         <v>5</v>
       </c>
       <c r="E77" t="str">
-        <v>B3</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>e523b75c-4ce8-4fe6-9327-e9e61b371f45</v>
+        <v>0f6e877b-fbd1-4c63-bcbb-136d17d0fc29</v>
       </c>
       <c r="B78" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C78" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D78">
         <v>5</v>
       </c>
       <c r="E78" t="str">
-        <v>B4</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>0f6e877b-fbd1-4c63-bcbb-136d17d0fc29</v>
+        <v>3af13ca6-b7e6-4c59-ab21-b8cc6432a36b</v>
       </c>
       <c r="B79" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C79" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
       </c>
       <c r="D79">
         <v>5</v>
       </c>
       <c r="E79" t="str">
-        <v>B5</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>3af13ca6-b7e6-4c59-ab21-b8cc6432a36b</v>
+        <v>3efab473-e43e-49f0-997a-8263c8e6b90c</v>
       </c>
       <c r="B80" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C80" t="str">
-        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
+        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
       </c>
       <c r="D80">
         <v>5</v>
       </c>
       <c r="E80" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>3efab473-e43e-49f0-997a-8263c8e6b90c</v>
+        <v>209f7473-3556-4101-9bce-f06ef19fcf16</v>
       </c>
       <c r="B81" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C81" t="str">
-        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
+        <v>bb7daa74-0f25-4289-9b11-4b838ebf5986</v>
       </c>
       <c r="D81">
         <v>5</v>
       </c>
       <c r="E81" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>209f7473-3556-4101-9bce-f06ef19fcf16</v>
+        <v>da09e6cb-e464-4adf-b13e-ce750e085870</v>
       </c>
       <c r="B82" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C82" t="str">
-        <v>bb7daa74-0f25-4289-9b11-4b838ebf5986</v>
+        <v>97620f89-d506-4934-89b6-c60208f0bb45</v>
       </c>
       <c r="D82">
         <v>5</v>
       </c>
       <c r="E82" t="str">
-        <v>C3</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>da09e6cb-e464-4adf-b13e-ce750e085870</v>
+        <v>2d4d048f-8db8-452e-a204-cd9406f3ced9</v>
       </c>
       <c r="B83" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C83" t="str">
-        <v>97620f89-d506-4934-89b6-c60208f0bb45</v>
+        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
       </c>
       <c r="D83">
         <v>5</v>
       </c>
       <c r="E83" t="str">
-        <v>C4</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>2d4d048f-8db8-452e-a204-cd9406f3ced9</v>
+        <v>9ad9cd96-4347-40c4-aed9-9b859c14742d</v>
       </c>
       <c r="B84" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C84" t="str">
-        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
+        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
       </c>
       <c r="D84">
         <v>5</v>
       </c>
       <c r="E84" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>9ad9cd96-4347-40c4-aed9-9b859c14742d</v>
+        <v>5e33e563-078a-4ecf-85f8-68ed56a48fa7</v>
       </c>
       <c r="B85" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C85" t="str">
-        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D85">
         <v>5</v>
       </c>
       <c r="E85" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>5e33e563-078a-4ecf-85f8-68ed56a48fa7</v>
+        <v>e67a7c17-267b-47e6-a3fc-f513b720b044</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
       </c>
       <c r="D86">
         <v>5</v>
       </c>
       <c r="E86" t="str">
-        <v>D3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>e67a7c17-267b-47e6-a3fc-f513b720b044</v>
+        <v>28785eaf-bc54-45a0-8e4a-19262f46fad6</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D87">
         <v>5</v>
       </c>
       <c r="E87" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>28785eaf-bc54-45a0-8e4a-19262f46fad6</v>
+        <v>c438df5b-a3c6-40b4-b893-6f2362a461fe</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
       </c>
       <c r="D88">
         <v>5</v>
       </c>
       <c r="E88" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>c438df5b-a3c6-40b4-b893-6f2362a461fe</v>
+        <v>f3240566-6e6d-4921-9488-a150f3a7700a</v>
       </c>
       <c r="B89" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C89" t="str">
-        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
+        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
       </c>
       <c r="D89">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E89" t="str">
-        <v>E2</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>f3240566-6e6d-4921-9488-a150f3a7700a</v>
+        <v>a719af9c-4c9e-466f-aa17-8de632fb55e7</v>
       </c>
       <c r="B90" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C90" t="str">
-        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E90" t="str">
         <v>A4</v>
@@ -9559,33 +9559,33 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>a719af9c-4c9e-466f-aa17-8de632fb55e7</v>
+        <v>fa7496b0-20a7-4064-84ad-355814b26567</v>
       </c>
       <c r="B91" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C91" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="D91">
         <v>3</v>
       </c>
       <c r="E91" t="str">
-        <v>A4</v>
+        <v>A5</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>fa7496b0-20a7-4064-84ad-355814b26567</v>
+        <v>06de1b62-8f26-446b-ad3c-dde81c5a0d6f</v>
       </c>
       <c r="B92" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C92" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>2450bd3d-4940-477d-8a08-abc3363fdc3a</v>
       </c>
       <c r="D92">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E92" t="str">
         <v>A5</v>
@@ -9593,16 +9593,16 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>06de1b62-8f26-446b-ad3c-dde81c5a0d6f</v>
+        <v>923170ca-7845-4dd1-ad9d-440b882bcc50</v>
       </c>
       <c r="B93" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C93" t="str">
-        <v>2450bd3d-4940-477d-8a08-abc3363fdc3a</v>
+        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
       </c>
       <c r="D93">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E93" t="str">
         <v>A5</v>
@@ -9610,87 +9610,87 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>923170ca-7845-4dd1-ad9d-440b882bcc50</v>
+        <v>965c12c4-0712-4ad9-98e8-04851b96be99</v>
       </c>
       <c r="B94" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C94" t="str">
-        <v>1df33560-ebf2-41ec-995c-52f3f1df78d5</v>
+        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
       </c>
       <c r="D94">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E94" t="str">
-        <v>A5</v>
+        <v>E4</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>965c12c4-0712-4ad9-98e8-04851b96be99</v>
+        <v>017004d5-e876-4457-8310-f4684c3fee1d</v>
       </c>
       <c r="B95" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C95" t="str">
-        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
+        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
       </c>
       <c r="D95">
         <v>4</v>
       </c>
       <c r="E95" t="str">
-        <v>E4</v>
+        <v>E3</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>017004d5-e876-4457-8310-f4684c3fee1d</v>
+        <v>a07aa251-f910-48a9-8d80-c09d726d361c</v>
       </c>
       <c r="B96" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C96" t="str">
-        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
+        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
       </c>
       <c r="D96">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E96" t="str">
-        <v>E3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>a07aa251-f910-48a9-8d80-c09d726d361c</v>
+        <v>534fa406-134f-483b-ba52-51a7fdecd1a2</v>
       </c>
       <c r="B97" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C97" t="str">
-        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
+        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
       </c>
       <c r="D97">
         <v>2</v>
       </c>
       <c r="E97" t="str">
-        <v>B2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>534fa406-134f-483b-ba52-51a7fdecd1a2</v>
+        <v>28aa8da1-d094-49c5-93a7-3ed287f33069</v>
       </c>
       <c r="B98" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C98" t="str">
-        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
+        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
       </c>
       <c r="D98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E98" t="str">
-        <v>B1</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="99">

</xml_diff>

<commit_message>
Update contestant ratings from C to B throughout the system
Removes "C" audition rating from schema, updates backup data by replacing "C" ratings with empty strings, and modifies contestant entries in the backup data, effectively removing "C" ratings.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f14cfbce-1dfc-4e32-b7f2-b6ab090302de
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/tFIh0qo
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -742,7 +742,7 @@
         <v>B</v>
       </c>
       <c r="I2" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J2" t="str">
         <v>Violet Hall</v>
@@ -1870,34 +1870,43 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="B38" t="str">
-        <v>Victoria Carter</v>
+        <v>Felicity Parker-Hill</v>
       </c>
       <c r="C38">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D38" t="str">
-        <v>Female</v>
+        <v>Not Specified</v>
       </c>
       <c r="E38" t="str">
-        <v>victoria.carter86@hotmail.com</v>
+        <v>felicity.parkerhill@endemolshine.com.au</v>
       </c>
       <c r="F38" t="str">
-        <v>(576) 929-4509</v>
+        <v>498086080</v>
       </c>
       <c r="G38" t="str">
-        <v>Long Beach</v>
+        <v>Melbourne</v>
       </c>
       <c r="H38" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="I38" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J38" t="str">
-        <v>Josiah Lopez, Ella Martinez</v>
+        <v>Peter Adamidis, Kathleen Reynolds</v>
+      </c>
+      <c r="K38" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L38" t="str">
+        <v>N</v>
+      </c>
+      <c r="M38" t="str">
+        <v>N/A</v>
       </c>
     </row>
     <row r="39">
@@ -2019,7 +2028,7 @@
         <v>C</v>
       </c>
       <c r="I42" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J42" t="str">
         <v>Emilia Thompson</v>
@@ -2027,159 +2036,150 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>e897bbe7-50a2-441c-9ba2-0d1c40619f32</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="B43" t="str">
-        <v>Chloe Williams</v>
+        <v>Ella Martinez</v>
       </c>
       <c r="C43">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D43" t="str">
         <v>Female</v>
       </c>
       <c r="E43" t="str">
-        <v>chloe.williams70@hotmail.com</v>
+        <v>ella.martinez67@hotmail.com</v>
       </c>
       <c r="F43" t="str">
-        <v>(398) 161-2308</v>
+        <v>(703) 898-3990</v>
       </c>
       <c r="G43" t="str">
-        <v>Los Angeles</v>
+        <v>Burbank</v>
       </c>
       <c r="H43" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I43" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J43" t="str">
+        <v>Josiah Lopez, Victoria Carter</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>6366884b-6583-493e-80bc-a1dff1926c59</v>
       </c>
       <c r="B44" t="str">
-        <v>Felicity Parker-Hill</v>
+        <v>Eleanor Allen</v>
       </c>
       <c r="C44">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="D44" t="str">
-        <v>Not Specified</v>
+        <v>Female</v>
       </c>
       <c r="E44" t="str">
-        <v>felicity.parkerhill@endemolshine.com.au</v>
+        <v>eleanor.allen67@outlook.com</v>
       </c>
       <c r="F44" t="str">
-        <v>498086080</v>
+        <v>(510) 261-1846</v>
       </c>
       <c r="G44" t="str">
-        <v>Melbourne</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H44" t="str">
-        <v/>
+        <v>A</v>
       </c>
       <c r="I44" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J44" t="str">
-        <v>Peter Adamidis, Kathleen Reynolds</v>
-      </c>
-      <c r="K44" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L44" t="str">
-        <v>N</v>
-      </c>
-      <c r="M44" t="str">
-        <v>N/A</v>
+        <v>Christopher Allen</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>6366884b-6583-493e-80bc-a1dff1926c59</v>
+        <v>e897bbe7-50a2-441c-9ba2-0d1c40619f32</v>
       </c>
       <c r="B45" t="str">
-        <v>Eleanor Allen</v>
+        <v>Chloe Williams</v>
       </c>
       <c r="C45">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D45" t="str">
         <v>Female</v>
       </c>
       <c r="E45" t="str">
-        <v>eleanor.allen67@outlook.com</v>
+        <v>chloe.williams70@hotmail.com</v>
       </c>
       <c r="F45" t="str">
-        <v>(510) 261-1846</v>
+        <v>(398) 161-2308</v>
       </c>
       <c r="G45" t="str">
         <v>Los Angeles</v>
       </c>
       <c r="H45" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I45" t="str">
         <v>available</v>
-      </c>
-      <c r="J45" t="str">
-        <v>Christopher Allen</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="B46" t="str">
-        <v>Naomi Moore</v>
+        <v>Victoria Carter</v>
       </c>
       <c r="C46">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D46" t="str">
         <v>Female</v>
       </c>
       <c r="E46" t="str">
-        <v>naomi.moore30@gmail.com</v>
+        <v>victoria.carter86@hotmail.com</v>
       </c>
       <c r="F46" t="str">
-        <v>(391) 998-1729</v>
+        <v>(576) 929-4509</v>
       </c>
       <c r="G46" t="str">
-        <v>Irvine</v>
+        <v>Long Beach</v>
       </c>
       <c r="H46" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I46" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J46" t="str">
-        <v>Isla Wright, Cora Roberts</v>
+        <v>Josiah Lopez, Ella Martinez</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="B47" t="str">
-        <v>Carter Harris</v>
+        <v>Naomi Moore</v>
       </c>
       <c r="C47">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D47" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E47" t="str">
-        <v>carter.harris82@yahoo.com</v>
+        <v>naomi.moore30@gmail.com</v>
       </c>
       <c r="F47" t="str">
-        <v>0412 175 744</v>
+        <v>(391) 998-1729</v>
       </c>
       <c r="G47" t="str">
-        <v>Geelong</v>
+        <v>Irvine</v>
       </c>
       <c r="H47" t="str">
         <v>C</v>
@@ -2187,28 +2187,31 @@
       <c r="I47" t="str">
         <v>available</v>
       </c>
+      <c r="J47" t="str">
+        <v>Isla Wright, Cora Roberts</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
       </c>
       <c r="B48" t="str">
-        <v>Noah Hernandez</v>
+        <v>Carter Harris</v>
       </c>
       <c r="C48">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D48" t="str">
         <v>Male</v>
       </c>
       <c r="E48" t="str">
-        <v>noah.hernandez9@hotmail.com</v>
+        <v>carter.harris82@yahoo.com</v>
       </c>
       <c r="F48" t="str">
-        <v>0404 855 230</v>
+        <v>0412 175 744</v>
       </c>
       <c r="G48" t="str">
-        <v>Cairns</v>
+        <v>Geelong</v>
       </c>
       <c r="H48" t="str">
         <v>C</v>
@@ -2219,86 +2222,86 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>49e2abec-5fbc-4b4e-9147-fc29f4df9e48</v>
+        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
       </c>
       <c r="B49" t="str">
-        <v>Ellie Allen</v>
+        <v>Noah Hernandez</v>
       </c>
       <c r="C49">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D49" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E49" t="str">
-        <v>ellie.allen18@hotmail.com</v>
+        <v>noah.hernandez9@hotmail.com</v>
       </c>
       <c r="F49" t="str">
-        <v>(303) 763-9138</v>
+        <v>0404 855 230</v>
       </c>
       <c r="G49" t="str">
-        <v>Stockton</v>
+        <v>Cairns</v>
       </c>
       <c r="H49" t="str">
-        <v>A+</v>
+        <v>C</v>
       </c>
       <c r="I49" t="str">
         <v>available</v>
-      </c>
-      <c r="J49" t="str">
-        <v>Emma Torres, Charlotte Hernandez</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
+        <v>49e2abec-5fbc-4b4e-9147-fc29f4df9e48</v>
       </c>
       <c r="B50" t="str">
-        <v>Nathan Allen</v>
+        <v>Ellie Allen</v>
       </c>
       <c r="C50">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D50" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E50" t="str">
-        <v>nathan.allen87@outlook.com</v>
+        <v>ellie.allen18@hotmail.com</v>
       </c>
       <c r="F50" t="str">
-        <v>0403 587 263</v>
+        <v>(303) 763-9138</v>
       </c>
       <c r="G50" t="str">
-        <v>Adelaide</v>
+        <v>Stockton</v>
       </c>
       <c r="H50" t="str">
-        <v>B+</v>
+        <v>A+</v>
       </c>
       <c r="I50" t="str">
         <v>available</v>
+      </c>
+      <c r="J50" t="str">
+        <v>Emma Torres, Charlotte Hernandez</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
       </c>
       <c r="B51" t="str">
-        <v>Aria Lopez</v>
+        <v>Nathan Allen</v>
       </c>
       <c r="C51">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D51" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E51" t="str">
-        <v>aria.lopez55@hotmail.com</v>
+        <v>nathan.allen87@outlook.com</v>
       </c>
       <c r="F51" t="str">
-        <v>0404 812 491</v>
+        <v>0403 587 263</v>
       </c>
       <c r="G51" t="str">
-        <v>Sydney</v>
+        <v>Adelaide</v>
       </c>
       <c r="H51" t="str">
         <v>B+</v>
@@ -2306,95 +2309,92 @@
       <c r="I51" t="str">
         <v>available</v>
       </c>
-      <c r="J51" t="str">
-        <v>Paisley Lee</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="B52" t="str">
-        <v>Grace King</v>
+        <v>Aria Lopez</v>
       </c>
       <c r="C52">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D52" t="str">
         <v>Female</v>
       </c>
       <c r="E52" t="str">
-        <v>grace.king1@yahoo.com</v>
+        <v>aria.lopez55@hotmail.com</v>
       </c>
       <c r="F52" t="str">
-        <v>(217) 721-5651</v>
+        <v>0404 812 491</v>
       </c>
       <c r="G52" t="str">
-        <v>Oakland</v>
+        <v>Sydney</v>
       </c>
       <c r="H52" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I52" t="str">
         <v>available</v>
       </c>
       <c r="J52" t="str">
-        <v>Gianna Hill</v>
+        <v>Paisley Lee</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
+        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
       </c>
       <c r="B53" t="str">
-        <v>Emilia Lopez</v>
+        <v>Grace King</v>
       </c>
       <c r="C53">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D53" t="str">
         <v>Female</v>
       </c>
       <c r="E53" t="str">
-        <v>emilia.lopez21@gmail.com</v>
+        <v>grace.king1@yahoo.com</v>
       </c>
       <c r="F53" t="str">
-        <v>0403 491 553</v>
+        <v>(217) 721-5651</v>
       </c>
       <c r="G53" t="str">
-        <v>Cairns</v>
+        <v>Oakland</v>
       </c>
       <c r="H53" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I53" t="str">
         <v>available</v>
       </c>
       <c r="J53" t="str">
-        <v>Aurora Rodriguez</v>
+        <v>Gianna Hill</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>c5fdfaeb-862e-43ab-bf0e-ff3e14e5dbb3</v>
+        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
       </c>
       <c r="B54" t="str">
-        <v>Hannah Martin</v>
+        <v>Emilia Lopez</v>
       </c>
       <c r="C54">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D54" t="str">
         <v>Female</v>
       </c>
       <c r="E54" t="str">
-        <v>hannah.martin78@yahoo.com</v>
+        <v>emilia.lopez21@gmail.com</v>
       </c>
       <c r="F54" t="str">
-        <v>0410 940 985</v>
+        <v>0403 491 553</v>
       </c>
       <c r="G54" t="str">
-        <v>Hobart</v>
+        <v>Cairns</v>
       </c>
       <c r="H54" t="str">
         <v>B</v>
@@ -2403,62 +2403,62 @@
         <v>available</v>
       </c>
       <c r="J54" t="str">
-        <v>Abigail Lee</v>
+        <v>Aurora Rodriguez</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
+        <v>c5fdfaeb-862e-43ab-bf0e-ff3e14e5dbb3</v>
       </c>
       <c r="B55" t="str">
-        <v>Stella Garcia</v>
+        <v>Hannah Martin</v>
       </c>
       <c r="C55">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="D55" t="str">
         <v>Female</v>
       </c>
       <c r="E55" t="str">
-        <v>stella.garcia89@hotmail.com</v>
+        <v>hannah.martin78@yahoo.com</v>
       </c>
       <c r="F55" t="str">
-        <v>0403 655 540</v>
+        <v>0410 940 985</v>
       </c>
       <c r="G55" t="str">
-        <v>Toowoomba</v>
+        <v>Hobart</v>
       </c>
       <c r="H55" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I55" t="str">
         <v>available</v>
       </c>
       <c r="J55" t="str">
-        <v>Emily Thomas</v>
+        <v>Abigail Lee</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
+        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
       </c>
       <c r="B56" t="str">
-        <v>Victoria Carter</v>
+        <v>Stella Garcia</v>
       </c>
       <c r="C56">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D56" t="str">
         <v>Female</v>
       </c>
       <c r="E56" t="str">
-        <v>victoria.carter74@gmail.com</v>
+        <v>stella.garcia89@hotmail.com</v>
       </c>
       <c r="F56" t="str">
-        <v>0411 641 632</v>
+        <v>0403 655 540</v>
       </c>
       <c r="G56" t="str">
-        <v>Gold Coast</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H56" t="str">
         <v>B+</v>
@@ -2467,94 +2467,94 @@
         <v>available</v>
       </c>
       <c r="J56" t="str">
-        <v>Emilia Miller</v>
+        <v>Emily Thomas</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
+        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
       </c>
       <c r="B57" t="str">
-        <v>Zoey Cook</v>
+        <v>Victoria Carter</v>
       </c>
       <c r="C57">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D57" t="str">
         <v>Female</v>
       </c>
       <c r="E57" t="str">
-        <v>zoey.cook63@yahoo.com</v>
+        <v>victoria.carter74@gmail.com</v>
       </c>
       <c r="F57" t="str">
-        <v>(559) 803-4092</v>
+        <v>0411 641 632</v>
       </c>
       <c r="G57" t="str">
-        <v>Fremont</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H57" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I57" t="str">
         <v>available</v>
       </c>
       <c r="J57" t="str">
-        <v>Hunter Scott</v>
+        <v>Emilia Miller</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
+        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
       </c>
       <c r="B58" t="str">
-        <v>Paisley Scott</v>
+        <v>Zoey Cook</v>
       </c>
       <c r="C58">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D58" t="str">
         <v>Female</v>
       </c>
       <c r="E58" t="str">
-        <v>paisley.scott78@yahoo.com</v>
+        <v>zoey.cook63@yahoo.com</v>
       </c>
       <c r="F58" t="str">
-        <v>0410 215 419</v>
+        <v>(559) 803-4092</v>
       </c>
       <c r="G58" t="str">
-        <v>Ballarat</v>
+        <v>Fremont</v>
       </c>
       <c r="H58" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I58" t="str">
         <v>available</v>
       </c>
       <c r="J58" t="str">
-        <v>Mia Roberts</v>
+        <v>Hunter Scott</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
+        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
       </c>
       <c r="B59" t="str">
-        <v>Abigail Jackson</v>
+        <v>Paisley Scott</v>
       </c>
       <c r="C59">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D59" t="str">
         <v>Female</v>
       </c>
       <c r="E59" t="str">
-        <v>abigail.jackson65@outlook.com</v>
+        <v>paisley.scott78@yahoo.com</v>
       </c>
       <c r="F59" t="str">
-        <v>0411 824 257</v>
+        <v>0410 215 419</v>
       </c>
       <c r="G59" t="str">
-        <v>Newcastle</v>
+        <v>Ballarat</v>
       </c>
       <c r="H59" t="str">
         <v>B+</v>
@@ -2562,98 +2562,98 @@
       <c r="I59" t="str">
         <v>available</v>
       </c>
+      <c r="J59" t="str">
+        <v>Mia Roberts</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
       </c>
       <c r="B60" t="str">
-        <v>Leah Diaz</v>
+        <v>Abigail Jackson</v>
       </c>
       <c r="C60">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D60" t="str">
         <v>Female</v>
       </c>
       <c r="E60" t="str">
-        <v>leah.diaz22@outlook.com</v>
+        <v>abigail.jackson65@outlook.com</v>
       </c>
       <c r="F60" t="str">
-        <v>(159) 664-9326</v>
+        <v>0411 824 257</v>
       </c>
       <c r="G60" t="str">
-        <v>Glendale</v>
+        <v>Newcastle</v>
       </c>
       <c r="H60" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I60" t="str">
         <v>available</v>
-      </c>
-      <c r="J60" t="str">
-        <v>Julian Nguyen, Lydia Allen</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="B61" t="str">
-        <v>Mason Hill</v>
+        <v>Leah Diaz</v>
       </c>
       <c r="C61">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D61" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E61" t="str">
-        <v>mason.hill27@outlook.com</v>
+        <v>leah.diaz22@outlook.com</v>
       </c>
       <c r="F61" t="str">
-        <v>0410 682 884</v>
+        <v>(159) 664-9326</v>
       </c>
       <c r="G61" t="str">
-        <v>Canberra</v>
+        <v>Glendale</v>
       </c>
       <c r="H61" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I61" t="str">
         <v>available</v>
+      </c>
+      <c r="J61" t="str">
+        <v>Julian Nguyen, Lydia Allen</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
       </c>
       <c r="B62" t="str">
-        <v>Ella Martinez</v>
+        <v>Mason Hill</v>
       </c>
       <c r="C62">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D62" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E62" t="str">
-        <v>ella.martinez67@hotmail.com</v>
+        <v>mason.hill27@outlook.com</v>
       </c>
       <c r="F62" t="str">
-        <v>(703) 898-3990</v>
+        <v>0410 682 884</v>
       </c>
       <c r="G62" t="str">
-        <v>Burbank</v>
+        <v>Canberra</v>
       </c>
       <c r="H62" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I62" t="str">
         <v>available</v>
-      </c>
-      <c r="J62" t="str">
-        <v>Josiah Lopez, Victoria Carter</v>
       </c>
     </row>
     <row r="63">
@@ -2806,10 +2806,10 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="B68" t="str">
-        <v>Isabella Brown</v>
+        <v>Sadie Williams</v>
       </c>
       <c r="C68">
         <v>55</v>
@@ -2818,77 +2818,80 @@
         <v>Female</v>
       </c>
       <c r="E68" t="str">
-        <v>isabella.brown43@outlook.com</v>
+        <v>sadie.williams7@icloud.com</v>
       </c>
       <c r="F68" t="str">
-        <v>0403 771 690</v>
+        <v>(175) 960-1387</v>
       </c>
       <c r="G68" t="str">
-        <v>Darwin</v>
+        <v>Anaheim</v>
       </c>
       <c r="H68" t="str">
         <v>B</v>
       </c>
       <c r="I68" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J68" t="str">
-        <v>Ella Anderson</v>
+        <v>Michael Campbell, Eleanor Hall</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>34685ff7-6e85-4bbd-b546-77cfe11d7f7d</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="B69" t="str">
-        <v>Grace Walker</v>
+        <v>Isabella Brown</v>
       </c>
       <c r="C69">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D69" t="str">
         <v>Female</v>
       </c>
       <c r="E69" t="str">
-        <v>grace.walker52@hotmail.com</v>
+        <v>isabella.brown43@outlook.com</v>
       </c>
       <c r="F69" t="str">
-        <v>0412 754 780</v>
+        <v>0403 771 690</v>
       </c>
       <c r="G69" t="str">
-        <v>Canberra</v>
+        <v>Darwin</v>
       </c>
       <c r="H69" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I69" t="str">
         <v>available</v>
+      </c>
+      <c r="J69" t="str">
+        <v>Ella Anderson</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>14ca564a-7d73-46a9-9bdd-e4924eac5eda</v>
+        <v>34685ff7-6e85-4bbd-b546-77cfe11d7f7d</v>
       </c>
       <c r="B70" t="str">
-        <v>Hailey Thompson</v>
+        <v>Grace Walker</v>
       </c>
       <c r="C70">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D70" t="str">
         <v>Female</v>
       </c>
       <c r="E70" t="str">
-        <v>hailey.thompson30@yahoo.com</v>
+        <v>grace.walker52@hotmail.com</v>
       </c>
       <c r="F70" t="str">
-        <v>(356) 680-9661</v>
+        <v>0412 754 780</v>
       </c>
       <c r="G70" t="str">
-        <v>Fremont</v>
+        <v>Canberra</v>
       </c>
       <c r="H70" t="str">
-        <v>B+</v>
+        <v>A+</v>
       </c>
       <c r="I70" t="str">
         <v>available</v>
@@ -2896,28 +2899,28 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
+        <v>14ca564a-7d73-46a9-9bdd-e4924eac5eda</v>
       </c>
       <c r="B71" t="str">
-        <v>Carter Hill</v>
+        <v>Hailey Thompson</v>
       </c>
       <c r="C71">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D71" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E71" t="str">
-        <v>carter.hill93@gmail.com</v>
+        <v>hailey.thompson30@yahoo.com</v>
       </c>
       <c r="F71" t="str">
-        <v>0404 349 309</v>
+        <v>(356) 680-9661</v>
       </c>
       <c r="G71" t="str">
-        <v>Newcastle</v>
+        <v>Fremont</v>
       </c>
       <c r="H71" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I71" t="str">
         <v>available</v>
@@ -2925,118 +2928,115 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>5b54b59b-b78d-4a12-906b-7f9069a82fb5</v>
+        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
       </c>
       <c r="B72" t="str">
-        <v>Amelia Lopez</v>
+        <v>Carter Hill</v>
       </c>
       <c r="C72">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D72" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E72" t="str">
-        <v>amelia.lopez92@yahoo.com</v>
+        <v>carter.hill93@gmail.com</v>
       </c>
       <c r="F72" t="str">
-        <v>(297) 700-2964</v>
+        <v>0404 349 309</v>
       </c>
       <c r="G72" t="str">
-        <v>Pomona</v>
+        <v>Newcastle</v>
       </c>
       <c r="H72" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I72" t="str">
         <v>available</v>
-      </c>
-      <c r="J72" t="str">
-        <v>Lillian Campbell</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
+        <v>5b54b59b-b78d-4a12-906b-7f9069a82fb5</v>
       </c>
       <c r="B73" t="str">
-        <v>Stella Hall</v>
+        <v>Amelia Lopez</v>
       </c>
       <c r="C73">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="D73" t="str">
         <v>Female</v>
       </c>
       <c r="E73" t="str">
-        <v>stella.hall72@gmail.com</v>
+        <v>amelia.lopez92@yahoo.com</v>
       </c>
       <c r="F73" t="str">
-        <v>0410 133 818</v>
+        <v>(297) 700-2964</v>
       </c>
       <c r="G73" t="str">
-        <v>Wollongong</v>
+        <v>Pomona</v>
       </c>
       <c r="H73" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I73" t="str">
         <v>available</v>
+      </c>
+      <c r="J73" t="str">
+        <v>Lillian Campbell</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>4f1d5a65-9d8d-4c5a-836a-f0ea71c91e56</v>
+        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
       </c>
       <c r="B74" t="str">
-        <v>Savannah Rivera</v>
+        <v>Stella Hall</v>
       </c>
       <c r="C74">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D74" t="str">
         <v>Female</v>
       </c>
       <c r="E74" t="str">
-        <v>savannah.rivera74@hotmail.com</v>
+        <v>stella.hall72@gmail.com</v>
       </c>
       <c r="F74" t="str">
-        <v>(132) 232-5005</v>
+        <v>0410 133 818</v>
       </c>
       <c r="G74" t="str">
-        <v>Stockton</v>
+        <v>Wollongong</v>
       </c>
       <c r="H74" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I74" t="str">
         <v>available</v>
-      </c>
-      <c r="J74" t="str">
-        <v>Penelope Williams</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>523bddcf-6298-42a0-b9cb-4deffb688143</v>
+        <v>4f1d5a65-9d8d-4c5a-836a-f0ea71c91e56</v>
       </c>
       <c r="B75" t="str">
-        <v>Brooklyn Rivera</v>
+        <v>Savannah Rivera</v>
       </c>
       <c r="C75">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D75" t="str">
         <v>Female</v>
       </c>
       <c r="E75" t="str">
-        <v>brooklyn.rivera69@outlook.com</v>
+        <v>savannah.rivera74@hotmail.com</v>
       </c>
       <c r="F75" t="str">
-        <v>(847) 715-1204</v>
+        <v>(132) 232-5005</v>
       </c>
       <c r="G75" t="str">
-        <v>Glendale</v>
+        <v>Stockton</v>
       </c>
       <c r="H75" t="str">
         <v>A+</v>
@@ -3045,103 +3045,103 @@
         <v>available</v>
       </c>
       <c r="J75" t="str">
-        <v>John Carter</v>
+        <v>Penelope Williams</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>cd2f354f-9f45-4422-af14-1c94758ec1c1</v>
+        <v>523bddcf-6298-42a0-b9cb-4deffb688143</v>
       </c>
       <c r="B76" t="str">
-        <v>Hannah Murphy</v>
+        <v>Brooklyn Rivera</v>
       </c>
       <c r="C76">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D76" t="str">
         <v>Female</v>
       </c>
       <c r="E76" t="str">
-        <v>hannah.murphy4@outlook.com</v>
+        <v>brooklyn.rivera69@outlook.com</v>
       </c>
       <c r="F76" t="str">
-        <v>(544) 415-8741</v>
+        <v>(847) 715-1204</v>
       </c>
       <c r="G76" t="str">
-        <v>Pomona</v>
+        <v>Glendale</v>
       </c>
       <c r="H76" t="str">
-        <v>A</v>
+        <v>A+</v>
       </c>
       <c r="I76" t="str">
         <v>available</v>
       </c>
       <c r="J76" t="str">
-        <v>Thomas Rivera</v>
+        <v>John Carter</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>cd2f354f-9f45-4422-af14-1c94758ec1c1</v>
       </c>
       <c r="B77" t="str">
-        <v>Sofia Williams</v>
+        <v>Hannah Murphy</v>
       </c>
       <c r="C77">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D77" t="str">
         <v>Female</v>
       </c>
       <c r="E77" t="str">
-        <v>sofia.williams60@outlook.com</v>
+        <v>hannah.murphy4@outlook.com</v>
       </c>
       <c r="F77" t="str">
-        <v>(745) 392-3827</v>
+        <v>(544) 415-8741</v>
       </c>
       <c r="G77" t="str">
-        <v>Newport Beach</v>
+        <v>Pomona</v>
       </c>
       <c r="H77" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I77" t="str">
         <v>available</v>
       </c>
       <c r="J77" t="str">
-        <v>Colton Harris, Sebastian Edwards</v>
+        <v>Thomas Rivera</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="B78" t="str">
-        <v>Sadie Williams</v>
+        <v>Sofia Williams</v>
       </c>
       <c r="C78">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D78" t="str">
         <v>Female</v>
       </c>
       <c r="E78" t="str">
-        <v>sadie.williams7@icloud.com</v>
+        <v>sofia.williams60@outlook.com</v>
       </c>
       <c r="F78" t="str">
-        <v>(175) 960-1387</v>
+        <v>(745) 392-3827</v>
       </c>
       <c r="G78" t="str">
-        <v>Anaheim</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H78" t="str">
         <v>B</v>
       </c>
       <c r="I78" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J78" t="str">
-        <v>Michael Campbell, Eleanor Hall</v>
+        <v>Colton Harris, Sebastian Edwards</v>
       </c>
     </row>
     <row r="79">
@@ -3998,118 +3998,121 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="B106" t="str">
-        <v>Hannah Jones</v>
+        <v>Eleanor Hall</v>
       </c>
       <c r="C106">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D106" t="str">
         <v>Female</v>
       </c>
       <c r="E106" t="str">
-        <v>hannah.jones85@yahoo.com</v>
+        <v>eleanor.hall7@yahoo.com</v>
       </c>
       <c r="F106" t="str">
-        <v>(644) 877-6251</v>
+        <v>(627) 443-5972</v>
       </c>
       <c r="G106" t="str">
-        <v>Sacramento</v>
+        <v>Stockton</v>
       </c>
       <c r="H106" t="str">
         <v>B</v>
       </c>
       <c r="I106" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J106" t="str">
-        <v>Thomas Nguyen, Henry Roberts</v>
+        <v>Michael Campbell, Sadie Williams</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
+        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
       </c>
       <c r="B107" t="str">
-        <v>Hazel Mitchell</v>
+        <v>Hannah Jones</v>
       </c>
       <c r="C107">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D107" t="str">
         <v>Female</v>
       </c>
       <c r="E107" t="str">
-        <v>hazel.mitchell91@gmail.com</v>
+        <v>hannah.jones85@yahoo.com</v>
       </c>
       <c r="F107" t="str">
-        <v>0400 683 761</v>
+        <v>(644) 877-6251</v>
       </c>
       <c r="G107" t="str">
-        <v>Perth</v>
+        <v>Sacramento</v>
       </c>
       <c r="H107" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I107" t="str">
         <v>available</v>
       </c>
       <c r="J107" t="str">
-        <v>Caroline Taylor</v>
+        <v>Thomas Nguyen, Henry Roberts</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>076ad666-a34b-4ae1-b91f-de785dbdf5ec</v>
+        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
       </c>
       <c r="B108" t="str">
-        <v>Nora Rogers</v>
+        <v>Hazel Mitchell</v>
       </c>
       <c r="C108">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D108" t="str">
         <v>Female</v>
       </c>
       <c r="E108" t="str">
-        <v>nora.rogers98@yahoo.com</v>
+        <v>hazel.mitchell91@gmail.com</v>
       </c>
       <c r="F108" t="str">
-        <v>(704) 607-6893</v>
+        <v>0400 683 761</v>
       </c>
       <c r="G108" t="str">
-        <v>Riverside</v>
+        <v>Perth</v>
       </c>
       <c r="H108" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I108" t="str">
         <v>available</v>
+      </c>
+      <c r="J108" t="str">
+        <v>Caroline Taylor</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>076ad666-a34b-4ae1-b91f-de785dbdf5ec</v>
       </c>
       <c r="B109" t="str">
-        <v>Allison Torres</v>
+        <v>Nora Rogers</v>
       </c>
       <c r="C109">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D109" t="str">
         <v>Female</v>
       </c>
       <c r="E109" t="str">
-        <v>allison.torres94@gmail.com</v>
+        <v>nora.rogers98@yahoo.com</v>
       </c>
       <c r="F109" t="str">
-        <v>(858) 153-7242</v>
+        <v>(704) 607-6893</v>
       </c>
       <c r="G109" t="str">
-        <v>Fremont</v>
+        <v>Riverside</v>
       </c>
       <c r="H109" t="str">
         <v>B</v>
@@ -4117,127 +4120,127 @@
       <c r="I109" t="str">
         <v>available</v>
       </c>
-      <c r="J109" t="str">
-        <v>Christian Rivera, Elena Green</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="B110" t="str">
-        <v>Serenity Campbell</v>
+        <v>Allison Torres</v>
       </c>
       <c r="C110">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D110" t="str">
         <v>Female</v>
       </c>
       <c r="E110" t="str">
-        <v>serenity.campbell1@yahoo.com</v>
+        <v>allison.torres94@gmail.com</v>
       </c>
       <c r="F110" t="str">
-        <v>(479) 565-5966</v>
+        <v>(858) 153-7242</v>
       </c>
       <c r="G110" t="str">
-        <v>Irvine</v>
+        <v>Fremont</v>
       </c>
       <c r="H110" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I110" t="str">
         <v>available</v>
       </c>
       <c r="J110" t="str">
-        <v>Jackson Jackson, Isaiah Green</v>
+        <v>Christian Rivera, Elena Green</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>bb7daa74-0f25-4289-9b11-4b838ebf5986</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="B111" t="str">
-        <v>Emma Torres</v>
+        <v>Serenity Campbell</v>
       </c>
       <c r="C111">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D111" t="str">
         <v>Female</v>
       </c>
       <c r="E111" t="str">
-        <v>emma.torres53@outlook.com</v>
+        <v>serenity.campbell1@yahoo.com</v>
       </c>
       <c r="F111" t="str">
-        <v>(809) 313-7642</v>
+        <v>(479) 565-5966</v>
       </c>
       <c r="G111" t="str">
-        <v>Bakersfield</v>
+        <v>Irvine</v>
       </c>
       <c r="H111" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I111" t="str">
         <v>available</v>
       </c>
       <c r="J111" t="str">
-        <v>Ellie Allen, Charlotte Hernandez</v>
+        <v>Jackson Jackson, Isaiah Green</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
+        <v>bb7daa74-0f25-4289-9b11-4b838ebf5986</v>
       </c>
       <c r="B112" t="str">
-        <v>Victoria Thompson</v>
+        <v>Emma Torres</v>
       </c>
       <c r="C112">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D112" t="str">
         <v>Female</v>
       </c>
       <c r="E112" t="str">
-        <v>victoria.thompson68@yahoo.com</v>
+        <v>emma.torres53@outlook.com</v>
       </c>
       <c r="F112" t="str">
-        <v>(793) 601-6884</v>
+        <v>(809) 313-7642</v>
       </c>
       <c r="G112" t="str">
-        <v>San Jose</v>
+        <v>Bakersfield</v>
       </c>
       <c r="H112" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I112" t="str">
         <v>available</v>
+      </c>
+      <c r="J112" t="str">
+        <v>Ellie Allen, Charlotte Hernandez</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>af09efbe-e83d-4046-8dc8-e6a06dfc0c40</v>
+        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
       </c>
       <c r="B113" t="str">
-        <v>Paisley Evans</v>
+        <v>Victoria Thompson</v>
       </c>
       <c r="C113">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D113" t="str">
         <v>Female</v>
       </c>
       <c r="E113" t="str">
-        <v>paisley.evans52@yahoo.com</v>
+        <v>victoria.thompson68@yahoo.com</v>
       </c>
       <c r="F113" t="str">
-        <v>(894) 250-9501</v>
+        <v>(793) 601-6884</v>
       </c>
       <c r="G113" t="str">
-        <v>Torrance</v>
+        <v>San Jose</v>
       </c>
       <c r="H113" t="str">
-        <v>B+</v>
+        <v>C</v>
       </c>
       <c r="I113" t="str">
         <v>available</v>
@@ -4245,28 +4248,28 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>fec80989-ab0f-471a-a4de-6c207e334f80</v>
+        <v>af09efbe-e83d-4046-8dc8-e6a06dfc0c40</v>
       </c>
       <c r="B114" t="str">
-        <v>Eliza Rivera</v>
+        <v>Paisley Evans</v>
       </c>
       <c r="C114">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D114" t="str">
         <v>Female</v>
       </c>
       <c r="E114" t="str">
-        <v>eliza.rivera29@yahoo.com</v>
+        <v>paisley.evans52@yahoo.com</v>
       </c>
       <c r="F114" t="str">
-        <v>(836) 154-6362</v>
+        <v>(894) 250-9501</v>
       </c>
       <c r="G114" t="str">
-        <v>Newport Beach</v>
+        <v>Torrance</v>
       </c>
       <c r="H114" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I114" t="str">
         <v>available</v>
@@ -4274,121 +4277,118 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>f6a281bb-caec-44cf-a596-a6e92d6e2610</v>
+        <v>fec80989-ab0f-471a-a4de-6c207e334f80</v>
       </c>
       <c r="B115" t="str">
-        <v>Leah Scott</v>
+        <v>Eliza Rivera</v>
       </c>
       <c r="C115">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D115" t="str">
         <v>Female</v>
       </c>
       <c r="E115" t="str">
-        <v>leah.scott74@gmail.com</v>
+        <v>eliza.rivera29@yahoo.com</v>
       </c>
       <c r="F115" t="str">
-        <v>0402 414 358</v>
+        <v>(836) 154-6362</v>
       </c>
       <c r="G115" t="str">
-        <v>Perth</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H115" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I115" t="str">
         <v>available</v>
-      </c>
-      <c r="J115" t="str">
-        <v>Harper Sanchez</v>
-      </c>
-      <c r="M115" t="str">
-        <v>Limited mobility - prefers ground floor seating</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>04993d9a-3a65-4d61-a0c8-591aabb2e72c</v>
+        <v>f6a281bb-caec-44cf-a596-a6e92d6e2610</v>
       </c>
       <c r="B116" t="str">
-        <v>Eliza Martinez</v>
+        <v>Leah Scott</v>
       </c>
       <c r="C116">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D116" t="str">
         <v>Female</v>
       </c>
       <c r="E116" t="str">
-        <v>eliza.martinez8@hotmail.com</v>
+        <v>leah.scott74@gmail.com</v>
       </c>
       <c r="F116" t="str">
-        <v>(881) 895-2168</v>
+        <v>0402 414 358</v>
       </c>
       <c r="G116" t="str">
-        <v>Torrance</v>
+        <v>Perth</v>
       </c>
       <c r="H116" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I116" t="str">
         <v>available</v>
+      </c>
+      <c r="J116" t="str">
+        <v>Harper Sanchez</v>
+      </c>
+      <c r="M116" t="str">
+        <v>Limited mobility - prefers ground floor seating</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>bf1fc0b1-7d88-41a5-ab6f-ee4c085fd344</v>
+        <v>04993d9a-3a65-4d61-a0c8-591aabb2e72c</v>
       </c>
       <c r="B117" t="str">
-        <v>Brooklyn Nguyen</v>
+        <v>Eliza Martinez</v>
       </c>
       <c r="C117">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D117" t="str">
         <v>Female</v>
       </c>
       <c r="E117" t="str">
-        <v>brooklyn.nguyen77@yahoo.com</v>
+        <v>eliza.martinez8@hotmail.com</v>
       </c>
       <c r="F117" t="str">
-        <v>(142) 872-1855</v>
+        <v>(881) 895-2168</v>
       </c>
       <c r="G117" t="str">
-        <v>Los Angeles</v>
+        <v>Torrance</v>
       </c>
       <c r="H117" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I117" t="str">
         <v>available</v>
-      </c>
-      <c r="J117" t="str">
-        <v>Naomi Brown</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>0fa47948-ca05-48a1-917a-bce2c13237ed</v>
+        <v>bf1fc0b1-7d88-41a5-ab6f-ee4c085fd344</v>
       </c>
       <c r="B118" t="str">
-        <v>Isabella Taylor</v>
+        <v>Brooklyn Nguyen</v>
       </c>
       <c r="C118">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D118" t="str">
         <v>Female</v>
       </c>
       <c r="E118" t="str">
-        <v>isabella.taylor65@yahoo.com</v>
+        <v>brooklyn.nguyen77@yahoo.com</v>
       </c>
       <c r="F118" t="str">
-        <v>(997) 957-4171</v>
+        <v>(142) 872-1855</v>
       </c>
       <c r="G118" t="str">
-        <v>Chula Vista</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H118" t="str">
         <v>A</v>
@@ -4396,31 +4396,34 @@
       <c r="I118" t="str">
         <v>available</v>
       </c>
+      <c r="J118" t="str">
+        <v>Naomi Brown</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>24928131-51b3-46f8-b43f-2cf989696f62</v>
+        <v>0fa47948-ca05-48a1-917a-bce2c13237ed</v>
       </c>
       <c r="B119" t="str">
-        <v>Amelia Garcia</v>
+        <v>Isabella Taylor</v>
       </c>
       <c r="C119">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D119" t="str">
         <v>Female</v>
       </c>
       <c r="E119" t="str">
-        <v>amelia.garcia16@gmail.com</v>
+        <v>isabella.taylor65@yahoo.com</v>
       </c>
       <c r="F119" t="str">
-        <v>(331) 367-3904</v>
+        <v>(997) 957-4171</v>
       </c>
       <c r="G119" t="str">
-        <v>Anaheim</v>
+        <v>Chula Vista</v>
       </c>
       <c r="H119" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I119" t="str">
         <v>available</v>
@@ -4428,57 +4431,54 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>50b098db-86f4-4a21-8425-ab03df8f7a40</v>
+        <v>24928131-51b3-46f8-b43f-2cf989696f62</v>
       </c>
       <c r="B120" t="str">
-        <v>Lillian Campbell</v>
+        <v>Amelia Garcia</v>
       </c>
       <c r="C120">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D120" t="str">
         <v>Female</v>
       </c>
       <c r="E120" t="str">
-        <v>lillian.campbell41@yahoo.com</v>
+        <v>amelia.garcia16@gmail.com</v>
       </c>
       <c r="F120" t="str">
-        <v>(945) 213-8284</v>
+        <v>(331) 367-3904</v>
       </c>
       <c r="G120" t="str">
-        <v>Pasadena</v>
+        <v>Anaheim</v>
       </c>
       <c r="H120" t="str">
-        <v>A+</v>
+        <v>B+</v>
       </c>
       <c r="I120" t="str">
         <v>available</v>
-      </c>
-      <c r="J120" t="str">
-        <v>Amelia Lopez</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>e9a3f4c7-c9ed-4fd1-a5a9-d3763ae52a55</v>
+        <v>50b098db-86f4-4a21-8425-ab03df8f7a40</v>
       </c>
       <c r="B121" t="str">
-        <v>Victoria Anderson</v>
+        <v>Lillian Campbell</v>
       </c>
       <c r="C121">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D121" t="str">
         <v>Female</v>
       </c>
       <c r="E121" t="str">
-        <v>victoria.anderson1@outlook.com</v>
+        <v>lillian.campbell41@yahoo.com</v>
       </c>
       <c r="F121" t="str">
-        <v>(622) 987-4829</v>
+        <v>(945) 213-8284</v>
       </c>
       <c r="G121" t="str">
-        <v>Sacramento</v>
+        <v>Pasadena</v>
       </c>
       <c r="H121" t="str">
         <v>A+</v>
@@ -4487,164 +4487,164 @@
         <v>available</v>
       </c>
       <c r="J121" t="str">
-        <v>Sophia Reyes</v>
+        <v>Amelia Lopez</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>9f873871-29cc-45f0-894c-c54745230689</v>
+        <v>e9a3f4c7-c9ed-4fd1-a5a9-d3763ae52a55</v>
       </c>
       <c r="B122" t="str">
-        <v>Sadie Wright</v>
+        <v>Victoria Anderson</v>
       </c>
       <c r="C122">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D122" t="str">
         <v>Female</v>
       </c>
       <c r="E122" t="str">
-        <v>sadie.wright75@hotmail.com</v>
+        <v>victoria.anderson1@outlook.com</v>
       </c>
       <c r="F122" t="str">
-        <v>(617) 145-9784</v>
+        <v>(622) 987-4829</v>
       </c>
       <c r="G122" t="str">
-        <v>Anaheim</v>
+        <v>Sacramento</v>
       </c>
       <c r="H122" t="str">
-        <v>C</v>
+        <v>A+</v>
       </c>
       <c r="I122" t="str">
         <v>available</v>
+      </c>
+      <c r="J122" t="str">
+        <v>Sophia Reyes</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>0d8894f6-9a60-421c-a7c0-144fe2f8c85f</v>
+        <v>9f873871-29cc-45f0-894c-c54745230689</v>
       </c>
       <c r="B123" t="str">
-        <v>Lydia Morris</v>
+        <v>Sadie Wright</v>
       </c>
       <c r="C123">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D123" t="str">
         <v>Female</v>
       </c>
       <c r="E123" t="str">
-        <v>lydia.morris1@gmail.com</v>
+        <v>sadie.wright75@hotmail.com</v>
       </c>
       <c r="F123" t="str">
-        <v>(565) 806-3217</v>
+        <v>(617) 145-9784</v>
       </c>
       <c r="G123" t="str">
-        <v>Burbank</v>
+        <v>Anaheim</v>
       </c>
       <c r="H123" t="str">
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="I123" t="str">
         <v>available</v>
-      </c>
-      <c r="J123" t="str">
-        <v>Logan Gomez</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>0d8894f6-9a60-421c-a7c0-144fe2f8c85f</v>
       </c>
       <c r="B124" t="str">
-        <v>Cora Mitchell</v>
+        <v>Lydia Morris</v>
       </c>
       <c r="C124">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D124" t="str">
         <v>Female</v>
       </c>
       <c r="E124" t="str">
-        <v>cora.mitchell80@icloud.com</v>
+        <v>lydia.morris1@gmail.com</v>
       </c>
       <c r="F124" t="str">
-        <v>(929) 139-3875</v>
+        <v>(565) 806-3217</v>
       </c>
       <c r="G124" t="str">
-        <v>Newport Beach</v>
+        <v>Burbank</v>
       </c>
       <c r="H124" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I124" t="str">
         <v>available</v>
       </c>
       <c r="J124" t="str">
-        <v>Christopher Carter</v>
+        <v>Logan Gomez</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="B125" t="str">
-        <v>Layla Lopez</v>
+        <v>Cora Mitchell</v>
       </c>
       <c r="C125">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D125" t="str">
         <v>Female</v>
       </c>
       <c r="E125" t="str">
-        <v>layla.lopez23@yahoo.com</v>
+        <v>cora.mitchell80@icloud.com</v>
       </c>
       <c r="F125" t="str">
-        <v>(607) 496-6102</v>
+        <v>(929) 139-3875</v>
       </c>
       <c r="G125" t="str">
-        <v>Los Angeles</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H125" t="str">
-        <v>C</v>
+        <v>B+</v>
       </c>
       <c r="I125" t="str">
         <v>available</v>
       </c>
       <c r="J125" t="str">
-        <v>Cora Lee</v>
+        <v>Christopher Carter</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
       </c>
       <c r="B126" t="str">
-        <v>Eleanor Hall</v>
+        <v>Layla Lopez</v>
       </c>
       <c r="C126">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D126" t="str">
         <v>Female</v>
       </c>
       <c r="E126" t="str">
-        <v>eleanor.hall7@yahoo.com</v>
+        <v>layla.lopez23@yahoo.com</v>
       </c>
       <c r="F126" t="str">
-        <v>(627) 443-5972</v>
+        <v>(607) 496-6102</v>
       </c>
       <c r="G126" t="str">
-        <v>Stockton</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H126" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I126" t="str">
         <v>available</v>
       </c>
       <c r="J126" t="str">
-        <v>Michael Campbell, Sadie Williams</v>
+        <v>Cora Lee</v>
       </c>
     </row>
     <row r="127">
@@ -4957,57 +4957,69 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B137" t="str">
-        <v>Julian Rivera</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C137">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D137" t="str">
-        <v>Male</v>
+        <v>Not Specified</v>
       </c>
       <c r="E137" t="str">
-        <v>julian.rivera31@outlook.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F137" t="str">
-        <v>0401 414 502</v>
+        <v>498086080</v>
       </c>
       <c r="G137" t="str">
-        <v>Perth</v>
+        <v>Footscray</v>
       </c>
       <c r="H137" t="str">
-        <v>B+</v>
+        <v/>
       </c>
       <c r="I137" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J137" t="str">
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
+      </c>
+      <c r="K137" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L137" t="str">
+        <v>N</v>
+      </c>
+      <c r="M137" t="str">
+        <v>N/A</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
+        <v>df6c0d97-fd38-4b65-8765-b11a4939bd3b</v>
       </c>
       <c r="B138" t="str">
-        <v>Lucas Thomas</v>
+        <v>Julian Rivera</v>
       </c>
       <c r="C138">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D138" t="str">
         <v>Male</v>
       </c>
       <c r="E138" t="str">
-        <v>lucas.thomas30@yahoo.com</v>
+        <v>julian.rivera31@outlook.com</v>
       </c>
       <c r="F138" t="str">
-        <v>0412 527 117</v>
+        <v>0401 414 502</v>
       </c>
       <c r="G138" t="str">
-        <v>Brisbane</v>
+        <v>Perth</v>
       </c>
       <c r="H138" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I138" t="str">
         <v>available</v>
@@ -5015,28 +5027,28 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
+        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
       </c>
       <c r="B139" t="str">
-        <v>Lily Walker</v>
+        <v>Lucas Thomas</v>
       </c>
       <c r="C139">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="D139" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E139" t="str">
-        <v>lily.walker96@outlook.com</v>
+        <v>lucas.thomas30@yahoo.com</v>
       </c>
       <c r="F139" t="str">
-        <v>0410 155 426</v>
+        <v>0412 527 117</v>
       </c>
       <c r="G139" t="str">
-        <v>Hobart</v>
+        <v>Brisbane</v>
       </c>
       <c r="H139" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I139" t="str">
         <v>available</v>
@@ -5044,22 +5056,22 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
+        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
       </c>
       <c r="B140" t="str">
-        <v>Liam Lewis</v>
+        <v>Lily Walker</v>
       </c>
       <c r="C140">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="D140" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E140" t="str">
-        <v>liam.lewis79@yahoo.com</v>
+        <v>lily.walker96@outlook.com</v>
       </c>
       <c r="F140" t="str">
-        <v>0404 203 198</v>
+        <v>0410 155 426</v>
       </c>
       <c r="G140" t="str">
         <v>Hobart</v>
@@ -5073,43 +5085,31 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
       </c>
       <c r="B141" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Liam Lewis</v>
       </c>
       <c r="C141">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D141" t="str">
-        <v>Not Specified</v>
+        <v>Male</v>
       </c>
       <c r="E141" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>liam.lewis79@yahoo.com</v>
       </c>
       <c r="F141" t="str">
-        <v>498086080</v>
+        <v>0404 203 198</v>
       </c>
       <c r="G141" t="str">
-        <v>Footscray</v>
+        <v>Hobart</v>
       </c>
       <c r="H141" t="str">
-        <v/>
+        <v>B+</v>
       </c>
       <c r="I141" t="str">
         <v>available</v>
-      </c>
-      <c r="J141" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
-      </c>
-      <c r="K141" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L141" t="str">
-        <v>N</v>
-      </c>
-      <c r="M141" t="str">
-        <v>N/A</v>
       </c>
     </row>
     <row r="142">
@@ -6229,249 +6229,249 @@
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
       </c>
       <c r="B179" t="str">
-        <v>Michael Campbell</v>
+        <v>Hannah Moore</v>
       </c>
       <c r="C179">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="D179" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E179" t="str">
-        <v>michael.campbell9@outlook.com</v>
+        <v>hannah.moore60@outlook.com</v>
       </c>
       <c r="F179" t="str">
-        <v>(176) 164-6950</v>
+        <v>(173) 685-3587</v>
       </c>
       <c r="G179" t="str">
-        <v>Glendale</v>
+        <v>Torrance</v>
       </c>
       <c r="H179" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I179" t="str">
         <v>available</v>
       </c>
       <c r="J179" t="str">
-        <v>Sadie Williams, Eleanor Hall</v>
+        <v>Alexander Campbell, Logan Nguyen</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="B180" t="str">
-        <v>Hannah Moore</v>
+        <v>Anthony Garcia</v>
       </c>
       <c r="C180">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="D180" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E180" t="str">
-        <v>hannah.moore60@outlook.com</v>
+        <v>anthony.garcia31@yahoo.com</v>
       </c>
       <c r="F180" t="str">
-        <v>(173) 685-3587</v>
+        <v>(249) 774-7265</v>
       </c>
       <c r="G180" t="str">
-        <v>Torrance</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H180" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I180" t="str">
         <v>available</v>
       </c>
       <c r="J180" t="str">
-        <v>Alexander Campbell, Logan Nguyen</v>
+        <v>Michael Johnson, Cameron Evans</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>97620f89-d506-4934-89b6-c60208f0bb45</v>
       </c>
       <c r="B181" t="str">
-        <v>Anthony Garcia</v>
+        <v>Charlotte Hernandez</v>
       </c>
       <c r="C181">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D181" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E181" t="str">
-        <v>anthony.garcia31@yahoo.com</v>
+        <v>charlotte.hernandez88@gmail.com</v>
       </c>
       <c r="F181" t="str">
-        <v>(249) 774-7265</v>
+        <v>(131) 448-5858</v>
       </c>
       <c r="G181" t="str">
-        <v>Santa Monica</v>
+        <v>San Jose</v>
       </c>
       <c r="H181" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I181" t="str">
         <v>available</v>
       </c>
       <c r="J181" t="str">
-        <v>Michael Johnson, Cameron Evans</v>
+        <v>Ellie Allen, Emma Torres</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>97620f89-d506-4934-89b6-c60208f0bb45</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="B182" t="str">
-        <v>Charlotte Hernandez</v>
+        <v>Grayson Morgan</v>
       </c>
       <c r="C182">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D182" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E182" t="str">
-        <v>charlotte.hernandez88@gmail.com</v>
+        <v>grayson.morgan95@outlook.com</v>
       </c>
       <c r="F182" t="str">
-        <v>(131) 448-5858</v>
+        <v>(524) 127-2584</v>
       </c>
       <c r="G182" t="str">
-        <v>San Jose</v>
+        <v>Irvine</v>
       </c>
       <c r="H182" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I182" t="str">
         <v>available</v>
       </c>
       <c r="J182" t="str">
-        <v>Ellie Allen, Emma Torres</v>
+        <v>Adam Hall, Valentina Morales</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
       </c>
       <c r="B183" t="str">
-        <v>Grayson Morgan</v>
+        <v>Audrey Hill</v>
       </c>
       <c r="C183">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D183" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E183" t="str">
-        <v>grayson.morgan95@outlook.com</v>
+        <v>audrey.hill20@outlook.com</v>
       </c>
       <c r="F183" t="str">
-        <v>(524) 127-2584</v>
+        <v>(688) 524-4712</v>
       </c>
       <c r="G183" t="str">
-        <v>Irvine</v>
+        <v>San Jose</v>
       </c>
       <c r="H183" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I183" t="str">
         <v>available</v>
       </c>
       <c r="J183" t="str">
-        <v>Adam Hall, Valentina Morales</v>
+        <v>Avery Taylor</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
+        <v>a1895f97-a947-4cf3-9bc3-6aa43cdc1339</v>
       </c>
       <c r="B184" t="str">
-        <v>Audrey Hill</v>
+        <v>Gabriella Smith</v>
       </c>
       <c r="C184">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D184" t="str">
         <v>Female</v>
       </c>
       <c r="E184" t="str">
-        <v>audrey.hill20@outlook.com</v>
+        <v>gabriella.smith91@hotmail.com</v>
       </c>
       <c r="F184" t="str">
-        <v>(688) 524-4712</v>
+        <v>(550) 121-2897</v>
       </c>
       <c r="G184" t="str">
-        <v>San Jose</v>
+        <v>Sacramento</v>
       </c>
       <c r="H184" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I184" t="str">
         <v>available</v>
       </c>
       <c r="J184" t="str">
-        <v>Avery Taylor</v>
+        <v>Julian Rivera</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>a1895f97-a947-4cf3-9bc3-6aa43cdc1339</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="B185" t="str">
-        <v>Gabriella Smith</v>
+        <v>Michael Campbell</v>
       </c>
       <c r="C185">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D185" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E185" t="str">
-        <v>gabriella.smith91@hotmail.com</v>
+        <v>michael.campbell9@outlook.com</v>
       </c>
       <c r="F185" t="str">
-        <v>(550) 121-2897</v>
+        <v>(176) 164-6950</v>
       </c>
       <c r="G185" t="str">
-        <v>Sacramento</v>
+        <v>Glendale</v>
       </c>
       <c r="H185" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I185" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J185" t="str">
-        <v>Julian Rivera</v>
+        <v>Sadie Williams, Eleanor Hall</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
+        <v>4fba0674-c979-4177-b29d-9a882e08ad0d</v>
       </c>
       <c r="B186" t="str">
-        <v>Christopher Allen</v>
+        <v>Autumn Lewis</v>
       </c>
       <c r="C186">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D186" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E186" t="str">
-        <v>christopher.allen60@yahoo.com</v>
+        <v>autumn.lewis97@outlook.com</v>
       </c>
       <c r="F186" t="str">
-        <v>(529) 787-8147</v>
+        <v>(841) 837-8640</v>
       </c>
       <c r="G186" t="str">
-        <v>Torrance</v>
+        <v>San Francisco</v>
       </c>
       <c r="H186" t="str">
         <v>B+</v>
@@ -6480,30 +6480,30 @@
         <v>available</v>
       </c>
       <c r="J186" t="str">
-        <v>Eleanor Allen</v>
+        <v>Noah Martinez</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>4fba0674-c979-4177-b29d-9a882e08ad0d</v>
+        <v>2450bd3d-4940-477d-8a08-abc3363fdc3a</v>
       </c>
       <c r="B187" t="str">
-        <v>Autumn Lewis</v>
+        <v>Ella Lopez</v>
       </c>
       <c r="C187">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D187" t="str">
         <v>Female</v>
       </c>
       <c r="E187" t="str">
-        <v>autumn.lewis97@outlook.com</v>
+        <v>ella.lopez65@outlook.com</v>
       </c>
       <c r="F187" t="str">
-        <v>(841) 837-8640</v>
+        <v>(192) 887-5779</v>
       </c>
       <c r="G187" t="str">
-        <v>San Francisco</v>
+        <v>Riverside</v>
       </c>
       <c r="H187" t="str">
         <v>B+</v>
@@ -6512,71 +6512,71 @@
         <v>available</v>
       </c>
       <c r="J187" t="str">
-        <v>Noah Martinez</v>
+        <v>Adam Edwards</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>2450bd3d-4940-477d-8a08-abc3363fdc3a</v>
+        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
       </c>
       <c r="B188" t="str">
-        <v>Ella Lopez</v>
+        <v>Grayson Edwards</v>
       </c>
       <c r="C188">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D188" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E188" t="str">
-        <v>ella.lopez65@outlook.com</v>
+        <v>grayson.edwards22@gmail.com</v>
       </c>
       <c r="F188" t="str">
-        <v>(192) 887-5779</v>
+        <v>(215) 129-3913</v>
       </c>
       <c r="G188" t="str">
-        <v>Riverside</v>
+        <v>Torrance</v>
       </c>
       <c r="H188" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I188" t="str">
         <v>available</v>
       </c>
       <c r="J188" t="str">
-        <v>Adam Edwards</v>
+        <v>Elizabeth Nelson, Joseph Anderson</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
+        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
       </c>
       <c r="B189" t="str">
-        <v>Grayson Edwards</v>
+        <v>Christopher Allen</v>
       </c>
       <c r="C189">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D189" t="str">
         <v>Male</v>
       </c>
       <c r="E189" t="str">
-        <v>grayson.edwards22@gmail.com</v>
+        <v>christopher.allen60@yahoo.com</v>
       </c>
       <c r="F189" t="str">
-        <v>(215) 129-3913</v>
+        <v>(529) 787-8147</v>
       </c>
       <c r="G189" t="str">
         <v>Torrance</v>
       </c>
       <c r="H189" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I189" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J189" t="str">
-        <v>Elizabeth Nelson, Joseph Anderson</v>
+        <v>Eleanor Allen</v>
       </c>
     </row>
     <row r="190">
@@ -7139,57 +7139,57 @@
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="B208" t="str">
-        <v>Colton Harris</v>
+        <v>Josiah Lopez</v>
       </c>
       <c r="C208">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D208" t="str">
         <v>Male</v>
       </c>
       <c r="E208" t="str">
-        <v>colton.harris98@icloud.com</v>
+        <v>josiah.lopez65@gmail.com</v>
       </c>
       <c r="F208" t="str">
-        <v>(583) 900-3294</v>
+        <v>(305) 140-9212</v>
       </c>
       <c r="G208" t="str">
-        <v>Newport Beach</v>
+        <v>Chula Vista</v>
       </c>
       <c r="H208" t="str">
         <v>B</v>
       </c>
       <c r="I208" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J208" t="str">
-        <v>Sebastian Edwards, Sofia Williams</v>
+        <v>Victoria Carter, Ella Martinez</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
       </c>
       <c r="B209" t="str">
-        <v>Sebastian Edwards</v>
+        <v>William Taylor</v>
       </c>
       <c r="C209">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D209" t="str">
         <v>Male</v>
       </c>
       <c r="E209" t="str">
-        <v>sebastian.edwards97@icloud.com</v>
+        <v>william.taylor84@hotmail.com</v>
       </c>
       <c r="F209" t="str">
-        <v>(348) 408-1134</v>
+        <v>(276) 538-1731</v>
       </c>
       <c r="G209" t="str">
-        <v>Los Angeles</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H209" t="str">
         <v>B</v>
@@ -7198,30 +7198,30 @@
         <v>available</v>
       </c>
       <c r="J209" t="str">
-        <v>Colton Harris, Sofia Williams</v>
+        <v>Victoria Scott</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
+        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
       </c>
       <c r="B210" t="str">
-        <v>William Taylor</v>
+        <v>Thomas Rivera</v>
       </c>
       <c r="C210">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D210" t="str">
         <v>Male</v>
       </c>
       <c r="E210" t="str">
-        <v>william.taylor84@hotmail.com</v>
+        <v>thomas.rivera13@yahoo.com</v>
       </c>
       <c r="F210" t="str">
-        <v>(276) 538-1731</v>
+        <v>(539) 243-6118</v>
       </c>
       <c r="G210" t="str">
-        <v>Newport Beach</v>
+        <v>Long Beach</v>
       </c>
       <c r="H210" t="str">
         <v>B</v>
@@ -7230,39 +7230,39 @@
         <v>available</v>
       </c>
       <c r="J210" t="str">
-        <v>Victoria Scott</v>
+        <v>Hannah Murphy</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="B211" t="str">
-        <v>Thomas Rivera</v>
+        <v>Colton Harris</v>
       </c>
       <c r="C211">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D211" t="str">
         <v>Male</v>
       </c>
       <c r="E211" t="str">
-        <v>thomas.rivera13@yahoo.com</v>
+        <v>colton.harris98@icloud.com</v>
       </c>
       <c r="F211" t="str">
-        <v>(539) 243-6118</v>
+        <v>(583) 900-3294</v>
       </c>
       <c r="G211" t="str">
-        <v>Long Beach</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H211" t="str">
         <v>B</v>
       </c>
       <c r="I211" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J211" t="str">
-        <v>Hannah Murphy</v>
+        <v>Sebastian Edwards, Sofia Williams</v>
       </c>
     </row>
     <row r="212">
@@ -7587,66 +7587,66 @@
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="B222" t="str">
-        <v>Christopher Carter</v>
+        <v>Sebastian Edwards</v>
       </c>
       <c r="C222">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D222" t="str">
         <v>Male</v>
       </c>
       <c r="E222" t="str">
-        <v>christopher.carter22@outlook.com</v>
+        <v>sebastian.edwards97@icloud.com</v>
       </c>
       <c r="F222" t="str">
-        <v>(176) 989-4341</v>
+        <v>(348) 408-1134</v>
       </c>
       <c r="G222" t="str">
         <v>Los Angeles</v>
       </c>
       <c r="H222" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I222" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J222" t="str">
-        <v>Cora Mitchell</v>
+        <v>Colton Harris, Sofia Williams</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
       </c>
       <c r="B223" t="str">
-        <v>Josiah Lopez</v>
+        <v>Christopher Carter</v>
       </c>
       <c r="C223">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D223" t="str">
         <v>Male</v>
       </c>
       <c r="E223" t="str">
-        <v>josiah.lopez65@gmail.com</v>
+        <v>christopher.carter22@outlook.com</v>
       </c>
       <c r="F223" t="str">
-        <v>(305) 140-9212</v>
+        <v>(176) 989-4341</v>
       </c>
       <c r="G223" t="str">
-        <v>Chula Vista</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H223" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="I223" t="str">
         <v>available</v>
       </c>
       <c r="J223" t="str">
-        <v>Victoria Carter, Ella Martinez</v>
+        <v>Cora Mitchell</v>
       </c>
     </row>
     <row r="224">
@@ -7683,66 +7683,57 @@
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>1a539e8e-7b02-422a-991f-99fdb84688f5</v>
       </c>
       <c r="B225" t="str">
-        <v>Peter Adamidis</v>
+        <v>Logan Lopez</v>
       </c>
       <c r="C225">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D225" t="str">
-        <v>Not Specified</v>
+        <v>Male</v>
       </c>
       <c r="E225" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>logan.lopez66@icloud.com</v>
       </c>
       <c r="F225" t="str">
-        <v>498086080</v>
+        <v>(283) 498-3157</v>
       </c>
       <c r="G225" t="str">
-        <v/>
+        <v>Burbank</v>
       </c>
       <c r="H225" t="str">
-        <v/>
+        <v>B+</v>
       </c>
       <c r="I225" t="str">
         <v>available</v>
       </c>
       <c r="J225" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
-      </c>
-      <c r="K225" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L225" t="str">
-        <v>Y</v>
-      </c>
-      <c r="M225" t="str">
-        <v>Broken Leg</v>
+        <v>Ava Mitchell</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>1a539e8e-7b02-422a-991f-99fdb84688f5</v>
+        <v>1b5fc1ce-1ed8-4255-a8a4-b02892b2b03a</v>
       </c>
       <c r="B226" t="str">
-        <v>Logan Lopez</v>
+        <v>Ava Mitchell</v>
       </c>
       <c r="C226">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D226" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E226" t="str">
-        <v>logan.lopez66@icloud.com</v>
+        <v>ava.mitchell87@icloud.com</v>
       </c>
       <c r="F226" t="str">
-        <v>(283) 498-3157</v>
+        <v>(211) 525-6721</v>
       </c>
       <c r="G226" t="str">
-        <v>Burbank</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H226" t="str">
         <v>B+</v>
@@ -7751,30 +7742,30 @@
         <v>available</v>
       </c>
       <c r="J226" t="str">
-        <v>Ava Mitchell</v>
+        <v>Logan Lopez</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>1b5fc1ce-1ed8-4255-a8a4-b02892b2b03a</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="B227" t="str">
-        <v>Ava Mitchell</v>
+        <v>Michael Johnson</v>
       </c>
       <c r="C227">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D227" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E227" t="str">
-        <v>ava.mitchell87@icloud.com</v>
+        <v>michael.johnson96@gmail.com</v>
       </c>
       <c r="F227" t="str">
-        <v>(211) 525-6721</v>
+        <v>(878) 132-4532</v>
       </c>
       <c r="G227" t="str">
-        <v>Santa Monica</v>
+        <v>Long Beach</v>
       </c>
       <c r="H227" t="str">
         <v>B+</v>
@@ -7783,30 +7774,30 @@
         <v>available</v>
       </c>
       <c r="J227" t="str">
-        <v>Logan Lopez</v>
+        <v>Anthony Garcia, Cameron Evans</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>ba63a5c0-c76e-4c1b-b6e4-afed15dfdcd4</v>
       </c>
       <c r="B228" t="str">
-        <v>Michael Johnson</v>
+        <v>Joseph Anderson</v>
       </c>
       <c r="C228">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D228" t="str">
         <v>Male</v>
       </c>
       <c r="E228" t="str">
-        <v>michael.johnson96@gmail.com</v>
+        <v>joseph.anderson2@outlook.com</v>
       </c>
       <c r="F228" t="str">
-        <v>(878) 132-4532</v>
+        <v>(433) 142-2338</v>
       </c>
       <c r="G228" t="str">
-        <v>Long Beach</v>
+        <v>Chula Vista</v>
       </c>
       <c r="H228" t="str">
         <v>B+</v>
@@ -7815,30 +7806,30 @@
         <v>available</v>
       </c>
       <c r="J228" t="str">
-        <v>Anthony Garcia, Cameron Evans</v>
+        <v>Elizabeth Nelson, Grayson Edwards</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>ba63a5c0-c76e-4c1b-b6e4-afed15dfdcd4</v>
+        <v>f878ab7f-ae59-4af0-b19a-e9bf4573c116</v>
       </c>
       <c r="B229" t="str">
-        <v>Joseph Anderson</v>
+        <v>William Allen</v>
       </c>
       <c r="C229">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D229" t="str">
         <v>Male</v>
       </c>
       <c r="E229" t="str">
-        <v>joseph.anderson2@outlook.com</v>
+        <v>william.allen62@hotmail.com</v>
       </c>
       <c r="F229" t="str">
-        <v>(433) 142-2338</v>
+        <v>(267) 463-7481</v>
       </c>
       <c r="G229" t="str">
-        <v>Chula Vista</v>
+        <v>San Jose</v>
       </c>
       <c r="H229" t="str">
         <v>B+</v>
@@ -7847,97 +7838,94 @@
         <v>available</v>
       </c>
       <c r="J229" t="str">
-        <v>Elizabeth Nelson, Grayson Edwards</v>
+        <v>Sadie Cook, Alexa Hall</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>f878ab7f-ae59-4af0-b19a-e9bf4573c116</v>
+        <v>8e30e99d-0594-4a73-840e-1f5ef32387ae</v>
       </c>
       <c r="B230" t="str">
-        <v>William Allen</v>
+        <v>Cameron Anderson</v>
       </c>
       <c r="C230">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D230" t="str">
         <v>Male</v>
       </c>
       <c r="E230" t="str">
-        <v>william.allen62@hotmail.com</v>
+        <v>cameron.anderson85@hotmail.com</v>
       </c>
       <c r="F230" t="str">
-        <v>(267) 463-7481</v>
+        <v>(960) 363-1976</v>
       </c>
       <c r="G230" t="str">
-        <v>San Jose</v>
+        <v>Glendale</v>
       </c>
       <c r="H230" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I230" t="str">
         <v>available</v>
       </c>
       <c r="J230" t="str">
-        <v>Sadie Cook, Alexa Hall</v>
+        <v>John Diaz</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>8e30e99d-0594-4a73-840e-1f5ef32387ae</v>
+        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
       </c>
       <c r="B231" t="str">
-        <v>Cameron Anderson</v>
+        <v>Cameron Lee</v>
       </c>
       <c r="C231">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D231" t="str">
         <v>Male</v>
       </c>
       <c r="E231" t="str">
-        <v>cameron.anderson85@hotmail.com</v>
+        <v>cameron.lee78@yahoo.com</v>
       </c>
       <c r="F231" t="str">
-        <v>(960) 363-1976</v>
+        <v>0404 821 708</v>
       </c>
       <c r="G231" t="str">
-        <v>Glendale</v>
+        <v>Cairns</v>
       </c>
       <c r="H231" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I231" t="str">
         <v>available</v>
-      </c>
-      <c r="J231" t="str">
-        <v>John Diaz</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
+        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
       </c>
       <c r="B232" t="str">
-        <v>Cameron Lee</v>
+        <v>Joshua Walker</v>
       </c>
       <c r="C232">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D232" t="str">
         <v>Male</v>
       </c>
       <c r="E232" t="str">
-        <v>cameron.lee78@yahoo.com</v>
+        <v>joshua.walker97@gmail.com</v>
       </c>
       <c r="F232" t="str">
-        <v>0404 821 708</v>
+        <v>0402 640 379</v>
       </c>
       <c r="G232" t="str">
-        <v>Cairns</v>
+        <v>Darwin</v>
       </c>
       <c r="H232" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I232" t="str">
         <v>available</v>
@@ -7945,63 +7933,75 @@
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
+        <v>5c5fe7f9-35dd-4685-af6b-e44a56c1d47c</v>
       </c>
       <c r="B233" t="str">
-        <v>Joshua Walker</v>
+        <v>Charlotte Johnson</v>
       </c>
       <c r="C233">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D233" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E233" t="str">
-        <v>joshua.walker97@gmail.com</v>
+        <v>charlotte.johnson36@yahoo.com</v>
       </c>
       <c r="F233" t="str">
-        <v>0402 640 379</v>
+        <v>0410 304 177</v>
       </c>
       <c r="G233" t="str">
-        <v>Darwin</v>
+        <v>Perth</v>
       </c>
       <c r="H233" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I233" t="str">
         <v>available</v>
+      </c>
+      <c r="J233" t="str">
+        <v>Audrey Martin</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>5c5fe7f9-35dd-4685-af6b-e44a56c1d47c</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B234" t="str">
-        <v>Charlotte Johnson</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C234">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="D234" t="str">
-        <v>Female</v>
+        <v>Not Specified</v>
       </c>
       <c r="E234" t="str">
-        <v>charlotte.johnson36@yahoo.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F234" t="str">
-        <v>0410 304 177</v>
+        <v>498086080</v>
       </c>
       <c r="G234" t="str">
-        <v>Perth</v>
+        <v/>
       </c>
       <c r="H234" t="str">
-        <v>A</v>
+        <v/>
       </c>
       <c r="I234" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J234" t="str">
-        <v>Audrey Martin</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+      </c>
+      <c r="K234" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L234" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M234" t="str">
+        <v>Broken Leg</v>
       </c>
     </row>
   </sheetData>
@@ -8013,7 +8013,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8063,13 +8063,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+        <v>0c9cdf6f-2744-4fa8-ac2c-7903630cc964</v>
       </c>
       <c r="B3" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -8078,9 +8078,281 @@
         <v>A1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>cdfbff11-dffb-48ca-9730-c003eafad551</v>
+      </c>
+      <c r="B4" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C4" t="str">
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>ec307a05-0c9f-4d9c-b3ac-bd2a4f90b2ca</v>
+      </c>
+      <c r="B5" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C5" t="str">
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>c6a2853e-bdf0-4b56-9115-b4cd6fae668f</v>
+      </c>
+      <c r="B6" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C6" t="str">
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>f6b07e56-eb3f-4a5e-b214-95c88bbaa0c7</v>
+      </c>
+      <c r="B7" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C7" t="str">
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>39564329-2bdc-40a0-a1f0-0f6a02ea6cc6</v>
+      </c>
+      <c r="B8" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C8" t="str">
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="str">
+        <v>B3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>84eea01a-5f44-44ff-b1b4-fb1bc6d7f92c</v>
+      </c>
+      <c r="B9" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C9" t="str">
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="str">
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>3c81026f-c7ed-4029-987b-f93d6863fc56</v>
+      </c>
+      <c r="B10" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C10" t="str">
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="str">
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>5ec7d4db-410a-43c4-bf88-be663609b7e8</v>
+      </c>
+      <c r="B11" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C11" t="str">
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="str">
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>8bcf9e67-e8d9-49ab-a577-0989cbd209dc</v>
+      </c>
+      <c r="B12" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C12" t="str">
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="str">
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>420d8ccc-a37c-4ebb-ba1d-a8e24622effa</v>
+      </c>
+      <c r="B13" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C13" t="str">
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="str">
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>7182f61e-a274-4941-8bba-9f9575dade8f</v>
+      </c>
+      <c r="B14" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C14" t="str">
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="str">
+        <v>D3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>bd86acd8-4a8e-4f43-a64f-3b91853917af</v>
+      </c>
+      <c r="B15" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C15" t="str">
+        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="str">
+        <v>E4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>47d96c97-e042-409f-adae-7dbdb75f0a1c</v>
+      </c>
+      <c r="B16" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C16" t="str">
+        <v>6366884b-6583-493e-80bc-a1dff1926c59</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="str">
+        <v>E3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>4c802f2b-1ed5-41a3-981a-8f4a01509d1e</v>
+      </c>
+      <c r="B17" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C17" t="str">
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>4bf072af-6998-44eb-96a8-c76eeb5c8947</v>
+      </c>
+      <c r="B18" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C18" t="str">
+        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="str">
+        <v>A5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+      </c>
+      <c r="B19" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C19" t="str">
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="str">
+        <v>A1</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H19"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Improve real-time updates with session-based WebSocket authentication
Adds WebSocket session authentication by parsing cookies from upgrade requests, implements client-side subscription logic in `useBookingMasterWebSocket`, and updates the backup data with new assignment entries.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: b5eaf0c6-3202-4415-a120-b06ec5af2935
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/jyPHGdw
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -68,8 +68,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8063,750 +8064,759 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>6b58308c-f80d-416c-9b6b-02f4314a33f4</v>
+        <v>de24e1b7-54f7-4944-86a8-442ceab4b214</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>A1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>ae186e42-c31d-4d22-b594-22ad500e037b</v>
+        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
       </c>
       <c r="B4" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C4" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <v>A2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>de24e1b7-54f7-4944-86a8-442ceab4b214</v>
+        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
       </c>
       <c r="B5" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C5" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="str">
-        <v>A3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
+        <v>f04ab471-1a9d-4e0c-8e4b-3d79e4d4882b</v>
       </c>
       <c r="B6" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C6" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="str">
-        <v>B1</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
       </c>
       <c r="B7" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C7" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="str">
-        <v>B2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>f04ab471-1a9d-4e0c-8e4b-3d79e4d4882b</v>
+        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
       </c>
       <c r="B8" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C8" t="str">
-        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
       </c>
       <c r="B9" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C9" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="str">
-        <v>A1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
+        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
       </c>
       <c r="B10" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C10" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="str">
-        <v>C1</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
       </c>
       <c r="B11" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C11" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="str">
-        <v>C2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
+        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
       </c>
       <c r="B12" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C12" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="str">
-        <v>C3</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
+        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
       </c>
       <c r="B13" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C13" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="str">
-        <v>D1</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
+        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
       </c>
       <c r="B14" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C14" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="str">
-        <v>D2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B15" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C15" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="str">
-        <v>D3</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
       </c>
       <c r="B16" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C16" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" t="str">
-        <v>E1</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
       </c>
       <c r="B17" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C17" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" t="str">
-        <v>E2</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
+        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
       </c>
       <c r="B18" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C18" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" t="str">
-        <v>A1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
+        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
       </c>
       <c r="B19" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C19" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19" t="str">
-        <v>A2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
+        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
       </c>
       <c r="B20" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C20" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="str">
-        <v>A3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
+        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
       </c>
       <c r="B21" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C21" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="str">
-        <v>B1</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
+        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
       </c>
       <c r="B22" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C22" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="str">
-        <v>B2</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
+        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
       </c>
       <c r="B23" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C23" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23" t="str">
-        <v>B3</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
+        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
       </c>
       <c r="B24" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C24" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" t="str">
-        <v>C1</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
+        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
       </c>
       <c r="B25" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C25" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="str">
-        <v>C2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
+        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
       </c>
       <c r="B26" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C26" t="str">
-        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="str">
-        <v>C3</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
+        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
       </c>
       <c r="B27" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C27" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="str">
-        <v>D1</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
+        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
       </c>
       <c r="B28" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C28" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="str">
-        <v>D2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
+        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
       </c>
       <c r="B29" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C29" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="str">
-        <v>D3</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
+        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
       </c>
       <c r="B30" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C30" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30" t="str">
-        <v>E1</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
+        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
       </c>
       <c r="B31" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C31" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" t="str">
-        <v>E2</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
+        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
       </c>
       <c r="B32" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C32" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" t="str">
-        <v>A1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
+        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
       </c>
       <c r="B33" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C33" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D33">
         <v>3</v>
       </c>
       <c r="E33" t="str">
-        <v>A2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
+        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
       </c>
       <c r="B34" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C34" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="str">
-        <v>A3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
+        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
       </c>
       <c r="B35" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C35" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="str">
-        <v>B1</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
+        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
       </c>
       <c r="B36" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C36" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D36">
         <v>3</v>
       </c>
       <c r="E36" t="str">
-        <v>B2</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
+        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
       </c>
       <c r="B37" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C37" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D37">
         <v>3</v>
       </c>
       <c r="E37" t="str">
-        <v>B3</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
+        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
       </c>
       <c r="B38" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C38" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="str">
-        <v>C1</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
+        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
       </c>
       <c r="B39" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C39" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
       </c>
       <c r="D39">
         <v>3</v>
       </c>
       <c r="E39" t="str">
-        <v>C2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
+        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
       </c>
       <c r="B40" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C40" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" t="str">
-        <v>C3</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
+        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
       </c>
       <c r="B41" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C41" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="str">
-        <v>D1</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
+        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
       </c>
       <c r="B42" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C42" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
       <c r="E42" t="str">
-        <v>D2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
+        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
       </c>
       <c r="B43" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C43" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
       </c>
       <c r="D43">
         <v>3</v>
       </c>
       <c r="E43" t="str">
-        <v>D3</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
+        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
       </c>
       <c r="B44" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C44" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E44" t="str">
-        <v>E1</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
+        <v>ae186e42-c31d-4d22-b594-22ad500e037b</v>
       </c>
       <c r="B45" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C45" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E45" t="str">
-        <v>E2</v>
+        <v>A2</v>
+      </c>
+      <c r="F45" s="1">
+        <v>46000.530885277774</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
+        <v>6b58308c-f80d-416c-9b6b-02f4314a33f4</v>
       </c>
       <c r="B46" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C46" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" t="str">
-        <v>A4</v>
+        <v>A1</v>
+      </c>
+      <c r="F46" s="1">
+        <v>46000.52605988426</v>
+      </c>
+      <c r="G46" s="1">
+        <v>46000.52717275463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add real-time synchronization for collaborative booking management
Implement WebSocket-based real-time synchronization for the booking master page, allowing multiple users to view and update information simultaneously without conflicts, and update documentation.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: d4c52227-271c-4332-8fe4-457bc2117fea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/jyPHGdw
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -8064,759 +8064,762 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>de24e1b7-54f7-4944-86a8-442ceab4b214</v>
+        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
+        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
       </c>
       <c r="B4" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C4" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
+        <v>f04ab471-1a9d-4e0c-8e4b-3d79e4d4882b</v>
       </c>
       <c r="B5" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C5" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>f04ab471-1a9d-4e0c-8e4b-3d79e4d4882b</v>
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
       </c>
       <c r="B6" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C6" t="str">
-        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="str">
-        <v>B3</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
       </c>
       <c r="B7" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C7" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="str">
-        <v>A1</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
+        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
       </c>
       <c r="B8" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C8" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
       </c>
       <c r="B9" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C9" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
+        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
       </c>
       <c r="B10" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C10" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
+        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
       </c>
       <c r="B11" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C11" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
+        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
       </c>
       <c r="B12" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C12" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
+        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
       </c>
       <c r="B13" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C13" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="str">
-        <v>D3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B14" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C14" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
       </c>
       <c r="B15" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C15" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
+        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
       </c>
       <c r="B16" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C16" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
+        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
       </c>
       <c r="B17" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C17" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
+        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
       </c>
       <c r="B18" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C18" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
+        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
       </c>
       <c r="B19" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C19" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
+        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
       </c>
       <c r="B20" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C20" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
+        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
       </c>
       <c r="B21" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C21" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
+        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
       </c>
       <c r="B22" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C22" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
+        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
       </c>
       <c r="B23" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C23" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
+        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
       </c>
       <c r="B24" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C24" t="str">
-        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
+        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
       </c>
       <c r="B25" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C25" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
+        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
       </c>
       <c r="B26" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C26" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
+        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
       </c>
       <c r="B27" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C27" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="str">
-        <v>D3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
+        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
       </c>
       <c r="B28" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C28" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
+        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
       </c>
       <c r="B29" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C29" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E29" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
+        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
       </c>
       <c r="B30" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C30" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D30">
         <v>3</v>
       </c>
       <c r="E30" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
+        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
       </c>
       <c r="B31" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C31" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D31">
         <v>3</v>
       </c>
       <c r="E31" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
+        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
       </c>
       <c r="B32" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C32" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
+        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
       </c>
       <c r="B33" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C33" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D33">
         <v>3</v>
       </c>
       <c r="E33" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
+        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
       </c>
       <c r="B34" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C34" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
+        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
       </c>
       <c r="B35" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C35" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
+        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
       </c>
       <c r="B36" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C36" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D36">
         <v>3</v>
       </c>
       <c r="E36" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
+        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
       </c>
       <c r="B37" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C37" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="D37">
         <v>3</v>
       </c>
       <c r="E37" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
+        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
       </c>
       <c r="B38" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C38" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
+        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
       </c>
       <c r="B39" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C39" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="D39">
         <v>3</v>
       </c>
       <c r="E39" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
+        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
       </c>
       <c r="B40" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C40" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
+        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
       </c>
       <c r="B41" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C41" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="str">
-        <v>D3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
+        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
       </c>
       <c r="B42" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C42" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
       <c r="E42" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
+        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
       </c>
       <c r="B43" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C43" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" t="str">
-        <v>E2</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
+        <v>6b58308c-f80d-416c-9b6b-02f4314a33f4</v>
       </c>
       <c r="B44" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C44" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44" t="str">
-        <v>A4</v>
+        <v>A1</v>
+      </c>
+      <c r="F44" s="1">
+        <v>46000.52605988426</v>
+      </c>
+      <c r="G44" s="1">
+        <v>46000.52717275463</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>ae186e42-c31d-4d22-b594-22ad500e037b</v>
+        <v>de24e1b7-54f7-4944-86a8-442ceab4b214</v>
       </c>
       <c r="B45" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C45" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
       <c r="F45" s="1">
-        <v>46000.530885277774</v>
+        <v>46000.53318922454</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>6b58308c-f80d-416c-9b6b-02f4314a33f4</v>
+        <v>ae186e42-c31d-4d22-b594-22ad500e037b</v>
       </c>
       <c r="B46" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C46" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
       <c r="F46" s="1">
-        <v>46000.52605988426</v>
-      </c>
-      <c r="G46" s="1">
-        <v>46000.52717275463</v>
+        <v>46000.530885277774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update contestant booking and record day export data
Update `exportedAt` timestamp, add `bookingEmailSent` for a contestant, and re-add a deleted contestant record to the backup file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: d1af2bc7-3d8a-48db-b679-2b5f5d890f68
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/jyPHGdw
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -8061,6 +8061,9 @@
       <c r="E2" t="str">
         <v>A2</v>
       </c>
+      <c r="F2" s="1">
+        <v>46000.53846564815</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -8115,648 +8118,651 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
       </c>
       <c r="B6" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C6" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="str">
-        <v>A1</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
+        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
       </c>
       <c r="B7" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C7" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
       </c>
       <c r="B8" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C8" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
+        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
       </c>
       <c r="B9" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C9" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
+        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
       </c>
       <c r="B10" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C10" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
+        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
       </c>
       <c r="B11" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C11" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
+        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
       </c>
       <c r="B12" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C12" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="str">
-        <v>D3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B13" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C13" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
       </c>
       <c r="B14" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C14" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
+        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
       </c>
       <c r="B15" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C15" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
+        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
       </c>
       <c r="B16" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C16" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
+        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
       </c>
       <c r="B17" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C17" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
+        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
       </c>
       <c r="B18" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C18" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
+        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
       </c>
       <c r="B19" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C19" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
+        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
       </c>
       <c r="B20" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C20" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
+        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
       </c>
       <c r="B21" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C21" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
+        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
       </c>
       <c r="B22" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C22" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
+        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
       </c>
       <c r="B23" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C23" t="str">
-        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
+        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
       </c>
       <c r="B24" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C24" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
+        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
       </c>
       <c r="B25" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C25" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
+        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
       </c>
       <c r="B26" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C26" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="str">
-        <v>D3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
+        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
       </c>
       <c r="B27" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C27" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
+        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
       </c>
       <c r="B28" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C28" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
+        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
       </c>
       <c r="B29" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C29" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D29">
         <v>3</v>
       </c>
       <c r="E29" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
+        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
       </c>
       <c r="B30" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C30" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D30">
         <v>3</v>
       </c>
       <c r="E30" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
+        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
       </c>
       <c r="B31" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C31" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D31">
         <v>3</v>
       </c>
       <c r="E31" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
+        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
       </c>
       <c r="B32" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C32" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
+        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
       </c>
       <c r="B33" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C33" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D33">
         <v>3</v>
       </c>
       <c r="E33" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
+        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
       </c>
       <c r="B34" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C34" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
+        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
       </c>
       <c r="B35" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C35" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
+        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
       </c>
       <c r="B36" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C36" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="D36">
         <v>3</v>
       </c>
       <c r="E36" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
+        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
       </c>
       <c r="B37" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C37" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
       </c>
       <c r="D37">
         <v>3</v>
       </c>
       <c r="E37" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
+        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
       </c>
       <c r="B38" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C38" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
+        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
       </c>
       <c r="B39" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C39" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="D39">
         <v>3</v>
       </c>
       <c r="E39" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
+        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
       </c>
       <c r="B40" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C40" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" t="str">
-        <v>D3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
+        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
       </c>
       <c r="B41" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C41" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
+        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
       </c>
       <c r="B42" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C42" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E42" t="str">
-        <v>E2</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
       </c>
       <c r="B43" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C43" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" t="str">
-        <v>A4</v>
+        <v>A1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>46000.538291944446</v>
       </c>
     </row>
     <row r="44">

</xml_diff>

<commit_message>
Add RX number input to winning money section and update database schema
Update modal and API to include RX number for seat assignments, and add rxNumber column to schema.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: a88af82a-e1f0-4b52-8537-379dfa834f82
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/EIw7CQ6
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -8398,36 +8398,36 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>6b58308c-f80d-416c-9b6b-02f4314a33f4</v>
+        <v>ae186e42-c31d-4d22-b594-22ad500e037b</v>
       </c>
       <c r="B22" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C22" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="str">
-        <v>B1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>ae186e42-c31d-4d22-b594-22ad500e037b</v>
+        <v>6b58308c-f80d-416c-9b6b-02f4314a33f4</v>
       </c>
       <c r="B23" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C23" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="str">
-        <v>B2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="24">
@@ -8750,7 +8750,7 @@
         <v>1</v>
       </c>
       <c r="E42" t="str">
-        <v>A3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="43">
@@ -8767,7 +8767,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="str">
-        <v>B3</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="44">
@@ -9438,87 +9438,87 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
+        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
       </c>
       <c r="B83" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C83" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="str">
-        <v>A2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
+        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
       </c>
       <c r="B84" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C84" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
       <c r="E84" t="str">
-        <v>D1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
       </c>
       <c r="B85" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C85" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D85">
         <v>1</v>
       </c>
       <c r="E85" t="str">
-        <v>E1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
+        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86" t="str">
-        <v>D2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
+        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="str">
-        <v>C3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="88">
@@ -9535,7 +9535,7 @@
         <v>1</v>
       </c>
       <c r="E88" t="str">
-        <v>A1</v>
+        <v>B1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include winning money details in seat assignment data
Add rxNumber, caseNumber, winningMoneyRole, and winningMoneyAmount to the API GET response for seat assignments in server/routes.ts.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 5f94e531-5ec0-4821-ae75-05fa345cfd07
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/EIw7CQ6
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -8789,753 +8789,753 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
       </c>
       <c r="B45" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C45" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45" t="str">
-        <v>C2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
+        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
       </c>
       <c r="B46" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C46" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46" t="str">
-        <v>D3</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
       </c>
       <c r="B47" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C47" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E47" t="str">
-        <v>E2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
+        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
       </c>
       <c r="B48" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C48" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
       <c r="E48" t="str">
-        <v>A1</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
+        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
       </c>
       <c r="B49" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C49" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D49">
         <v>2</v>
       </c>
       <c r="E49" t="str">
-        <v>A2</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
+        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
       </c>
       <c r="B50" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C50" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D50">
         <v>2</v>
       </c>
       <c r="E50" t="str">
-        <v>A3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
+        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
       </c>
       <c r="B51" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C51" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51" t="str">
-        <v>B1</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
+        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
       </c>
       <c r="B52" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C52" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="D52">
         <v>2</v>
       </c>
       <c r="E52" t="str">
-        <v>B2</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
+        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
       </c>
       <c r="B53" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C53" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
       </c>
       <c r="D53">
         <v>2</v>
       </c>
       <c r="E53" t="str">
-        <v>B3</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
+        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
       </c>
       <c r="B54" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C54" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D54">
         <v>2</v>
       </c>
       <c r="E54" t="str">
-        <v>C1</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
+        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
       </c>
       <c r="B55" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C55" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D55">
         <v>2</v>
       </c>
       <c r="E55" t="str">
-        <v>C2</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
+        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
       </c>
       <c r="B56" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C56" t="str">
-        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
       <c r="E56" t="str">
-        <v>C3</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
+        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
       </c>
       <c r="B57" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C57" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="D57">
         <v>2</v>
       </c>
       <c r="E57" t="str">
-        <v>D1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
+        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
       </c>
       <c r="B58" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C58" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="D58">
         <v>2</v>
       </c>
       <c r="E58" t="str">
-        <v>D2</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
+        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
       </c>
       <c r="B59" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C59" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E59" t="str">
-        <v>D3</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
+        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
       </c>
       <c r="B60" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C60" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E60" t="str">
-        <v>E1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
+        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
       </c>
       <c r="B61" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C61" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E61" t="str">
-        <v>E2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
+        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
       </c>
       <c r="B62" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C62" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D62">
         <v>3</v>
       </c>
       <c r="E62" t="str">
-        <v>A1</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
+        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
       </c>
       <c r="B63" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C63" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D63">
         <v>3</v>
       </c>
       <c r="E63" t="str">
-        <v>A2</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
+        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
       </c>
       <c r="B64" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C64" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D64">
         <v>3</v>
       </c>
       <c r="E64" t="str">
-        <v>A3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
+        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
       </c>
       <c r="B65" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C65" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D65">
         <v>3</v>
       </c>
       <c r="E65" t="str">
-        <v>B1</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
+        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
       </c>
       <c r="B66" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C66" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D66">
         <v>3</v>
       </c>
       <c r="E66" t="str">
-        <v>B2</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
+        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
       </c>
       <c r="B67" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C67" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="D67">
         <v>3</v>
       </c>
       <c r="E67" t="str">
-        <v>B3</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
+        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
       </c>
       <c r="B68" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C68" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
       </c>
       <c r="D68">
         <v>3</v>
       </c>
       <c r="E68" t="str">
-        <v>C1</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
+        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
       </c>
       <c r="B69" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C69" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="D69">
         <v>3</v>
       </c>
       <c r="E69" t="str">
-        <v>C2</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
+        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
       </c>
       <c r="B70" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C70" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="D70">
         <v>3</v>
       </c>
       <c r="E70" t="str">
-        <v>C3</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
+        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
       </c>
       <c r="B71" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C71" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
       </c>
       <c r="D71">
         <v>3</v>
       </c>
       <c r="E71" t="str">
-        <v>D1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
+        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
       </c>
       <c r="B72" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C72" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
       </c>
       <c r="D72">
         <v>3</v>
       </c>
       <c r="E72" t="str">
-        <v>D2</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
+        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
       </c>
       <c r="B73" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C73" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
       </c>
       <c r="D73">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E73" t="str">
-        <v>D3</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
       </c>
       <c r="B74" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C74" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E74" t="str">
-        <v>E1</v>
+        <v>A1</v>
+      </c>
+      <c r="F74" s="1">
+        <v>46000.538291944446</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
+        <v>e914a306-fff3-4997-a092-87302be1bda0</v>
       </c>
       <c r="B75" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C75" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
       </c>
       <c r="D75">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E75" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
+        <v>64318131-3a36-4d14-a6ce-2699b7013fe5</v>
       </c>
       <c r="B76" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C76" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E76" t="str">
-        <v>A4</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+        <v>3b230921-6709-4bb4-b5dc-fd764580c535</v>
       </c>
       <c r="B77" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C77" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77" t="str">
-        <v>A1</v>
-      </c>
-      <c r="F77" s="1">
-        <v>46000.538291944446</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>e914a306-fff3-4997-a092-87302be1bda0</v>
+        <v>8fd02704-d4d6-498b-a9f9-66180b64176b</v>
       </c>
       <c r="B78" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C78" t="str">
-        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78" t="str">
-        <v>A1</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>64318131-3a36-4d14-a6ce-2699b7013fe5</v>
+        <v>40079e20-52ad-4652-afcd-333795a7592d</v>
       </c>
       <c r="B79" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C79" t="str">
-        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79" t="str">
-        <v>A2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>3b230921-6709-4bb4-b5dc-fd764580c535</v>
+        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
       </c>
       <c r="B80" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C80" t="str">
-        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="str">
-        <v>A3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>8fd02704-d4d6-498b-a9f9-66180b64176b</v>
+        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
       </c>
       <c r="B81" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C81" t="str">
-        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" t="str">
-        <v>A4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>40079e20-52ad-4652-afcd-333795a7592d</v>
+        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
       </c>
       <c r="B82" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C82" t="str">
-        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="E82" t="str">
-        <v>B1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
+        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
       </c>
       <c r="B83" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C83" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="str">
-        <v>D1</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
       </c>
       <c r="B84" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C84" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
       <c r="E84" t="str">
-        <v>E1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
+        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
       </c>
       <c r="B85" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C85" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="D85">
         <v>1</v>
       </c>
       <c r="E85" t="str">
-        <v>D2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
+        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86" t="str">
-        <v>C3</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
+        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="str">
-        <v>B2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88" t="str">
-        <v>B1</v>
+        <v>E2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add contestant names to the winning money modal
Update WinningMoneyModal to accept and display contestantName prop.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 0d37e4e8-8049-4c8c-91dd-ed2eda5e8d4e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/EIw7CQ6
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9506,36 +9506,36 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="str">
-        <v>D3</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88" t="str">
-        <v>E2</v>
+        <v>D3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve winners display by preventing data caching and adding logging
Add Cache-Control headers to /api/seat-assignments/with-winning-money to prevent HTTP caching and ensure fresh data retrieval, alongside console logging for debugging.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 59619525-e659-4326-bd50-5f4334a064db
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/EIw7CQ6
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9489,36 +9489,36 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86" t="str">
-        <v>C2</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="str">
-        <v>E2</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="88">

</xml_diff>

<commit_message>
Fix display of winner information and improve data filtering logic
Adjusted the filtering logic for winners data to ensure both a valid role and amount are present, and added cache-busting headers to the routes. Also updated the automatic backup data to reflect current winning information.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f37ba160-9a26-4750-a512-5bd6d049fca2
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/8ul6HS6
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9404,19 +9404,19 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B81" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C81" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="82">
@@ -9489,19 +9489,19 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86" t="str">
-        <v>E2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="87">

</xml_diff>

<commit_message>
Show contestants who have won money on the winners page
Modify the winners endpoint to query the database directly for contestants with winning money, exporting the database connection and explicitly selecting required columns.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: cf90e706-419f-481b-94ef-c45aee5791d1
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/8ul6HS6
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9404,19 +9404,19 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
       </c>
       <c r="B81" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C81" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" t="str">
-        <v>E2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="82">
@@ -9489,53 +9489,53 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="str">
-        <v>C2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
+        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88" t="str">
-        <v>D3</v>
+        <v>C2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix winners page data display by correcting API route order
Correct the order of API routes to properly fetch data for the winners page and update documentation.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: cf0cfd9f-45fb-4a62-9ac1-6bac7ddfc6ea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/VSLkcOO
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -8959,336 +8959,339 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
+        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
       </c>
       <c r="B55" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C55" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D55">
         <v>2</v>
       </c>
       <c r="E55" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
+        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
       </c>
       <c r="B56" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C56" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
       <c r="E56" t="str">
-        <v>D3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
+        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
       </c>
       <c r="B57" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C57" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="D57">
         <v>2</v>
       </c>
       <c r="E57" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
+        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
       </c>
       <c r="B58" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C58" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E58" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
+        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
       </c>
       <c r="B59" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C59" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D59">
         <v>3</v>
       </c>
       <c r="E59" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
+        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
       </c>
       <c r="B60" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C60" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D60">
         <v>3</v>
       </c>
       <c r="E60" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
+        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
       </c>
       <c r="B61" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C61" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D61">
         <v>3</v>
       </c>
       <c r="E61" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
+        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
       </c>
       <c r="B62" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C62" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D62">
         <v>3</v>
       </c>
       <c r="E62" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
+        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
       </c>
       <c r="B63" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C63" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D63">
         <v>3</v>
       </c>
       <c r="E63" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
+        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
       </c>
       <c r="B64" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C64" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D64">
         <v>3</v>
       </c>
       <c r="E64" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
+        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
       </c>
       <c r="B65" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C65" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D65">
         <v>3</v>
       </c>
       <c r="E65" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
+        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
       </c>
       <c r="B66" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C66" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="D66">
         <v>3</v>
       </c>
       <c r="E66" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
+        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
       </c>
       <c r="B67" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C67" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
       </c>
       <c r="D67">
         <v>3</v>
       </c>
       <c r="E67" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
+        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
       </c>
       <c r="B68" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C68" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="D68">
         <v>3</v>
       </c>
       <c r="E68" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
+        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
       </c>
       <c r="B69" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C69" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="D69">
         <v>3</v>
       </c>
       <c r="E69" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
+        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
       </c>
       <c r="B70" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C70" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
       </c>
       <c r="D70">
         <v>3</v>
       </c>
       <c r="E70" t="str">
-        <v>D3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
+        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
       </c>
       <c r="B71" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C71" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
       </c>
       <c r="D71">
         <v>3</v>
       </c>
       <c r="E71" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
+        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
       </c>
       <c r="B72" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C72" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
       </c>
       <c r="D72">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E72" t="str">
-        <v>E2</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
       </c>
       <c r="B73" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C73" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="D73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E73" t="str">
-        <v>A4</v>
+        <v>A1</v>
+      </c>
+      <c r="F73" s="1">
+        <v>46000.538291944446</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+        <v>e914a306-fff3-4997-a092-87302be1bda0</v>
       </c>
       <c r="B74" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C74" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -9296,212 +9299,209 @@
       <c r="E74" t="str">
         <v>A1</v>
       </c>
-      <c r="F74" s="1">
-        <v>46000.538291944446</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>e914a306-fff3-4997-a092-87302be1bda0</v>
+        <v>64318131-3a36-4d14-a6ce-2699b7013fe5</v>
       </c>
       <c r="B75" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C75" t="str">
-        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>64318131-3a36-4d14-a6ce-2699b7013fe5</v>
+        <v>3b230921-6709-4bb4-b5dc-fd764580c535</v>
       </c>
       <c r="B76" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C76" t="str">
-        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>3b230921-6709-4bb4-b5dc-fd764580c535</v>
+        <v>8fd02704-d4d6-498b-a9f9-66180b64176b</v>
       </c>
       <c r="B77" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C77" t="str">
-        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
+        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77" t="str">
-        <v>A3</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>8fd02704-d4d6-498b-a9f9-66180b64176b</v>
+        <v>40079e20-52ad-4652-afcd-333795a7592d</v>
       </c>
       <c r="B78" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C78" t="str">
-        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78" t="str">
-        <v>A4</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>40079e20-52ad-4652-afcd-333795a7592d</v>
+        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
       </c>
       <c r="B79" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C79" t="str">
-        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79" t="str">
-        <v>B1</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
+        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
       </c>
       <c r="B80" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C80" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="str">
-        <v>D1</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
+        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
       </c>
       <c r="B81" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C81" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" t="str">
-        <v>D3</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
+        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
       </c>
       <c r="B82" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C82" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="E82" t="str">
-        <v>D2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
+        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
       </c>
       <c r="B83" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C83" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="str">
-        <v>C3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
+        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
       </c>
       <c r="B84" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C84" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
       <c r="E84" t="str">
-        <v>B2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B85" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C85" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D85">
         <v>1</v>
       </c>
       <c r="E85" t="str">
-        <v>B1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86" t="str">
-        <v>E2</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="87">
@@ -9523,19 +9523,19 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E88" t="str">
-        <v>C2</v>
+        <v>D2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make notes in booking master expandable with toggle Add state to track expanded notes and conditionally render input or textarea for expandable notes column in booking master.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f22f566b-a281-4287-a073-5d9bddde658c
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/LuBJ9EM
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -759,121 +759,121 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>992418b2-3029-4752-9552-0aa886433657</v>
+        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
       </c>
       <c r="B3" t="str">
-        <v>Zoe Brown</v>
+        <v>Emilia Miller</v>
       </c>
       <c r="C3">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" t="str">
         <v>Female</v>
       </c>
       <c r="E3" t="str">
-        <v>zoe.brown45@outlook.com</v>
+        <v>emilia.miller56@outlook.com</v>
       </c>
       <c r="F3" t="str">
-        <v>0401 578 107</v>
+        <v>0403 506 698</v>
       </c>
       <c r="G3" t="str">
-        <v>Sydney</v>
+        <v>Melbourne</v>
       </c>
       <c r="H3" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I3" t="str">
         <v>assigned</v>
       </c>
       <c r="J3" t="str">
-        <v>Chloe Jones</v>
+        <v>Victoria Carter</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>992418b2-3029-4752-9552-0aa886433657</v>
       </c>
       <c r="B4" t="str">
-        <v>Paisley Lee</v>
+        <v>Zoe Brown</v>
       </c>
       <c r="C4">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D4" t="str">
         <v>Female</v>
       </c>
       <c r="E4" t="str">
-        <v>paisley.lee78@hotmail.com</v>
+        <v>zoe.brown45@outlook.com</v>
       </c>
       <c r="F4" t="str">
-        <v>0400 179 607</v>
+        <v>0401 578 107</v>
       </c>
       <c r="G4" t="str">
-        <v>Ballarat</v>
+        <v>Sydney</v>
       </c>
       <c r="H4" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I4" t="str">
         <v>assigned</v>
       </c>
       <c r="J4" t="str">
-        <v>Aria Lopez</v>
+        <v>Chloe Jones</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="B5" t="str">
-        <v>Olivia Gonzalez</v>
+        <v>Paisley Lee</v>
       </c>
       <c r="C5">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D5" t="str">
         <v>Female</v>
       </c>
       <c r="E5" t="str">
-        <v>olivia.gonzalez77@hotmail.com</v>
+        <v>paisley.lee78@hotmail.com</v>
       </c>
       <c r="F5" t="str">
-        <v>(982) 690-7408</v>
+        <v>0400 179 607</v>
       </c>
       <c r="G5" t="str">
-        <v>Long Beach</v>
+        <v>Ballarat</v>
       </c>
       <c r="H5" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I5" t="str">
         <v>assigned</v>
       </c>
       <c r="J5" t="str">
-        <v>Eliana Green</v>
+        <v>Aria Lopez</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
       </c>
       <c r="B6" t="str">
-        <v>Hannah Torres</v>
+        <v>Olivia Gonzalez</v>
       </c>
       <c r="C6">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D6" t="str">
         <v>Female</v>
       </c>
       <c r="E6" t="str">
-        <v>hannah.torres86@yahoo.com</v>
+        <v>olivia.gonzalez77@hotmail.com</v>
       </c>
       <c r="F6" t="str">
-        <v>0402 688 409</v>
+        <v>(982) 690-7408</v>
       </c>
       <c r="G6" t="str">
-        <v>Wollongong</v>
+        <v>Long Beach</v>
       </c>
       <c r="H6" t="str">
         <v>B+</v>
@@ -882,68 +882,62 @@
         <v>assigned</v>
       </c>
       <c r="J6" t="str">
-        <v>Audrey Thomas</v>
+        <v>Eliana Green</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
       </c>
       <c r="B7" t="str">
-        <v>Ella Anderson</v>
+        <v>Hannah Torres</v>
       </c>
       <c r="C7">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D7" t="str">
         <v>Female</v>
       </c>
       <c r="E7" t="str">
-        <v>ella.anderson1@yahoo.com</v>
+        <v>hannah.torres86@yahoo.com</v>
       </c>
       <c r="F7" t="str">
-        <v>0412 908 910</v>
+        <v>0402 688 409</v>
       </c>
       <c r="G7" t="str">
-        <v>Geelong</v>
+        <v>Wollongong</v>
       </c>
       <c r="H7" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I7" t="str">
         <v>assigned</v>
       </c>
       <c r="J7" t="str">
-        <v>Isabella Brown</v>
-      </c>
-      <c r="L7" t="str">
-        <v/>
-      </c>
-      <c r="M7" t="str">
-        <v/>
+        <v>Audrey Thomas</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="B8" t="str">
-        <v>Ella Gutierrez</v>
+        <v>Ella Anderson</v>
       </c>
       <c r="C8">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D8" t="str">
         <v>Female</v>
       </c>
       <c r="E8" t="str">
-        <v>ella.gutierrez43@gmail.com</v>
+        <v>ella.anderson1@yahoo.com</v>
       </c>
       <c r="F8" t="str">
-        <v>(220) 105-1876</v>
+        <v>0412 908 910</v>
       </c>
       <c r="G8" t="str">
-        <v>Irvine</v>
+        <v>Geelong</v>
       </c>
       <c r="H8" t="str">
         <v>B</v>
@@ -952,254 +946,260 @@
         <v>assigned</v>
       </c>
       <c r="J8" t="str">
-        <v>Nora Lee</v>
+        <v>Isabella Brown</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
+        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
       </c>
       <c r="B9" t="str">
-        <v>Jackson Young</v>
+        <v>Ella Gutierrez</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D9" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E9" t="str">
-        <v>jackson.young79@yahoo.com</v>
+        <v>ella.gutierrez43@gmail.com</v>
       </c>
       <c r="F9" t="str">
-        <v>0412 940 993</v>
+        <v>(220) 105-1876</v>
       </c>
       <c r="G9" t="str">
-        <v>Ballarat</v>
+        <v>Irvine</v>
       </c>
       <c r="H9" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I9" t="str">
         <v>assigned</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Nora Lee</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
+        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
       </c>
       <c r="B10" t="str">
-        <v>Emilia Miller</v>
+        <v>Jackson Young</v>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D10" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E10" t="str">
-        <v>emilia.miller56@outlook.com</v>
+        <v>jackson.young79@yahoo.com</v>
       </c>
       <c r="F10" t="str">
-        <v>0403 506 698</v>
+        <v>0412 940 993</v>
       </c>
       <c r="G10" t="str">
-        <v>Melbourne</v>
+        <v>Ballarat</v>
       </c>
       <c r="H10" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I10" t="str">
-        <v>available</v>
-      </c>
-      <c r="J10" t="str">
-        <v>Victoria Carter</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
+        <v>c49dde07-b870-477a-82b6-a0354611093f</v>
       </c>
       <c r="B11" t="str">
-        <v>Harper Lewis</v>
+        <v>Mia Carter</v>
       </c>
       <c r="C11">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D11" t="str">
         <v>Female</v>
       </c>
       <c r="E11" t="str">
-        <v>harper.lewis57@hotmail.com</v>
+        <v>mia.carter78@hotmail.com</v>
       </c>
       <c r="F11" t="str">
-        <v>0411 652 121</v>
+        <v>(419) 735-1016</v>
       </c>
       <c r="G11" t="str">
-        <v>Geelong</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H11" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I11" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J11" t="str">
-        <v>Audrey Ramirez</v>
-      </c>
-      <c r="M11" t="str">
-        <v>Back issues - needs lumbar support chair</v>
+        <v>Evelyn Ortiz</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
+        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
       </c>
       <c r="B12" t="str">
-        <v>Audrey Ramirez</v>
+        <v>Harper Lewis</v>
       </c>
       <c r="C12">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D12" t="str">
         <v>Female</v>
       </c>
       <c r="E12" t="str">
-        <v>audrey.ramirez12@gmail.com</v>
+        <v>harper.lewis57@hotmail.com</v>
       </c>
       <c r="F12" t="str">
-        <v>0411 212 619</v>
+        <v>0411 652 121</v>
       </c>
       <c r="G12" t="str">
-        <v>Brisbane</v>
+        <v>Geelong</v>
       </c>
       <c r="H12" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I12" t="str">
         <v>available</v>
       </c>
       <c r="J12" t="str">
-        <v>Harper Lewis</v>
+        <v>Audrey Ramirez</v>
+      </c>
+      <c r="M12" t="str">
+        <v>Back issues - needs lumbar support chair</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
+        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
       </c>
       <c r="B13" t="str">
-        <v>Audrey Smith</v>
+        <v>Audrey Ramirez</v>
       </c>
       <c r="C13">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D13" t="str">
         <v>Female</v>
       </c>
       <c r="E13" t="str">
-        <v>audrey.smith66@gmail.com</v>
+        <v>audrey.ramirez12@gmail.com</v>
       </c>
       <c r="F13" t="str">
-        <v>0410 904 568</v>
+        <v>0411 212 619</v>
       </c>
       <c r="G13" t="str">
-        <v>Ballarat</v>
+        <v>Brisbane</v>
       </c>
       <c r="H13" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I13" t="str">
         <v>available</v>
       </c>
       <c r="J13" t="str">
-        <v>Grace Scott</v>
+        <v>Harper Lewis</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>0669e014-c952-45fd-9791-36cbe1d51444</v>
+        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
       </c>
       <c r="B14" t="str">
-        <v>Sofia Williams</v>
+        <v>Audrey Smith</v>
       </c>
       <c r="C14">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D14" t="str">
         <v>Female</v>
       </c>
       <c r="E14" t="str">
-        <v>sofia.williams39@yahoo.com</v>
+        <v>audrey.smith66@gmail.com</v>
       </c>
       <c r="F14" t="str">
-        <v>0403 299 421</v>
+        <v>0410 904 568</v>
       </c>
       <c r="G14" t="str">
-        <v>Geelong</v>
+        <v>Ballarat</v>
       </c>
       <c r="H14" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I14" t="str">
         <v>available</v>
       </c>
       <c r="J14" t="str">
-        <v>Maya Moore</v>
+        <v>Grace Scott</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+        <v>0669e014-c952-45fd-9791-36cbe1d51444</v>
       </c>
       <c r="B15" t="str">
-        <v>Emilia Thompson</v>
+        <v>Sofia Williams</v>
       </c>
       <c r="C15">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D15" t="str">
         <v>Female</v>
       </c>
       <c r="E15" t="str">
-        <v>emilia.thompson0@gmail.com</v>
+        <v>sofia.williams39@yahoo.com</v>
       </c>
       <c r="F15" t="str">
-        <v>0404 992 451</v>
+        <v>0403 299 421</v>
       </c>
       <c r="G15" t="str">
-        <v>Perth</v>
+        <v>Geelong</v>
       </c>
       <c r="H15" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I15" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J15" t="str">
-        <v>Violet Hall</v>
+        <v>Maya Moore</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
       </c>
       <c r="B16" t="str">
-        <v>Evelyn Sanchez</v>
+        <v>Emilia Thompson</v>
       </c>
       <c r="C16">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D16" t="str">
         <v>Female</v>
       </c>
       <c r="E16" t="str">
-        <v>evelyn.sanchez9@gmail.com</v>
+        <v>emilia.thompson0@gmail.com</v>
       </c>
       <c r="F16" t="str">
-        <v>0404 119 469</v>
+        <v>0404 992 451</v>
       </c>
       <c r="G16" t="str">
-        <v>Gold Coast</v>
+        <v>Perth</v>
       </c>
       <c r="H16" t="str">
         <v>B</v>
@@ -1208,39 +1208,39 @@
         <v>assigned</v>
       </c>
       <c r="J16" t="str">
-        <v>Chloe Flores</v>
+        <v>Violet Hall</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>c49dde07-b870-477a-82b6-a0354611093f</v>
+        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
       </c>
       <c r="B17" t="str">
-        <v>Mia Carter</v>
+        <v>Evelyn Sanchez</v>
       </c>
       <c r="C17">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" t="str">
         <v>Female</v>
       </c>
       <c r="E17" t="str">
-        <v>mia.carter78@hotmail.com</v>
+        <v>evelyn.sanchez9@gmail.com</v>
       </c>
       <c r="F17" t="str">
-        <v>(419) 735-1016</v>
+        <v>0404 119 469</v>
       </c>
       <c r="G17" t="str">
-        <v>Newport Beach</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H17" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I17" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J17" t="str">
-        <v>Evelyn Ortiz</v>
+        <v>Chloe Flores</v>
       </c>
     </row>
     <row r="18">
@@ -1809,57 +1809,57 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
+        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
       </c>
       <c r="B36" t="str">
-        <v>Paisley Scott</v>
+        <v>Victoria Carter</v>
       </c>
       <c r="C36">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D36" t="str">
         <v>Female</v>
       </c>
       <c r="E36" t="str">
-        <v>paisley.scott78@yahoo.com</v>
+        <v>victoria.carter74@gmail.com</v>
       </c>
       <c r="F36" t="str">
-        <v>0410 215 419</v>
+        <v>0411 641 632</v>
       </c>
       <c r="G36" t="str">
-        <v>Ballarat</v>
+        <v>Gold Coast</v>
       </c>
       <c r="H36" t="str">
         <v>B+</v>
       </c>
       <c r="I36" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J36" t="str">
-        <v>Mia Roberts</v>
+        <v>Emilia Miller</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>e897bbe7-50a2-441c-9ba2-0d1c40619f32</v>
+        <v>c4e002c2-94ef-471f-b43d-e6b2a8d35a1c</v>
       </c>
       <c r="B37" t="str">
-        <v>Chloe Williams</v>
+        <v>Paisley Scott</v>
       </c>
       <c r="C37">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D37" t="str">
         <v>Female</v>
       </c>
       <c r="E37" t="str">
-        <v>chloe.williams70@hotmail.com</v>
+        <v>paisley.scott78@yahoo.com</v>
       </c>
       <c r="F37" t="str">
-        <v>(398) 161-2308</v>
+        <v>0410 215 419</v>
       </c>
       <c r="G37" t="str">
-        <v>Los Angeles</v>
+        <v>Ballarat</v>
       </c>
       <c r="H37" t="str">
         <v>B+</v>
@@ -1867,133 +1867,133 @@
       <c r="I37" t="str">
         <v>available</v>
       </c>
+      <c r="J37" t="str">
+        <v>Mia Roberts</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
+        <v>e897bbe7-50a2-441c-9ba2-0d1c40619f32</v>
       </c>
       <c r="B38" t="str">
-        <v>Zoey Cook</v>
+        <v>Chloe Williams</v>
       </c>
       <c r="C38">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D38" t="str">
         <v>Female</v>
       </c>
       <c r="E38" t="str">
-        <v>zoey.cook63@yahoo.com</v>
+        <v>chloe.williams70@hotmail.com</v>
       </c>
       <c r="F38" t="str">
-        <v>(559) 803-4092</v>
+        <v>(398) 161-2308</v>
       </c>
       <c r="G38" t="str">
-        <v>Fremont</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H38" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I38" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J38" t="str">
-        <v>Hunter Scott</v>
+        <v>available</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>6366884b-6583-493e-80bc-a1dff1926c59</v>
+        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
       </c>
       <c r="B39" t="str">
-        <v>Eleanor Allen</v>
+        <v>Zoey Cook</v>
       </c>
       <c r="C39">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D39" t="str">
         <v>Female</v>
       </c>
       <c r="E39" t="str">
-        <v>eleanor.allen67@outlook.com</v>
+        <v>zoey.cook63@yahoo.com</v>
       </c>
       <c r="F39" t="str">
-        <v>(510) 261-1846</v>
+        <v>(559) 803-4092</v>
       </c>
       <c r="G39" t="str">
-        <v>Los Angeles</v>
+        <v>Fremont</v>
       </c>
       <c r="H39" t="str">
         <v>A</v>
       </c>
       <c r="I39" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J39" t="str">
-        <v>Christopher Allen</v>
+        <v>Hunter Scott</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>6366884b-6583-493e-80bc-a1dff1926c59</v>
       </c>
       <c r="B40" t="str">
-        <v>Ella Martinez</v>
+        <v>Eleanor Allen</v>
       </c>
       <c r="C40">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D40" t="str">
         <v>Female</v>
       </c>
       <c r="E40" t="str">
-        <v>ella.martinez67@hotmail.com</v>
+        <v>eleanor.allen67@outlook.com</v>
       </c>
       <c r="F40" t="str">
-        <v>(703) 898-3990</v>
+        <v>(510) 261-1846</v>
       </c>
       <c r="G40" t="str">
-        <v>Burbank</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H40" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I40" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J40" t="str">
-        <v>Josiah Lopez, Victoria Carter</v>
+        <v>Christopher Allen</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="B41" t="str">
-        <v>Victoria Carter</v>
+        <v>Ella Martinez</v>
       </c>
       <c r="C41">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D41" t="str">
         <v>Female</v>
       </c>
       <c r="E41" t="str">
-        <v>victoria.carter74@gmail.com</v>
+        <v>ella.martinez67@hotmail.com</v>
       </c>
       <c r="F41" t="str">
-        <v>0411 641 632</v>
+        <v>(703) 898-3990</v>
       </c>
       <c r="G41" t="str">
-        <v>Gold Coast</v>
+        <v>Burbank</v>
       </c>
       <c r="H41" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I41" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J41" t="str">
-        <v>Emilia Miller</v>
+        <v>Josiah Lopez, Victoria Carter</v>
       </c>
     </row>
     <row r="42">
@@ -3841,89 +3841,92 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
+        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
       </c>
       <c r="B101" t="str">
-        <v>Piper Green</v>
+        <v>Layla Lopez</v>
       </c>
       <c r="C101">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D101" t="str">
         <v>Female</v>
       </c>
       <c r="E101" t="str">
-        <v>piper.green82@hotmail.com</v>
+        <v>layla.lopez23@yahoo.com</v>
       </c>
       <c r="F101" t="str">
-        <v>(678) 816-2263</v>
+        <v>(607) 496-6102</v>
       </c>
       <c r="G101" t="str">
-        <v>Burbank</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H101" t="str">
         <v>B</v>
       </c>
       <c r="I101" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J101" t="str">
-        <v>Josiah Brown</v>
+        <v>Cora Lee</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>af09efbe-e83d-4046-8dc8-e6a06dfc0c40</v>
+        <v>0d8894f6-9a60-421c-a7c0-144fe2f8c85f</v>
       </c>
       <c r="B102" t="str">
-        <v>Paisley Evans</v>
+        <v>Lydia Morris</v>
       </c>
       <c r="C102">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D102" t="str">
         <v>Female</v>
       </c>
       <c r="E102" t="str">
-        <v>paisley.evans52@yahoo.com</v>
+        <v>lydia.morris1@gmail.com</v>
       </c>
       <c r="F102" t="str">
-        <v>(894) 250-9501</v>
+        <v>(565) 806-3217</v>
       </c>
       <c r="G102" t="str">
-        <v>Torrance</v>
+        <v>Burbank</v>
       </c>
       <c r="H102" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I102" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J102" t="str">
+        <v>Logan Gomez</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>fec80989-ab0f-471a-a4de-6c207e334f80</v>
+        <v>af09efbe-e83d-4046-8dc8-e6a06dfc0c40</v>
       </c>
       <c r="B103" t="str">
-        <v>Eliza Rivera</v>
+        <v>Paisley Evans</v>
       </c>
       <c r="C103">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D103" t="str">
         <v>Female</v>
       </c>
       <c r="E103" t="str">
-        <v>eliza.rivera29@yahoo.com</v>
+        <v>paisley.evans52@yahoo.com</v>
       </c>
       <c r="F103" t="str">
-        <v>(836) 154-6362</v>
+        <v>(894) 250-9501</v>
       </c>
       <c r="G103" t="str">
-        <v>Newport Beach</v>
+        <v>Torrance</v>
       </c>
       <c r="H103" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I103" t="str">
         <v>available</v>
@@ -3931,121 +3934,118 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>f6a281bb-caec-44cf-a596-a6e92d6e2610</v>
+        <v>fec80989-ab0f-471a-a4de-6c207e334f80</v>
       </c>
       <c r="B104" t="str">
-        <v>Leah Scott</v>
+        <v>Eliza Rivera</v>
       </c>
       <c r="C104">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D104" t="str">
         <v>Female</v>
       </c>
       <c r="E104" t="str">
-        <v>leah.scott74@gmail.com</v>
+        <v>eliza.rivera29@yahoo.com</v>
       </c>
       <c r="F104" t="str">
-        <v>0402 414 358</v>
+        <v>(836) 154-6362</v>
       </c>
       <c r="G104" t="str">
-        <v>Perth</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H104" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I104" t="str">
         <v>available</v>
       </c>
-      <c r="J104" t="str">
-        <v>Harper Sanchez</v>
-      </c>
-      <c r="M104" t="str">
-        <v>Limited mobility - prefers ground floor seating</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>04993d9a-3a65-4d61-a0c8-591aabb2e72c</v>
+        <v>f6a281bb-caec-44cf-a596-a6e92d6e2610</v>
       </c>
       <c r="B105" t="str">
-        <v>Eliza Martinez</v>
+        <v>Leah Scott</v>
       </c>
       <c r="C105">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D105" t="str">
         <v>Female</v>
       </c>
       <c r="E105" t="str">
-        <v>eliza.martinez8@hotmail.com</v>
+        <v>leah.scott74@gmail.com</v>
       </c>
       <c r="F105" t="str">
-        <v>(881) 895-2168</v>
+        <v>0402 414 358</v>
       </c>
       <c r="G105" t="str">
-        <v>Torrance</v>
+        <v>Perth</v>
       </c>
       <c r="H105" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I105" t="str">
         <v>available</v>
       </c>
+      <c r="J105" t="str">
+        <v>Harper Sanchez</v>
+      </c>
+      <c r="M105" t="str">
+        <v>Limited mobility - prefers ground floor seating</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>bf1fc0b1-7d88-41a5-ab6f-ee4c085fd344</v>
+        <v>04993d9a-3a65-4d61-a0c8-591aabb2e72c</v>
       </c>
       <c r="B106" t="str">
-        <v>Brooklyn Nguyen</v>
+        <v>Eliza Martinez</v>
       </c>
       <c r="C106">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D106" t="str">
         <v>Female</v>
       </c>
       <c r="E106" t="str">
-        <v>brooklyn.nguyen77@yahoo.com</v>
+        <v>eliza.martinez8@hotmail.com</v>
       </c>
       <c r="F106" t="str">
-        <v>(142) 872-1855</v>
+        <v>(881) 895-2168</v>
       </c>
       <c r="G106" t="str">
-        <v>Los Angeles</v>
+        <v>Torrance</v>
       </c>
       <c r="H106" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I106" t="str">
         <v>available</v>
       </c>
-      <c r="J106" t="str">
-        <v>Naomi Brown</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>0fa47948-ca05-48a1-917a-bce2c13237ed</v>
+        <v>bf1fc0b1-7d88-41a5-ab6f-ee4c085fd344</v>
       </c>
       <c r="B107" t="str">
-        <v>Isabella Taylor</v>
+        <v>Brooklyn Nguyen</v>
       </c>
       <c r="C107">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D107" t="str">
         <v>Female</v>
       </c>
       <c r="E107" t="str">
-        <v>isabella.taylor65@yahoo.com</v>
+        <v>brooklyn.nguyen77@yahoo.com</v>
       </c>
       <c r="F107" t="str">
-        <v>(997) 957-4171</v>
+        <v>(142) 872-1855</v>
       </c>
       <c r="G107" t="str">
-        <v>Chula Vista</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H107" t="str">
         <v>A</v>
@@ -4053,31 +4053,34 @@
       <c r="I107" t="str">
         <v>available</v>
       </c>
+      <c r="J107" t="str">
+        <v>Naomi Brown</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>24928131-51b3-46f8-b43f-2cf989696f62</v>
+        <v>0fa47948-ca05-48a1-917a-bce2c13237ed</v>
       </c>
       <c r="B108" t="str">
-        <v>Amelia Garcia</v>
+        <v>Isabella Taylor</v>
       </c>
       <c r="C108">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D108" t="str">
         <v>Female</v>
       </c>
       <c r="E108" t="str">
-        <v>amelia.garcia16@gmail.com</v>
+        <v>isabella.taylor65@yahoo.com</v>
       </c>
       <c r="F108" t="str">
-        <v>(331) 367-3904</v>
+        <v>(997) 957-4171</v>
       </c>
       <c r="G108" t="str">
-        <v>Anaheim</v>
+        <v>Chula Vista</v>
       </c>
       <c r="H108" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I108" t="str">
         <v>available</v>
@@ -4085,57 +4088,54 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>50b098db-86f4-4a21-8425-ab03df8f7a40</v>
+        <v>24928131-51b3-46f8-b43f-2cf989696f62</v>
       </c>
       <c r="B109" t="str">
-        <v>Lillian Campbell</v>
+        <v>Amelia Garcia</v>
       </c>
       <c r="C109">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D109" t="str">
         <v>Female</v>
       </c>
       <c r="E109" t="str">
-        <v>lillian.campbell41@yahoo.com</v>
+        <v>amelia.garcia16@gmail.com</v>
       </c>
       <c r="F109" t="str">
-        <v>(945) 213-8284</v>
+        <v>(331) 367-3904</v>
       </c>
       <c r="G109" t="str">
-        <v>Pasadena</v>
+        <v>Anaheim</v>
       </c>
       <c r="H109" t="str">
-        <v>A+</v>
+        <v>B+</v>
       </c>
       <c r="I109" t="str">
         <v>available</v>
       </c>
-      <c r="J109" t="str">
-        <v>Amelia Lopez</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>e9a3f4c7-c9ed-4fd1-a5a9-d3763ae52a55</v>
+        <v>50b098db-86f4-4a21-8425-ab03df8f7a40</v>
       </c>
       <c r="B110" t="str">
-        <v>Victoria Anderson</v>
+        <v>Lillian Campbell</v>
       </c>
       <c r="C110">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D110" t="str">
         <v>Female</v>
       </c>
       <c r="E110" t="str">
-        <v>victoria.anderson1@outlook.com</v>
+        <v>lillian.campbell41@yahoo.com</v>
       </c>
       <c r="F110" t="str">
-        <v>(622) 987-4829</v>
+        <v>(945) 213-8284</v>
       </c>
       <c r="G110" t="str">
-        <v>Sacramento</v>
+        <v>Pasadena</v>
       </c>
       <c r="H110" t="str">
         <v>A+</v>
@@ -4144,71 +4144,71 @@
         <v>available</v>
       </c>
       <c r="J110" t="str">
-        <v>Sophia Reyes</v>
+        <v>Amelia Lopez</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>0d8894f6-9a60-421c-a7c0-144fe2f8c85f</v>
+        <v>e9a3f4c7-c9ed-4fd1-a5a9-d3763ae52a55</v>
       </c>
       <c r="B111" t="str">
-        <v>Lydia Morris</v>
+        <v>Victoria Anderson</v>
       </c>
       <c r="C111">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D111" t="str">
         <v>Female</v>
       </c>
       <c r="E111" t="str">
-        <v>lydia.morris1@gmail.com</v>
+        <v>victoria.anderson1@outlook.com</v>
       </c>
       <c r="F111" t="str">
-        <v>(565) 806-3217</v>
+        <v>(622) 987-4829</v>
       </c>
       <c r="G111" t="str">
-        <v>Burbank</v>
+        <v>Sacramento</v>
       </c>
       <c r="H111" t="str">
-        <v>A</v>
+        <v>A+</v>
       </c>
       <c r="I111" t="str">
         <v>available</v>
       </c>
       <c r="J111" t="str">
-        <v>Logan Gomez</v>
+        <v>Sophia Reyes</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
       </c>
       <c r="B112" t="str">
-        <v>Cora Mitchell</v>
+        <v>Piper Green</v>
       </c>
       <c r="C112">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D112" t="str">
         <v>Female</v>
       </c>
       <c r="E112" t="str">
-        <v>cora.mitchell80@icloud.com</v>
+        <v>piper.green82@hotmail.com</v>
       </c>
       <c r="F112" t="str">
-        <v>(929) 139-3875</v>
+        <v>(678) 816-2263</v>
       </c>
       <c r="G112" t="str">
-        <v>Newport Beach</v>
+        <v>Burbank</v>
       </c>
       <c r="H112" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I112" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J112" t="str">
-        <v>Christopher Carter</v>
+        <v>Josiah Brown</v>
       </c>
     </row>
     <row r="113">
@@ -4396,34 +4396,34 @@
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="B119" t="str">
-        <v>Avery Taylor</v>
+        <v>Cora Mitchell</v>
       </c>
       <c r="C119">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D119" t="str">
         <v>Female</v>
       </c>
       <c r="E119" t="str">
-        <v>avery.taylor87@outlook.com</v>
+        <v>cora.mitchell80@icloud.com</v>
       </c>
       <c r="F119" t="str">
-        <v>(299) 491-7680</v>
+        <v>(929) 139-3875</v>
       </c>
       <c r="G119" t="str">
-        <v>Los Angeles</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H119" t="str">
         <v>B+</v>
       </c>
       <c r="I119" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J119" t="str">
-        <v>Audrey Hill</v>
+        <v>Christopher Carter</v>
       </c>
     </row>
     <row r="120">
@@ -4521,34 +4521,34 @@
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
+        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
       </c>
       <c r="B123" t="str">
-        <v>Layla Lopez</v>
+        <v>Avery Taylor</v>
       </c>
       <c r="C123">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D123" t="str">
         <v>Female</v>
       </c>
       <c r="E123" t="str">
-        <v>layla.lopez23@yahoo.com</v>
+        <v>avery.taylor87@outlook.com</v>
       </c>
       <c r="F123" t="str">
-        <v>(607) 496-6102</v>
+        <v>(299) 491-7680</v>
       </c>
       <c r="G123" t="str">
         <v>Los Angeles</v>
       </c>
       <c r="H123" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I123" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J123" t="str">
-        <v>Cora Lee</v>
+        <v>Audrey Hill</v>
       </c>
     </row>
     <row r="124">
@@ -5697,57 +5697,57 @@
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
+        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
       </c>
       <c r="B162" t="str">
-        <v>Grayson Edwards</v>
+        <v>Audrey Hill</v>
       </c>
       <c r="C162">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D162" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E162" t="str">
-        <v>grayson.edwards22@gmail.com</v>
+        <v>audrey.hill20@outlook.com</v>
       </c>
       <c r="F162" t="str">
-        <v>(215) 129-3913</v>
+        <v>(688) 524-4712</v>
       </c>
       <c r="G162" t="str">
-        <v>Torrance</v>
+        <v>San Jose</v>
       </c>
       <c r="H162" t="str">
         <v>B</v>
       </c>
       <c r="I162" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J162" t="str">
-        <v>Elizabeth Nelson, Joseph Anderson</v>
+        <v>Avery Taylor</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
       </c>
       <c r="B163" t="str">
-        <v>Cameron Evans</v>
+        <v>Grayson Edwards</v>
       </c>
       <c r="C163">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D163" t="str">
         <v>Male</v>
       </c>
       <c r="E163" t="str">
-        <v>cameron.evans55@outlook.com</v>
+        <v>grayson.edwards22@gmail.com</v>
       </c>
       <c r="F163" t="str">
-        <v>(535) 743-7467</v>
+        <v>(215) 129-3913</v>
       </c>
       <c r="G163" t="str">
-        <v>Fremont</v>
+        <v>Torrance</v>
       </c>
       <c r="H163" t="str">
         <v>B</v>
@@ -5756,103 +5756,103 @@
         <v>assigned</v>
       </c>
       <c r="J163" t="str">
-        <v>Michael Johnson, Anthony Garcia</v>
+        <v>Elizabeth Nelson, Joseph Anderson</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="B164" t="str">
-        <v>Sadie Cook</v>
+        <v>Cameron Evans</v>
       </c>
       <c r="C164">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D164" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E164" t="str">
-        <v>sadie.cook9@yahoo.com</v>
+        <v>cameron.evans55@outlook.com</v>
       </c>
       <c r="F164" t="str">
-        <v>(382) 126-7672</v>
+        <v>(535) 743-7467</v>
       </c>
       <c r="G164" t="str">
-        <v>Santa Monica</v>
+        <v>Fremont</v>
       </c>
       <c r="H164" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I164" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J164" t="str">
-        <v>William Allen, Alexa Hall</v>
+        <v>Michael Johnson, Anthony Garcia</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
       </c>
       <c r="B165" t="str">
-        <v>Julian Nguyen</v>
+        <v>Sadie Cook</v>
       </c>
       <c r="C165">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D165" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E165" t="str">
-        <v>julian.nguyen22@outlook.com</v>
+        <v>sadie.cook9@yahoo.com</v>
       </c>
       <c r="F165" t="str">
-        <v>(382) 722-8118</v>
+        <v>(382) 126-7672</v>
       </c>
       <c r="G165" t="str">
-        <v>Long Beach</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H165" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I165" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J165" t="str">
-        <v>Leah Diaz, Lydia Allen</v>
+        <v>William Allen, Alexa Hall</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="B166" t="str">
-        <v>Audrey Hill</v>
+        <v>Julian Nguyen</v>
       </c>
       <c r="C166">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D166" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E166" t="str">
-        <v>audrey.hill20@outlook.com</v>
+        <v>julian.nguyen22@outlook.com</v>
       </c>
       <c r="F166" t="str">
-        <v>(688) 524-4712</v>
+        <v>(382) 722-8118</v>
       </c>
       <c r="G166" t="str">
-        <v>San Jose</v>
+        <v>Long Beach</v>
       </c>
       <c r="H166" t="str">
         <v>B</v>
       </c>
       <c r="I166" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J166" t="str">
-        <v>Avery Taylor</v>
+        <v>Leah Diaz, Lydia Allen</v>
       </c>
     </row>
     <row r="167">
@@ -6291,7 +6291,7 @@
         <v>B</v>
       </c>
       <c r="I180" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J180" t="str">
         <v>Alexander Campbell, Logan Nguyen</v>
@@ -6601,22 +6601,22 @@
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
+        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
       </c>
       <c r="B191" t="str">
-        <v>Josiah Brown</v>
+        <v>Alexander Campbell</v>
       </c>
       <c r="C191">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D191" t="str">
         <v>Male</v>
       </c>
       <c r="E191" t="str">
-        <v>josiah.brown19@hotmail.com</v>
+        <v>alexander.campbell71@gmail.com</v>
       </c>
       <c r="F191" t="str">
-        <v>(678) 449-3168</v>
+        <v>(131) 840-1169</v>
       </c>
       <c r="G191" t="str">
         <v>Fresno</v>
@@ -6625,10 +6625,10 @@
         <v>A</v>
       </c>
       <c r="I191" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J191" t="str">
-        <v>Piper Green</v>
+        <v>Logan Nguyen, Hannah Moore</v>
       </c>
     </row>
     <row r="192">
@@ -6753,7 +6753,7 @@
         <v>B+</v>
       </c>
       <c r="I195" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J195" t="str">
         <v>Alexander Campbell, Hannah Moore</v>
@@ -7049,95 +7049,95 @@
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
       </c>
       <c r="B205" t="str">
-        <v>Carter Harris</v>
+        <v>Josiah Brown</v>
       </c>
       <c r="C205">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D205" t="str">
         <v>Male</v>
       </c>
       <c r="E205" t="str">
-        <v>carter.harris82@yahoo.com</v>
+        <v>josiah.brown19@hotmail.com</v>
       </c>
       <c r="F205" t="str">
-        <v>0412 175 744</v>
+        <v>(678) 449-3168</v>
       </c>
       <c r="G205" t="str">
-        <v>Geelong</v>
+        <v>Fresno</v>
       </c>
       <c r="H205" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I205" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J205" t="str">
+        <v>Piper Green</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>f26a0638-511f-4440-ae1a-2ae052df470f</v>
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
       </c>
       <c r="B206" t="str">
-        <v>Caleb Brown</v>
+        <v>Carter Harris</v>
       </c>
       <c r="C206">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D206" t="str">
         <v>Male</v>
       </c>
       <c r="E206" t="str">
-        <v>caleb.brown13@yahoo.com</v>
+        <v>carter.harris82@yahoo.com</v>
       </c>
       <c r="F206" t="str">
-        <v>(130) 920-6765</v>
+        <v>0412 175 744</v>
       </c>
       <c r="G206" t="str">
-        <v>Irvine</v>
+        <v>Geelong</v>
       </c>
       <c r="H206" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I206" t="str">
         <v>available</v>
       </c>
-      <c r="J206" t="str">
-        <v>Jackson Murphy</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
+        <v>f26a0638-511f-4440-ae1a-2ae052df470f</v>
       </c>
       <c r="B207" t="str">
-        <v>Alexander Campbell</v>
+        <v>Caleb Brown</v>
       </c>
       <c r="C207">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D207" t="str">
         <v>Male</v>
       </c>
       <c r="E207" t="str">
-        <v>alexander.campbell71@gmail.com</v>
+        <v>caleb.brown13@yahoo.com</v>
       </c>
       <c r="F207" t="str">
-        <v>(131) 840-1169</v>
+        <v>(130) 920-6765</v>
       </c>
       <c r="G207" t="str">
-        <v>Fresno</v>
+        <v>Irvine</v>
       </c>
       <c r="H207" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I207" t="str">
         <v>available</v>
       </c>
       <c r="J207" t="str">
-        <v>Logan Nguyen, Hannah Moore</v>
+        <v>Jackson Murphy</v>
       </c>
     </row>
     <row r="208">
@@ -7235,25 +7235,25 @@
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>ba63a5c0-c76e-4c1b-b6e4-afed15dfdcd4</v>
+        <v>f878ab7f-ae59-4af0-b19a-e9bf4573c116</v>
       </c>
       <c r="B211" t="str">
-        <v>Joseph Anderson</v>
+        <v>William Allen</v>
       </c>
       <c r="C211">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D211" t="str">
         <v>Male</v>
       </c>
       <c r="E211" t="str">
-        <v>joseph.anderson2@outlook.com</v>
+        <v>william.allen62@hotmail.com</v>
       </c>
       <c r="F211" t="str">
-        <v>(433) 142-2338</v>
+        <v>(267) 463-7481</v>
       </c>
       <c r="G211" t="str">
-        <v>Chula Vista</v>
+        <v>San Jose</v>
       </c>
       <c r="H211" t="str">
         <v>B+</v>
@@ -7262,94 +7262,94 @@
         <v>available</v>
       </c>
       <c r="J211" t="str">
-        <v>Elizabeth Nelson, Grayson Edwards</v>
+        <v>Sadie Cook, Alexa Hall</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>f878ab7f-ae59-4af0-b19a-e9bf4573c116</v>
+        <v>8e30e99d-0594-4a73-840e-1f5ef32387ae</v>
       </c>
       <c r="B212" t="str">
-        <v>William Allen</v>
+        <v>Cameron Anderson</v>
       </c>
       <c r="C212">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D212" t="str">
         <v>Male</v>
       </c>
       <c r="E212" t="str">
-        <v>william.allen62@hotmail.com</v>
+        <v>cameron.anderson85@hotmail.com</v>
       </c>
       <c r="F212" t="str">
-        <v>(267) 463-7481</v>
+        <v>(960) 363-1976</v>
       </c>
       <c r="G212" t="str">
-        <v>San Jose</v>
+        <v>Glendale</v>
       </c>
       <c r="H212" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I212" t="str">
         <v>available</v>
       </c>
       <c r="J212" t="str">
-        <v>Sadie Cook, Alexa Hall</v>
+        <v>John Diaz</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>8e30e99d-0594-4a73-840e-1f5ef32387ae</v>
+        <v>1a539e8e-7b02-422a-991f-99fdb84688f5</v>
       </c>
       <c r="B213" t="str">
-        <v>Cameron Anderson</v>
+        <v>Logan Lopez</v>
       </c>
       <c r="C213">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D213" t="str">
         <v>Male</v>
       </c>
       <c r="E213" t="str">
-        <v>cameron.anderson85@hotmail.com</v>
+        <v>logan.lopez66@icloud.com</v>
       </c>
       <c r="F213" t="str">
-        <v>(960) 363-1976</v>
+        <v>(283) 498-3157</v>
       </c>
       <c r="G213" t="str">
-        <v>Glendale</v>
+        <v>Burbank</v>
       </c>
       <c r="H213" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I213" t="str">
         <v>available</v>
       </c>
       <c r="J213" t="str">
-        <v>John Diaz</v>
+        <v>Ava Mitchell</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>1a539e8e-7b02-422a-991f-99fdb84688f5</v>
+        <v>1b5fc1ce-1ed8-4255-a8a4-b02892b2b03a</v>
       </c>
       <c r="B214" t="str">
-        <v>Logan Lopez</v>
+        <v>Ava Mitchell</v>
       </c>
       <c r="C214">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D214" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E214" t="str">
-        <v>logan.lopez66@icloud.com</v>
+        <v>ava.mitchell87@icloud.com</v>
       </c>
       <c r="F214" t="str">
-        <v>(283) 498-3157</v>
+        <v>(211) 525-6721</v>
       </c>
       <c r="G214" t="str">
-        <v>Burbank</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H214" t="str">
         <v>B+</v>
@@ -7358,62 +7358,65 @@
         <v>available</v>
       </c>
       <c r="J214" t="str">
-        <v>Ava Mitchell</v>
+        <v>Logan Lopez</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>1b5fc1ce-1ed8-4255-a8a4-b02892b2b03a</v>
+        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
       </c>
       <c r="B215" t="str">
-        <v>Ava Mitchell</v>
+        <v>Emily Thomas</v>
       </c>
       <c r="C215">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D215" t="str">
         <v>Female</v>
       </c>
       <c r="E215" t="str">
-        <v>ava.mitchell87@icloud.com</v>
+        <v>emily.thomas25@outlook.com</v>
       </c>
       <c r="F215" t="str">
-        <v>(211) 525-6721</v>
+        <v>0402 648 577</v>
       </c>
       <c r="G215" t="str">
-        <v>Santa Monica</v>
+        <v>Geelong</v>
       </c>
       <c r="H215" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I215" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J215" t="str">
-        <v>Logan Lopez</v>
+        <v>Stella Garcia</v>
+      </c>
+      <c r="M215" t="str">
+        <v>Knee replacement - cannot climb stairs</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
+        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
       </c>
       <c r="B216" t="str">
-        <v>Emily Thomas</v>
+        <v>Aria Scott</v>
       </c>
       <c r="C216">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D216" t="str">
         <v>Female</v>
       </c>
       <c r="E216" t="str">
-        <v>emily.thomas25@outlook.com</v>
+        <v>aria.scott42@outlook.com</v>
       </c>
       <c r="F216" t="str">
-        <v>0402 648 577</v>
+        <v>0401 330 548</v>
       </c>
       <c r="G216" t="str">
-        <v>Geelong</v>
+        <v>Hobart</v>
       </c>
       <c r="H216" t="str">
         <v>B</v>
@@ -7422,33 +7425,30 @@
         <v>assigned</v>
       </c>
       <c r="J216" t="str">
-        <v>Stella Garcia</v>
-      </c>
-      <c r="M216" t="str">
-        <v>Knee replacement - cannot climb stairs</v>
+        <v>Maya Hernandez</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
+        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
       </c>
       <c r="B217" t="str">
-        <v>Aria Scott</v>
+        <v>Cora Lee</v>
       </c>
       <c r="C217">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D217" t="str">
         <v>Female</v>
       </c>
       <c r="E217" t="str">
-        <v>aria.scott42@outlook.com</v>
+        <v>cora.lee40@hotmail.com</v>
       </c>
       <c r="F217" t="str">
-        <v>0401 330 548</v>
+        <v>(406) 886-5180</v>
       </c>
       <c r="G217" t="str">
-        <v>Hobart</v>
+        <v>Fresno</v>
       </c>
       <c r="H217" t="str">
         <v>B</v>
@@ -7457,30 +7457,30 @@
         <v>assigned</v>
       </c>
       <c r="J217" t="str">
-        <v>Maya Hernandez</v>
+        <v>Layla Lopez</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>ba63a5c0-c76e-4c1b-b6e4-afed15dfdcd4</v>
       </c>
       <c r="B218" t="str">
-        <v>Michael Johnson</v>
+        <v>Joseph Anderson</v>
       </c>
       <c r="C218">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D218" t="str">
         <v>Male</v>
       </c>
       <c r="E218" t="str">
-        <v>michael.johnson96@gmail.com</v>
+        <v>joseph.anderson2@outlook.com</v>
       </c>
       <c r="F218" t="str">
-        <v>(878) 132-4532</v>
+        <v>(433) 142-2338</v>
       </c>
       <c r="G218" t="str">
-        <v>Long Beach</v>
+        <v>Chula Vista</v>
       </c>
       <c r="H218" t="str">
         <v>B+</v>
@@ -7489,62 +7489,65 @@
         <v>assigned</v>
       </c>
       <c r="J218" t="str">
-        <v>Anthony Garcia, Cameron Evans</v>
+        <v>Elizabeth Nelson, Grayson Edwards</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="B219" t="str">
-        <v>Cameron Lee</v>
+        <v>Michael Johnson</v>
       </c>
       <c r="C219">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D219" t="str">
         <v>Male</v>
       </c>
       <c r="E219" t="str">
-        <v>cameron.lee78@yahoo.com</v>
+        <v>michael.johnson96@gmail.com</v>
       </c>
       <c r="F219" t="str">
-        <v>0404 821 708</v>
+        <v>(878) 132-4532</v>
       </c>
       <c r="G219" t="str">
-        <v>Cairns</v>
+        <v>Long Beach</v>
       </c>
       <c r="H219" t="str">
         <v>B+</v>
       </c>
       <c r="I219" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J219" t="str">
+        <v>Anthony Garcia, Cameron Evans</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
+        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
       </c>
       <c r="B220" t="str">
-        <v>Joshua Walker</v>
+        <v>Cameron Lee</v>
       </c>
       <c r="C220">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D220" t="str">
         <v>Male</v>
       </c>
       <c r="E220" t="str">
-        <v>joshua.walker97@gmail.com</v>
+        <v>cameron.lee78@yahoo.com</v>
       </c>
       <c r="F220" t="str">
-        <v>0402 640 379</v>
+        <v>0404 821 708</v>
       </c>
       <c r="G220" t="str">
-        <v>Darwin</v>
+        <v>Cairns</v>
       </c>
       <c r="H220" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I220" t="str">
         <v>available</v>
@@ -7552,107 +7555,104 @@
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>5c5fe7f9-35dd-4685-af6b-e44a56c1d47c</v>
+        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
       </c>
       <c r="B221" t="str">
-        <v>Charlotte Johnson</v>
+        <v>Joshua Walker</v>
       </c>
       <c r="C221">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D221" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E221" t="str">
-        <v>charlotte.johnson36@yahoo.com</v>
+        <v>joshua.walker97@gmail.com</v>
       </c>
       <c r="F221" t="str">
-        <v>0410 304 177</v>
+        <v>0402 640 379</v>
       </c>
       <c r="G221" t="str">
-        <v>Perth</v>
+        <v>Darwin</v>
       </c>
       <c r="H221" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I221" t="str">
         <v>available</v>
       </c>
-      <c r="J221" t="str">
-        <v>Audrey Martin</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>5c5fe7f9-35dd-4685-af6b-e44a56c1d47c</v>
       </c>
       <c r="B222" t="str">
-        <v>Peter Adamidis</v>
+        <v>Charlotte Johnson</v>
       </c>
       <c r="C222">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D222" t="str">
-        <v>Not Specified</v>
+        <v>Female</v>
       </c>
       <c r="E222" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>charlotte.johnson36@yahoo.com</v>
       </c>
       <c r="F222" t="str">
-        <v>498086080</v>
+        <v>0410 304 177</v>
       </c>
       <c r="G222" t="str">
-        <v/>
+        <v>Perth</v>
       </c>
       <c r="H222" t="str">
-        <v/>
+        <v>A</v>
       </c>
       <c r="I222" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J222" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
-      </c>
-      <c r="K222" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L222" t="str">
-        <v>Y</v>
-      </c>
-      <c r="M222" t="str">
-        <v>Broken Leg</v>
+        <v>Audrey Martin</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B223" t="str">
-        <v>Cora Lee</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C223">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D223" t="str">
-        <v>Female</v>
+        <v>Not Specified</v>
       </c>
       <c r="E223" t="str">
-        <v>cora.lee40@hotmail.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F223" t="str">
-        <v>(406) 886-5180</v>
+        <v>498086080</v>
       </c>
       <c r="G223" t="str">
-        <v>Fresno</v>
+        <v/>
       </c>
       <c r="H223" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="I223" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J223" t="str">
-        <v>Layla Lopez</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+      </c>
+      <c r="K223" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L223" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M223" t="str">
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="224">
@@ -7823,42 +7823,42 @@
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>c347dd65-5ee0-40a6-9fce-2500b3aed70c</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="B229" t="str">
-        <v>Logan Gomez</v>
+        <v>Adam Hall</v>
       </c>
       <c r="C229">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D229" t="str">
         <v>Male</v>
       </c>
       <c r="E229" t="str">
-        <v>logan.gomez89@outlook.com</v>
+        <v>adam.hall35@outlook.com</v>
       </c>
       <c r="F229" t="str">
-        <v>(628) 585-4251</v>
+        <v>(742) 142-5313</v>
       </c>
       <c r="G229" t="str">
-        <v>San Diego</v>
+        <v>Santa Ana</v>
       </c>
       <c r="H229" t="str">
         <v>B</v>
       </c>
       <c r="I229" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J229" t="str">
-        <v>Lydia Morris</v>
+        <v>Grayson Morgan, Valentina Morales</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
+        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
       </c>
       <c r="B230" t="str">
-        <v>Christopher Carter</v>
+        <v>Nolan Ortiz</v>
       </c>
       <c r="C230">
         <v>42</v>
@@ -7867,42 +7867,42 @@
         <v>Male</v>
       </c>
       <c r="E230" t="str">
-        <v>christopher.carter22@outlook.com</v>
+        <v>nolan.ortiz57@gmail.com</v>
       </c>
       <c r="F230" t="str">
-        <v>(176) 989-4341</v>
+        <v>(473) 870-4585</v>
       </c>
       <c r="G230" t="str">
-        <v>Los Angeles</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H230" t="str">
         <v>B</v>
       </c>
       <c r="I230" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J230" t="str">
-        <v>Cora Mitchell</v>
+        <v>Cameron Clark</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>5965e7f9-ebf0-4e66-a197-03be16110662</v>
       </c>
       <c r="B231" t="str">
-        <v>Adam Hall</v>
+        <v>Cameron Clark</v>
       </c>
       <c r="C231">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D231" t="str">
         <v>Male</v>
       </c>
       <c r="E231" t="str">
-        <v>adam.hall35@outlook.com</v>
+        <v>cameron.clark37@gmail.com</v>
       </c>
       <c r="F231" t="str">
-        <v>(742) 142-5313</v>
+        <v>(267) 288-3549</v>
       </c>
       <c r="G231" t="str">
         <v>Santa Ana</v>
@@ -7914,30 +7914,30 @@
         <v>assigned</v>
       </c>
       <c r="J231" t="str">
-        <v>Grayson Morgan, Valentina Morales</v>
+        <v>Nolan Ortiz</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
+        <v>644e41d7-b99e-4381-99a9-65d5ee89ad50</v>
       </c>
       <c r="B232" t="str">
-        <v>Nolan Ortiz</v>
+        <v>Hunter Scott</v>
       </c>
       <c r="C232">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D232" t="str">
         <v>Male</v>
       </c>
       <c r="E232" t="str">
-        <v>nolan.ortiz57@gmail.com</v>
+        <v>hunter.scott37@outlook.com</v>
       </c>
       <c r="F232" t="str">
-        <v>(473) 870-4585</v>
+        <v>(477) 130-2066</v>
       </c>
       <c r="G232" t="str">
-        <v>Santa Monica</v>
+        <v>Torrance</v>
       </c>
       <c r="H232" t="str">
         <v>B</v>
@@ -7946,30 +7946,30 @@
         <v>assigned</v>
       </c>
       <c r="J232" t="str">
-        <v>Cameron Clark</v>
+        <v>Zoey Cook</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>5965e7f9-ebf0-4e66-a197-03be16110662</v>
+        <v>c347dd65-5ee0-40a6-9fce-2500b3aed70c</v>
       </c>
       <c r="B233" t="str">
-        <v>Cameron Clark</v>
+        <v>Logan Gomez</v>
       </c>
       <c r="C233">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D233" t="str">
         <v>Male</v>
       </c>
       <c r="E233" t="str">
-        <v>cameron.clark37@gmail.com</v>
+        <v>logan.gomez89@outlook.com</v>
       </c>
       <c r="F233" t="str">
-        <v>(267) 288-3549</v>
+        <v>(628) 585-4251</v>
       </c>
       <c r="G233" t="str">
-        <v>Santa Ana</v>
+        <v>San Diego</v>
       </c>
       <c r="H233" t="str">
         <v>B</v>
@@ -7978,30 +7978,30 @@
         <v>assigned</v>
       </c>
       <c r="J233" t="str">
-        <v>Nolan Ortiz</v>
+        <v>Lydia Morris</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>644e41d7-b99e-4381-99a9-65d5ee89ad50</v>
+        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
       </c>
       <c r="B234" t="str">
-        <v>Hunter Scott</v>
+        <v>Christopher Carter</v>
       </c>
       <c r="C234">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D234" t="str">
         <v>Male</v>
       </c>
       <c r="E234" t="str">
-        <v>hunter.scott37@outlook.com</v>
+        <v>christopher.carter22@outlook.com</v>
       </c>
       <c r="F234" t="str">
-        <v>(477) 130-2066</v>
+        <v>(176) 989-4341</v>
       </c>
       <c r="G234" t="str">
-        <v>Torrance</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H234" t="str">
         <v>B</v>
@@ -8010,7 +8010,7 @@
         <v>assigned</v>
       </c>
       <c r="J234" t="str">
-        <v>Zoey Cook</v>
+        <v>Cora Mitchell</v>
       </c>
     </row>
   </sheetData>
@@ -8022,7 +8022,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H128"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8806,84 +8806,84 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>9d124ee2-b502-40e4-b28d-ebad65c39b47</v>
+        <v>abc90884-7bb5-47f2-bc0b-4618e71a6160</v>
       </c>
       <c r="B46" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C46" t="str">
-        <v>992418b2-3029-4752-9552-0aa886433657</v>
+        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" t="str">
-        <v>B5</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>f8801735-8ea8-4a63-896a-919be32a44a0</v>
+        <v>39f49fe8-d5e6-4790-a8c0-4bc8ff1cb5d3</v>
       </c>
       <c r="B47" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C47" t="str">
-        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
+        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" t="str">
-        <v>B4</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>51966534-1ea0-4c1f-9217-1334ae64e274</v>
+        <v>95a00fca-6d4c-460a-b294-864513db20f6</v>
       </c>
       <c r="B48" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C48" t="str">
-        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
+        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E48" t="str">
-        <v>A4</v>
+        <v>A5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>761f886f-529b-4094-9c04-a64fcf32a930</v>
+        <v>903a4e48-22f8-4231-beba-74c783ae42dd</v>
       </c>
       <c r="B49" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C49" t="str">
-        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
+        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E49" t="str">
-        <v>A5</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>119fe5b8-f8f9-445d-be8c-d5f3a8abb9cf</v>
+        <v>05236319-f53b-4884-b851-575c73357f94</v>
       </c>
       <c r="B50" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C50" t="str">
-        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
+        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
       </c>
       <c r="D50">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E50" t="str">
         <v>B2</v>
@@ -8891,33 +8891,33 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>11e7e46f-069e-440f-abfe-f9fee913f706</v>
+        <v>9d124ee2-b502-40e4-b28d-ebad65c39b47</v>
       </c>
       <c r="B51" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C51" t="str">
-        <v>4f5224b0-063d-43fd-9435-f5c2723f61ed</v>
+        <v>992418b2-3029-4752-9552-0aa886433657</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E51" t="str">
-        <v>B3</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>e63e61bd-5df7-45fa-984d-fcbac9fd47a3</v>
+        <v>f8801735-8ea8-4a63-896a-919be32a44a0</v>
       </c>
       <c r="B52" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C52" t="str">
-        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
+        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
       </c>
       <c r="D52">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E52" t="str">
         <v>B4</v>
@@ -8925,996 +8925,1302 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>e09faaf3-ec66-45a1-814a-689e80e97567</v>
+        <v>51966534-1ea0-4c1f-9217-1334ae64e274</v>
       </c>
       <c r="B53" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C53" t="str">
-        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
+        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
       </c>
       <c r="D53">
         <v>5</v>
       </c>
       <c r="E53" t="str">
-        <v>C1</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>e88328a9-4229-4115-8080-d544ac0d52da</v>
+        <v>761f886f-529b-4094-9c04-a64fcf32a930</v>
       </c>
       <c r="B54" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C54" t="str">
-        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
+        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
       </c>
       <c r="D54">
         <v>5</v>
       </c>
       <c r="E54" t="str">
-        <v>C2</v>
+        <v>A5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>b87b1294-5c2b-461f-a5ae-4a9e47cd5022</v>
+        <v>119fe5b8-f8f9-445d-be8c-d5f3a8abb9cf</v>
       </c>
       <c r="B55" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C55" t="str">
-        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
+        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
       </c>
       <c r="D55">
         <v>5</v>
       </c>
       <c r="E55" t="str">
-        <v>C3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>0bf53c3e-bb5c-4b11-8eb5-d242a41ffdf3</v>
+        <v>11e7e46f-069e-440f-abfe-f9fee913f706</v>
       </c>
       <c r="B56" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C56" t="str">
-        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
+        <v>4f5224b0-063d-43fd-9435-f5c2723f61ed</v>
       </c>
       <c r="D56">
         <v>5</v>
       </c>
       <c r="E56" t="str">
-        <v>C4</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>d013561b-40a6-4b73-9205-f625e31e2b8b</v>
+        <v>e63e61bd-5df7-45fa-984d-fcbac9fd47a3</v>
       </c>
       <c r="B57" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C57" t="str">
-        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
+        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
       </c>
       <c r="D57">
         <v>5</v>
       </c>
       <c r="E57" t="str">
-        <v>D1</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>0495fa93-25ec-42cf-baea-0795d1e11ef5</v>
+        <v>e09faaf3-ec66-45a1-814a-689e80e97567</v>
       </c>
       <c r="B58" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C58" t="str">
-        <v>644e41d7-b99e-4381-99a9-65d5ee89ad50</v>
+        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
       </c>
       <c r="D58">
         <v>5</v>
       </c>
       <c r="E58" t="str">
-        <v>D2</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>ed31b312-db35-4c68-b7a9-a90a6e150e36</v>
+        <v>e88328a9-4229-4115-8080-d544ac0d52da</v>
       </c>
       <c r="B59" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C59" t="str">
-        <v>cd2f354f-9f45-4422-af14-1c94758ec1c1</v>
+        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
       </c>
       <c r="D59">
         <v>5</v>
       </c>
       <c r="E59" t="str">
-        <v>D3</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>ed95bf26-add0-459b-97df-6299a34137b1</v>
+        <v>b87b1294-5c2b-461f-a5ae-4a9e47cd5022</v>
       </c>
       <c r="B60" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C60" t="str">
-        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
+        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
       </c>
       <c r="D60">
         <v>5</v>
       </c>
       <c r="E60" t="str">
-        <v>D4</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>1dde0982-8406-4022-9da3-e90925e3d2a2</v>
+        <v>0bf53c3e-bb5c-4b11-8eb5-d242a41ffdf3</v>
       </c>
       <c r="B61" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C61" t="str">
-        <v>9d6b206c-c62d-4b71-b83d-fb61ac2fd06b</v>
+        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
       </c>
       <c r="D61">
         <v>5</v>
       </c>
       <c r="E61" t="str">
-        <v>E1</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>bf4931ff-0b09-49e2-bf7a-5c6c07f059ab</v>
+        <v>d013561b-40a6-4b73-9205-f625e31e2b8b</v>
       </c>
       <c r="B62" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C62" t="str">
-        <v>5e93a4d1-9d7c-4b53-9898-a1ae2a0319c1</v>
+        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
       </c>
       <c r="D62">
         <v>5</v>
       </c>
       <c r="E62" t="str">
-        <v>E2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>878bd12f-f08a-4560-bbca-b0d6f34eca7f</v>
+        <v>0495fa93-25ec-42cf-baea-0795d1e11ef5</v>
       </c>
       <c r="B63" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C63" t="str">
-        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
+        <v>644e41d7-b99e-4381-99a9-65d5ee89ad50</v>
       </c>
       <c r="D63">
         <v>5</v>
       </c>
       <c r="E63" t="str">
-        <v>B5</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>f04ab471-1a9d-4e0c-8e4b-3d79e4d4882b</v>
+        <v>ed31b312-db35-4c68-b7a9-a90a6e150e36</v>
       </c>
       <c r="B64" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C64" t="str">
-        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
+        <v>cd2f354f-9f45-4422-af14-1c94758ec1c1</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E64" t="str">
-        <v>B3</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>de24e1b7-54f7-4944-86a8-442ceab4b214</v>
+        <v>ed95bf26-add0-459b-97df-6299a34137b1</v>
       </c>
       <c r="B65" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C65" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E65" t="str">
-        <v>A3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
+        <v>1dde0982-8406-4022-9da3-e90925e3d2a2</v>
       </c>
       <c r="B66" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C66" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>9d6b206c-c62d-4b71-b83d-fb61ac2fd06b</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E66" t="str">
-        <v>A1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
+        <v>bf4931ff-0b09-49e2-bf7a-5c6c07f059ab</v>
       </c>
       <c r="B67" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C67" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>5e93a4d1-9d7c-4b53-9898-a1ae2a0319c1</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E67" t="str">
-        <v>A2</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
+        <v>878bd12f-f08a-4560-bbca-b0d6f34eca7f</v>
       </c>
       <c r="B68" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C68" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
       </c>
       <c r="D68">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E68" t="str">
-        <v>A3</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
+        <v>27cd1874-4bb0-4c8c-a33d-bce7d3953d7c</v>
       </c>
       <c r="B69" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C69" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>ba63a5c0-c76e-4c1b-b6e4-afed15dfdcd4</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E69" t="str">
-        <v>B1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
+        <v>f04ab471-1a9d-4e0c-8e4b-3d79e4d4882b</v>
       </c>
       <c r="B70" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C70" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
+        <v>de24e1b7-54f7-4944-86a8-442ceab4b214</v>
       </c>
       <c r="B71" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C71" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E71" t="str">
-        <v>B3</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
+        <v>41908319-8972-43d7-9b08-206bf042c511</v>
       </c>
       <c r="B72" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C72" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
       </c>
       <c r="D72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E72" t="str">
-        <v>C1</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
+        <v>f71c41ee-f916-4b81-a663-25408201b8a6</v>
       </c>
       <c r="B73" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C73" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
       </c>
       <c r="D73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E73" t="str">
-        <v>C2</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
+        <v>6d7cac97-d6fa-45e9-b53d-a4889f77a4b8</v>
       </c>
       <c r="B74" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C74" t="str">
-        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
+        <v>0d8894f6-9a60-421c-a7c0-144fe2f8c85f</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E74" t="str">
-        <v>C3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
+        <v>21537b52-b6c8-4c1c-bb96-efc216606cf8</v>
       </c>
       <c r="B75" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C75" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>c347dd65-5ee0-40a6-9fce-2500b3aed70c</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E75" t="str">
-        <v>D1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
+        <v>e332b5a1-cf4b-4ae7-8764-836bd91437d7</v>
       </c>
       <c r="B76" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C76" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E76" t="str">
-        <v>D3</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
+        <v>247fa2d4-3c08-4707-9dbf-04c5599db34b</v>
       </c>
       <c r="B77" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C77" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E77" t="str">
-        <v>E1</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
+        <v>93ba3613-4c25-42cd-a803-3ae23c8a3af1</v>
       </c>
       <c r="B78" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C78" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E78" t="str">
-        <v>E2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
+        <v>c66603aa-a436-4839-9ac0-1423aa046b6f</v>
       </c>
       <c r="B79" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C79" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
       </c>
       <c r="D79">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E79" t="str">
-        <v>A1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
+        <v>18514c0d-89a5-4589-b5d5-6e5ee2b359a1</v>
       </c>
       <c r="B80" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C80" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E80" t="str">
-        <v>A2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
+        <v>bb12148c-a2b5-4934-a7d3-e374408e192a</v>
       </c>
       <c r="B81" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C81" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E81" t="str">
-        <v>A3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
+        <v>62b60541-5bb1-45f5-b550-2565f503ffd9</v>
       </c>
       <c r="B82" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C82" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
       </c>
       <c r="D82">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E82" t="str">
-        <v>B1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
+        <v>9c903808-fa4e-4126-8535-061627923006</v>
       </c>
       <c r="B83" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C83" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>c49dde07-b870-477a-82b6-a0354611093f</v>
       </c>
       <c r="D83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E83" t="str">
-        <v>B2</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
+        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
       </c>
       <c r="B84" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C84" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D84">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E84" t="str">
-        <v>B3</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
+        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
       </c>
       <c r="B85" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C85" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="D85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E85" t="str">
-        <v>C1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
+        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="D86">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E86" t="str">
-        <v>C2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
+        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D87">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E87" t="str">
-        <v>C3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
+        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E88" t="str">
-        <v>D1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
+        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
       </c>
       <c r="B89" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C89" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D89">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E89" t="str">
-        <v>D2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
+        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
       </c>
       <c r="B90" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C90" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E90" t="str">
-        <v>D3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
+        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
       </c>
       <c r="B91" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C91" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="D91">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E91" t="str">
-        <v>E1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
+        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
       </c>
       <c r="B92" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C92" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
       </c>
       <c r="D92">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E92" t="str">
-        <v>E2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
+        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
       </c>
       <c r="B93" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C93" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D93">
         <v>2</v>
       </c>
       <c r="E93" t="str">
-        <v>A4</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
       </c>
       <c r="B94" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C94" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E94" t="str">
-        <v>A1</v>
-      </c>
-      <c r="F94" s="1">
-        <v>46000.538291944446</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>e914a306-fff3-4997-a092-87302be1bda0</v>
+        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
       </c>
       <c r="B95" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C95" t="str">
-        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E95" t="str">
-        <v>A1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>64318131-3a36-4d14-a6ce-2699b7013fe5</v>
+        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
       </c>
       <c r="B96" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C96" t="str">
-        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96" t="str">
-        <v>A2</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>3b230921-6709-4bb4-b5dc-fd764580c535</v>
+        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
       </c>
       <c r="B97" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C97" t="str">
-        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E97" t="str">
-        <v>A3</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>8fd02704-d4d6-498b-a9f9-66180b64176b</v>
+        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
       </c>
       <c r="B98" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C98" t="str">
-        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E98" t="str">
-        <v>A4</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>40079e20-52ad-4652-afcd-333795a7592d</v>
+        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
       </c>
       <c r="B99" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C99" t="str">
-        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E99" t="str">
-        <v>B1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
+        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
       </c>
       <c r="B100" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C100" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E100" t="str">
-        <v>D1</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
       </c>
       <c r="B101" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C101" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E101" t="str">
-        <v>E1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
+        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
       </c>
       <c r="B102" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C102" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E102" t="str">
-        <v>D2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
+        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
       </c>
       <c r="B103" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C103" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E103" t="str">
-        <v>C3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
+        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
       </c>
       <c r="B104" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C104" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E104" t="str">
-        <v>B2</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
+        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
       </c>
       <c r="B105" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C105" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E105" t="str">
-        <v>B1</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
       </c>
       <c r="B106" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C106" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E106" t="str">
-        <v>E2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
+        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
       </c>
       <c r="B107" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C107" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E107" t="str">
-        <v>C1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
       </c>
       <c r="B108" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C108" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E108" t="str">
-        <v>C2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
+        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
       </c>
       <c r="B109" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C109" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
       </c>
       <c r="D109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E109" t="str">
-        <v>D2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
+        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
       </c>
       <c r="B110" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C110" t="str">
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+      </c>
+      <c r="D110">
+        <v>3</v>
+      </c>
+      <c r="E110" t="str">
+        <v>E2</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
+      </c>
+      <c r="B111" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C111" t="str">
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
+      <c r="E111" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+      </c>
+      <c r="B112" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C112" t="str">
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112" t="str">
+        <v>A1</v>
+      </c>
+      <c r="F112" s="1">
+        <v>46000.538291944446</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>e914a306-fff3-4997-a092-87302be1bda0</v>
+      </c>
+      <c r="B113" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C113" t="str">
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>64318131-3a36-4d14-a6ce-2699b7013fe5</v>
+      </c>
+      <c r="B114" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C114" t="str">
+        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>3b230921-6709-4bb4-b5dc-fd764580c535</v>
+      </c>
+      <c r="B115" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C115" t="str">
+        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>8fd02704-d4d6-498b-a9f9-66180b64176b</v>
+      </c>
+      <c r="B116" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C116" t="str">
+        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>40079e20-52ad-4652-afcd-333795a7592d</v>
+      </c>
+      <c r="B117" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C117" t="str">
+        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
+      </c>
+      <c r="B118" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C118" t="str">
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118" t="str">
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+      </c>
+      <c r="B119" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C119" t="str">
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119" t="str">
+        <v>E1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
+      </c>
+      <c r="B120" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C120" t="str">
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120" t="str">
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
+      </c>
+      <c r="B121" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C121" t="str">
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121" t="str">
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
+      </c>
+      <c r="B122" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C122" t="str">
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
+      </c>
+      <c r="B123" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C123" t="str">
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+      </c>
+      <c r="B124" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C124" t="str">
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124" t="str">
+        <v>E2</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
+      </c>
+      <c r="B125" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C125" t="str">
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125" t="str">
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+      </c>
+      <c r="B126" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C126" t="str">
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126" t="str">
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
+      </c>
+      <c r="B127" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C127" t="str">
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+      </c>
+      <c r="D127">
+        <v>2</v>
+      </c>
+      <c r="E127" t="str">
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>385ae883-11fc-4366-bdc9-aa7d308cbed7</v>
+      </c>
+      <c r="B128" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C128" t="str">
         <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
-      <c r="D110">
+      <c r="D128">
         <v>1</v>
       </c>
-      <c r="E110" t="str">
+      <c r="E128" t="str">
         <v>D3</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H110"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H128"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Improve booking master with wider email column and new filter
Add state and UI elements for filtering by mobility/medical notes, and increase email column width in the booking master component.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: c0bba8e9-2e26-453a-9a0e-1b9806651fe7
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/LuBJ9EM
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -8415,16 +8415,16 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>6b58308c-f80d-416c-9b6b-02f4314a33f4</v>
+        <v>a97926fa-e299-48be-85b1-e1343993016e</v>
       </c>
       <c r="B23" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C23" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>55099144-967b-4cf2-b4ed-3cfe46413c92</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" t="str">
         <v>A1</v>
@@ -8432,1022 +8432,1025 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>a97926fa-e299-48be-85b1-e1343993016e</v>
+        <v>a04b9cdf-0d05-470d-9579-53050bf1b69f</v>
       </c>
       <c r="B24" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C24" t="str">
-        <v>55099144-967b-4cf2-b4ed-3cfe46413c92</v>
+        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" t="str">
-        <v>A1</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>a04b9cdf-0d05-470d-9579-53050bf1b69f</v>
+        <v>2d6fdbfc-4ce4-4f0f-ba31-f5c3767b5bf5</v>
       </c>
       <c r="B25" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C25" t="str">
-        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
+        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="str">
-        <v>D3</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>2d6fdbfc-4ce4-4f0f-ba31-f5c3767b5bf5</v>
+        <v>d6ecfe08-434d-4976-953e-104a37395b18</v>
       </c>
       <c r="B26" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C26" t="str">
-        <v>ef837da0-c81f-4113-a389-db5e46ffaf4d</v>
+        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>d6ecfe08-434d-4976-953e-104a37395b18</v>
+        <v>c134ba6a-ddb7-4120-aed0-1ea7d0e15bfb</v>
       </c>
       <c r="B27" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C27" t="str">
-        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
+        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="str">
-        <v>A3</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>c134ba6a-ddb7-4120-aed0-1ea7d0e15bfb</v>
+        <v>31c38900-45f8-41f9-9ab0-9f456a22cc19</v>
       </c>
       <c r="B28" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C28" t="str">
-        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
+        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="str">
-        <v>A4</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>31c38900-45f8-41f9-9ab0-9f456a22cc19</v>
+        <v>adc97863-865a-446e-a358-dc9f417aa045</v>
       </c>
       <c r="B29" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C29" t="str">
-        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
+        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>adc97863-865a-446e-a358-dc9f417aa045</v>
+        <v>9c0bc3bf-f674-4ebb-8830-9f6ddb35f439</v>
       </c>
       <c r="B30" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C30" t="str">
-        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
+        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>9c0bc3bf-f674-4ebb-8830-9f6ddb35f439</v>
+        <v>fd79c7f9-c2e0-422e-88a0-b8e4788c5ac3</v>
       </c>
       <c r="B31" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C31" t="str">
-        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
+        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" t="str">
-        <v>B3</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>fd79c7f9-c2e0-422e-88a0-b8e4788c5ac3</v>
+        <v>81983df4-6d98-4079-997a-b15e4992f0c2</v>
       </c>
       <c r="B32" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C32" t="str">
-        <v>ef94ff15-5215-4ecd-9ad1-9ac44fd0e56a</v>
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32" t="str">
-        <v>B4</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>81983df4-6d98-4079-997a-b15e4992f0c2</v>
+        <v>877d9b81-b96c-49af-8522-ef897840f2c0</v>
       </c>
       <c r="B33" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C33" t="str">
-        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
+        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
       <c r="E33" t="str">
-        <v>B5</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>877d9b81-b96c-49af-8522-ef897840f2c0</v>
+        <v>7c0b3acd-b99e-4207-b47e-2a531410627d</v>
       </c>
       <c r="B34" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C34" t="str">
-        <v>2811bf99-369b-4c0a-b5d6-4ff46cd7aa5e</v>
+        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
       </c>
       <c r="D34">
         <v>2</v>
       </c>
       <c r="E34" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>7c0b3acd-b99e-4207-b47e-2a531410627d</v>
+        <v>f7e3b01b-afaf-4c03-9826-6e5040f8804b</v>
       </c>
       <c r="B35" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C35" t="str">
-        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
+        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
       </c>
       <c r="D35">
         <v>2</v>
       </c>
       <c r="E35" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>f7e3b01b-afaf-4c03-9826-6e5040f8804b</v>
+        <v>f77f8950-24a9-4561-9e88-09c9d8058861</v>
       </c>
       <c r="B36" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C36" t="str">
-        <v>6ddd3228-f125-4d3e-88e2-157cd730b552</v>
+        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
       </c>
       <c r="D36">
         <v>2</v>
       </c>
       <c r="E36" t="str">
-        <v>C3</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>f77f8950-24a9-4561-9e88-09c9d8058861</v>
+        <v>ba728530-2c43-4629-a4ba-702f3ad076f7</v>
       </c>
       <c r="B37" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C37" t="str">
-        <v>40727c14-a30e-4e3b-8b64-0359d25efc0c</v>
+        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="E37" t="str">
-        <v>C4</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>ba728530-2c43-4629-a4ba-702f3ad076f7</v>
+        <v>307628e8-9f84-4bac-930b-c3975e190a5a</v>
       </c>
       <c r="B38" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C38" t="str">
-        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
+        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
       <c r="E38" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>307628e8-9f84-4bac-930b-c3975e190a5a</v>
+        <v>babf86d1-c049-47d3-85e9-dc4f0808f2aa</v>
       </c>
       <c r="B39" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C39" t="str">
-        <v>adb0c362-d095-4bfd-98dc-c93920fd22d6</v>
+        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
       <c r="E39" t="str">
-        <v>D2</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>babf86d1-c049-47d3-85e9-dc4f0808f2aa</v>
+        <v>5b34f428-822a-45f8-b317-88ee6aeff326</v>
       </c>
       <c r="B40" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C40" t="str">
-        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
+        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
       <c r="E40" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>5b34f428-822a-45f8-b317-88ee6aeff326</v>
+        <v>e2691b74-54bf-4ddf-903d-dcb57ab9d1c7</v>
       </c>
       <c r="B41" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C41" t="str">
-        <v>45c0fc2b-415d-475a-998d-934235565d6b</v>
+        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
       <c r="E41" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>e2691b74-54bf-4ddf-903d-dcb57ab9d1c7</v>
+        <v>a7f75281-d9f7-4feb-b1a8-06e8e021789d</v>
       </c>
       <c r="B42" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C42" t="str">
-        <v>d7b0dd51-8aea-4b32-bb8d-8b60271fc6c9</v>
+        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
       </c>
       <c r="D42">
         <v>2</v>
       </c>
       <c r="E42" t="str">
-        <v>E2</v>
+        <v>E3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>a7f75281-d9f7-4feb-b1a8-06e8e021789d</v>
+        <v>e41f9c69-762a-42e6-a22a-01d0f90c7a27</v>
       </c>
       <c r="B43" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C43" t="str">
-        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
+        <v>d1a4099f-cc65-41a4-8aa3-72e7788e4944</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
       <c r="E43" t="str">
-        <v>E3</v>
+        <v>E4</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>e41f9c69-762a-42e6-a22a-01d0f90c7a27</v>
+        <v>05e39e15-6494-4290-995c-10b090a68418</v>
       </c>
       <c r="B44" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C44" t="str">
-        <v>d1a4099f-cc65-41a4-8aa3-72e7788e4944</v>
+        <v>783b418b-9b0d-482c-a01b-75072978141f</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44" t="str">
-        <v>E4</v>
+        <v>A5</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>05e39e15-6494-4290-995c-10b090a68418</v>
+        <v>abc90884-7bb5-47f2-bc0b-4618e71a6160</v>
       </c>
       <c r="B45" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C45" t="str">
-        <v>783b418b-9b0d-482c-a01b-75072978141f</v>
+        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45" t="str">
-        <v>A5</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>abc90884-7bb5-47f2-bc0b-4618e71a6160</v>
+        <v>39f49fe8-d5e6-4790-a8c0-4bc8ff1cb5d3</v>
       </c>
       <c r="B46" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C46" t="str">
-        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
+        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="str">
-        <v>A3</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>39f49fe8-d5e6-4790-a8c0-4bc8ff1cb5d3</v>
+        <v>95a00fca-6d4c-460a-b294-864513db20f6</v>
       </c>
       <c r="B47" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C47" t="str">
-        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
+        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" t="str">
-        <v>A4</v>
+        <v>A5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>95a00fca-6d4c-460a-b294-864513db20f6</v>
+        <v>903a4e48-22f8-4231-beba-74c783ae42dd</v>
       </c>
       <c r="B48" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C48" t="str">
-        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
+        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="str">
-        <v>A5</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>903a4e48-22f8-4231-beba-74c783ae42dd</v>
+        <v>05236319-f53b-4884-b851-575c73357f94</v>
       </c>
       <c r="B49" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C49" t="str">
-        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
+        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>05236319-f53b-4884-b851-575c73357f94</v>
+        <v>9d124ee2-b502-40e4-b28d-ebad65c39b47</v>
       </c>
       <c r="B50" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C50" t="str">
-        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
+        <v>992418b2-3029-4752-9552-0aa886433657</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E50" t="str">
-        <v>B2</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>9d124ee2-b502-40e4-b28d-ebad65c39b47</v>
+        <v>f8801735-8ea8-4a63-896a-919be32a44a0</v>
       </c>
       <c r="B51" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C51" t="str">
-        <v>992418b2-3029-4752-9552-0aa886433657</v>
+        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51" t="str">
-        <v>B5</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>f8801735-8ea8-4a63-896a-919be32a44a0</v>
+        <v>51966534-1ea0-4c1f-9217-1334ae64e274</v>
       </c>
       <c r="B52" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C52" t="str">
-        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
+        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E52" t="str">
-        <v>B4</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>51966534-1ea0-4c1f-9217-1334ae64e274</v>
+        <v>761f886f-529b-4094-9c04-a64fcf32a930</v>
       </c>
       <c r="B53" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C53" t="str">
-        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
+        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
       </c>
       <c r="D53">
         <v>5</v>
       </c>
       <c r="E53" t="str">
-        <v>A4</v>
+        <v>A5</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>761f886f-529b-4094-9c04-a64fcf32a930</v>
+        <v>119fe5b8-f8f9-445d-be8c-d5f3a8abb9cf</v>
       </c>
       <c r="B54" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C54" t="str">
-        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
+        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
       </c>
       <c r="D54">
         <v>5</v>
       </c>
       <c r="E54" t="str">
-        <v>A5</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>119fe5b8-f8f9-445d-be8c-d5f3a8abb9cf</v>
+        <v>11e7e46f-069e-440f-abfe-f9fee913f706</v>
       </c>
       <c r="B55" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C55" t="str">
-        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
+        <v>4f5224b0-063d-43fd-9435-f5c2723f61ed</v>
       </c>
       <c r="D55">
         <v>5</v>
       </c>
       <c r="E55" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>11e7e46f-069e-440f-abfe-f9fee913f706</v>
+        <v>e63e61bd-5df7-45fa-984d-fcbac9fd47a3</v>
       </c>
       <c r="B56" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C56" t="str">
-        <v>4f5224b0-063d-43fd-9435-f5c2723f61ed</v>
+        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
       </c>
       <c r="D56">
         <v>5</v>
       </c>
       <c r="E56" t="str">
-        <v>B3</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>e63e61bd-5df7-45fa-984d-fcbac9fd47a3</v>
+        <v>e09faaf3-ec66-45a1-814a-689e80e97567</v>
       </c>
       <c r="B57" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C57" t="str">
-        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
+        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
       </c>
       <c r="D57">
         <v>5</v>
       </c>
       <c r="E57" t="str">
-        <v>B4</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>e09faaf3-ec66-45a1-814a-689e80e97567</v>
+        <v>e88328a9-4229-4115-8080-d544ac0d52da</v>
       </c>
       <c r="B58" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C58" t="str">
-        <v>699a6b21-dcdf-4a6c-a093-53af77ccdedb</v>
+        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
       </c>
       <c r="D58">
         <v>5</v>
       </c>
       <c r="E58" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>e88328a9-4229-4115-8080-d544ac0d52da</v>
+        <v>b87b1294-5c2b-461f-a5ae-4a9e47cd5022</v>
       </c>
       <c r="B59" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C59" t="str">
-        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
+        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
       </c>
       <c r="D59">
         <v>5</v>
       </c>
       <c r="E59" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>b87b1294-5c2b-461f-a5ae-4a9e47cd5022</v>
+        <v>0bf53c3e-bb5c-4b11-8eb5-d242a41ffdf3</v>
       </c>
       <c r="B60" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C60" t="str">
-        <v>da957311-60b3-4bfc-b980-ac0506dccd20</v>
+        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
       </c>
       <c r="D60">
         <v>5</v>
       </c>
       <c r="E60" t="str">
-        <v>C3</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>0bf53c3e-bb5c-4b11-8eb5-d242a41ffdf3</v>
+        <v>d013561b-40a6-4b73-9205-f625e31e2b8b</v>
       </c>
       <c r="B61" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C61" t="str">
-        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
+        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
       </c>
       <c r="D61">
         <v>5</v>
       </c>
       <c r="E61" t="str">
-        <v>C4</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>d013561b-40a6-4b73-9205-f625e31e2b8b</v>
+        <v>0495fa93-25ec-42cf-baea-0795d1e11ef5</v>
       </c>
       <c r="B62" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C62" t="str">
-        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
+        <v>644e41d7-b99e-4381-99a9-65d5ee89ad50</v>
       </c>
       <c r="D62">
         <v>5</v>
       </c>
       <c r="E62" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>0495fa93-25ec-42cf-baea-0795d1e11ef5</v>
+        <v>ed31b312-db35-4c68-b7a9-a90a6e150e36</v>
       </c>
       <c r="B63" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C63" t="str">
-        <v>644e41d7-b99e-4381-99a9-65d5ee89ad50</v>
+        <v>cd2f354f-9f45-4422-af14-1c94758ec1c1</v>
       </c>
       <c r="D63">
         <v>5</v>
       </c>
       <c r="E63" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>ed31b312-db35-4c68-b7a9-a90a6e150e36</v>
+        <v>ed95bf26-add0-459b-97df-6299a34137b1</v>
       </c>
       <c r="B64" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C64" t="str">
-        <v>cd2f354f-9f45-4422-af14-1c94758ec1c1</v>
+        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
       </c>
       <c r="D64">
         <v>5</v>
       </c>
       <c r="E64" t="str">
-        <v>D3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>ed95bf26-add0-459b-97df-6299a34137b1</v>
+        <v>1dde0982-8406-4022-9da3-e90925e3d2a2</v>
       </c>
       <c r="B65" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C65" t="str">
-        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
+        <v>9d6b206c-c62d-4b71-b83d-fb61ac2fd06b</v>
       </c>
       <c r="D65">
         <v>5</v>
       </c>
       <c r="E65" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>1dde0982-8406-4022-9da3-e90925e3d2a2</v>
+        <v>bf4931ff-0b09-49e2-bf7a-5c6c07f059ab</v>
       </c>
       <c r="B66" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C66" t="str">
-        <v>9d6b206c-c62d-4b71-b83d-fb61ac2fd06b</v>
+        <v>5e93a4d1-9d7c-4b53-9898-a1ae2a0319c1</v>
       </c>
       <c r="D66">
         <v>5</v>
       </c>
       <c r="E66" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>bf4931ff-0b09-49e2-bf7a-5c6c07f059ab</v>
+        <v>878bd12f-f08a-4560-bbca-b0d6f34eca7f</v>
       </c>
       <c r="B67" t="str">
         <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C67" t="str">
-        <v>5e93a4d1-9d7c-4b53-9898-a1ae2a0319c1</v>
+        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
       </c>
       <c r="D67">
         <v>5</v>
       </c>
       <c r="E67" t="str">
-        <v>E2</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>878bd12f-f08a-4560-bbca-b0d6f34eca7f</v>
+        <v>27cd1874-4bb0-4c8c-a33d-bce7d3953d7c</v>
       </c>
       <c r="B68" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C68" t="str">
-        <v>292da493-0524-4ee4-b911-1bb34e328b8c</v>
+        <v>ba63a5c0-c76e-4c1b-b6e4-afed15dfdcd4</v>
       </c>
       <c r="D68">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E68" t="str">
-        <v>B5</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>27cd1874-4bb0-4c8c-a33d-bce7d3953d7c</v>
+        <v>f04ab471-1a9d-4e0c-8e4b-3d79e4d4882b</v>
       </c>
       <c r="B69" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C69" t="str">
-        <v>ba63a5c0-c76e-4c1b-b6e4-afed15dfdcd4</v>
+        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="E69" t="str">
-        <v>E2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>f04ab471-1a9d-4e0c-8e4b-3d79e4d4882b</v>
+        <v>de24e1b7-54f7-4944-86a8-442ceab4b214</v>
       </c>
       <c r="B70" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C70" t="str">
-        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D70">
         <v>1</v>
       </c>
       <c r="E70" t="str">
-        <v>B3</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>de24e1b7-54f7-4944-86a8-442ceab4b214</v>
+        <v>41908319-8972-43d7-9b08-206bf042c511</v>
       </c>
       <c r="B71" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C71" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" t="str">
-        <v>A3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>41908319-8972-43d7-9b08-206bf042c511</v>
+        <v>f71c41ee-f916-4b81-a663-25408201b8a6</v>
       </c>
       <c r="B72" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C72" t="str">
-        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
+        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72" t="str">
-        <v>B3</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>f71c41ee-f916-4b81-a663-25408201b8a6</v>
+        <v>6d7cac97-d6fa-45e9-b53d-a4889f77a4b8</v>
       </c>
       <c r="B73" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C73" t="str">
-        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
+        <v>0d8894f6-9a60-421c-a7c0-144fe2f8c85f</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73" t="str">
-        <v>B4</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>6d7cac97-d6fa-45e9-b53d-a4889f77a4b8</v>
+        <v>21537b52-b6c8-4c1c-bb96-efc216606cf8</v>
       </c>
       <c r="B74" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C74" t="str">
-        <v>0d8894f6-9a60-421c-a7c0-144fe2f8c85f</v>
+        <v>c347dd65-5ee0-40a6-9fce-2500b3aed70c</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>21537b52-b6c8-4c1c-bb96-efc216606cf8</v>
+        <v>e332b5a1-cf4b-4ae7-8764-836bd91437d7</v>
       </c>
       <c r="B75" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C75" t="str">
-        <v>c347dd65-5ee0-40a6-9fce-2500b3aed70c</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>e332b5a1-cf4b-4ae7-8764-836bd91437d7</v>
+        <v>247fa2d4-3c08-4707-9dbf-04c5599db34b</v>
       </c>
       <c r="B76" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C76" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76" t="str">
-        <v>C3</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>247fa2d4-3c08-4707-9dbf-04c5599db34b</v>
+        <v>93ba3613-4c25-42cd-a803-3ae23c8a3af1</v>
       </c>
       <c r="B77" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C77" t="str">
-        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
+        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77" t="str">
-        <v>C4</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>93ba3613-4c25-42cd-a803-3ae23c8a3af1</v>
+        <v>c66603aa-a436-4839-9ac0-1423aa046b6f</v>
       </c>
       <c r="B78" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C78" t="str">
-        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
+        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>c66603aa-a436-4839-9ac0-1423aa046b6f</v>
+        <v>18514c0d-89a5-4589-b5d5-6e5ee2b359a1</v>
       </c>
       <c r="B79" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C79" t="str">
-        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
+        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>18514c0d-89a5-4589-b5d5-6e5ee2b359a1</v>
+        <v>bb12148c-a2b5-4934-a7d3-e374408e192a</v>
       </c>
       <c r="B80" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C80" t="str">
-        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
+        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="str">
-        <v>D3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>bb12148c-a2b5-4934-a7d3-e374408e192a</v>
+        <v>62b60541-5bb1-45f5-b550-2565f503ffd9</v>
       </c>
       <c r="B81" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C81" t="str">
-        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
+        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>62b60541-5bb1-45f5-b550-2565f503ffd9</v>
+        <v>9c903808-fa4e-4126-8535-061627923006</v>
       </c>
       <c r="B82" t="str">
         <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C82" t="str">
-        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
+        <v>c49dde07-b870-477a-82b6-a0354611093f</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="E82" t="str">
-        <v>E1</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>9c903808-fa4e-4126-8535-061627923006</v>
+        <v>6b58308c-f80d-416c-9b6b-02f4314a33f4</v>
       </c>
       <c r="B83" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C83" t="str">
-        <v>c49dde07-b870-477a-82b6-a0354611093f</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="str">
-        <v>B5</v>
+        <v>A1</v>
+      </c>
+      <c r="H83" t="str">
+        <v>idhsaiufahsdiufhasidufhuaidfhaisduhfaisuhfiuasdhfiuasdfiuasdhfiuadhsfiuadshfiuahsdifuahsdufuaishdfiudhf</v>
       </c>
     </row>
     <row r="84">

</xml_diff>

<commit_message>
Add a double confirmation to reset the seating chart safely
Implement a two-step confirmation dialog for the seating chart reset function in `seating-chart-page.tsx` to prevent accidental data loss.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 7a243cde-2a5b-46e9-aca9-fcc9fdf1281f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/LuBJ9EM
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9450,7 +9450,7 @@
         <v>A1</v>
       </c>
       <c r="H83" t="str">
-        <v>idhsaiufahsdiufhasidufhuaidfhaisduhfaisuhfiuasdhfiuasdfiuasdhfiuadhsfiuadshfiuahsdifuahsdufuaishdfiudhf</v>
+        <v/>
       </c>
     </row>
     <row r="84">
@@ -10036,155 +10036,155 @@
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
+        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
       </c>
       <c r="B118" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C118" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D118">
         <v>1</v>
       </c>
       <c r="E118" t="str">
-        <v>D1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>4186c00e-c265-4dd5-a5d0-4df7882a204b</v>
+        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
       </c>
       <c r="B119" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C119" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D119">
         <v>1</v>
       </c>
       <c r="E119" t="str">
-        <v>E1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>4714b65d-0643-42ca-a7a2-8459962131a8</v>
+        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
       </c>
       <c r="B120" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C120" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D120">
         <v>1</v>
       </c>
       <c r="E120" t="str">
-        <v>D2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>f979bc94-69a6-4473-be4f-3533f76cae2b</v>
+        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
       </c>
       <c r="B121" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C121" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="D121">
         <v>1</v>
       </c>
       <c r="E121" t="str">
-        <v>C3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>b6f1d429-67e4-45b4-a204-d05480319da0</v>
+        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
       </c>
       <c r="B122" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C122" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="D122">
         <v>1</v>
       </c>
       <c r="E122" t="str">
-        <v>B2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>5ecac9a7-a6b9-48f1-a93b-557a39838f17</v>
+        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
       </c>
       <c r="B123" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C123" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D123">
         <v>1</v>
       </c>
       <c r="E123" t="str">
-        <v>B1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>6bde6343-e29a-442a-9189-6dccf7f25850</v>
+        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
       </c>
       <c r="B124" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C124" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D124">
         <v>1</v>
       </c>
       <c r="E124" t="str">
-        <v>E2</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>1c3f244b-b164-4904-a5f1-1524195b494a</v>
+        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
       </c>
       <c r="B125" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C125" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D125">
         <v>1</v>
       </c>
       <c r="E125" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>eef4b984-c474-4f43-aeed-197faa279405</v>
+        <v>0d5bf843-81f3-4a36-925e-2ac5a65f3543</v>
       </c>
       <c r="B126" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C126" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D126">
         <v>1</v>
       </c>
       <c r="E126" t="str">
-        <v>C2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="127">

</xml_diff>

<commit_message>
Update winners page to display contestant and winnings information in a table
Modify the `winners.tsx` component to implement a new table structure with grouped headers for 'RECORD', 'CONTESTANTS', and 'WINNINGS' sections, along with associated data columns. Update `automatic-backup.json` to reflect new contestant data and availability status.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 2e501015-3316-4000-ab7d-12462effd0ce
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/LuBJ9EM
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -980,69 +980,69 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>c49dde07-b870-477a-82b6-a0354611093f</v>
+        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
       </c>
       <c r="B10" t="str">
-        <v>Mia Carter</v>
+        <v>Harper Lewis</v>
       </c>
       <c r="C10">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D10" t="str">
         <v>Female</v>
       </c>
       <c r="E10" t="str">
-        <v>mia.carter78@hotmail.com</v>
+        <v>harper.lewis57@hotmail.com</v>
       </c>
       <c r="F10" t="str">
-        <v>(419) 735-1016</v>
+        <v>0411 652 121</v>
       </c>
       <c r="G10" t="str">
-        <v>Newport Beach</v>
+        <v>Geelong</v>
       </c>
       <c r="H10" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I10" t="str">
         <v>assigned</v>
       </c>
       <c r="J10" t="str">
-        <v>Evelyn Ortiz</v>
+        <v>Audrey Ramirez</v>
+      </c>
+      <c r="M10" t="str">
+        <v>Back issues - needs lumbar support chair</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
+        <v>c49dde07-b870-477a-82b6-a0354611093f</v>
       </c>
       <c r="B11" t="str">
-        <v>Harper Lewis</v>
+        <v>Mia Carter</v>
       </c>
       <c r="C11">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D11" t="str">
         <v>Female</v>
       </c>
       <c r="E11" t="str">
-        <v>harper.lewis57@hotmail.com</v>
+        <v>mia.carter78@hotmail.com</v>
       </c>
       <c r="F11" t="str">
-        <v>0411 652 121</v>
+        <v>(419) 735-1016</v>
       </c>
       <c r="G11" t="str">
-        <v>Geelong</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H11" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I11" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J11" t="str">
-        <v>Audrey Ramirez</v>
-      </c>
-      <c r="M11" t="str">
-        <v>Back issues - needs lumbar support chair</v>
+        <v>Evelyn Ortiz</v>
       </c>
     </row>
     <row r="12">
@@ -1071,7 +1071,7 @@
         <v>B+</v>
       </c>
       <c r="I12" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J12" t="str">
         <v>Harper Lewis</v>
@@ -1833,7 +1833,7 @@
         <v>B</v>
       </c>
       <c r="I36" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J36" t="str">
         <v>Josiah Lopez, Ella Martinez</v>
@@ -1990,7 +1990,7 @@
         <v>B</v>
       </c>
       <c r="I41" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J41" t="str">
         <v>Josiah Lopez, Victoria Carter</v>
@@ -2614,22 +2614,22 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>14ca564a-7d73-46a9-9bdd-e4924eac5eda</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="B62" t="str">
-        <v>Hailey Thompson</v>
+        <v>Avery Cruz</v>
       </c>
       <c r="C62">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D62" t="str">
         <v>Female</v>
       </c>
       <c r="E62" t="str">
-        <v>hailey.thompson30@yahoo.com</v>
+        <v>avery.cruz48@yahoo.com</v>
       </c>
       <c r="F62" t="str">
-        <v>(356) 680-9661</v>
+        <v>(405) 750-6185</v>
       </c>
       <c r="G62" t="str">
         <v>Fremont</v>
@@ -2638,123 +2638,123 @@
         <v>B+</v>
       </c>
       <c r="I62" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J62" t="str">
+        <v>Lydia Torres, Mia Anderson</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
+        <v>14ca564a-7d73-46a9-9bdd-e4924eac5eda</v>
       </c>
       <c r="B63" t="str">
-        <v>Stella Martinez</v>
+        <v>Hailey Thompson</v>
       </c>
       <c r="C63">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D63" t="str">
         <v>Female</v>
       </c>
       <c r="E63" t="str">
-        <v>stella.martinez75@gmail.com</v>
+        <v>hailey.thompson30@yahoo.com</v>
       </c>
       <c r="F63" t="str">
-        <v>0404 227 272</v>
+        <v>(356) 680-9661</v>
       </c>
       <c r="G63" t="str">
-        <v>Ballarat</v>
+        <v>Fremont</v>
       </c>
       <c r="H63" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I63" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>9d6b206c-c62d-4b71-b83d-fb61ac2fd06b</v>
+        <v>47cc1288-cbc0-4159-a52d-924c8912434d</v>
       </c>
       <c r="B64" t="str">
-        <v>Paisley Brown</v>
+        <v>Stella Martinez</v>
       </c>
       <c r="C64">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D64" t="str">
         <v>Female</v>
       </c>
       <c r="E64" t="str">
-        <v>paisley.brown87@outlook.com</v>
+        <v>stella.martinez75@gmail.com</v>
       </c>
       <c r="F64" t="str">
-        <v>(164) 124-5926</v>
+        <v>0404 227 272</v>
       </c>
       <c r="G64" t="str">
-        <v>Anaheim</v>
+        <v>Ballarat</v>
       </c>
       <c r="H64" t="str">
         <v>B</v>
       </c>
       <c r="I64" t="str">
         <v>assigned</v>
-      </c>
-      <c r="J64" t="str">
-        <v>Amelia Nguyen</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>4f1d5a65-9d8d-4c5a-836a-f0ea71c91e56</v>
+        <v>9d6b206c-c62d-4b71-b83d-fb61ac2fd06b</v>
       </c>
       <c r="B65" t="str">
-        <v>Savannah Rivera</v>
+        <v>Paisley Brown</v>
       </c>
       <c r="C65">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="D65" t="str">
         <v>Female</v>
       </c>
       <c r="E65" t="str">
-        <v>savannah.rivera74@hotmail.com</v>
+        <v>paisley.brown87@outlook.com</v>
       </c>
       <c r="F65" t="str">
-        <v>(132) 232-5005</v>
+        <v>(164) 124-5926</v>
       </c>
       <c r="G65" t="str">
-        <v>Stockton</v>
+        <v>Anaheim</v>
       </c>
       <c r="H65" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I65" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J65" t="str">
-        <v>Penelope Williams</v>
+        <v>Amelia Nguyen</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>523bddcf-6298-42a0-b9cb-4deffb688143</v>
+        <v>4f1d5a65-9d8d-4c5a-836a-f0ea71c91e56</v>
       </c>
       <c r="B66" t="str">
-        <v>Brooklyn Rivera</v>
+        <v>Savannah Rivera</v>
       </c>
       <c r="C66">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D66" t="str">
         <v>Female</v>
       </c>
       <c r="E66" t="str">
-        <v>brooklyn.rivera69@outlook.com</v>
+        <v>savannah.rivera74@hotmail.com</v>
       </c>
       <c r="F66" t="str">
-        <v>(847) 715-1204</v>
+        <v>(132) 232-5005</v>
       </c>
       <c r="G66" t="str">
-        <v>Glendale</v>
+        <v>Stockton</v>
       </c>
       <c r="H66" t="str">
         <v>A+</v>
@@ -2763,39 +2763,39 @@
         <v>available</v>
       </c>
       <c r="J66" t="str">
-        <v>John Carter</v>
+        <v>Penelope Williams</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>523bddcf-6298-42a0-b9cb-4deffb688143</v>
       </c>
       <c r="B67" t="str">
-        <v>Avery Cruz</v>
+        <v>Brooklyn Rivera</v>
       </c>
       <c r="C67">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D67" t="str">
         <v>Female</v>
       </c>
       <c r="E67" t="str">
-        <v>avery.cruz48@yahoo.com</v>
+        <v>brooklyn.rivera69@outlook.com</v>
       </c>
       <c r="F67" t="str">
-        <v>(405) 750-6185</v>
+        <v>(847) 715-1204</v>
       </c>
       <c r="G67" t="str">
-        <v>Fremont</v>
+        <v>Glendale</v>
       </c>
       <c r="H67" t="str">
-        <v>B+</v>
+        <v>A+</v>
       </c>
       <c r="I67" t="str">
         <v>available</v>
       </c>
       <c r="J67" t="str">
-        <v>Lydia Torres, Mia Anderson</v>
+        <v>John Carter</v>
       </c>
     </row>
     <row r="68">
@@ -4181,95 +4181,95 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="B112" t="str">
-        <v>Piper Green</v>
+        <v>Valentina Morales</v>
       </c>
       <c r="C112">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D112" t="str">
         <v>Female</v>
       </c>
       <c r="E112" t="str">
-        <v>piper.green82@hotmail.com</v>
+        <v>valentina.morales27@icloud.com</v>
       </c>
       <c r="F112" t="str">
-        <v>(678) 816-2263</v>
+        <v>(896) 204-3978</v>
       </c>
       <c r="G112" t="str">
-        <v>Burbank</v>
+        <v>San Jose</v>
       </c>
       <c r="H112" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I112" t="str">
         <v>assigned</v>
       </c>
       <c r="J112" t="str">
-        <v>Josiah Brown</v>
+        <v>Adam Hall, Grayson Morgan</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
+        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
       </c>
       <c r="B113" t="str">
-        <v>Victoria Thompson</v>
+        <v>Piper Green</v>
       </c>
       <c r="C113">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D113" t="str">
         <v>Female</v>
       </c>
       <c r="E113" t="str">
-        <v>victoria.thompson68@yahoo.com</v>
+        <v>piper.green82@hotmail.com</v>
       </c>
       <c r="F113" t="str">
-        <v>(793) 601-6884</v>
+        <v>(678) 816-2263</v>
       </c>
       <c r="G113" t="str">
-        <v>San Jose</v>
+        <v>Burbank</v>
       </c>
       <c r="H113" t="str">
         <v>B</v>
       </c>
       <c r="I113" t="str">
         <v>assigned</v>
+      </c>
+      <c r="J113" t="str">
+        <v>Josiah Brown</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
       </c>
       <c r="B114" t="str">
-        <v>Lydia Torres</v>
+        <v>Victoria Thompson</v>
       </c>
       <c r="C114">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D114" t="str">
         <v>Female</v>
       </c>
       <c r="E114" t="str">
-        <v>lydia.torres72@yahoo.com</v>
+        <v>victoria.thompson68@yahoo.com</v>
       </c>
       <c r="F114" t="str">
-        <v>(828) 773-4386</v>
+        <v>(793) 601-6884</v>
       </c>
       <c r="G114" t="str">
-        <v>Anaheim</v>
+        <v>San Jose</v>
       </c>
       <c r="H114" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I114" t="str">
-        <v>available</v>
-      </c>
-      <c r="J114" t="str">
-        <v>Avery Cruz, Mia Anderson</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="115">
@@ -4303,252 +4303,252 @@
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="B116" t="str">
-        <v>Allison Torres</v>
+        <v>Lydia Torres</v>
       </c>
       <c r="C116">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D116" t="str">
         <v>Female</v>
       </c>
       <c r="E116" t="str">
-        <v>allison.torres94@gmail.com</v>
+        <v>lydia.torres72@yahoo.com</v>
       </c>
       <c r="F116" t="str">
-        <v>(858) 153-7242</v>
+        <v>(828) 773-4386</v>
       </c>
       <c r="G116" t="str">
-        <v>Fremont</v>
+        <v>Anaheim</v>
       </c>
       <c r="H116" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I116" t="str">
         <v>assigned</v>
       </c>
       <c r="J116" t="str">
-        <v>Christian Rivera, Elena Green</v>
+        <v>Avery Cruz, Mia Anderson</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="B117" t="str">
-        <v>Ryan Lewis</v>
+        <v>Allison Torres</v>
       </c>
       <c r="C117">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D117" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E117" t="str">
-        <v>ryan.lewis85@yahoo.com</v>
+        <v>allison.torres94@gmail.com</v>
       </c>
       <c r="F117" t="str">
-        <v>0400 187 811</v>
+        <v>(858) 153-7242</v>
       </c>
       <c r="G117" t="str">
-        <v>Canberra</v>
+        <v>Fremont</v>
       </c>
       <c r="H117" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I117" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J117" t="str">
+        <v>Christian Rivera, Elena Green</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
       </c>
       <c r="B118" t="str">
-        <v>Cora Mitchell</v>
+        <v>Ryan Lewis</v>
       </c>
       <c r="C118">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D118" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E118" t="str">
-        <v>cora.mitchell80@icloud.com</v>
+        <v>ryan.lewis85@yahoo.com</v>
       </c>
       <c r="F118" t="str">
-        <v>(929) 139-3875</v>
+        <v>0400 187 811</v>
       </c>
       <c r="G118" t="str">
-        <v>Newport Beach</v>
+        <v>Canberra</v>
       </c>
       <c r="H118" t="str">
         <v>B+</v>
       </c>
       <c r="I118" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J118" t="str">
-        <v>Christopher Carter</v>
+        <v>available</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="B119" t="str">
-        <v>Hannah Jones</v>
+        <v>Cora Mitchell</v>
       </c>
       <c r="C119">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D119" t="str">
         <v>Female</v>
       </c>
       <c r="E119" t="str">
-        <v>hannah.jones85@yahoo.com</v>
+        <v>cora.mitchell80@icloud.com</v>
       </c>
       <c r="F119" t="str">
-        <v>(644) 877-6251</v>
+        <v>(929) 139-3875</v>
       </c>
       <c r="G119" t="str">
-        <v>Sacramento</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H119" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I119" t="str">
         <v>assigned</v>
       </c>
       <c r="J119" t="str">
-        <v>Thomas Nguyen, Henry Roberts</v>
+        <v>Christopher Carter</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>4e28a208-5278-410d-b375-d9c77ba144d7</v>
+        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
       </c>
       <c r="B120" t="str">
-        <v>Riley Scott</v>
+        <v>Hannah Jones</v>
       </c>
       <c r="C120">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D120" t="str">
         <v>Female</v>
       </c>
       <c r="E120" t="str">
-        <v>riley.scott58@hotmail.com</v>
+        <v>hannah.jones85@yahoo.com</v>
       </c>
       <c r="F120" t="str">
-        <v>(848) 718-3465</v>
+        <v>(644) 877-6251</v>
       </c>
       <c r="G120" t="str">
-        <v>San Francisco</v>
+        <v>Sacramento</v>
       </c>
       <c r="H120" t="str">
         <v>B</v>
       </c>
       <c r="I120" t="str">
         <v>assigned</v>
+      </c>
+      <c r="J120" t="str">
+        <v>Thomas Nguyen, Henry Roberts</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
+        <v>4e28a208-5278-410d-b375-d9c77ba144d7</v>
       </c>
       <c r="B121" t="str">
-        <v>Penelope Williams</v>
+        <v>Riley Scott</v>
       </c>
       <c r="C121">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D121" t="str">
         <v>Female</v>
       </c>
       <c r="E121" t="str">
-        <v>penelope.williams29@hotmail.com</v>
+        <v>riley.scott58@hotmail.com</v>
       </c>
       <c r="F121" t="str">
-        <v>(735) 691-4267</v>
+        <v>(848) 718-3465</v>
       </c>
       <c r="G121" t="str">
-        <v>Sacramento</v>
+        <v>San Francisco</v>
       </c>
       <c r="H121" t="str">
         <v>B</v>
       </c>
       <c r="I121" t="str">
         <v>assigned</v>
-      </c>
-      <c r="J121" t="str">
-        <v>Savannah Rivera</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
+        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
       </c>
       <c r="B122" t="str">
-        <v>Avery Taylor</v>
+        <v>Penelope Williams</v>
       </c>
       <c r="C122">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D122" t="str">
         <v>Female</v>
       </c>
       <c r="E122" t="str">
-        <v>avery.taylor87@outlook.com</v>
+        <v>penelope.williams29@hotmail.com</v>
       </c>
       <c r="F122" t="str">
-        <v>(299) 491-7680</v>
+        <v>(735) 691-4267</v>
       </c>
       <c r="G122" t="str">
-        <v>Los Angeles</v>
+        <v>Sacramento</v>
       </c>
       <c r="H122" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I122" t="str">
         <v>assigned</v>
       </c>
       <c r="J122" t="str">
-        <v>Audrey Hill</v>
+        <v>Savannah Rivera</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
       </c>
       <c r="B123" t="str">
-        <v>Valentina Morales</v>
+        <v>Avery Taylor</v>
       </c>
       <c r="C123">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D123" t="str">
         <v>Female</v>
       </c>
       <c r="E123" t="str">
-        <v>valentina.morales27@icloud.com</v>
+        <v>avery.taylor87@outlook.com</v>
       </c>
       <c r="F123" t="str">
-        <v>(896) 204-3978</v>
+        <v>(299) 491-7680</v>
       </c>
       <c r="G123" t="str">
-        <v>San Jose</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H123" t="str">
         <v>B+</v>
       </c>
       <c r="I123" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J123" t="str">
-        <v>Adam Hall, Grayson Morgan</v>
+        <v>Audrey Hill</v>
       </c>
     </row>
     <row r="124">
@@ -5761,66 +5761,66 @@
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="B164" t="str">
-        <v>Anthony Garcia</v>
+        <v>Grayson Morgan</v>
       </c>
       <c r="C164">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D164" t="str">
         <v>Male</v>
       </c>
       <c r="E164" t="str">
-        <v>anthony.garcia31@yahoo.com</v>
+        <v>grayson.morgan95@outlook.com</v>
       </c>
       <c r="F164" t="str">
-        <v>(249) 774-7265</v>
+        <v>(524) 127-2584</v>
       </c>
       <c r="G164" t="str">
-        <v>Santa Monica</v>
+        <v>Irvine</v>
       </c>
       <c r="H164" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I164" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J164" t="str">
-        <v>Michael Johnson, Cameron Evans</v>
+        <v>Adam Hall, Valentina Morales</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="B165" t="str">
-        <v>Grayson Morgan</v>
+        <v>Cameron Evans</v>
       </c>
       <c r="C165">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D165" t="str">
         <v>Male</v>
       </c>
       <c r="E165" t="str">
-        <v>grayson.morgan95@outlook.com</v>
+        <v>cameron.evans55@outlook.com</v>
       </c>
       <c r="F165" t="str">
-        <v>(524) 127-2584</v>
+        <v>(535) 743-7467</v>
       </c>
       <c r="G165" t="str">
-        <v>Irvine</v>
+        <v>Fremont</v>
       </c>
       <c r="H165" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I165" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J165" t="str">
-        <v>Adam Hall, Valentina Morales</v>
+        <v>Michael Johnson, Anthony Garcia</v>
       </c>
     </row>
     <row r="166">
@@ -5889,34 +5889,34 @@
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="B168" t="str">
-        <v>Cameron Evans</v>
+        <v>Anthony Garcia</v>
       </c>
       <c r="C168">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D168" t="str">
         <v>Male</v>
       </c>
       <c r="E168" t="str">
-        <v>cameron.evans55@outlook.com</v>
+        <v>anthony.garcia31@yahoo.com</v>
       </c>
       <c r="F168" t="str">
-        <v>(535) 743-7467</v>
+        <v>(249) 774-7265</v>
       </c>
       <c r="G168" t="str">
-        <v>Fremont</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H168" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I168" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J168" t="str">
-        <v>Michael Johnson, Anthony Garcia</v>
+        <v>Michael Johnson, Cameron Evans</v>
       </c>
     </row>
     <row r="169">
@@ -6881,7 +6881,7 @@
         <v>B</v>
       </c>
       <c r="I199" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J199" t="str">
         <v>Avery Cruz, Lydia Torres</v>
@@ -6889,89 +6889,89 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="B200" t="str">
-        <v>Elijah Miller</v>
+        <v>Josiah Lopez</v>
       </c>
       <c r="C200">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="D200" t="str">
         <v>Male</v>
       </c>
       <c r="E200" t="str">
-        <v>elijah.miller73@outlook.com</v>
+        <v>josiah.lopez65@gmail.com</v>
       </c>
       <c r="F200" t="str">
-        <v>(967) 645-5202</v>
+        <v>(305) 140-9212</v>
       </c>
       <c r="G200" t="str">
-        <v>Pasadena</v>
+        <v>Chula Vista</v>
       </c>
       <c r="H200" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I200" t="str">
         <v>assigned</v>
       </c>
       <c r="J200" t="str">
-        <v>Sophia Flores</v>
+        <v>Victoria Carter, Ella Martinez</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
       </c>
       <c r="B201" t="str">
-        <v>Grace King</v>
+        <v>Elijah Miller</v>
       </c>
       <c r="C201">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D201" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E201" t="str">
-        <v>grace.king1@yahoo.com</v>
+        <v>elijah.miller73@outlook.com</v>
       </c>
       <c r="F201" t="str">
-        <v>(217) 721-5651</v>
+        <v>(967) 645-5202</v>
       </c>
       <c r="G201" t="str">
-        <v>Oakland</v>
+        <v>Pasadena</v>
       </c>
       <c r="H201" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I201" t="str">
         <v>assigned</v>
       </c>
       <c r="J201" t="str">
-        <v>Gianna Hill</v>
+        <v>Sophia Flores</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
+        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
       </c>
       <c r="B202" t="str">
-        <v>Thomas Rivera</v>
+        <v>Grace King</v>
       </c>
       <c r="C202">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D202" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E202" t="str">
-        <v>thomas.rivera13@yahoo.com</v>
+        <v>grace.king1@yahoo.com</v>
       </c>
       <c r="F202" t="str">
-        <v>(539) 243-6118</v>
+        <v>(217) 721-5651</v>
       </c>
       <c r="G202" t="str">
-        <v>Long Beach</v>
+        <v>Oakland</v>
       </c>
       <c r="H202" t="str">
         <v>B</v>
@@ -6980,164 +6980,164 @@
         <v>assigned</v>
       </c>
       <c r="J202" t="str">
-        <v>Hannah Murphy</v>
+        <v>Gianna Hill</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
       </c>
       <c r="B203" t="str">
-        <v>Christian Rivera</v>
+        <v>Thomas Rivera</v>
       </c>
       <c r="C203">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D203" t="str">
         <v>Male</v>
       </c>
       <c r="E203" t="str">
-        <v>christian.rivera21@outlook.com</v>
+        <v>thomas.rivera13@yahoo.com</v>
       </c>
       <c r="F203" t="str">
-        <v>(913) 900-2520</v>
+        <v>(539) 243-6118</v>
       </c>
       <c r="G203" t="str">
-        <v>Burbank</v>
+        <v>Long Beach</v>
       </c>
       <c r="H203" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I203" t="str">
         <v>assigned</v>
       </c>
       <c r="J203" t="str">
-        <v>Allison Torres, Elena Green</v>
+        <v>Hannah Murphy</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="B204" t="str">
-        <v>Josiah Brown</v>
+        <v>Christian Rivera</v>
       </c>
       <c r="C204">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="D204" t="str">
         <v>Male</v>
       </c>
       <c r="E204" t="str">
-        <v>josiah.brown19@hotmail.com</v>
+        <v>christian.rivera21@outlook.com</v>
       </c>
       <c r="F204" t="str">
-        <v>(678) 449-3168</v>
+        <v>(913) 900-2520</v>
       </c>
       <c r="G204" t="str">
-        <v>Fresno</v>
+        <v>Burbank</v>
       </c>
       <c r="H204" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I204" t="str">
         <v>assigned</v>
       </c>
       <c r="J204" t="str">
-        <v>Piper Green</v>
+        <v>Allison Torres, Elena Green</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
       </c>
       <c r="B205" t="str">
-        <v>Carter Harris</v>
+        <v>Josiah Brown</v>
       </c>
       <c r="C205">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D205" t="str">
         <v>Male</v>
       </c>
       <c r="E205" t="str">
-        <v>carter.harris82@yahoo.com</v>
+        <v>josiah.brown19@hotmail.com</v>
       </c>
       <c r="F205" t="str">
-        <v>0412 175 744</v>
+        <v>(678) 449-3168</v>
       </c>
       <c r="G205" t="str">
-        <v>Geelong</v>
+        <v>Fresno</v>
       </c>
       <c r="H205" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I205" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J205" t="str">
+        <v>Piper Green</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>f26a0638-511f-4440-ae1a-2ae052df470f</v>
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
       </c>
       <c r="B206" t="str">
-        <v>Caleb Brown</v>
+        <v>Carter Harris</v>
       </c>
       <c r="C206">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D206" t="str">
         <v>Male</v>
       </c>
       <c r="E206" t="str">
-        <v>caleb.brown13@yahoo.com</v>
+        <v>carter.harris82@yahoo.com</v>
       </c>
       <c r="F206" t="str">
-        <v>(130) 920-6765</v>
+        <v>0412 175 744</v>
       </c>
       <c r="G206" t="str">
-        <v>Irvine</v>
+        <v>Geelong</v>
       </c>
       <c r="H206" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I206" t="str">
         <v>available</v>
       </c>
-      <c r="J206" t="str">
-        <v>Jackson Murphy</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>f26a0638-511f-4440-ae1a-2ae052df470f</v>
       </c>
       <c r="B207" t="str">
-        <v>Josiah Lopez</v>
+        <v>Caleb Brown</v>
       </c>
       <c r="C207">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D207" t="str">
         <v>Male</v>
       </c>
       <c r="E207" t="str">
-        <v>josiah.lopez65@gmail.com</v>
+        <v>caleb.brown13@yahoo.com</v>
       </c>
       <c r="F207" t="str">
-        <v>(305) 140-9212</v>
+        <v>(130) 920-6765</v>
       </c>
       <c r="G207" t="str">
-        <v>Chula Vista</v>
+        <v>Irvine</v>
       </c>
       <c r="H207" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I207" t="str">
         <v>available</v>
       </c>
       <c r="J207" t="str">
-        <v>Victoria Carter, Ella Martinez</v>
+        <v>Jackson Murphy</v>
       </c>
     </row>
     <row r="208">
@@ -7584,75 +7584,75 @@
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="B222" t="str">
-        <v>Michael Johnson</v>
+        <v>Peter Adamidis</v>
       </c>
       <c r="C222">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D222" t="str">
-        <v>Male</v>
+        <v>Not Specified</v>
       </c>
       <c r="E222" t="str">
-        <v>michael.johnson96@gmail.com</v>
+        <v>peter.adamidis@gmail.com</v>
       </c>
       <c r="F222" t="str">
-        <v>(878) 132-4532</v>
+        <v>498086080</v>
       </c>
       <c r="G222" t="str">
-        <v>Long Beach</v>
+        <v/>
       </c>
       <c r="H222" t="str">
-        <v>B+</v>
+        <v/>
       </c>
       <c r="I222" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J222" t="str">
-        <v>Anthony Garcia, Cameron Evans</v>
+        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
+      </c>
+      <c r="K222" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L222" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M222" t="str">
+        <v>Broken Leg</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="B223" t="str">
-        <v>Peter Adamidis</v>
+        <v>Michael Johnson</v>
       </c>
       <c r="C223">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D223" t="str">
-        <v>Not Specified</v>
+        <v>Male</v>
       </c>
       <c r="E223" t="str">
-        <v>peter.adamidis@gmail.com</v>
+        <v>michael.johnson96@gmail.com</v>
       </c>
       <c r="F223" t="str">
-        <v>498086080</v>
+        <v>(878) 132-4532</v>
       </c>
       <c r="G223" t="str">
-        <v/>
+        <v>Long Beach</v>
       </c>
       <c r="H223" t="str">
-        <v/>
+        <v>B+</v>
       </c>
       <c r="I223" t="str">
         <v>assigned</v>
       </c>
       <c r="J223" t="str">
-        <v>Kathleen Reynolds, Felicity Parker-Hill</v>
-      </c>
-      <c r="K223" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L223" t="str">
-        <v>Y</v>
-      </c>
-      <c r="M223" t="str">
-        <v>Broken Leg</v>
+        <v>Anthony Garcia, Cameron Evans</v>
       </c>
     </row>
     <row r="224">
@@ -8007,7 +8007,7 @@
         <v>B</v>
       </c>
       <c r="I234" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J234" t="str">
         <v>Grayson Morgan, Valentina Morales</v>
@@ -8022,7 +8022,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H128"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9384,169 +9384,169 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
+        <v>94238789-3e48-4182-951f-ad6c22b56835</v>
       </c>
       <c r="B80" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C80" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E80" t="str">
-        <v>A1</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
+        <v>6ab36c0e-515a-4bef-92dc-5f197b5d66be</v>
       </c>
       <c r="B81" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C81" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E81" t="str">
-        <v>A2</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
+        <v>7b182117-dcd9-43dc-a84d-a4e9594886c9</v>
       </c>
       <c r="B82" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C82" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E82" t="str">
-        <v>A3</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
+        <v>03afd3fb-96ea-4d73-a8d0-f7ce1aed5926</v>
       </c>
       <c r="B83" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C83" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E83" t="str">
-        <v>B1</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
+        <v>b0984b8a-bb17-41cf-90cd-23d2387d955f</v>
       </c>
       <c r="B84" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C84" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="D84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E84" t="str">
-        <v>B2</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
+        <v>6bd3a81c-aa8a-4591-b7d4-de153efd709e</v>
       </c>
       <c r="B85" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C85" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E85" t="str">
-        <v>B3</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
+        <v>5ad79264-8134-4448-88b4-524092d74579</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E86" t="str">
-        <v>C1</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
+        <v>96073236-7911-4388-a7d8-3ff0ae72438c</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="D87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E87" t="str">
-        <v>C2</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
+        <v>4dd4af72-076f-4236-8a75-e635bcb3cfbd</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
+        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
       </c>
       <c r="D88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E88" t="str">
-        <v>C3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
+        <v>e2b43d20-55d6-424e-be30-93c17e352ed4</v>
       </c>
       <c r="B89" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C89" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E89" t="str">
         <v>D1</v>
@@ -9554,254 +9554,254 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
+        <v>c028037f-f828-4337-8b1b-3ec2dfa0c230</v>
       </c>
       <c r="B90" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C90" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E90" t="str">
-        <v>D3</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
+        <v>5ee4db13-eb2e-4434-9130-82e771b95f47</v>
       </c>
       <c r="B91" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C91" t="str">
-        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E91" t="str">
-        <v>E1</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
+        <v>a92643c4-bcdd-4d8c-828c-e3ddadc55a49</v>
       </c>
       <c r="B92" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C92" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
       </c>
       <c r="D92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E92" t="str">
-        <v>E2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
+        <v>afeecde8-8988-402f-99c4-c48da0f942cf</v>
       </c>
       <c r="B93" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C93" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
       </c>
       <c r="D93">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E93" t="str">
-        <v>A1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
+        <v>b396cb42-cc76-4350-89e8-98b94de4815d</v>
       </c>
       <c r="B94" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C94" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D94">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E94" t="str">
-        <v>A2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
+        <v>24e9391d-f1db-42e8-bf49-d8a50c6924a4</v>
       </c>
       <c r="B95" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C95" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="D95">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E95" t="str">
-        <v>A3</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
+        <v>5f3f2f6f-9c39-49d2-8992-ccaec88be285</v>
       </c>
       <c r="B96" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C96" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="D96">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E96" t="str">
-        <v>B1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
+        <v>0690114d-d0d8-4037-9a28-d510723b7e61</v>
       </c>
       <c r="B97" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C97" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D97">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E97" t="str">
-        <v>B2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
+        <v>9044d7ab-e884-4032-b97c-d8a8c1fe1e8d</v>
       </c>
       <c r="B98" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C98" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D98">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E98" t="str">
-        <v>B3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
+        <v>d8ab2aa6-f759-423e-ba36-95e19395f7e1</v>
       </c>
       <c r="B99" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C99" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D99">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E99" t="str">
-        <v>C1</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
+        <v>06479481-5b19-439e-b90b-b66c53b4b1b9</v>
       </c>
       <c r="B100" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C100" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="D100">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E100" t="str">
-        <v>C2</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
+        <v>14eafb47-bc4e-4314-8c84-c9ccd79c48e8</v>
       </c>
       <c r="B101" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C101" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="D101">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E101" t="str">
-        <v>C3</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
+        <v>4a33a5a3-b9e2-4572-bfae-7a07cc18cab4</v>
       </c>
       <c r="B102" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C102" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
       </c>
       <c r="D102">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E102" t="str">
-        <v>D1</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
+        <v>632a22c8-adb5-48e4-ae03-86b5b416926f</v>
       </c>
       <c r="B103" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C103" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D103">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E103" t="str">
-        <v>D2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
+        <v>e0bbac1a-ae2c-423f-8e95-33f1adad8dc2</v>
       </c>
       <c r="B104" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C104" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D104">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E104" t="str">
         <v>D3</v>
@@ -9809,16 +9809,16 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
+        <v>24e758b6-4ef6-4995-96d5-483fda8a9d64</v>
       </c>
       <c r="B105" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C105" t="str">
-        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+        <v>bcc86f75-9a60-406c-be7c-4f31ea5c30ef</v>
       </c>
       <c r="D105">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E105" t="str">
         <v>E1</v>
@@ -9826,16 +9826,16 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
+        <v>c7d873c9-6f65-40c6-ad2e-d5e386b74027</v>
       </c>
       <c r="B106" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C106" t="str">
-        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="D106">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E106" t="str">
         <v>E2</v>
@@ -9843,146 +9843,384 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
+        <v>5a54412a-9678-4001-8abf-6a6eb155c1e4</v>
       </c>
       <c r="B107" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C107" t="str">
-        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E107" t="str">
-        <v>A4</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+        <v>a95ab828-c44f-4fea-88a8-faa563ef3e25</v>
       </c>
       <c r="B108" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C108" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E108" t="str">
-        <v>A1</v>
-      </c>
-      <c r="F108" s="1">
-        <v>46000.538291944446</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>e914a306-fff3-4997-a092-87302be1bda0</v>
+        <v>887cbea0-1e69-44fb-b419-5c42ea7c1a87</v>
       </c>
       <c r="B109" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C109" t="str">
-        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E109" t="str">
-        <v>A1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>64318131-3a36-4d14-a6ce-2699b7013fe5</v>
+        <v>f6bd49a9-db23-44f1-9b32-84531f956b4f</v>
       </c>
       <c r="B110" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C110" t="str">
-        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E110" t="str">
-        <v>A2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>3b230921-6709-4bb4-b5dc-fd764580c535</v>
+        <v>a33050c8-c302-43e8-b68f-edc8511e8a25</v>
       </c>
       <c r="B111" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C111" t="str">
-        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E111" t="str">
-        <v>A3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>8fd02704-d4d6-498b-a9f9-66180b64176b</v>
+        <v>489d808e-b5d9-4d37-a0bf-6d38b6e944d6</v>
       </c>
       <c r="B112" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C112" t="str">
-        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E112" t="str">
-        <v>A4</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>40079e20-52ad-4652-afcd-333795a7592d</v>
+        <v>9239f2c8-8dff-49ae-a8f0-15cd14b10b4b</v>
       </c>
       <c r="B113" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C113" t="str">
-        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E113" t="str">
-        <v>B1</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
+        <v>87018188-dea2-488d-bbc5-93511f010e3c</v>
       </c>
       <c r="B114" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C114" t="str">
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+      </c>
+      <c r="D114">
+        <v>3</v>
+      </c>
+      <c r="E114" t="str">
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>de4be42d-21dc-4643-bb31-1a6bafe8b8cc</v>
+      </c>
+      <c r="B115" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C115" t="str">
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+      <c r="E115" t="str">
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>bea17053-72b9-4ca5-9625-5555aca8ca24</v>
+      </c>
+      <c r="B116" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C116" t="str">
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+      </c>
+      <c r="D116">
+        <v>3</v>
+      </c>
+      <c r="E116" t="str">
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>3e276ae2-bdb0-484a-9cfa-955e6b4ba8e2</v>
+      </c>
+      <c r="B117" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C117" t="str">
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+      </c>
+      <c r="D117">
+        <v>3</v>
+      </c>
+      <c r="E117" t="str">
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>5a1ae218-ce7d-4c8c-a2da-d630963af6f4</v>
+      </c>
+      <c r="B118" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C118" t="str">
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+      </c>
+      <c r="D118">
+        <v>3</v>
+      </c>
+      <c r="E118" t="str">
+        <v>D3</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>9dfb721b-6ee8-410c-8d7a-874ee0c4f5e1</v>
+      </c>
+      <c r="B119" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C119" t="str">
+        <v>dbb200b8-766c-4984-9724-f68192d88939</v>
+      </c>
+      <c r="D119">
+        <v>3</v>
+      </c>
+      <c r="E119" t="str">
+        <v>E1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>c0c1eeb3-ed06-4cb6-99bf-5b992835c4b3</v>
+      </c>
+      <c r="B120" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C120" t="str">
+        <v>aa6fa282-9894-4b21-a871-c9725586c397</v>
+      </c>
+      <c r="D120">
+        <v>3</v>
+      </c>
+      <c r="E120" t="str">
+        <v>E2</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>d966ee91-cd0e-4a0d-a751-798b92b03e60</v>
+      </c>
+      <c r="B121" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C121" t="str">
+        <v>df712cc5-31d8-4341-b177-6603bf089235</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
+      </c>
+      <c r="E121" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>47ec0204-7cf6-4afb-9b9e-a91324cdf4a9</v>
+      </c>
+      <c r="B122" t="str">
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+      </c>
+      <c r="C122" t="str">
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122" t="str">
+        <v>A1</v>
+      </c>
+      <c r="F122" s="1">
+        <v>46000.538291944446</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>e914a306-fff3-4997-a092-87302be1bda0</v>
+      </c>
+      <c r="B123" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C123" t="str">
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>64318131-3a36-4d14-a6ce-2699b7013fe5</v>
+      </c>
+      <c r="B124" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C124" t="str">
+        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>3b230921-6709-4bb4-b5dc-fd764580c535</v>
+      </c>
+      <c r="B125" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C125" t="str">
+        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>8fd02704-d4d6-498b-a9f9-66180b64176b</v>
+      </c>
+      <c r="B126" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C126" t="str">
+        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126" t="str">
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>40079e20-52ad-4652-afcd-333795a7592d</v>
+      </c>
+      <c r="B127" t="str">
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+      </c>
+      <c r="C127" t="str">
+        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>313caa2c-fc70-4c67-992c-01c66df3af1f</v>
+      </c>
+      <c r="B128" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C128" t="str">
         <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
-      <c r="D114">
+      <c r="D128">
         <v>2</v>
       </c>
-      <c r="E114" t="str">
+      <c r="E128" t="str">
         <v>D2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H114"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H128"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update winners table to display only the entered RX number
Fix the display of the RX DAY column in the winners table to show only the entered RX number, removing the redundant recordDayId.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f7c285b1-4e53-479d-8648-5698aa222cac
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/LuBJ9EM
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9554,53 +9554,53 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>94238789-3e48-4182-951f-ad6c22b56835</v>
+        <v>b0984b8a-bb17-41cf-90cd-23d2387d955f</v>
       </c>
       <c r="B90" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C90" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="D90">
         <v>1</v>
       </c>
       <c r="E90" t="str">
-        <v>E1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>b0984b8a-bb17-41cf-90cd-23d2387d955f</v>
+        <v>03afd3fb-96ea-4d73-a8d0-f7ce1aed5926</v>
       </c>
       <c r="B91" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C91" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D91">
         <v>1</v>
       </c>
       <c r="E91" t="str">
-        <v>A2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>03afd3fb-96ea-4d73-a8d0-f7ce1aed5926</v>
+        <v>94238789-3e48-4182-951f-ad6c22b56835</v>
       </c>
       <c r="B92" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C92" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="str">
-        <v>A1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="93">

</xml_diff>

<commit_message>
Update winning money modal to match user's desired field order
Reorders fields in the `WinningMoneyModal` component and adds new fields to the database backup schema.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 94e029c5-9ca8-4c99-9e76-042ea7eb1fa4
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/ZFgseqs
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9588,36 +9588,36 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>94238789-3e48-4182-951f-ad6c22b56835</v>
+        <v>6bd3a81c-aa8a-4591-b7d4-de153efd709e</v>
       </c>
       <c r="B92" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C92" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="str">
-        <v>E1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>6bd3a81c-aa8a-4591-b7d4-de153efd709e</v>
+        <v>94238789-3e48-4182-951f-ad6c22b56835</v>
       </c>
       <c r="B93" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C93" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
       <c r="E93" t="str">
-        <v>A3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="94">

</xml_diff>

<commit_message>
Add new player fields to allow saving of case amounts and winnings
Fix issue in `updateSeatAssignmentWorkflow` by adding `caseAmount`, `quickCash`, `bankOfferTaken`, `spinTheWheel`, and `prize` to the `allowedFields` object, enabling persistent storage of these player-specific financial details.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 13dd137b-94ec-4629-a851-14991b5454c3
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/ZFgseqs
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9588,36 +9588,36 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>6bd3a81c-aa8a-4591-b7d4-de153efd709e</v>
+        <v>94238789-3e48-4182-951f-ad6c22b56835</v>
       </c>
       <c r="B92" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C92" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="str">
-        <v>A3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>94238789-3e48-4182-951f-ad6c22b56835</v>
+        <v>6bd3a81c-aa8a-4591-b7d4-de153efd709e</v>
       </c>
       <c r="B93" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C93" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
       <c r="E93" t="str">
-        <v>E1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="94">

</xml_diff>

<commit_message>
Update winnings screen to use a dropdown for case numbers
Modify WinningMoneyModal to accept blockNumber and assignments, and change the case number input to a Select dropdown (1-22) that dynamically filters out already used case numbers within the same block. Update SeatingChartPage to pass necessary props to the modal.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: e33da256-43df-4099-920a-082332919526
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/ZFgseqs
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -9520,104 +9520,104 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>5ad79264-8134-4448-88b4-524092d74579</v>
+        <v>5ee4db13-eb2e-4434-9130-82e771b95f47</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88" t="str">
-        <v>B1</v>
+        <v>E3</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>5ee4db13-eb2e-4434-9130-82e771b95f47</v>
+        <v>b0984b8a-bb17-41cf-90cd-23d2387d955f</v>
       </c>
       <c r="B89" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C89" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
       <c r="E89" t="str">
-        <v>E3</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>b0984b8a-bb17-41cf-90cd-23d2387d955f</v>
+        <v>03afd3fb-96ea-4d73-a8d0-f7ce1aed5926</v>
       </c>
       <c r="B90" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C90" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D90">
         <v>1</v>
       </c>
       <c r="E90" t="str">
-        <v>A2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>03afd3fb-96ea-4d73-a8d0-f7ce1aed5926</v>
+        <v>94238789-3e48-4182-951f-ad6c22b56835</v>
       </c>
       <c r="B91" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C91" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D91">
         <v>1</v>
       </c>
       <c r="E91" t="str">
-        <v>A1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>94238789-3e48-4182-951f-ad6c22b56835</v>
+        <v>6bd3a81c-aa8a-4591-b7d4-de153efd709e</v>
       </c>
       <c r="B92" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C92" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" t="str">
-        <v>E1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>6bd3a81c-aa8a-4591-b7d4-de153efd709e</v>
+        <v>5ad79264-8134-4448-88b4-524092d74579</v>
       </c>
       <c r="B93" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C93" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
       <c r="E93" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="94">

</xml_diff>

<commit_message>
Improve contestant assignment consistency by applying demographic rules to all placements
Move the BlockScore type definition and apply demographic balancing rules to solo contestant assignments, ensuring consistent distribution across blocks.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 486fae39-183c-45b9-845f-6855c1d8e2bd
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/rmVdDTs
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,10 +5,11 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
-    <sheet name="Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
-    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
+    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
+    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
+    <sheet name="Groups" sheetId="5" r:id="rId5"/>
+    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -1965,182 +1966,182 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
       </c>
       <c r="B41" t="str">
-        <v>Leah Diaz</v>
+        <v>Zoey Cook</v>
       </c>
       <c r="C41">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D41" t="str">
         <v>Female</v>
       </c>
       <c r="E41" t="str">
-        <v>leah.diaz22@outlook.com</v>
+        <v>zoey.cook63@yahoo.com</v>
       </c>
       <c r="F41" t="str">
-        <v>(159) 664-9326</v>
+        <v>(559) 803-4092</v>
       </c>
       <c r="G41" t="str">
-        <v>Glendale</v>
+        <v>Fremont</v>
       </c>
       <c r="H41" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I41" t="str">
         <v>available</v>
       </c>
       <c r="J41" t="str">
-        <v>Julian Nguyen, Lydia Allen</v>
+        <v>Hunter Scott</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>49e2abec-5fbc-4b4e-9147-fc29f4df9e48</v>
       </c>
       <c r="B42" t="str">
-        <v>Naomi Moore</v>
+        <v>Ellie Allen</v>
       </c>
       <c r="C42">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D42" t="str">
         <v>Female</v>
       </c>
       <c r="E42" t="str">
-        <v>naomi.moore30@gmail.com</v>
+        <v>ellie.allen18@hotmail.com</v>
       </c>
       <c r="F42" t="str">
-        <v>(391) 998-1729</v>
+        <v>(303) 763-9138</v>
       </c>
       <c r="G42" t="str">
-        <v>Irvine</v>
+        <v>Stockton</v>
       </c>
       <c r="H42" t="str">
-        <v>B</v>
+        <v>A+</v>
       </c>
       <c r="I42" t="str">
         <v>available</v>
       </c>
       <c r="J42" t="str">
-        <v>Isla Wright, Cora Roberts</v>
+        <v>Emma Torres, Charlotte Hernandez</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>d3525475-4eef-4712-ba77-a79cea16ef55</v>
+        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
       </c>
       <c r="B43" t="str">
-        <v>Zoey Cook</v>
+        <v>Abigail Jackson</v>
       </c>
       <c r="C43">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D43" t="str">
         <v>Female</v>
       </c>
       <c r="E43" t="str">
-        <v>zoey.cook63@yahoo.com</v>
+        <v>abigail.jackson65@outlook.com</v>
       </c>
       <c r="F43" t="str">
-        <v>(559) 803-4092</v>
+        <v>0411 824 257</v>
       </c>
       <c r="G43" t="str">
-        <v>Fremont</v>
+        <v>Newcastle</v>
       </c>
       <c r="H43" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I43" t="str">
         <v>available</v>
-      </c>
-      <c r="J43" t="str">
-        <v>Hunter Scott</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>49e2abec-5fbc-4b4e-9147-fc29f4df9e48</v>
+        <v>55099144-967b-4cf2-b4ed-3cfe46413c92</v>
       </c>
       <c r="B44" t="str">
-        <v>Ellie Allen</v>
+        <v>Maya Hernandez</v>
       </c>
       <c r="C44">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D44" t="str">
         <v>Female</v>
       </c>
       <c r="E44" t="str">
-        <v>ellie.allen18@hotmail.com</v>
+        <v>maya.hernandez32@outlook.com</v>
       </c>
       <c r="F44" t="str">
-        <v>(303) 763-9138</v>
+        <v>0400 358 904</v>
       </c>
       <c r="G44" t="str">
-        <v>Stockton</v>
+        <v>Brisbane</v>
       </c>
       <c r="H44" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I44" t="str">
         <v>available</v>
       </c>
       <c r="J44" t="str">
-        <v>Emma Torres, Charlotte Hernandez</v>
+        <v>Aria Scott</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="B45" t="str">
-        <v>Abigail Jackson</v>
+        <v>Leah Diaz</v>
       </c>
       <c r="C45">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D45" t="str">
         <v>Female</v>
       </c>
       <c r="E45" t="str">
-        <v>abigail.jackson65@outlook.com</v>
+        <v>leah.diaz22@outlook.com</v>
       </c>
       <c r="F45" t="str">
-        <v>0411 824 257</v>
+        <v>(159) 664-9326</v>
       </c>
       <c r="G45" t="str">
-        <v>Newcastle</v>
+        <v>Glendale</v>
       </c>
       <c r="H45" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I45" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J45" t="str">
+        <v>Julian Nguyen, Lydia Allen</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>55099144-967b-4cf2-b4ed-3cfe46413c92</v>
+        <v>c5fdfaeb-862e-43ab-bf0e-ff3e14e5dbb3</v>
       </c>
       <c r="B46" t="str">
-        <v>Maya Hernandez</v>
+        <v>Hannah Martin</v>
       </c>
       <c r="C46">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D46" t="str">
         <v>Female</v>
       </c>
       <c r="E46" t="str">
-        <v>maya.hernandez32@outlook.com</v>
+        <v>hannah.martin78@yahoo.com</v>
       </c>
       <c r="F46" t="str">
-        <v>0400 358 904</v>
+        <v>0410 940 985</v>
       </c>
       <c r="G46" t="str">
-        <v>Brisbane</v>
+        <v>Hobart</v>
       </c>
       <c r="H46" t="str">
         <v>B</v>
@@ -2149,39 +2150,39 @@
         <v>available</v>
       </c>
       <c r="J46" t="str">
-        <v>Aria Scott</v>
+        <v>Abigail Lee</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>c5fdfaeb-862e-43ab-bf0e-ff3e14e5dbb3</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="B47" t="str">
-        <v>Hannah Martin</v>
+        <v>Naomi Moore</v>
       </c>
       <c r="C47">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D47" t="str">
         <v>Female</v>
       </c>
       <c r="E47" t="str">
-        <v>hannah.martin78@yahoo.com</v>
+        <v>naomi.moore30@gmail.com</v>
       </c>
       <c r="F47" t="str">
-        <v>0410 940 985</v>
+        <v>(391) 998-1729</v>
       </c>
       <c r="G47" t="str">
-        <v>Hobart</v>
+        <v>Irvine</v>
       </c>
       <c r="H47" t="str">
         <v>B</v>
       </c>
       <c r="I47" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J47" t="str">
-        <v>Abigail Lee</v>
+        <v>Isla Wright, Cora Roberts</v>
       </c>
     </row>
     <row r="48">
@@ -2837,63 +2838,63 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="B69" t="str">
-        <v>Carter Hill</v>
+        <v>Sofia Williams</v>
       </c>
       <c r="C69">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="D69" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E69" t="str">
-        <v>carter.hill93@gmail.com</v>
+        <v>sofia.williams60@outlook.com</v>
       </c>
       <c r="F69" t="str">
-        <v>0404 349 309</v>
+        <v>(745) 392-3827</v>
       </c>
       <c r="G69" t="str">
-        <v>Newcastle</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H69" t="str">
         <v>B</v>
       </c>
       <c r="I69" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J69" t="str">
+        <v>Colton Harris, Sebastian Edwards</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>25370fa8-38bb-4172-9e02-23a59fcfd87a</v>
       </c>
       <c r="B70" t="str">
-        <v>Sofia Williams</v>
+        <v>Carter Hill</v>
       </c>
       <c r="C70">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="D70" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E70" t="str">
-        <v>sofia.williams60@outlook.com</v>
+        <v>carter.hill93@gmail.com</v>
       </c>
       <c r="F70" t="str">
-        <v>(745) 392-3827</v>
+        <v>0404 349 309</v>
       </c>
       <c r="G70" t="str">
-        <v>Newport Beach</v>
+        <v>Newcastle</v>
       </c>
       <c r="H70" t="str">
         <v>B</v>
       </c>
       <c r="I70" t="str">
         <v>available</v>
-      </c>
-      <c r="J70" t="str">
-        <v>Colton Harris, Sebastian Edwards</v>
       </c>
     </row>
     <row r="71">
@@ -3270,25 +3271,25 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>182bd5d2-7f68-4c83-b156-e80856f3b6b7</v>
       </c>
       <c r="B83" t="str">
-        <v>Isla Wright</v>
+        <v>Mason Nelson</v>
       </c>
       <c r="C83">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D83" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E83" t="str">
-        <v>isla.wright1@yahoo.com</v>
+        <v>mason.nelson14@hotmail.com</v>
       </c>
       <c r="F83" t="str">
-        <v>(231) 918-9825</v>
+        <v>0403 485 650</v>
       </c>
       <c r="G83" t="str">
-        <v>Pasadena</v>
+        <v>Canberra</v>
       </c>
       <c r="H83" t="str">
         <v>B+</v>
@@ -3296,159 +3297,159 @@
       <c r="I83" t="str">
         <v>available</v>
       </c>
-      <c r="J83" t="str">
-        <v>Naomi Moore, Cora Roberts</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
       </c>
       <c r="B84" t="str">
-        <v>Lydia Allen</v>
+        <v>Grace Scott</v>
       </c>
       <c r="C84">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D84" t="str">
         <v>Female</v>
       </c>
       <c r="E84" t="str">
-        <v>lydia.allen73@icloud.com</v>
+        <v>grace.scott40@outlook.com</v>
       </c>
       <c r="F84" t="str">
-        <v>(363) 934-8723</v>
+        <v>0401 870 853</v>
       </c>
       <c r="G84" t="str">
-        <v>Oakland</v>
+        <v>Ballarat</v>
       </c>
       <c r="H84" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I84" t="str">
         <v>available</v>
       </c>
       <c r="J84" t="str">
-        <v>Julian Nguyen, Leah Diaz</v>
+        <v>Emily Moore</v>
+      </c>
+      <c r="M84" t="str">
+        <v>Hearing impaired - requires front row seating</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>182bd5d2-7f68-4c83-b156-e80856f3b6b7</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="B85" t="str">
-        <v>Mason Nelson</v>
+        <v>Elena Green</v>
       </c>
       <c r="C85">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D85" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E85" t="str">
-        <v>mason.nelson14@hotmail.com</v>
+        <v>elena.green83@gmail.com</v>
       </c>
       <c r="F85" t="str">
-        <v>0403 485 650</v>
+        <v>(274) 515-8123</v>
       </c>
       <c r="G85" t="str">
-        <v>Canberra</v>
+        <v>San Diego</v>
       </c>
       <c r="H85" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I85" t="str">
         <v>available</v>
+      </c>
+      <c r="J85" t="str">
+        <v>Allison Torres, Christian Rivera</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
       </c>
       <c r="B86" t="str">
-        <v>Grace Scott</v>
+        <v>Olivia Nelson</v>
       </c>
       <c r="C86">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D86" t="str">
         <v>Female</v>
       </c>
       <c r="E86" t="str">
-        <v>grace.scott40@outlook.com</v>
+        <v>olivia.nelson14@gmail.com</v>
       </c>
       <c r="F86" t="str">
-        <v>0401 870 853</v>
+        <v>(582) 644-7834</v>
       </c>
       <c r="G86" t="str">
-        <v>Ballarat</v>
+        <v>Bakersfield</v>
       </c>
       <c r="H86" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I86" t="str">
         <v>available</v>
       </c>
       <c r="J86" t="str">
-        <v>Emily Moore</v>
-      </c>
-      <c r="M86" t="str">
-        <v>Hearing impaired - requires front row seating</v>
+        <v>Joseph Stewart, Madelyn Martinez</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
       </c>
       <c r="B87" t="str">
-        <v>Elena Green</v>
+        <v>Eliana Green</v>
       </c>
       <c r="C87">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D87" t="str">
         <v>Female</v>
       </c>
       <c r="E87" t="str">
-        <v>elena.green83@gmail.com</v>
+        <v>eliana.green54@gmail.com</v>
       </c>
       <c r="F87" t="str">
-        <v>(274) 515-8123</v>
+        <v>(894) 795-3178</v>
       </c>
       <c r="G87" t="str">
-        <v>San Diego</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H87" t="str">
         <v>A</v>
       </c>
       <c r="I87" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J87" t="str">
-        <v>Allison Torres, Christian Rivera</v>
+        <v>Olivia Gonzalez</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
       </c>
       <c r="B88" t="str">
-        <v>Olivia Nelson</v>
+        <v>Victoria Scott</v>
       </c>
       <c r="C88">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D88" t="str">
         <v>Female</v>
       </c>
       <c r="E88" t="str">
-        <v>olivia.nelson14@gmail.com</v>
+        <v>victoria.scott67@icloud.com</v>
       </c>
       <c r="F88" t="str">
-        <v>(582) 644-7834</v>
+        <v>(507) 166-2977</v>
       </c>
       <c r="G88" t="str">
-        <v>Bakersfield</v>
+        <v>Torrance</v>
       </c>
       <c r="H88" t="str">
         <v>B</v>
@@ -3457,94 +3458,91 @@
         <v>available</v>
       </c>
       <c r="J88" t="str">
-        <v>Joseph Stewart, Madelyn Martinez</v>
+        <v>William Taylor</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
+        <v>0dd7de5c-0409-45e3-84a5-5f2ffbd591d8</v>
       </c>
       <c r="B89" t="str">
-        <v>Eliana Green</v>
+        <v>Harper Sanchez</v>
       </c>
       <c r="C89">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D89" t="str">
         <v>Female</v>
       </c>
       <c r="E89" t="str">
-        <v>eliana.green54@gmail.com</v>
+        <v>harper.sanchez76@gmail.com</v>
       </c>
       <c r="F89" t="str">
-        <v>(894) 795-3178</v>
+        <v>0411 422 972</v>
       </c>
       <c r="G89" t="str">
-        <v>Los Angeles</v>
+        <v>Geelong</v>
       </c>
       <c r="H89" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I89" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J89" t="str">
-        <v>Olivia Gonzalez</v>
+        <v>Leah Scott</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
+        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
       </c>
       <c r="B90" t="str">
-        <v>Victoria Scott</v>
+        <v>Hunter Jackson</v>
       </c>
       <c r="C90">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D90" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E90" t="str">
-        <v>victoria.scott67@icloud.com</v>
+        <v>hunter.jackson50@outlook.com</v>
       </c>
       <c r="F90" t="str">
-        <v>(507) 166-2977</v>
+        <v>0404 841 788</v>
       </c>
       <c r="G90" t="str">
-        <v>Torrance</v>
+        <v>Townsville</v>
       </c>
       <c r="H90" t="str">
         <v>B</v>
       </c>
       <c r="I90" t="str">
         <v>available</v>
-      </c>
-      <c r="J90" t="str">
-        <v>William Taylor</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>0dd7de5c-0409-45e3-84a5-5f2ffbd591d8</v>
+        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
       </c>
       <c r="B91" t="str">
-        <v>Harper Sanchez</v>
+        <v>Oliver Rivera</v>
       </c>
       <c r="C91">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D91" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E91" t="str">
-        <v>harper.sanchez76@gmail.com</v>
+        <v>oliver.rivera58@outlook.com</v>
       </c>
       <c r="F91" t="str">
-        <v>0411 422 972</v>
+        <v>0412 991 121</v>
       </c>
       <c r="G91" t="str">
-        <v>Geelong</v>
+        <v>Canberra</v>
       </c>
       <c r="H91" t="str">
         <v>B</v>
@@ -3552,31 +3550,31 @@
       <c r="I91" t="str">
         <v>available</v>
       </c>
-      <c r="J91" t="str">
-        <v>Leah Scott</v>
+      <c r="M91" t="str">
+        <v>Requires wheelchair access</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
+        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
       </c>
       <c r="B92" t="str">
-        <v>Hunter Jackson</v>
+        <v>Evelyn Clark</v>
       </c>
       <c r="C92">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="D92" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E92" t="str">
-        <v>hunter.jackson50@outlook.com</v>
+        <v>evelyn.clark47@outlook.com</v>
       </c>
       <c r="F92" t="str">
-        <v>0404 841 788</v>
+        <v>0410 941 656</v>
       </c>
       <c r="G92" t="str">
-        <v>Townsville</v>
+        <v>Hobart</v>
       </c>
       <c r="H92" t="str">
         <v>B</v>
@@ -3587,98 +3585,101 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
+        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
       </c>
       <c r="B93" t="str">
-        <v>Oliver Rivera</v>
+        <v>Aurora Rodriguez</v>
       </c>
       <c r="C93">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D93" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E93" t="str">
-        <v>oliver.rivera58@outlook.com</v>
+        <v>aurora.rodriguez20@yahoo.com</v>
       </c>
       <c r="F93" t="str">
-        <v>0412 991 121</v>
+        <v>0404 720 692</v>
       </c>
       <c r="G93" t="str">
-        <v>Canberra</v>
+        <v>Hobart</v>
       </c>
       <c r="H93" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I93" t="str">
         <v>available</v>
       </c>
+      <c r="J93" t="str">
+        <v>Emilia Lopez</v>
+      </c>
       <c r="M93" t="str">
-        <v>Requires wheelchair access</v>
+        <v>Arthritis - prefers aisle seating for easy exit</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>f693d8fc-436b-426a-9bca-0b141221ab3f</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="B94" t="str">
-        <v>Evelyn Clark</v>
+        <v>Lydia Allen</v>
       </c>
       <c r="C94">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D94" t="str">
         <v>Female</v>
       </c>
       <c r="E94" t="str">
-        <v>evelyn.clark47@outlook.com</v>
+        <v>lydia.allen73@icloud.com</v>
       </c>
       <c r="F94" t="str">
-        <v>0410 941 656</v>
+        <v>(363) 934-8723</v>
       </c>
       <c r="G94" t="str">
-        <v>Hobart</v>
+        <v>Oakland</v>
       </c>
       <c r="H94" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I94" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J94" t="str">
+        <v>Julian Nguyen, Leah Diaz</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>852226e3-fccb-4228-8627-5dc42cfe4387</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="B95" t="str">
-        <v>Aurora Rodriguez</v>
+        <v>Isla Wright</v>
       </c>
       <c r="C95">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D95" t="str">
         <v>Female</v>
       </c>
       <c r="E95" t="str">
-        <v>aurora.rodriguez20@yahoo.com</v>
+        <v>isla.wright1@yahoo.com</v>
       </c>
       <c r="F95" t="str">
-        <v>0404 720 692</v>
+        <v>(231) 918-9825</v>
       </c>
       <c r="G95" t="str">
-        <v>Hobart</v>
+        <v>Pasadena</v>
       </c>
       <c r="H95" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I95" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J95" t="str">
-        <v>Emilia Lopez</v>
-      </c>
-      <c r="M95" t="str">
-        <v>Arthritis - prefers aisle seating for easy exit</v>
+        <v>Naomi Moore, Cora Roberts</v>
       </c>
     </row>
     <row r="96">
@@ -3715,34 +3716,34 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
+        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
       </c>
       <c r="B97" t="str">
-        <v>Hannah Jones</v>
+        <v>Piper Green</v>
       </c>
       <c r="C97">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D97" t="str">
         <v>Female</v>
       </c>
       <c r="E97" t="str">
-        <v>hannah.jones85@yahoo.com</v>
+        <v>piper.green82@hotmail.com</v>
       </c>
       <c r="F97" t="str">
-        <v>(644) 877-6251</v>
+        <v>(678) 816-2263</v>
       </c>
       <c r="G97" t="str">
-        <v>Sacramento</v>
+        <v>Burbank</v>
       </c>
       <c r="H97" t="str">
         <v>B</v>
       </c>
       <c r="I97" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J97" t="str">
-        <v>Thomas Nguyen, Henry Roberts</v>
+        <v>Josiah Brown</v>
       </c>
     </row>
     <row r="98">
@@ -3840,89 +3841,89 @@
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
+        <v>bf1fc0b1-7d88-41a5-ab6f-ee4c085fd344</v>
       </c>
       <c r="B101" t="str">
-        <v>Layla Lopez</v>
+        <v>Brooklyn Nguyen</v>
       </c>
       <c r="C101">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D101" t="str">
         <v>Female</v>
       </c>
       <c r="E101" t="str">
-        <v>layla.lopez23@yahoo.com</v>
+        <v>brooklyn.nguyen77@yahoo.com</v>
       </c>
       <c r="F101" t="str">
-        <v>(607) 496-6102</v>
+        <v>(142) 872-1855</v>
       </c>
       <c r="G101" t="str">
         <v>Los Angeles</v>
       </c>
       <c r="H101" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I101" t="str">
         <v>available</v>
       </c>
       <c r="J101" t="str">
-        <v>Cora Lee</v>
+        <v>Naomi Brown</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>bf1fc0b1-7d88-41a5-ab6f-ee4c085fd344</v>
+        <v>50b098db-86f4-4a21-8425-ab03df8f7a40</v>
       </c>
       <c r="B102" t="str">
-        <v>Brooklyn Nguyen</v>
+        <v>Lillian Campbell</v>
       </c>
       <c r="C102">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D102" t="str">
         <v>Female</v>
       </c>
       <c r="E102" t="str">
-        <v>brooklyn.nguyen77@yahoo.com</v>
+        <v>lillian.campbell41@yahoo.com</v>
       </c>
       <c r="F102" t="str">
-        <v>(142) 872-1855</v>
+        <v>(945) 213-8284</v>
       </c>
       <c r="G102" t="str">
-        <v>Los Angeles</v>
+        <v>Pasadena</v>
       </c>
       <c r="H102" t="str">
-        <v>A</v>
+        <v>A+</v>
       </c>
       <c r="I102" t="str">
         <v>available</v>
       </c>
       <c r="J102" t="str">
-        <v>Naomi Brown</v>
+        <v>Amelia Lopez</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>50b098db-86f4-4a21-8425-ab03df8f7a40</v>
+        <v>e9a3f4c7-c9ed-4fd1-a5a9-d3763ae52a55</v>
       </c>
       <c r="B103" t="str">
-        <v>Lillian Campbell</v>
+        <v>Victoria Anderson</v>
       </c>
       <c r="C103">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D103" t="str">
         <v>Female</v>
       </c>
       <c r="E103" t="str">
-        <v>lillian.campbell41@yahoo.com</v>
+        <v>victoria.anderson1@outlook.com</v>
       </c>
       <c r="F103" t="str">
-        <v>(945) 213-8284</v>
+        <v>(622) 987-4829</v>
       </c>
       <c r="G103" t="str">
-        <v>Pasadena</v>
+        <v>Sacramento</v>
       </c>
       <c r="H103" t="str">
         <v>A+</v>
@@ -3931,94 +3932,91 @@
         <v>available</v>
       </c>
       <c r="J103" t="str">
-        <v>Amelia Lopez</v>
+        <v>Sophia Reyes</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>e9a3f4c7-c9ed-4fd1-a5a9-d3763ae52a55</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="B104" t="str">
-        <v>Victoria Anderson</v>
+        <v>Cora Mitchell</v>
       </c>
       <c r="C104">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D104" t="str">
         <v>Female</v>
       </c>
       <c r="E104" t="str">
-        <v>victoria.anderson1@outlook.com</v>
+        <v>cora.mitchell80@icloud.com</v>
       </c>
       <c r="F104" t="str">
-        <v>(622) 987-4829</v>
+        <v>(929) 139-3875</v>
       </c>
       <c r="G104" t="str">
-        <v>Sacramento</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H104" t="str">
-        <v>A+</v>
+        <v>B+</v>
       </c>
       <c r="I104" t="str">
         <v>available</v>
       </c>
       <c r="J104" t="str">
-        <v>Sophia Reyes</v>
+        <v>Christopher Carter</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
+        <v>9f873871-29cc-45f0-894c-c54745230689</v>
       </c>
       <c r="B105" t="str">
-        <v>Piper Green</v>
+        <v>Sadie Wright</v>
       </c>
       <c r="C105">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D105" t="str">
         <v>Female</v>
       </c>
       <c r="E105" t="str">
-        <v>piper.green82@hotmail.com</v>
+        <v>sadie.wright75@hotmail.com</v>
       </c>
       <c r="F105" t="str">
-        <v>(678) 816-2263</v>
+        <v>(617) 145-9784</v>
       </c>
       <c r="G105" t="str">
-        <v>Burbank</v>
+        <v>Anaheim</v>
       </c>
       <c r="H105" t="str">
         <v>B</v>
       </c>
       <c r="I105" t="str">
         <v>available</v>
-      </c>
-      <c r="J105" t="str">
-        <v>Josiah Brown</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="B106" t="str">
-        <v>Cora Mitchell</v>
+        <v>Serenity Campbell</v>
       </c>
       <c r="C106">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D106" t="str">
         <v>Female</v>
       </c>
       <c r="E106" t="str">
-        <v>cora.mitchell80@icloud.com</v>
+        <v>serenity.campbell1@yahoo.com</v>
       </c>
       <c r="F106" t="str">
-        <v>(929) 139-3875</v>
+        <v>(479) 565-5966</v>
       </c>
       <c r="G106" t="str">
-        <v>Newport Beach</v>
+        <v>Irvine</v>
       </c>
       <c r="H106" t="str">
         <v>B+</v>
@@ -4027,123 +4025,123 @@
         <v>available</v>
       </c>
       <c r="J106" t="str">
-        <v>Christopher Carter</v>
+        <v>Jackson Jackson, Isaiah Green</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>9f873871-29cc-45f0-894c-c54745230689</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="B107" t="str">
-        <v>Sadie Wright</v>
+        <v>Eleanor Hall</v>
       </c>
       <c r="C107">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D107" t="str">
         <v>Female</v>
       </c>
       <c r="E107" t="str">
-        <v>sadie.wright75@hotmail.com</v>
+        <v>eleanor.hall7@yahoo.com</v>
       </c>
       <c r="F107" t="str">
-        <v>(617) 145-9784</v>
+        <v>(627) 443-5972</v>
       </c>
       <c r="G107" t="str">
-        <v>Anaheim</v>
+        <v>Stockton</v>
       </c>
       <c r="H107" t="str">
         <v>B</v>
       </c>
       <c r="I107" t="str">
         <v>available</v>
+      </c>
+      <c r="J107" t="str">
+        <v>Michael Campbell, Sadie Williams</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
       </c>
       <c r="B108" t="str">
-        <v>Serenity Campbell</v>
+        <v>Hannah Jones</v>
       </c>
       <c r="C108">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D108" t="str">
         <v>Female</v>
       </c>
       <c r="E108" t="str">
-        <v>serenity.campbell1@yahoo.com</v>
+        <v>hannah.jones85@yahoo.com</v>
       </c>
       <c r="F108" t="str">
-        <v>(479) 565-5966</v>
+        <v>(644) 877-6251</v>
       </c>
       <c r="G108" t="str">
-        <v>Irvine</v>
+        <v>Sacramento</v>
       </c>
       <c r="H108" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I108" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J108" t="str">
-        <v>Jackson Jackson, Isaiah Green</v>
+        <v>Thomas Nguyen, Henry Roberts</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
       </c>
       <c r="B109" t="str">
-        <v>Eleanor Hall</v>
+        <v>Ryan Lewis</v>
       </c>
       <c r="C109">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="D109" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E109" t="str">
-        <v>eleanor.hall7@yahoo.com</v>
+        <v>ryan.lewis85@yahoo.com</v>
       </c>
       <c r="F109" t="str">
-        <v>(627) 443-5972</v>
+        <v>0400 187 811</v>
       </c>
       <c r="G109" t="str">
-        <v>Stockton</v>
+        <v>Canberra</v>
       </c>
       <c r="H109" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I109" t="str">
         <v>available</v>
-      </c>
-      <c r="J109" t="str">
-        <v>Michael Campbell, Sadie Williams</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
+        <v>24928131-51b3-46f8-b43f-2cf989696f62</v>
       </c>
       <c r="B110" t="str">
-        <v>Ryan Lewis</v>
+        <v>Amelia Garcia</v>
       </c>
       <c r="C110">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D110" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E110" t="str">
-        <v>ryan.lewis85@yahoo.com</v>
+        <v>amelia.garcia16@gmail.com</v>
       </c>
       <c r="F110" t="str">
-        <v>0400 187 811</v>
+        <v>(331) 367-3904</v>
       </c>
       <c r="G110" t="str">
-        <v>Canberra</v>
+        <v>Anaheim</v>
       </c>
       <c r="H110" t="str">
         <v>B+</v>
@@ -4154,25 +4152,25 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>24928131-51b3-46f8-b43f-2cf989696f62</v>
+        <v>af09efbe-e83d-4046-8dc8-e6a06dfc0c40</v>
       </c>
       <c r="B111" t="str">
-        <v>Amelia Garcia</v>
+        <v>Paisley Evans</v>
       </c>
       <c r="C111">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D111" t="str">
         <v>Female</v>
       </c>
       <c r="E111" t="str">
-        <v>amelia.garcia16@gmail.com</v>
+        <v>paisley.evans52@yahoo.com</v>
       </c>
       <c r="F111" t="str">
-        <v>(331) 367-3904</v>
+        <v>(894) 250-9501</v>
       </c>
       <c r="G111" t="str">
-        <v>Anaheim</v>
+        <v>Torrance</v>
       </c>
       <c r="H111" t="str">
         <v>B+</v>
@@ -4183,95 +4181,98 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>af09efbe-e83d-4046-8dc8-e6a06dfc0c40</v>
+        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
       </c>
       <c r="B112" t="str">
-        <v>Paisley Evans</v>
+        <v>Penelope Williams</v>
       </c>
       <c r="C112">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D112" t="str">
         <v>Female</v>
       </c>
       <c r="E112" t="str">
-        <v>paisley.evans52@yahoo.com</v>
+        <v>penelope.williams29@hotmail.com</v>
       </c>
       <c r="F112" t="str">
-        <v>(894) 250-9501</v>
+        <v>(735) 691-4267</v>
       </c>
       <c r="G112" t="str">
-        <v>Torrance</v>
+        <v>Sacramento</v>
       </c>
       <c r="H112" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I112" t="str">
         <v>available</v>
+      </c>
+      <c r="J112" t="str">
+        <v>Savannah Rivera</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
+        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
       </c>
       <c r="B113" t="str">
-        <v>Penelope Williams</v>
+        <v>Avery Taylor</v>
       </c>
       <c r="C113">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D113" t="str">
         <v>Female</v>
       </c>
       <c r="E113" t="str">
-        <v>penelope.williams29@hotmail.com</v>
+        <v>avery.taylor87@outlook.com</v>
       </c>
       <c r="F113" t="str">
-        <v>(735) 691-4267</v>
+        <v>(299) 491-7680</v>
       </c>
       <c r="G113" t="str">
-        <v>Sacramento</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H113" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I113" t="str">
         <v>available</v>
       </c>
       <c r="J113" t="str">
-        <v>Savannah Rivera</v>
+        <v>Audrey Hill</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
+        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
       </c>
       <c r="B114" t="str">
-        <v>Avery Taylor</v>
+        <v>Layla Lopez</v>
       </c>
       <c r="C114">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D114" t="str">
         <v>Female</v>
       </c>
       <c r="E114" t="str">
-        <v>avery.taylor87@outlook.com</v>
+        <v>layla.lopez23@yahoo.com</v>
       </c>
       <c r="F114" t="str">
-        <v>(299) 491-7680</v>
+        <v>(607) 496-6102</v>
       </c>
       <c r="G114" t="str">
         <v>Los Angeles</v>
       </c>
       <c r="H114" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I114" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J114" t="str">
-        <v>Audrey Hill</v>
+        <v>Cora Lee</v>
       </c>
     </row>
     <row r="115">
@@ -5095,95 +5096,98 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="B142" t="str">
-        <v>Kathleen Reynolds</v>
+        <v>Cora Roberts</v>
       </c>
       <c r="C142">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D142" t="str">
-        <v>Not Specified</v>
+        <v>Female</v>
       </c>
       <c r="E142" t="str">
-        <v>kathleenmonicareynolds@gmail.com</v>
+        <v>cora.roberts57@hotmail.com</v>
       </c>
       <c r="F142" t="str">
-        <v>498086080</v>
+        <v>(141) 743-6838</v>
       </c>
       <c r="G142" t="str">
-        <v>Footscray</v>
+        <v>Bakersfield</v>
       </c>
       <c r="H142" t="str">
-        <v/>
+        <v>B</v>
       </c>
       <c r="I142" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J142" t="str">
-        <v>Peter Adamidis, Felicity Parker-Hill</v>
-      </c>
-      <c r="K142" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
-      </c>
-      <c r="L142" t="str">
-        <v>N</v>
-      </c>
-      <c r="M142" t="str">
-        <v>N/A</v>
+        <v>Isla Wright, Naomi Moore</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="B143" t="str">
-        <v>Abigail Williams</v>
+        <v>Kathleen Reynolds</v>
       </c>
       <c r="C143">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D143" t="str">
-        <v>Female</v>
+        <v>Not Specified</v>
       </c>
       <c r="E143" t="str">
-        <v>abigail.williams45@yahoo.com</v>
+        <v>kathleenmonicareynolds@gmail.com</v>
       </c>
       <c r="F143" t="str">
-        <v>0403 497 445</v>
+        <v>498086080</v>
       </c>
       <c r="G143" t="str">
-        <v>Toowoomba</v>
+        <v>Footscray</v>
       </c>
       <c r="H143" t="str">
-        <v>B</v>
+        <v/>
       </c>
       <c r="I143" t="str">
         <v>available</v>
+      </c>
+      <c r="J143" t="str">
+        <v>Peter Adamidis, Felicity Parker-Hill</v>
+      </c>
+      <c r="K143" t="str">
+        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+      </c>
+      <c r="L143" t="str">
+        <v>N</v>
+      </c>
+      <c r="M143" t="str">
+        <v>N/A</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
       </c>
       <c r="B144" t="str">
-        <v>Ethan Taylor</v>
+        <v>Abigail Williams</v>
       </c>
       <c r="C144">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="D144" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E144" t="str">
-        <v>ethan.taylor22@yahoo.com</v>
+        <v>abigail.williams45@yahoo.com</v>
       </c>
       <c r="F144" t="str">
-        <v>0410 363 173</v>
+        <v>0403 497 445</v>
       </c>
       <c r="G144" t="str">
-        <v>Adelaide</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H144" t="str">
         <v>B</v>
@@ -5194,34 +5198,31 @@
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
       </c>
       <c r="B145" t="str">
-        <v>Cora Roberts</v>
+        <v>Ethan Taylor</v>
       </c>
       <c r="C145">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D145" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E145" t="str">
-        <v>cora.roberts57@hotmail.com</v>
+        <v>ethan.taylor22@yahoo.com</v>
       </c>
       <c r="F145" t="str">
-        <v>(141) 743-6838</v>
+        <v>0410 363 173</v>
       </c>
       <c r="G145" t="str">
-        <v>Bakersfield</v>
+        <v>Adelaide</v>
       </c>
       <c r="H145" t="str">
         <v>B</v>
       </c>
       <c r="I145" t="str">
         <v>available</v>
-      </c>
-      <c r="J145" t="str">
-        <v>Isla Wright, Naomi Moore</v>
       </c>
     </row>
     <row r="146">
@@ -5522,57 +5523,57 @@
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="B156" t="str">
-        <v>Sadie Cook</v>
+        <v>Julian Nguyen</v>
       </c>
       <c r="C156">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D156" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E156" t="str">
-        <v>sadie.cook9@yahoo.com</v>
+        <v>julian.nguyen22@outlook.com</v>
       </c>
       <c r="F156" t="str">
-        <v>(382) 126-7672</v>
+        <v>(382) 722-8118</v>
       </c>
       <c r="G156" t="str">
-        <v>Santa Monica</v>
+        <v>Long Beach</v>
       </c>
       <c r="H156" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I156" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J156" t="str">
-        <v>William Allen, Alexa Hall</v>
+        <v>Leah Diaz, Lydia Allen</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>258eb0f3-5b73-4b6f-abb9-86c6ccb99d1f</v>
+        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
       </c>
       <c r="B157" t="str">
-        <v>Mateo Phillips</v>
+        <v>Sadie Cook</v>
       </c>
       <c r="C157">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D157" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E157" t="str">
-        <v>mateo.phillips59@outlook.com</v>
+        <v>sadie.cook9@yahoo.com</v>
       </c>
       <c r="F157" t="str">
-        <v>(155) 680-1162</v>
+        <v>(382) 126-7672</v>
       </c>
       <c r="G157" t="str">
-        <v>Sacramento</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H157" t="str">
         <v>B+</v>
@@ -5580,28 +5581,31 @@
       <c r="I157" t="str">
         <v>available</v>
       </c>
+      <c r="J157" t="str">
+        <v>William Allen, Alexa Hall</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>c2103c22-c825-4633-a461-495c55747ed3</v>
+        <v>258eb0f3-5b73-4b6f-abb9-86c6ccb99d1f</v>
       </c>
       <c r="B158" t="str">
-        <v>Alice Robinson</v>
+        <v>Mateo Phillips</v>
       </c>
       <c r="C158">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D158" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E158" t="str">
-        <v>alice.robinson56@hotmail.com</v>
+        <v>mateo.phillips59@outlook.com</v>
       </c>
       <c r="F158" t="str">
-        <v>(251) 325-5554</v>
+        <v>(155) 680-1162</v>
       </c>
       <c r="G158" t="str">
-        <v>Anaheim</v>
+        <v>Sacramento</v>
       </c>
       <c r="H158" t="str">
         <v>B+</v>
@@ -5612,25 +5616,25 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>c2103c22-c825-4633-a461-495c55747ed3</v>
       </c>
       <c r="B159" t="str">
-        <v>Grayson Morgan</v>
+        <v>Alice Robinson</v>
       </c>
       <c r="C159">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D159" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E159" t="str">
-        <v>grayson.morgan95@outlook.com</v>
+        <v>alice.robinson56@hotmail.com</v>
       </c>
       <c r="F159" t="str">
-        <v>(524) 127-2584</v>
+        <v>(251) 325-5554</v>
       </c>
       <c r="G159" t="str">
-        <v>Irvine</v>
+        <v>Anaheim</v>
       </c>
       <c r="H159" t="str">
         <v>B+</v>
@@ -5638,101 +5642,98 @@
       <c r="I159" t="str">
         <v>available</v>
       </c>
-      <c r="J159" t="str">
-        <v>Adam Hall, Valentina Morales</v>
-      </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="B160" t="str">
-        <v>Anthony Garcia</v>
+        <v>Grayson Morgan</v>
       </c>
       <c r="C160">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D160" t="str">
         <v>Male</v>
       </c>
       <c r="E160" t="str">
-        <v>anthony.garcia31@yahoo.com</v>
+        <v>grayson.morgan95@outlook.com</v>
       </c>
       <c r="F160" t="str">
-        <v>(249) 774-7265</v>
+        <v>(524) 127-2584</v>
       </c>
       <c r="G160" t="str">
-        <v>Santa Monica</v>
+        <v>Irvine</v>
       </c>
       <c r="H160" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I160" t="str">
         <v>available</v>
       </c>
       <c r="J160" t="str">
-        <v>Michael Johnson, Cameron Evans</v>
+        <v>Adam Hall, Valentina Morales</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>10ec31e6-c6da-4957-9768-c5fcefe79c6b</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="B161" t="str">
-        <v>Emma Turner</v>
+        <v>Anthony Garcia</v>
       </c>
       <c r="C161">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D161" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E161" t="str">
-        <v>emma.turner16@outlook.com</v>
+        <v>anthony.garcia31@yahoo.com</v>
       </c>
       <c r="F161" t="str">
-        <v>(656) 213-9003</v>
+        <v>(249) 774-7265</v>
       </c>
       <c r="G161" t="str">
-        <v>Pomona</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H161" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I161" t="str">
         <v>available</v>
+      </c>
+      <c r="J161" t="str">
+        <v>Michael Johnson, Cameron Evans</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>10ec31e6-c6da-4957-9768-c5fcefe79c6b</v>
       </c>
       <c r="B162" t="str">
-        <v>Julian Nguyen</v>
+        <v>Emma Turner</v>
       </c>
       <c r="C162">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D162" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E162" t="str">
-        <v>julian.nguyen22@outlook.com</v>
+        <v>emma.turner16@outlook.com</v>
       </c>
       <c r="F162" t="str">
-        <v>(382) 722-8118</v>
+        <v>(656) 213-9003</v>
       </c>
       <c r="G162" t="str">
-        <v>Long Beach</v>
+        <v>Pomona</v>
       </c>
       <c r="H162" t="str">
         <v>B</v>
       </c>
       <c r="I162" t="str">
         <v>available</v>
-      </c>
-      <c r="J162" t="str">
-        <v>Leah Diaz, Lydia Allen</v>
       </c>
     </row>
     <row r="163">
@@ -6391,185 +6392,182 @@
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="B184" t="str">
-        <v>Josiah Brown</v>
+        <v>Christian Rivera</v>
       </c>
       <c r="C184">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="D184" t="str">
         <v>Male</v>
       </c>
       <c r="E184" t="str">
-        <v>josiah.brown19@hotmail.com</v>
+        <v>christian.rivera21@outlook.com</v>
       </c>
       <c r="F184" t="str">
-        <v>(678) 449-3168</v>
+        <v>(913) 900-2520</v>
       </c>
       <c r="G184" t="str">
-        <v>Fresno</v>
+        <v>Burbank</v>
       </c>
       <c r="H184" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I184" t="str">
         <v>available</v>
       </c>
       <c r="J184" t="str">
-        <v>Piper Green</v>
+        <v>Allison Torres, Elena Green</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>d1a89d8f-bd2f-40db-a5d5-ef8dc3e3aa54</v>
       </c>
       <c r="B185" t="str">
-        <v>Christian Rivera</v>
+        <v>Mason Hernandez</v>
       </c>
       <c r="C185">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D185" t="str">
         <v>Male</v>
       </c>
       <c r="E185" t="str">
-        <v>christian.rivera21@outlook.com</v>
+        <v>mason.hernandez15@gmail.com</v>
       </c>
       <c r="F185" t="str">
-        <v>(913) 900-2520</v>
+        <v>(880) 425-4186</v>
       </c>
       <c r="G185" t="str">
-        <v>Burbank</v>
+        <v>San Jose</v>
       </c>
       <c r="H185" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I185" t="str">
         <v>available</v>
-      </c>
-      <c r="J185" t="str">
-        <v>Allison Torres, Elena Green</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>d1a89d8f-bd2f-40db-a5d5-ef8dc3e3aa54</v>
+        <v>e2c7fa0a-1d97-4430-b83c-5099c5831757</v>
       </c>
       <c r="B186" t="str">
-        <v>Mason Hernandez</v>
+        <v>John Carter</v>
       </c>
       <c r="C186">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D186" t="str">
         <v>Male</v>
       </c>
       <c r="E186" t="str">
-        <v>mason.hernandez15@gmail.com</v>
+        <v>john.carter42@outlook.com</v>
       </c>
       <c r="F186" t="str">
-        <v>(880) 425-4186</v>
+        <v>(160) 507-8767</v>
       </c>
       <c r="G186" t="str">
-        <v>San Jose</v>
+        <v>Pasadena</v>
       </c>
       <c r="H186" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I186" t="str">
         <v>available</v>
+      </c>
+      <c r="J186" t="str">
+        <v>Brooklyn Rivera</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>e2c7fa0a-1d97-4430-b83c-5099c5831757</v>
+        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
       </c>
       <c r="B187" t="str">
-        <v>John Carter</v>
+        <v>Elijah Miller</v>
       </c>
       <c r="C187">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="D187" t="str">
         <v>Male</v>
       </c>
       <c r="E187" t="str">
-        <v>john.carter42@outlook.com</v>
+        <v>elijah.miller73@outlook.com</v>
       </c>
       <c r="F187" t="str">
-        <v>(160) 507-8767</v>
+        <v>(967) 645-5202</v>
       </c>
       <c r="G187" t="str">
         <v>Pasadena</v>
       </c>
       <c r="H187" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I187" t="str">
         <v>available</v>
       </c>
       <c r="J187" t="str">
-        <v>Brooklyn Rivera</v>
+        <v>Sophia Flores</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
       </c>
       <c r="B188" t="str">
-        <v>Elijah Miller</v>
+        <v>Carter Harris</v>
       </c>
       <c r="C188">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D188" t="str">
         <v>Male</v>
       </c>
       <c r="E188" t="str">
-        <v>elijah.miller73@outlook.com</v>
+        <v>carter.harris82@yahoo.com</v>
       </c>
       <c r="F188" t="str">
-        <v>(967) 645-5202</v>
+        <v>0412 175 744</v>
       </c>
       <c r="G188" t="str">
-        <v>Pasadena</v>
+        <v>Geelong</v>
       </c>
       <c r="H188" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I188" t="str">
         <v>available</v>
-      </c>
-      <c r="J188" t="str">
-        <v>Sophia Flores</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+        <v>340ad2e5-95a9-4eb5-a113-e7f9f0e5d704</v>
       </c>
       <c r="B189" t="str">
-        <v>Carter Harris</v>
+        <v>Jaxon Cook</v>
       </c>
       <c r="C189">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D189" t="str">
         <v>Male</v>
       </c>
       <c r="E189" t="str">
-        <v>carter.harris82@yahoo.com</v>
+        <v>jaxon.cook73@yahoo.com</v>
       </c>
       <c r="F189" t="str">
-        <v>0412 175 744</v>
+        <v>(190) 120-3429</v>
       </c>
       <c r="G189" t="str">
-        <v>Geelong</v>
+        <v>Fresno</v>
       </c>
       <c r="H189" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I189" t="str">
         <v>available</v>
@@ -6577,89 +6575,89 @@
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>340ad2e5-95a9-4eb5-a113-e7f9f0e5d704</v>
+        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
       </c>
       <c r="B190" t="str">
-        <v>Jaxon Cook</v>
+        <v>Thomas Rivera</v>
       </c>
       <c r="C190">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D190" t="str">
         <v>Male</v>
       </c>
       <c r="E190" t="str">
-        <v>jaxon.cook73@yahoo.com</v>
+        <v>thomas.rivera13@yahoo.com</v>
       </c>
       <c r="F190" t="str">
-        <v>(190) 120-3429</v>
+        <v>(539) 243-6118</v>
       </c>
       <c r="G190" t="str">
-        <v>Fresno</v>
+        <v>Long Beach</v>
       </c>
       <c r="H190" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I190" t="str">
         <v>available</v>
+      </c>
+      <c r="J190" t="str">
+        <v>Hannah Murphy</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
+        <v>e8c7986a-699a-4e43-9b2d-52ca42510a36</v>
       </c>
       <c r="B191" t="str">
-        <v>Thomas Rivera</v>
+        <v>Matthew Torres</v>
       </c>
       <c r="C191">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D191" t="str">
         <v>Male</v>
       </c>
       <c r="E191" t="str">
-        <v>thomas.rivera13@yahoo.com</v>
+        <v>matthew.torres76@yahoo.com</v>
       </c>
       <c r="F191" t="str">
-        <v>(539) 243-6118</v>
+        <v>(432) 516-9920</v>
       </c>
       <c r="G191" t="str">
-        <v>Long Beach</v>
+        <v>Sacramento</v>
       </c>
       <c r="H191" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I191" t="str">
         <v>available</v>
-      </c>
-      <c r="J191" t="str">
-        <v>Hannah Murphy</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>e8c7986a-699a-4e43-9b2d-52ca42510a36</v>
+        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
       </c>
       <c r="B192" t="str">
-        <v>Matthew Torres</v>
+        <v>Noah Hernandez</v>
       </c>
       <c r="C192">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D192" t="str">
         <v>Male</v>
       </c>
       <c r="E192" t="str">
-        <v>matthew.torres76@yahoo.com</v>
+        <v>noah.hernandez9@hotmail.com</v>
       </c>
       <c r="F192" t="str">
-        <v>(432) 516-9920</v>
+        <v>0404 855 230</v>
       </c>
       <c r="G192" t="str">
-        <v>Sacramento</v>
+        <v>Cairns</v>
       </c>
       <c r="H192" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I192" t="str">
         <v>available</v>
@@ -6667,54 +6665,57 @@
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
+        <v>35c73937-3dd5-4fb3-a5df-d900cabdacba</v>
       </c>
       <c r="B193" t="str">
-        <v>Noah Hernandez</v>
+        <v>Jackson Murphy</v>
       </c>
       <c r="C193">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D193" t="str">
         <v>Male</v>
       </c>
       <c r="E193" t="str">
-        <v>noah.hernandez9@hotmail.com</v>
+        <v>jackson.murphy91@yahoo.com</v>
       </c>
       <c r="F193" t="str">
-        <v>0404 855 230</v>
+        <v>(572) 305-7237</v>
       </c>
       <c r="G193" t="str">
-        <v>Cairns</v>
+        <v>Riverside</v>
       </c>
       <c r="H193" t="str">
         <v>B</v>
       </c>
       <c r="I193" t="str">
         <v>available</v>
+      </c>
+      <c r="J193" t="str">
+        <v>Caleb Brown</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>35c73937-3dd5-4fb3-a5df-d900cabdacba</v>
+        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
       </c>
       <c r="B194" t="str">
-        <v>Jackson Murphy</v>
+        <v>William Taylor</v>
       </c>
       <c r="C194">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D194" t="str">
         <v>Male</v>
       </c>
       <c r="E194" t="str">
-        <v>jackson.murphy91@yahoo.com</v>
+        <v>william.taylor84@hotmail.com</v>
       </c>
       <c r="F194" t="str">
-        <v>(572) 305-7237</v>
+        <v>(276) 538-1731</v>
       </c>
       <c r="G194" t="str">
-        <v>Riverside</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H194" t="str">
         <v>B</v>
@@ -6723,27 +6724,27 @@
         <v>available</v>
       </c>
       <c r="J194" t="str">
-        <v>Caleb Brown</v>
+        <v>Victoria Scott</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="B195" t="str">
-        <v>William Taylor</v>
+        <v>Colton Harris</v>
       </c>
       <c r="C195">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D195" t="str">
         <v>Male</v>
       </c>
       <c r="E195" t="str">
-        <v>william.taylor84@hotmail.com</v>
+        <v>colton.harris98@icloud.com</v>
       </c>
       <c r="F195" t="str">
-        <v>(276) 538-1731</v>
+        <v>(583) 900-3294</v>
       </c>
       <c r="G195" t="str">
         <v>Newport Beach</v>
@@ -6752,39 +6753,42 @@
         <v>B</v>
       </c>
       <c r="I195" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J195" t="str">
-        <v>Victoria Scott</v>
+        <v>Sebastian Edwards, Sofia Williams</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>befe2d5d-0583-45ac-939e-ab57370e2d4f</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="B196" t="str">
-        <v>Daniel Taylor</v>
+        <v>Sebastian Edwards</v>
       </c>
       <c r="C196">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D196" t="str">
         <v>Male</v>
       </c>
       <c r="E196" t="str">
-        <v>daniel.taylor53@gmail.com</v>
+        <v>sebastian.edwards97@icloud.com</v>
       </c>
       <c r="F196" t="str">
-        <v>(543) 329-4768</v>
+        <v>(348) 408-1134</v>
       </c>
       <c r="G196" t="str">
-        <v>Pomona</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H196" t="str">
         <v>B</v>
       </c>
       <c r="I196" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J196" t="str">
+        <v>Colton Harris, Sofia Williams</v>
       </c>
     </row>
     <row r="197">
@@ -6813,7 +6817,7 @@
         <v>B</v>
       </c>
       <c r="I197" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J197" t="str">
         <v>Henry Roberts, Hannah Jones</v>
@@ -6821,153 +6825,150 @@
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
+        <v>befe2d5d-0583-45ac-939e-ab57370e2d4f</v>
       </c>
       <c r="B198" t="str">
-        <v>Logan Nguyen</v>
+        <v>Daniel Taylor</v>
       </c>
       <c r="C198">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D198" t="str">
         <v>Male</v>
       </c>
       <c r="E198" t="str">
-        <v>logan.nguyen23@hotmail.com</v>
+        <v>daniel.taylor53@gmail.com</v>
       </c>
       <c r="F198" t="str">
-        <v>(278) 620-7089</v>
+        <v>(543) 329-4768</v>
       </c>
       <c r="G198" t="str">
-        <v>Torrance</v>
+        <v>Pomona</v>
       </c>
       <c r="H198" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I198" t="str">
         <v>available</v>
-      </c>
-      <c r="J198" t="str">
-        <v>Alexander Campbell, Hannah Moore</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>f26a0638-511f-4440-ae1a-2ae052df470f</v>
+        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
       </c>
       <c r="B199" t="str">
-        <v>Caleb Brown</v>
+        <v>Josiah Brown</v>
       </c>
       <c r="C199">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D199" t="str">
         <v>Male</v>
       </c>
       <c r="E199" t="str">
-        <v>caleb.brown13@yahoo.com</v>
+        <v>josiah.brown19@hotmail.com</v>
       </c>
       <c r="F199" t="str">
-        <v>(130) 920-6765</v>
+        <v>(678) 449-3168</v>
       </c>
       <c r="G199" t="str">
-        <v>Irvine</v>
+        <v>Fresno</v>
       </c>
       <c r="H199" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I199" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J199" t="str">
-        <v>Jackson Murphy</v>
+        <v>Piper Green</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
       </c>
       <c r="B200" t="str">
-        <v>Grace King</v>
+        <v>Logan Nguyen</v>
       </c>
       <c r="C200">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D200" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E200" t="str">
-        <v>grace.king1@yahoo.com</v>
+        <v>logan.nguyen23@hotmail.com</v>
       </c>
       <c r="F200" t="str">
-        <v>(217) 721-5651</v>
+        <v>(278) 620-7089</v>
       </c>
       <c r="G200" t="str">
-        <v>Oakland</v>
+        <v>Torrance</v>
       </c>
       <c r="H200" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I200" t="str">
         <v>available</v>
       </c>
       <c r="J200" t="str">
-        <v>Gianna Hill</v>
+        <v>Alexander Campbell, Hannah Moore</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
+        <v>f26a0638-511f-4440-ae1a-2ae052df470f</v>
       </c>
       <c r="B201" t="str">
-        <v>Alexander Campbell</v>
+        <v>Caleb Brown</v>
       </c>
       <c r="C201">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D201" t="str">
         <v>Male</v>
       </c>
       <c r="E201" t="str">
-        <v>alexander.campbell71@gmail.com</v>
+        <v>caleb.brown13@yahoo.com</v>
       </c>
       <c r="F201" t="str">
-        <v>(131) 840-1169</v>
+        <v>(130) 920-6765</v>
       </c>
       <c r="G201" t="str">
-        <v>Fresno</v>
+        <v>Irvine</v>
       </c>
       <c r="H201" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I201" t="str">
         <v>available</v>
       </c>
       <c r="J201" t="str">
-        <v>Logan Nguyen, Hannah Moore</v>
+        <v>Jackson Murphy</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
       </c>
       <c r="B202" t="str">
-        <v>Colton Harris</v>
+        <v>Grace King</v>
       </c>
       <c r="C202">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D202" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E202" t="str">
-        <v>colton.harris98@icloud.com</v>
+        <v>grace.king1@yahoo.com</v>
       </c>
       <c r="F202" t="str">
-        <v>(583) 900-3294</v>
+        <v>(217) 721-5651</v>
       </c>
       <c r="G202" t="str">
-        <v>Newport Beach</v>
+        <v>Oakland</v>
       </c>
       <c r="H202" t="str">
         <v>B</v>
@@ -6976,39 +6977,39 @@
         <v>available</v>
       </c>
       <c r="J202" t="str">
-        <v>Sebastian Edwards, Sofia Williams</v>
+        <v>Gianna Hill</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
       </c>
       <c r="B203" t="str">
-        <v>Sebastian Edwards</v>
+        <v>Alexander Campbell</v>
       </c>
       <c r="C203">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D203" t="str">
         <v>Male</v>
       </c>
       <c r="E203" t="str">
-        <v>sebastian.edwards97@icloud.com</v>
+        <v>alexander.campbell71@gmail.com</v>
       </c>
       <c r="F203" t="str">
-        <v>(348) 408-1134</v>
+        <v>(131) 840-1169</v>
       </c>
       <c r="G203" t="str">
-        <v>Los Angeles</v>
+        <v>Fresno</v>
       </c>
       <c r="H203" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I203" t="str">
         <v>available</v>
       </c>
       <c r="J203" t="str">
-        <v>Colton Harris, Sofia Williams</v>
+        <v>Logan Nguyen, Hannah Moore</v>
       </c>
     </row>
     <row r="204">
@@ -7537,25 +7538,25 @@
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
+        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
       </c>
       <c r="B220" t="str">
-        <v>Cora Lee</v>
+        <v>Chloe Jones</v>
       </c>
       <c r="C220">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D220" t="str">
         <v>Female</v>
       </c>
       <c r="E220" t="str">
-        <v>cora.lee40@hotmail.com</v>
+        <v>chloe.jones20@outlook.com</v>
       </c>
       <c r="F220" t="str">
-        <v>(406) 886-5180</v>
+        <v>0411 294 635</v>
       </c>
       <c r="G220" t="str">
-        <v>Fresno</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H220" t="str">
         <v>B</v>
@@ -7564,30 +7565,30 @@
         <v>available</v>
       </c>
       <c r="J220" t="str">
-        <v>Layla Lopez</v>
+        <v>Zoe Brown</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>dd2de8e6-e7c9-40e4-8308-27a14e5f00da</v>
+        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
       </c>
       <c r="B221" t="str">
-        <v>Chloe Jones</v>
+        <v>Emily Thomas</v>
       </c>
       <c r="C221">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D221" t="str">
         <v>Female</v>
       </c>
       <c r="E221" t="str">
-        <v>chloe.jones20@outlook.com</v>
+        <v>emily.thomas25@outlook.com</v>
       </c>
       <c r="F221" t="str">
-        <v>0411 294 635</v>
+        <v>0402 648 577</v>
       </c>
       <c r="G221" t="str">
-        <v>Toowoomba</v>
+        <v>Geelong</v>
       </c>
       <c r="H221" t="str">
         <v>B</v>
@@ -7596,42 +7597,42 @@
         <v>available</v>
       </c>
       <c r="J221" t="str">
-        <v>Zoe Brown</v>
+        <v>Stella Garcia</v>
+      </c>
+      <c r="M221" t="str">
+        <v>Knee replacement - cannot climb stairs</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>b09d810a-6eb0-4ea8-ac8b-df27315049f1</v>
+        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
       </c>
       <c r="B222" t="str">
-        <v>Emily Thomas</v>
+        <v>Cora Lee</v>
       </c>
       <c r="C222">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D222" t="str">
         <v>Female</v>
       </c>
       <c r="E222" t="str">
-        <v>emily.thomas25@outlook.com</v>
+        <v>cora.lee40@hotmail.com</v>
       </c>
       <c r="F222" t="str">
-        <v>0402 648 577</v>
+        <v>(406) 886-5180</v>
       </c>
       <c r="G222" t="str">
-        <v>Geelong</v>
+        <v>Fresno</v>
       </c>
       <c r="H222" t="str">
         <v>B</v>
       </c>
       <c r="I222" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J222" t="str">
-        <v>Stella Garcia</v>
-      </c>
-      <c r="M222" t="str">
-        <v>Knee replacement - cannot climb stairs</v>
+        <v>Layla Lopez</v>
       </c>
     </row>
     <row r="223">
@@ -12371,6 +12372,301 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Block</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="F1" t="str">
+        <v>BookingEmailSent</v>
+      </c>
+      <c r="G1" t="str">
+        <v>ConfirmedRSVP</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>6d4b9121-e2b5-4974-8e85-1834a8c84ee5</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>A1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>a3523548-7ed4-4a88-9916-8f3919e47ca8</v>
+      </c>
+      <c r="B3" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C3" t="str">
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>A2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>7004601b-f38b-47f6-9c6f-7a8387efddd2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C4" t="str">
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
+        <v>A3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>455ab020-7fcc-4e25-8b05-9bc9ef954631</v>
+      </c>
+      <c r="B5" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C5" t="str">
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="str">
+        <v>B1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>1cb60061-9319-4b40-96a4-3c1f83ac9bba</v>
+      </c>
+      <c r="B6" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C6" t="str">
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <v>B2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>d3f3ab45-af63-49d7-9ad5-99314ae6123b</v>
+      </c>
+      <c r="B7" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C7" t="str">
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="str">
+        <v>B3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>9d10a085-11bd-4012-a3b3-4c60ac5c7553</v>
+      </c>
+      <c r="B8" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C8" t="str">
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="str">
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>e0a5a271-2412-4113-8e30-50b8d9d3dc64</v>
+      </c>
+      <c r="B9" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C9" t="str">
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="str">
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>8063d451-75a6-4a31-9f70-e46edff46949</v>
+      </c>
+      <c r="B10" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C10" t="str">
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="str">
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>0b034f2f-91e5-4a26-9e8a-d84ed98cc844</v>
+      </c>
+      <c r="B11" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C11" t="str">
+        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="str">
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>1c7e5f34-2112-4ab1-8314-549d6c26ecab</v>
+      </c>
+      <c r="B12" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C12" t="str">
+        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="str">
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>4c676a14-cab5-41a7-8b29-5e1f1d347663</v>
+      </c>
+      <c r="B13" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C13" t="str">
+        <v>5addacf0-a31c-4412-982a-3f0d8f1c6d07</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="str">
+        <v>D3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>0ce09a58-3d17-4791-856a-d556e2b5f996</v>
+      </c>
+      <c r="B14" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C14" t="str">
+        <v>b28a73f8-5094-4b00-be67-223342b0e1d5</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="str">
+        <v>D4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>17cc7ee9-e31a-4fe7-8445-dd2015eb0c08</v>
+      </c>
+      <c r="B15" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C15" t="str">
+        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="str">
+        <v>E1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>4e8dba21-e04b-4bc5-a401-355f8fd27706</v>
+      </c>
+      <c r="B16" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C16" t="str">
+        <v>e4b4c1c5-d581-43e6-89d9-d3cee5153165</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="str">
+        <v>E2</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H16"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12428,7 +12724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -12490,7 +12786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -12882,7 +13178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add missing winning money details to seating assignment data
Fix an issue where the `rxEpNumber` was not included in the seat assignments endpoint response, preventing it from being displayed and saved correctly.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 01cd5e0a-0d4a-4019-8b1b-6638a78c6e37
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/LAohLrb
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -13170,240 +13170,240 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>cb62b970-7194-4872-9fc3-92a543d01f39</v>
+        <v>26b4f1ab-ed56-48cd-9fd3-c457cd9d3c40</v>
       </c>
       <c r="B47" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C47" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" t="str">
-        <v>A1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>26945441-ea86-4493-a389-00ade06c7d37</v>
+        <v>cb62b970-7194-4872-9fc3-92a543d01f39</v>
       </c>
       <c r="B48" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C48" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="str">
-        <v>A2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>5297fdf0-8524-4546-a9e5-75c4b7595db7</v>
+        <v>26945441-ea86-4493-a389-00ade06c7d37</v>
       </c>
       <c r="B49" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C49" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="str">
-        <v>A3</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>1eb3e2c4-236f-4b99-a085-f991d9c2106b</v>
+        <v>5297fdf0-8524-4546-a9e5-75c4b7595db7</v>
       </c>
       <c r="B50" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C50" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50" t="str">
-        <v>B1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>32e4e84d-d241-4470-9b3b-210beb9afe12</v>
+        <v>1eb3e2c4-236f-4b99-a085-f991d9c2106b</v>
       </c>
       <c r="B51" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C51" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51" t="str">
-        <v>B2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>bfd354a2-712a-4be3-a1bb-3f13e4f52550</v>
+        <v>32e4e84d-d241-4470-9b3b-210beb9afe12</v>
       </c>
       <c r="B52" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C52" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52" t="str">
-        <v>B3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>eaa76e1c-43f0-4ecb-94bb-b16bb9beffae</v>
+        <v>bfd354a2-712a-4be3-a1bb-3f13e4f52550</v>
       </c>
       <c r="B53" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C53" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="str">
-        <v>C1</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>c2b4d4be-64b7-41c5-a958-e3d8c99fc790</v>
+        <v>eaa76e1c-43f0-4ecb-94bb-b16bb9beffae</v>
       </c>
       <c r="B54" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C54" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="str">
-        <v>C2</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>96ecc4ef-fd63-4393-b7df-9423b5df0868</v>
+        <v>c2b4d4be-64b7-41c5-a958-e3d8c99fc790</v>
       </c>
       <c r="B55" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C55" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="str">
-        <v>C3</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>cb41808d-c7e0-4faf-8129-a2e53357c14a</v>
+        <v>96ecc4ef-fd63-4393-b7df-9423b5df0868</v>
       </c>
       <c r="B56" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C56" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56" t="str">
-        <v>D1</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>46b7e745-083b-41b0-b8fa-a0391457260b</v>
+        <v>cb41808d-c7e0-4faf-8129-a2e53357c14a</v>
       </c>
       <c r="B57" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C57" t="str">
-        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="str">
-        <v>D2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>bc7f838a-b8a5-4f40-9451-6e5b608931ed</v>
+        <v>46b7e745-083b-41b0-b8fa-a0391457260b</v>
       </c>
       <c r="B58" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C58" t="str">
-        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
+        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="str">
-        <v>D3</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>bc22ad22-1b7c-446d-8cd9-8d1a90cafebd</v>
+        <v>bc7f838a-b8a5-4f40-9451-6e5b608931ed</v>
       </c>
       <c r="B59" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C59" t="str">
-        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
+        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="str">
-        <v>D4</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>26b4f1ab-ed56-48cd-9fd3-c457cd9d3c40</v>
+        <v>bc22ad22-1b7c-446d-8cd9-8d1a90cafebd</v>
       </c>
       <c r="B60" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C60" t="str">
-        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
+        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60" t="str">
-        <v>E1</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="61">

</xml_diff>

<commit_message>
Add editable TX information to the winners display and management section
Adds new fields for TX Number, TX Date, Notified of TX, and Photos Sent to the seatAssignments schema and updates the winners page to display and allow inline editing of this information with a toggleable section.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 60fc2edc-5523-475e-8d62-87778b36d1b2
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/8huVKa0
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -13187,189 +13187,189 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>cb62b970-7194-4872-9fc3-92a543d01f39</v>
+        <v>46b7e745-083b-41b0-b8fa-a0391457260b</v>
       </c>
       <c r="B48" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C48" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="str">
-        <v>A1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>26945441-ea86-4493-a389-00ade06c7d37</v>
+        <v>cb62b970-7194-4872-9fc3-92a543d01f39</v>
       </c>
       <c r="B49" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C49" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="str">
-        <v>A2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>5297fdf0-8524-4546-a9e5-75c4b7595db7</v>
+        <v>26945441-ea86-4493-a389-00ade06c7d37</v>
       </c>
       <c r="B50" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C50" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50" t="str">
-        <v>A3</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>1eb3e2c4-236f-4b99-a085-f991d9c2106b</v>
+        <v>5297fdf0-8524-4546-a9e5-75c4b7595db7</v>
       </c>
       <c r="B51" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C51" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51" t="str">
-        <v>B1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>32e4e84d-d241-4470-9b3b-210beb9afe12</v>
+        <v>1eb3e2c4-236f-4b99-a085-f991d9c2106b</v>
       </c>
       <c r="B52" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C52" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52" t="str">
-        <v>B2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>bfd354a2-712a-4be3-a1bb-3f13e4f52550</v>
+        <v>32e4e84d-d241-4470-9b3b-210beb9afe12</v>
       </c>
       <c r="B53" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C53" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="str">
-        <v>B3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>eaa76e1c-43f0-4ecb-94bb-b16bb9beffae</v>
+        <v>bfd354a2-712a-4be3-a1bb-3f13e4f52550</v>
       </c>
       <c r="B54" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C54" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="str">
-        <v>C1</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>c2b4d4be-64b7-41c5-a958-e3d8c99fc790</v>
+        <v>eaa76e1c-43f0-4ecb-94bb-b16bb9beffae</v>
       </c>
       <c r="B55" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C55" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="str">
-        <v>C2</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>96ecc4ef-fd63-4393-b7df-9423b5df0868</v>
+        <v>c2b4d4be-64b7-41c5-a958-e3d8c99fc790</v>
       </c>
       <c r="B56" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C56" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56" t="str">
-        <v>C3</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>cb41808d-c7e0-4faf-8129-a2e53357c14a</v>
+        <v>96ecc4ef-fd63-4393-b7df-9423b5df0868</v>
       </c>
       <c r="B57" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C57" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="str">
-        <v>D1</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>46b7e745-083b-41b0-b8fa-a0391457260b</v>
+        <v>cb41808d-c7e0-4faf-8129-a2e53357c14a</v>
       </c>
       <c r="B58" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C58" t="str">
-        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="str">
-        <v>D2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="59">

</xml_diff>

<commit_message>
Reduce font size in winners table to fit content on one line
Update `winners.tsx` to change font sizes from `text-sm` to `text-xs` and adjust `font-medium` on contestant names.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 2abd7263-320b-447a-87c3-ad013ab63281
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/ax8ARrG
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -2170,25 +2170,25 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
+        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
       </c>
       <c r="B47" t="str">
-        <v>Nathan Allen</v>
+        <v>Abigail Jackson</v>
       </c>
       <c r="C47">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D47" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E47" t="str">
-        <v>nathan.allen87@outlook.com</v>
+        <v>abigail.jackson65@outlook.com</v>
       </c>
       <c r="F47" t="str">
-        <v>0403 587 263</v>
+        <v>0411 824 257</v>
       </c>
       <c r="G47" t="str">
-        <v>Adelaide</v>
+        <v>Newcastle</v>
       </c>
       <c r="H47" t="str">
         <v>B+</v>
@@ -2199,89 +2199,89 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
       </c>
       <c r="B48" t="str">
-        <v>Aria Lopez</v>
+        <v>Nathan Allen</v>
       </c>
       <c r="C48">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D48" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E48" t="str">
-        <v>aria.lopez55@hotmail.com</v>
+        <v>nathan.allen87@outlook.com</v>
       </c>
       <c r="F48" t="str">
-        <v>0404 812 491</v>
+        <v>0403 587 263</v>
       </c>
       <c r="G48" t="str">
-        <v>Sydney</v>
+        <v>Adelaide</v>
       </c>
       <c r="H48" t="str">
         <v>B+</v>
       </c>
       <c r="I48" t="str">
-        <v>available</v>
-      </c>
-      <c r="J48" t="str">
-        <v>Paisley Lee</v>
+        <v>assigned</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="B49" t="str">
-        <v>Mason Hill</v>
+        <v>Aria Lopez</v>
       </c>
       <c r="C49">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D49" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E49" t="str">
-        <v>mason.hill27@outlook.com</v>
+        <v>aria.lopez55@hotmail.com</v>
       </c>
       <c r="F49" t="str">
-        <v>0410 682 884</v>
+        <v>0404 812 491</v>
       </c>
       <c r="G49" t="str">
-        <v>Canberra</v>
+        <v>Sydney</v>
       </c>
       <c r="H49" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I49" t="str">
         <v>available</v>
       </c>
+      <c r="J49" t="str">
+        <v>Paisley Lee</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
+        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
       </c>
       <c r="B50" t="str">
-        <v>Ryan Williams</v>
+        <v>Mason Hill</v>
       </c>
       <c r="C50">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D50" t="str">
         <v>Male</v>
       </c>
       <c r="E50" t="str">
-        <v>ryan.williams82@hotmail.com</v>
+        <v>mason.hill27@outlook.com</v>
       </c>
       <c r="F50" t="str">
-        <v>0401 450 673</v>
+        <v>0410 682 884</v>
       </c>
       <c r="G50" t="str">
-        <v>Perth</v>
+        <v>Canberra</v>
       </c>
       <c r="H50" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I50" t="str">
         <v>available</v>
@@ -2289,28 +2289,28 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>0a153155-dcf5-4d56-9ed1-8960501157f8</v>
+        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
       </c>
       <c r="B51" t="str">
-        <v>Aurora Gonzalez</v>
+        <v>Ryan Williams</v>
       </c>
       <c r="C51">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D51" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E51" t="str">
-        <v>aurora.gonzalez29@outlook.com</v>
+        <v>ryan.williams82@hotmail.com</v>
       </c>
       <c r="F51" t="str">
-        <v>0404 610 172</v>
+        <v>0401 450 673</v>
       </c>
       <c r="G51" t="str">
-        <v>Toowoomba</v>
+        <v>Perth</v>
       </c>
       <c r="H51" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I51" t="str">
         <v>available</v>
@@ -2318,28 +2318,28 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
+        <v>0a153155-dcf5-4d56-9ed1-8960501157f8</v>
       </c>
       <c r="B52" t="str">
-        <v>Abigail Jackson</v>
+        <v>Aurora Gonzalez</v>
       </c>
       <c r="C52">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D52" t="str">
         <v>Female</v>
       </c>
       <c r="E52" t="str">
-        <v>abigail.jackson65@outlook.com</v>
+        <v>aurora.gonzalez29@outlook.com</v>
       </c>
       <c r="F52" t="str">
-        <v>0411 824 257</v>
+        <v>0404 610 172</v>
       </c>
       <c r="G52" t="str">
-        <v>Newcastle</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H52" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I52" t="str">
         <v>available</v>
@@ -5837,95 +5837,95 @@
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
+        <v>f85f167d-7dd5-420d-86b5-ec8861b2bc1a</v>
       </c>
       <c r="B166" t="str">
-        <v>Sadie Cook</v>
+        <v>Michael Carter</v>
       </c>
       <c r="C166">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D166" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E166" t="str">
-        <v>sadie.cook9@yahoo.com</v>
+        <v>michael.carter90@outlook.com</v>
       </c>
       <c r="F166" t="str">
-        <v>(382) 126-7672</v>
+        <v>(377) 714-4320</v>
       </c>
       <c r="G166" t="str">
-        <v>Santa Monica</v>
+        <v>Burbank</v>
       </c>
       <c r="H166" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I166" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J166" t="str">
-        <v>William Allen, Alexa Hall</v>
+        <v>available</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>f85f167d-7dd5-420d-86b5-ec8861b2bc1a</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="B167" t="str">
-        <v>Michael Carter</v>
+        <v>Anthony Garcia</v>
       </c>
       <c r="C167">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D167" t="str">
         <v>Male</v>
       </c>
       <c r="E167" t="str">
-        <v>michael.carter90@outlook.com</v>
+        <v>anthony.garcia31@yahoo.com</v>
       </c>
       <c r="F167" t="str">
-        <v>(377) 714-4320</v>
+        <v>(249) 774-7265</v>
       </c>
       <c r="G167" t="str">
-        <v>Burbank</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H167" t="str">
         <v>A</v>
       </c>
       <c r="I167" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J167" t="str">
+        <v>Michael Johnson, Cameron Evans</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
       </c>
       <c r="B168" t="str">
-        <v>Anthony Garcia</v>
+        <v>Sadie Cook</v>
       </c>
       <c r="C168">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D168" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E168" t="str">
-        <v>anthony.garcia31@yahoo.com</v>
+        <v>sadie.cook9@yahoo.com</v>
       </c>
       <c r="F168" t="str">
-        <v>(249) 774-7265</v>
+        <v>(382) 126-7672</v>
       </c>
       <c r="G168" t="str">
         <v>Santa Monica</v>
       </c>
       <c r="H168" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I168" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J168" t="str">
-        <v>Michael Johnson, Cameron Evans</v>
+        <v>William Allen, Alexa Hall</v>
       </c>
     </row>
     <row r="169">
@@ -7206,57 +7206,60 @@
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
+        <v>f878ab7f-ae59-4af0-b19a-e9bf4573c116</v>
       </c>
       <c r="B210" t="str">
-        <v>Joshua Walker</v>
+        <v>William Allen</v>
       </c>
       <c r="C210">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D210" t="str">
         <v>Male</v>
       </c>
       <c r="E210" t="str">
-        <v>joshua.walker97@gmail.com</v>
+        <v>william.allen62@hotmail.com</v>
       </c>
       <c r="F210" t="str">
-        <v>0402 640 379</v>
+        <v>(267) 463-7481</v>
       </c>
       <c r="G210" t="str">
-        <v>Darwin</v>
+        <v>San Jose</v>
       </c>
       <c r="H210" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I210" t="str">
         <v>available</v>
       </c>
+      <c r="J210" t="str">
+        <v>Sadie Cook, Alexa Hall</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
+        <v>7bfb9432-4b59-4ceb-895d-e03ae4837f91</v>
       </c>
       <c r="B211" t="str">
-        <v>Cameron Lee</v>
+        <v>Joshua Walker</v>
       </c>
       <c r="C211">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D211" t="str">
         <v>Male</v>
       </c>
       <c r="E211" t="str">
-        <v>cameron.lee78@yahoo.com</v>
+        <v>joshua.walker97@gmail.com</v>
       </c>
       <c r="F211" t="str">
-        <v>0404 821 708</v>
+        <v>0402 640 379</v>
       </c>
       <c r="G211" t="str">
-        <v>Cairns</v>
+        <v>Darwin</v>
       </c>
       <c r="H211" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I211" t="str">
         <v>available</v>
@@ -7264,34 +7267,31 @@
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>f878ab7f-ae59-4af0-b19a-e9bf4573c116</v>
+        <v>efe20d3d-2162-4ff8-a8ff-4102e5d3f3ab</v>
       </c>
       <c r="B212" t="str">
-        <v>William Allen</v>
+        <v>Cameron Lee</v>
       </c>
       <c r="C212">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D212" t="str">
         <v>Male</v>
       </c>
       <c r="E212" t="str">
-        <v>william.allen62@hotmail.com</v>
+        <v>cameron.lee78@yahoo.com</v>
       </c>
       <c r="F212" t="str">
-        <v>(267) 463-7481</v>
+        <v>0404 821 708</v>
       </c>
       <c r="G212" t="str">
-        <v>San Jose</v>
+        <v>Cairns</v>
       </c>
       <c r="H212" t="str">
         <v>B+</v>
       </c>
       <c r="I212" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J212" t="str">
-        <v>Sadie Cook, Alexa Hall</v>
+        <v>available</v>
       </c>
     </row>
     <row r="213">
@@ -12372,7 +12372,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H126"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -13170,13 +13170,13 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>26b4f1ab-ed56-48cd-9fd3-c457cd9d3c40</v>
+        <v>a973a84d-478a-485f-94de-6087fbbcf4db</v>
       </c>
       <c r="B47" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C47" t="str">
-        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
+        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -13408,1146 +13408,1129 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>45c4c12e-6b34-47df-95f5-c0b7cd51be62</v>
+        <v>f065c3ae-b3d0-41b7-9d86-a8d5c479a109</v>
       </c>
       <c r="B61" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C61" t="str">
-        <v>f878ab7f-ae59-4af0-b19a-e9bf4573c116</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>f065c3ae-b3d0-41b7-9d86-a8d5c479a109</v>
+        <v>06f766ea-d7da-466f-8680-ccf581aa3021</v>
       </c>
       <c r="B62" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C62" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>06f766ea-d7da-466f-8680-ccf581aa3021</v>
+        <v>ea24a502-2868-4f93-9970-cf9f8e255d2c</v>
       </c>
       <c r="B63" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C63" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
       <c r="E63" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>ea24a502-2868-4f93-9970-cf9f8e255d2c</v>
+        <v>00ba14b8-7cf2-4192-a185-0a43775a7488</v>
       </c>
       <c r="B64" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C64" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="D64">
         <v>2</v>
       </c>
       <c r="E64" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>00ba14b8-7cf2-4192-a185-0a43775a7488</v>
+        <v>e124948f-d7f2-4ec6-b08d-23f8d0acb339</v>
       </c>
       <c r="B65" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C65" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="D65">
         <v>2</v>
       </c>
       <c r="E65" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>e124948f-d7f2-4ec6-b08d-23f8d0acb339</v>
+        <v>d4b474d0-1709-44b2-8861-d5872c1c5e6a</v>
       </c>
       <c r="B66" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C66" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
       </c>
       <c r="D66">
         <v>2</v>
       </c>
       <c r="E66" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>d4b474d0-1709-44b2-8861-d5872c1c5e6a</v>
+        <v>745992f0-ac23-42e2-8ee3-e54fb99365a0</v>
       </c>
       <c r="B67" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C67" t="str">
-        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D67">
         <v>2</v>
       </c>
       <c r="E67" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>745992f0-ac23-42e2-8ee3-e54fb99365a0</v>
+        <v>03a2b03a-057c-43b7-b6af-0ab394f3b5e3</v>
       </c>
       <c r="B68" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C68" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D68">
         <v>2</v>
       </c>
       <c r="E68" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>03a2b03a-057c-43b7-b6af-0ab394f3b5e3</v>
+        <v>6de96bda-2c08-4d80-8a5d-fa332cb0310a</v>
       </c>
       <c r="B69" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C69" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D69">
         <v>2</v>
       </c>
       <c r="E69" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>6de96bda-2c08-4d80-8a5d-fa332cb0310a</v>
+        <v>4893e237-56e6-4e4f-9581-55e6b16e6b2d</v>
       </c>
       <c r="B70" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C70" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="D70">
         <v>2</v>
       </c>
       <c r="E70" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>4893e237-56e6-4e4f-9581-55e6b16e6b2d</v>
+        <v>280c4149-fae0-4ee3-a3c6-15850fcbbe7b</v>
       </c>
       <c r="B71" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C71" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
       </c>
       <c r="D71">
         <v>2</v>
       </c>
       <c r="E71" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>280c4149-fae0-4ee3-a3c6-15850fcbbe7b</v>
+        <v>afcf99dd-2962-4dfe-9ac2-65cad52fa304</v>
       </c>
       <c r="B72" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C72" t="str">
-        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
+        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
       </c>
       <c r="D72">
         <v>2</v>
       </c>
       <c r="E72" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>afcf99dd-2962-4dfe-9ac2-65cad52fa304</v>
+        <v>7ab0a58c-f172-4d2c-88d9-4c0d2ccba604</v>
       </c>
       <c r="B73" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C73" t="str">
-        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
+        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
       </c>
       <c r="D73">
         <v>2</v>
       </c>
       <c r="E73" t="str">
-        <v>D3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>7ab0a58c-f172-4d2c-88d9-4c0d2ccba604</v>
+        <v>ce373f18-c7ff-4bf1-b9d1-3bf50965aa04</v>
       </c>
       <c r="B74" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C74" t="str">
-        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
+        <v>4f5224b0-063d-43fd-9435-f5c2723f61ed</v>
       </c>
       <c r="D74">
         <v>2</v>
       </c>
       <c r="E74" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>ce373f18-c7ff-4bf1-b9d1-3bf50965aa04</v>
+        <v>c88c1c42-d69d-4730-9a2d-f8efc1658996</v>
       </c>
       <c r="B75" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C75" t="str">
-        <v>4f5224b0-063d-43fd-9435-f5c2723f61ed</v>
+        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
       </c>
       <c r="D75">
         <v>2</v>
       </c>
       <c r="E75" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>c88c1c42-d69d-4730-9a2d-f8efc1658996</v>
+        <v>a473386f-cc07-4cef-87da-01fa6adf2771</v>
       </c>
       <c r="B76" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C76" t="str">
-        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E76" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>a473386f-cc07-4cef-87da-01fa6adf2771</v>
+        <v>473e708c-8bf7-4f0a-8544-f4e81ff1bb47</v>
       </c>
       <c r="B77" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C77" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D77">
         <v>3</v>
       </c>
       <c r="E77" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>473e708c-8bf7-4f0a-8544-f4e81ff1bb47</v>
+        <v>96ab8a7e-2cde-41fb-b942-7d6312684de8</v>
       </c>
       <c r="B78" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C78" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D78">
         <v>3</v>
       </c>
       <c r="E78" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>96ab8a7e-2cde-41fb-b942-7d6312684de8</v>
+        <v>5d644bba-6dab-429c-b526-89625b56db19</v>
       </c>
       <c r="B79" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C79" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D79">
         <v>3</v>
       </c>
       <c r="E79" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>5d644bba-6dab-429c-b526-89625b56db19</v>
+        <v>af2a101a-f4a8-4627-bd25-93ef66e48262</v>
       </c>
       <c r="B80" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C80" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D80">
         <v>3</v>
       </c>
       <c r="E80" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>af2a101a-f4a8-4627-bd25-93ef66e48262</v>
+        <v>3dda78fb-9a68-4939-b87b-8efd47b0dd5a</v>
       </c>
       <c r="B81" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C81" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D81">
         <v>3</v>
       </c>
       <c r="E81" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>3dda78fb-9a68-4939-b87b-8efd47b0dd5a</v>
+        <v>0a11b842-5aad-47f6-b92e-7af6f3c62657</v>
       </c>
       <c r="B82" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C82" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
       </c>
       <c r="D82">
         <v>3</v>
       </c>
       <c r="E82" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>0a11b842-5aad-47f6-b92e-7af6f3c62657</v>
+        <v>76e0bcb4-5c73-4cce-b466-5a2cd8dbaf61</v>
       </c>
       <c r="B83" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C83" t="str">
-        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
+        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
       </c>
       <c r="D83">
         <v>3</v>
       </c>
       <c r="E83" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>76e0bcb4-5c73-4cce-b466-5a2cd8dbaf61</v>
+        <v>4c73f602-4dbe-47ef-b958-67daf7b28744</v>
       </c>
       <c r="B84" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C84" t="str">
-        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
+        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
       </c>
       <c r="D84">
         <v>3</v>
       </c>
       <c r="E84" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>4c73f602-4dbe-47ef-b958-67daf7b28744</v>
+        <v>7ce1874e-a410-4afc-94c2-7794c1e619f9</v>
       </c>
       <c r="B85" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C85" t="str">
-        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D85">
         <v>3</v>
       </c>
       <c r="E85" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>7ce1874e-a410-4afc-94c2-7794c1e619f9</v>
+        <v>12337fbf-7541-4b4e-9303-5491374c685a</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D86">
         <v>3</v>
       </c>
       <c r="E86" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>12337fbf-7541-4b4e-9303-5491374c685a</v>
+        <v>18cad17d-234b-4ec6-8c04-2dd8bea45343</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
       </c>
       <c r="D87">
         <v>3</v>
       </c>
       <c r="E87" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>18cad17d-234b-4ec6-8c04-2dd8bea45343</v>
+        <v>a09b35b6-164d-4249-bafa-740b28da3ce8</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
+        <v>222469f4-a8d9-4550-b6ee-db9d00e24edd</v>
       </c>
       <c r="D88">
         <v>3</v>
       </c>
       <c r="E88" t="str">
-        <v>D3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>a09b35b6-164d-4249-bafa-740b28da3ce8</v>
+        <v>7ea55a54-59fa-463c-88f9-73ffd8e3dec8</v>
       </c>
       <c r="B89" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C89" t="str">
-        <v>222469f4-a8d9-4550-b6ee-db9d00e24edd</v>
+        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
       </c>
       <c r="D89">
         <v>3</v>
       </c>
       <c r="E89" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>7ea55a54-59fa-463c-88f9-73ffd8e3dec8</v>
+        <v>d27ad266-2110-4926-93b0-c7e71ce5bc45</v>
       </c>
       <c r="B90" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C90" t="str">
-        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
+        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
       </c>
       <c r="D90">
         <v>3</v>
       </c>
       <c r="E90" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>d27ad266-2110-4926-93b0-c7e71ce5bc45</v>
+        <v>eebd49a3-d1b0-4177-b18a-ec1603978f5d</v>
       </c>
       <c r="B91" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C91" t="str">
-        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D91">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E91" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>eebd49a3-d1b0-4177-b18a-ec1603978f5d</v>
+        <v>b5a2e616-5171-4231-87f6-f58e8239287d</v>
       </c>
       <c r="B92" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C92" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D92">
         <v>4</v>
       </c>
       <c r="E92" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>b5a2e616-5171-4231-87f6-f58e8239287d</v>
+        <v>42f10f1e-793f-45d4-93af-a5c85452f0dd</v>
       </c>
       <c r="B93" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C93" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
       </c>
       <c r="D93">
         <v>4</v>
       </c>
       <c r="E93" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>42f10f1e-793f-45d4-93af-a5c85452f0dd</v>
+        <v>6a0e8104-0b31-4883-b455-46fbc1183d62</v>
       </c>
       <c r="B94" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C94" t="str">
-        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
       </c>
       <c r="D94">
         <v>4</v>
       </c>
       <c r="E94" t="str">
-        <v>A3</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>6a0e8104-0b31-4883-b455-46fbc1183d62</v>
+        <v>41d0a46c-55bf-42c7-a7c4-6581992f61c3</v>
       </c>
       <c r="B95" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C95" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="D95">
         <v>4</v>
       </c>
       <c r="E95" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>41d0a46c-55bf-42c7-a7c4-6581992f61c3</v>
+        <v>803aa685-24e1-4980-b321-08219eece77d</v>
       </c>
       <c r="B96" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C96" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="D96">
         <v>4</v>
       </c>
       <c r="E96" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>803aa685-24e1-4980-b321-08219eece77d</v>
+        <v>0222f18f-7587-4801-83b6-6d7e76962b81</v>
       </c>
       <c r="B97" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C97" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="D97">
         <v>4</v>
       </c>
       <c r="E97" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>0222f18f-7587-4801-83b6-6d7e76962b81</v>
+        <v>fd77b985-5669-4c99-8266-fe48862ad73a</v>
       </c>
       <c r="B98" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C98" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="D98">
         <v>4</v>
       </c>
       <c r="E98" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>fd77b985-5669-4c99-8266-fe48862ad73a</v>
+        <v>29c45ddd-6bc5-41f0-bb49-e45d878188a8</v>
       </c>
       <c r="B99" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C99" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
       </c>
       <c r="D99">
         <v>4</v>
       </c>
       <c r="E99" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>29c45ddd-6bc5-41f0-bb49-e45d878188a8</v>
+        <v>1a282447-a4a0-4793-bab3-23c5a357da0c</v>
       </c>
       <c r="B100" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C100" t="str">
-        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D100">
         <v>4</v>
       </c>
       <c r="E100" t="str">
-        <v>C3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>1a282447-a4a0-4793-bab3-23c5a357da0c</v>
+        <v>bc95cf9f-7c8c-4047-ad73-82ed7ac31f59</v>
       </c>
       <c r="B101" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C101" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D101">
         <v>4</v>
       </c>
       <c r="E101" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>bc95cf9f-7c8c-4047-ad73-82ed7ac31f59</v>
+        <v>d4e2f177-077a-4414-875c-d008e87b6517</v>
       </c>
       <c r="B102" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C102" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D102">
         <v>4</v>
       </c>
       <c r="E102" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>d4e2f177-077a-4414-875c-d008e87b6517</v>
+        <v>9b333e56-5752-4319-bf42-5123b15f41a0</v>
       </c>
       <c r="B103" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C103" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
       </c>
       <c r="D103">
         <v>4</v>
       </c>
       <c r="E103" t="str">
-        <v>D3</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>9b333e56-5752-4319-bf42-5123b15f41a0</v>
+        <v>57a18db4-3934-4e3b-b225-3bcbb301ccb0</v>
       </c>
       <c r="B104" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C104" t="str">
-        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
+        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
       </c>
       <c r="D104">
         <v>4</v>
       </c>
       <c r="E104" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>57a18db4-3934-4e3b-b225-3bcbb301ccb0</v>
+        <v>a4f70468-25c0-4e83-8200-b5a88ea81bb2</v>
       </c>
       <c r="B105" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C105" t="str">
-        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
       </c>
       <c r="D105">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E105" t="str">
-        <v>E2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>a4f70468-25c0-4e83-8200-b5a88ea81bb2</v>
+        <v>adea01dd-088f-4ac8-87e7-5ee909db8c28</v>
       </c>
       <c r="B106" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C106" t="str">
-        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
       </c>
       <c r="D106">
         <v>5</v>
       </c>
       <c r="E106" t="str">
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>adea01dd-088f-4ac8-87e7-5ee909db8c28</v>
+        <v>bbc61a88-7c16-472b-b9ca-6099d25d721e</v>
       </c>
       <c r="B107" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C107" t="str">
-        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
       </c>
       <c r="D107">
         <v>5</v>
       </c>
       <c r="E107" t="str">
-        <v>A2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>bbc61a88-7c16-472b-b9ca-6099d25d721e</v>
+        <v>815541ea-4e52-452e-86d7-46f16986b060</v>
       </c>
       <c r="B108" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C108" t="str">
-        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
+        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
       </c>
       <c r="D108">
         <v>5</v>
       </c>
       <c r="E108" t="str">
-        <v>A3</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>815541ea-4e52-452e-86d7-46f16986b060</v>
+        <v>dd4f1361-aae2-4f6d-8e94-ba37f43e4d89</v>
       </c>
       <c r="B109" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C109" t="str">
-        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
+        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
       </c>
       <c r="D109">
         <v>5</v>
       </c>
       <c r="E109" t="str">
-        <v>A4</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>dd4f1361-aae2-4f6d-8e94-ba37f43e4d89</v>
+        <v>5b94a741-673a-4116-a95d-a451421525ab</v>
       </c>
       <c r="B110" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C110" t="str">
-        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
+        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
       </c>
       <c r="D110">
         <v>5</v>
       </c>
       <c r="E110" t="str">
-        <v>B1</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>5b94a741-673a-4116-a95d-a451421525ab</v>
+        <v>b6718d91-2f83-4455-8e0d-457c776c9101</v>
       </c>
       <c r="B111" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C111" t="str">
-        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
+        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
       </c>
       <c r="D111">
         <v>5</v>
       </c>
       <c r="E111" t="str">
-        <v>B2</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>b6718d91-2f83-4455-8e0d-457c776c9101</v>
+        <v>a2319e36-25b9-4901-95ca-7be604232784</v>
       </c>
       <c r="B112" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C112" t="str">
-        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
+        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
       </c>
       <c r="D112">
         <v>5</v>
       </c>
       <c r="E112" t="str">
-        <v>B3</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>a2319e36-25b9-4901-95ca-7be604232784</v>
+        <v>69a00148-c195-41b6-b676-b37b911e0501</v>
       </c>
       <c r="B113" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C113" t="str">
-        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
+        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
       </c>
       <c r="D113">
         <v>5</v>
       </c>
       <c r="E113" t="str">
-        <v>B4</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>69a00148-c195-41b6-b676-b37b911e0501</v>
+        <v>2e49d904-64ee-443c-aaca-9c63066a1f3f</v>
       </c>
       <c r="B114" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C114" t="str">
-        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
+        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
       </c>
       <c r="D114">
         <v>5</v>
       </c>
       <c r="E114" t="str">
-        <v>B5</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>2e49d904-64ee-443c-aaca-9c63066a1f3f</v>
+        <v>fcbc1d59-1625-44fe-a710-b186b719e48e</v>
       </c>
       <c r="B115" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C115" t="str">
-        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
+        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
       </c>
       <c r="D115">
         <v>5</v>
       </c>
       <c r="E115" t="str">
-        <v>C1</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>fcbc1d59-1625-44fe-a710-b186b719e48e</v>
+        <v>29b71713-fa5d-47a8-bad9-80d7eb24caeb</v>
       </c>
       <c r="B116" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C116" t="str">
-        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
+        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
       </c>
       <c r="D116">
         <v>5</v>
       </c>
       <c r="E116" t="str">
-        <v>C2</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>29b71713-fa5d-47a8-bad9-80d7eb24caeb</v>
+        <v>fb0d2557-0d04-4f3b-a255-591ab6025b2e</v>
       </c>
       <c r="B117" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C117" t="str">
-        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
+        <v>9f873871-29cc-45f0-894c-c54745230689</v>
       </c>
       <c r="D117">
         <v>5</v>
       </c>
       <c r="E117" t="str">
-        <v>C3</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>fb0d2557-0d04-4f3b-a255-591ab6025b2e</v>
+        <v>59c9d82b-5fe5-4222-9451-4aeca52fbe4c</v>
       </c>
       <c r="B118" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C118" t="str">
-        <v>9f873871-29cc-45f0-894c-c54745230689</v>
+        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
       </c>
       <c r="D118">
         <v>5</v>
       </c>
       <c r="E118" t="str">
-        <v>C4</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>59c9d82b-5fe5-4222-9451-4aeca52fbe4c</v>
+        <v>4bd1651a-6337-4459-b562-22f49804881e</v>
       </c>
       <c r="B119" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C119" t="str">
-        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
+        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
       </c>
       <c r="D119">
         <v>5</v>
       </c>
       <c r="E119" t="str">
-        <v>D1</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>4bd1651a-6337-4459-b562-22f49804881e</v>
+        <v>76361c32-4730-4a80-85c7-d8527a983168</v>
       </c>
       <c r="B120" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C120" t="str">
-        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
+        <v>076ad666-a34b-4ae1-b91f-de785dbdf5ec</v>
       </c>
       <c r="D120">
         <v>5</v>
       </c>
       <c r="E120" t="str">
-        <v>D2</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>76361c32-4730-4a80-85c7-d8527a983168</v>
+        <v>ac5f6dff-c75f-4064-bbff-c02af8506b49</v>
       </c>
       <c r="B121" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C121" t="str">
-        <v>076ad666-a34b-4ae1-b91f-de785dbdf5ec</v>
+        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
       </c>
       <c r="D121">
         <v>5</v>
       </c>
       <c r="E121" t="str">
-        <v>D3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>ac5f6dff-c75f-4064-bbff-c02af8506b49</v>
+        <v>be8f0518-0a03-477b-bc47-6339f48138b7</v>
       </c>
       <c r="B122" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C122" t="str">
-        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
+        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
       </c>
       <c r="D122">
         <v>5</v>
       </c>
       <c r="E122" t="str">
-        <v>D4</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>be8f0518-0a03-477b-bc47-6339f48138b7</v>
+        <v>4ff7518f-d926-4281-8920-473d76a91b19</v>
       </c>
       <c r="B123" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C123" t="str">
-        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
+        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
       </c>
       <c r="D123">
         <v>5</v>
       </c>
       <c r="E123" t="str">
-        <v>E1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>4ff7518f-d926-4281-8920-473d76a91b19</v>
+        <v>5a3eb837-9cc6-4e24-b138-1c56478bf199</v>
       </c>
       <c r="B124" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C124" t="str">
-        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
       </c>
       <c r="D124">
         <v>5</v>
       </c>
       <c r="E124" t="str">
-        <v>E2</v>
+        <v>E3</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>5a3eb837-9cc6-4e24-b138-1c56478bf199</v>
+        <v>47b50888-f2ee-4542-8d26-fd291becaf39</v>
       </c>
       <c r="B125" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C125" t="str">
-        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
+        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
       </c>
       <c r="D125">
         <v>5</v>
       </c>
       <c r="E125" t="str">
-        <v>E3</v>
+        <v>E4</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>47b50888-f2ee-4542-8d26-fd291becaf39</v>
+        <v>4edebf2c-170e-4642-b349-bf2c638e5869</v>
       </c>
       <c r="B126" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C126" t="str">
-        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
+        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
       </c>
       <c r="D126">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E126" t="str">
-        <v>E4</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="str">
-        <v>4edebf2c-170e-4642-b349-bf2c638e5869</v>
-      </c>
-      <c r="B127" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C127" t="str">
-        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
-      </c>
-      <c r="D127">
-        <v>6</v>
-      </c>
-      <c r="E127" t="str">
         <v>A1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H127"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H126"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update data caching logic to improve performance and accuracy
Refactor query invalidation strategies in seating chart components to be more targeted, removing redundant calls and optimizing data fetching for consistency. Update backup file timestamps and adjust contestant availability status.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: 9b460902-9d62-4e1a-bf01-524831930d8a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/TyjjPdU
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -2170,25 +2170,25 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
+        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
       </c>
       <c r="B47" t="str">
-        <v>Abigail Jackson</v>
+        <v>Nathan Allen</v>
       </c>
       <c r="C47">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="D47" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E47" t="str">
-        <v>abigail.jackson65@outlook.com</v>
+        <v>nathan.allen87@outlook.com</v>
       </c>
       <c r="F47" t="str">
-        <v>0411 824 257</v>
+        <v>0403 587 263</v>
       </c>
       <c r="G47" t="str">
-        <v>Newcastle</v>
+        <v>Adelaide</v>
       </c>
       <c r="H47" t="str">
         <v>B+</v>
@@ -2199,89 +2199,89 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>f5233693-d357-4cac-a660-70ef0398a969</v>
+        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
       </c>
       <c r="B48" t="str">
-        <v>Nathan Allen</v>
+        <v>Aria Lopez</v>
       </c>
       <c r="C48">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D48" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E48" t="str">
-        <v>nathan.allen87@outlook.com</v>
+        <v>aria.lopez55@hotmail.com</v>
       </c>
       <c r="F48" t="str">
-        <v>0403 587 263</v>
+        <v>0404 812 491</v>
       </c>
       <c r="G48" t="str">
-        <v>Adelaide</v>
+        <v>Sydney</v>
       </c>
       <c r="H48" t="str">
         <v>B+</v>
       </c>
       <c r="I48" t="str">
-        <v>assigned</v>
+        <v>available</v>
+      </c>
+      <c r="J48" t="str">
+        <v>Paisley Lee</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>29fc5656-fb78-4c9b-9800-b68957bc0a07</v>
+        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
       </c>
       <c r="B49" t="str">
-        <v>Aria Lopez</v>
+        <v>Mason Hill</v>
       </c>
       <c r="C49">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D49" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E49" t="str">
-        <v>aria.lopez55@hotmail.com</v>
+        <v>mason.hill27@outlook.com</v>
       </c>
       <c r="F49" t="str">
-        <v>0404 812 491</v>
+        <v>0410 682 884</v>
       </c>
       <c r="G49" t="str">
-        <v>Sydney</v>
+        <v>Canberra</v>
       </c>
       <c r="H49" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I49" t="str">
         <v>available</v>
       </c>
-      <c r="J49" t="str">
-        <v>Paisley Lee</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>adfcb6e3-82cb-46b9-8fb8-069fb91e2d4f</v>
+        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
       </c>
       <c r="B50" t="str">
-        <v>Mason Hill</v>
+        <v>Ryan Williams</v>
       </c>
       <c r="C50">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D50" t="str">
         <v>Male</v>
       </c>
       <c r="E50" t="str">
-        <v>mason.hill27@outlook.com</v>
+        <v>ryan.williams82@hotmail.com</v>
       </c>
       <c r="F50" t="str">
-        <v>0410 682 884</v>
+        <v>0401 450 673</v>
       </c>
       <c r="G50" t="str">
-        <v>Canberra</v>
+        <v>Perth</v>
       </c>
       <c r="H50" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I50" t="str">
         <v>available</v>
@@ -2289,25 +2289,25 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>d609a3ee-08af-4d16-aa51-c67e35cfa5c9</v>
+        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
       </c>
       <c r="B51" t="str">
-        <v>Ryan Williams</v>
+        <v>Abigail Jackson</v>
       </c>
       <c r="C51">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D51" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E51" t="str">
-        <v>ryan.williams82@hotmail.com</v>
+        <v>abigail.jackson65@outlook.com</v>
       </c>
       <c r="F51" t="str">
-        <v>0401 450 673</v>
+        <v>0411 824 257</v>
       </c>
       <c r="G51" t="str">
-        <v>Perth</v>
+        <v>Newcastle</v>
       </c>
       <c r="H51" t="str">
         <v>B+</v>
@@ -3777,147 +3777,147 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>076ad666-a34b-4ae1-b91f-de785dbdf5ec</v>
       </c>
       <c r="B99" t="str">
-        <v>Cora Mitchell</v>
+        <v>Nora Rogers</v>
       </c>
       <c r="C99">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D99" t="str">
         <v>Female</v>
       </c>
       <c r="E99" t="str">
-        <v>cora.mitchell80@icloud.com</v>
+        <v>nora.rogers98@yahoo.com</v>
       </c>
       <c r="F99" t="str">
-        <v>(929) 139-3875</v>
+        <v>(704) 607-6893</v>
       </c>
       <c r="G99" t="str">
-        <v>Newport Beach</v>
+        <v>Riverside</v>
       </c>
       <c r="H99" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I99" t="str">
         <v>assigned</v>
       </c>
-      <c r="J99" t="str">
-        <v>Christopher Carter</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>076ad666-a34b-4ae1-b91f-de785dbdf5ec</v>
+        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
       </c>
       <c r="B100" t="str">
-        <v>Nora Rogers</v>
+        <v>Ryan Lewis</v>
       </c>
       <c r="C100">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D100" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E100" t="str">
-        <v>nora.rogers98@yahoo.com</v>
+        <v>ryan.lewis85@yahoo.com</v>
       </c>
       <c r="F100" t="str">
-        <v>(704) 607-6893</v>
+        <v>0400 187 811</v>
       </c>
       <c r="G100" t="str">
-        <v>Riverside</v>
+        <v>Canberra</v>
       </c>
       <c r="H100" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I100" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>ca152dfe-8ddb-45c8-b084-8a5c9e6dacfa</v>
+        <v>bf1fc0b1-7d88-41a5-ab6f-ee4c085fd344</v>
       </c>
       <c r="B101" t="str">
-        <v>Ryan Lewis</v>
+        <v>Brooklyn Nguyen</v>
       </c>
       <c r="C101">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D101" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E101" t="str">
-        <v>ryan.lewis85@yahoo.com</v>
+        <v>brooklyn.nguyen77@yahoo.com</v>
       </c>
       <c r="F101" t="str">
-        <v>0400 187 811</v>
+        <v>(142) 872-1855</v>
       </c>
       <c r="G101" t="str">
-        <v>Canberra</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H101" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I101" t="str">
         <v>available</v>
       </c>
+      <c r="J101" t="str">
+        <v>Naomi Brown</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>bf1fc0b1-7d88-41a5-ab6f-ee4c085fd344</v>
+        <v>50b098db-86f4-4a21-8425-ab03df8f7a40</v>
       </c>
       <c r="B102" t="str">
-        <v>Brooklyn Nguyen</v>
+        <v>Lillian Campbell</v>
       </c>
       <c r="C102">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D102" t="str">
         <v>Female</v>
       </c>
       <c r="E102" t="str">
-        <v>brooklyn.nguyen77@yahoo.com</v>
+        <v>lillian.campbell41@yahoo.com</v>
       </c>
       <c r="F102" t="str">
-        <v>(142) 872-1855</v>
+        <v>(945) 213-8284</v>
       </c>
       <c r="G102" t="str">
-        <v>Los Angeles</v>
+        <v>Pasadena</v>
       </c>
       <c r="H102" t="str">
-        <v>A</v>
+        <v>A+</v>
       </c>
       <c r="I102" t="str">
         <v>available</v>
       </c>
       <c r="J102" t="str">
-        <v>Naomi Brown</v>
+        <v>Amelia Lopez</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>50b098db-86f4-4a21-8425-ab03df8f7a40</v>
+        <v>e9a3f4c7-c9ed-4fd1-a5a9-d3763ae52a55</v>
       </c>
       <c r="B103" t="str">
-        <v>Lillian Campbell</v>
+        <v>Victoria Anderson</v>
       </c>
       <c r="C103">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D103" t="str">
         <v>Female</v>
       </c>
       <c r="E103" t="str">
-        <v>lillian.campbell41@yahoo.com</v>
+        <v>victoria.anderson1@outlook.com</v>
       </c>
       <c r="F103" t="str">
-        <v>(945) 213-8284</v>
+        <v>(622) 987-4829</v>
       </c>
       <c r="G103" t="str">
-        <v>Pasadena</v>
+        <v>Sacramento</v>
       </c>
       <c r="H103" t="str">
         <v>A+</v>
@@ -3926,219 +3926,219 @@
         <v>available</v>
       </c>
       <c r="J103" t="str">
-        <v>Amelia Lopez</v>
+        <v>Sophia Reyes</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>e9a3f4c7-c9ed-4fd1-a5a9-d3763ae52a55</v>
+        <v>af09efbe-e83d-4046-8dc8-e6a06dfc0c40</v>
       </c>
       <c r="B104" t="str">
-        <v>Victoria Anderson</v>
+        <v>Paisley Evans</v>
       </c>
       <c r="C104">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D104" t="str">
         <v>Female</v>
       </c>
       <c r="E104" t="str">
-        <v>victoria.anderson1@outlook.com</v>
+        <v>paisley.evans52@yahoo.com</v>
       </c>
       <c r="F104" t="str">
-        <v>(622) 987-4829</v>
+        <v>(894) 250-9501</v>
       </c>
       <c r="G104" t="str">
-        <v>Sacramento</v>
+        <v>Torrance</v>
       </c>
       <c r="H104" t="str">
-        <v>A+</v>
+        <v>B+</v>
       </c>
       <c r="I104" t="str">
         <v>available</v>
       </c>
-      <c r="J104" t="str">
-        <v>Sophia Reyes</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>af09efbe-e83d-4046-8dc8-e6a06dfc0c40</v>
+        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
       </c>
       <c r="B105" t="str">
-        <v>Paisley Evans</v>
+        <v>Hazel Mitchell</v>
       </c>
       <c r="C105">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D105" t="str">
         <v>Female</v>
       </c>
       <c r="E105" t="str">
-        <v>paisley.evans52@yahoo.com</v>
+        <v>hazel.mitchell91@gmail.com</v>
       </c>
       <c r="F105" t="str">
-        <v>(894) 250-9501</v>
+        <v>0400 683 761</v>
       </c>
       <c r="G105" t="str">
-        <v>Torrance</v>
+        <v>Perth</v>
       </c>
       <c r="H105" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I105" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J105" t="str">
+        <v>Caroline Taylor</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
+        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
       </c>
       <c r="B106" t="str">
-        <v>Hazel Mitchell</v>
+        <v>Piper Green</v>
       </c>
       <c r="C106">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D106" t="str">
         <v>Female</v>
       </c>
       <c r="E106" t="str">
-        <v>hazel.mitchell91@gmail.com</v>
+        <v>piper.green82@hotmail.com</v>
       </c>
       <c r="F106" t="str">
-        <v>0400 683 761</v>
+        <v>(678) 816-2263</v>
       </c>
       <c r="G106" t="str">
-        <v>Perth</v>
+        <v>Burbank</v>
       </c>
       <c r="H106" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I106" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J106" t="str">
-        <v>Caroline Taylor</v>
+        <v>Josiah Brown</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>e7129d06-9fe4-44dd-afce-e4faeebfe1a9</v>
+        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
       </c>
       <c r="B107" t="str">
-        <v>Piper Green</v>
+        <v>Penelope Williams</v>
       </c>
       <c r="C107">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D107" t="str">
         <v>Female</v>
       </c>
       <c r="E107" t="str">
-        <v>piper.green82@hotmail.com</v>
+        <v>penelope.williams29@hotmail.com</v>
       </c>
       <c r="F107" t="str">
-        <v>(678) 816-2263</v>
+        <v>(735) 691-4267</v>
       </c>
       <c r="G107" t="str">
-        <v>Burbank</v>
+        <v>Sacramento</v>
       </c>
       <c r="H107" t="str">
         <v>B</v>
       </c>
       <c r="I107" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J107" t="str">
-        <v>Josiah Brown</v>
+        <v>Savannah Rivera</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
+        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
       </c>
       <c r="B108" t="str">
-        <v>Penelope Williams</v>
+        <v>Avery Taylor</v>
       </c>
       <c r="C108">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D108" t="str">
         <v>Female</v>
       </c>
       <c r="E108" t="str">
-        <v>penelope.williams29@hotmail.com</v>
+        <v>avery.taylor87@outlook.com</v>
       </c>
       <c r="F108" t="str">
-        <v>(735) 691-4267</v>
+        <v>(299) 491-7680</v>
       </c>
       <c r="G108" t="str">
-        <v>Sacramento</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H108" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I108" t="str">
         <v>assigned</v>
       </c>
       <c r="J108" t="str">
-        <v>Savannah Rivera</v>
+        <v>Audrey Hill</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="B109" t="str">
-        <v>Avery Taylor</v>
+        <v>Eleanor Hall</v>
       </c>
       <c r="C109">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D109" t="str">
         <v>Female</v>
       </c>
       <c r="E109" t="str">
-        <v>avery.taylor87@outlook.com</v>
+        <v>eleanor.hall7@yahoo.com</v>
       </c>
       <c r="F109" t="str">
-        <v>(299) 491-7680</v>
+        <v>(627) 443-5972</v>
       </c>
       <c r="G109" t="str">
-        <v>Los Angeles</v>
+        <v>Stockton</v>
       </c>
       <c r="H109" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I109" t="str">
         <v>assigned</v>
       </c>
       <c r="J109" t="str">
-        <v>Audrey Hill</v>
+        <v>Michael Campbell, Sadie Williams</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>4e28a208-5278-410d-b375-d9c77ba144d7</v>
       </c>
       <c r="B110" t="str">
-        <v>Eleanor Hall</v>
+        <v>Riley Scott</v>
       </c>
       <c r="C110">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D110" t="str">
         <v>Female</v>
       </c>
       <c r="E110" t="str">
-        <v>eleanor.hall7@yahoo.com</v>
+        <v>riley.scott58@hotmail.com</v>
       </c>
       <c r="F110" t="str">
-        <v>(627) 443-5972</v>
+        <v>(848) 718-3465</v>
       </c>
       <c r="G110" t="str">
-        <v>Stockton</v>
+        <v>San Francisco</v>
       </c>
       <c r="H110" t="str">
         <v>B</v>
@@ -4146,31 +4146,28 @@
       <c r="I110" t="str">
         <v>assigned</v>
       </c>
-      <c r="J110" t="str">
-        <v>Michael Campbell, Sadie Williams</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>4e28a208-5278-410d-b375-d9c77ba144d7</v>
+        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
       </c>
       <c r="B111" t="str">
-        <v>Riley Scott</v>
+        <v>Victoria Thompson</v>
       </c>
       <c r="C111">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D111" t="str">
         <v>Female</v>
       </c>
       <c r="E111" t="str">
-        <v>riley.scott58@hotmail.com</v>
+        <v>victoria.thompson68@yahoo.com</v>
       </c>
       <c r="F111" t="str">
-        <v>(848) 718-3465</v>
+        <v>(793) 601-6884</v>
       </c>
       <c r="G111" t="str">
-        <v>San Francisco</v>
+        <v>San Jose</v>
       </c>
       <c r="H111" t="str">
         <v>B</v>
@@ -4181,71 +4178,71 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="B112" t="str">
-        <v>Victoria Thompson</v>
+        <v>Serenity Campbell</v>
       </c>
       <c r="C112">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D112" t="str">
         <v>Female</v>
       </c>
       <c r="E112" t="str">
-        <v>victoria.thompson68@yahoo.com</v>
+        <v>serenity.campbell1@yahoo.com</v>
       </c>
       <c r="F112" t="str">
-        <v>(793) 601-6884</v>
+        <v>(479) 565-5966</v>
       </c>
       <c r="G112" t="str">
-        <v>San Jose</v>
+        <v>Irvine</v>
       </c>
       <c r="H112" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I112" t="str">
         <v>assigned</v>
       </c>
+      <c r="J112" t="str">
+        <v>Jackson Jackson, Isaiah Green</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>24928131-51b3-46f8-b43f-2cf989696f62</v>
       </c>
       <c r="B113" t="str">
-        <v>Serenity Campbell</v>
+        <v>Amelia Garcia</v>
       </c>
       <c r="C113">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D113" t="str">
         <v>Female</v>
       </c>
       <c r="E113" t="str">
-        <v>serenity.campbell1@yahoo.com</v>
+        <v>amelia.garcia16@gmail.com</v>
       </c>
       <c r="F113" t="str">
-        <v>(479) 565-5966</v>
+        <v>(331) 367-3904</v>
       </c>
       <c r="G113" t="str">
-        <v>Irvine</v>
+        <v>Anaheim</v>
       </c>
       <c r="H113" t="str">
         <v>B+</v>
       </c>
       <c r="I113" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J113" t="str">
-        <v>Jackson Jackson, Isaiah Green</v>
+        <v>available</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>24928131-51b3-46f8-b43f-2cf989696f62</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="B114" t="str">
-        <v>Amelia Garcia</v>
+        <v>Valentina Morales</v>
       </c>
       <c r="C114">
         <v>37</v>
@@ -4254,51 +4251,54 @@
         <v>Female</v>
       </c>
       <c r="E114" t="str">
-        <v>amelia.garcia16@gmail.com</v>
+        <v>valentina.morales27@icloud.com</v>
       </c>
       <c r="F114" t="str">
-        <v>(331) 367-3904</v>
+        <v>(896) 204-3978</v>
       </c>
       <c r="G114" t="str">
-        <v>Anaheim</v>
+        <v>San Jose</v>
       </c>
       <c r="H114" t="str">
         <v>B+</v>
       </c>
       <c r="I114" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J114" t="str">
+        <v>Adam Hall, Grayson Morgan</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
       </c>
       <c r="B115" t="str">
-        <v>Valentina Morales</v>
+        <v>Cora Mitchell</v>
       </c>
       <c r="C115">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D115" t="str">
         <v>Female</v>
       </c>
       <c r="E115" t="str">
-        <v>valentina.morales27@icloud.com</v>
+        <v>cora.mitchell80@icloud.com</v>
       </c>
       <c r="F115" t="str">
-        <v>(896) 204-3978</v>
+        <v>(929) 139-3875</v>
       </c>
       <c r="G115" t="str">
-        <v>San Jose</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H115" t="str">
         <v>B+</v>
       </c>
       <c r="I115" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J115" t="str">
-        <v>Adam Hall, Grayson Morgan</v>
+        <v>Christopher Carter</v>
       </c>
     </row>
     <row r="116">
@@ -7637,25 +7637,25 @@
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="B223" t="str">
-        <v>Christopher Carter</v>
+        <v>Adam Hall</v>
       </c>
       <c r="C223">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D223" t="str">
         <v>Male</v>
       </c>
       <c r="E223" t="str">
-        <v>christopher.carter22@outlook.com</v>
+        <v>adam.hall35@outlook.com</v>
       </c>
       <c r="F223" t="str">
-        <v>(176) 989-4341</v>
+        <v>(742) 142-5313</v>
       </c>
       <c r="G223" t="str">
-        <v>Los Angeles</v>
+        <v>Santa Ana</v>
       </c>
       <c r="H223" t="str">
         <v>B</v>
@@ -7664,155 +7664,155 @@
         <v>assigned</v>
       </c>
       <c r="J223" t="str">
-        <v>Cora Mitchell</v>
+        <v>Grayson Morgan, Valentina Morales</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
       </c>
       <c r="B224" t="str">
-        <v>Adam Hall</v>
+        <v>Aria Nguyen</v>
       </c>
       <c r="C224">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D224" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E224" t="str">
-        <v>adam.hall35@outlook.com</v>
+        <v>aria.nguyen36@gmail.com</v>
       </c>
       <c r="F224" t="str">
-        <v>(742) 142-5313</v>
+        <v>0401 618 716</v>
       </c>
       <c r="G224" t="str">
-        <v>Santa Ana</v>
+        <v>Sydney</v>
       </c>
       <c r="H224" t="str">
         <v>B</v>
       </c>
       <c r="I224" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J224" t="str">
-        <v>Grayson Morgan, Valentina Morales</v>
+        <v>available</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>f68d2771-4820-4fef-b156-093280aeea67</v>
+        <v>5965e7f9-ebf0-4e66-a197-03be16110662</v>
       </c>
       <c r="B225" t="str">
-        <v>Aria Nguyen</v>
+        <v>Cameron Clark</v>
       </c>
       <c r="C225">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D225" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E225" t="str">
-        <v>aria.nguyen36@gmail.com</v>
+        <v>cameron.clark37@gmail.com</v>
       </c>
       <c r="F225" t="str">
-        <v>0401 618 716</v>
+        <v>(267) 288-3549</v>
       </c>
       <c r="G225" t="str">
-        <v>Sydney</v>
+        <v>Santa Ana</v>
       </c>
       <c r="H225" t="str">
         <v>B</v>
       </c>
       <c r="I225" t="str">
-        <v>available</v>
+        <v>assigned</v>
+      </c>
+      <c r="J225" t="str">
+        <v>Nolan Ortiz</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>5965e7f9-ebf0-4e66-a197-03be16110662</v>
+        <v>644e41d7-b99e-4381-99a9-65d5ee89ad50</v>
       </c>
       <c r="B226" t="str">
-        <v>Cameron Clark</v>
+        <v>Hunter Scott</v>
       </c>
       <c r="C226">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D226" t="str">
         <v>Male</v>
       </c>
       <c r="E226" t="str">
-        <v>cameron.clark37@gmail.com</v>
+        <v>hunter.scott37@outlook.com</v>
       </c>
       <c r="F226" t="str">
-        <v>(267) 288-3549</v>
+        <v>(477) 130-2066</v>
       </c>
       <c r="G226" t="str">
-        <v>Santa Ana</v>
+        <v>Torrance</v>
       </c>
       <c r="H226" t="str">
         <v>B</v>
       </c>
       <c r="I226" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J226" t="str">
-        <v>Nolan Ortiz</v>
+        <v>Zoey Cook</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>644e41d7-b99e-4381-99a9-65d5ee89ad50</v>
+        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
       </c>
       <c r="B227" t="str">
-        <v>Hunter Scott</v>
+        <v>Nolan Ortiz</v>
       </c>
       <c r="C227">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D227" t="str">
         <v>Male</v>
       </c>
       <c r="E227" t="str">
-        <v>hunter.scott37@outlook.com</v>
+        <v>nolan.ortiz57@gmail.com</v>
       </c>
       <c r="F227" t="str">
-        <v>(477) 130-2066</v>
+        <v>(473) 870-4585</v>
       </c>
       <c r="G227" t="str">
-        <v>Torrance</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H227" t="str">
         <v>B</v>
       </c>
       <c r="I227" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J227" t="str">
-        <v>Zoey Cook</v>
+        <v>Cameron Clark</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>d279968e-2739-4860-92b0-61f1c31b6a72</v>
+        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
       </c>
       <c r="B228" t="str">
-        <v>Nolan Ortiz</v>
+        <v>Maya Moore</v>
       </c>
       <c r="C228">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D228" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E228" t="str">
-        <v>nolan.ortiz57@gmail.com</v>
+        <v>maya.moore54@outlook.com</v>
       </c>
       <c r="F228" t="str">
-        <v>(473) 870-4585</v>
+        <v>0400 718 585</v>
       </c>
       <c r="G228" t="str">
-        <v>Santa Monica</v>
+        <v>Toowoomba</v>
       </c>
       <c r="H228" t="str">
         <v>B</v>
@@ -7821,39 +7821,39 @@
         <v>assigned</v>
       </c>
       <c r="J228" t="str">
-        <v>Cameron Clark</v>
+        <v>Sofia Williams</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>b8c1889f-fd66-4304-90d7-bd50422cbc52</v>
+        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
       </c>
       <c r="B229" t="str">
-        <v>Maya Moore</v>
+        <v>Christopher Carter</v>
       </c>
       <c r="C229">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D229" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E229" t="str">
-        <v>maya.moore54@outlook.com</v>
+        <v>christopher.carter22@outlook.com</v>
       </c>
       <c r="F229" t="str">
-        <v>0400 718 585</v>
+        <v>(176) 989-4341</v>
       </c>
       <c r="G229" t="str">
-        <v>Toowoomba</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H229" t="str">
         <v>B</v>
       </c>
       <c r="I229" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J229" t="str">
-        <v>Sofia Williams</v>
+        <v>Cora Mitchell</v>
       </c>
     </row>
     <row r="230">
@@ -12372,7 +12372,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H126"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -13170,1367 +13170,1316 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>a973a84d-478a-485f-94de-6087fbbcf4db</v>
+        <v>bc7f838a-b8a5-4f40-9451-6e5b608931ed</v>
       </c>
       <c r="B47" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C47" t="str">
-        <v>9b54470e-fe91-4ebb-b0aa-becf22a8cc3c</v>
+        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" t="str">
-        <v>E1</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>46b7e745-083b-41b0-b8fa-a0391457260b</v>
+        <v>bc22ad22-1b7c-446d-8cd9-8d1a90cafebd</v>
       </c>
       <c r="B48" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C48" t="str">
-        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
+        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="str">
-        <v>D2</v>
+        <v>E4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>cb62b970-7194-4872-9fc3-92a543d01f39</v>
+        <v>96ecc4ef-fd63-4393-b7df-9423b5df0868</v>
       </c>
       <c r="B49" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C49" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="str">
-        <v>A1</v>
+        <v>E3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>26945441-ea86-4493-a389-00ade06c7d37</v>
+        <v>cb62b970-7194-4872-9fc3-92a543d01f39</v>
       </c>
       <c r="B50" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C50" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50" t="str">
-        <v>A2</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>5297fdf0-8524-4546-a9e5-75c4b7595db7</v>
+        <v>26945441-ea86-4493-a389-00ade06c7d37</v>
       </c>
       <c r="B51" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C51" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51" t="str">
-        <v>A3</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>1eb3e2c4-236f-4b99-a085-f991d9c2106b</v>
+        <v>5297fdf0-8524-4546-a9e5-75c4b7595db7</v>
       </c>
       <c r="B52" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C52" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52" t="str">
-        <v>B1</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>32e4e84d-d241-4470-9b3b-210beb9afe12</v>
+        <v>1eb3e2c4-236f-4b99-a085-f991d9c2106b</v>
       </c>
       <c r="B53" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C53" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="str">
-        <v>B2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>bfd354a2-712a-4be3-a1bb-3f13e4f52550</v>
+        <v>32e4e84d-d241-4470-9b3b-210beb9afe12</v>
       </c>
       <c r="B54" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C54" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="str">
-        <v>B3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>eaa76e1c-43f0-4ecb-94bb-b16bb9beffae</v>
+        <v>bfd354a2-712a-4be3-a1bb-3f13e4f52550</v>
       </c>
       <c r="B55" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C55" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="str">
-        <v>C1</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>c2b4d4be-64b7-41c5-a958-e3d8c99fc790</v>
+        <v>eaa76e1c-43f0-4ecb-94bb-b16bb9beffae</v>
       </c>
       <c r="B56" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C56" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56" t="str">
-        <v>C2</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>96ecc4ef-fd63-4393-b7df-9423b5df0868</v>
+        <v>c2b4d4be-64b7-41c5-a958-e3d8c99fc790</v>
       </c>
       <c r="B57" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C57" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="str">
-        <v>C3</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>cb41808d-c7e0-4faf-8129-a2e53357c14a</v>
+        <v>f065c3ae-b3d0-41b7-9d86-a8d5c479a109</v>
       </c>
       <c r="B58" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C58" t="str">
-        <v>3dcd887e-9357-49a1-be20-96ba912e33bf</v>
+        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E58" t="str">
-        <v>D1</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>bc7f838a-b8a5-4f40-9451-6e5b608931ed</v>
+        <v>06f766ea-d7da-466f-8680-ccf581aa3021</v>
       </c>
       <c r="B59" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C59" t="str">
-        <v>a8f50ac0-29e0-4209-a524-83ca7878b0ca</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59" t="str">
-        <v>D3</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>bc22ad22-1b7c-446d-8cd9-8d1a90cafebd</v>
+        <v>ea24a502-2868-4f93-9970-cf9f8e255d2c</v>
       </c>
       <c r="B60" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C60" t="str">
-        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
+        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E60" t="str">
-        <v>D4</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>f065c3ae-b3d0-41b7-9d86-a8d5c479a109</v>
+        <v>00ba14b8-7cf2-4192-a185-0a43775a7488</v>
       </c>
       <c r="B61" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C61" t="str">
-        <v>fc97dba8-a877-4547-b6c9-0c6b058b1c94</v>
+        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
       <c r="E61" t="str">
-        <v>A1</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>06f766ea-d7da-466f-8680-ccf581aa3021</v>
+        <v>e124948f-d7f2-4ec6-b08d-23f8d0acb339</v>
       </c>
       <c r="B62" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C62" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62" t="str">
-        <v>A2</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>ea24a502-2868-4f93-9970-cf9f8e255d2c</v>
+        <v>d4b474d0-1709-44b2-8861-d5872c1c5e6a</v>
       </c>
       <c r="B63" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C63" t="str">
-        <v>151541b8-8cbb-452a-b532-1a0df3d1d4b6</v>
+        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
       <c r="E63" t="str">
-        <v>A3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>00ba14b8-7cf2-4192-a185-0a43775a7488</v>
+        <v>745992f0-ac23-42e2-8ee3-e54fb99365a0</v>
       </c>
       <c r="B64" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C64" t="str">
-        <v>703385ff-46f6-4b8f-9998-1e18951304e0</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="D64">
         <v>2</v>
       </c>
       <c r="E64" t="str">
-        <v>B1</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>e124948f-d7f2-4ec6-b08d-23f8d0acb339</v>
+        <v>03a2b03a-057c-43b7-b6af-0ab394f3b5e3</v>
       </c>
       <c r="B65" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C65" t="str">
-        <v>443fcd0e-727d-4035-ab6a-c3df01515271</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
       <c r="D65">
         <v>2</v>
       </c>
       <c r="E65" t="str">
-        <v>B2</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>d4b474d0-1709-44b2-8861-d5872c1c5e6a</v>
+        <v>6de96bda-2c08-4d80-8a5d-fa332cb0310a</v>
       </c>
       <c r="B66" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C66" t="str">
-        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="D66">
         <v>2</v>
       </c>
       <c r="E66" t="str">
-        <v>B3</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>745992f0-ac23-42e2-8ee3-e54fb99365a0</v>
+        <v>4893e237-56e6-4e4f-9581-55e6b16e6b2d</v>
       </c>
       <c r="B67" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C67" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
       </c>
       <c r="D67">
         <v>2</v>
       </c>
       <c r="E67" t="str">
-        <v>C1</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>03a2b03a-057c-43b7-b6af-0ab394f3b5e3</v>
+        <v>280c4149-fae0-4ee3-a3c6-15850fcbbe7b</v>
       </c>
       <c r="B68" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C68" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
       </c>
       <c r="D68">
         <v>2</v>
       </c>
       <c r="E68" t="str">
-        <v>C2</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>6de96bda-2c08-4d80-8a5d-fa332cb0310a</v>
+        <v>afcf99dd-2962-4dfe-9ac2-65cad52fa304</v>
       </c>
       <c r="B69" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C69" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
       </c>
       <c r="D69">
         <v>2</v>
       </c>
       <c r="E69" t="str">
-        <v>C3</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>4893e237-56e6-4e4f-9581-55e6b16e6b2d</v>
+        <v>7ab0a58c-f172-4d2c-88d9-4c0d2ccba604</v>
       </c>
       <c r="B70" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C70" t="str">
-        <v>5a16ef0a-cce8-4d1b-bfa5-3892331170c1</v>
+        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
       </c>
       <c r="D70">
         <v>2</v>
       </c>
       <c r="E70" t="str">
-        <v>D1</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>280c4149-fae0-4ee3-a3c6-15850fcbbe7b</v>
+        <v>ce373f18-c7ff-4bf1-b9d1-3bf50965aa04</v>
       </c>
       <c r="B71" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C71" t="str">
-        <v>567e589d-b232-43c2-9d30-3ff1e359f372</v>
+        <v>4f5224b0-063d-43fd-9435-f5c2723f61ed</v>
       </c>
       <c r="D71">
         <v>2</v>
       </c>
       <c r="E71" t="str">
-        <v>D2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>afcf99dd-2962-4dfe-9ac2-65cad52fa304</v>
+        <v>c88c1c42-d69d-4730-9a2d-f8efc1658996</v>
       </c>
       <c r="B72" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C72" t="str">
-        <v>2738f18e-1f2e-44d7-aa26-778ed59438ac</v>
+        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
       </c>
       <c r="D72">
         <v>2</v>
       </c>
       <c r="E72" t="str">
-        <v>D3</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>7ab0a58c-f172-4d2c-88d9-4c0d2ccba604</v>
+        <v>a473386f-cc07-4cef-87da-01fa6adf2771</v>
       </c>
       <c r="B73" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C73" t="str">
-        <v>f960de1f-a40f-4281-9d39-2a7822335b9b</v>
+        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
       </c>
       <c r="D73">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E73" t="str">
-        <v>D4</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>ce373f18-c7ff-4bf1-b9d1-3bf50965aa04</v>
+        <v>473e708c-8bf7-4f0a-8544-f4e81ff1bb47</v>
       </c>
       <c r="B74" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C74" t="str">
-        <v>4f5224b0-063d-43fd-9435-f5c2723f61ed</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E74" t="str">
-        <v>E1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>c88c1c42-d69d-4730-9a2d-f8efc1658996</v>
+        <v>96ab8a7e-2cde-41fb-b942-7d6312684de8</v>
       </c>
       <c r="B75" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C75" t="str">
-        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
+        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E75" t="str">
-        <v>E2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>a473386f-cc07-4cef-87da-01fa6adf2771</v>
+        <v>5d644bba-6dab-429c-b526-89625b56db19</v>
       </c>
       <c r="B76" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C76" t="str">
-        <v>6b672a17-fbf7-4b44-841d-dc10fbe8cbce</v>
+        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
       </c>
       <c r="D76">
         <v>3</v>
       </c>
       <c r="E76" t="str">
-        <v>A1</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>473e708c-8bf7-4f0a-8544-f4e81ff1bb47</v>
+        <v>af2a101a-f4a8-4627-bd25-93ef66e48262</v>
       </c>
       <c r="B77" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C77" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
       </c>
       <c r="D77">
         <v>3</v>
       </c>
       <c r="E77" t="str">
-        <v>A2</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>96ab8a7e-2cde-41fb-b942-7d6312684de8</v>
+        <v>3dda78fb-9a68-4939-b87b-8efd47b0dd5a</v>
       </c>
       <c r="B78" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C78" t="str">
-        <v>1c24b746-78a8-49cd-9c4d-3d22726dbc1b</v>
+        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
       </c>
       <c r="D78">
         <v>3</v>
       </c>
       <c r="E78" t="str">
-        <v>A3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>5d644bba-6dab-429c-b526-89625b56db19</v>
+        <v>0a11b842-5aad-47f6-b92e-7af6f3c62657</v>
       </c>
       <c r="B79" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C79" t="str">
-        <v>b498fd02-c816-4b07-976f-1100495bf38b</v>
+        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
       </c>
       <c r="D79">
         <v>3</v>
       </c>
       <c r="E79" t="str">
-        <v>B1</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>af2a101a-f4a8-4627-bd25-93ef66e48262</v>
+        <v>76e0bcb4-5c73-4cce-b466-5a2cd8dbaf61</v>
       </c>
       <c r="B80" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C80" t="str">
-        <v>a3363acf-3338-40ec-a745-9aef8dca39fc</v>
+        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
       </c>
       <c r="D80">
         <v>3</v>
       </c>
       <c r="E80" t="str">
-        <v>B2</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>3dda78fb-9a68-4939-b87b-8efd47b0dd5a</v>
+        <v>4c73f602-4dbe-47ef-b958-67daf7b28744</v>
       </c>
       <c r="B81" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C81" t="str">
-        <v>49fbe592-0995-4321-b8af-fbe859ca414c</v>
+        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
       </c>
       <c r="D81">
         <v>3</v>
       </c>
       <c r="E81" t="str">
-        <v>B3</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>0a11b842-5aad-47f6-b92e-7af6f3c62657</v>
+        <v>7ce1874e-a410-4afc-94c2-7794c1e619f9</v>
       </c>
       <c r="B82" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C82" t="str">
-        <v>c284df19-568f-44d7-9ddf-b63e5af17f4a</v>
+        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
       </c>
       <c r="D82">
         <v>3</v>
       </c>
       <c r="E82" t="str">
-        <v>C1</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>76e0bcb4-5c73-4cce-b466-5a2cd8dbaf61</v>
+        <v>12337fbf-7541-4b4e-9303-5491374c685a</v>
       </c>
       <c r="B83" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C83" t="str">
-        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
+        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
       </c>
       <c r="D83">
         <v>3</v>
       </c>
       <c r="E83" t="str">
-        <v>C2</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>4c73f602-4dbe-47ef-b958-67daf7b28744</v>
+        <v>18cad17d-234b-4ec6-8c04-2dd8bea45343</v>
       </c>
       <c r="B84" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C84" t="str">
-        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
+        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
       </c>
       <c r="D84">
         <v>3</v>
       </c>
       <c r="E84" t="str">
-        <v>C3</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>7ce1874e-a410-4afc-94c2-7794c1e619f9</v>
+        <v>a09b35b6-164d-4249-bafa-740b28da3ce8</v>
       </c>
       <c r="B85" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C85" t="str">
-        <v>42504e80-d5df-4b97-a283-eb96728c425f</v>
+        <v>222469f4-a8d9-4550-b6ee-db9d00e24edd</v>
       </c>
       <c r="D85">
         <v>3</v>
       </c>
       <c r="E85" t="str">
-        <v>D1</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>12337fbf-7541-4b4e-9303-5491374c685a</v>
+        <v>7ea55a54-59fa-463c-88f9-73ffd8e3dec8</v>
       </c>
       <c r="B86" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C86" t="str">
-        <v>bb319a54-7dbf-4a05-bd7f-8f2f6aa6b414</v>
+        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
       </c>
       <c r="D86">
         <v>3</v>
       </c>
       <c r="E86" t="str">
-        <v>D2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>18cad17d-234b-4ec6-8c04-2dd8bea45343</v>
+        <v>d27ad266-2110-4926-93b0-c7e71ce5bc45</v>
       </c>
       <c r="B87" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C87" t="str">
-        <v>2d659242-2255-4502-b333-781c9b2645fd</v>
+        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
       </c>
       <c r="D87">
         <v>3</v>
       </c>
       <c r="E87" t="str">
-        <v>D3</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>a09b35b6-164d-4249-bafa-740b28da3ce8</v>
+        <v>eebd49a3-d1b0-4177-b18a-ec1603978f5d</v>
       </c>
       <c r="B88" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C88" t="str">
-        <v>222469f4-a8d9-4550-b6ee-db9d00e24edd</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E88" t="str">
-        <v>D4</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>7ea55a54-59fa-463c-88f9-73ffd8e3dec8</v>
+        <v>b5a2e616-5171-4231-87f6-f58e8239287d</v>
       </c>
       <c r="B89" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C89" t="str">
-        <v>6849995e-3474-4988-87b0-1db2638461ca</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D89">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E89" t="str">
-        <v>E1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>d27ad266-2110-4926-93b0-c7e71ce5bc45</v>
+        <v>42f10f1e-793f-45d4-93af-a5c85452f0dd</v>
       </c>
       <c r="B90" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C90" t="str">
-        <v>1adac400-525f-40f4-8b6d-20df8ce78e9d</v>
+        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E90" t="str">
-        <v>E2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>eebd49a3-d1b0-4177-b18a-ec1603978f5d</v>
+        <v>6a0e8104-0b31-4883-b455-46fbc1183d62</v>
       </c>
       <c r="B91" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C91" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
       </c>
       <c r="D91">
         <v>4</v>
       </c>
       <c r="E91" t="str">
-        <v>A1</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>b5a2e616-5171-4231-87f6-f58e8239287d</v>
+        <v>41d0a46c-55bf-42c7-a7c4-6581992f61c3</v>
       </c>
       <c r="B92" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C92" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="D92">
         <v>4</v>
       </c>
       <c r="E92" t="str">
-        <v>A2</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>42f10f1e-793f-45d4-93af-a5c85452f0dd</v>
+        <v>803aa685-24e1-4980-b321-08219eece77d</v>
       </c>
       <c r="B93" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C93" t="str">
-        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="D93">
         <v>4</v>
       </c>
       <c r="E93" t="str">
-        <v>A3</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>6a0e8104-0b31-4883-b455-46fbc1183d62</v>
+        <v>0222f18f-7587-4801-83b6-6d7e76962b81</v>
       </c>
       <c r="B94" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C94" t="str">
-        <v>97108062-7918-4f7f-a3f7-92bcbc478acd</v>
+        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
       </c>
       <c r="D94">
         <v>4</v>
       </c>
       <c r="E94" t="str">
-        <v>B1</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>41d0a46c-55bf-42c7-a7c4-6581992f61c3</v>
+        <v>fd77b985-5669-4c99-8266-fe48862ad73a</v>
       </c>
       <c r="B95" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C95" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="D95">
         <v>4</v>
       </c>
       <c r="E95" t="str">
-        <v>B2</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>803aa685-24e1-4980-b321-08219eece77d</v>
+        <v>29c45ddd-6bc5-41f0-bb49-e45d878188a8</v>
       </c>
       <c r="B96" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C96" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
       </c>
       <c r="D96">
         <v>4</v>
       </c>
       <c r="E96" t="str">
-        <v>B3</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>0222f18f-7587-4801-83b6-6d7e76962b81</v>
+        <v>1a282447-a4a0-4793-bab3-23c5a357da0c</v>
       </c>
       <c r="B97" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C97" t="str">
-        <v>d4340206-46f8-4128-a64d-b1a7ca7bbdb5</v>
+        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
       </c>
       <c r="D97">
         <v>4</v>
       </c>
       <c r="E97" t="str">
-        <v>C1</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>fd77b985-5669-4c99-8266-fe48862ad73a</v>
+        <v>bc95cf9f-7c8c-4047-ad73-82ed7ac31f59</v>
       </c>
       <c r="B98" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C98" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
       </c>
       <c r="D98">
         <v>4</v>
       </c>
       <c r="E98" t="str">
-        <v>C2</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>29c45ddd-6bc5-41f0-bb49-e45d878188a8</v>
+        <v>d4e2f177-077a-4414-875c-d008e87b6517</v>
       </c>
       <c r="B99" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C99" t="str">
-        <v>feb78ceb-dd95-455d-8b7d-fc0019ae54c8</v>
+        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
       </c>
       <c r="D99">
         <v>4</v>
       </c>
       <c r="E99" t="str">
-        <v>C3</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>1a282447-a4a0-4793-bab3-23c5a357da0c</v>
+        <v>9b333e56-5752-4319-bf42-5123b15f41a0</v>
       </c>
       <c r="B100" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C100" t="str">
-        <v>d698b1de-6641-45c6-aa63-f577d2b634bb</v>
+        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
       </c>
       <c r="D100">
         <v>4</v>
       </c>
       <c r="E100" t="str">
-        <v>D1</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>bc95cf9f-7c8c-4047-ad73-82ed7ac31f59</v>
+        <v>57a18db4-3934-4e3b-b225-3bcbb301ccb0</v>
       </c>
       <c r="B101" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C101" t="str">
-        <v>0ccaf8bc-6ade-4ad6-9537-92f9829a6502</v>
+        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
       </c>
       <c r="D101">
         <v>4</v>
       </c>
       <c r="E101" t="str">
-        <v>D2</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>d4e2f177-077a-4414-875c-d008e87b6517</v>
+        <v>a4f70468-25c0-4e83-8200-b5a88ea81bb2</v>
       </c>
       <c r="B102" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C102" t="str">
-        <v>28603f95-d5f6-47ab-88c4-0d79742a6b02</v>
+        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
       </c>
       <c r="D102">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E102" t="str">
-        <v>D3</v>
+        <v>A1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>9b333e56-5752-4319-bf42-5123b15f41a0</v>
+        <v>adea01dd-088f-4ac8-87e7-5ee909db8c28</v>
       </c>
       <c r="B103" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C103" t="str">
-        <v>94116225-6732-4c15-9e4b-66f7727602d5</v>
+        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
       </c>
       <c r="D103">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E103" t="str">
-        <v>E1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>57a18db4-3934-4e3b-b225-3bcbb301ccb0</v>
+        <v>bbc61a88-7c16-472b-b9ca-6099d25d721e</v>
       </c>
       <c r="B104" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C104" t="str">
-        <v>22cf4684-eeba-4ed3-8f61-746028381f4d</v>
+        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
       </c>
       <c r="D104">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E104" t="str">
-        <v>E2</v>
+        <v>A3</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>a4f70468-25c0-4e83-8200-b5a88ea81bb2</v>
+        <v>815541ea-4e52-452e-86d7-46f16986b060</v>
       </c>
       <c r="B105" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C105" t="str">
-        <v>0fc0ae2d-4068-4972-a5b1-963c241e317a</v>
+        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
       </c>
       <c r="D105">
         <v>5</v>
       </c>
       <c r="E105" t="str">
-        <v>A1</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>adea01dd-088f-4ac8-87e7-5ee909db8c28</v>
+        <v>dd4f1361-aae2-4f6d-8e94-ba37f43e4d89</v>
       </c>
       <c r="B106" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C106" t="str">
-        <v>347bdea3-79f6-4991-9601-b2d86513429e</v>
+        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
       </c>
       <c r="D106">
         <v>5</v>
       </c>
       <c r="E106" t="str">
-        <v>A2</v>
+        <v>B1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>bbc61a88-7c16-472b-b9ca-6099d25d721e</v>
+        <v>5b94a741-673a-4116-a95d-a451421525ab</v>
       </c>
       <c r="B107" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C107" t="str">
-        <v>c9e05b47-6028-4cd1-b568-57342a489141</v>
+        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
       </c>
       <c r="D107">
         <v>5</v>
       </c>
       <c r="E107" t="str">
-        <v>A3</v>
+        <v>B2</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>815541ea-4e52-452e-86d7-46f16986b060</v>
+        <v>b6718d91-2f83-4455-8e0d-457c776c9101</v>
       </c>
       <c r="B108" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C108" t="str">
-        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
+        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
       </c>
       <c r="D108">
         <v>5</v>
       </c>
       <c r="E108" t="str">
-        <v>A4</v>
+        <v>B3</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>dd4f1361-aae2-4f6d-8e94-ba37f43e4d89</v>
+        <v>a2319e36-25b9-4901-95ca-7be604232784</v>
       </c>
       <c r="B109" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C109" t="str">
-        <v>94d903d4-dbc0-4052-87a8-ca32773ca839</v>
+        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
       </c>
       <c r="D109">
         <v>5</v>
       </c>
       <c r="E109" t="str">
-        <v>B1</v>
+        <v>B4</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>5b94a741-673a-4116-a95d-a451421525ab</v>
+        <v>69a00148-c195-41b6-b676-b37b911e0501</v>
       </c>
       <c r="B110" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C110" t="str">
-        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
+        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
       </c>
       <c r="D110">
         <v>5</v>
       </c>
       <c r="E110" t="str">
-        <v>B2</v>
+        <v>B5</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>b6718d91-2f83-4455-8e0d-457c776c9101</v>
+        <v>2e49d904-64ee-443c-aaca-9c63066a1f3f</v>
       </c>
       <c r="B111" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C111" t="str">
-        <v>5c31add6-7626-46c5-a3e1-0e452ead739d</v>
+        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
       </c>
       <c r="D111">
         <v>5</v>
       </c>
       <c r="E111" t="str">
-        <v>B3</v>
+        <v>C1</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>a2319e36-25b9-4901-95ca-7be604232784</v>
+        <v>fcbc1d59-1625-44fe-a710-b186b719e48e</v>
       </c>
       <c r="B112" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C112" t="str">
-        <v>a2ff3ad7-7964-4523-bf18-ce9994a910da</v>
+        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
       </c>
       <c r="D112">
         <v>5</v>
       </c>
       <c r="E112" t="str">
-        <v>B4</v>
+        <v>C2</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>69a00148-c195-41b6-b676-b37b911e0501</v>
+        <v>29b71713-fa5d-47a8-bad9-80d7eb24caeb</v>
       </c>
       <c r="B113" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C113" t="str">
-        <v>939eed5c-b520-4a34-8d08-2243d6aa41c1</v>
+        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
       </c>
       <c r="D113">
         <v>5</v>
       </c>
       <c r="E113" t="str">
-        <v>B5</v>
+        <v>C3</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>2e49d904-64ee-443c-aaca-9c63066a1f3f</v>
+        <v>fb0d2557-0d04-4f3b-a255-591ab6025b2e</v>
       </c>
       <c r="B114" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C114" t="str">
-        <v>cd648690-8cd1-44b6-be26-0521038f442f</v>
+        <v>9f873871-29cc-45f0-894c-c54745230689</v>
       </c>
       <c r="D114">
         <v>5</v>
       </c>
       <c r="E114" t="str">
-        <v>C1</v>
+        <v>C4</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>fcbc1d59-1625-44fe-a710-b186b719e48e</v>
+        <v>59c9d82b-5fe5-4222-9451-4aeca52fbe4c</v>
       </c>
       <c r="B115" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C115" t="str">
-        <v>bf283832-25b8-4d7f-9e0f-ef2f10903233</v>
+        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
       </c>
       <c r="D115">
         <v>5</v>
       </c>
       <c r="E115" t="str">
-        <v>C2</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>29b71713-fa5d-47a8-bad9-80d7eb24caeb</v>
+        <v>4bd1651a-6337-4459-b562-22f49804881e</v>
       </c>
       <c r="B116" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C116" t="str">
-        <v>7728eead-ab7c-467f-bb41-2abd7952591a</v>
+        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
       </c>
       <c r="D116">
         <v>5</v>
       </c>
       <c r="E116" t="str">
-        <v>C3</v>
+        <v>D2</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>fb0d2557-0d04-4f3b-a255-591ab6025b2e</v>
+        <v>76361c32-4730-4a80-85c7-d8527a983168</v>
       </c>
       <c r="B117" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C117" t="str">
-        <v>9f873871-29cc-45f0-894c-c54745230689</v>
+        <v>076ad666-a34b-4ae1-b91f-de785dbdf5ec</v>
       </c>
       <c r="D117">
         <v>5</v>
       </c>
       <c r="E117" t="str">
-        <v>C4</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>59c9d82b-5fe5-4222-9451-4aeca52fbe4c</v>
+        <v>ac5f6dff-c75f-4064-bbff-c02af8506b49</v>
       </c>
       <c r="B118" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C118" t="str">
-        <v>410dbe34-810b-4a5d-8731-985738541b4b</v>
+        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
       </c>
       <c r="D118">
         <v>5</v>
       </c>
       <c r="E118" t="str">
-        <v>D1</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>4bd1651a-6337-4459-b562-22f49804881e</v>
+        <v>be8f0518-0a03-477b-bc47-6339f48138b7</v>
       </c>
       <c r="B119" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C119" t="str">
-        <v>700fc657-988b-4d49-9814-25b1df35cefc</v>
+        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
       </c>
       <c r="D119">
         <v>5</v>
       </c>
       <c r="E119" t="str">
-        <v>D2</v>
+        <v>E1</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>76361c32-4730-4a80-85c7-d8527a983168</v>
+        <v>4ff7518f-d926-4281-8920-473d76a91b19</v>
       </c>
       <c r="B120" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C120" t="str">
-        <v>076ad666-a34b-4ae1-b91f-de785dbdf5ec</v>
+        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
       </c>
       <c r="D120">
         <v>5</v>
       </c>
       <c r="E120" t="str">
-        <v>D3</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>ac5f6dff-c75f-4064-bbff-c02af8506b49</v>
+        <v>5a3eb837-9cc6-4e24-b138-1c56478bf199</v>
       </c>
       <c r="B121" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C121" t="str">
-        <v>0e8f635e-8f06-4224-a2cc-4263ac307ba2</v>
+        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
       </c>
       <c r="D121">
         <v>5</v>
       </c>
       <c r="E121" t="str">
-        <v>D4</v>
+        <v>E3</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>be8f0518-0a03-477b-bc47-6339f48138b7</v>
+        <v>47b50888-f2ee-4542-8d26-fd291becaf39</v>
       </c>
       <c r="B122" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C122" t="str">
-        <v>59bae9a1-93b9-471d-a2b7-074918634f6b</v>
+        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
       </c>
       <c r="D122">
         <v>5</v>
       </c>
       <c r="E122" t="str">
-        <v>E1</v>
+        <v>E4</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>4ff7518f-d926-4281-8920-473d76a91b19</v>
+        <v>4edebf2c-170e-4642-b349-bf2c638e5869</v>
       </c>
       <c r="B123" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C123" t="str">
-        <v>39b7a0a4-be8b-49f1-a5af-c5a105e0ab58</v>
+        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
       </c>
       <c r="D123">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E123" t="str">
-        <v>E2</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="str">
-        <v>5a3eb837-9cc6-4e24-b138-1c56478bf199</v>
-      </c>
-      <c r="B124" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C124" t="str">
-        <v>a8fa9125-28f1-47e1-adba-784701975e68</v>
-      </c>
-      <c r="D124">
-        <v>5</v>
-      </c>
-      <c r="E124" t="str">
-        <v>E3</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="str">
-        <v>47b50888-f2ee-4542-8d26-fd291becaf39</v>
-      </c>
-      <c r="B125" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C125" t="str">
-        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
-      </c>
-      <c r="D125">
-        <v>5</v>
-      </c>
-      <c r="E125" t="str">
-        <v>E4</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="str">
-        <v>4edebf2c-170e-4642-b349-bf2c638e5869</v>
-      </c>
-      <c r="B126" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C126" t="str">
-        <v>dc8716d3-5841-439f-a3e4-3e7bd8306e66</v>
-      </c>
-      <c r="D126">
-        <v>6</v>
-      </c>
-      <c r="E126" t="str">
         <v>A1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H126"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H123"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -15050,7 +14999,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -15089,44 +15038,61 @@
         <v>46001.254457083334</v>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
+    <row r="3">
       <c r="A3" t="str">
-        <v>fa4948a9-b0d8-40b2-a711-a69c078b430f</v>
+        <v>8408c349-ac9b-49ab-989d-44cfabae6ca5</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
+        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
+      </c>
+      <c r="D3" t="str">
+        <v>.</v>
+      </c>
+      <c r="E3" s="1">
+        <v>46004.18743818287</v>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4" t="str">
+        <v>fa4948a9-b0d8-40b2-a711-a69c078b430f</v>
+      </c>
+      <c r="B4" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C4" t="str">
         <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
       </c>
-      <c r="D3" t="str" xml:space="preserve">
+      <c r="D4" t="str" xml:space="preserve">
         <v xml:space="preserve">Rebook from March
 </v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <v>46003.218646828704</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
+    <row r="5">
+      <c r="A5" t="str">
         <v>95999c56-5e18-4ae1-a665-5628a8b3082b</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B5" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C5" t="str">
         <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D5" t="str">
         <v>Standby - eligible for reschedule</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E5" s="1">
         <v>46001.26070648148</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improve contestant selection and seating chart experience
Introduces a searchable contestant selection dialog with filtering and sorting, enhances the seating chart page with new icons and UI elements, and updates backup data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 351416c7-debb-45a6-b46a-f995a2c14a22
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/HqzwbpC
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -13187,36 +13187,36 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>bc22ad22-1b7c-446d-8cd9-8d1a90cafebd</v>
+        <v>96ecc4ef-fd63-4393-b7df-9423b5df0868</v>
       </c>
       <c r="B48" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C48" t="str">
-        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="str">
-        <v>E4</v>
+        <v>D3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>96ecc4ef-fd63-4393-b7df-9423b5df0868</v>
+        <v>bc22ad22-1b7c-446d-8cd9-8d1a90cafebd</v>
       </c>
       <c r="B49" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C49" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="str">
-        <v>E3</v>
+        <v>D4</v>
       </c>
     </row>
     <row r="50">

</xml_diff>

<commit_message>
Improve database connection stability and prevent application crashes
Add error handling to the database connection pool in `server/db.ts` to gracefully manage Neon serverless idle timeouts and prevent application crashes. Update `storage/backups/automatic-backup.json` with new `exportedAt` timestamp and modified contestant/record day data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ce9a873d-9cff-405e-afae-b69c7d597a39
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 05908455-f60c-460e-9c99-a58f92a7cded
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/ce9a873d-9cff-405e-afae-b69c7d597a39/65cMUpb
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -12545,36 +12545,36 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>0b9e3538-2d1f-4380-8f25-a1d785645eee</v>
+        <v>6d85f4a7-815e-4c53-b08f-c5a65723bdfa</v>
       </c>
       <c r="B14" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C14" t="str">
-        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
+        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="str">
-        <v>E1</v>
+        <v>E4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>6d85f4a7-815e-4c53-b08f-c5a65723bdfa</v>
+        <v>0b9e3538-2d1f-4380-8f25-a1d785645eee</v>
       </c>
       <c r="B15" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C15" t="str">
-        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
+        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="str">
-        <v>E2</v>
+        <v>E3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add customizable email content and update appearance for availability management
Introduces editable email subject, headline, intro, instructions, button text, and footer in availability management. Updates the availability response page with a Deal or No Deal aesthetic, including custom background gradients and title styling. Modifies the server route to accept and use these new email content fields, alongside logic for dynamically fetching and embedding banner images into the email template. Also includes adjustments to the backup file and seat label data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f123b9d7-6af8-472a-a75c-70d0b78d0583
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: 269c51cf-7774-4f44-99c6-bc04c380fd4e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/f123b9d7-6af8-472a-a75c-70d0b78d0583/saP9O0O
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -12494,33 +12494,33 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>b55d9cdb-874f-4133-91b3-10f1ac5810e2</v>
+        <v>d1ab6da5-7837-4eef-8547-ea7ff17f58c3</v>
       </c>
       <c r="B11" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C11" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="str">
-        <v>D3</v>
+        <v>D1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>bc9f9233-1d8e-4fc9-9d80-21737c57f5f6</v>
+        <v>28f83ab1-3a7e-4e9b-82bf-7e37383d13ff</v>
       </c>
       <c r="B12" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C12" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="str">
         <v>D2</v>
@@ -12528,53 +12528,53 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>ba25a5c3-0c4c-42fb-a6cf-8891cc5befd8</v>
+        <v>b55d9cdb-874f-4133-91b3-10f1ac5810e2</v>
       </c>
       <c r="B13" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C13" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="str">
-        <v>D1</v>
+        <v>E3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>d1ab6da5-7837-4eef-8547-ea7ff17f58c3</v>
+        <v>bc9f9233-1d8e-4fc9-9d80-21737c57f5f6</v>
       </c>
       <c r="B14" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C14" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="str">
-        <v>D1</v>
+        <v>E2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>28f83ab1-3a7e-4e9b-82bf-7e37383d13ff</v>
+        <v>ba25a5c3-0c4c-42fb-a6cf-8891cc5befd8</v>
       </c>
       <c r="B15" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C15" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
+        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" t="str">
-        <v>D2</v>
+        <v>E1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a checkbox column to track paperwork completion on the day of the event
Introduces the `paperworkOnDay` timestamp field to the `seat_assignments` table and updates the `BookingMaster` component in the frontend to display and manage this new column with a distinct visual style.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f123b9d7-6af8-472a-a75c-70d0b78d0583
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: db0cfd0b-1cbf-49c6-9aff-88e8ecf1a825
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/f123b9d7-6af8-472a-a75c-70d0b78d0583/97roLxs
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,11 +5,10 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
-    <sheet name="Groups" sheetId="5" r:id="rId5"/>
-    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
-    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
+    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -1817,165 +1816,168 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
+        <v>2e7a82a4-998c-4f82-a686-5a4d0bcc725b</v>
       </c>
       <c r="B33" t="str">
-        <v>Ella Gutierrez</v>
+        <v>Jessica Newton</v>
       </c>
       <c r="C33">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D33" t="str">
         <v>Female</v>
       </c>
       <c r="E33" t="str">
-        <v>ella.gutierrez43@gmail.com</v>
+        <v>jessicamareenewton@gmail.com</v>
       </c>
       <c r="F33" t="str">
-        <v>(220) 105-1876</v>
+        <v>403316735</v>
       </c>
       <c r="G33" t="str">
-        <v>Irvine</v>
+        <v xml:space="preserve">Melbourne </v>
       </c>
       <c r="H33" t="str">
         <v>B</v>
       </c>
       <c r="I33" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J33" t="str">
-        <v>Nora Lee</v>
+        <v>Carl Mikhail SEVILLANO, Jessica Newton, Carolina Sevillano, Manuel Sevillano</v>
+      </c>
+      <c r="K33" t="str">
+        <v>23259da3-85da-4d69-a2bc-f1e643c3e4a5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>2e7a82a4-998c-4f82-a686-5a4d0bcc725b</v>
+        <v>bf0f24b8-c7b2-4c41-8bbe-993b8806c243</v>
       </c>
       <c r="B34" t="str">
-        <v>Jessica Newton</v>
+        <v>Chloe Wilson</v>
       </c>
       <c r="C34">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D34" t="str">
         <v>Female</v>
       </c>
       <c r="E34" t="str">
-        <v>jessicamareenewton@gmail.com</v>
+        <v>chloeshaniawilson@hotmail.com</v>
       </c>
       <c r="F34" t="str">
-        <v>403316735</v>
+        <v>439717876</v>
       </c>
       <c r="G34" t="str">
-        <v xml:space="preserve">Melbourne </v>
+        <v xml:space="preserve">Mount clear </v>
       </c>
       <c r="H34" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I34" t="str">
         <v>available</v>
       </c>
       <c r="J34" t="str">
-        <v>Carl Mikhail SEVILLANO, Jessica Newton, Carolina Sevillano, Manuel Sevillano</v>
+        <v>Jayne Parkinson</v>
       </c>
       <c r="K34" t="str">
-        <v>23259da3-85da-4d69-a2bc-f1e643c3e4a5</v>
+        <v>1d8a7e45-0b40-4677-bf88-ed8c29eb0e03</v>
+      </c>
+      <c r="M34" t="str">
+        <v>NA</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>bf0f24b8-c7b2-4c41-8bbe-993b8806c243</v>
+        <v>7e5c8e3d-1708-4b56-b262-e6c2743e4865</v>
       </c>
       <c r="B35" t="str">
-        <v>Chloe Wilson</v>
+        <v>Christian  Veri</v>
       </c>
       <c r="C35">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D35" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E35" t="str">
-        <v>chloeshaniawilson@hotmail.com</v>
+        <v>christian.veri04@gmail.com</v>
       </c>
       <c r="F35" t="str">
-        <v>439717876</v>
+        <v>490766823</v>
       </c>
       <c r="G35" t="str">
-        <v xml:space="preserve">Mount clear </v>
+        <v>Melbourne</v>
       </c>
       <c r="H35" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I35" t="str">
         <v>available</v>
       </c>
       <c r="J35" t="str">
-        <v>Jayne Parkinson</v>
+        <v>Christian Veri, Natasha Veri, Frank Veri, Gianna Veri</v>
       </c>
       <c r="K35" t="str">
-        <v>1d8a7e45-0b40-4677-bf88-ed8c29eb0e03</v>
-      </c>
-      <c r="M35" t="str">
-        <v>NA</v>
+        <v>5414f8e6-7fb4-4979-abf0-151495e1cfff</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>7e5c8e3d-1708-4b56-b262-e6c2743e4865</v>
+        <v>1b90e38c-6849-41d7-8b76-6e886b542be5</v>
       </c>
       <c r="B36" t="str">
-        <v>Christian  Veri</v>
+        <v>Nermina Malic</v>
       </c>
       <c r="C36">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="D36" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E36" t="str">
-        <v>christian.veri04@gmail.com</v>
+        <v>n.malic@hotmail.com</v>
       </c>
       <c r="F36" t="str">
-        <v>490766823</v>
+        <v>431480024</v>
       </c>
       <c r="G36" t="str">
-        <v>Melbourne</v>
+        <v>Altona meadows</v>
       </c>
       <c r="H36" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I36" t="str">
         <v>available</v>
       </c>
       <c r="J36" t="str">
-        <v>Christian Veri, Natasha Veri, Frank Veri, Gianna Veri</v>
+        <v>Ivana Pavic</v>
       </c>
       <c r="K36" t="str">
-        <v>5414f8e6-7fb4-4979-abf0-151495e1cfff</v>
+        <v>d7082c1c-800b-4072-8c4c-6b07681145f4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>1b90e38c-6849-41d7-8b76-6e886b542be5</v>
+        <v>5d5e3785-ca4f-4312-96ff-4a0d79884a70</v>
       </c>
       <c r="B37" t="str">
-        <v>Nermina Malic</v>
+        <v>Charlotte Rowson</v>
       </c>
       <c r="C37">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D37" t="str">
         <v>Female</v>
       </c>
       <c r="E37" t="str">
-        <v>n.malic@hotmail.com</v>
+        <v>rowschar@gmail.com</v>
       </c>
       <c r="F37" t="str">
-        <v>431480024</v>
+        <v>426195518</v>
       </c>
       <c r="G37" t="str">
-        <v>Altona meadows</v>
+        <v>Abbotsford</v>
       </c>
       <c r="H37" t="str">
         <v>B+</v>
@@ -1984,33 +1986,36 @@
         <v>available</v>
       </c>
       <c r="J37" t="str">
-        <v>Ivana Pavic</v>
+        <v>Madison Bartholomew</v>
       </c>
       <c r="K37" t="str">
-        <v>d7082c1c-800b-4072-8c4c-6b07681145f4</v>
+        <v>ba7c8f2a-7027-4b21-9a88-82709f083acb</v>
+      </c>
+      <c r="M37" t="str">
+        <v>NA</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>5d5e3785-ca4f-4312-96ff-4a0d79884a70</v>
+        <v>6c100962-ee82-41d1-afdf-6810823ea88e</v>
       </c>
       <c r="B38" t="str">
-        <v>Charlotte Rowson</v>
+        <v>Madeleine  Floros</v>
       </c>
       <c r="C38">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D38" t="str">
         <v>Female</v>
       </c>
       <c r="E38" t="str">
-        <v>rowschar@gmail.com</v>
+        <v>mfloros@y7mail.com</v>
       </c>
       <c r="F38" t="str">
-        <v>426195518</v>
+        <v>413533385</v>
       </c>
       <c r="G38" t="str">
-        <v>Abbotsford</v>
+        <v>Bundoora</v>
       </c>
       <c r="H38" t="str">
         <v>B+</v>
@@ -2019,68 +2024,68 @@
         <v>available</v>
       </c>
       <c r="J38" t="str">
-        <v>Madison Bartholomew</v>
+        <v>Claudia Floros</v>
       </c>
       <c r="K38" t="str">
-        <v>ba7c8f2a-7027-4b21-9a88-82709f083acb</v>
-      </c>
-      <c r="M38" t="str">
-        <v>NA</v>
+        <v>d31fd676-cd74-4239-9827-4bfd973cc237</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
+        <v>2d64b97f-64bb-4190-abdf-5a2a9d37c810</v>
       </c>
       <c r="B39" t="str">
-        <v>Naomi Moore</v>
+        <v>Wendy  Manton</v>
       </c>
       <c r="C39">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D39" t="str">
         <v>Female</v>
       </c>
       <c r="E39" t="str">
-        <v>naomi.moore30@gmail.com</v>
+        <v>wendymantonxo7@gmail.com</v>
       </c>
       <c r="F39" t="str">
-        <v>(391) 998-1729</v>
+        <v>439858211</v>
       </c>
       <c r="G39" t="str">
-        <v>Irvine</v>
+        <v xml:space="preserve">Melbourne </v>
       </c>
       <c r="H39" t="str">
         <v>B</v>
       </c>
       <c r="I39" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J39" t="str">
-        <v>Isla Wright, Cora Roberts</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>Jodi Kett</v>
+      </c>
+      <c r="K39" t="str">
+        <v>cbf209b8-2a31-4cf9-bc54-83485fa4051d</v>
+      </c>
+    </row>
+    <row r="40" xml:space="preserve">
       <c r="A40" t="str">
-        <v>6c100962-ee82-41d1-afdf-6810823ea88e</v>
+        <v>4f8c4348-e7af-42bc-93d9-bdf0b8e1585e</v>
       </c>
       <c r="B40" t="str">
-        <v>Madeleine  Floros</v>
+        <v>SOPHIE ARMES</v>
       </c>
       <c r="C40">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="D40" t="str">
         <v>Female</v>
       </c>
       <c r="E40" t="str">
-        <v>mfloros@y7mail.com</v>
+        <v>sophievaudeleau@hotmail.com</v>
       </c>
       <c r="F40" t="str">
-        <v>413533385</v>
+        <v>401235498</v>
       </c>
       <c r="G40" t="str">
-        <v>Bundoora</v>
+        <v>HIGHTON</v>
       </c>
       <c r="H40" t="str">
         <v>B+</v>
@@ -2088,218 +2093,212 @@
       <c r="I40" t="str">
         <v>available</v>
       </c>
-      <c r="J40" t="str">
-        <v>Claudia Floros</v>
-      </c>
-      <c r="K40" t="str">
-        <v>d31fd676-cd74-4239-9827-4bfd973cc237</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>2d64b97f-64bb-4190-abdf-5a2a9d37c810</v>
-      </c>
-      <c r="B41" t="str">
-        <v>Wendy  Manton</v>
-      </c>
-      <c r="C41">
-        <v>67</v>
-      </c>
-      <c r="D41" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E41" t="str">
-        <v>wendymantonxo7@gmail.com</v>
-      </c>
-      <c r="F41" t="str">
-        <v>439858211</v>
-      </c>
-      <c r="G41" t="str">
-        <v xml:space="preserve">Melbourne </v>
-      </c>
-      <c r="H41" t="str">
-        <v>B</v>
-      </c>
-      <c r="I41" t="str">
-        <v>available</v>
-      </c>
-      <c r="J41" t="str">
-        <v>Jodi Kett</v>
-      </c>
-      <c r="K41" t="str">
-        <v>cbf209b8-2a31-4cf9-bc54-83485fa4051d</v>
-      </c>
-    </row>
-    <row r="42" xml:space="preserve">
-      <c r="A42" t="str">
-        <v>4f8c4348-e7af-42bc-93d9-bdf0b8e1585e</v>
-      </c>
-      <c r="B42" t="str">
-        <v>SOPHIE ARMES</v>
-      </c>
-      <c r="C42">
-        <v>54</v>
-      </c>
-      <c r="D42" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E42" t="str">
-        <v>sophievaudeleau@hotmail.com</v>
-      </c>
-      <c r="F42" t="str">
-        <v>401235498</v>
-      </c>
-      <c r="G42" t="str">
-        <v>HIGHTON</v>
-      </c>
-      <c r="H42" t="str">
-        <v>B+</v>
-      </c>
-      <c r="I42" t="str">
-        <v>available</v>
-      </c>
-      <c r="J42" t="str" xml:space="preserve">
+      <c r="J40" t="str" xml:space="preserve">
         <v xml:space="preserve">Sophie Armes - Player_x000d_
 Edward Armes - Son_x000d_
 Pamela Stone - Friend_x000d_
 Sheila Hawe - Friend_x000d_
 </v>
       </c>
-      <c r="K42" t="str">
+      <c r="K40" t="str">
         <v>d64a0044-98eb-47c9-a610-f16b009bfcb4</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="str">
+    <row r="41">
+      <c r="A41" t="str">
         <v>4c6757f5-c98a-41a1-bc6f-783d02a7e884</v>
       </c>
-      <c r="B43" t="str">
+      <c r="B41" t="str">
         <v>Matthew Bailey</v>
       </c>
-      <c r="C43">
+      <c r="C41">
         <v>38</v>
       </c>
-      <c r="D43" t="str">
-        <v>Male</v>
-      </c>
-      <c r="E43" t="str">
+      <c r="D41" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E41" t="str">
         <v>m.bailey23@hotmail.com</v>
       </c>
-      <c r="F43" t="str">
+      <c r="F41" t="str">
         <v>423462472</v>
       </c>
-      <c r="G43" t="str">
+      <c r="G41" t="str">
         <v>Craigieburn</v>
       </c>
-      <c r="H43" t="str">
-        <v>B+</v>
-      </c>
-      <c r="I43" t="str">
-        <v>available</v>
-      </c>
-      <c r="J43" t="str">
+      <c r="H41" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I41" t="str">
+        <v>available</v>
+      </c>
+      <c r="J41" t="str">
         <v>matthew bailey, simone bailey</v>
       </c>
-      <c r="K43" t="str">
+      <c r="K41" t="str">
         <v>0d1c49df-1962-42f1-9457-855ef54578e6</v>
       </c>
     </row>
-    <row r="44" xml:space="preserve">
-      <c r="A44" t="str">
+    <row r="42" xml:space="preserve">
+      <c r="A42" t="str">
         <v>7ef0a863-f193-4ea2-b6b1-9f6990d9c72b</v>
       </c>
-      <c r="B44" t="str">
+      <c r="B42" t="str">
         <v>EDWARD Armes</v>
       </c>
-      <c r="C44">
+      <c r="C42">
         <v>21</v>
       </c>
-      <c r="D44" t="str">
-        <v>Male</v>
-      </c>
-      <c r="E44" t="str">
+      <c r="D42" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E42" t="str">
         <v>edarmes99@gmail.com</v>
       </c>
-      <c r="F44" t="str">
+      <c r="F42" t="str">
         <v>439861309</v>
       </c>
-      <c r="G44" t="str">
+      <c r="G42" t="str">
         <v xml:space="preserve">Geelong </v>
       </c>
-      <c r="H44" t="str">
-        <v>B+</v>
-      </c>
-      <c r="I44" t="str">
-        <v>available</v>
-      </c>
-      <c r="J44" t="str" xml:space="preserve">
+      <c r="H42" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I42" t="str">
+        <v>available</v>
+      </c>
+      <c r="J42" t="str" xml:space="preserve">
         <v xml:space="preserve">Sophie Armes - Player_x000d_
 Edward Armes - Son_x000d_
 Pamela Stone - Friend_x000d_
 Sheila Hawe - Friend</v>
       </c>
-      <c r="K44" t="str">
+      <c r="K42" t="str">
         <v>d64a0044-98eb-47c9-a610-f16b009bfcb4</v>
       </c>
     </row>
-    <row r="45" xml:space="preserve">
-      <c r="A45" t="str">
+    <row r="43" xml:space="preserve">
+      <c r="A43" t="str">
         <v>fe448c1e-878b-4ce5-b11f-de34f1d7ad19</v>
       </c>
-      <c r="B45" t="str">
+      <c r="B43" t="str">
         <v>Antigoni  Simmons</v>
       </c>
-      <c r="C45">
+      <c r="C43">
         <v>34</v>
       </c>
-      <c r="D45" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E45" t="str">
+      <c r="D43" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E43" t="str">
         <v>antigoni_trianta@outlook.com</v>
       </c>
-      <c r="F45" t="str">
+      <c r="F43" t="str">
         <v>431186284</v>
       </c>
-      <c r="G45" t="str">
+      <c r="G43" t="str">
         <v xml:space="preserve">Melbourne </v>
       </c>
-      <c r="H45" t="str">
-        <v>B+</v>
-      </c>
-      <c r="I45" t="str">
-        <v>available</v>
-      </c>
-      <c r="J45" t="str" xml:space="preserve">
+      <c r="H43" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I43" t="str">
+        <v>available</v>
+      </c>
+      <c r="J43" t="str" xml:space="preserve">
         <v xml:space="preserve">Jamie Simmons - Needs to Apply_x000d_
 Alex Triantafylidis - Mum (tri-anta-fell-ease)_x000d_
 </v>
       </c>
-      <c r="K45" t="str">
+      <c r="K43" t="str">
         <v>b24e1d25-603c-49cb-97d3-f44db7487a00</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>acb3e630-d526-4057-b545-aa192312bdbd</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Tejas Deshmukh</v>
+      </c>
+      <c r="C44">
+        <v>35</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E44" t="str">
+        <v>arch.tejasd@gmail.com</v>
+      </c>
+      <c r="F44" t="str">
+        <v>481988781</v>
+      </c>
+      <c r="G44" t="str">
+        <v>Melton South</v>
+      </c>
+      <c r="H44" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I44" t="str">
+        <v>available</v>
+      </c>
+      <c r="J44" t="str">
+        <v>Tejas Deshmukh, Chaitali Bhanushali</v>
+      </c>
+      <c r="K44" t="str">
+        <v>ea07ea19-44f5-4443-8d44-890ef7a5078a</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>47072c44-a802-4d24-962c-1654f4e2b639</v>
+      </c>
+      <c r="B45" t="str">
+        <v>gaylene piscopo</v>
+      </c>
+      <c r="C45">
+        <v>22</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E45" t="str">
+        <v>gayleneeepiscopo03@gmail.com</v>
+      </c>
+      <c r="F45" t="str">
+        <v>499626264</v>
+      </c>
+      <c r="G45" t="str">
+        <v>Victoria</v>
+      </c>
+      <c r="H45" t="str">
+        <v>B</v>
+      </c>
+      <c r="I45" t="str">
+        <v>available</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>acb3e630-d526-4057-b545-aa192312bdbd</v>
+        <v>712e4c3c-2bc9-486c-9fd0-42ce55f8247f</v>
       </c>
       <c r="B46" t="str">
-        <v>Tejas Deshmukh</v>
+        <v>Kellie Fefelic</v>
       </c>
       <c r="C46">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D46" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E46" t="str">
-        <v>arch.tejasd@gmail.com</v>
+        <v>kemalafelic@gmail.com</v>
       </c>
       <c r="F46" t="str">
-        <v>481988781</v>
+        <v>452090905</v>
       </c>
       <c r="G46" t="str">
-        <v>Melton South</v>
+        <v>Mornington</v>
       </c>
       <c r="H46" t="str">
         <v>B+</v>
@@ -2308,36 +2307,39 @@
         <v>available</v>
       </c>
       <c r="J46" t="str">
-        <v>Tejas Deshmukh, Chaitali Bhanushali</v>
+        <v>Philip Heywood</v>
       </c>
       <c r="K46" t="str">
-        <v>ea07ea19-44f5-4443-8d44-890ef7a5078a</v>
+        <v>54189d4e-7afc-4225-a6cb-28a8fff1a856</v>
+      </c>
+      <c r="M46" t="str">
+        <v>NA</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>47072c44-a802-4d24-962c-1654f4e2b639</v>
+        <v>1cfa5805-2855-4ff9-9175-697120cf327a</v>
       </c>
       <c r="B47" t="str">
-        <v>gaylene piscopo</v>
+        <v>Abrar Musa</v>
       </c>
       <c r="C47">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D47" t="str">
         <v>Female</v>
       </c>
       <c r="E47" t="str">
-        <v>gayleneeepiscopo03@gmail.com</v>
+        <v>abrarmusa459@gmail.com</v>
       </c>
       <c r="F47" t="str">
-        <v>499626264</v>
+        <v>412610736</v>
       </c>
       <c r="G47" t="str">
-        <v>Victoria</v>
+        <v>SPRINGVALE SOUTH</v>
       </c>
       <c r="H47" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I47" t="str">
         <v>available</v>
@@ -2345,25 +2347,25 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>712e4c3c-2bc9-486c-9fd0-42ce55f8247f</v>
+        <v>3a3ae62d-7e17-46a1-b4ca-f3edde675c9a</v>
       </c>
       <c r="B48" t="str">
-        <v>Kellie Fefelic</v>
+        <v>Huda Hayek</v>
       </c>
       <c r="C48">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D48" t="str">
         <v>Female</v>
       </c>
       <c r="E48" t="str">
-        <v>kemalafelic@gmail.com</v>
+        <v>Huda_hayek@yahoo.com.au</v>
       </c>
       <c r="F48" t="str">
-        <v>452090905</v>
+        <v>413787207</v>
       </c>
       <c r="G48" t="str">
-        <v>Mornington</v>
+        <v xml:space="preserve">Melbourne </v>
       </c>
       <c r="H48" t="str">
         <v>B+</v>
@@ -2372,10 +2374,10 @@
         <v>available</v>
       </c>
       <c r="J48" t="str">
-        <v>Philip Heywood</v>
+        <v>Fadey Souied</v>
       </c>
       <c r="K48" t="str">
-        <v>54189d4e-7afc-4225-a6cb-28a8fff1a856</v>
+        <v>1edf8348-87ac-4690-a22c-ef5721f32b81</v>
       </c>
       <c r="M48" t="str">
         <v>NA</v>
@@ -2383,54 +2385,60 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>1cfa5805-2855-4ff9-9175-697120cf327a</v>
+        <v>11ad6470-961f-4c41-9474-0159c23c81bd</v>
       </c>
       <c r="B49" t="str">
-        <v>Abrar Musa</v>
+        <v>Caron Miller</v>
       </c>
       <c r="C49">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="D49" t="str">
         <v>Female</v>
       </c>
       <c r="E49" t="str">
-        <v>abrarmusa459@gmail.com</v>
+        <v>mistyjasper@hotmail.com</v>
       </c>
       <c r="F49" t="str">
-        <v>412610736</v>
+        <v>417331948</v>
       </c>
       <c r="G49" t="str">
-        <v>SPRINGVALE SOUTH</v>
+        <v>Narre Warren East</v>
       </c>
       <c r="H49" t="str">
         <v>B+</v>
       </c>
       <c r="I49" t="str">
         <v>available</v>
+      </c>
+      <c r="J49" t="str">
+        <v>Victoria Morrison</v>
+      </c>
+      <c r="K49" t="str">
+        <v>bc5440fa-e979-4a58-9300-e0349edf8d54</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>3a3ae62d-7e17-46a1-b4ca-f3edde675c9a</v>
+        <v>cff9458b-cbd8-491e-9a5f-2171891b3f66</v>
       </c>
       <c r="B50" t="str">
-        <v>Huda Hayek</v>
+        <v>Shana Kent</v>
       </c>
       <c r="C50">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D50" t="str">
         <v>Female</v>
       </c>
       <c r="E50" t="str">
-        <v>Huda_hayek@yahoo.com.au</v>
+        <v>banna12sk@hotmail.com</v>
       </c>
       <c r="F50" t="str">
-        <v>413787207</v>
+        <v>408333616</v>
       </c>
       <c r="G50" t="str">
-        <v xml:space="preserve">Melbourne </v>
+        <v xml:space="preserve">Hurstbridge </v>
       </c>
       <c r="H50" t="str">
         <v>B+</v>
@@ -2439,36 +2447,33 @@
         <v>available</v>
       </c>
       <c r="J50" t="str">
-        <v>Fadey Souied</v>
+        <v>Daughter - Emma Kent.  - needs to apply</v>
       </c>
       <c r="K50" t="str">
-        <v>1edf8348-87ac-4690-a22c-ef5721f32b81</v>
-      </c>
-      <c r="M50" t="str">
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>96b83e8d-93db-4d09-9d4f-2398e8c44538</v>
+      </c>
+    </row>
+    <row r="51" xml:space="preserve">
       <c r="A51" t="str">
-        <v>11ad6470-961f-4c41-9474-0159c23c81bd</v>
+        <v>32b624eb-d8d0-4725-b366-f8c07b803eee</v>
       </c>
       <c r="B51" t="str">
-        <v>Caron Miller</v>
+        <v>amy milbourne</v>
       </c>
       <c r="C51">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="D51" t="str">
         <v>Female</v>
       </c>
       <c r="E51" t="str">
-        <v>mistyjasper@hotmail.com</v>
+        <v>amy.milbourne005@gmail.com</v>
       </c>
       <c r="F51" t="str">
-        <v>417331948</v>
+        <v>474656699</v>
       </c>
       <c r="G51" t="str">
-        <v>Narre Warren East</v>
+        <v>haven</v>
       </c>
       <c r="H51" t="str">
         <v>B+</v>
@@ -2476,119 +2481,113 @@
       <c r="I51" t="str">
         <v>available</v>
       </c>
-      <c r="J51" t="str">
-        <v>Victoria Morrison</v>
-      </c>
-      <c r="K51" t="str">
-        <v>bc5440fa-e979-4a58-9300-e0349edf8d54</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="str">
-        <v>cff9458b-cbd8-491e-9a5f-2171891b3f66</v>
-      </c>
-      <c r="B52" t="str">
-        <v>Shana Kent</v>
-      </c>
-      <c r="C52">
-        <v>45</v>
-      </c>
-      <c r="D52" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E52" t="str">
-        <v>banna12sk@hotmail.com</v>
-      </c>
-      <c r="F52" t="str">
-        <v>408333616</v>
-      </c>
-      <c r="G52" t="str">
-        <v xml:space="preserve">Hurstbridge </v>
-      </c>
-      <c r="H52" t="str">
-        <v>B+</v>
-      </c>
-      <c r="I52" t="str">
-        <v>available</v>
-      </c>
-      <c r="J52" t="str">
-        <v>Daughter - Emma Kent.  - needs to apply</v>
-      </c>
-      <c r="K52" t="str">
-        <v>96b83e8d-93db-4d09-9d4f-2398e8c44538</v>
-      </c>
-    </row>
-    <row r="53" xml:space="preserve">
-      <c r="A53" t="str">
-        <v>32b624eb-d8d0-4725-b366-f8c07b803eee</v>
-      </c>
-      <c r="B53" t="str">
-        <v>amy milbourne</v>
-      </c>
-      <c r="C53">
-        <v>20</v>
-      </c>
-      <c r="D53" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E53" t="str">
-        <v>amy.milbourne005@gmail.com</v>
-      </c>
-      <c r="F53" t="str">
-        <v>474656699</v>
-      </c>
-      <c r="G53" t="str">
-        <v>haven</v>
-      </c>
-      <c r="H53" t="str">
-        <v>B+</v>
-      </c>
-      <c r="I53" t="str">
-        <v>available</v>
-      </c>
-      <c r="J53" t="str" xml:space="preserve">
+      <c r="J51" t="str" xml:space="preserve">
         <v xml:space="preserve">amy milbourne (MAIN PLAYER - B+)_x000d_
 Keely Elliott (B-)_x000d_
 Kate Ryan (B+)_x000d_
 </v>
       </c>
-      <c r="K53" t="str">
+      <c r="K51" t="str">
         <v>fc1a8405-88ef-43cc-a677-2d1bdc00bb6a</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>6b9babbd-6769-4410-bb4c-e9b9c9a4e966</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Angelina Butler</v>
+      </c>
+      <c r="C52">
+        <v>23</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Angelinab31@hotmail.com</v>
+      </c>
+      <c r="F52" t="str">
+        <v>433646367</v>
+      </c>
+      <c r="G52" t="str">
+        <v>Wangaratta</v>
+      </c>
+      <c r="H52" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I52" t="str">
+        <v>available</v>
+      </c>
+      <c r="J52" t="str">
+        <v>Angelina Butler, Ebony Norris, Caragh Butler</v>
+      </c>
+      <c r="K52" t="str">
+        <v>c5549c5d-d4f2-46cd-a749-5c78710368b5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Leah Diaz</v>
+      </c>
+      <c r="C53">
+        <v>37</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E53" t="str">
+        <v>leah.diaz22@outlook.com</v>
+      </c>
+      <c r="F53" t="str">
+        <v>(159) 664-9326</v>
+      </c>
+      <c r="G53" t="str">
+        <v>Glendale</v>
+      </c>
+      <c r="H53" t="str">
+        <v>B</v>
+      </c>
+      <c r="I53" t="str">
+        <v>available</v>
+      </c>
+      <c r="J53" t="str">
+        <v>Julian Nguyen, Lydia Allen</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>6b9babbd-6769-4410-bb4c-e9b9c9a4e966</v>
+        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
       </c>
       <c r="B54" t="str">
-        <v>Angelina Butler</v>
+        <v>Naomi Moore</v>
       </c>
       <c r="C54">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D54" t="str">
         <v>Female</v>
       </c>
       <c r="E54" t="str">
-        <v>Angelinab31@hotmail.com</v>
+        <v>naomi.moore30@gmail.com</v>
       </c>
       <c r="F54" t="str">
-        <v>433646367</v>
+        <v>(391) 998-1729</v>
       </c>
       <c r="G54" t="str">
-        <v>Wangaratta</v>
+        <v>Irvine</v>
       </c>
       <c r="H54" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I54" t="str">
         <v>available</v>
       </c>
       <c r="J54" t="str">
-        <v>Angelina Butler, Ebony Norris, Caragh Butler</v>
-      </c>
-      <c r="K54" t="str">
-        <v>c5549c5d-d4f2-46cd-a749-5c78710368b5</v>
+        <v>Isla Wright, Cora Roberts</v>
       </c>
     </row>
     <row r="55">
@@ -2625,34 +2624,34 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
+        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
       </c>
       <c r="B56" t="str">
-        <v>Leah Diaz</v>
+        <v>Ella Gutierrez</v>
       </c>
       <c r="C56">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D56" t="str">
         <v>Female</v>
       </c>
       <c r="E56" t="str">
-        <v>leah.diaz22@outlook.com</v>
+        <v>ella.gutierrez43@gmail.com</v>
       </c>
       <c r="F56" t="str">
-        <v>(159) 664-9326</v>
+        <v>(220) 105-1876</v>
       </c>
       <c r="G56" t="str">
-        <v>Glendale</v>
+        <v>Irvine</v>
       </c>
       <c r="H56" t="str">
         <v>B</v>
       </c>
       <c r="I56" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J56" t="str">
-        <v>Julian Nguyen, Lydia Allen</v>
+        <v>Nora Lee</v>
       </c>
     </row>
     <row r="57">
@@ -2681,7 +2680,7 @@
         <v>B</v>
       </c>
       <c r="I57" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J57" t="str">
         <v>Colton Harris, Sebastian Edwards</v>
@@ -2713,7 +2712,7 @@
         <v>A</v>
       </c>
       <c r="I58" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J58" t="str">
         <v>Julian Nguyen, Leah Diaz</v>
@@ -2745,7 +2744,7 @@
         <v>B+</v>
       </c>
       <c r="I59" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J59" t="str">
         <v>Naomi Moore, Cora Roberts</v>
@@ -2777,7 +2776,7 @@
         <v>A</v>
       </c>
       <c r="I60" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J60" t="str">
         <v>Allison Torres, Christian Rivera</v>
@@ -2817,63 +2816,63 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>4e28a208-5278-410d-b375-d9c77ba144d7</v>
+        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
       </c>
       <c r="B62" t="str">
-        <v>Riley Scott</v>
+        <v>Allison Torres</v>
       </c>
       <c r="C62">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D62" t="str">
         <v>Female</v>
       </c>
       <c r="E62" t="str">
-        <v>riley.scott58@hotmail.com</v>
+        <v>allison.torres94@gmail.com</v>
       </c>
       <c r="F62" t="str">
-        <v>(848) 718-3465</v>
+        <v>(858) 153-7242</v>
       </c>
       <c r="G62" t="str">
-        <v>San Francisco</v>
+        <v>Fremont</v>
       </c>
       <c r="H62" t="str">
         <v>B</v>
       </c>
       <c r="I62" t="str">
         <v>available</v>
+      </c>
+      <c r="J62" t="str">
+        <v>Christian Rivera, Elena Green</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
+        <v>4e28a208-5278-410d-b375-d9c77ba144d7</v>
       </c>
       <c r="B63" t="str">
-        <v>Allison Torres</v>
+        <v>Riley Scott</v>
       </c>
       <c r="C63">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D63" t="str">
         <v>Female</v>
       </c>
       <c r="E63" t="str">
-        <v>allison.torres94@gmail.com</v>
+        <v>riley.scott58@hotmail.com</v>
       </c>
       <c r="F63" t="str">
-        <v>(858) 153-7242</v>
+        <v>(848) 718-3465</v>
       </c>
       <c r="G63" t="str">
-        <v>Fremont</v>
+        <v>San Francisco</v>
       </c>
       <c r="H63" t="str">
         <v>B</v>
       </c>
       <c r="I63" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J63" t="str">
-        <v>Christian Rivera, Elena Green</v>
+        <v>available</v>
       </c>
     </row>
     <row r="64">
@@ -3593,272 +3592,275 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
+        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
       </c>
       <c r="B87" t="str">
-        <v>Ethan Taylor</v>
+        <v>Nora Lee</v>
       </c>
       <c r="C87">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D87" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E87" t="str">
-        <v>ethan.taylor22@yahoo.com</v>
+        <v>nora.lee56@hotmail.com</v>
       </c>
       <c r="F87" t="str">
-        <v>0410 363 173</v>
+        <v>(171) 825-3697</v>
       </c>
       <c r="G87" t="str">
-        <v>Adelaide</v>
+        <v>Pasadena</v>
       </c>
       <c r="H87" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I87" t="str">
         <v>available</v>
+      </c>
+      <c r="J87" t="str">
+        <v>Ella Gutierrez</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
+        <v>d6c29b29-46c2-458d-9ed6-9955afb17b95</v>
       </c>
       <c r="B88" t="str">
-        <v>Cora Roberts</v>
+        <v>Ethan Taylor</v>
       </c>
       <c r="C88">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D88" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E88" t="str">
-        <v>cora.roberts57@hotmail.com</v>
+        <v>ethan.taylor22@yahoo.com</v>
       </c>
       <c r="F88" t="str">
-        <v>(141) 743-6838</v>
+        <v>0410 363 173</v>
       </c>
       <c r="G88" t="str">
-        <v>Bakersfield</v>
+        <v>Adelaide</v>
       </c>
       <c r="H88" t="str">
         <v>B</v>
       </c>
       <c r="I88" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J88" t="str">
-        <v>Isla Wright, Naomi Moore</v>
+        <v>available</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
+        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
       </c>
       <c r="B89" t="str">
-        <v>Madelyn Martinez</v>
+        <v>Cora Roberts</v>
       </c>
       <c r="C89">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D89" t="str">
         <v>Female</v>
       </c>
       <c r="E89" t="str">
-        <v>madelyn.martinez94@gmail.com</v>
+        <v>cora.roberts57@hotmail.com</v>
       </c>
       <c r="F89" t="str">
-        <v>(576) 468-3300</v>
+        <v>(141) 743-6838</v>
       </c>
       <c r="G89" t="str">
-        <v>Pasadena</v>
+        <v>Bakersfield</v>
       </c>
       <c r="H89" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I89" t="str">
         <v>available</v>
       </c>
       <c r="J89" t="str">
-        <v>Olivia Nelson, Joseph Stewart</v>
+        <v>Isla Wright, Naomi Moore</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
+        <v>d3db689e-5aed-4049-9588-adf3d1a49ae0</v>
       </c>
       <c r="B90" t="str">
-        <v>Emily Johnson</v>
+        <v>Madelyn Martinez</v>
       </c>
       <c r="C90">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D90" t="str">
         <v>Female</v>
       </c>
       <c r="E90" t="str">
-        <v>emily.johnson58@hotmail.com</v>
+        <v>madelyn.martinez94@gmail.com</v>
       </c>
       <c r="F90" t="str">
-        <v>0412 663 939</v>
+        <v>(576) 468-3300</v>
       </c>
       <c r="G90" t="str">
-        <v>Perth</v>
+        <v>Pasadena</v>
       </c>
       <c r="H90" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I90" t="str">
         <v>available</v>
+      </c>
+      <c r="J90" t="str">
+        <v>Olivia Nelson, Joseph Stewart</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
+        <v>ad836319-db56-4a08-bca6-a8e3f19c37a8</v>
       </c>
       <c r="B91" t="str">
-        <v>Stella Green</v>
+        <v>Emily Johnson</v>
       </c>
       <c r="C91">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D91" t="str">
         <v>Female</v>
       </c>
       <c r="E91" t="str">
-        <v>stella.green92@gmail.com</v>
+        <v>emily.johnson58@hotmail.com</v>
       </c>
       <c r="F91" t="str">
-        <v>0404 230 858</v>
+        <v>0412 663 939</v>
       </c>
       <c r="G91" t="str">
-        <v>Wollongong</v>
+        <v>Perth</v>
       </c>
       <c r="H91" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I91" t="str">
         <v>available</v>
-      </c>
-      <c r="J91" t="str">
-        <v>Everly Torres</v>
-      </c>
-      <c r="M91" t="str">
-        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
+        <v>e2f70c5c-0a8d-4055-8281-2ad2ae2e0cd6</v>
       </c>
       <c r="B92" t="str">
-        <v>Lily Walker</v>
+        <v>Stella Green</v>
       </c>
       <c r="C92">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D92" t="str">
         <v>Female</v>
       </c>
       <c r="E92" t="str">
-        <v>lily.walker96@outlook.com</v>
+        <v>stella.green92@gmail.com</v>
       </c>
       <c r="F92" t="str">
-        <v>0410 155 426</v>
+        <v>0404 230 858</v>
       </c>
       <c r="G92" t="str">
-        <v>Hobart</v>
+        <v>Wollongong</v>
       </c>
       <c r="H92" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I92" t="str">
         <v>available</v>
+      </c>
+      <c r="J92" t="str">
+        <v>Everly Torres</v>
+      </c>
+      <c r="M92" t="str">
+        <v>Vision impaired - needs assistance</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
+        <v>8774a9f4-b951-41cc-b6bd-809a709cb6ea</v>
       </c>
       <c r="B93" t="str">
-        <v>Aurora Williams</v>
+        <v>Lily Walker</v>
       </c>
       <c r="C93">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="D93" t="str">
         <v>Female</v>
       </c>
       <c r="E93" t="str">
-        <v>aurora.williams76@outlook.com</v>
+        <v>lily.walker96@outlook.com</v>
       </c>
       <c r="F93" t="str">
-        <v>0401 416 170</v>
+        <v>0410 155 426</v>
       </c>
       <c r="G93" t="str">
-        <v>Darwin</v>
+        <v>Hobart</v>
       </c>
       <c r="H93" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I93" t="str">
         <v>available</v>
-      </c>
-      <c r="M93" t="str">
-        <v>Uses walking cane</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
+        <v>e15c67b6-0680-4284-a8aa-a525b34c592d</v>
       </c>
       <c r="B94" t="str">
-        <v>Scarlett Lopez</v>
+        <v>Aurora Williams</v>
       </c>
       <c r="C94">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="D94" t="str">
         <v>Female</v>
       </c>
       <c r="E94" t="str">
-        <v>scarlett.lopez53@yahoo.com</v>
+        <v>aurora.williams76@outlook.com</v>
       </c>
       <c r="F94" t="str">
-        <v>0400 509 641</v>
+        <v>0401 416 170</v>
       </c>
       <c r="G94" t="str">
-        <v>Sydney</v>
+        <v>Darwin</v>
       </c>
       <c r="H94" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I94" t="str">
         <v>available</v>
+      </c>
+      <c r="M94" t="str">
+        <v>Uses walking cane</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
+        <v>bf5a6984-f656-4e23-9646-85829e9daffe</v>
       </c>
       <c r="B95" t="str">
-        <v>Liam Lewis</v>
+        <v>Scarlett Lopez</v>
       </c>
       <c r="C95">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="D95" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E95" t="str">
-        <v>liam.lewis79@yahoo.com</v>
+        <v>scarlett.lopez53@yahoo.com</v>
       </c>
       <c r="F95" t="str">
-        <v>0404 203 198</v>
+        <v>0400 509 641</v>
       </c>
       <c r="G95" t="str">
-        <v>Hobart</v>
+        <v>Sydney</v>
       </c>
       <c r="H95" t="str">
         <v>B+</v>
@@ -3869,34 +3871,31 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
+        <v>e166fd4f-73eb-4bea-b8be-3acdee4f9fdc</v>
       </c>
       <c r="B96" t="str">
-        <v>Nora Lee</v>
+        <v>Liam Lewis</v>
       </c>
       <c r="C96">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D96" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E96" t="str">
-        <v>nora.lee56@hotmail.com</v>
+        <v>liam.lewis79@yahoo.com</v>
       </c>
       <c r="F96" t="str">
-        <v>(171) 825-3697</v>
+        <v>0404 203 198</v>
       </c>
       <c r="G96" t="str">
-        <v>Pasadena</v>
+        <v>Hobart</v>
       </c>
       <c r="H96" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I96" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J96" t="str">
-        <v>Ella Gutierrez</v>
+        <v>available</v>
       </c>
     </row>
     <row r="97">
@@ -4473,54 +4472,57 @@
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>cc9dcc8f-9593-4b7e-b4dd-723de93b6b04</v>
+        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
       </c>
       <c r="B116" t="str">
-        <v>Aiden Cook</v>
+        <v>Julian Nguyen</v>
       </c>
       <c r="C116">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="D116" t="str">
         <v>Male</v>
       </c>
       <c r="E116" t="str">
-        <v>aiden.cook93@yahoo.com</v>
+        <v>julian.nguyen22@outlook.com</v>
       </c>
       <c r="F116" t="str">
-        <v>(959) 986-7207</v>
+        <v>(382) 722-8118</v>
       </c>
       <c r="G116" t="str">
-        <v>Pomona</v>
+        <v>Long Beach</v>
       </c>
       <c r="H116" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I116" t="str">
         <v>available</v>
+      </c>
+      <c r="J116" t="str">
+        <v>Leah Diaz, Lydia Allen</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>7a0a1a0e-a2dd-4f19-94ff-54601fcfb0e1</v>
+        <v>cc9dcc8f-9593-4b7e-b4dd-723de93b6b04</v>
       </c>
       <c r="B117" t="str">
-        <v>Alexander Reyes</v>
+        <v>Aiden Cook</v>
       </c>
       <c r="C117">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D117" t="str">
         <v>Male</v>
       </c>
       <c r="E117" t="str">
-        <v>alexander.reyes92@icloud.com</v>
+        <v>aiden.cook93@yahoo.com</v>
       </c>
       <c r="F117" t="str">
-        <v>(434) 933-1740</v>
+        <v>(959) 986-7207</v>
       </c>
       <c r="G117" t="str">
-        <v>Newport Beach</v>
+        <v>Pomona</v>
       </c>
       <c r="H117" t="str">
         <v>A+</v>
@@ -4531,118 +4533,118 @@
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
+        <v>7a0a1a0e-a2dd-4f19-94ff-54601fcfb0e1</v>
       </c>
       <c r="B118" t="str">
-        <v>Christopher Allen</v>
+        <v>Alexander Reyes</v>
       </c>
       <c r="C118">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D118" t="str">
         <v>Male</v>
       </c>
       <c r="E118" t="str">
-        <v>christopher.allen60@yahoo.com</v>
+        <v>alexander.reyes92@icloud.com</v>
       </c>
       <c r="F118" t="str">
-        <v>(529) 787-8147</v>
+        <v>(434) 933-1740</v>
       </c>
       <c r="G118" t="str">
-        <v>Torrance</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H118" t="str">
-        <v>B+</v>
+        <v>A+</v>
       </c>
       <c r="I118" t="str">
         <v>available</v>
-      </c>
-      <c r="J118" t="str">
-        <v>Eleanor Allen</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
+        <v>3f9d95b9-bedc-4620-9aa3-9bc8669de2af</v>
       </c>
       <c r="B119" t="str">
-        <v>Jackson Jackson</v>
+        <v>Christopher Allen</v>
       </c>
       <c r="C119">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D119" t="str">
         <v>Male</v>
       </c>
       <c r="E119" t="str">
-        <v>jackson.jackson86@icloud.com</v>
+        <v>christopher.allen60@yahoo.com</v>
       </c>
       <c r="F119" t="str">
-        <v>(858) 306-7989</v>
+        <v>(529) 787-8147</v>
       </c>
       <c r="G119" t="str">
-        <v>Oakland</v>
+        <v>Torrance</v>
       </c>
       <c r="H119" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I119" t="str">
         <v>available</v>
       </c>
       <c r="J119" t="str">
-        <v>Serenity Campbell, Isaiah Green</v>
+        <v>Eleanor Allen</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>258eb0f3-5b73-4b6f-abb9-86c6ccb99d1f</v>
+        <v>9e0ff879-df04-4a3f-b572-8633acb77cee</v>
       </c>
       <c r="B120" t="str">
-        <v>Mateo Phillips</v>
+        <v>Jackson Jackson</v>
       </c>
       <c r="C120">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D120" t="str">
         <v>Male</v>
       </c>
       <c r="E120" t="str">
-        <v>mateo.phillips59@outlook.com</v>
+        <v>jackson.jackson86@icloud.com</v>
       </c>
       <c r="F120" t="str">
-        <v>(155) 680-1162</v>
+        <v>(858) 306-7989</v>
       </c>
       <c r="G120" t="str">
-        <v>Sacramento</v>
+        <v>Oakland</v>
       </c>
       <c r="H120" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I120" t="str">
         <v>available</v>
+      </c>
+      <c r="J120" t="str">
+        <v>Serenity Campbell, Isaiah Green</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>c2103c22-c825-4633-a461-495c55747ed3</v>
+        <v>258eb0f3-5b73-4b6f-abb9-86c6ccb99d1f</v>
       </c>
       <c r="B121" t="str">
-        <v>Alice Robinson</v>
+        <v>Mateo Phillips</v>
       </c>
       <c r="C121">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D121" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E121" t="str">
-        <v>alice.robinson56@hotmail.com</v>
+        <v>mateo.phillips59@outlook.com</v>
       </c>
       <c r="F121" t="str">
-        <v>(251) 325-5554</v>
+        <v>(155) 680-1162</v>
       </c>
       <c r="G121" t="str">
-        <v>Anaheim</v>
+        <v>Sacramento</v>
       </c>
       <c r="H121" t="str">
         <v>B+</v>
@@ -4653,89 +4655,86 @@
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>4fba0674-c979-4177-b29d-9a882e08ad0d</v>
+        <v>c2103c22-c825-4633-a461-495c55747ed3</v>
       </c>
       <c r="B122" t="str">
-        <v>Autumn Lewis</v>
+        <v>Alice Robinson</v>
       </c>
       <c r="C122">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D122" t="str">
         <v>Female</v>
       </c>
       <c r="E122" t="str">
-        <v>autumn.lewis97@outlook.com</v>
+        <v>alice.robinson56@hotmail.com</v>
       </c>
       <c r="F122" t="str">
-        <v>(841) 837-8640</v>
+        <v>(251) 325-5554</v>
       </c>
       <c r="G122" t="str">
-        <v>San Francisco</v>
+        <v>Anaheim</v>
       </c>
       <c r="H122" t="str">
         <v>B+</v>
       </c>
       <c r="I122" t="str">
         <v>available</v>
-      </c>
-      <c r="J122" t="str">
-        <v>Noah Martinez</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
+        <v>4fba0674-c979-4177-b29d-9a882e08ad0d</v>
       </c>
       <c r="B123" t="str">
-        <v>Grayson Edwards</v>
+        <v>Autumn Lewis</v>
       </c>
       <c r="C123">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D123" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E123" t="str">
-        <v>grayson.edwards22@gmail.com</v>
+        <v>autumn.lewis97@outlook.com</v>
       </c>
       <c r="F123" t="str">
-        <v>(215) 129-3913</v>
+        <v>(841) 837-8640</v>
       </c>
       <c r="G123" t="str">
-        <v>Torrance</v>
+        <v>San Francisco</v>
       </c>
       <c r="H123" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I123" t="str">
         <v>available</v>
       </c>
       <c r="J123" t="str">
-        <v>Elizabeth Nelson, Joseph Anderson</v>
+        <v>Noah Martinez</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
+        <v>224212bc-76fd-40f4-903d-8a0a1d6163e3</v>
       </c>
       <c r="B124" t="str">
-        <v>Cameron Evans</v>
+        <v>Grayson Edwards</v>
       </c>
       <c r="C124">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D124" t="str">
         <v>Male</v>
       </c>
       <c r="E124" t="str">
-        <v>cameron.evans55@outlook.com</v>
+        <v>grayson.edwards22@gmail.com</v>
       </c>
       <c r="F124" t="str">
-        <v>(535) 743-7467</v>
+        <v>(215) 129-3913</v>
       </c>
       <c r="G124" t="str">
-        <v>Fremont</v>
+        <v>Torrance</v>
       </c>
       <c r="H124" t="str">
         <v>B</v>
@@ -4744,216 +4743,216 @@
         <v>available</v>
       </c>
       <c r="J124" t="str">
-        <v>Michael Johnson, Anthony Garcia</v>
+        <v>Elizabeth Nelson, Joseph Anderson</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>10ec31e6-c6da-4957-9768-c5fcefe79c6b</v>
+        <v>bede75d6-a4ec-4fe3-907f-35108a2b4b10</v>
       </c>
       <c r="B125" t="str">
-        <v>Emma Turner</v>
+        <v>Cameron Evans</v>
       </c>
       <c r="C125">
         <v>33</v>
       </c>
       <c r="D125" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E125" t="str">
-        <v>emma.turner16@outlook.com</v>
+        <v>cameron.evans55@outlook.com</v>
       </c>
       <c r="F125" t="str">
-        <v>(656) 213-9003</v>
+        <v>(535) 743-7467</v>
       </c>
       <c r="G125" t="str">
-        <v>Pomona</v>
+        <v>Fremont</v>
       </c>
       <c r="H125" t="str">
         <v>B</v>
       </c>
       <c r="I125" t="str">
         <v>available</v>
+      </c>
+      <c r="J125" t="str">
+        <v>Michael Johnson, Anthony Garcia</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>a1895f97-a947-4cf3-9bc3-6aa43cdc1339</v>
+        <v>10ec31e6-c6da-4957-9768-c5fcefe79c6b</v>
       </c>
       <c r="B126" t="str">
-        <v>Gabriella Smith</v>
+        <v>Emma Turner</v>
       </c>
       <c r="C126">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D126" t="str">
         <v>Female</v>
       </c>
       <c r="E126" t="str">
-        <v>gabriella.smith91@hotmail.com</v>
+        <v>emma.turner16@outlook.com</v>
       </c>
       <c r="F126" t="str">
-        <v>(550) 121-2897</v>
+        <v>(656) 213-9003</v>
       </c>
       <c r="G126" t="str">
-        <v>Sacramento</v>
+        <v>Pomona</v>
       </c>
       <c r="H126" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I126" t="str">
         <v>available</v>
-      </c>
-      <c r="J126" t="str">
-        <v>Julian Rivera</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
+        <v>a1895f97-a947-4cf3-9bc3-6aa43cdc1339</v>
       </c>
       <c r="B127" t="str">
-        <v>Audrey Hill</v>
+        <v>Gabriella Smith</v>
       </c>
       <c r="C127">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D127" t="str">
         <v>Female</v>
       </c>
       <c r="E127" t="str">
-        <v>audrey.hill20@outlook.com</v>
+        <v>gabriella.smith91@hotmail.com</v>
       </c>
       <c r="F127" t="str">
-        <v>(688) 524-4712</v>
+        <v>(550) 121-2897</v>
       </c>
       <c r="G127" t="str">
-        <v>San Jose</v>
+        <v>Sacramento</v>
       </c>
       <c r="H127" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I127" t="str">
         <v>available</v>
       </c>
       <c r="J127" t="str">
-        <v>Avery Taylor</v>
+        <v>Julian Rivera</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>2450bd3d-4940-477d-8a08-abc3363fdc3a</v>
+        <v>4501044d-6fd4-4a45-83a0-416599928b1f</v>
       </c>
       <c r="B128" t="str">
-        <v>Ella Lopez</v>
+        <v>Audrey Hill</v>
       </c>
       <c r="C128">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D128" t="str">
         <v>Female</v>
       </c>
       <c r="E128" t="str">
-        <v>ella.lopez65@outlook.com</v>
+        <v>audrey.hill20@outlook.com</v>
       </c>
       <c r="F128" t="str">
-        <v>(192) 887-5779</v>
+        <v>(688) 524-4712</v>
       </c>
       <c r="G128" t="str">
-        <v>Riverside</v>
+        <v>San Jose</v>
       </c>
       <c r="H128" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I128" t="str">
         <v>available</v>
       </c>
       <c r="J128" t="str">
-        <v>Adam Edwards</v>
+        <v>Avery Taylor</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>f85f167d-7dd5-420d-86b5-ec8861b2bc1a</v>
+        <v>2450bd3d-4940-477d-8a08-abc3363fdc3a</v>
       </c>
       <c r="B129" t="str">
-        <v>Michael Carter</v>
+        <v>Ella Lopez</v>
       </c>
       <c r="C129">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D129" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E129" t="str">
-        <v>michael.carter90@outlook.com</v>
+        <v>ella.lopez65@outlook.com</v>
       </c>
       <c r="F129" t="str">
-        <v>(377) 714-4320</v>
+        <v>(192) 887-5779</v>
       </c>
       <c r="G129" t="str">
-        <v>Burbank</v>
+        <v>Riverside</v>
       </c>
       <c r="H129" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I129" t="str">
         <v>available</v>
+      </c>
+      <c r="J129" t="str">
+        <v>Adam Edwards</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
+        <v>f85f167d-7dd5-420d-86b5-ec8861b2bc1a</v>
       </c>
       <c r="B130" t="str">
-        <v>Michael Campbell</v>
+        <v>Michael Carter</v>
       </c>
       <c r="C130">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D130" t="str">
         <v>Male</v>
       </c>
       <c r="E130" t="str">
-        <v>michael.campbell9@outlook.com</v>
+        <v>michael.carter90@outlook.com</v>
       </c>
       <c r="F130" t="str">
-        <v>(176) 164-6950</v>
+        <v>(377) 714-4320</v>
       </c>
       <c r="G130" t="str">
-        <v>Glendale</v>
+        <v>Burbank</v>
       </c>
       <c r="H130" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I130" t="str">
         <v>available</v>
-      </c>
-      <c r="J130" t="str">
-        <v>Sadie Williams, Eleanor Hall</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
+        <v>9d8995c7-d5a1-4644-848d-dca4e81371af</v>
       </c>
       <c r="B131" t="str">
-        <v>Sadie Cook</v>
+        <v>Michael Campbell</v>
       </c>
       <c r="C131">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D131" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E131" t="str">
-        <v>sadie.cook9@yahoo.com</v>
+        <v>michael.campbell9@outlook.com</v>
       </c>
       <c r="F131" t="str">
-        <v>(382) 126-7672</v>
+        <v>(176) 164-6950</v>
       </c>
       <c r="G131" t="str">
-        <v>Santa Monica</v>
+        <v>Glendale</v>
       </c>
       <c r="H131" t="str">
         <v>B+</v>
@@ -4962,103 +4961,103 @@
         <v>available</v>
       </c>
       <c r="J131" t="str">
-        <v>William Allen, Alexa Hall</v>
+        <v>Sadie Williams, Eleanor Hall</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
+        <v>ea1b059a-dde4-49c1-92b8-b9fd09c84bb7</v>
       </c>
       <c r="B132" t="str">
-        <v>Anthony Garcia</v>
+        <v>Sadie Cook</v>
       </c>
       <c r="C132">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D132" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E132" t="str">
-        <v>anthony.garcia31@yahoo.com</v>
+        <v>sadie.cook9@yahoo.com</v>
       </c>
       <c r="F132" t="str">
-        <v>(249) 774-7265</v>
+        <v>(382) 126-7672</v>
       </c>
       <c r="G132" t="str">
         <v>Santa Monica</v>
       </c>
       <c r="H132" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I132" t="str">
         <v>available</v>
       </c>
       <c r="J132" t="str">
-        <v>Michael Johnson, Cameron Evans</v>
+        <v>William Allen, Alexa Hall</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>921da7b6-596c-4a0e-a647-022bbd8cef26</v>
+        <v>cacb8de7-16c5-4332-9d25-a6794d8a23b3</v>
       </c>
       <c r="B133" t="str">
-        <v>John Diaz</v>
+        <v>Anthony Garcia</v>
       </c>
       <c r="C133">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="D133" t="str">
         <v>Male</v>
       </c>
       <c r="E133" t="str">
-        <v>john.diaz17@icloud.com</v>
+        <v>anthony.garcia31@yahoo.com</v>
       </c>
       <c r="F133" t="str">
-        <v>(251) 432-3565</v>
+        <v>(249) 774-7265</v>
       </c>
       <c r="G133" t="str">
-        <v>Pomona</v>
+        <v>Santa Monica</v>
       </c>
       <c r="H133" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I133" t="str">
         <v>available</v>
       </c>
       <c r="J133" t="str">
-        <v>Cameron Anderson</v>
+        <v>Michael Johnson, Cameron Evans</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
+        <v>921da7b6-596c-4a0e-a647-022bbd8cef26</v>
       </c>
       <c r="B134" t="str">
-        <v>Julian Nguyen</v>
+        <v>John Diaz</v>
       </c>
       <c r="C134">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="D134" t="str">
         <v>Male</v>
       </c>
       <c r="E134" t="str">
-        <v>julian.nguyen22@outlook.com</v>
+        <v>john.diaz17@icloud.com</v>
       </c>
       <c r="F134" t="str">
-        <v>(382) 722-8118</v>
+        <v>(251) 432-3565</v>
       </c>
       <c r="G134" t="str">
-        <v>Long Beach</v>
+        <v>Pomona</v>
       </c>
       <c r="H134" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I134" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J134" t="str">
-        <v>Leah Diaz, Lydia Allen</v>
+        <v>Cameron Anderson</v>
       </c>
     </row>
     <row r="135">
@@ -5342,86 +5341,89 @@
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>c6c464e0-123d-4cc9-8b28-0ecbd0a6ce5f</v>
+        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
       </c>
       <c r="B144" t="str">
-        <v>Matthew Anderson</v>
+        <v>Colton Harris</v>
       </c>
       <c r="C144">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D144" t="str">
         <v>Male</v>
       </c>
       <c r="E144" t="str">
-        <v>matthew.anderson56@icloud.com</v>
+        <v>colton.harris98@icloud.com</v>
       </c>
       <c r="F144" t="str">
-        <v>(853) 972-9742</v>
+        <v>(583) 900-3294</v>
       </c>
       <c r="G144" t="str">
-        <v>Irvine</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H144" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I144" t="str">
         <v>available</v>
+      </c>
+      <c r="J144" t="str">
+        <v>Sebastian Edwards, Sofia Williams</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>0497247b-bf9a-4f46-a562-05f1892687ce</v>
+        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
       </c>
       <c r="B145" t="str">
-        <v>Henry Roberts</v>
+        <v>Sebastian Edwards</v>
       </c>
       <c r="C145">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D145" t="str">
         <v>Male</v>
       </c>
       <c r="E145" t="str">
-        <v>henry.roberts93@outlook.com</v>
+        <v>sebastian.edwards97@icloud.com</v>
       </c>
       <c r="F145" t="str">
-        <v>(654) 727-7734</v>
+        <v>(348) 408-1134</v>
       </c>
       <c r="G145" t="str">
-        <v>Burbank</v>
+        <v>Los Angeles</v>
       </c>
       <c r="H145" t="str">
-        <v>A+</v>
+        <v>B</v>
       </c>
       <c r="I145" t="str">
         <v>available</v>
       </c>
       <c r="J145" t="str">
-        <v>Thomas Nguyen, Hannah Jones</v>
+        <v>Colton Harris, Sofia Williams</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>5260c12e-e864-4bff-bd02-32d2c84a9a95</v>
+        <v>c6c464e0-123d-4cc9-8b28-0ecbd0a6ce5f</v>
       </c>
       <c r="B146" t="str">
-        <v>Alexander Baker</v>
+        <v>Matthew Anderson</v>
       </c>
       <c r="C146">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D146" t="str">
         <v>Male</v>
       </c>
       <c r="E146" t="str">
-        <v>alexander.baker64@hotmail.com</v>
+        <v>matthew.anderson56@icloud.com</v>
       </c>
       <c r="F146" t="str">
-        <v>(434) 373-1503</v>
+        <v>(853) 972-9742</v>
       </c>
       <c r="G146" t="str">
-        <v>Stockton</v>
+        <v>Irvine</v>
       </c>
       <c r="H146" t="str">
         <v>A+</v>
@@ -5432,103 +5434,103 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
+        <v>0497247b-bf9a-4f46-a562-05f1892687ce</v>
       </c>
       <c r="B147" t="str">
-        <v>William Taylor</v>
+        <v>Henry Roberts</v>
       </c>
       <c r="C147">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D147" t="str">
         <v>Male</v>
       </c>
       <c r="E147" t="str">
-        <v>william.taylor84@hotmail.com</v>
+        <v>henry.roberts93@outlook.com</v>
       </c>
       <c r="F147" t="str">
-        <v>(276) 538-1731</v>
+        <v>(654) 727-7734</v>
       </c>
       <c r="G147" t="str">
-        <v>Newport Beach</v>
+        <v>Burbank</v>
       </c>
       <c r="H147" t="str">
-        <v>B</v>
+        <v>A+</v>
       </c>
       <c r="I147" t="str">
         <v>available</v>
       </c>
       <c r="J147" t="str">
-        <v>Victoria Scott</v>
+        <v>Thomas Nguyen, Hannah Jones</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
+        <v>5260c12e-e864-4bff-bd02-32d2c84a9a95</v>
       </c>
       <c r="B148" t="str">
-        <v>Christian Rivera</v>
+        <v>Alexander Baker</v>
       </c>
       <c r="C148">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D148" t="str">
         <v>Male</v>
       </c>
       <c r="E148" t="str">
-        <v>christian.rivera21@outlook.com</v>
+        <v>alexander.baker64@hotmail.com</v>
       </c>
       <c r="F148" t="str">
-        <v>(913) 900-2520</v>
+        <v>(434) 373-1503</v>
       </c>
       <c r="G148" t="str">
-        <v>Burbank</v>
+        <v>Stockton</v>
       </c>
       <c r="H148" t="str">
-        <v>B+</v>
+        <v>A+</v>
       </c>
       <c r="I148" t="str">
         <v>available</v>
-      </c>
-      <c r="J148" t="str">
-        <v>Allison Torres, Elena Green</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>d1a89d8f-bd2f-40db-a5d5-ef8dc3e3aa54</v>
+        <v>06d38f0c-6780-4d6a-97b8-f28ec52ced34</v>
       </c>
       <c r="B149" t="str">
-        <v>Mason Hernandez</v>
+        <v>William Taylor</v>
       </c>
       <c r="C149">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D149" t="str">
         <v>Male</v>
       </c>
       <c r="E149" t="str">
-        <v>mason.hernandez15@gmail.com</v>
+        <v>william.taylor84@hotmail.com</v>
       </c>
       <c r="F149" t="str">
-        <v>(880) 425-4186</v>
+        <v>(276) 538-1731</v>
       </c>
       <c r="G149" t="str">
-        <v>San Jose</v>
+        <v>Newport Beach</v>
       </c>
       <c r="H149" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I149" t="str">
         <v>available</v>
+      </c>
+      <c r="J149" t="str">
+        <v>Victoria Scott</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>e2c7fa0a-1d97-4430-b83c-5099c5831757</v>
+        <v>ce7b894b-705d-49f7-a6a3-e0a7fe953a10</v>
       </c>
       <c r="B150" t="str">
-        <v>John Carter</v>
+        <v>Christian Rivera</v>
       </c>
       <c r="C150">
         <v>51</v>
@@ -5537,109 +5539,109 @@
         <v>Male</v>
       </c>
       <c r="E150" t="str">
-        <v>john.carter42@outlook.com</v>
+        <v>christian.rivera21@outlook.com</v>
       </c>
       <c r="F150" t="str">
-        <v>(160) 507-8767</v>
+        <v>(913) 900-2520</v>
       </c>
       <c r="G150" t="str">
-        <v>Pasadena</v>
+        <v>Burbank</v>
       </c>
       <c r="H150" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I150" t="str">
         <v>available</v>
       </c>
       <c r="J150" t="str">
-        <v>Brooklyn Rivera</v>
+        <v>Allison Torres, Elena Green</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
+        <v>d1a89d8f-bd2f-40db-a5d5-ef8dc3e3aa54</v>
       </c>
       <c r="B151" t="str">
-        <v>Colton Harris</v>
+        <v>Mason Hernandez</v>
       </c>
       <c r="C151">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D151" t="str">
         <v>Male</v>
       </c>
       <c r="E151" t="str">
-        <v>colton.harris98@icloud.com</v>
+        <v>mason.hernandez15@gmail.com</v>
       </c>
       <c r="F151" t="str">
-        <v>(583) 900-3294</v>
+        <v>(880) 425-4186</v>
       </c>
       <c r="G151" t="str">
-        <v>Newport Beach</v>
+        <v>San Jose</v>
       </c>
       <c r="H151" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I151" t="str">
-        <v>assigned</v>
-      </c>
-      <c r="J151" t="str">
-        <v>Sebastian Edwards, Sofia Williams</v>
+        <v>available</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
+        <v>e2c7fa0a-1d97-4430-b83c-5099c5831757</v>
       </c>
       <c r="B152" t="str">
-        <v>Carter Harris</v>
+        <v>John Carter</v>
       </c>
       <c r="C152">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D152" t="str">
         <v>Male</v>
       </c>
       <c r="E152" t="str">
-        <v>carter.harris82@yahoo.com</v>
+        <v>john.carter42@outlook.com</v>
       </c>
       <c r="F152" t="str">
-        <v>0412 175 744</v>
+        <v>(160) 507-8767</v>
       </c>
       <c r="G152" t="str">
-        <v>Geelong</v>
+        <v>Pasadena</v>
       </c>
       <c r="H152" t="str">
         <v>B</v>
       </c>
       <c r="I152" t="str">
         <v>available</v>
+      </c>
+      <c r="J152" t="str">
+        <v>Brooklyn Rivera</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>340ad2e5-95a9-4eb5-a113-e7f9f0e5d704</v>
+        <v>0bb2a1aa-a74d-4711-a2ea-609663a77b4d</v>
       </c>
       <c r="B153" t="str">
-        <v>Jaxon Cook</v>
+        <v>Carter Harris</v>
       </c>
       <c r="C153">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D153" t="str">
         <v>Male</v>
       </c>
       <c r="E153" t="str">
-        <v>jaxon.cook73@yahoo.com</v>
+        <v>carter.harris82@yahoo.com</v>
       </c>
       <c r="F153" t="str">
-        <v>(190) 120-3429</v>
+        <v>0412 175 744</v>
       </c>
       <c r="G153" t="str">
-        <v>Fresno</v>
+        <v>Geelong</v>
       </c>
       <c r="H153" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I153" t="str">
         <v>available</v>
@@ -5647,22 +5649,22 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
+        <v>340ad2e5-95a9-4eb5-a113-e7f9f0e5d704</v>
       </c>
       <c r="B154" t="str">
-        <v>Alexander Campbell</v>
+        <v>Jaxon Cook</v>
       </c>
       <c r="C154">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D154" t="str">
         <v>Male</v>
       </c>
       <c r="E154" t="str">
-        <v>alexander.campbell71@gmail.com</v>
+        <v>jaxon.cook73@yahoo.com</v>
       </c>
       <c r="F154" t="str">
-        <v>(131) 840-1169</v>
+        <v>(190) 120-3429</v>
       </c>
       <c r="G154" t="str">
         <v>Fresno</v>
@@ -5673,16 +5675,13 @@
       <c r="I154" t="str">
         <v>available</v>
       </c>
-      <c r="J154" t="str">
-        <v>Logan Nguyen, Hannah Moore</v>
-      </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>e8c7986a-699a-4e43-9b2d-52ca42510a36</v>
+        <v>9ad191d8-a3b3-478d-9318-781d3156afaa</v>
       </c>
       <c r="B155" t="str">
-        <v>Matthew Torres</v>
+        <v>Alexander Campbell</v>
       </c>
       <c r="C155">
         <v>34</v>
@@ -5691,13 +5690,13 @@
         <v>Male</v>
       </c>
       <c r="E155" t="str">
-        <v>matthew.torres76@yahoo.com</v>
+        <v>alexander.campbell71@gmail.com</v>
       </c>
       <c r="F155" t="str">
-        <v>(432) 516-9920</v>
+        <v>(131) 840-1169</v>
       </c>
       <c r="G155" t="str">
-        <v>Sacramento</v>
+        <v>Fresno</v>
       </c>
       <c r="H155" t="str">
         <v>A</v>
@@ -5705,31 +5704,34 @@
       <c r="I155" t="str">
         <v>available</v>
       </c>
+      <c r="J155" t="str">
+        <v>Logan Nguyen, Hannah Moore</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
+        <v>e8c7986a-699a-4e43-9b2d-52ca42510a36</v>
       </c>
       <c r="B156" t="str">
-        <v>Noah Hernandez</v>
+        <v>Matthew Torres</v>
       </c>
       <c r="C156">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D156" t="str">
         <v>Male</v>
       </c>
       <c r="E156" t="str">
-        <v>noah.hernandez9@hotmail.com</v>
+        <v>matthew.torres76@yahoo.com</v>
       </c>
       <c r="F156" t="str">
-        <v>0404 855 230</v>
+        <v>(432) 516-9920</v>
       </c>
       <c r="G156" t="str">
-        <v>Cairns</v>
+        <v>Sacramento</v>
       </c>
       <c r="H156" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I156" t="str">
         <v>available</v>
@@ -5737,57 +5739,54 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
+        <v>9efd8ec8-0e91-45d9-804b-518939fbac76</v>
       </c>
       <c r="B157" t="str">
-        <v>Josiah Lopez</v>
+        <v>Noah Hernandez</v>
       </c>
       <c r="C157">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D157" t="str">
         <v>Male</v>
       </c>
       <c r="E157" t="str">
-        <v>josiah.lopez65@gmail.com</v>
+        <v>noah.hernandez9@hotmail.com</v>
       </c>
       <c r="F157" t="str">
-        <v>(305) 140-9212</v>
+        <v>0404 855 230</v>
       </c>
       <c r="G157" t="str">
-        <v>Chula Vista</v>
+        <v>Cairns</v>
       </c>
       <c r="H157" t="str">
         <v>B</v>
       </c>
       <c r="I157" t="str">
         <v>available</v>
-      </c>
-      <c r="J157" t="str">
-        <v>Victoria Carter, Ella Martinez</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
+        <v>8dfd710f-c1f0-43ee-b26d-13d05de4598b</v>
       </c>
       <c r="B158" t="str">
-        <v>Mia Anderson</v>
+        <v>Josiah Lopez</v>
       </c>
       <c r="C158">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D158" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E158" t="str">
-        <v>mia.anderson0@yahoo.com</v>
+        <v>josiah.lopez65@gmail.com</v>
       </c>
       <c r="F158" t="str">
-        <v>(574) 806-3609</v>
+        <v>(305) 140-9212</v>
       </c>
       <c r="G158" t="str">
-        <v>Stockton</v>
+        <v>Chula Vista</v>
       </c>
       <c r="H158" t="str">
         <v>B</v>
@@ -5796,30 +5795,30 @@
         <v>available</v>
       </c>
       <c r="J158" t="str">
-        <v>Avery Cruz, Lydia Torres</v>
+        <v>Victoria Carter, Ella Martinez</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
+        <v>924c70dd-25ce-4725-8a88-173a3af33a7f</v>
       </c>
       <c r="B159" t="str">
-        <v>Grace King</v>
+        <v>Mia Anderson</v>
       </c>
       <c r="C159">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D159" t="str">
         <v>Female</v>
       </c>
       <c r="E159" t="str">
-        <v>grace.king1@yahoo.com</v>
+        <v>mia.anderson0@yahoo.com</v>
       </c>
       <c r="F159" t="str">
-        <v>(217) 721-5651</v>
+        <v>(574) 806-3609</v>
       </c>
       <c r="G159" t="str">
-        <v>Oakland</v>
+        <v>Stockton</v>
       </c>
       <c r="H159" t="str">
         <v>B</v>
@@ -5828,219 +5827,219 @@
         <v>available</v>
       </c>
       <c r="J159" t="str">
-        <v>Gianna Hill</v>
+        <v>Avery Cruz, Lydia Torres</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>f26a0638-511f-4440-ae1a-2ae052df470f</v>
+        <v>93e72347-d9bf-4fb1-b06c-7cb5a2edcc2a</v>
       </c>
       <c r="B160" t="str">
-        <v>Caleb Brown</v>
+        <v>Grace King</v>
       </c>
       <c r="C160">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D160" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E160" t="str">
-        <v>caleb.brown13@yahoo.com</v>
+        <v>grace.king1@yahoo.com</v>
       </c>
       <c r="F160" t="str">
-        <v>(130) 920-6765</v>
+        <v>(217) 721-5651</v>
       </c>
       <c r="G160" t="str">
-        <v>Irvine</v>
+        <v>Oakland</v>
       </c>
       <c r="H160" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I160" t="str">
         <v>available</v>
       </c>
       <c r="J160" t="str">
-        <v>Jackson Murphy</v>
+        <v>Gianna Hill</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
+        <v>f26a0638-511f-4440-ae1a-2ae052df470f</v>
       </c>
       <c r="B161" t="str">
-        <v>Thomas Rivera</v>
+        <v>Caleb Brown</v>
       </c>
       <c r="C161">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D161" t="str">
         <v>Male</v>
       </c>
       <c r="E161" t="str">
-        <v>thomas.rivera13@yahoo.com</v>
+        <v>caleb.brown13@yahoo.com</v>
       </c>
       <c r="F161" t="str">
-        <v>(539) 243-6118</v>
+        <v>(130) 920-6765</v>
       </c>
       <c r="G161" t="str">
-        <v>Long Beach</v>
+        <v>Irvine</v>
       </c>
       <c r="H161" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I161" t="str">
         <v>available</v>
       </c>
       <c r="J161" t="str">
-        <v>Hannah Murphy</v>
+        <v>Jackson Murphy</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>befe2d5d-0583-45ac-939e-ab57370e2d4f</v>
+        <v>d035c0a6-d30e-4ca3-b8c2-9becb2842da7</v>
       </c>
       <c r="B162" t="str">
-        <v>Daniel Taylor</v>
+        <v>Thomas Rivera</v>
       </c>
       <c r="C162">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D162" t="str">
         <v>Male</v>
       </c>
       <c r="E162" t="str">
-        <v>daniel.taylor53@gmail.com</v>
+        <v>thomas.rivera13@yahoo.com</v>
       </c>
       <c r="F162" t="str">
-        <v>(543) 329-4768</v>
+        <v>(539) 243-6118</v>
       </c>
       <c r="G162" t="str">
-        <v>Pomona</v>
+        <v>Long Beach</v>
       </c>
       <c r="H162" t="str">
         <v>B</v>
       </c>
       <c r="I162" t="str">
         <v>available</v>
+      </c>
+      <c r="J162" t="str">
+        <v>Hannah Murphy</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
+        <v>befe2d5d-0583-45ac-939e-ab57370e2d4f</v>
       </c>
       <c r="B163" t="str">
-        <v>Logan Nguyen</v>
+        <v>Daniel Taylor</v>
       </c>
       <c r="C163">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D163" t="str">
         <v>Male</v>
       </c>
       <c r="E163" t="str">
-        <v>logan.nguyen23@hotmail.com</v>
+        <v>daniel.taylor53@gmail.com</v>
       </c>
       <c r="F163" t="str">
-        <v>(278) 620-7089</v>
+        <v>(543) 329-4768</v>
       </c>
       <c r="G163" t="str">
-        <v>Torrance</v>
+        <v>Pomona</v>
       </c>
       <c r="H163" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I163" t="str">
         <v>available</v>
-      </c>
-      <c r="J163" t="str">
-        <v>Alexander Campbell, Hannah Moore</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
+        <v>5cb68000-430e-4dc3-9afa-c9c5cca864c0</v>
       </c>
       <c r="B164" t="str">
-        <v>Elijah Miller</v>
+        <v>Logan Nguyen</v>
       </c>
       <c r="C164">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D164" t="str">
         <v>Male</v>
       </c>
       <c r="E164" t="str">
-        <v>elijah.miller73@outlook.com</v>
+        <v>logan.nguyen23@hotmail.com</v>
       </c>
       <c r="F164" t="str">
-        <v>(967) 645-5202</v>
+        <v>(278) 620-7089</v>
       </c>
       <c r="G164" t="str">
-        <v>Pasadena</v>
+        <v>Torrance</v>
       </c>
       <c r="H164" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I164" t="str">
         <v>available</v>
       </c>
       <c r="J164" t="str">
-        <v>Sophia Flores</v>
+        <v>Alexander Campbell, Hannah Moore</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
+        <v>7772949f-f87d-480b-87ab-71f7500e8bd3</v>
       </c>
       <c r="B165" t="str">
-        <v>Thomas Nguyen</v>
+        <v>Elijah Miller</v>
       </c>
       <c r="C165">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D165" t="str">
         <v>Male</v>
       </c>
       <c r="E165" t="str">
-        <v>thomas.nguyen88@yahoo.com</v>
+        <v>elijah.miller73@outlook.com</v>
       </c>
       <c r="F165" t="str">
-        <v>(163) 406-8750</v>
+        <v>(967) 645-5202</v>
       </c>
       <c r="G165" t="str">
-        <v>Pomona</v>
+        <v>Pasadena</v>
       </c>
       <c r="H165" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I165" t="str">
         <v>available</v>
       </c>
       <c r="J165" t="str">
-        <v>Henry Roberts, Hannah Jones</v>
+        <v>Sophia Flores</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
+        <v>6aa67d72-8123-41b4-9298-7f5d1e89aef7</v>
       </c>
       <c r="B166" t="str">
-        <v>Joseph Stewart</v>
+        <v>Thomas Nguyen</v>
       </c>
       <c r="C166">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D166" t="str">
         <v>Male</v>
       </c>
       <c r="E166" t="str">
-        <v>joseph.stewart94@outlook.com</v>
+        <v>thomas.nguyen88@yahoo.com</v>
       </c>
       <c r="F166" t="str">
-        <v>(101) 920-4176</v>
+        <v>(163) 406-8750</v>
       </c>
       <c r="G166" t="str">
-        <v>Stockton</v>
+        <v>Pomona</v>
       </c>
       <c r="H166" t="str">
         <v>B</v>
@@ -6049,39 +6048,39 @@
         <v>available</v>
       </c>
       <c r="J166" t="str">
-        <v>Olivia Nelson, Madelyn Martinez</v>
+        <v>Henry Roberts, Hannah Jones</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
+        <v>29b3a5cd-ea7d-4673-9db4-7886660a791f</v>
       </c>
       <c r="B167" t="str">
-        <v>Sebastian Edwards</v>
+        <v>Joseph Stewart</v>
       </c>
       <c r="C167">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D167" t="str">
         <v>Male</v>
       </c>
       <c r="E167" t="str">
-        <v>sebastian.edwards97@icloud.com</v>
+        <v>joseph.stewart94@outlook.com</v>
       </c>
       <c r="F167" t="str">
-        <v>(348) 408-1134</v>
+        <v>(101) 920-4176</v>
       </c>
       <c r="G167" t="str">
-        <v>Los Angeles</v>
+        <v>Stockton</v>
       </c>
       <c r="H167" t="str">
         <v>B</v>
       </c>
       <c r="I167" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J167" t="str">
-        <v>Colton Harris, Sofia Williams</v>
+        <v>Olivia Nelson, Madelyn Martinez</v>
       </c>
     </row>
     <row r="168">
@@ -11400,7 +11399,7 @@
         <v>B+</v>
       </c>
       <c r="I347" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
     </row>
   </sheetData>
@@ -11412,284 +11411,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Block</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Seat</v>
-      </c>
-      <c r="F1" t="str">
-        <v>BookingEmailSent</v>
-      </c>
-      <c r="G1" t="str">
-        <v>ConfirmedRSVP</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2b3dffc7-5ec2-4950-9434-bcd2d0ad89e1</v>
-      </c>
-      <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>f9d68052-4310-45c2-a5a9-64c272347899</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="str">
-        <v>C3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>6d85f4a7-815e-4c53-b08f-c5a65723bdfa</v>
-      </c>
-      <c r="B3" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C3" t="str">
-        <v>a614b69c-4f6c-49fa-a490-24d7e4a60da9</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="str">
-        <v>A4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>0b9e3538-2d1f-4380-8f25-a1d785645eee</v>
-      </c>
-      <c r="B4" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C4" t="str">
-        <v>d2e4b795-48d9-43e4-8ebe-6916a61a544e</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="str">
-        <v>A5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>0c2a0504-54c8-4237-8e4d-b5e7b3ccfd05</v>
-      </c>
-      <c r="B5" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C5" t="str">
-        <v>efeba788-8d57-40b3-a3f9-e134a40931ac</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="str">
-        <v>B1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>df33aaa7-def9-4af2-abe0-e025a23aa642</v>
-      </c>
-      <c r="B6" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C6" t="str">
-        <v>b22d1d02-9344-4922-9be8-d8d05a79b0b0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="str">
-        <v>B2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>74c8eb7d-740c-4c1a-b163-74a812c4542d</v>
-      </c>
-      <c r="B7" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C7" t="str">
-        <v>8d8070dd-3ee6-476f-aaf2-631e80f67ef7</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="str">
-        <v>B3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>dead1675-84f2-483d-b78e-dc88a0a019d6</v>
-      </c>
-      <c r="B8" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C8" t="str">
-        <v>81759c6b-da11-4c0e-9e96-92aa20964b06</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="str">
-        <v>C3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>5d682f27-9575-4708-8ea2-9afd63d3ff6c</v>
-      </c>
-      <c r="B9" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C9" t="str">
-        <v>8819a806-f5b1-4b58-95f5-91489df570ac</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="str">
-        <v>C2</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>840b43ba-b87d-4264-84c9-1dc5d5938540</v>
-      </c>
-      <c r="B10" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C10" t="str">
-        <v>b57be3ad-f74f-4f2b-aa79-6e410d2c199b</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="str">
-        <v>C1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>d1ab6da5-7837-4eef-8547-ea7ff17f58c3</v>
-      </c>
-      <c r="B11" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C11" t="str">
-        <v>50b3a8f6-823f-477c-b52d-5b4fba4edbd2</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="str">
-        <v>D1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>28f83ab1-3a7e-4e9b-82bf-7e37383d13ff</v>
-      </c>
-      <c r="B12" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C12" t="str">
-        <v>a3199cca-1aa6-4060-b6cd-0320712376ba</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" t="str">
-        <v>D2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>b55d9cdb-874f-4133-91b3-10f1ac5810e2</v>
-      </c>
-      <c r="B13" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C13" t="str">
-        <v>6116506f-31f1-444e-bd83-2991a5335470</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="str">
-        <v>E3</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>bc9f9233-1d8e-4fc9-9d80-21737c57f5f6</v>
-      </c>
-      <c r="B14" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C14" t="str">
-        <v>17e4dd39-8810-472c-b1a9-52382fbe0c79</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="str">
-        <v>E2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>ba25a5c3-0c4c-42fb-a6cf-8891cc5befd8</v>
-      </c>
-      <c r="B15" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C15" t="str">
-        <v>36fd980a-62d1-491b-97d6-079c33195e3d</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="str">
-        <v>E1</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H15"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11747,7 +11468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B39"/>
   <sheetViews>
@@ -12073,7 +11794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -12465,7 +12186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Distinguish standby contestants on the seating chart with a new color
Adds a `wasStandby` boolean to `SeatData` and updates styling logic in `SeatCard` to apply purple (#f3e8ff background, #9333ea border) when `wasStandby` is true. Backend logic in `routes.ts` now identifies seated standby contestants.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f123b9d7-6af8-472a-a75c-70d0b78d0583
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 2dbf69b7-1eed-4fd1-86e0-101f1bd7c590
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/f123b9d7-6af8-472a-a75c-70d0b78d0583/6I5ulvT
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,10 +5,11 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
-    <sheet name="Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
-    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
+    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
+    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
+    <sheet name="Groups" sheetId="5" r:id="rId5"/>
+    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -11411,6 +11412,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Block</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="F1" t="str">
+        <v>BookingEmailSent</v>
+      </c>
+      <c r="G1" t="str">
+        <v>ConfirmedRSVP</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>8a50bf67-8261-4ac0-ab7c-72c9fc4c6559</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2" t="str">
+        <v>E3</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11435,13 +11493,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>a11b3754-0163-43a3-8112-793c87694f2e</v>
+        <v>31d2ce8a-617f-451e-a2a4-9a92fc3f17e2</v>
       </c>
       <c r="B2" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
+        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
       </c>
       <c r="D2" t="str">
         <v>seated</v>
@@ -11449,16 +11507,16 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>31d2ce8a-617f-451e-a2a4-9a92fc3f17e2</v>
+        <v>a11b3754-0163-43a3-8112-793c87694f2e</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
+        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
       </c>
       <c r="D3" t="str">
-        <v>pending</v>
+        <v>seated</v>
       </c>
     </row>
   </sheetData>
@@ -11468,7 +11526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B39"/>
   <sheetViews>
@@ -11794,7 +11852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -12186,7 +12244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Lock producer dropdown when record day is locked
Update SeatingChartPage to disable the producer dropdown when the record day is locked. Reset seat assignments and standby status in backup data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f123b9d7-6af8-472a-a75c-70d0b78d0583
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: e8b2dd54-22a2-44d2-ba17-c1b0163964f5
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/f123b9d7-6af8-472a-a75c-70d0b78d0583/6I5ulvT
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,11 +5,10 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
-    <sheet name="Groups" sheetId="5" r:id="rId5"/>
-    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
-    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
+    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -2809,7 +2808,7 @@
         <v>A</v>
       </c>
       <c r="I61" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J61" t="str">
         <v>Olivia Gonzalez</v>
@@ -11412,63 +11411,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Block</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Seat</v>
-      </c>
-      <c r="F1" t="str">
-        <v>BookingEmailSent</v>
-      </c>
-      <c r="G1" t="str">
-        <v>ConfirmedRSVP</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>8a50bf67-8261-4ac0-ab7c-72c9fc4c6559</v>
-      </c>
-      <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2" t="str">
-        <v>E3</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11502,7 +11444,7 @@
         <v>40c53847-674f-43b5-8678-2decb3d42133</v>
       </c>
       <c r="D2" t="str">
-        <v>seated</v>
+        <v>pending</v>
       </c>
     </row>
     <row r="3">
@@ -11526,7 +11468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B39"/>
   <sheetViews>
@@ -11852,7 +11794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -12244,7 +12186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add standby mode to booking master and update backup data
Introduce a standby mode toggle in the booking master interface, allowing users to view and manage standby contestants without seat allocation. This commit also includes updates to the automatic backup files for record days and block types to reflect new data structures and entries.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f123b9d7-6af8-472a-a75c-70d0b78d0583
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: 91c66823-00da-4f1e-8619-50aa31082162
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/f123b9d7-6af8-472a-a75c-70d0b78d0583/6I5ulvT
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -427,27 +427,27 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-02-05</v>
+        <v>2026-02-04</v>
       </c>
       <c r="C2" t="str">
-        <v>RX EP 6 - 10</v>
+        <v>RX EP 1 - 5</v>
       </c>
       <c r="D2" t="str">
-        <v>draft</v>
+        <v>ready</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-02-06</v>
+        <v>2026-02-05</v>
       </c>
       <c r="C3" t="str">
-        <v>RX EP 11 - 15</v>
+        <v>RX EP 6 - 10</v>
       </c>
       <c r="D3" t="str">
         <v>draft</v>
@@ -455,13 +455,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-02-09</v>
+        <v>2026-02-06</v>
       </c>
       <c r="C4" t="str">
-        <v>RX EP 16 - 20</v>
+        <v>RX EP 11 - 15</v>
       </c>
       <c r="D4" t="str">
         <v>draft</v>
@@ -469,13 +469,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2ee609d2-1a2d-440c-801d-0eb0bfc47a2f</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-02-10</v>
+        <v>2026-02-09</v>
       </c>
       <c r="C5" t="str">
-        <v>RX EP 21 - 25</v>
+        <v>RX EP 16 - 20</v>
       </c>
       <c r="D5" t="str">
         <v>draft</v>
@@ -483,13 +483,13 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>59f9cd94-162d-413c-9797-5a881676a706</v>
+        <v>2ee609d2-1a2d-440c-801d-0eb0bfc47a2f</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-02-11</v>
+        <v>2026-02-10</v>
       </c>
       <c r="C6" t="str">
-        <v>RX EP 26 - 30</v>
+        <v>RX EP 21 - 25</v>
       </c>
       <c r="D6" t="str">
         <v>draft</v>
@@ -497,13 +497,13 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>c68366bd-1541-45fc-a22f-47ef139f16ec</v>
+        <v>59f9cd94-162d-413c-9797-5a881676a706</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-02-17</v>
+        <v>2026-02-11</v>
       </c>
       <c r="C7" t="str">
-        <v>RX EP 31 - 35</v>
+        <v>RX EP 26 - 30</v>
       </c>
       <c r="D7" t="str">
         <v>draft</v>
@@ -511,13 +511,13 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
+        <v>c68366bd-1541-45fc-a22f-47ef139f16ec</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-02-18</v>
+        <v>2026-02-17</v>
       </c>
       <c r="C8" t="str">
-        <v>RX EP 36 - 40</v>
+        <v>RX EP 31 - 35</v>
       </c>
       <c r="D8" t="str">
         <v>draft</v>
@@ -525,13 +525,13 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>04617609-04e6-4fa6-8023-ff7dede3c93a</v>
+        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-02-19</v>
+        <v>2026-02-18</v>
       </c>
       <c r="C9" t="str">
-        <v>RX EP 41 - 45</v>
+        <v>RX EP 36 - 40</v>
       </c>
       <c r="D9" t="str">
         <v>draft</v>
@@ -539,13 +539,13 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>80991c27-1587-4869-be9c-dc2a96950499</v>
+        <v>04617609-04e6-4fa6-8023-ff7dede3c93a</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-02-20</v>
+        <v>2026-02-19</v>
       </c>
       <c r="C10" t="str">
-        <v>RX EP 46 - 50</v>
+        <v>RX EP 41 - 45</v>
       </c>
       <c r="D10" t="str">
         <v>draft</v>
@@ -553,13 +553,13 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>274e9d90-48a5-404b-af78-739e1457158d</v>
+        <v>80991c27-1587-4869-be9c-dc2a96950499</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-02-24</v>
+        <v>2026-02-20</v>
       </c>
       <c r="C11" t="str">
-        <v>RX EP 51 - 55</v>
+        <v>RX EP 46 - 50</v>
       </c>
       <c r="D11" t="str">
         <v>draft</v>
@@ -567,13 +567,13 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>dcf33543-4096-425f-a8a1-2015851bd687</v>
+        <v>274e9d90-48a5-404b-af78-739e1457158d</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-02-25</v>
+        <v>2026-02-24</v>
       </c>
       <c r="C12" t="str">
-        <v>RX EP 56 - 60</v>
+        <v>RX EP 51 - 55</v>
       </c>
       <c r="D12" t="str">
         <v>draft</v>
@@ -581,13 +581,13 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>d3473fc2-fb62-4612-ae98-bf4765ba61e4</v>
+        <v>dcf33543-4096-425f-a8a1-2015851bd687</v>
       </c>
       <c r="B13" t="str">
-        <v>2026-02-26</v>
+        <v>2026-02-25</v>
       </c>
       <c r="C13" t="str">
-        <v>RX EP 61 - 65</v>
+        <v>RX EP 56 - 60</v>
       </c>
       <c r="D13" t="str">
         <v>draft</v>
@@ -595,13 +595,13 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>48bf0bd2-280f-44ac-806d-f1ae9f44712a</v>
+        <v>d3473fc2-fb62-4612-ae98-bf4765ba61e4</v>
       </c>
       <c r="B14" t="str">
-        <v>2026-03-02</v>
+        <v>2026-02-26</v>
       </c>
       <c r="C14" t="str">
-        <v>RX EP 66 - 70</v>
+        <v>RX EP 61 - 65</v>
       </c>
       <c r="D14" t="str">
         <v>draft</v>
@@ -609,13 +609,13 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>d06d32c7-51a5-4efd-9234-75c79c7c72d6</v>
+        <v>48bf0bd2-280f-44ac-806d-f1ae9f44712a</v>
       </c>
       <c r="B15" t="str">
-        <v>2026-03-03</v>
+        <v>2026-03-02</v>
       </c>
       <c r="C15" t="str">
-        <v>RX EP 71 - 75</v>
+        <v>RX EP 66 - 70</v>
       </c>
       <c r="D15" t="str">
         <v>draft</v>
@@ -623,13 +623,13 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>1da0c632-a3e1-46c0-8e8a-37753630608a</v>
+        <v>d06d32c7-51a5-4efd-9234-75c79c7c72d6</v>
       </c>
       <c r="B16" t="str">
-        <v>2026-03-04</v>
+        <v>2026-03-03</v>
       </c>
       <c r="C16" t="str">
-        <v>RX EP 76 - 80</v>
+        <v>RX EP 71 - 75</v>
       </c>
       <c r="D16" t="str">
         <v>draft</v>
@@ -637,13 +637,13 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>f159ca53-ea3d-4568-9403-7f15cd73dac8</v>
+        <v>1da0c632-a3e1-46c0-8e8a-37753630608a</v>
       </c>
       <c r="B17" t="str">
-        <v>2026-03-05</v>
+        <v>2026-03-04</v>
       </c>
       <c r="C17" t="str">
-        <v>RX EP 81 - 85</v>
+        <v>RX EP 76 - 80</v>
       </c>
       <c r="D17" t="str">
         <v>draft</v>
@@ -651,16 +651,16 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>f159ca53-ea3d-4568-9403-7f15cd73dac8</v>
       </c>
       <c r="B18" t="str">
-        <v>2026-02-04</v>
+        <v>2026-03-05</v>
       </c>
       <c r="C18" t="str">
-        <v>RX EP 1 - 5</v>
+        <v>RX EP 81 - 85</v>
       </c>
       <c r="D18" t="str">
-        <v>ready</v>
+        <v>draft</v>
       </c>
     </row>
   </sheetData>
@@ -11817,13 +11817,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>4d9813bd-7b99-4771-8da1-ad6fa01c1c6a</v>
+        <v>b248391e-18a0-4a53-bb54-8a0953ee2107</v>
       </c>
       <c r="B2" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="str">
         <v>PB</v>
@@ -11831,41 +11831,41 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>0aa42536-5b93-4be9-b0f5-95b1834f5cbf</v>
+        <v>60ae8d96-a0a8-4bf5-ab37-7d9bbc68104a</v>
       </c>
       <c r="B3" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="str">
-        <v>NPB</v>
+        <v>PB</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>ecc52a7a-af9e-483f-acfd-a9f947700b0c</v>
+        <v>19e49e78-cb04-48f1-b38c-1b5ae955926c</v>
       </c>
       <c r="B4" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" t="str">
-        <v>PB</v>
+        <v>NPB</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>d549fe45-cf7d-48a4-80c8-ad5d61aff471</v>
+        <v>ff774508-8faa-437d-b90c-98020b4fce99</v>
       </c>
       <c r="B5" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" t="str">
         <v>PB</v>
@@ -11873,38 +11873,38 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>9a62a9c4-3466-4b55-b61e-18cd2c67c4c1</v>
+        <v>a2d47c69-208d-44d2-9033-3b6ab96616bd</v>
       </c>
       <c r="B6" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6" t="str">
-        <v>NPB</v>
+        <v>PB</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>5b28e1f6-5c8a-4113-8834-9e8ab82228d6</v>
+        <v>d1e4b23c-d687-4444-8a8d-c54032f59162</v>
       </c>
       <c r="B7" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" t="str">
-        <v>PB</v>
+        <v>NPB</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>1d8f41b4-ac68-4c0d-89d5-3b22e715bc79</v>
+        <v>51e9e36b-3d3e-42bb-87d4-4f6a5085828d</v>
       </c>
       <c r="B8" t="str">
-        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -11915,10 +11915,10 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>ef4554b1-e13a-4273-b9e6-c22d7e345256</v>
+        <v>4d9813bd-7b99-4771-8da1-ad6fa01c1c6a</v>
       </c>
       <c r="B9" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -11929,10 +11929,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>a679d473-0969-4bba-8648-2709c720fd24</v>
+        <v>0aa42536-5b93-4be9-b0f5-95b1834f5cbf</v>
       </c>
       <c r="B10" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -11943,10 +11943,10 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>4ef50f67-0475-4c43-9591-c16952e5bb9d</v>
+        <v>ecc52a7a-af9e-483f-acfd-a9f947700b0c</v>
       </c>
       <c r="B11" t="str">
-        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -11957,13 +11957,13 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>10be29ee-cd87-4370-993f-5ec424bdf89a</v>
+        <v>d549fe45-cf7d-48a4-80c8-ad5d61aff471</v>
       </c>
       <c r="B12" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="str">
         <v>PB</v>
@@ -11971,41 +11971,41 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>5a87fc3a-f172-456c-8817-1d2e9f749c41</v>
+        <v>9a62a9c4-3466-4b55-b61e-18cd2c67c4c1</v>
       </c>
       <c r="B13" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
       <c r="D13" t="str">
-        <v>PB</v>
+        <v>NPB</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>ae5c8cf8-cd08-4a5b-9aa5-fdcd1f521fec</v>
+        <v>5b28e1f6-5c8a-4113-8834-9e8ab82228d6</v>
       </c>
       <c r="B14" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D14" t="str">
-        <v>NPB</v>
+        <v>PB</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>932323f8-f98a-4463-9650-1af4327df3a0</v>
+        <v>1d8f41b4-ac68-4c0d-89d5-3b22e715bc79</v>
       </c>
       <c r="B15" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>8de562bb-e594-47dd-a50f-ee78c14c0dde</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D15" t="str">
         <v>PB</v>
@@ -12013,13 +12013,13 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>53eb80a7-59e5-4b78-b5f0-a3b366587096</v>
+        <v>ef4554b1-e13a-4273-b9e6-c22d7e345256</v>
       </c>
       <c r="B16" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" t="str">
         <v>PB</v>
@@ -12027,41 +12027,41 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>690c620f-62d8-4293-b265-ce93eda1b896</v>
+        <v>a679d473-0969-4bba-8648-2709c720fd24</v>
       </c>
       <c r="B17" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="str">
-        <v>PB</v>
+        <v>NPB</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>306f44e0-79d0-424a-9eb7-126bbf71f301</v>
+        <v>4ef50f67-0475-4c43-9591-c16952e5bb9d</v>
       </c>
       <c r="B18" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>4ca4a7ea-c1ac-44e5-9533-fdd34522899d</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" t="str">
-        <v>NPB</v>
+        <v>PB</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>badc1981-587e-4ebe-a4ca-d09f25a98a6b</v>
+        <v>10be29ee-cd87-4370-993f-5ec424bdf89a</v>
       </c>
       <c r="B19" t="str">
-        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D19" t="str">
         <v>PB</v>
@@ -12069,13 +12069,13 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>321d3111-fcc3-4246-8800-231133dd823d</v>
+        <v>5a87fc3a-f172-456c-8817-1d2e9f749c41</v>
       </c>
       <c r="B20" t="str">
-        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D20" t="str">
         <v>PB</v>
@@ -12083,27 +12083,27 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>b248391e-18a0-4a53-bb54-8a0953ee2107</v>
+        <v>ae5c8cf8-cd08-4a5b-9aa5-fdcd1f521fec</v>
       </c>
       <c r="B21" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D21" t="str">
-        <v>PB</v>
+        <v>NPB</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>60ae8d96-a0a8-4bf5-ab37-7d9bbc68104a</v>
+        <v>932323f8-f98a-4463-9650-1af4327df3a0</v>
       </c>
       <c r="B22" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" t="str">
         <v>PB</v>
@@ -12111,27 +12111,27 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>19e49e78-cb04-48f1-b38c-1b5ae955926c</v>
+        <v>53eb80a7-59e5-4b78-b5f0-a3b366587096</v>
       </c>
       <c r="B23" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23" t="str">
-        <v>NPB</v>
+        <v>PB</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>ff774508-8faa-437d-b90c-98020b4fce99</v>
+        <v>690c620f-62d8-4293-b265-ce93eda1b896</v>
       </c>
       <c r="B24" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D24" t="str">
         <v>PB</v>
@@ -12139,41 +12139,41 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>a2d47c69-208d-44d2-9033-3b6ab96616bd</v>
+        <v>306f44e0-79d0-424a-9eb7-126bbf71f301</v>
       </c>
       <c r="B25" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="str">
-        <v>PB</v>
+        <v>NPB</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>d1e4b23c-d687-4444-8a8d-c54032f59162</v>
+        <v>badc1981-587e-4ebe-a4ca-d09f25a98a6b</v>
       </c>
       <c r="B26" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D26" t="str">
-        <v>NPB</v>
+        <v>PB</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>51e9e36b-3d3e-42bb-87d4-4f6a5085828d</v>
+        <v>321d3111-fcc3-4246-8800-231133dd823d</v>
       </c>
       <c r="B27" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>eec54567-3e21-424c-8d62-28772c0a6c25</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D27" t="str">
         <v>PB</v>
@@ -12212,71 +12212,71 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>03f5c6b5-b47c-40de-9554-c0d6fb75930b</v>
+        <v>8408c349-ac9b-49ab-989d-44cfabae6ca5</v>
       </c>
       <c r="B2" t="str">
-        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C2" t="str">
-        <v>6366884b-6583-493e-80bc-a1dff1926c59</v>
+        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
       </c>
       <c r="D2" t="str">
-        <v>Cant do feb - book in march onwards</v>
+        <v>.</v>
       </c>
       <c r="E2" s="1">
-        <v>46001.254457083334</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>46004.18743818287</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>8408c349-ac9b-49ab-989d-44cfabae6ca5</v>
+        <v>fa4948a9-b0d8-40b2-a711-a69c078b430f</v>
       </c>
       <c r="B3" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C3" t="str">
-        <v>b2c7422d-5caa-41a4-8352-77a36b30b055</v>
-      </c>
-      <c r="D3" t="str">
-        <v>.</v>
+        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
+      </c>
+      <c r="D3" t="str" xml:space="preserve">
+        <v xml:space="preserve">Rebook from March
+</v>
       </c>
       <c r="E3" s="1">
-        <v>46004.18743818287</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
+        <v>46003.218646828704</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="str">
-        <v>fa4948a9-b0d8-40b2-a711-a69c078b430f</v>
+        <v>95999c56-5e18-4ae1-a665-5628a8b3082b</v>
       </c>
       <c r="B4" t="str">
         <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
       </c>
       <c r="C4" t="str">
-        <v>4f5756e4-c006-4d04-a9bc-7a2de0fdf149</v>
-      </c>
-      <c r="D4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Rebook from March
-</v>
+        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Standby - eligible for reschedule</v>
       </c>
       <c r="E4" s="1">
-        <v>46003.218646828704</v>
+        <v>46001.26070648148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>95999c56-5e18-4ae1-a665-5628a8b3082b</v>
+        <v>03f5c6b5-b47c-40de-9554-c0d6fb75930b</v>
       </c>
       <c r="B5" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+        <v>abce05e1-0917-4949-a374-ef5f941df712</v>
       </c>
       <c r="C5" t="str">
-        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
+        <v>6366884b-6583-493e-80bc-a1dff1926c59</v>
       </c>
       <c r="D5" t="str">
-        <v>Standby - eligible for reschedule</v>
+        <v>Cant do feb - book in march onwards</v>
       </c>
       <c r="E5" s="1">
-        <v>46001.26070648148</v>
+        <v>46001.254457083334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Highlight standby contestants moved into seats with purple coloring
Update frontend row styling to use `wasStandby` boolean for highlighting seated standbys in the booking master.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f123b9d7-6af8-472a-a75c-70d0b78d0583
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 8e6401e0-8b01-4fe1-a9cc-c264706cba1e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/f123b9d7-6af8-472a-a75c-70d0b78d0583/6I5ulvT
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,10 +5,11 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
-    <sheet name="Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
-    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
+    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
+    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
+    <sheet name="Groups" sheetId="5" r:id="rId5"/>
+    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -2808,7 +2809,7 @@
         <v>A</v>
       </c>
       <c r="I61" t="str">
-        <v>available</v>
+        <v>assigned</v>
       </c>
       <c r="J61" t="str">
         <v>Olivia Gonzalez</v>
@@ -11411,6 +11412,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>RecordDayID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ContestantID</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Block</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="F1" t="str">
+        <v>BookingEmailSent</v>
+      </c>
+      <c r="G1" t="str">
+        <v>ConfirmedRSVP</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>b48e7d62-bac6-46c6-ac16-28cb999e41ad</v>
+      </c>
+      <c r="B2" t="str">
+        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2" t="str">
+        <v>E4</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11444,7 +11502,7 @@
         <v>40c53847-674f-43b5-8678-2decb3d42133</v>
       </c>
       <c r="D2" t="str">
-        <v>pending</v>
+        <v>seated</v>
       </c>
     </row>
     <row r="3">
@@ -11468,7 +11526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B39"/>
   <sheetViews>
@@ -11794,7 +11852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -12186,7 +12244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Improve cursor accuracy when moving standbys on the seating chart
Add a DragOverlay for standbys and disable drop animations to ensure accurate cursor tracking during drag-and-drop operations.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f123b9d7-6af8-472a-a75c-70d0b78d0583
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: b6567325-3196-4ce7-8c52-b33d8ed0f449
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/f123b9d7-6af8-472a-a75c-70d0b78d0583/6I5ulvT
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -1248,57 +1248,63 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
+        <v>f445658c-a35b-4a62-baa4-1661e03155bf</v>
       </c>
       <c r="B17" t="str">
-        <v>Olivia Gonzalez</v>
+        <v>Wadzanayi Chitambo</v>
       </c>
       <c r="C17">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D17" t="str">
         <v>Female</v>
       </c>
       <c r="E17" t="str">
-        <v>olivia.gonzalez77@hotmail.com</v>
+        <v>wadzichitambo@gmail.com</v>
       </c>
       <c r="F17" t="str">
-        <v>(982) 690-7408</v>
+        <v>415052242</v>
       </c>
       <c r="G17" t="str">
-        <v>Long Beach</v>
+        <v>Pascoe Vale South</v>
       </c>
       <c r="H17" t="str">
         <v>B+</v>
       </c>
       <c r="I17" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J17" t="str">
-        <v>Eliana Green</v>
+        <v>Ashlee Skrzelinski</v>
+      </c>
+      <c r="K17" t="str">
+        <v>daa8fd8b-8af2-4382-9127-051623496ba7</v>
+      </c>
+      <c r="M17" t="str">
+        <v>NA</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>f445658c-a35b-4a62-baa4-1661e03155bf</v>
+        <v>35b50f34-12bf-4c1c-b6c2-391130aa3d18</v>
       </c>
       <c r="B18" t="str">
-        <v>Wadzanayi Chitambo</v>
+        <v>Corbin Eather</v>
       </c>
       <c r="C18">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D18" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E18" t="str">
-        <v>wadzichitambo@gmail.com</v>
+        <v>Corby1909@hotmail.com</v>
       </c>
       <c r="F18" t="str">
-        <v>415052242</v>
+        <v>487992952</v>
       </c>
       <c r="G18" t="str">
-        <v>Pascoe Vale South</v>
+        <v>Portland</v>
       </c>
       <c r="H18" t="str">
         <v>B+</v>
@@ -1307,141 +1313,138 @@
         <v>available</v>
       </c>
       <c r="J18" t="str">
-        <v>Ashlee Skrzelinski</v>
+        <v>SOLO</v>
       </c>
       <c r="K18" t="str">
-        <v>daa8fd8b-8af2-4382-9127-051623496ba7</v>
-      </c>
-      <c r="M18" t="str">
-        <v>NA</v>
+        <v>65d7aafc-81dc-4167-9597-567ea7a89170</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>35b50f34-12bf-4c1c-b6c2-391130aa3d18</v>
+        <v>5e5010fe-f694-44c1-a8d2-e4cc4a2d05b9</v>
       </c>
       <c r="B19" t="str">
-        <v>Corbin Eather</v>
+        <v>Charlie Davidson</v>
       </c>
       <c r="C19">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D19" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E19" t="str">
-        <v>Corby1909@hotmail.com</v>
+        <v>Charlieisabelle8@gmail.com</v>
       </c>
       <c r="F19" t="str">
-        <v>487992952</v>
+        <v>404109356</v>
       </c>
       <c r="G19" t="str">
-        <v>Portland</v>
+        <v>Ringwood</v>
       </c>
       <c r="H19" t="str">
-        <v>B+</v>
+        <v>B</v>
       </c>
       <c r="I19" t="str">
         <v>available</v>
       </c>
       <c r="J19" t="str">
-        <v>SOLO</v>
+        <v>Corey Mcormond, Charlie Davidson</v>
       </c>
       <c r="K19" t="str">
-        <v>65d7aafc-81dc-4167-9597-567ea7a89170</v>
+        <v>0968969b-26ec-43d9-a744-b41541fbb225</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>5e5010fe-f694-44c1-a8d2-e4cc4a2d05b9</v>
+        <v>42d96626-bafe-4dec-8c66-a44c22fdc359</v>
       </c>
       <c r="B20" t="str">
-        <v>Charlie Davidson</v>
+        <v>Daniel Montalto</v>
       </c>
       <c r="C20">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D20" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E20" t="str">
-        <v>Charlieisabelle8@gmail.com</v>
+        <v>Montecarr91@gmail.com</v>
       </c>
       <c r="F20" t="str">
-        <v>404109356</v>
+        <v>401883434</v>
       </c>
       <c r="G20" t="str">
-        <v>Ringwood</v>
+        <v xml:space="preserve">Melbourne </v>
       </c>
       <c r="H20" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I20" t="str">
         <v>available</v>
       </c>
       <c r="J20" t="str">
-        <v>Corey Mcormond, Charlie Davidson</v>
+        <v>maree montalto</v>
       </c>
       <c r="K20" t="str">
-        <v>0968969b-26ec-43d9-a744-b41541fbb225</v>
+        <v>e352b4d8-3eeb-4f15-9257-317bb0a46dde</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>42d96626-bafe-4dec-8c66-a44c22fdc359</v>
+        <v>f15ce3f4-a66b-445b-a168-2a6dc069b8c3</v>
       </c>
       <c r="B21" t="str">
-        <v>Daniel Montalto</v>
+        <v>Glenda  Fleming</v>
       </c>
       <c r="C21">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D21" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E21" t="str">
-        <v>Montecarr91@gmail.com</v>
+        <v>glendafleming@bigpond.com</v>
       </c>
       <c r="F21" t="str">
-        <v>401883434</v>
+        <v>400967493</v>
       </c>
       <c r="G21" t="str">
-        <v xml:space="preserve">Melbourne </v>
+        <v xml:space="preserve">Nambrok </v>
       </c>
       <c r="H21" t="str">
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="I21" t="str">
         <v>available</v>
       </c>
       <c r="J21" t="str">
-        <v>maree montalto</v>
+        <v>Steven Fleming, Kye Embrey, Glenda Fleming</v>
       </c>
       <c r="K21" t="str">
-        <v>e352b4d8-3eeb-4f15-9257-317bb0a46dde</v>
+        <v>fb2c36e3-f601-41a8-8c3a-c62b9e0c9902</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>f15ce3f4-a66b-445b-a168-2a6dc069b8c3</v>
+        <v>3f912084-15ed-4cf2-a9bd-69808d91878e</v>
       </c>
       <c r="B22" t="str">
-        <v>Glenda  Fleming</v>
+        <v>Cazz Chandler</v>
       </c>
       <c r="C22">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D22" t="str">
         <v>Female</v>
       </c>
       <c r="E22" t="str">
-        <v>glendafleming@bigpond.com</v>
+        <v>cazzchandler@gmail.com</v>
       </c>
       <c r="F22" t="str">
-        <v>400967493</v>
+        <v>408538891</v>
       </c>
       <c r="G22" t="str">
-        <v xml:space="preserve">Nambrok </v>
+        <v>Edithvale</v>
       </c>
       <c r="H22" t="str">
         <v>B+</v>
@@ -1450,33 +1453,33 @@
         <v>available</v>
       </c>
       <c r="J22" t="str">
-        <v>Steven Fleming, Kye Embrey, Glenda Fleming</v>
+        <v>Gabby Chandler</v>
       </c>
       <c r="K22" t="str">
-        <v>fb2c36e3-f601-41a8-8c3a-c62b9e0c9902</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>6dcdeddf-c5a3-4ee4-aef0-0ec71e6fea37</v>
+      </c>
+    </row>
+    <row r="23" xml:space="preserve">
       <c r="A23" t="str">
-        <v>3f912084-15ed-4cf2-a9bd-69808d91878e</v>
+        <v>cec35e1e-b6fa-4f31-a961-a4484c3ba77a</v>
       </c>
       <c r="B23" t="str">
-        <v>Cazz Chandler</v>
+        <v>Grace Bee</v>
       </c>
       <c r="C23">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D23" t="str">
         <v>Female</v>
       </c>
       <c r="E23" t="str">
-        <v>cazzchandler@gmail.com</v>
+        <v>graceyybee@gmail.com</v>
       </c>
       <c r="F23" t="str">
-        <v>408538891</v>
+        <v>426996862</v>
       </c>
       <c r="G23" t="str">
-        <v>Edithvale</v>
+        <v>Geelong</v>
       </c>
       <c r="H23" t="str">
         <v>B+</v>
@@ -1484,218 +1487,218 @@
       <c r="I23" t="str">
         <v>available</v>
       </c>
-      <c r="J23" t="str">
-        <v>Gabby Chandler</v>
-      </c>
-      <c r="K23" t="str">
-        <v>6dcdeddf-c5a3-4ee4-aef0-0ec71e6fea37</v>
-      </c>
-    </row>
-    <row r="24" xml:space="preserve">
-      <c r="A24" t="str">
-        <v>cec35e1e-b6fa-4f31-a961-a4484c3ba77a</v>
-      </c>
-      <c r="B24" t="str">
-        <v>Grace Bee</v>
-      </c>
-      <c r="C24">
-        <v>20</v>
-      </c>
-      <c r="D24" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E24" t="str">
-        <v>graceyybee@gmail.com</v>
-      </c>
-      <c r="F24" t="str">
-        <v>426996862</v>
-      </c>
-      <c r="G24" t="str">
-        <v>Geelong</v>
-      </c>
-      <c r="H24" t="str">
-        <v>B+</v>
-      </c>
-      <c r="I24" t="str">
-        <v>available</v>
-      </c>
-      <c r="J24" t="str" xml:space="preserve">
+      <c r="J23" t="str" xml:space="preserve">
         <v xml:space="preserve">Friends_x000d_
 Grace Bee_x000d_
 Klara Nuc-Kraljak</v>
       </c>
+      <c r="K23" t="str">
+        <v>26b75180-660d-4b2d-8e59-da58bf4ed2b9</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>299508d3-5643-4142-833b-a85b93e42b8c</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Maddy Rottinger</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E24" t="str">
+        <v>maddyrottinger@gmail.com</v>
+      </c>
+      <c r="F24" t="str">
+        <v>449812432</v>
+      </c>
+      <c r="G24" t="str">
+        <v xml:space="preserve">Melbourne </v>
+      </c>
+      <c r="H24" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I24" t="str">
+        <v>available</v>
+      </c>
+      <c r="J24" t="str">
+        <v>Maddy Rottinger, David Rottinger</v>
+      </c>
       <c r="K24" t="str">
-        <v>26b75180-660d-4b2d-8e59-da58bf4ed2b9</v>
+        <v>f1cb34d7-7872-4b03-b696-27dc9ecf6cf5</v>
+      </c>
+      <c r="L24" t="str">
+        <v xml:space="preserve">I have Autism but no need for any accommodation </v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>299508d3-5643-4142-833b-a85b93e42b8c</v>
+        <v>86f383a1-d202-4a69-b5d4-ae3c3580e928</v>
       </c>
       <c r="B25" t="str">
-        <v>Maddy Rottinger</v>
+        <v>Alessandro Amati</v>
       </c>
       <c r="C25">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D25" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E25" t="str">
-        <v>maddyrottinger@gmail.com</v>
+        <v>Alessandro.amati88@gmail.com</v>
       </c>
       <c r="F25" t="str">
-        <v>449812432</v>
+        <v xml:space="preserve">0414 080 042 </v>
       </c>
       <c r="G25" t="str">
         <v xml:space="preserve">Melbourne </v>
       </c>
       <c r="H25" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I25" t="str">
         <v>available</v>
       </c>
       <c r="J25" t="str">
-        <v>Maddy Rottinger, David Rottinger</v>
+        <v>Judy Robinet</v>
       </c>
       <c r="K25" t="str">
-        <v>f1cb34d7-7872-4b03-b696-27dc9ecf6cf5</v>
-      </c>
-      <c r="L25" t="str">
-        <v xml:space="preserve">I have Autism but no need for any accommodation </v>
+        <v>a18330d2-0770-499f-96f6-75e67e2a75d4</v>
+      </c>
+      <c r="M25" t="str">
+        <v>NA</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>86f383a1-d202-4a69-b5d4-ae3c3580e928</v>
+        <v>54083857-1734-43ee-a749-a567e1c8a0b0</v>
       </c>
       <c r="B26" t="str">
-        <v>Alessandro Amati</v>
+        <v>Jodi Kett</v>
       </c>
       <c r="C26">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D26" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E26" t="str">
-        <v>Alessandro.amati88@gmail.com</v>
+        <v>Jkett985@gmail.com</v>
       </c>
       <c r="F26" t="str">
-        <v xml:space="preserve">0414 080 042 </v>
+        <v>410716195</v>
       </c>
       <c r="G26" t="str">
-        <v xml:space="preserve">Melbourne </v>
+        <v>Lalor</v>
       </c>
       <c r="H26" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I26" t="str">
         <v>available</v>
       </c>
       <c r="J26" t="str">
-        <v>Judy Robinet</v>
+        <v>Wendy Manton</v>
       </c>
       <c r="K26" t="str">
-        <v>a18330d2-0770-499f-96f6-75e67e2a75d4</v>
-      </c>
-      <c r="M26" t="str">
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>cbf209b8-2a31-4cf9-bc54-83485fa4051d</v>
+      </c>
+    </row>
+    <row r="27" xml:space="preserve">
       <c r="A27" t="str">
-        <v>54083857-1734-43ee-a749-a567e1c8a0b0</v>
+        <v>6080cf05-adb5-4efe-974e-9b2317006ab4</v>
       </c>
       <c r="B27" t="str">
-        <v>Jodi Kett</v>
+        <v>Brooke Finn</v>
       </c>
       <c r="C27">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D27" t="str">
         <v>Female</v>
       </c>
       <c r="E27" t="str">
-        <v>Jkett985@gmail.com</v>
+        <v>Brookefinn13@gmail.com</v>
       </c>
       <c r="F27" t="str">
-        <v>410716195</v>
+        <v>447139482</v>
       </c>
       <c r="G27" t="str">
-        <v>Lalor</v>
+        <v>Geelong</v>
       </c>
       <c r="H27" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I27" t="str">
         <v>available</v>
       </c>
-      <c r="J27" t="str">
-        <v>Wendy Manton</v>
-      </c>
-      <c r="K27" t="str">
-        <v>cbf209b8-2a31-4cf9-bc54-83485fa4051d</v>
-      </c>
-    </row>
-    <row r="28" xml:space="preserve">
-      <c r="A28" t="str">
-        <v>6080cf05-adb5-4efe-974e-9b2317006ab4</v>
-      </c>
-      <c r="B28" t="str">
-        <v>Brooke Finn</v>
-      </c>
-      <c r="C28">
-        <v>27</v>
-      </c>
-      <c r="D28" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E28" t="str">
-        <v>Brookefinn13@gmail.com</v>
-      </c>
-      <c r="F28" t="str">
-        <v>447139482</v>
-      </c>
-      <c r="G28" t="str">
-        <v>Geelong</v>
-      </c>
-      <c r="H28" t="str">
-        <v>B+</v>
-      </c>
-      <c r="I28" t="str">
-        <v>available</v>
-      </c>
-      <c r="J28" t="str" xml:space="preserve">
+      <c r="J27" t="str" xml:space="preserve">
         <v xml:space="preserve">renee ullrich, brooke finn, Jemah Finn_x000d_
 </v>
       </c>
+      <c r="K27" t="str">
+        <v>67044596-c8f7-4375-a21f-2b0349eb7637</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>c43df161-b4c3-448c-a813-8636f1b5a4bd</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Sam Marden</v>
+      </c>
+      <c r="C28">
+        <v>46</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E28" t="str">
+        <v>sammarden@gmail.com</v>
+      </c>
+      <c r="F28" t="str">
+        <v xml:space="preserve">0452 037 334 </v>
+      </c>
+      <c r="G28" t="str">
+        <v xml:space="preserve">Chelsea </v>
+      </c>
+      <c r="H28" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I28" t="str">
+        <v>available</v>
+      </c>
+      <c r="J28" t="str">
+        <v>Sister - Janelle marden...she need sto apply</v>
+      </c>
       <c r="K28" t="str">
-        <v>67044596-c8f7-4375-a21f-2b0349eb7637</v>
+        <v>6ade295b-882d-462d-a68b-2d985302d9db</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>c43df161-b4c3-448c-a813-8636f1b5a4bd</v>
+        <v>56c75621-ec89-47b1-a7a0-9963b388b9e8</v>
       </c>
       <c r="B29" t="str">
-        <v>Sam Marden</v>
+        <v>Emily Leos</v>
       </c>
       <c r="C29">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="D29" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E29" t="str">
-        <v>sammarden@gmail.com</v>
+        <v>emilymarie.leos@gmail.com</v>
       </c>
       <c r="F29" t="str">
-        <v xml:space="preserve">0452 037 334 </v>
+        <v>415128111</v>
       </c>
       <c r="G29" t="str">
-        <v xml:space="preserve">Chelsea </v>
+        <v>Preston</v>
       </c>
       <c r="H29" t="str">
         <v>B+</v>
@@ -1704,42 +1707,42 @@
         <v>available</v>
       </c>
       <c r="J29" t="str">
-        <v>Sister - Janelle marden...she need sto apply</v>
+        <v>Ethan Bell</v>
       </c>
       <c r="K29" t="str">
-        <v>6ade295b-882d-462d-a68b-2d985302d9db</v>
+        <v>ff0b886a-f8ef-41e4-a628-3dabf997ba58</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>56c75621-ec89-47b1-a7a0-9963b388b9e8</v>
+        <v>fb165133-2b4f-4814-8d53-3ec6f3fed750</v>
       </c>
       <c r="B30" t="str">
-        <v>Emily Leos</v>
+        <v>Ethan Bell</v>
       </c>
       <c r="C30">
         <v>24</v>
       </c>
       <c r="D30" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E30" t="str">
-        <v>emilymarie.leos@gmail.com</v>
+        <v>e.bell2001@outlook.com.au</v>
       </c>
       <c r="F30" t="str">
-        <v>415128111</v>
+        <v>412377981</v>
       </c>
       <c r="G30" t="str">
-        <v>Preston</v>
+        <v>melbourne</v>
       </c>
       <c r="H30" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I30" t="str">
         <v>available</v>
       </c>
       <c r="J30" t="str">
-        <v>Ethan Bell</v>
+        <v>Emily Leos</v>
       </c>
       <c r="K30" t="str">
         <v>ff0b886a-f8ef-41e4-a628-3dabf997ba58</v>
@@ -1747,72 +1750,69 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>fb165133-2b4f-4814-8d53-3ec6f3fed750</v>
+        <v>d5609f39-77f4-40b0-a9e0-105f50805765</v>
       </c>
       <c r="B31" t="str">
-        <v>Ethan Bell</v>
+        <v>Carl Mikhail SEVILLANO</v>
       </c>
       <c r="C31">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" t="str">
         <v>Male</v>
       </c>
       <c r="E31" t="str">
-        <v>e.bell2001@outlook.com.au</v>
+        <v>mikkisevillano@gmail.com</v>
       </c>
       <c r="F31" t="str">
-        <v>412377981</v>
+        <v>424795297</v>
       </c>
       <c r="G31" t="str">
-        <v>melbourne</v>
+        <v>Sydenham</v>
       </c>
       <c r="H31" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I31" t="str">
         <v>available</v>
       </c>
       <c r="J31" t="str">
-        <v>Emily Leos</v>
+        <v>Carl Mikhail SEVILLANO, Jessica Newton, Carolina Sevillano, Manuel Sevillano</v>
       </c>
       <c r="K31" t="str">
-        <v>ff0b886a-f8ef-41e4-a628-3dabf997ba58</v>
+        <v>23259da3-85da-4d69-a2bc-f1e643c3e4a5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>d5609f39-77f4-40b0-a9e0-105f50805765</v>
+        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
       </c>
       <c r="B32" t="str">
-        <v>Carl Mikhail SEVILLANO</v>
+        <v>Olivia Gonzalez</v>
       </c>
       <c r="C32">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D32" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E32" t="str">
-        <v>mikkisevillano@gmail.com</v>
+        <v>olivia.gonzalez77@hotmail.com</v>
       </c>
       <c r="F32" t="str">
-        <v>424795297</v>
+        <v>(982) 690-7408</v>
       </c>
       <c r="G32" t="str">
-        <v>Sydenham</v>
+        <v>Long Beach</v>
       </c>
       <c r="H32" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="I32" t="str">
         <v>available</v>
       </c>
       <c r="J32" t="str">
-        <v>Carl Mikhail SEVILLANO, Jessica Newton, Carolina Sevillano, Manuel Sevillano</v>
-      </c>
-      <c r="K32" t="str">
-        <v>23259da3-85da-4d69-a2bc-f1e643c3e4a5</v>
+        <v>Eliana Green</v>
       </c>
     </row>
     <row r="33">
@@ -11469,7 +11469,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11505,23 +11505,9 @@
         <v>seated</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>a11b3754-0163-43a3-8112-793c87694f2e</v>
-      </c>
-      <c r="B3" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C3" t="str">
-        <v>40a64316-1fb5-4a09-8c9d-14bbc19036d1</v>
-      </c>
-      <c r="D3" t="str">
-        <v>seated</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Preserve paperwork status when rescheduling contestants to new dates
Modify routes and storage to carry over `paperworkSent` and `paperworkReceived` timestamps from canceled assignments to new seat assignments. Update `canceled_assignments` schema to include these fields.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f123b9d7-6af8-472a-a75c-70d0b78d0583
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 7570d25b-8171-4b54-9f82-17e2027223e7
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/f123b9d7-6af8-472a-a75c-70d0b78d0583/cV9bEaO
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -5,11 +5,10 @@
   <sheets>
     <sheet name="Record Days" sheetId="1" r:id="rId1"/>
     <sheet name="Contestants" sheetId="2" r:id="rId2"/>
-    <sheet name="Seat Assignments" sheetId="3" r:id="rId3"/>
-    <sheet name="Standbys" sheetId="4" r:id="rId4"/>
-    <sheet name="Groups" sheetId="5" r:id="rId5"/>
-    <sheet name="Block Types" sheetId="6" r:id="rId6"/>
-    <sheet name="Canceled Assignments" sheetId="7" r:id="rId7"/>
+    <sheet name="Standbys" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Block Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Canceled Assignments" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -2809,7 +2808,7 @@
         <v>A</v>
       </c>
       <c r="I61" t="str">
-        <v>assigned</v>
+        <v>available</v>
       </c>
       <c r="J61" t="str">
         <v>Olivia Gonzalez</v>
@@ -11412,63 +11411,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>RecordDayID</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ContestantID</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Block</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Seat</v>
-      </c>
-      <c r="F1" t="str">
-        <v>BookingEmailSent</v>
-      </c>
-      <c r="G1" t="str">
-        <v>ConfirmedRSVP</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Notes</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>b48e7d62-bac6-46c6-ac16-28cb999e41ad</v>
-      </c>
-      <c r="B2" t="str">
-        <v>e432f0fe-1383-44a2-990c-5f787da5008a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>40c53847-674f-43b5-8678-2decb3d42133</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2" t="str">
-        <v>E4</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11502,7 +11444,7 @@
         <v>40c53847-674f-43b5-8678-2decb3d42133</v>
       </c>
       <c r="D2" t="str">
-        <v>seated</v>
+        <v>pending</v>
       </c>
     </row>
   </sheetData>
@@ -11512,7 +11454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B39"/>
   <sheetViews>
@@ -11838,7 +11780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -12230,7 +12172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update booking master to show correct contestant statuses and assignments
Fixes the display of contestant statuses on the booking master page by mapping raw status values to user-friendly labels, and corrects contestant group assignments in the backup data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f123b9d7-6af8-472a-a75c-70d0b78d0583
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: d10d131c-daae-4288-9345-089ff7d56944
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4ca2a1f8-42ce-4303-beff-eb92e3283d4c/f123b9d7-6af8-472a-a75c-70d0b78d0583/lYwRcev
</commit_message>
<xml_diff>
--- a/storage/backups/automatic-backup.xlsx
+++ b/storage/backups/automatic-backup.xlsx
@@ -720,25 +720,25 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>87467196-8e6a-4aa4-a098-051eeae34713</v>
+        <v>5c3852ec-d7b5-4916-a398-829cd32746c6</v>
       </c>
       <c r="B2" t="str">
-        <v>Matthew Sjostrom</v>
+        <v>Maddie Streader</v>
       </c>
       <c r="C2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D2" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E2" t="str">
-        <v>mattbenko01@gmail.com</v>
+        <v>maddiestreader@outlook.com</v>
       </c>
       <c r="F2" t="str">
-        <v>451710041</v>
+        <v>413901065</v>
       </c>
       <c r="G2" t="str">
-        <v>Prahran</v>
+        <v>Doncaster</v>
       </c>
       <c r="H2" t="str">
         <v>B+</v>
@@ -747,132 +747,138 @@
         <v>available</v>
       </c>
       <c r="J2" t="str">
-        <v>Roxanne Benko, Matthew Sjostrom, Lauren Namua</v>
+        <v>Marc Cuspilli</v>
       </c>
       <c r="K2" t="str">
-        <v>5fe641da-4067-49a7-bae7-e63413b3e404</v>
+        <v>8a692ea1-5300-494c-8074-19f479c5284d</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>5c3852ec-d7b5-4916-a398-829cd32746c6</v>
+        <v>41823bfb-d4b8-402c-97f4-109282880398</v>
       </c>
       <c r="B3" t="str">
-        <v>Maddie Streader</v>
+        <v>Jynese Bernard</v>
       </c>
       <c r="C3">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D3" t="str">
         <v>Female</v>
       </c>
       <c r="E3" t="str">
-        <v>maddiestreader@outlook.com</v>
+        <v>LADEMOISELLE81@GMAIL.COM</v>
       </c>
       <c r="F3" t="str">
-        <v>413901065</v>
+        <v>422223257</v>
       </c>
       <c r="G3" t="str">
-        <v>Doncaster</v>
+        <v>Preston</v>
       </c>
       <c r="H3" t="str">
         <v>B+</v>
       </c>
       <c r="I3" t="str">
         <v>available</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Marc Cuspilli</v>
-      </c>
-      <c r="K3" t="str">
-        <v>8a692ea1-5300-494c-8074-19f479c5284d</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>41823bfb-d4b8-402c-97f4-109282880398</v>
+        <v>03349789-5ef5-461b-b37e-ceaa6d5bfed1</v>
       </c>
       <c r="B4" t="str">
-        <v>Jynese Bernard</v>
+        <v>Emma Hall</v>
       </c>
       <c r="C4">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D4" t="str">
         <v>Female</v>
       </c>
       <c r="E4" t="str">
-        <v>LADEMOISELLE81@GMAIL.COM</v>
+        <v>emmaj.hall@bigpond.com</v>
       </c>
       <c r="F4" t="str">
-        <v>422223257</v>
+        <v>433792195</v>
       </c>
       <c r="G4" t="str">
-        <v>Preston</v>
+        <v>Melbourne</v>
       </c>
       <c r="H4" t="str">
         <v>B+</v>
       </c>
       <c r="I4" t="str">
         <v>available</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Emma Hall, Emma Heine, Charlotte Hastie</v>
+      </c>
+      <c r="K4" t="str">
+        <v>6f3cbd80-aae5-463e-836b-f1ecf0c504a2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>03349789-5ef5-461b-b37e-ceaa6d5bfed1</v>
+        <v>c388f104-81db-45a7-a92d-a5c012b99daf</v>
       </c>
       <c r="B5" t="str">
-        <v>Emma Hall</v>
+        <v>Eva Irwin</v>
       </c>
       <c r="C5">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D5" t="str">
         <v>Female</v>
       </c>
       <c r="E5" t="str">
-        <v>emmaj.hall@bigpond.com</v>
+        <v>evairwin00@gmail.com</v>
       </c>
       <c r="F5" t="str">
-        <v>433792195</v>
+        <v>413427475</v>
       </c>
       <c r="G5" t="str">
-        <v>Melbourne</v>
+        <v>Spring Gully</v>
       </c>
       <c r="H5" t="str">
-        <v>B+</v>
+        <v>A</v>
       </c>
       <c r="I5" t="str">
         <v>available</v>
       </c>
       <c r="J5" t="str">
-        <v>Emma Hall, Emma Heine, Charlotte Hastie</v>
+        <v xml:space="preserve">Solo </v>
       </c>
       <c r="K5" t="str">
-        <v>6f3cbd80-aae5-463e-836b-f1ecf0c504a2</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>3e3161fd-95f1-4ce9-9810-0ab1d377e2b2</v>
+      </c>
+      <c r="L5" t="str">
+        <v>I’m currently in a moon boot, will be off it after the 2nd of April</v>
+      </c>
+      <c r="M5" t="str">
+        <v xml:space="preserve">No </v>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
       <c r="A6" t="str">
-        <v>c388f104-81db-45a7-a92d-a5c012b99daf</v>
+        <v>ffc26030-f308-47e2-b44e-448f1a6baffc</v>
       </c>
       <c r="B6" t="str">
-        <v>Eva Irwin</v>
+        <v>Kerry Wellington</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="D6" t="str">
         <v>Female</v>
       </c>
       <c r="E6" t="str">
-        <v>evairwin00@gmail.com</v>
+        <v>Kmaddernwellington@gmail.com</v>
       </c>
       <c r="F6" t="str">
-        <v>413427475</v>
+        <v>490757330</v>
       </c>
       <c r="G6" t="str">
-        <v>Spring Gully</v>
+        <v>Carrum</v>
       </c>
       <c r="H6" t="str">
         <v>A</v>
@@ -880,79 +886,67 @@
       <c r="I6" t="str">
         <v>available</v>
       </c>
-      <c r="J6" t="str">
-        <v xml:space="preserve">Solo </v>
-      </c>
-      <c r="K6" t="str">
-        <v>3e3161fd-95f1-4ce9-9810-0ab1d377e2b2</v>
-      </c>
-      <c r="L6" t="str">
-        <v>I’m currently in a moon boot, will be off it after the 2nd of April</v>
-      </c>
-      <c r="M6" t="str">
-        <v xml:space="preserve">No </v>
-      </c>
-    </row>
-    <row r="7" xml:space="preserve">
-      <c r="A7" t="str">
-        <v>ffc26030-f308-47e2-b44e-448f1a6baffc</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Kerry Wellington</v>
-      </c>
-      <c r="C7">
-        <v>60</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Kmaddernwellington@gmail.com</v>
-      </c>
-      <c r="F7" t="str">
-        <v>490757330</v>
-      </c>
-      <c r="G7" t="str">
-        <v>Carrum</v>
-      </c>
-      <c r="H7" t="str">
-        <v>A</v>
-      </c>
-      <c r="I7" t="str">
-        <v>available</v>
-      </c>
-      <c r="J7" t="str" xml:space="preserve">
+      <c r="J6" t="str" xml:space="preserve">
         <v xml:space="preserve">Would be a group of up to 8 ladies._x000d_
 Amanda Hobbs_x000d_
 Kerry Wellington_x000d_
 Edwina Muir_x000d_
 </v>
       </c>
-      <c r="K7" t="str">
+      <c r="K6" t="str">
         <v>5b77330c-45dc-4177-b704-50e8d2e75d75</v>
       </c>
     </row>
-    <row r="8">
+    <row r="7">
+      <c r="A7" t="str">
+        <v>40f872e2-b313-4e89-addc-bcfcbdce79aa</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Farrah King</v>
+      </c>
+      <c r="C7">
+        <v>43</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Cherrychikita@hotmail.com</v>
+      </c>
+      <c r="F7" t="str">
+        <v>401193923</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Hadfield</v>
+      </c>
+      <c r="H7" t="str">
+        <v>A</v>
+      </c>
+      <c r="I7" t="str">
+        <v>available</v>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
       <c r="A8" t="str">
-        <v>40f872e2-b313-4e89-addc-bcfcbdce79aa</v>
+        <v>711a9a1e-1b83-49e1-9c15-d494cdcf9796</v>
       </c>
       <c r="B8" t="str">
-        <v>Farrah King</v>
+        <v>Edwina Muir</v>
       </c>
       <c r="C8">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D8" t="str">
         <v>Female</v>
       </c>
       <c r="E8" t="str">
-        <v>Cherrychikita@hotmail.com</v>
+        <v>maeemuir@tpg.com.au</v>
       </c>
       <c r="F8" t="str">
-        <v>401193923</v>
+        <v>439781947</v>
       </c>
       <c r="G8" t="str">
-        <v>Hadfield</v>
+        <v>Mt Eliza</v>
       </c>
       <c r="H8" t="str">
         <v>A</v>
@@ -960,105 +954,111 @@
       <c r="I8" t="str">
         <v>available</v>
       </c>
-    </row>
-    <row r="9" xml:space="preserve">
-      <c r="A9" t="str">
-        <v>711a9a1e-1b83-49e1-9c15-d494cdcf9796</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Edwina Muir</v>
-      </c>
-      <c r="C9">
-        <v>58</v>
-      </c>
-      <c r="D9" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E9" t="str">
-        <v>maeemuir@tpg.com.au</v>
-      </c>
-      <c r="F9" t="str">
-        <v>439781947</v>
-      </c>
-      <c r="G9" t="str">
-        <v>Mt Eliza</v>
-      </c>
-      <c r="H9" t="str">
-        <v>A</v>
-      </c>
-      <c r="I9" t="str">
-        <v>available</v>
-      </c>
-      <c r="J9" t="str" xml:space="preserve">
+      <c r="J8" t="str" xml:space="preserve">
         <v xml:space="preserve">Would be a group of up to 8 ladies._x000d_
 Amanda Hobbs_x000d_
 Kerry Wellington_x000d_
 Edwina Muir_x000d_
 </v>
       </c>
+      <c r="K8" t="str">
+        <v>5b77330c-45dc-4177-b704-50e8d2e75d75</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>24be11e0-6dfe-4b44-8d9f-162ec3002134</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Vivienne Degran</v>
+      </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E9" t="str">
+        <v>vrdegran@gmail.com</v>
+      </c>
+      <c r="F9" t="str">
+        <v>424953901</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Templestowe Lower</v>
+      </c>
+      <c r="H9" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I9" t="str">
+        <v>available</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Andrew Stringer</v>
+      </c>
       <c r="K9" t="str">
-        <v>5b77330c-45dc-4177-b704-50e8d2e75d75</v>
+        <v>59e24653-3037-4c9a-aaf1-2e7ed15cfee4</v>
+      </c>
+      <c r="L9" t="str">
+        <v xml:space="preserve">I have ADHD which I don't consider a disability. I wasn't going to say anything but got anxious about how specific you wanted me to be and then I overthought it.  </v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>24be11e0-6dfe-4b44-8d9f-162ec3002134</v>
+        <v>05ef4417-fb40-46b7-8dfd-3c178684509e</v>
       </c>
       <c r="B10" t="str">
+        <v>Andrew Stringer</v>
+      </c>
+      <c r="C10">
+        <v>37</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E10" t="str">
+        <v>a_string@hotmail.com</v>
+      </c>
+      <c r="F10" t="str">
+        <v>417534471</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Lower Templestowe</v>
+      </c>
+      <c r="H10" t="str">
+        <v>B+</v>
+      </c>
+      <c r="I10" t="str">
+        <v>available</v>
+      </c>
+      <c r="J10" t="str">
         <v>Vivienne Degran</v>
-      </c>
-      <c r="C10">
-        <v>36</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Female</v>
-      </c>
-      <c r="E10" t="str">
-        <v>vrdegran@gmail.com</v>
-      </c>
-      <c r="F10" t="str">
-        <v>424953901</v>
-      </c>
-      <c r="G10" t="str">
-        <v>Templestowe Lower</v>
-      </c>
-      <c r="H10" t="str">
-        <v>B+</v>
-      </c>
-      <c r="I10" t="str">
-        <v>available</v>
-      </c>
-      <c r="J10" t="str">
-        <v>Andrew Stringer</v>
       </c>
       <c r="K10" t="str">
         <v>59e24653-3037-4c9a-aaf1-2e7ed15cfee4</v>
       </c>
-      <c r="L10" t="str">
-        <v xml:space="preserve">I have ADHD which I don't consider a disability. I wasn't going to say anything but got anxious about how specific you wanted me to be and then I overthought it.  </v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>05ef4417-fb40-46b7-8dfd-3c178684509e</v>
+        <v>3292e33d-7639-461a-8a89-7088c0d90926</v>
       </c>
       <c r="B11" t="str">
-        <v>Andrew Stringer</v>
+        <v>Sophia papas</v>
       </c>
       <c r="C11">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D11" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E11" t="str">
-        <v>a_string@hotmail.com</v>
+        <v>sophiapapas6@hotmail.com</v>
       </c>
       <c r="F11" t="str">
-        <v>417534471</v>
+        <v>498868739</v>
       </c>
       <c r="G11" t="str">
-        <v>Lower Templestowe</v>
+        <v>Melbourne</v>
       </c>
       <c r="H11" t="str">
         <v>B+</v>
@@ -1067,33 +1067,33 @@
         <v>available</v>
       </c>
       <c r="J11" t="str">
-        <v>Vivienne Degran</v>
+        <v>Effie Vlangos, Christina papas, Sophia papas</v>
       </c>
       <c r="K11" t="str">
-        <v>59e24653-3037-4c9a-aaf1-2e7ed15cfee4</v>
+        <v>465f25a6-51b9-4661-9750-a89a88d3bc67</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>3292e33d-7639-461a-8a89-7088c0d90926</v>
+        <v>bc9034ab-64c0-4b4a-ab31-63704a9798ce</v>
       </c>
       <c r="B12" t="str">
-        <v>Sophia papas</v>
+        <v>Shane Gruis</v>
       </c>
       <c r="C12">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D12" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E12" t="str">
-        <v>sophiapapas6@hotmail.com</v>
+        <v>shaneg87@hotmail.com</v>
       </c>
       <c r="F12" t="str">
-        <v>498868739</v>
+        <v>407714293</v>
       </c>
       <c r="G12" t="str">
-        <v>Melbourne</v>
+        <v xml:space="preserve">Traralgon </v>
       </c>
       <c r="H12" t="str">
         <v>B+</v>
@@ -1102,97 +1102,100 @@
         <v>available</v>
       </c>
       <c r="J12" t="str">
-        <v>Effie Vlangos, Christina papas, Sophia papas</v>
+        <v>Brooke Monaghan</v>
       </c>
       <c r="K12" t="str">
-        <v>465f25a6-51b9-4661-9750-a89a88d3bc67</v>
+        <v>a768bfd0-4262-44dc-b6bb-e1b7e45ea930</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>bc9034ab-64c0-4b4a-ab31-63704a9798ce</v>
+        <v>dc9d5c0e-64f3-4361-bd0b-c6e1d71050d7</v>
       </c>
       <c r="B13" t="str">
-        <v>Shane Gruis</v>
+        <v>Hannah Mclaughlin</v>
       </c>
       <c r="C13">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D13" t="str">
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="E13" t="str">
-        <v>shaneg87@hotmail.com</v>
+        <v>Hannahlmclaughlin@gmail.com</v>
       </c>
       <c r="F13" t="str">
-        <v>407714293</v>
+        <v>402367400</v>
       </c>
       <c r="G13" t="str">
-        <v xml:space="preserve">Traralgon </v>
+        <v>Melbourne</v>
       </c>
       <c r="H13" t="str">
         <v>B+</v>
       </c>
       <c r="I13" t="str">
         <v>available</v>
-      </c>
-      <c r="J13" t="str">
-        <v>Brooke Monaghan</v>
-      </c>
-      <c r="K13" t="str">
-        <v>a768bfd0-4262-44dc-b6bb-e1b7e45ea930</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>dc9d5c0e-64f3-4361-bd0b-c6e1d71050d7</v>
+        <v>b422c78b-6705-4b03-94ee-6bdd0b4715ac</v>
       </c>
       <c r="B14" t="str">
-        <v>Hannah Mclaughlin</v>
+        <v>Susan McKenna</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D14" t="str">
         <v>Female</v>
       </c>
       <c r="E14" t="str">
-        <v>Hannahlmclaughlin@gmail.com</v>
+        <v>suemckenna627@gmail.com</v>
       </c>
       <c r="F14" t="str">
-        <v>402367400</v>
+        <v>455215555</v>
       </c>
       <c r="G14" t="str">
-        <v>Melbourne</v>
+        <v>Officer South</v>
       </c>
       <c r="H14" t="str">
         <v>B+</v>
       </c>
       <c r="I14" t="str">
         <v>available</v>
+      </c>
+      <c r="J14" t="str">
+        <v>SOLO</v>
+      </c>
+      <c r="K14" t="str">
+        <v>65d7aafc-81dc-4167-9597-567ea7a89170</v>
+      </c>
+      <c r="M14" t="str">
+        <v>NA</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>b422c78b-6705-4b03-94ee-6bdd0b4715ac</v>
+        <v>df2f5cbc-b306-437c-99c6-700cbbf31c71</v>
       </c>
       <c r="B15" t="str">
-        <v>Susan McKenna</v>
+        <v>Hayley Jenkins</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D15" t="str">
         <v>Female</v>
       </c>
       <c r="E15" t="str">
-        <v>suemckenna627@gmail.com</v>
+        <v>hkarynjenkins@gmail.com</v>
       </c>
       <c r="F15" t="str">
-        <v>455215555</v>
+        <v>405270888</v>
       </c>
       <c r="G15" t="str">
-        <v>Officer South</v>
+        <v>BENTLEIGH EAST</v>
       </c>
       <c r="H15" t="str">
         <v>B+</v>
@@ -1201,36 +1204,33 @@
         <v>available</v>
       </c>
       <c r="J15" t="str">
-        <v>SOLO</v>
+        <v>Paragi Doshi</v>
       </c>
       <c r="K15" t="str">
-        <v>65d7aafc-81dc-4167-9597-567ea7a89170</v>
-      </c>
-      <c r="M15" t="str">
-        <v>NA</v>
+        <v>6387251b-466b-408c-9aee-fcf8a05d21b7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>df2f5cbc-b306-437c-99c6-700cbbf31c71</v>
+        <v>87467196-8e6a-4aa4-a098-051eeae34713</v>
       </c>
       <c r="B16" t="str">
-        <v>Hayley Jenkins</v>
+        <v>Matthew Sjostrom</v>
       </c>
       <c r="C16">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D16" t="str">
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="E16" t="str">
-        <v>hkarynjenkins@gmail.com</v>
+        <v>mattbenko01@gmail.com</v>
       </c>
       <c r="F16" t="str">
-        <v>405270888</v>
+        <v>451710041</v>
       </c>
       <c r="G16" t="str">
-        <v>BENTLEIGH EAST</v>
+        <v>Prahran</v>
       </c>
       <c r="H16" t="str">
         <v>B+</v>
@@ -1239,10 +1239,7 @@
         <v>available</v>
       </c>
       <c r="J16" t="str">
-        <v>Paragi Doshi</v>
-      </c>
-      <c r="K16" t="str">
-        <v>6387251b-466b-408c-9aee-fcf8a05d21b7</v>
+        <v>Roxanne Benko, Matthew Sjostrom, Lauren Namua</v>
       </c>
     </row>
     <row r="17">

</xml_diff>